<commit_message>
a new job undie
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Equip.xlsx
+++ b/ConfigData/Xlsx/Equip.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" activeTab="3"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
   </bookViews>
   <sheets>
     <sheet name="头盔" sheetId="3" r:id="rId1"/>
@@ -274,7 +274,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="219">
   <si>
     <t>wuqi01</t>
   </si>
@@ -950,7 +950,18 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>21100108|InitJobEquipEnd</t>
+    <t>21100109|InitJobEquipEnd</t>
+  </si>
+  <si>
+    <t>40;15;45</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>toukui29</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>骨盔</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -2793,8 +2804,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A3:M11" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
-  <autoFilter ref="A3:M11"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A3:M12" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
+  <autoFilter ref="A3:M12"/>
   <sortState ref="A4:T40">
     <sortCondition ref="A27"/>
   </sortState>
@@ -3176,10 +3187,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:K1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -3604,8 +3615,8 @@
       </c>
     </row>
     <row r="11" spans="1:13">
-      <c r="A11" s="7" t="s">
-        <v>215</v>
+      <c r="A11" s="7">
+        <v>21100108</v>
       </c>
       <c r="B11" s="10" t="s">
         <v>114</v>
@@ -3642,6 +3653,47 @@
       </c>
       <c r="M11" s="11" t="s">
         <v>212</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>218</v>
+      </c>
+      <c r="C12" s="10">
+        <v>0</v>
+      </c>
+      <c r="D12" s="10">
+        <v>1</v>
+      </c>
+      <c r="E12" s="1">
+        <v>1</v>
+      </c>
+      <c r="F12" s="10">
+        <v>1</v>
+      </c>
+      <c r="G12" s="10">
+        <v>1</v>
+      </c>
+      <c r="H12" s="7">
+        <v>70</v>
+      </c>
+      <c r="I12" s="7">
+        <v>0</v>
+      </c>
+      <c r="J12" s="12">
+        <v>11000009</v>
+      </c>
+      <c r="K12" t="s">
+        <v>216</v>
+      </c>
+      <c r="L12">
+        <v>31000009</v>
+      </c>
+      <c r="M12" s="11" t="s">
+        <v>217</v>
       </c>
     </row>
   </sheetData>
@@ -6296,8 +6348,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:K1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>

</xml_diff>

<commit_message>
#44 equip effect update
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Equip.xlsx
+++ b/ConfigData/Xlsx/Equip.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="36" windowWidth="18132" windowHeight="8388"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
   </bookViews>
   <sheets>
     <sheet name="头盔" sheetId="3" r:id="rId1"/>
@@ -1784,6 +1784,41 @@
         <name val="宋体"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="thin">
@@ -2178,60 +2213,6 @@
         <name val="宋体"/>
         <scheme val="minor"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -2886,37 +2867,37 @@
     <tableColumn id="5" name="Position" dataDxfId="21"/>
     <tableColumn id="8" name="LvNeed" dataDxfId="20"/>
     <tableColumn id="9" name="Value" dataDxfId="19"/>
-    <tableColumn id="10" name="AtkP" dataDxfId="18"/>
-    <tableColumn id="16" name="VitP" dataDxfId="17"/>
-    <tableColumn id="19" name="Job" dataDxfId="16"/>
-    <tableColumn id="18" name="EnergyRate" dataDxfId="15"/>
+    <tableColumn id="10" name="AtkP" dataDxfId="1"/>
+    <tableColumn id="16" name="VitP" dataDxfId="0"/>
+    <tableColumn id="19" name="Job" dataDxfId="18"/>
+    <tableColumn id="18" name="EnergyRate" dataDxfId="17"/>
     <tableColumn id="20" name="SpecialSkill"/>
-    <tableColumn id="17" name="Url" dataDxfId="14"/>
+    <tableColumn id="17" name="Url" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:M26" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:M26" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
   <autoFilter ref="A3:M26"/>
   <sortState ref="A4:J26">
     <sortCondition ref="A3:A26"/>
   </sortState>
   <tableColumns count="13">
-    <tableColumn id="1" name="Id" dataDxfId="11"/>
-    <tableColumn id="2" name="Name" dataDxfId="10"/>
-    <tableColumn id="3" name="Quality" dataDxfId="9"/>
-    <tableColumn id="4" name="Level" dataDxfId="8"/>
-    <tableColumn id="5" name="Position" dataDxfId="7"/>
-    <tableColumn id="7" name="LvNeed" dataDxfId="6"/>
-    <tableColumn id="8" name="Value" dataDxfId="5"/>
-    <tableColumn id="9" name="AtkP" dataDxfId="4"/>
-    <tableColumn id="16" name="VitP" dataDxfId="3"/>
-    <tableColumn id="18" name="Job" dataDxfId="2"/>
-    <tableColumn id="19" name="EnergyRate" dataDxfId="1"/>
+    <tableColumn id="1" name="Id" dataDxfId="13"/>
+    <tableColumn id="2" name="Name" dataDxfId="12"/>
+    <tableColumn id="3" name="Quality" dataDxfId="11"/>
+    <tableColumn id="4" name="Level" dataDxfId="10"/>
+    <tableColumn id="5" name="Position" dataDxfId="9"/>
+    <tableColumn id="7" name="LvNeed" dataDxfId="8"/>
+    <tableColumn id="8" name="Value" dataDxfId="7"/>
+    <tableColumn id="9" name="AtkP" dataDxfId="6"/>
+    <tableColumn id="16" name="VitP" dataDxfId="5"/>
+    <tableColumn id="18" name="Job" dataDxfId="4"/>
+    <tableColumn id="19" name="EnergyRate" dataDxfId="3"/>
     <tableColumn id="20" name="SpecialSkill"/>
-    <tableColumn id="17" name="Url" dataDxfId="0"/>
+    <tableColumn id="17" name="Url" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3212,18 +3193,18 @@
   <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="7" width="5.6640625" customWidth="1"/>
-    <col min="8" max="9" width="5.44140625" customWidth="1"/>
-    <col min="10" max="10" width="10.109375" customWidth="1"/>
-    <col min="11" max="11" width="8.44140625" customWidth="1"/>
-    <col min="12" max="12" width="10.109375" customWidth="1"/>
-    <col min="15" max="15" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="7" width="5.625" customWidth="1"/>
+    <col min="8" max="9" width="5.5" customWidth="1"/>
+    <col min="10" max="10" width="10.125" customWidth="1"/>
+    <col min="11" max="11" width="8.5" customWidth="1"/>
+    <col min="12" max="12" width="10.125" customWidth="1"/>
+    <col min="15" max="15" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="79.5" customHeight="1">
@@ -3778,13 +3759,13 @@
       <selection activeCell="I1" sqref="I1:K1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="3" max="5" width="5.44140625" customWidth="1"/>
-    <col min="6" max="7" width="6.44140625" customWidth="1"/>
-    <col min="8" max="9" width="5.109375" customWidth="1"/>
-    <col min="10" max="12" width="8.6640625" customWidth="1"/>
-    <col min="15" max="15" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="5.5" customWidth="1"/>
+    <col min="6" max="7" width="6.5" customWidth="1"/>
+    <col min="8" max="9" width="5.125" customWidth="1"/>
+    <col min="10" max="12" width="8.625" customWidth="1"/>
+    <col min="15" max="15" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="42.75" customHeight="1">
@@ -5074,15 +5055,16 @@
   <dimension ref="A1:M32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="3" max="7" width="6.44140625" customWidth="1"/>
-    <col min="8" max="10" width="5.33203125" customWidth="1"/>
-    <col min="11" max="12" width="9.44140625" customWidth="1"/>
-    <col min="15" max="15" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="7" width="6.5" customWidth="1"/>
+    <col min="8" max="10" width="5.375" customWidth="1"/>
+    <col min="11" max="12" width="9.5" customWidth="1"/>
+    <col min="15" max="15" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="65.25" customHeight="1">
@@ -5234,7 +5216,7 @@
         <v>0</v>
       </c>
       <c r="I4" s="7">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="J4" s="7">
         <v>0</v>
@@ -5275,7 +5257,7 @@
         <v>0</v>
       </c>
       <c r="I5" s="7">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="J5" s="7">
         <v>0</v>
@@ -5316,7 +5298,7 @@
         <v>0</v>
       </c>
       <c r="I6" s="7">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="J6" s="7">
         <v>0</v>
@@ -5357,7 +5339,7 @@
         <v>0</v>
       </c>
       <c r="I7" s="7">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="J7" s="7">
         <v>0</v>
@@ -5398,7 +5380,7 @@
         <v>0</v>
       </c>
       <c r="I8" s="7">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="J8" s="7">
         <v>0</v>
@@ -5439,7 +5421,7 @@
         <v>0</v>
       </c>
       <c r="I9" s="7">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="J9" s="7">
         <v>0</v>
@@ -5480,7 +5462,7 @@
         <v>0</v>
       </c>
       <c r="I10" s="7">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="J10" s="7">
         <v>0</v>
@@ -5521,7 +5503,7 @@
         <v>0</v>
       </c>
       <c r="I11" s="7">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="J11" s="7">
         <v>0</v>
@@ -5562,7 +5544,7 @@
         <v>0</v>
       </c>
       <c r="I12" s="7">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="J12" s="7">
         <v>0</v>
@@ -5603,7 +5585,7 @@
         <v>0</v>
       </c>
       <c r="I13" s="7">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="J13" s="7">
         <v>0</v>
@@ -5644,7 +5626,7 @@
         <v>0</v>
       </c>
       <c r="I14" s="7">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="J14" s="7">
         <v>0</v>
@@ -5685,7 +5667,7 @@
         <v>0</v>
       </c>
       <c r="I15" s="7">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="J15" s="7">
         <v>0</v>
@@ -5726,7 +5708,7 @@
         <v>0</v>
       </c>
       <c r="I16" s="7">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="J16" s="7">
         <v>0</v>
@@ -5767,7 +5749,7 @@
         <v>0</v>
       </c>
       <c r="I17" s="7">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="J17" s="7">
         <v>0</v>
@@ -5808,7 +5790,7 @@
         <v>0</v>
       </c>
       <c r="I18" s="7">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="J18" s="7">
         <v>0</v>
@@ -5849,7 +5831,7 @@
         <v>0</v>
       </c>
       <c r="I19" s="7">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="J19" s="7">
         <v>0</v>
@@ -5890,7 +5872,7 @@
         <v>0</v>
       </c>
       <c r="I20" s="7">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="J20" s="7">
         <v>0</v>
@@ -5931,7 +5913,7 @@
         <v>0</v>
       </c>
       <c r="I21" s="7">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="J21" s="7">
         <v>0</v>
@@ -5972,7 +5954,7 @@
         <v>0</v>
       </c>
       <c r="I22" s="7">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="J22" s="7">
         <v>0</v>
@@ -6013,7 +5995,7 @@
         <v>0</v>
       </c>
       <c r="I23" s="7">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="J23" s="7">
         <v>0</v>
@@ -6054,7 +6036,7 @@
         <v>0</v>
       </c>
       <c r="I24" s="7">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="J24" s="7">
         <v>0</v>
@@ -6095,7 +6077,7 @@
         <v>0</v>
       </c>
       <c r="I25" s="7">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="J25" s="7">
         <v>0</v>
@@ -6136,7 +6118,7 @@
         <v>0</v>
       </c>
       <c r="I26" s="7">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="J26" s="7">
         <v>0</v>
@@ -6177,7 +6159,7 @@
         <v>0</v>
       </c>
       <c r="I27" s="7">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="J27" s="7">
         <v>0</v>
@@ -6218,7 +6200,7 @@
         <v>0</v>
       </c>
       <c r="I28" s="7">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="J28" s="7">
         <v>0</v>
@@ -6259,7 +6241,7 @@
         <v>0</v>
       </c>
       <c r="I29" s="7">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="J29" s="7">
         <v>0</v>
@@ -6300,7 +6282,7 @@
         <v>0</v>
       </c>
       <c r="I30" s="7">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="J30" s="7">
         <v>0</v>
@@ -6341,7 +6323,7 @@
         <v>0</v>
       </c>
       <c r="I31" s="7">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="J31" s="7">
         <v>0</v>
@@ -6382,7 +6364,7 @@
         <v>0</v>
       </c>
       <c r="I32" s="7">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="J32" s="7">
         <v>0</v>
@@ -6415,12 +6397,12 @@
       <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="3" max="7" width="6.21875" customWidth="1"/>
-    <col min="8" max="10" width="4.77734375" customWidth="1"/>
-    <col min="11" max="12" width="5.88671875" customWidth="1"/>
-    <col min="16" max="16" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="7" width="6.25" customWidth="1"/>
+    <col min="8" max="10" width="4.75" customWidth="1"/>
+    <col min="11" max="12" width="5.875" customWidth="1"/>
+    <col min="16" max="16" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="64.5" customHeight="1">

</xml_diff>

<commit_message>
close #44 finish the normal effect support
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Equip.xlsx
+++ b/ConfigData/Xlsx/Equip.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
+    <workbookView xWindow="600" yWindow="36" windowWidth="18132" windowHeight="8388" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="头盔" sheetId="3" r:id="rId1"/>
@@ -1784,41 +1784,6 @@
         <name val="宋体"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="thin">
@@ -2196,6 +2161,41 @@
         <name val="宋体"/>
         <scheme val="minor"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -2867,37 +2867,37 @@
     <tableColumn id="5" name="Position" dataDxfId="21"/>
     <tableColumn id="8" name="LvNeed" dataDxfId="20"/>
     <tableColumn id="9" name="Value" dataDxfId="19"/>
-    <tableColumn id="10" name="AtkP" dataDxfId="1"/>
-    <tableColumn id="16" name="VitP" dataDxfId="0"/>
-    <tableColumn id="19" name="Job" dataDxfId="18"/>
-    <tableColumn id="18" name="EnergyRate" dataDxfId="17"/>
+    <tableColumn id="10" name="AtkP" dataDxfId="18"/>
+    <tableColumn id="16" name="VitP" dataDxfId="17"/>
+    <tableColumn id="19" name="Job" dataDxfId="16"/>
+    <tableColumn id="18" name="EnergyRate" dataDxfId="15"/>
     <tableColumn id="20" name="SpecialSkill"/>
-    <tableColumn id="17" name="Url" dataDxfId="16"/>
+    <tableColumn id="17" name="Url" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:M26" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:M26" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
   <autoFilter ref="A3:M26"/>
   <sortState ref="A4:J26">
     <sortCondition ref="A3:A26"/>
   </sortState>
   <tableColumns count="13">
-    <tableColumn id="1" name="Id" dataDxfId="13"/>
-    <tableColumn id="2" name="Name" dataDxfId="12"/>
-    <tableColumn id="3" name="Quality" dataDxfId="11"/>
-    <tableColumn id="4" name="Level" dataDxfId="10"/>
-    <tableColumn id="5" name="Position" dataDxfId="9"/>
-    <tableColumn id="7" name="LvNeed" dataDxfId="8"/>
-    <tableColumn id="8" name="Value" dataDxfId="7"/>
-    <tableColumn id="9" name="AtkP" dataDxfId="6"/>
-    <tableColumn id="16" name="VitP" dataDxfId="5"/>
-    <tableColumn id="18" name="Job" dataDxfId="4"/>
-    <tableColumn id="19" name="EnergyRate" dataDxfId="3"/>
+    <tableColumn id="1" name="Id" dataDxfId="11"/>
+    <tableColumn id="2" name="Name" dataDxfId="10"/>
+    <tableColumn id="3" name="Quality" dataDxfId="9"/>
+    <tableColumn id="4" name="Level" dataDxfId="8"/>
+    <tableColumn id="5" name="Position" dataDxfId="7"/>
+    <tableColumn id="7" name="LvNeed" dataDxfId="6"/>
+    <tableColumn id="8" name="Value" dataDxfId="5"/>
+    <tableColumn id="9" name="AtkP" dataDxfId="4"/>
+    <tableColumn id="16" name="VitP" dataDxfId="3"/>
+    <tableColumn id="18" name="Job" dataDxfId="2"/>
+    <tableColumn id="19" name="EnergyRate" dataDxfId="1"/>
     <tableColumn id="20" name="SpecialSkill"/>
-    <tableColumn id="17" name="Url" dataDxfId="2"/>
+    <tableColumn id="17" name="Url" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3192,19 +3192,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="7" width="5.625" customWidth="1"/>
-    <col min="8" max="9" width="5.5" customWidth="1"/>
-    <col min="10" max="10" width="10.125" customWidth="1"/>
-    <col min="11" max="11" width="8.5" customWidth="1"/>
-    <col min="12" max="12" width="10.125" customWidth="1"/>
-    <col min="15" max="15" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="7" width="5.6640625" customWidth="1"/>
+    <col min="8" max="9" width="5.44140625" customWidth="1"/>
+    <col min="10" max="10" width="10.109375" customWidth="1"/>
+    <col min="11" max="11" width="8.44140625" customWidth="1"/>
+    <col min="12" max="12" width="10.109375" customWidth="1"/>
+    <col min="15" max="15" width="9.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="79.5" customHeight="1">
@@ -3353,7 +3353,7 @@
         <v>1</v>
       </c>
       <c r="H4" s="7">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="I4" s="7">
         <v>0</v>
@@ -3394,7 +3394,7 @@
         <v>1</v>
       </c>
       <c r="H5" s="7">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="I5" s="7">
         <v>0</v>
@@ -3435,7 +3435,7 @@
         <v>1</v>
       </c>
       <c r="H6" s="7">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="I6" s="7">
         <v>0</v>
@@ -3476,7 +3476,7 @@
         <v>1</v>
       </c>
       <c r="H7" s="7">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="I7" s="7">
         <v>0</v>
@@ -3517,7 +3517,7 @@
         <v>1</v>
       </c>
       <c r="H8" s="7">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="I8" s="7">
         <v>0</v>
@@ -3558,7 +3558,7 @@
         <v>1</v>
       </c>
       <c r="H9" s="7">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="I9" s="7">
         <v>0</v>
@@ -3599,7 +3599,7 @@
         <v>1</v>
       </c>
       <c r="H10" s="7">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="I10" s="7">
         <v>0</v>
@@ -3640,7 +3640,7 @@
         <v>1</v>
       </c>
       <c r="H11" s="7">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="I11" s="7">
         <v>0</v>
@@ -3681,7 +3681,7 @@
         <v>1</v>
       </c>
       <c r="H12" s="7">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="I12" s="7">
         <v>0</v>
@@ -3721,8 +3721,8 @@
       <c r="G13" s="10">
         <v>1</v>
       </c>
-      <c r="H13" s="10">
-        <v>70</v>
+      <c r="H13" s="7">
+        <v>50</v>
       </c>
       <c r="I13" s="10">
         <v>0</v>
@@ -3756,16 +3756,16 @@
   <dimension ref="A1:M31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:K1048576"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="3" max="5" width="5.5" customWidth="1"/>
-    <col min="6" max="7" width="6.5" customWidth="1"/>
-    <col min="8" max="9" width="5.125" customWidth="1"/>
-    <col min="10" max="12" width="8.625" customWidth="1"/>
-    <col min="15" max="15" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="5.44140625" customWidth="1"/>
+    <col min="6" max="7" width="6.44140625" customWidth="1"/>
+    <col min="8" max="9" width="5.109375" customWidth="1"/>
+    <col min="10" max="12" width="8.6640625" customWidth="1"/>
+    <col min="15" max="15" width="9.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="42.75" customHeight="1">
@@ -5058,13 +5058,13 @@
       <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="7" width="6.5" customWidth="1"/>
-    <col min="8" max="10" width="5.375" customWidth="1"/>
-    <col min="11" max="12" width="9.5" customWidth="1"/>
-    <col min="15" max="15" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="7" width="6.44140625" customWidth="1"/>
+    <col min="8" max="10" width="5.33203125" customWidth="1"/>
+    <col min="11" max="12" width="9.44140625" customWidth="1"/>
+    <col min="15" max="15" width="9.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="65.25" customHeight="1">
@@ -6393,16 +6393,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="3" max="7" width="6.25" customWidth="1"/>
-    <col min="8" max="10" width="4.75" customWidth="1"/>
-    <col min="11" max="12" width="5.875" customWidth="1"/>
-    <col min="16" max="16" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="7" width="6.21875" customWidth="1"/>
+    <col min="8" max="10" width="4.77734375" customWidth="1"/>
+    <col min="11" max="12" width="5.88671875" customWidth="1"/>
+    <col min="16" max="16" width="9.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="64.5" customHeight="1">
@@ -6554,7 +6554,7 @@
         <v>0</v>
       </c>
       <c r="I4" s="7">
-        <v>200</v>
+        <v>30</v>
       </c>
       <c r="J4" s="7">
         <v>0</v>
@@ -6595,7 +6595,7 @@
         <v>0</v>
       </c>
       <c r="I5" s="7">
-        <v>200</v>
+        <v>30</v>
       </c>
       <c r="J5" s="7">
         <v>0</v>
@@ -6636,7 +6636,7 @@
         <v>0</v>
       </c>
       <c r="I6" s="7">
-        <v>200</v>
+        <v>30</v>
       </c>
       <c r="J6" s="7">
         <v>0</v>
@@ -6677,7 +6677,7 @@
         <v>0</v>
       </c>
       <c r="I7" s="7">
-        <v>200</v>
+        <v>30</v>
       </c>
       <c r="J7" s="7">
         <v>0</v>
@@ -6718,7 +6718,7 @@
         <v>0</v>
       </c>
       <c r="I8" s="7">
-        <v>200</v>
+        <v>30</v>
       </c>
       <c r="J8" s="7">
         <v>0</v>
@@ -6759,7 +6759,7 @@
         <v>0</v>
       </c>
       <c r="I9" s="7">
-        <v>200</v>
+        <v>30</v>
       </c>
       <c r="J9" s="7">
         <v>0</v>
@@ -6800,7 +6800,7 @@
         <v>0</v>
       </c>
       <c r="I10" s="7">
-        <v>200</v>
+        <v>30</v>
       </c>
       <c r="J10" s="7">
         <v>0</v>
@@ -6841,7 +6841,7 @@
         <v>0</v>
       </c>
       <c r="I11" s="7">
-        <v>200</v>
+        <v>30</v>
       </c>
       <c r="J11" s="7">
         <v>0</v>
@@ -6882,7 +6882,7 @@
         <v>0</v>
       </c>
       <c r="I12" s="7">
-        <v>200</v>
+        <v>30</v>
       </c>
       <c r="J12" s="7">
         <v>0</v>
@@ -6923,7 +6923,7 @@
         <v>0</v>
       </c>
       <c r="I13" s="7">
-        <v>200</v>
+        <v>30</v>
       </c>
       <c r="J13" s="7">
         <v>0</v>
@@ -6964,7 +6964,7 @@
         <v>0</v>
       </c>
       <c r="I14" s="7">
-        <v>200</v>
+        <v>30</v>
       </c>
       <c r="J14" s="7">
         <v>0</v>
@@ -7005,7 +7005,7 @@
         <v>0</v>
       </c>
       <c r="I15" s="7">
-        <v>200</v>
+        <v>30</v>
       </c>
       <c r="J15" s="7">
         <v>0</v>
@@ -7046,7 +7046,7 @@
         <v>0</v>
       </c>
       <c r="I16" s="7">
-        <v>200</v>
+        <v>30</v>
       </c>
       <c r="J16" s="7">
         <v>0</v>
@@ -7087,7 +7087,7 @@
         <v>0</v>
       </c>
       <c r="I17" s="7">
-        <v>200</v>
+        <v>30</v>
       </c>
       <c r="J17" s="7">
         <v>0</v>
@@ -7128,7 +7128,7 @@
         <v>0</v>
       </c>
       <c r="I18" s="7">
-        <v>200</v>
+        <v>30</v>
       </c>
       <c r="J18" s="7">
         <v>0</v>
@@ -7169,7 +7169,7 @@
         <v>0</v>
       </c>
       <c r="I19" s="7">
-        <v>200</v>
+        <v>30</v>
       </c>
       <c r="J19" s="7">
         <v>0</v>
@@ -7210,7 +7210,7 @@
         <v>0</v>
       </c>
       <c r="I20" s="7">
-        <v>200</v>
+        <v>30</v>
       </c>
       <c r="J20" s="7">
         <v>0</v>
@@ -7251,7 +7251,7 @@
         <v>0</v>
       </c>
       <c r="I21" s="7">
-        <v>200</v>
+        <v>30</v>
       </c>
       <c r="J21" s="7">
         <v>0</v>
@@ -7292,7 +7292,7 @@
         <v>0</v>
       </c>
       <c r="I22" s="7">
-        <v>200</v>
+        <v>30</v>
       </c>
       <c r="J22" s="7">
         <v>0</v>
@@ -7333,7 +7333,7 @@
         <v>0</v>
       </c>
       <c r="I23" s="7">
-        <v>200</v>
+        <v>30</v>
       </c>
       <c r="J23" s="7">
         <v>0</v>
@@ -7374,7 +7374,7 @@
         <v>0</v>
       </c>
       <c r="I24" s="7">
-        <v>200</v>
+        <v>30</v>
       </c>
       <c r="J24" s="7">
         <v>0</v>
@@ -7415,7 +7415,7 @@
         <v>0</v>
       </c>
       <c r="I25" s="7">
-        <v>200</v>
+        <v>30</v>
       </c>
       <c r="J25" s="7">
         <v>0</v>
@@ -7456,7 +7456,7 @@
         <v>0</v>
       </c>
       <c r="I26" s="7">
-        <v>200</v>
+        <v>30</v>
       </c>
       <c r="J26" s="7">
         <v>0</v>

</xml_diff>

<commit_message>
card region show in deckview clearly
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Equip.xlsx
+++ b/ConfigData/Xlsx/Equip.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="36" windowWidth="18132" windowHeight="8388" activeTab="3"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
   </bookViews>
   <sheets>
     <sheet name="头盔" sheetId="3" r:id="rId1"/>
@@ -274,7 +274,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="225">
   <si>
     <t>wuqi01</t>
   </si>
@@ -901,26 +901,6 @@
     <t>EnergyRate</t>
   </si>
   <si>
-    <t>45;25;30</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>50;20;30</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>35;15;50</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>40;15;45</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>45;15;40</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>0;0;0</t>
   </si>
   <si>
@@ -950,10 +930,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>40;15;45</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>toukui29</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -970,6 +946,46 @@
   </si>
   <si>
     <t>斗篷</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>60;20;20</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>60;20;20</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>60;15;25</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>60;25;15</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>55;20;25</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>50;10;40</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>50;15;35</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>55;10;35</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>55;10;35</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>50;20;30</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -3192,19 +3208,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4:K13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="7" width="5.6640625" customWidth="1"/>
-    <col min="8" max="9" width="5.44140625" customWidth="1"/>
-    <col min="10" max="10" width="10.109375" customWidth="1"/>
-    <col min="11" max="11" width="8.44140625" customWidth="1"/>
-    <col min="12" max="12" width="10.109375" customWidth="1"/>
-    <col min="15" max="15" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="7" width="5.625" customWidth="1"/>
+    <col min="8" max="9" width="5.5" customWidth="1"/>
+    <col min="10" max="10" width="10.125" customWidth="1"/>
+    <col min="11" max="11" width="8.5" customWidth="1"/>
+    <col min="12" max="12" width="10.125" customWidth="1"/>
+    <col min="15" max="15" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="79.5" customHeight="1">
@@ -3242,7 +3258,7 @@
         <v>199</v>
       </c>
       <c r="L1" s="8" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="M1" s="8" t="s">
         <v>180</v>
@@ -3283,7 +3299,7 @@
         <v>200</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="M2" s="3" t="s">
         <v>172</v>
@@ -3324,7 +3340,7 @@
         <v>201</v>
       </c>
       <c r="L3" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="M3" t="s">
         <v>187</v>
@@ -3332,7 +3348,7 @@
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="7" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>119</v>
@@ -3361,8 +3377,8 @@
       <c r="J4" s="12">
         <v>11000001</v>
       </c>
-      <c r="K4" s="12" t="s">
-        <v>202</v>
+      <c r="K4" t="s">
+        <v>215</v>
       </c>
       <c r="L4">
         <v>31000001</v>
@@ -3402,8 +3418,8 @@
       <c r="J5" s="12">
         <v>11000002</v>
       </c>
-      <c r="K5" s="12" t="s">
-        <v>202</v>
+      <c r="K5" t="s">
+        <v>216</v>
       </c>
       <c r="L5">
         <v>31000002</v>
@@ -3443,8 +3459,8 @@
       <c r="J6" s="12">
         <v>11000003</v>
       </c>
-      <c r="K6" s="12" t="s">
-        <v>202</v>
+      <c r="K6" t="s">
+        <v>217</v>
       </c>
       <c r="L6">
         <v>31000003</v>
@@ -3458,7 +3474,7 @@
         <v>21100104</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="C7" s="10">
         <v>0</v>
@@ -3484,8 +3500,8 @@
       <c r="J7" s="12">
         <v>11000004</v>
       </c>
-      <c r="K7" s="12" t="s">
-        <v>202</v>
+      <c r="K7" t="s">
+        <v>218</v>
       </c>
       <c r="L7">
         <v>31000004</v>
@@ -3525,8 +3541,8 @@
       <c r="J8" s="12">
         <v>11000005</v>
       </c>
-      <c r="K8" s="12" t="s">
-        <v>203</v>
+      <c r="K8" t="s">
+        <v>219</v>
       </c>
       <c r="L8">
         <v>31000005</v>
@@ -3566,8 +3582,8 @@
       <c r="J9" s="12">
         <v>11000006</v>
       </c>
-      <c r="K9" s="12" t="s">
-        <v>204</v>
+      <c r="K9" t="s">
+        <v>220</v>
       </c>
       <c r="L9">
         <v>31000006</v>
@@ -3607,8 +3623,8 @@
       <c r="J10" s="12">
         <v>11000007</v>
       </c>
-      <c r="K10" s="12" t="s">
-        <v>205</v>
+      <c r="K10" t="s">
+        <v>221</v>
       </c>
       <c r="L10">
         <v>31000007</v>
@@ -3648,14 +3664,14 @@
       <c r="J11" s="12">
         <v>11000008</v>
       </c>
-      <c r="K11" s="12" t="s">
-        <v>206</v>
+      <c r="K11" t="s">
+        <v>222</v>
       </c>
       <c r="L11">
         <v>31000008</v>
       </c>
       <c r="M11" s="11" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
     </row>
     <row r="12" spans="1:13">
@@ -3663,7 +3679,7 @@
         <v>21100109</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="C12" s="10">
         <v>0</v>
@@ -3690,21 +3706,21 @@
         <v>11000009</v>
       </c>
       <c r="K12" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="L12">
         <v>31000009</v>
       </c>
       <c r="M12" s="11" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
     </row>
     <row r="13" spans="1:13">
       <c r="A13" s="13" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="C13" s="10">
         <v>0</v>
@@ -3730,14 +3746,14 @@
       <c r="J13" s="12">
         <v>11000010</v>
       </c>
-      <c r="K13" s="12" t="s">
-        <v>215</v>
+      <c r="K13" t="s">
+        <v>224</v>
       </c>
       <c r="L13">
         <v>31000010</v>
       </c>
       <c r="M13" s="11" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
     </row>
   </sheetData>
@@ -3759,13 +3775,13 @@
       <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="3" max="5" width="5.44140625" customWidth="1"/>
-    <col min="6" max="7" width="6.44140625" customWidth="1"/>
-    <col min="8" max="9" width="5.109375" customWidth="1"/>
-    <col min="10" max="12" width="8.6640625" customWidth="1"/>
-    <col min="15" max="15" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="5.5" customWidth="1"/>
+    <col min="6" max="7" width="6.5" customWidth="1"/>
+    <col min="8" max="9" width="5.125" customWidth="1"/>
+    <col min="10" max="12" width="8.625" customWidth="1"/>
+    <col min="15" max="15" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="42.75" customHeight="1">
@@ -3803,7 +3819,7 @@
         <v>199</v>
       </c>
       <c r="L1" s="8" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="M1" s="8" t="s">
         <v>180</v>
@@ -3844,7 +3860,7 @@
         <v>200</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="M2" s="3" t="s">
         <v>172</v>
@@ -3885,7 +3901,7 @@
         <v>201</v>
       </c>
       <c r="L3" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="M3" t="s">
         <v>187</v>
@@ -3923,7 +3939,7 @@
         <v>0</v>
       </c>
       <c r="K4" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="L4">
         <v>0</v>
@@ -3964,7 +3980,7 @@
         <v>0</v>
       </c>
       <c r="K5" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="L5">
         <v>0</v>
@@ -4005,7 +4021,7 @@
         <v>0</v>
       </c>
       <c r="K6" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="L6">
         <v>0</v>
@@ -4046,7 +4062,7 @@
         <v>0</v>
       </c>
       <c r="K7" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="L7">
         <v>0</v>
@@ -4087,7 +4103,7 @@
         <v>0</v>
       </c>
       <c r="K8" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="L8">
         <v>0</v>
@@ -4128,7 +4144,7 @@
         <v>0</v>
       </c>
       <c r="K9" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="L9">
         <v>0</v>
@@ -4169,7 +4185,7 @@
         <v>0</v>
       </c>
       <c r="K10" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="L10">
         <v>0</v>
@@ -4210,7 +4226,7 @@
         <v>0</v>
       </c>
       <c r="K11" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="L11">
         <v>0</v>
@@ -4251,7 +4267,7 @@
         <v>0</v>
       </c>
       <c r="K12" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="L12">
         <v>0</v>
@@ -4292,7 +4308,7 @@
         <v>0</v>
       </c>
       <c r="K13" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="L13">
         <v>0</v>
@@ -4333,7 +4349,7 @@
         <v>0</v>
       </c>
       <c r="K14" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="L14">
         <v>0</v>
@@ -4374,7 +4390,7 @@
         <v>0</v>
       </c>
       <c r="K15" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="L15">
         <v>0</v>
@@ -4415,7 +4431,7 @@
         <v>0</v>
       </c>
       <c r="K16" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="L16">
         <v>0</v>
@@ -4456,7 +4472,7 @@
         <v>0</v>
       </c>
       <c r="K17" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="L17">
         <v>0</v>
@@ -4497,7 +4513,7 @@
         <v>0</v>
       </c>
       <c r="K18" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="L18">
         <v>0</v>
@@ -4538,7 +4554,7 @@
         <v>0</v>
       </c>
       <c r="K19" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="L19">
         <v>0</v>
@@ -4579,7 +4595,7 @@
         <v>0</v>
       </c>
       <c r="K20" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="L20">
         <v>0</v>
@@ -4620,7 +4636,7 @@
         <v>0</v>
       </c>
       <c r="K21" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="L21">
         <v>0</v>
@@ -4661,7 +4677,7 @@
         <v>0</v>
       </c>
       <c r="K22" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="L22">
         <v>0</v>
@@ -4702,7 +4718,7 @@
         <v>0</v>
       </c>
       <c r="K23" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="L23">
         <v>0</v>
@@ -4743,7 +4759,7 @@
         <v>0</v>
       </c>
       <c r="K24" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="L24">
         <v>0</v>
@@ -4784,7 +4800,7 @@
         <v>0</v>
       </c>
       <c r="K25" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="L25">
         <v>0</v>
@@ -4825,7 +4841,7 @@
         <v>0</v>
       </c>
       <c r="K26" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="L26">
         <v>0</v>
@@ -4866,7 +4882,7 @@
         <v>0</v>
       </c>
       <c r="K27" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="L27">
         <v>0</v>
@@ -4907,7 +4923,7 @@
         <v>0</v>
       </c>
       <c r="K28" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="L28">
         <v>0</v>
@@ -4948,7 +4964,7 @@
         <v>0</v>
       </c>
       <c r="K29" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="L29">
         <v>0</v>
@@ -4989,7 +5005,7 @@
         <v>0</v>
       </c>
       <c r="K30" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="L30">
         <v>0</v>
@@ -5030,7 +5046,7 @@
         <v>0</v>
       </c>
       <c r="K31" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="L31">
         <v>0</v>
@@ -5058,13 +5074,13 @@
       <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="7" width="6.44140625" customWidth="1"/>
-    <col min="8" max="10" width="5.33203125" customWidth="1"/>
-    <col min="11" max="12" width="9.44140625" customWidth="1"/>
-    <col min="15" max="15" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="7" width="6.5" customWidth="1"/>
+    <col min="8" max="10" width="5.375" customWidth="1"/>
+    <col min="11" max="12" width="9.5" customWidth="1"/>
+    <col min="15" max="15" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="65.25" customHeight="1">
@@ -5102,7 +5118,7 @@
         <v>199</v>
       </c>
       <c r="L1" s="8" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="M1" s="8" t="s">
         <v>180</v>
@@ -5143,7 +5159,7 @@
         <v>200</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="M2" s="3" t="s">
         <v>172</v>
@@ -5184,7 +5200,7 @@
         <v>201</v>
       </c>
       <c r="L3" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="M3" t="s">
         <v>187</v>
@@ -5222,7 +5238,7 @@
         <v>0</v>
       </c>
       <c r="K4" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="L4">
         <v>0</v>
@@ -5263,7 +5279,7 @@
         <v>0</v>
       </c>
       <c r="K5" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="L5">
         <v>0</v>
@@ -5304,7 +5320,7 @@
         <v>0</v>
       </c>
       <c r="K6" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="L6">
         <v>0</v>
@@ -5345,7 +5361,7 @@
         <v>0</v>
       </c>
       <c r="K7" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="L7">
         <v>0</v>
@@ -5386,7 +5402,7 @@
         <v>0</v>
       </c>
       <c r="K8" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="L8">
         <v>0</v>
@@ -5427,7 +5443,7 @@
         <v>0</v>
       </c>
       <c r="K9" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="L9">
         <v>0</v>
@@ -5468,7 +5484,7 @@
         <v>0</v>
       </c>
       <c r="K10" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="L10">
         <v>0</v>
@@ -5509,7 +5525,7 @@
         <v>0</v>
       </c>
       <c r="K11" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="L11">
         <v>0</v>
@@ -5550,7 +5566,7 @@
         <v>0</v>
       </c>
       <c r="K12" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="L12">
         <v>0</v>
@@ -5591,7 +5607,7 @@
         <v>0</v>
       </c>
       <c r="K13" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="L13">
         <v>0</v>
@@ -5632,7 +5648,7 @@
         <v>0</v>
       </c>
       <c r="K14" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="L14">
         <v>0</v>
@@ -5673,7 +5689,7 @@
         <v>0</v>
       </c>
       <c r="K15" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="L15">
         <v>0</v>
@@ -5714,7 +5730,7 @@
         <v>0</v>
       </c>
       <c r="K16" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="L16">
         <v>0</v>
@@ -5755,7 +5771,7 @@
         <v>0</v>
       </c>
       <c r="K17" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="L17">
         <v>0</v>
@@ -5796,7 +5812,7 @@
         <v>0</v>
       </c>
       <c r="K18" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="L18">
         <v>0</v>
@@ -5837,7 +5853,7 @@
         <v>0</v>
       </c>
       <c r="K19" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="L19">
         <v>0</v>
@@ -5878,7 +5894,7 @@
         <v>0</v>
       </c>
       <c r="K20" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="L20">
         <v>0</v>
@@ -5919,7 +5935,7 @@
         <v>0</v>
       </c>
       <c r="K21" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="L21">
         <v>0</v>
@@ -5960,7 +5976,7 @@
         <v>0</v>
       </c>
       <c r="K22" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="L22">
         <v>0</v>
@@ -6001,7 +6017,7 @@
         <v>0</v>
       </c>
       <c r="K23" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="L23">
         <v>0</v>
@@ -6042,7 +6058,7 @@
         <v>0</v>
       </c>
       <c r="K24" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="L24">
         <v>0</v>
@@ -6083,7 +6099,7 @@
         <v>0</v>
       </c>
       <c r="K25" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="L25">
         <v>0</v>
@@ -6124,7 +6140,7 @@
         <v>0</v>
       </c>
       <c r="K26" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="L26">
         <v>0</v>
@@ -6165,7 +6181,7 @@
         <v>0</v>
       </c>
       <c r="K27" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="L27">
         <v>0</v>
@@ -6206,7 +6222,7 @@
         <v>0</v>
       </c>
       <c r="K28" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="L28">
         <v>0</v>
@@ -6247,7 +6263,7 @@
         <v>0</v>
       </c>
       <c r="K29" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="L29">
         <v>0</v>
@@ -6288,7 +6304,7 @@
         <v>0</v>
       </c>
       <c r="K30" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="L30">
         <v>0</v>
@@ -6329,7 +6345,7 @@
         <v>0</v>
       </c>
       <c r="K31" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="L31">
         <v>0</v>
@@ -6370,7 +6386,7 @@
         <v>0</v>
       </c>
       <c r="K32" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="L32">
         <v>0</v>
@@ -6393,16 +6409,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="3" max="7" width="6.21875" customWidth="1"/>
-    <col min="8" max="10" width="4.77734375" customWidth="1"/>
-    <col min="11" max="12" width="5.88671875" customWidth="1"/>
-    <col min="16" max="16" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="7" width="6.25" customWidth="1"/>
+    <col min="8" max="10" width="4.75" customWidth="1"/>
+    <col min="11" max="12" width="5.875" customWidth="1"/>
+    <col min="16" max="16" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="64.5" customHeight="1">
@@ -6440,7 +6456,7 @@
         <v>199</v>
       </c>
       <c r="L1" s="8" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="M1" s="8" t="s">
         <v>180</v>
@@ -6481,7 +6497,7 @@
         <v>200</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="M2" s="3" t="s">
         <v>172</v>
@@ -6522,7 +6538,7 @@
         <v>201</v>
       </c>
       <c r="L3" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="M3" t="s">
         <v>187</v>
@@ -6560,7 +6576,7 @@
         <v>0</v>
       </c>
       <c r="K4" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="L4">
         <v>0</v>
@@ -6601,7 +6617,7 @@
         <v>0</v>
       </c>
       <c r="K5" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="L5">
         <v>0</v>
@@ -6642,7 +6658,7 @@
         <v>0</v>
       </c>
       <c r="K6" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="L6">
         <v>0</v>
@@ -6683,7 +6699,7 @@
         <v>0</v>
       </c>
       <c r="K7" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="L7">
         <v>0</v>
@@ -6724,7 +6740,7 @@
         <v>0</v>
       </c>
       <c r="K8" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="L8">
         <v>0</v>
@@ -6765,7 +6781,7 @@
         <v>0</v>
       </c>
       <c r="K9" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="L9">
         <v>0</v>
@@ -6806,7 +6822,7 @@
         <v>0</v>
       </c>
       <c r="K10" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="L10">
         <v>0</v>
@@ -6847,7 +6863,7 @@
         <v>0</v>
       </c>
       <c r="K11" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="L11">
         <v>0</v>
@@ -6888,7 +6904,7 @@
         <v>0</v>
       </c>
       <c r="K12" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="L12">
         <v>0</v>
@@ -6929,7 +6945,7 @@
         <v>0</v>
       </c>
       <c r="K13" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="L13">
         <v>0</v>
@@ -6970,7 +6986,7 @@
         <v>0</v>
       </c>
       <c r="K14" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="L14">
         <v>0</v>
@@ -7011,7 +7027,7 @@
         <v>0</v>
       </c>
       <c r="K15" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="L15">
         <v>0</v>
@@ -7052,7 +7068,7 @@
         <v>0</v>
       </c>
       <c r="K16" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="L16">
         <v>0</v>
@@ -7093,7 +7109,7 @@
         <v>0</v>
       </c>
       <c r="K17" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="L17">
         <v>0</v>
@@ -7134,7 +7150,7 @@
         <v>0</v>
       </c>
       <c r="K18" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="L18">
         <v>0</v>
@@ -7175,7 +7191,7 @@
         <v>0</v>
       </c>
       <c r="K19" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="L19">
         <v>0</v>
@@ -7216,7 +7232,7 @@
         <v>0</v>
       </c>
       <c r="K20" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="L20">
         <v>0</v>
@@ -7257,7 +7273,7 @@
         <v>0</v>
       </c>
       <c r="K21" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="L21">
         <v>0</v>
@@ -7298,7 +7314,7 @@
         <v>0</v>
       </c>
       <c r="K22" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="L22">
         <v>0</v>
@@ -7339,7 +7355,7 @@
         <v>0</v>
       </c>
       <c r="K23" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="L23">
         <v>0</v>
@@ -7380,7 +7396,7 @@
         <v>0</v>
       </c>
       <c r="K24" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="L24">
         <v>0</v>
@@ -7421,7 +7437,7 @@
         <v>0</v>
       </c>
       <c r="K25" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="L25">
         <v>0</v>
@@ -7462,7 +7478,7 @@
         <v>0</v>
       </c>
       <c r="K26" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="L26">
         <v>0</v>

</xml_diff>

<commit_message>
change the hero skill
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Equip.xlsx
+++ b/ConfigData/Xlsx/Equip.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
+    <workbookView xWindow="600" yWindow="36" windowWidth="18132" windowHeight="8388"/>
   </bookViews>
   <sheets>
     <sheet name="头盔" sheetId="3" r:id="rId1"/>
@@ -3209,18 +3209,18 @@
   <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4:K13"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="7" width="5.625" customWidth="1"/>
-    <col min="8" max="9" width="5.5" customWidth="1"/>
-    <col min="10" max="10" width="10.125" customWidth="1"/>
-    <col min="11" max="11" width="8.5" customWidth="1"/>
-    <col min="12" max="12" width="10.125" customWidth="1"/>
-    <col min="15" max="15" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="7" width="5.6640625" customWidth="1"/>
+    <col min="8" max="9" width="5.44140625" customWidth="1"/>
+    <col min="10" max="10" width="10.109375" customWidth="1"/>
+    <col min="11" max="11" width="8.44140625" customWidth="1"/>
+    <col min="12" max="12" width="10.109375" customWidth="1"/>
+    <col min="15" max="15" width="9.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="79.5" customHeight="1">
@@ -3775,13 +3775,13 @@
       <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="3" max="5" width="5.5" customWidth="1"/>
-    <col min="6" max="7" width="6.5" customWidth="1"/>
-    <col min="8" max="9" width="5.125" customWidth="1"/>
-    <col min="10" max="12" width="8.625" customWidth="1"/>
-    <col min="15" max="15" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="5.44140625" customWidth="1"/>
+    <col min="6" max="7" width="6.44140625" customWidth="1"/>
+    <col min="8" max="9" width="5.109375" customWidth="1"/>
+    <col min="10" max="12" width="8.6640625" customWidth="1"/>
+    <col min="15" max="15" width="9.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="42.75" customHeight="1">
@@ -5074,13 +5074,13 @@
       <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="7" width="6.5" customWidth="1"/>
-    <col min="8" max="10" width="5.375" customWidth="1"/>
-    <col min="11" max="12" width="9.5" customWidth="1"/>
-    <col min="15" max="15" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="7" width="6.44140625" customWidth="1"/>
+    <col min="8" max="10" width="5.33203125" customWidth="1"/>
+    <col min="11" max="12" width="9.44140625" customWidth="1"/>
+    <col min="15" max="15" width="9.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="65.25" customHeight="1">
@@ -6413,12 +6413,12 @@
       <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="3" max="7" width="6.25" customWidth="1"/>
-    <col min="8" max="10" width="4.75" customWidth="1"/>
-    <col min="11" max="12" width="5.875" customWidth="1"/>
-    <col min="16" max="16" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="7" width="6.21875" customWidth="1"/>
+    <col min="8" max="10" width="4.77734375" customWidth="1"/>
+    <col min="11" max="12" width="5.88671875" customWidth="1"/>
+    <col min="16" max="16" width="9.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="64.5" customHeight="1">

</xml_diff>

<commit_message>
Update the EnergyGenerator system
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Equip.xlsx
+++ b/ConfigData/Xlsx/Equip.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="36" windowWidth="18132" windowHeight="8388"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="头盔" sheetId="3" r:id="rId1"/>
@@ -274,7 +274,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="216">
   <si>
     <t>wuqi01</t>
   </si>
@@ -949,43 +949,7 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>60;20;20</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>60;20;20</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>60;15;25</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>60;25;15</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>55;20;25</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>50;10;40</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>50;15;35</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>55;10;35</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>55;10;35</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>50;20;30</t>
+    <t>15;0;-15</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -3208,19 +3172,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="7" width="5.6640625" customWidth="1"/>
-    <col min="8" max="9" width="5.44140625" customWidth="1"/>
-    <col min="10" max="10" width="10.109375" customWidth="1"/>
-    <col min="11" max="11" width="8.44140625" customWidth="1"/>
-    <col min="12" max="12" width="10.109375" customWidth="1"/>
-    <col min="15" max="15" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="7" width="5.625" customWidth="1"/>
+    <col min="8" max="9" width="5.5" customWidth="1"/>
+    <col min="10" max="10" width="10.125" customWidth="1"/>
+    <col min="11" max="11" width="6.375" customWidth="1"/>
+    <col min="12" max="12" width="10.125" customWidth="1"/>
+    <col min="15" max="15" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="79.5" customHeight="1">
@@ -3378,7 +3342,7 @@
         <v>11000001</v>
       </c>
       <c r="K4" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="L4">
         <v>31000001</v>
@@ -3419,7 +3383,7 @@
         <v>11000002</v>
       </c>
       <c r="K5" t="s">
-        <v>216</v>
+        <v>203</v>
       </c>
       <c r="L5">
         <v>31000002</v>
@@ -3460,7 +3424,7 @@
         <v>11000003</v>
       </c>
       <c r="K6" t="s">
-        <v>217</v>
+        <v>203</v>
       </c>
       <c r="L6">
         <v>31000003</v>
@@ -3501,7 +3465,7 @@
         <v>11000004</v>
       </c>
       <c r="K7" t="s">
-        <v>218</v>
+        <v>203</v>
       </c>
       <c r="L7">
         <v>31000004</v>
@@ -3542,7 +3506,7 @@
         <v>11000005</v>
       </c>
       <c r="K8" t="s">
-        <v>219</v>
+        <v>203</v>
       </c>
       <c r="L8">
         <v>31000005</v>
@@ -3583,7 +3547,7 @@
         <v>11000006</v>
       </c>
       <c r="K9" t="s">
-        <v>220</v>
+        <v>203</v>
       </c>
       <c r="L9">
         <v>31000006</v>
@@ -3624,7 +3588,7 @@
         <v>11000007</v>
       </c>
       <c r="K10" t="s">
-        <v>221</v>
+        <v>203</v>
       </c>
       <c r="L10">
         <v>31000007</v>
@@ -3665,7 +3629,7 @@
         <v>11000008</v>
       </c>
       <c r="K11" t="s">
-        <v>222</v>
+        <v>203</v>
       </c>
       <c r="L11">
         <v>31000008</v>
@@ -3706,7 +3670,7 @@
         <v>11000009</v>
       </c>
       <c r="K12" t="s">
-        <v>223</v>
+        <v>203</v>
       </c>
       <c r="L12">
         <v>31000009</v>
@@ -3747,7 +3711,7 @@
         <v>11000010</v>
       </c>
       <c r="K13" t="s">
-        <v>224</v>
+        <v>203</v>
       </c>
       <c r="L13">
         <v>31000010</v>
@@ -3775,13 +3739,13 @@
       <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="3" max="5" width="5.44140625" customWidth="1"/>
-    <col min="6" max="7" width="6.44140625" customWidth="1"/>
-    <col min="8" max="9" width="5.109375" customWidth="1"/>
-    <col min="10" max="12" width="8.6640625" customWidth="1"/>
-    <col min="15" max="15" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="5.5" customWidth="1"/>
+    <col min="6" max="7" width="6.5" customWidth="1"/>
+    <col min="8" max="9" width="5.125" customWidth="1"/>
+    <col min="10" max="12" width="8.625" customWidth="1"/>
+    <col min="15" max="15" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="42.75" customHeight="1">
@@ -5074,13 +5038,13 @@
       <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="7" width="6.44140625" customWidth="1"/>
-    <col min="8" max="10" width="5.33203125" customWidth="1"/>
-    <col min="11" max="12" width="9.44140625" customWidth="1"/>
-    <col min="15" max="15" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="7" width="6.5" customWidth="1"/>
+    <col min="8" max="10" width="5.375" customWidth="1"/>
+    <col min="11" max="12" width="9.5" customWidth="1"/>
+    <col min="15" max="15" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="65.25" customHeight="1">
@@ -6409,16 +6373,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="3" max="7" width="6.21875" customWidth="1"/>
-    <col min="8" max="10" width="4.77734375" customWidth="1"/>
-    <col min="11" max="12" width="5.88671875" customWidth="1"/>
-    <col min="16" max="16" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="7" width="6.25" customWidth="1"/>
+    <col min="8" max="9" width="4.75" customWidth="1"/>
+    <col min="10" max="10" width="5.875" customWidth="1"/>
+    <col min="11" max="11" width="9.125" customWidth="1"/>
+    <col min="12" max="12" width="5.875" customWidth="1"/>
+    <col min="16" max="16" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="64.5" customHeight="1">
@@ -6658,7 +6624,7 @@
         <v>0</v>
       </c>
       <c r="K6" t="s">
-        <v>202</v>
+        <v>215</v>
       </c>
       <c r="L6">
         <v>0</v>

</xml_diff>

<commit_message>
add equip image and some data
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Equip.xlsx
+++ b/ConfigData/Xlsx/Equip.xlsx
@@ -31,7 +31,7 @@
     <author>Administrator</author>
   </authors>
   <commentList>
-    <comment ref="R1" authorId="0" shapeId="0">
+    <comment ref="S1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -62,22 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="82">
-  <si>
-    <t>wuqi01</t>
-  </si>
-  <si>
-    <t>学徒袍</t>
-  </si>
-  <si>
-    <t>hujia01</t>
-  </si>
-  <si>
-    <t>金戒指</t>
-  </si>
-  <si>
-    <t>jiezhi01</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="97">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -143,10 +128,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>木棍</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>0;0;0</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -360,14 +341,95 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>1;3;6</t>
+    <t>草屋</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
     <t>zhulou1</t>
-  </si>
-  <si>
-    <t>草屋</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>qizhi1</t>
+  </si>
+  <si>
+    <t>蓝色旗帜</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>wuqi1</t>
+  </si>
+  <si>
+    <t>弓箭</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>0;0;0</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>qiang1</t>
+  </si>
+  <si>
+    <t>石墙</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>瞭望台</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>jianzhu1</t>
+  </si>
+  <si>
+    <t>7;9</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>怪物攻击加成</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>MonsterAtk</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>怪物生命加成</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>MonsterHp</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>EquipMonsterPickDelegate</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>怪物选取</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>PickMethod</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>m.IsRace("Human")</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>描述</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Des</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -586,7 +648,7 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="47">
+  <fills count="46">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -798,12 +860,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1133,7 +1189,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1173,82 +1229,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="39" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="39" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="39" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="39" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="38" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="39" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="20" fillId="38" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="41" borderId="0" xfId="0" applyFill="1">
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="42" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="41" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="42" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="20" fillId="41" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="43" borderId="0" xfId="0" applyFill="1">
+    <xf numFmtId="0" fontId="0" fillId="42" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="44" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="43" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="45" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="20" fillId="44" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="13" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="46" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="39" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="39" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="39" borderId="12" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="39" borderId="13" xfId="0" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="45" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1">
@@ -1302,7 +1313,36 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="26">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -1340,6 +1380,93 @@
           <bgColor theme="1" tint="4.9989318521683403E-2"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -1577,6 +1704,35 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
         <scheme val="minor"/>
       </font>
       <fill>
@@ -2910,7 +3066,6 @@
           <cell r="A162">
             <v>55900028</v>
           </cell>
-          <cell r="Y162"/>
         </row>
         <row r="163">
           <cell r="A163">
@@ -3133,7 +3288,7 @@
             <v>55990001</v>
           </cell>
           <cell r="Y190">
-            <v>15</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="191">
@@ -3141,7 +3296,7 @@
             <v>55990002</v>
           </cell>
           <cell r="Y191">
-            <v>15</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="192">
@@ -3149,7 +3304,7 @@
             <v>55990003</v>
           </cell>
           <cell r="Y192">
-            <v>15</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="193">
@@ -3157,7 +3312,7 @@
             <v>55990004</v>
           </cell>
           <cell r="Y193">
-            <v>15</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="194">
@@ -3165,7 +3320,7 @@
             <v>55990005</v>
           </cell>
           <cell r="Y194">
-            <v>15</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="195">
@@ -3173,7 +3328,7 @@
             <v>55990006</v>
           </cell>
           <cell r="Y195">
-            <v>15</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="196">
@@ -3181,7 +3336,7 @@
             <v>55990011</v>
           </cell>
           <cell r="Y196">
-            <v>15</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="197">
@@ -3189,7 +3344,7 @@
             <v>55990012</v>
           </cell>
           <cell r="Y197">
-            <v>15</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="198">
@@ -3197,7 +3352,7 @@
             <v>55990013</v>
           </cell>
           <cell r="Y198">
-            <v>15</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="199">
@@ -3205,7 +3360,7 @@
             <v>55990014</v>
           </cell>
           <cell r="Y199">
-            <v>15</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="200">
@@ -3213,7 +3368,7 @@
             <v>55990015</v>
           </cell>
           <cell r="Y200">
-            <v>15</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="201">
@@ -3221,7 +3376,7 @@
             <v>55990016</v>
           </cell>
           <cell r="Y201">
-            <v>15</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="202">
@@ -4749,45 +4904,49 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:AB7" totalsRowShown="0">
-  <autoFilter ref="A3:AB7"/>
-  <sortState ref="A4:AB7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:AF8" totalsRowShown="0">
+  <autoFilter ref="A3:AF8"/>
+  <sortState ref="A4:AF7">
     <sortCondition ref="A3:A7"/>
   </sortState>
-  <tableColumns count="28">
+  <tableColumns count="32">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="Name"/>
-    <tableColumn id="3" name="Quality" dataDxfId="20">
-      <calculatedColumnFormula>IF(O4&gt;=23,4,IF(AND(O4&gt;=18,O4&lt;23),3,IF(AND(O4&gt;=13,O4&lt;18),2,IF(AND(O4&gt;=8,O4&lt;13),1,0))))</calculatedColumnFormula>
+    <tableColumn id="32" name="Des" dataDxfId="0"/>
+    <tableColumn id="3" name="Quality" dataDxfId="25">
+      <calculatedColumnFormula>IF(P4&gt;=23,4,IF(AND(P4&gt;=18,P4&lt;23),3,IF(AND(P4&gt;=13,P4&lt;18),2,IF(AND(P4&gt;=8,P4&lt;13),1,0))))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" name="Position"/>
-    <tableColumn id="19" name="Value"/>
+    <tableColumn id="19" name="Value" dataDxfId="24"/>
     <tableColumn id="11" name="AtkR"/>
     <tableColumn id="8" name="VitR"/>
-    <tableColumn id="6" name="Def" dataDxfId="19"/>
-    <tableColumn id="22" name="Mag" dataDxfId="18"/>
-    <tableColumn id="27" name="Spd" dataDxfId="17"/>
-    <tableColumn id="26" name="Hit" dataDxfId="16"/>
-    <tableColumn id="25" name="Dhit" dataDxfId="15"/>
-    <tableColumn id="24" name="Crt" dataDxfId="14"/>
-    <tableColumn id="23" name="Luk" dataDxfId="13"/>
-    <tableColumn id="28" name="Sum" dataDxfId="12">
-      <calculatedColumnFormula>F4+G4+ SUM(H4:N4)*5+U4+V4</calculatedColumnFormula>
+    <tableColumn id="6" name="Def" dataDxfId="23"/>
+    <tableColumn id="22" name="Mag" dataDxfId="22"/>
+    <tableColumn id="27" name="Spd" dataDxfId="21"/>
+    <tableColumn id="26" name="Hit" dataDxfId="20"/>
+    <tableColumn id="25" name="Dhit" dataDxfId="19"/>
+    <tableColumn id="24" name="Crt" dataDxfId="18"/>
+    <tableColumn id="23" name="Luk" dataDxfId="17"/>
+    <tableColumn id="28" name="Sum" dataDxfId="16">
+      <calculatedColumnFormula>G4+H4+ SUM(I4:O4)*5+Y4+Z4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="Range" dataDxfId="11"/>
-    <tableColumn id="4" name="SlotId" dataDxfId="10"/>
-    <tableColumn id="9" name="EnergyRate" dataDxfId="9"/>
+    <tableColumn id="12" name="Range" dataDxfId="15"/>
+    <tableColumn id="4" name="SlotId" dataDxfId="14"/>
+    <tableColumn id="9" name="EnergyRate" dataDxfId="13"/>
     <tableColumn id="7" name="Durable"/>
     <tableColumn id="20" name="HeroSkillId"/>
+    <tableColumn id="29" name="MonsterAtk" dataDxfId="8"/>
+    <tableColumn id="30" name="MonsterHp" dataDxfId="7"/>
+    <tableColumn id="31" name="PickMethod" dataDxfId="6"/>
     <tableColumn id="21" name="~SkillMark2"/>
-    <tableColumn id="18" name="~SkillMark22" dataDxfId="8">
-      <calculatedColumnFormula>IF(ISBLANK(W4),0, LOOKUP(W4,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*X4/100)</calculatedColumnFormula>
+    <tableColumn id="18" name="~SkillMark22" dataDxfId="12">
+      <calculatedColumnFormula>IF(ISBLANK(AA4),0, LOOKUP(AA4,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AB4/100)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="13" name="CommonSkillId"/>
     <tableColumn id="14" name="CommonSkillRate"/>
-    <tableColumn id="15" name="Disable" dataDxfId="7"/>
-    <tableColumn id="17" name="RandomDrop" dataDxfId="6"/>
-    <tableColumn id="16" name="CanMerge" dataDxfId="5"/>
+    <tableColumn id="15" name="Disable" dataDxfId="11"/>
+    <tableColumn id="17" name="RandomDrop" dataDxfId="10"/>
+    <tableColumn id="16" name="CanMerge" dataDxfId="9"/>
     <tableColumn id="10" name="Url"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -5115,603 +5274,744 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB7"/>
+  <dimension ref="A1:AF8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S4" sqref="S4"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="5.5" customWidth="1"/>
-    <col min="5" max="5" width="6.5" customWidth="1"/>
-    <col min="6" max="7" width="5.125" customWidth="1"/>
-    <col min="8" max="15" width="4.5" customWidth="1"/>
-    <col min="16" max="16" width="5.125" customWidth="1"/>
-    <col min="17" max="17" width="16.875" customWidth="1"/>
-    <col min="18" max="18" width="8.625" customWidth="1"/>
-    <col min="19" max="19" width="5" customWidth="1"/>
-    <col min="20" max="21" width="8.625" customWidth="1"/>
-    <col min="22" max="22" width="5.875" customWidth="1"/>
-    <col min="23" max="23" width="8.625" customWidth="1"/>
-    <col min="24" max="24" width="5.25" customWidth="1"/>
-    <col min="25" max="27" width="6" customWidth="1"/>
-    <col min="30" max="30" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.75" customWidth="1"/>
+    <col min="4" max="5" width="5.5" customWidth="1"/>
+    <col min="6" max="6" width="6.5" customWidth="1"/>
+    <col min="7" max="8" width="5.125" customWidth="1"/>
+    <col min="9" max="16" width="4.5" customWidth="1"/>
+    <col min="17" max="17" width="5.125" customWidth="1"/>
+    <col min="18" max="18" width="16.875" customWidth="1"/>
+    <col min="19" max="19" width="8.625" customWidth="1"/>
+    <col min="20" max="20" width="5" customWidth="1"/>
+    <col min="21" max="21" width="8.625" customWidth="1"/>
+    <col min="22" max="23" width="4.875" customWidth="1"/>
+    <col min="24" max="24" width="16.375" customWidth="1"/>
+    <col min="25" max="25" width="8.625" customWidth="1"/>
+    <col min="26" max="26" width="5.875" customWidth="1"/>
+    <col min="27" max="27" width="8.625" customWidth="1"/>
+    <col min="28" max="28" width="5.25" customWidth="1"/>
+    <col min="29" max="31" width="6" customWidth="1"/>
+    <col min="34" max="34" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="60.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:32" ht="60.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="J1" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="K1" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="L1" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="M1" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="N1" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="O1" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="P1" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q1" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="R1" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="S1" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="T1" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="U1" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="V1" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="W1" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="X1" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="Y1" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z1" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA1" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB1" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC1" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="AD1" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="AE1" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="8" t="s">
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.15">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="K2" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="L2" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="M2" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="N2" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="O2" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="P2" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q2" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="R2" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="S2" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="T2" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="U2" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="V2" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="W2" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="X2" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="Y2" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z2" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA2" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="AB2" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="AE2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="AF2" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="B3" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="C3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D3" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E3" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="J3" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="K3" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="L3" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="M3" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="N3" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="O3" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="P3" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q3" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="R3" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="S3" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="T3" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="H1" s="28" t="s">
-        <v>59</v>
-      </c>
-      <c r="I1" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="J1" s="28" t="s">
-        <v>61</v>
-      </c>
-      <c r="K1" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="L1" s="28" t="s">
-        <v>63</v>
-      </c>
-      <c r="M1" s="28" t="s">
-        <v>64</v>
-      </c>
-      <c r="N1" s="28" t="s">
-        <v>65</v>
-      </c>
-      <c r="O1" s="22" t="s">
+      <c r="U3" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="V3" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="W3" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="X3" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="Y3" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z3" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA3" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB3" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.15">
+      <c r="A4" s="1">
+        <v>21100001</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="P1" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q1" s="25" t="s">
+      <c r="C4" s="1"/>
+      <c r="D4" s="1">
+        <f>IF(P4&gt;=23,4,IF(AND(P4&gt;=18,P4&lt;23),3,IF(AND(P4&gt;=13,P4&lt;18),2,IF(AND(P4&gt;=8,P4&lt;13),1,0))))</f>
+        <v>0</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0</v>
+      </c>
+      <c r="H4" s="1">
+        <v>5</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0</v>
+      </c>
+      <c r="L4" s="1">
+        <v>0</v>
+      </c>
+      <c r="M4" s="1">
+        <v>0</v>
+      </c>
+      <c r="N4" s="1">
+        <v>0</v>
+      </c>
+      <c r="O4" s="1">
+        <v>0</v>
+      </c>
+      <c r="P4" s="1">
+        <f t="shared" ref="P4:P5" si="0">G4+H4+ SUM(I4:O4)*5+Y4+Z4</f>
+        <v>5</v>
+      </c>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T4" s="1">
+        <v>10</v>
+      </c>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
+      <c r="W4" s="1"/>
+      <c r="X4" s="1"/>
+      <c r="Y4" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="1">
+        <f>IF(ISBLANK(AA4),0, LOOKUP(AA4,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AB4/100)</f>
+        <v>0</v>
+      </c>
+      <c r="AA4" s="1"/>
+      <c r="AB4" s="1"/>
+      <c r="AC4" s="1"/>
+      <c r="AD4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AE4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF4" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.15">
+      <c r="A5" s="1">
+        <v>21200001</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="R1" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="S1" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="T1" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="U1" s="25" t="s">
-        <v>50</v>
-      </c>
-      <c r="V1" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="W1" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="X1" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="Y1" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="Z1" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="AA1" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="AB1" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.15">
-      <c r="A2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H2" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="I2" s="29" t="s">
-        <v>66</v>
-      </c>
-      <c r="J2" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="K2" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="L2" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="M2" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="N2" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="O2" s="23" t="s">
-        <v>74</v>
-      </c>
-      <c r="P2" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q2" s="26" t="s">
-        <v>77</v>
-      </c>
-      <c r="R2" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="S2" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="T2" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="U2" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="V2" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="W2" s="23" t="s">
-        <v>58</v>
-      </c>
-      <c r="X2" s="23" t="s">
-        <v>58</v>
-      </c>
-      <c r="Y2" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z2" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="AA2" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="AB2" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.15">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="H3" s="30" t="s">
-        <v>67</v>
-      </c>
-      <c r="I3" s="30" t="s">
-        <v>68</v>
-      </c>
-      <c r="J3" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="K3" s="30" t="s">
-        <v>69</v>
-      </c>
-      <c r="L3" s="30" t="s">
-        <v>70</v>
-      </c>
-      <c r="M3" s="30" t="s">
-        <v>71</v>
-      </c>
-      <c r="N3" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="O3" s="24" t="s">
-        <v>75</v>
-      </c>
-      <c r="P3" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q3" s="27" t="s">
-        <v>78</v>
-      </c>
-      <c r="R3" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="S3" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="T3" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="U3" s="27" t="s">
-        <v>49</v>
-      </c>
-      <c r="V3" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="W3" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="X3" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>46</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>44</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.15">
-      <c r="A4" s="15">
-        <v>21100101</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="C4" s="16">
-        <f>IF(O4&gt;=23,4,IF(AND(O4&gt;=18,O4&lt;23),3,IF(AND(O4&gt;=13,O4&lt;18),2,IF(AND(O4&gt;=8,O4&lt;13),1,0))))</f>
-        <v>0</v>
-      </c>
-      <c r="D4" s="17">
+      <c r="C5" s="1"/>
+      <c r="D5" s="1">
+        <f t="shared" ref="D5:D6" si="1">IF(P5&gt;=23,4,IF(AND(P5&gt;=18,P5&lt;23),3,IF(AND(P5&gt;=13,P5&lt;18),2,IF(AND(P5&gt;=8,P5&lt;13),1,0))))</f>
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
+        <v>2</v>
+      </c>
+      <c r="F5" s="1">
         <v>1</v>
       </c>
-      <c r="E4" s="15">
-        <v>1</v>
-      </c>
-      <c r="F4" s="15">
-        <v>0</v>
-      </c>
-      <c r="G4" s="15">
-        <v>5</v>
-      </c>
-      <c r="H4" s="32">
-        <v>0</v>
-      </c>
-      <c r="I4" s="15">
-        <v>0</v>
-      </c>
-      <c r="J4" s="15">
-        <v>0</v>
-      </c>
-      <c r="K4" s="15">
-        <v>0</v>
-      </c>
-      <c r="L4" s="15">
-        <v>0</v>
-      </c>
-      <c r="M4" s="15">
-        <v>0</v>
-      </c>
-      <c r="N4" s="15">
-        <v>0</v>
-      </c>
-      <c r="O4" s="33">
-        <f t="shared" ref="O4:O5" si="0">F4+G4+ SUM(H4:N4)*5+U4+V4</f>
-        <v>5</v>
-      </c>
-      <c r="P4" s="15"/>
-      <c r="Q4" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="R4" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="S4" s="18">
-        <v>99</v>
-      </c>
-      <c r="T4" s="18"/>
-      <c r="U4" s="18">
-        <v>0</v>
-      </c>
-      <c r="V4" s="18">
-        <f>IF(ISBLANK(W4),0, LOOKUP(W4,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*X4/100)</f>
-        <v>0</v>
-      </c>
-      <c r="W4" s="18"/>
-      <c r="X4" s="18"/>
-      <c r="Y4" s="20"/>
-      <c r="Z4" s="20"/>
-      <c r="AA4" s="20"/>
-      <c r="AB4" s="15" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.15">
-      <c r="A5" s="14">
-        <v>21200101</v>
-      </c>
-      <c r="B5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="31">
-        <f t="shared" ref="C5:C6" si="1">IF(O5&gt;=23,4,IF(AND(O5&gt;=18,O5&lt;23),3,IF(AND(O5&gt;=13,O5&lt;18),2,IF(AND(O5&gt;=8,O5&lt;13),1,0))))</f>
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>2</v>
-      </c>
-      <c r="E5">
-        <v>10</v>
-      </c>
-      <c r="F5">
-        <v>5</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5" s="34">
-        <v>0</v>
-      </c>
-      <c r="I5" s="13">
-        <v>0</v>
-      </c>
-      <c r="J5" s="13">
-        <v>0</v>
-      </c>
-      <c r="K5" s="13">
-        <v>0</v>
-      </c>
-      <c r="L5" s="13">
-        <v>0</v>
-      </c>
-      <c r="M5" s="13">
-        <v>0</v>
-      </c>
-      <c r="N5" s="13">
-        <v>0</v>
-      </c>
-      <c r="O5" s="35">
+      <c r="G5" s="1">
+        <v>0</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0</v>
+      </c>
+      <c r="I5" s="1">
+        <v>0</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0</v>
+      </c>
+      <c r="K5" s="1">
+        <v>0</v>
+      </c>
+      <c r="L5" s="1">
+        <v>0</v>
+      </c>
+      <c r="M5" s="1">
+        <v>0</v>
+      </c>
+      <c r="N5" s="1">
+        <v>0</v>
+      </c>
+      <c r="O5" s="1">
+        <v>0</v>
+      </c>
+      <c r="P5" s="1">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="R5" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="S5">
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T5" s="1">
         <v>10</v>
       </c>
-      <c r="U5">
-        <v>0</v>
-      </c>
-      <c r="V5">
-        <f>IF(ISBLANK(W5),0, LOOKUP(W5,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*X5/100)</f>
-        <v>0</v>
-      </c>
-      <c r="Y5" s="21"/>
-      <c r="Z5" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="AA5" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="AB5" t="s">
-        <v>0</v>
+      <c r="U5" s="1"/>
+      <c r="V5" s="1"/>
+      <c r="W5" s="1">
+        <v>10</v>
+      </c>
+      <c r="X5" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="Y5" s="1">
+        <v>5</v>
+      </c>
+      <c r="Z5" s="1">
+        <f>IF(ISBLANK(AA5),0, LOOKUP(AA5,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AB5/100)</f>
+        <v>0</v>
+      </c>
+      <c r="AA5" s="1"/>
+      <c r="AB5" s="1"/>
+      <c r="AC5" s="1"/>
+      <c r="AD5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AE5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF5" s="1" t="s">
+        <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.15">
-      <c r="A6" s="14">
-        <v>21300101</v>
-      </c>
-      <c r="B6" s="16" t="s">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.15">
+      <c r="A6" s="1">
+        <v>21300001</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>3</v>
+      </c>
+      <c r="F6" s="1">
         <v>1</v>
       </c>
-      <c r="C6" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D6" s="16">
-        <v>3</v>
-      </c>
-      <c r="E6" s="18">
+      <c r="G6" s="1">
+        <v>5</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0</v>
+      </c>
+      <c r="I6" s="1">
+        <v>0</v>
+      </c>
+      <c r="J6" s="1">
+        <v>0</v>
+      </c>
+      <c r="K6" s="1">
+        <v>0</v>
+      </c>
+      <c r="L6" s="1">
+        <v>0</v>
+      </c>
+      <c r="M6" s="1">
+        <v>0</v>
+      </c>
+      <c r="N6" s="1">
+        <v>0</v>
+      </c>
+      <c r="O6" s="1">
+        <v>0</v>
+      </c>
+      <c r="P6" s="1">
+        <f t="shared" ref="P6" si="2">G6+H6+ SUM(I6:O6)*5+Y6+Z6</f>
+        <v>5</v>
+      </c>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T6" s="1">
         <v>10</v>
       </c>
-      <c r="F6" s="18">
-        <v>0</v>
-      </c>
-      <c r="G6" s="18">
+      <c r="U6" s="1"/>
+      <c r="V6" s="1"/>
+      <c r="W6" s="1"/>
+      <c r="X6" s="1"/>
+      <c r="Y6" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="1">
+        <f>IF(ISBLANK(AA6),0, LOOKUP(AA6,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AB6/100)</f>
+        <v>0</v>
+      </c>
+      <c r="AA6" s="1"/>
+      <c r="AB6" s="1"/>
+      <c r="AC6" s="1"/>
+      <c r="AD6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AE6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF6" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.15">
+      <c r="A7">
+        <v>21400001</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="23">
+        <f t="shared" ref="D7" si="3">IF(P7&gt;=23,4,IF(AND(P7&gt;=18,P7&lt;23),3,IF(AND(P7&gt;=13,P7&lt;18),2,IF(AND(P7&gt;=8,P7&lt;13),1,0))))</f>
+        <v>0</v>
+      </c>
+      <c r="E7" s="1">
+        <v>4</v>
+      </c>
+      <c r="F7" s="1">
+        <v>1</v>
+      </c>
+      <c r="G7" s="7">
+        <v>0</v>
+      </c>
+      <c r="H7" s="7">
+        <v>0</v>
+      </c>
+      <c r="I7" s="24">
+        <v>1</v>
+      </c>
+      <c r="J7" s="7">
+        <v>0</v>
+      </c>
+      <c r="K7" s="7">
+        <v>0</v>
+      </c>
+      <c r="L7" s="7">
+        <v>0</v>
+      </c>
+      <c r="M7" s="7">
+        <v>0</v>
+      </c>
+      <c r="N7" s="7">
+        <v>0</v>
+      </c>
+      <c r="O7" s="7">
+        <v>0</v>
+      </c>
+      <c r="P7" s="25">
+        <f t="shared" ref="P7" si="4">G7+H7+ SUM(I7:O7)*5+Y7+Z7</f>
         <v>5</v>
       </c>
-      <c r="H6" s="36">
-        <v>0</v>
-      </c>
-      <c r="I6" s="37">
-        <v>0</v>
-      </c>
-      <c r="J6" s="37">
-        <v>0</v>
-      </c>
-      <c r="K6" s="37">
-        <v>0</v>
-      </c>
-      <c r="L6" s="37">
-        <v>0</v>
-      </c>
-      <c r="M6" s="37">
-        <v>0</v>
-      </c>
-      <c r="N6" s="37">
-        <v>0</v>
-      </c>
-      <c r="O6" s="38">
-        <f t="shared" ref="O6" si="2">F6+G6+ SUM(H6:N6)*5+U6+V6</f>
+      <c r="Q7" s="7"/>
+      <c r="R7" s="7"/>
+      <c r="S7" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="T7">
+        <v>10</v>
+      </c>
+      <c r="Y7">
+        <v>0</v>
+      </c>
+      <c r="Z7">
+        <f>IF(ISBLANK(AA7),0, LOOKUP(AA7,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AB7/100)</f>
+        <v>0</v>
+      </c>
+      <c r="AC7" s="13"/>
+      <c r="AD7" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="AE7" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF7" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.15">
+      <c r="A8">
+        <v>21500001</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="23">
+        <f t="shared" ref="D8" si="5">IF(P8&gt;=23,4,IF(AND(P8&gt;=18,P8&lt;23),3,IF(AND(P8&gt;=13,P8&lt;18),2,IF(AND(P8&gt;=8,P8&lt;13),1,0))))</f>
+        <v>0</v>
+      </c>
+      <c r="E8" s="1">
         <v>5</v>
       </c>
-      <c r="P6" s="18"/>
-      <c r="Q6" s="18"/>
-      <c r="R6" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="S6" s="18">
+      <c r="F8" s="1">
+        <v>1</v>
+      </c>
+      <c r="G8" s="7">
+        <v>0</v>
+      </c>
+      <c r="H8" s="7">
+        <v>0</v>
+      </c>
+      <c r="I8" s="24">
+        <v>0</v>
+      </c>
+      <c r="J8" s="7">
+        <v>0</v>
+      </c>
+      <c r="K8" s="7">
+        <v>0</v>
+      </c>
+      <c r="L8" s="7">
+        <v>1</v>
+      </c>
+      <c r="M8" s="7">
+        <v>0</v>
+      </c>
+      <c r="N8" s="7">
+        <v>0</v>
+      </c>
+      <c r="O8" s="7">
+        <v>0</v>
+      </c>
+      <c r="P8" s="25">
+        <f t="shared" ref="P8" si="6">G8+H8+ SUM(I8:O8)*5+Y8+Z8</f>
+        <v>5</v>
+      </c>
+      <c r="Q8" s="7"/>
+      <c r="R8" s="7"/>
+      <c r="S8" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="T8">
         <v>10</v>
       </c>
-      <c r="T6" s="18"/>
-      <c r="U6" s="18">
-        <v>0</v>
-      </c>
-      <c r="V6" s="18">
-        <f>IF(ISBLANK(W6),0, LOOKUP(W6,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*X6/100)</f>
-        <v>0</v>
-      </c>
-      <c r="W6" s="18"/>
-      <c r="X6" s="18"/>
-      <c r="Y6" s="20"/>
-      <c r="Z6" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="AA6" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="AB6" s="19" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.15">
-      <c r="A7">
-        <v>21400101</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="31">
-        <f t="shared" ref="C7" si="3">IF(O7&gt;=23,4,IF(AND(O7&gt;=18,O7&lt;23),3,IF(AND(O7&gt;=13,O7&lt;18),2,IF(AND(O7&gt;=8,O7&lt;13),1,0))))</f>
-        <v>0</v>
-      </c>
-      <c r="D7" s="1">
-        <v>4</v>
-      </c>
-      <c r="E7">
-        <v>10</v>
-      </c>
-      <c r="F7" s="7">
-        <v>0</v>
-      </c>
-      <c r="G7" s="7">
-        <v>0</v>
-      </c>
-      <c r="H7" s="39">
-        <v>0</v>
-      </c>
-      <c r="I7" s="7">
-        <v>0</v>
-      </c>
-      <c r="J7" s="7">
-        <v>0</v>
-      </c>
-      <c r="K7" s="7">
-        <v>0</v>
-      </c>
-      <c r="L7" s="7">
-        <v>0</v>
-      </c>
-      <c r="M7" s="7">
-        <v>0</v>
-      </c>
-      <c r="N7" s="7">
-        <v>0</v>
-      </c>
-      <c r="O7" s="40">
-        <f t="shared" ref="O7" si="4">F7+G7+ SUM(H7:N7)*5+U7+V7</f>
-        <v>0</v>
-      </c>
-      <c r="P7" s="7"/>
-      <c r="Q7" s="7"/>
-      <c r="R7" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="S7">
-        <v>10</v>
-      </c>
-      <c r="U7">
-        <v>0</v>
-      </c>
-      <c r="V7">
-        <f>IF(ISBLANK(W7),0, LOOKUP(W7,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*X7/100)</f>
-        <v>0</v>
-      </c>
-      <c r="Y7" s="21"/>
-      <c r="Z7" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="AA7" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="AB7" s="2" t="s">
-        <v>4</v>
+      <c r="Y8">
+        <v>0</v>
+      </c>
+      <c r="Z8">
+        <f>IF(ISBLANK(AA8),0, LOOKUP(AA8,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AB8/100)</f>
+        <v>0</v>
+      </c>
+      <c r="AC8" s="13"/>
+      <c r="AD8" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="AE8" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF8" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="C4:C7">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="greaterThanOrEqual">
+  <conditionalFormatting sqref="D7:D8">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThanOrEqual">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5743,15 +6043,15 @@
   <sheetData>
     <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" s="11" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" s="11" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -5766,7 +6066,7 @@
         <v>3</v>
       </c>
       <c r="F4" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.15">
@@ -5865,7 +6165,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A10" s="12" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B10" s="10">
         <v>36</v>

</xml_diff>

<commit_message>
add the equip show effect during battle
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Equip.xlsx
+++ b/ConfigData/Xlsx/Equip.xlsx
@@ -20,7 +20,7 @@
   </externalReferences>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="5" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -31,7 +31,7 @@
     <author>Administrator</author>
   </authors>
   <commentList>
-    <comment ref="S1" authorId="0" shapeId="0">
+    <comment ref="T1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="204">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -780,6 +780,42 @@
   </si>
   <si>
     <t>3;6;9</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>箭矢</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Arrow</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>arrow</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>arrowred</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>bullet</t>
+  </si>
+  <si>
+    <t>spear</t>
+  </si>
+  <si>
+    <t>bluepea</t>
+  </si>
+  <si>
+    <t>electball</t>
+  </si>
+  <si>
+    <t>laser</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1682,7 +1718,26 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="26">
+  <dxfs count="27">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -1720,6 +1775,144 @@
           <bgColor theme="1" tint="4.9989318521683403E-2"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -1936,10 +2129,14 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
         <scheme val="minor"/>
       </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -1980,148 +2177,6 @@
         <horizontal/>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -3436,6 +3491,7 @@
           <cell r="A162">
             <v>55900028</v>
           </cell>
+          <cell r="Y162"/>
         </row>
         <row r="163">
           <cell r="A163">
@@ -4154,7 +4210,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="数据透视表1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="值" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="数据透视表1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="值" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:D5" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="32">
     <pivotField dataField="1" showAll="0"/>
@@ -4231,15 +4287,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:AF46" totalsRowShown="0">
-  <autoFilter ref="A3:AF46"/>
-  <sortState ref="A4:AF28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:AG46" totalsRowShown="0">
+  <autoFilter ref="A3:AG46"/>
+  <sortState ref="A4:AG28">
     <sortCondition ref="A3:A28"/>
   </sortState>
-  <tableColumns count="32">
+  <tableColumns count="33">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="Name"/>
-    <tableColumn id="32" name="Des" dataDxfId="13"/>
+    <tableColumn id="32" name="Des" dataDxfId="26"/>
     <tableColumn id="3" name="Quality" dataDxfId="25">
       <calculatedColumnFormula>IF(P4&gt;=23,4,IF(AND(P4&gt;=18,P4&lt;23),3,IF(AND(P4&gt;=13,P4&lt;18),2,IF(AND(P4&gt;=8,P4&lt;13),1,0))))</calculatedColumnFormula>
     </tableColumn>
@@ -4249,33 +4305,34 @@
     </tableColumn>
     <tableColumn id="11" name="AtkR"/>
     <tableColumn id="8" name="VitR"/>
-    <tableColumn id="6" name="Def" dataDxfId="12"/>
-    <tableColumn id="22" name="Mag" dataDxfId="11"/>
-    <tableColumn id="27" name="Spd" dataDxfId="10"/>
-    <tableColumn id="26" name="Hit" dataDxfId="9"/>
-    <tableColumn id="25" name="Dhit" dataDxfId="8"/>
-    <tableColumn id="24" name="Crt" dataDxfId="7"/>
-    <tableColumn id="23" name="Luk" dataDxfId="6"/>
-    <tableColumn id="28" name="Sum" dataDxfId="5">
-      <calculatedColumnFormula>G4+H4+ SUM(I4:O4)*5+Y4+Z4</calculatedColumnFormula>
+    <tableColumn id="6" name="Def" dataDxfId="23"/>
+    <tableColumn id="22" name="Mag" dataDxfId="22"/>
+    <tableColumn id="27" name="Spd" dataDxfId="21"/>
+    <tableColumn id="26" name="Hit" dataDxfId="20"/>
+    <tableColumn id="25" name="Dhit" dataDxfId="19"/>
+    <tableColumn id="24" name="Crt" dataDxfId="18"/>
+    <tableColumn id="23" name="Luk" dataDxfId="17"/>
+    <tableColumn id="28" name="Sum" dataDxfId="16">
+      <calculatedColumnFormula>G4+H4+ SUM(I4:O4)*5+Z4+AA4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="Range" dataDxfId="23"/>
-    <tableColumn id="4" name="SlotId" dataDxfId="22"/>
-    <tableColumn id="9" name="EnergyRate" dataDxfId="21"/>
+    <tableColumn id="12" name="Range" dataDxfId="15"/>
+    <tableColumn id="33" name="Arrow" dataDxfId="0"/>
+    <tableColumn id="4" name="SlotId" dataDxfId="14"/>
+    <tableColumn id="9" name="EnergyRate" dataDxfId="13"/>
     <tableColumn id="7" name="Durable"/>
     <tableColumn id="20" name="HeroSkillId"/>
-    <tableColumn id="29" name="MonsterAtk" dataDxfId="16"/>
-    <tableColumn id="30" name="MonsterHp" dataDxfId="15"/>
-    <tableColumn id="31" name="PickMethod" dataDxfId="14"/>
+    <tableColumn id="29" name="MonsterAtk" dataDxfId="12"/>
+    <tableColumn id="30" name="MonsterHp" dataDxfId="11"/>
+    <tableColumn id="31" name="PickMethod" dataDxfId="10"/>
     <tableColumn id="21" name="~SkillMark2"/>
-    <tableColumn id="18" name="~SkillMark22" dataDxfId="20">
-      <calculatedColumnFormula>IF(ISBLANK(AA4),0, LOOKUP(AA4,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AB4/100)</calculatedColumnFormula>
+    <tableColumn id="18" name="~SkillMark22" dataDxfId="9">
+      <calculatedColumnFormula>IF(ISBLANK(AB4),0, LOOKUP(AB4,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC4/100)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="13" name="CommonSkillId"/>
     <tableColumn id="14" name="CommonSkillRate"/>
-    <tableColumn id="15" name="Disable" dataDxfId="19"/>
-    <tableColumn id="17" name="RandomDrop" dataDxfId="18"/>
-    <tableColumn id="16" name="CanMerge" dataDxfId="17"/>
+    <tableColumn id="15" name="Disable" dataDxfId="8"/>
+    <tableColumn id="17" name="RandomDrop" dataDxfId="7"/>
+    <tableColumn id="16" name="CanMerge" dataDxfId="6"/>
     <tableColumn id="10" name="Url"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -4603,10 +4660,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF46"/>
+  <dimension ref="A1:AG46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="R15" sqref="R15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -4617,22 +4674,22 @@
     <col min="6" max="6" width="6.5" customWidth="1"/>
     <col min="7" max="8" width="5.125" customWidth="1"/>
     <col min="9" max="16" width="4.5" customWidth="1"/>
-    <col min="17" max="17" width="5.125" customWidth="1"/>
-    <col min="18" max="18" width="16.875" customWidth="1"/>
-    <col min="19" max="19" width="8.625" customWidth="1"/>
-    <col min="20" max="20" width="5" customWidth="1"/>
-    <col min="21" max="21" width="8.625" customWidth="1"/>
-    <col min="22" max="23" width="4.875" customWidth="1"/>
-    <col min="24" max="24" width="16.375" customWidth="1"/>
-    <col min="25" max="25" width="8.625" customWidth="1"/>
-    <col min="26" max="26" width="5.875" customWidth="1"/>
-    <col min="27" max="27" width="8.625" customWidth="1"/>
-    <col min="28" max="28" width="5.25" customWidth="1"/>
-    <col min="29" max="31" width="6" customWidth="1"/>
-    <col min="34" max="34" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="5.125" customWidth="1"/>
+    <col min="19" max="19" width="16.875" customWidth="1"/>
+    <col min="20" max="20" width="8.625" customWidth="1"/>
+    <col min="21" max="21" width="5" customWidth="1"/>
+    <col min="22" max="22" width="8.625" customWidth="1"/>
+    <col min="23" max="24" width="4.875" customWidth="1"/>
+    <col min="25" max="25" width="16.375" customWidth="1"/>
+    <col min="26" max="26" width="8.625" customWidth="1"/>
+    <col min="27" max="27" width="5.875" customWidth="1"/>
+    <col min="28" max="28" width="8.625" customWidth="1"/>
+    <col min="29" max="29" width="5.25" customWidth="1"/>
+    <col min="30" max="32" width="6" customWidth="1"/>
+    <col min="35" max="35" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" ht="60.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:33" ht="60.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="8" t="s">
         <v>2</v>
       </c>
@@ -4685,52 +4742,55 @@
         <v>45</v>
       </c>
       <c r="R1" s="16" t="s">
+        <v>194</v>
+      </c>
+      <c r="S1" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="S1" s="16" t="s">
+      <c r="T1" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="T1" s="16" t="s">
+      <c r="U1" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="U1" s="16" t="s">
+      <c r="V1" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="V1" s="16" t="s">
+      <c r="W1" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="W1" s="16" t="s">
+      <c r="X1" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="X1" s="16" t="s">
+      <c r="Y1" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="Y1" s="16" t="s">
+      <c r="Z1" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="Z1" s="13" t="s">
+      <c r="AA1" s="13" t="s">
         <v>40</v>
-      </c>
-      <c r="AA1" s="13" t="s">
-        <v>50</v>
       </c>
       <c r="AB1" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="AC1" s="8" t="s">
+      <c r="AC1" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="AD1" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="AD1" s="8" t="s">
+      <c r="AE1" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="AE1" s="8" t="s">
+      <c r="AF1" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="AF1" s="8" t="s">
+      <c r="AG1" s="8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -4783,52 +4843,55 @@
         <v>0</v>
       </c>
       <c r="R2" s="17" t="s">
+        <v>195</v>
+      </c>
+      <c r="S2" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="S2" s="17" t="s">
+      <c r="T2" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="T2" s="17" t="s">
-        <v>0</v>
-      </c>
       <c r="U2" s="17" t="s">
         <v>0</v>
       </c>
       <c r="V2" s="17" t="s">
-        <v>84</v>
+        <v>0</v>
       </c>
       <c r="W2" s="17" t="s">
         <v>84</v>
       </c>
       <c r="X2" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="Y2" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="Y2" s="17" t="s">
+      <c r="Z2" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="Z2" s="14" t="s">
+      <c r="AA2" s="14" t="s">
         <v>41</v>
-      </c>
-      <c r="AA2" s="14" t="s">
-        <v>51</v>
       </c>
       <c r="AB2" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="AC2" s="3" t="s">
+      <c r="AC2" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="AD2" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="AD2" s="3" t="s">
-        <v>36</v>
       </c>
       <c r="AE2" s="3" t="s">
         <v>36</v>
       </c>
       <c r="AF2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG2" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -4881,52 +4944,55 @@
         <v>26</v>
       </c>
       <c r="R3" s="18" t="s">
+        <v>196</v>
+      </c>
+      <c r="S3" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="S3" s="18" t="s">
+      <c r="T3" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="T3" s="18" t="s">
+      <c r="U3" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="U3" s="18" t="s">
+      <c r="V3" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="V3" s="18" t="s">
+      <c r="W3" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="W3" s="18" t="s">
+      <c r="X3" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="X3" s="18" t="s">
+      <c r="Y3" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="Y3" s="18" t="s">
+      <c r="Z3" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="Z3" s="15" t="s">
+      <c r="AA3" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="AA3" s="15" t="s">
+      <c r="AB3" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="AB3" s="15" t="s">
+      <c r="AC3" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="AC3" t="s">
+      <c r="AD3" t="s">
         <v>33</v>
       </c>
-      <c r="AD3" t="s">
+      <c r="AE3" t="s">
         <v>39</v>
       </c>
-      <c r="AE3" t="s">
+      <c r="AF3" t="s">
         <v>37</v>
       </c>
-      <c r="AF3" t="s">
+      <c r="AG3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A4" s="1">
         <v>21100001</v>
       </c>
@@ -4935,7 +5001,7 @@
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1">
-        <f>IF(P4&gt;=23,4,IF(AND(P4&gt;=18,P4&lt;23),3,IF(AND(P4&gt;=13,P4&lt;18),2,IF(AND(P4&gt;=8,P4&lt;13),1,0))))</f>
+        <f t="shared" ref="D4:D14" si="0">IF(P4&gt;=23,4,IF(AND(P4&gt;=18,P4&lt;23),3,IF(AND(P4&gt;=13,P4&lt;18),2,IF(AND(P4&gt;=8,P4&lt;13),1,0))))</f>
         <v>0</v>
       </c>
       <c r="E4" s="1">
@@ -4973,44 +5039,45 @@
         <v>0</v>
       </c>
       <c r="P4" s="24">
-        <f t="shared" ref="P4:P15" si="0">G4+H4+ SUM(I4:O4)*5+Y4+Z4</f>
+        <f t="shared" ref="P4:P15" si="1">G4+H4+ SUM(I4:O4)*5+Z4+AA4</f>
         <v>-5</v>
       </c>
       <c r="Q4" s="1"/>
-      <c r="R4" s="1" t="s">
+      <c r="R4" s="1"/>
+      <c r="S4" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="S4" s="1" t="s">
+      <c r="T4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T4" s="1">
+      <c r="U4" s="1">
         <v>10</v>
       </c>
-      <c r="U4" s="1"/>
       <c r="V4" s="1"/>
       <c r="W4" s="1"/>
       <c r="X4" s="1"/>
-      <c r="Y4" s="1">
+      <c r="Y4" s="1"/>
+      <c r="Z4" s="1">
         <v>-10</v>
       </c>
-      <c r="Z4" s="1">
-        <f>IF(ISBLANK(AA4),0, LOOKUP(AA4,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AB4/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AA4" s="1"/>
+      <c r="AA4" s="1">
+        <f>IF(ISBLANK(AB4),0, LOOKUP(AB4,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC4/100)</f>
+        <v>0</v>
+      </c>
       <c r="AB4" s="1"/>
       <c r="AC4" s="1"/>
-      <c r="AD4" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="AD4" s="1"/>
       <c r="AE4" s="1" t="s">
         <v>34</v>
       </c>
       <c r="AF4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG4" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A5" s="1">
         <v>21100002</v>
       </c>
@@ -5019,14 +5086,14 @@
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1">
-        <f>IF(P5&gt;=23,4,IF(AND(P5&gt;=18,P5&lt;23),3,IF(AND(P5&gt;=13,P5&lt;18),2,IF(AND(P5&gt;=8,P5&lt;13),1,0))))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E5" s="1">
         <v>1</v>
       </c>
       <c r="F5" s="1">
-        <f t="shared" ref="F5:F44" si="1">D5*50+50</f>
+        <f t="shared" ref="F5:F44" si="2">D5*50+50</f>
         <v>100</v>
       </c>
       <c r="G5" s="1">
@@ -5057,44 +5124,45 @@
         <v>0</v>
       </c>
       <c r="P5" s="24">
-        <f>G5+H5+ SUM(I5:O5)*5+Y5+Z5</f>
+        <f t="shared" ref="P5:P14" si="3">G5+H5+ SUM(I5:O5)*5+Z5+AA5</f>
         <v>10</v>
       </c>
       <c r="Q5" s="25"/>
-      <c r="R5" s="25" t="s">
+      <c r="R5" s="25"/>
+      <c r="S5" s="25" t="s">
         <v>97</v>
       </c>
-      <c r="S5" s="1" t="s">
+      <c r="T5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T5" s="1">
+      <c r="U5" s="1">
         <v>10</v>
       </c>
-      <c r="U5" s="1"/>
       <c r="V5" s="1"/>
       <c r="W5" s="1"/>
       <c r="X5" s="1"/>
-      <c r="Y5" s="1">
-        <v>0</v>
-      </c>
-      <c r="Z5" s="28">
-        <f>IF(ISBLANK(AA5),0, LOOKUP(AA5,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AB5/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AA5" s="1"/>
+      <c r="Y5" s="1"/>
+      <c r="Z5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="28">
+        <f>IF(ISBLANK(AB5),0, LOOKUP(AB5,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC5/100)</f>
+        <v>0</v>
+      </c>
       <c r="AB5" s="1"/>
-      <c r="AC5" s="26"/>
-      <c r="AD5" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="AC5" s="1"/>
+      <c r="AD5" s="26"/>
       <c r="AE5" s="1" t="s">
         <v>34</v>
       </c>
       <c r="AF5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG5" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A6" s="1">
         <v>21100003</v>
       </c>
@@ -5103,14 +5171,14 @@
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1">
-        <f>IF(P6&gt;=23,4,IF(AND(P6&gt;=18,P6&lt;23),3,IF(AND(P6&gt;=13,P6&lt;18),2,IF(AND(P6&gt;=8,P6&lt;13),1,0))))</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="E6" s="1">
         <v>1</v>
       </c>
       <c r="F6" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>150</v>
       </c>
       <c r="G6" s="1">
@@ -5141,44 +5209,45 @@
         <v>0</v>
       </c>
       <c r="P6" s="27">
-        <f>G6+H6+ SUM(I6:O6)*5+Y6+Z6</f>
+        <f t="shared" si="3"/>
         <v>14</v>
       </c>
       <c r="Q6" s="25"/>
-      <c r="R6" s="25" t="s">
+      <c r="R6" s="25"/>
+      <c r="S6" s="25" t="s">
         <v>100</v>
       </c>
-      <c r="S6" s="1" t="s">
+      <c r="T6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T6" s="1">
+      <c r="U6" s="1">
         <v>10</v>
       </c>
-      <c r="U6" s="1"/>
       <c r="V6" s="1"/>
       <c r="W6" s="1"/>
       <c r="X6" s="1"/>
-      <c r="Y6" s="1">
-        <v>0</v>
-      </c>
-      <c r="Z6" s="28">
-        <f>IF(ISBLANK(AA6),0, LOOKUP(AA6,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AB6/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AA6" s="1"/>
+      <c r="Y6" s="1"/>
+      <c r="Z6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="28">
+        <f>IF(ISBLANK(AB6),0, LOOKUP(AB6,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC6/100)</f>
+        <v>0</v>
+      </c>
       <c r="AB6" s="1"/>
-      <c r="AC6" s="26"/>
-      <c r="AD6" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="AC6" s="1"/>
+      <c r="AD6" s="26"/>
       <c r="AE6" s="1" t="s">
         <v>34</v>
       </c>
       <c r="AF6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG6" s="1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A7" s="1">
         <v>21100004</v>
       </c>
@@ -5187,14 +5256,14 @@
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1">
-        <f>IF(P7&gt;=23,4,IF(AND(P7&gt;=18,P7&lt;23),3,IF(AND(P7&gt;=13,P7&lt;18),2,IF(AND(P7&gt;=8,P7&lt;13),1,0))))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E7" s="1">
         <v>1</v>
       </c>
       <c r="F7" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="G7" s="1">
@@ -5225,44 +5294,45 @@
         <v>0</v>
       </c>
       <c r="P7" s="24">
-        <f>G7+H7+ SUM(I7:O7)*5+Y7+Z7</f>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="Q7" s="25"/>
-      <c r="R7" s="25" t="s">
+      <c r="R7" s="25"/>
+      <c r="S7" s="25" t="s">
         <v>104</v>
       </c>
-      <c r="S7" s="1" t="s">
+      <c r="T7" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="T7" s="1">
+      <c r="U7" s="1">
         <v>10</v>
       </c>
-      <c r="U7" s="1"/>
       <c r="V7" s="1"/>
       <c r="W7" s="1"/>
       <c r="X7" s="1"/>
-      <c r="Y7" s="1">
-        <v>0</v>
-      </c>
-      <c r="Z7" s="28">
-        <f>IF(ISBLANK(AA7),0, LOOKUP(AA7,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AB7/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AA7" s="1"/>
+      <c r="Y7" s="1"/>
+      <c r="Z7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="28">
+        <f>IF(ISBLANK(AB7),0, LOOKUP(AB7,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC7/100)</f>
+        <v>0</v>
+      </c>
       <c r="AB7" s="1"/>
-      <c r="AC7" s="26"/>
-      <c r="AD7" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="AC7" s="1"/>
+      <c r="AD7" s="26"/>
       <c r="AE7" s="1" t="s">
         <v>34</v>
       </c>
       <c r="AF7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG7" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A8" s="1">
         <v>21100005</v>
       </c>
@@ -5271,14 +5341,14 @@
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1">
-        <f>IF(P8&gt;=23,4,IF(AND(P8&gt;=18,P8&lt;23),3,IF(AND(P8&gt;=13,P8&lt;18),2,IF(AND(P8&gt;=8,P8&lt;13),1,0))))</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="E8" s="1">
         <v>1</v>
       </c>
       <c r="F8" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>150</v>
       </c>
       <c r="G8" s="1">
@@ -5309,44 +5379,45 @@
         <v>0</v>
       </c>
       <c r="P8" s="27">
-        <f>G8+H8+ SUM(I8:O8)*5+Y8+Z8</f>
+        <f t="shared" si="3"/>
         <v>13</v>
       </c>
       <c r="Q8" s="25"/>
-      <c r="R8" s="25" t="s">
+      <c r="R8" s="25"/>
+      <c r="S8" s="25" t="s">
         <v>107</v>
       </c>
-      <c r="S8" s="1" t="s">
+      <c r="T8" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="T8" s="1">
+      <c r="U8" s="1">
         <v>10</v>
       </c>
-      <c r="U8" s="1"/>
       <c r="V8" s="1"/>
       <c r="W8" s="1"/>
       <c r="X8" s="1"/>
-      <c r="Y8" s="1">
-        <v>0</v>
-      </c>
-      <c r="Z8" s="28">
-        <f>IF(ISBLANK(AA8),0, LOOKUP(AA8,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AB8/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AA8" s="1"/>
+      <c r="Y8" s="1"/>
+      <c r="Z8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA8" s="28">
+        <f>IF(ISBLANK(AB8),0, LOOKUP(AB8,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC8/100)</f>
+        <v>0</v>
+      </c>
       <c r="AB8" s="1"/>
-      <c r="AC8" s="26"/>
-      <c r="AD8" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="AC8" s="1"/>
+      <c r="AD8" s="26"/>
       <c r="AE8" s="1" t="s">
         <v>34</v>
       </c>
       <c r="AF8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG8" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A9" s="1">
         <v>21100006</v>
       </c>
@@ -5355,14 +5426,14 @@
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1">
-        <f>IF(P9&gt;=23,4,IF(AND(P9&gt;=18,P9&lt;23),3,IF(AND(P9&gt;=13,P9&lt;18),2,IF(AND(P9&gt;=8,P9&lt;13),1,0))))</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="E9" s="1">
         <v>1</v>
       </c>
       <c r="F9" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>250</v>
       </c>
       <c r="G9" s="1">
@@ -5393,44 +5464,45 @@
         <v>0</v>
       </c>
       <c r="P9" s="24">
-        <f>G9+H9+ SUM(I9:O9)*5+Y9+Z9</f>
+        <f t="shared" si="3"/>
         <v>25</v>
       </c>
       <c r="Q9" s="25"/>
-      <c r="R9" s="25" t="s">
+      <c r="R9" s="25"/>
+      <c r="S9" s="25" t="s">
         <v>110</v>
       </c>
-      <c r="S9" s="1" t="s">
+      <c r="T9" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="T9" s="1">
+      <c r="U9" s="1">
         <v>10</v>
       </c>
-      <c r="U9" s="1"/>
       <c r="V9" s="1"/>
       <c r="W9" s="1"/>
       <c r="X9" s="1"/>
-      <c r="Y9" s="1">
+      <c r="Y9" s="1"/>
+      <c r="Z9" s="1">
         <v>10</v>
       </c>
-      <c r="Z9" s="28">
-        <f>IF(ISBLANK(AA9),0, LOOKUP(AA9,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AB9/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AA9" s="1"/>
+      <c r="AA9" s="28">
+        <f>IF(ISBLANK(AB9),0, LOOKUP(AB9,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC9/100)</f>
+        <v>0</v>
+      </c>
       <c r="AB9" s="1"/>
-      <c r="AC9" s="26"/>
-      <c r="AD9" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="AC9" s="1"/>
+      <c r="AD9" s="26"/>
       <c r="AE9" s="1" t="s">
         <v>34</v>
       </c>
       <c r="AF9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG9" s="1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A10" s="1">
         <v>21100007</v>
       </c>
@@ -5439,14 +5511,14 @@
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1">
-        <f>IF(P10&gt;=23,4,IF(AND(P10&gt;=18,P10&lt;23),3,IF(AND(P10&gt;=13,P10&lt;18),2,IF(AND(P10&gt;=8,P10&lt;13),1,0))))</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="E10" s="1">
         <v>1</v>
       </c>
       <c r="F10" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>150</v>
       </c>
       <c r="G10" s="1">
@@ -5477,44 +5549,45 @@
         <v>0</v>
       </c>
       <c r="P10" s="27">
-        <f>G10+H10+ SUM(I10:O10)*5+Y10+Z10</f>
+        <f t="shared" si="3"/>
         <v>14</v>
       </c>
       <c r="Q10" s="25"/>
-      <c r="R10" s="25" t="s">
+      <c r="R10" s="25"/>
+      <c r="S10" s="25" t="s">
         <v>97</v>
       </c>
-      <c r="S10" s="1" t="s">
+      <c r="T10" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="T10" s="1">
+      <c r="U10" s="1">
         <v>10</v>
       </c>
-      <c r="U10" s="1"/>
       <c r="V10" s="1"/>
       <c r="W10" s="1"/>
       <c r="X10" s="1"/>
-      <c r="Y10" s="1">
-        <v>0</v>
-      </c>
-      <c r="Z10" s="28">
-        <f>IF(ISBLANK(AA10),0, LOOKUP(AA10,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AB10/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AA10" s="1"/>
+      <c r="Y10" s="1"/>
+      <c r="Z10" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA10" s="28">
+        <f>IF(ISBLANK(AB10),0, LOOKUP(AB10,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC10/100)</f>
+        <v>0</v>
+      </c>
       <c r="AB10" s="1"/>
-      <c r="AC10" s="26"/>
-      <c r="AD10" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="AC10" s="1"/>
+      <c r="AD10" s="26"/>
       <c r="AE10" s="1" t="s">
         <v>34</v>
       </c>
       <c r="AF10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG10" s="1" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A11" s="1">
         <v>21100008</v>
       </c>
@@ -5523,14 +5596,14 @@
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1">
-        <f>IF(P11&gt;=23,4,IF(AND(P11&gt;=18,P11&lt;23),3,IF(AND(P11&gt;=13,P11&lt;18),2,IF(AND(P11&gt;=8,P11&lt;13),1,0))))</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="E11" s="1">
         <v>1</v>
       </c>
       <c r="F11" s="1">
-        <f t="shared" ref="F11:F12" si="2">D11*50+50</f>
+        <f t="shared" ref="F11:F12" si="4">D11*50+50</f>
         <v>250</v>
       </c>
       <c r="G11" s="1">
@@ -5561,44 +5634,45 @@
         <v>0</v>
       </c>
       <c r="P11" s="24">
-        <f>G11+H11+ SUM(I11:O11)*5+Y11+Z11</f>
+        <f t="shared" si="3"/>
         <v>25</v>
       </c>
       <c r="Q11" s="25"/>
-      <c r="R11" s="25" t="s">
+      <c r="R11" s="25"/>
+      <c r="S11" s="25" t="s">
         <v>183</v>
       </c>
-      <c r="S11" s="1" t="s">
+      <c r="T11" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="T11" s="1">
+      <c r="U11" s="1">
         <v>10</v>
       </c>
-      <c r="U11" s="1"/>
       <c r="V11" s="1"/>
       <c r="W11" s="1"/>
       <c r="X11" s="1"/>
-      <c r="Y11" s="1">
-        <v>0</v>
-      </c>
-      <c r="Z11" s="28">
-        <f>IF(ISBLANK(AA11),0, LOOKUP(AA11,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AB11/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AA11" s="1"/>
+      <c r="Y11" s="1"/>
+      <c r="Z11" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA11" s="28">
+        <f>IF(ISBLANK(AB11),0, LOOKUP(AB11,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC11/100)</f>
+        <v>0</v>
+      </c>
       <c r="AB11" s="1"/>
-      <c r="AC11" s="26"/>
-      <c r="AD11" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="AC11" s="1"/>
+      <c r="AD11" s="26"/>
       <c r="AE11" s="1" t="s">
         <v>34</v>
       </c>
       <c r="AF11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG11" s="1" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A12" s="1">
         <v>21100009</v>
       </c>
@@ -5607,14 +5681,14 @@
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1">
-        <f>IF(P12&gt;=23,4,IF(AND(P12&gt;=18,P12&lt;23),3,IF(AND(P12&gt;=13,P12&lt;18),2,IF(AND(P12&gt;=8,P12&lt;13),1,0))))</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="E12" s="1">
         <v>1</v>
       </c>
       <c r="F12" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>200</v>
       </c>
       <c r="G12" s="1">
@@ -5645,44 +5719,45 @@
         <v>0</v>
       </c>
       <c r="P12" s="27">
-        <f>G12+H12+ SUM(I12:O12)*5+Y12+Z12</f>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
       <c r="Q12" s="25"/>
-      <c r="R12" s="25" t="s">
+      <c r="R12" s="25"/>
+      <c r="S12" s="25" t="s">
         <v>187</v>
       </c>
-      <c r="S12" s="1" t="s">
+      <c r="T12" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="T12" s="1">
+      <c r="U12" s="1">
         <v>10</v>
       </c>
-      <c r="U12" s="1"/>
       <c r="V12" s="1"/>
       <c r="W12" s="1"/>
       <c r="X12" s="1"/>
-      <c r="Y12" s="1">
-        <v>0</v>
-      </c>
-      <c r="Z12" s="28">
-        <f>IF(ISBLANK(AA12),0, LOOKUP(AA12,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AB12/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AA12" s="1"/>
+      <c r="Y12" s="1"/>
+      <c r="Z12" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA12" s="28">
+        <f>IF(ISBLANK(AB12),0, LOOKUP(AB12,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC12/100)</f>
+        <v>0</v>
+      </c>
       <c r="AB12" s="1"/>
-      <c r="AC12" s="26"/>
-      <c r="AD12" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="AC12" s="1"/>
+      <c r="AD12" s="26"/>
       <c r="AE12" s="1" t="s">
         <v>34</v>
       </c>
       <c r="AF12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG12" s="1" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A13" s="1">
         <v>21100010</v>
       </c>
@@ -5691,14 +5766,14 @@
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1">
-        <f>IF(P13&gt;=23,4,IF(AND(P13&gt;=18,P13&lt;23),3,IF(AND(P13&gt;=13,P13&lt;18),2,IF(AND(P13&gt;=8,P13&lt;13),1,0))))</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E13" s="1">
         <v>1</v>
       </c>
       <c r="F13" s="1">
-        <f t="shared" ref="F13:F14" si="3">D13*50+50</f>
+        <f t="shared" ref="F13:F14" si="5">D13*50+50</f>
         <v>50</v>
       </c>
       <c r="G13" s="1">
@@ -5729,44 +5804,45 @@
         <v>0</v>
       </c>
       <c r="P13" s="24">
-        <f>G13+H13+ SUM(I13:O13)*5+Y13+Z13</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="Q13" s="25"/>
-      <c r="R13" s="25" t="s">
+      <c r="R13" s="25"/>
+      <c r="S13" s="25" t="s">
         <v>190</v>
       </c>
-      <c r="S13" s="1" t="s">
+      <c r="T13" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="T13" s="1">
+      <c r="U13" s="1">
         <v>10</v>
       </c>
-      <c r="U13" s="1"/>
       <c r="V13" s="1"/>
       <c r="W13" s="1"/>
       <c r="X13" s="1"/>
-      <c r="Y13" s="1">
+      <c r="Y13" s="1"/>
+      <c r="Z13" s="1">
         <v>-10</v>
       </c>
-      <c r="Z13" s="28">
-        <f>IF(ISBLANK(AA13),0, LOOKUP(AA13,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AB13/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AA13" s="1"/>
+      <c r="AA13" s="28">
+        <f>IF(ISBLANK(AB13),0, LOOKUP(AB13,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC13/100)</f>
+        <v>0</v>
+      </c>
       <c r="AB13" s="1"/>
-      <c r="AC13" s="26"/>
-      <c r="AD13" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="AC13" s="1"/>
+      <c r="AD13" s="26"/>
       <c r="AE13" s="1" t="s">
         <v>34</v>
       </c>
       <c r="AF13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG13" s="1" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A14" s="1">
         <v>21100011</v>
       </c>
@@ -5775,14 +5851,14 @@
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1">
-        <f>IF(P14&gt;=23,4,IF(AND(P14&gt;=18,P14&lt;23),3,IF(AND(P14&gt;=13,P14&lt;18),2,IF(AND(P14&gt;=8,P14&lt;13),1,0))))</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="E14" s="1">
         <v>1</v>
       </c>
       <c r="F14" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>200</v>
       </c>
       <c r="G14" s="1">
@@ -5813,44 +5889,45 @@
         <v>0</v>
       </c>
       <c r="P14" s="27">
-        <f>G14+H14+ SUM(I14:O14)*5+Y14+Z14</f>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
       <c r="Q14" s="25"/>
-      <c r="R14" s="25" t="s">
+      <c r="R14" s="25"/>
+      <c r="S14" s="25" t="s">
         <v>193</v>
       </c>
-      <c r="S14" s="1" t="s">
+      <c r="T14" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="T14" s="1">
+      <c r="U14" s="1">
         <v>10</v>
       </c>
-      <c r="U14" s="1"/>
       <c r="V14" s="1"/>
       <c r="W14" s="1"/>
       <c r="X14" s="1"/>
-      <c r="Y14" s="1">
-        <v>0</v>
-      </c>
-      <c r="Z14" s="28">
-        <f>IF(ISBLANK(AA14),0, LOOKUP(AA14,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AB14/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AA14" s="1"/>
+      <c r="Y14" s="1"/>
+      <c r="Z14" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA14" s="28">
+        <f>IF(ISBLANK(AB14),0, LOOKUP(AB14,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC14/100)</f>
+        <v>0</v>
+      </c>
       <c r="AB14" s="1"/>
-      <c r="AC14" s="26"/>
-      <c r="AD14" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="AC14" s="1"/>
+      <c r="AD14" s="26"/>
       <c r="AE14" s="1" t="s">
         <v>34</v>
       </c>
       <c r="AF14" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG14" s="1" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A15" s="1">
         <v>21200001</v>
       </c>
@@ -5861,84 +5938,85 @@
         <v>129</v>
       </c>
       <c r="D15" s="1">
-        <f t="shared" ref="D15:D19" si="4">IF(P15&gt;=23,4,IF(AND(P15&gt;=18,P15&lt;23),3,IF(AND(P15&gt;=13,P15&lt;18),2,IF(AND(P15&gt;=8,P15&lt;13),1,0))))</f>
+        <f t="shared" ref="D15:D19" si="6">IF(P15&gt;=23,4,IF(AND(P15&gt;=18,P15&lt;23),3,IF(AND(P15&gt;=13,P15&lt;18),2,IF(AND(P15&gt;=8,P15&lt;13),1,0))))</f>
         <v>1</v>
       </c>
       <c r="E15" s="1">
         <v>2</v>
       </c>
       <c r="F15" s="1">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="G15" s="1">
+        <v>0</v>
+      </c>
+      <c r="H15" s="1">
+        <v>0</v>
+      </c>
+      <c r="I15" s="23">
+        <v>0</v>
+      </c>
+      <c r="J15" s="7">
+        <v>0</v>
+      </c>
+      <c r="K15" s="7">
+        <v>0</v>
+      </c>
+      <c r="L15" s="7">
+        <v>0</v>
+      </c>
+      <c r="M15" s="7">
+        <v>0</v>
+      </c>
+      <c r="N15" s="7">
+        <v>0</v>
+      </c>
+      <c r="O15" s="7">
+        <v>0</v>
+      </c>
+      <c r="P15" s="24">
         <f t="shared" si="1"/>
-        <v>100</v>
-      </c>
-      <c r="G15" s="1">
-        <v>0</v>
-      </c>
-      <c r="H15" s="1">
-        <v>0</v>
-      </c>
-      <c r="I15" s="23">
-        <v>0</v>
-      </c>
-      <c r="J15" s="7">
-        <v>0</v>
-      </c>
-      <c r="K15" s="7">
-        <v>0</v>
-      </c>
-      <c r="L15" s="7">
-        <v>0</v>
-      </c>
-      <c r="M15" s="7">
-        <v>0</v>
-      </c>
-      <c r="N15" s="7">
-        <v>0</v>
-      </c>
-      <c r="O15" s="7">
-        <v>0</v>
-      </c>
-      <c r="P15" s="24">
-        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
-      <c r="S15" s="1" t="s">
+      <c r="S15" s="1"/>
+      <c r="T15" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T15" s="1">
+      <c r="U15" s="1">
         <v>10</v>
       </c>
-      <c r="U15" s="1"/>
       <c r="V15" s="1"/>
-      <c r="W15" s="1">
+      <c r="W15" s="1"/>
+      <c r="X15" s="1">
         <v>20</v>
       </c>
-      <c r="X15" s="1" t="s">
+      <c r="Y15" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="Y15" s="1">
+      <c r="Z15" s="1">
         <v>10</v>
       </c>
-      <c r="Z15" s="1">
-        <f>IF(ISBLANK(AA15),0, LOOKUP(AA15,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AB15/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AA15" s="1"/>
+      <c r="AA15" s="1">
+        <f>IF(ISBLANK(AB15),0, LOOKUP(AB15,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC15/100)</f>
+        <v>0</v>
+      </c>
       <c r="AB15" s="1"/>
       <c r="AC15" s="1"/>
-      <c r="AD15" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="AD15" s="1"/>
       <c r="AE15" s="1" t="s">
         <v>34</v>
       </c>
       <c r="AF15" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG15" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A16" s="1">
         <v>21200002</v>
       </c>
@@ -5949,14 +6027,14 @@
         <v>128</v>
       </c>
       <c r="D16" s="1">
-        <f t="shared" ref="D16:D17" si="5">IF(P16&gt;=23,4,IF(AND(P16&gt;=18,P16&lt;23),3,IF(AND(P16&gt;=13,P16&lt;18),2,IF(AND(P16&gt;=8,P16&lt;13),1,0))))</f>
+        <f t="shared" ref="D16:D17" si="7">IF(P16&gt;=23,4,IF(AND(P16&gt;=18,P16&lt;23),3,IF(AND(P16&gt;=13,P16&lt;18),2,IF(AND(P16&gt;=8,P16&lt;13),1,0))))</f>
         <v>2</v>
       </c>
       <c r="E16" s="1">
         <v>2</v>
       </c>
       <c r="F16" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>150</v>
       </c>
       <c r="G16" s="1">
@@ -5987,48 +6065,49 @@
         <v>0</v>
       </c>
       <c r="P16" s="24">
-        <f t="shared" ref="P16:P17" si="6">G16+H16+ SUM(I16:O16)*5+Y16+Z16</f>
+        <f t="shared" ref="P16:P17" si="8">G16+H16+ SUM(I16:O16)*5+Z16+AA16</f>
         <v>14</v>
       </c>
       <c r="Q16" s="1"/>
       <c r="R16" s="1"/>
-      <c r="S16" s="1" t="s">
+      <c r="S16" s="1"/>
+      <c r="T16" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="T16" s="1">
+      <c r="U16" s="1">
         <v>10</v>
       </c>
-      <c r="U16" s="1"/>
-      <c r="V16" s="1">
-        <v>14</v>
-      </c>
+      <c r="V16" s="1"/>
       <c r="W16" s="1">
         <v>14</v>
       </c>
-      <c r="X16" s="1" t="s">
+      <c r="X16" s="1">
+        <v>14</v>
+      </c>
+      <c r="Y16" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="Y16" s="1">
+      <c r="Z16" s="1">
         <v>14</v>
       </c>
-      <c r="Z16" s="1">
-        <f>IF(ISBLANK(AA16),0, LOOKUP(AA16,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AB16/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AA16" s="1"/>
+      <c r="AA16" s="1">
+        <f>IF(ISBLANK(AB16),0, LOOKUP(AB16,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC16/100)</f>
+        <v>0</v>
+      </c>
       <c r="AB16" s="1"/>
       <c r="AC16" s="1"/>
-      <c r="AD16" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="AD16" s="1"/>
       <c r="AE16" s="1" t="s">
         <v>34</v>
       </c>
       <c r="AF16" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG16" s="1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="17" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A17" s="1">
         <v>21200003</v>
       </c>
@@ -6039,14 +6118,14 @@
         <v>130</v>
       </c>
       <c r="D17" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="E17" s="1">
         <v>2</v>
       </c>
       <c r="F17" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="G17" s="1">
@@ -6077,46 +6156,47 @@
         <v>0</v>
       </c>
       <c r="P17" s="24">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>12.5</v>
       </c>
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
-      <c r="S17" s="1" t="s">
+      <c r="S17" s="1"/>
+      <c r="T17" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="T17" s="1">
+      <c r="U17" s="1">
         <v>10</v>
       </c>
-      <c r="U17" s="1"/>
-      <c r="V17" s="1">
+      <c r="V17" s="1"/>
+      <c r="W17" s="1">
         <v>25</v>
       </c>
-      <c r="W17" s="1"/>
-      <c r="X17" s="1" t="s">
+      <c r="X17" s="1"/>
+      <c r="Y17" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="Y17" s="1">
+      <c r="Z17" s="1">
         <v>12.5</v>
       </c>
-      <c r="Z17" s="1">
-        <f>IF(ISBLANK(AA17),0, LOOKUP(AA17,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AB17/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AA17" s="1"/>
+      <c r="AA17" s="1">
+        <f>IF(ISBLANK(AB17),0, LOOKUP(AB17,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC17/100)</f>
+        <v>0</v>
+      </c>
       <c r="AB17" s="1"/>
       <c r="AC17" s="1"/>
-      <c r="AD17" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="AD17" s="1"/>
       <c r="AE17" s="1" t="s">
         <v>34</v>
       </c>
       <c r="AF17" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG17" s="1" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A18" s="1">
         <v>21200004</v>
       </c>
@@ -6127,14 +6207,14 @@
         <v>131</v>
       </c>
       <c r="D18" s="1">
-        <f t="shared" ref="D18" si="7">IF(P18&gt;=23,4,IF(AND(P18&gt;=18,P18&lt;23),3,IF(AND(P18&gt;=13,P18&lt;18),2,IF(AND(P18&gt;=8,P18&lt;13),1,0))))</f>
+        <f t="shared" ref="D18" si="9">IF(P18&gt;=23,4,IF(AND(P18&gt;=18,P18&lt;23),3,IF(AND(P18&gt;=13,P18&lt;18),2,IF(AND(P18&gt;=8,P18&lt;13),1,0))))</f>
         <v>2</v>
       </c>
       <c r="E18" s="1">
         <v>2</v>
       </c>
       <c r="F18" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>150</v>
       </c>
       <c r="G18" s="1">
@@ -6165,48 +6245,49 @@
         <v>0</v>
       </c>
       <c r="P18" s="24">
-        <f t="shared" ref="P18" si="8">G18+H18+ SUM(I18:O18)*5+Y18+Z18</f>
+        <f t="shared" ref="P18" si="10">G18+H18+ SUM(I18:O18)*5+Z18+AA18</f>
         <v>14</v>
       </c>
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
-      <c r="S18" s="1" t="s">
+      <c r="S18" s="1"/>
+      <c r="T18" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="T18" s="1">
+      <c r="U18" s="1">
         <v>10</v>
       </c>
-      <c r="U18" s="1"/>
-      <c r="V18" s="1">
-        <v>14</v>
-      </c>
+      <c r="V18" s="1"/>
       <c r="W18" s="1">
         <v>14</v>
       </c>
-      <c r="X18" s="1" t="s">
+      <c r="X18" s="1">
+        <v>14</v>
+      </c>
+      <c r="Y18" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="Y18" s="1">
+      <c r="Z18" s="1">
         <v>14</v>
       </c>
-      <c r="Z18" s="1">
-        <f>IF(ISBLANK(AA18),0, LOOKUP(AA18,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AB18/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AA18" s="1"/>
+      <c r="AA18" s="1">
+        <f>IF(ISBLANK(AB18),0, LOOKUP(AB18,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC18/100)</f>
+        <v>0</v>
+      </c>
       <c r="AB18" s="1"/>
       <c r="AC18" s="1"/>
-      <c r="AD18" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="AD18" s="1"/>
       <c r="AE18" s="1" t="s">
         <v>34</v>
       </c>
       <c r="AF18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG18" s="1" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="19" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A19" s="1">
         <v>21300001</v>
       </c>
@@ -6215,14 +6296,14 @@
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E19" s="1">
         <v>3</v>
       </c>
       <c r="F19" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>50</v>
       </c>
       <c r="G19" s="1">
@@ -6253,42 +6334,45 @@
         <v>0</v>
       </c>
       <c r="P19" s="24">
-        <f t="shared" ref="P19" si="9">G19+H19+ SUM(I19:O19)*5+Y19+Z19</f>
+        <f t="shared" ref="P19" si="11">G19+H19+ SUM(I19:O19)*5+Z19+AA19</f>
         <v>5</v>
       </c>
       <c r="Q19" s="1"/>
-      <c r="R19" s="1"/>
-      <c r="S19" s="1" t="s">
+      <c r="R19" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="S19" s="1"/>
+      <c r="T19" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T19" s="1">
+      <c r="U19" s="1">
         <v>10</v>
       </c>
-      <c r="U19" s="1"/>
       <c r="V19" s="1"/>
       <c r="W19" s="1"/>
       <c r="X19" s="1"/>
-      <c r="Y19" s="1">
-        <v>0</v>
-      </c>
+      <c r="Y19" s="1"/>
       <c r="Z19" s="1">
-        <f>IF(ISBLANK(AA19),0, LOOKUP(AA19,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AB19/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AA19" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="AA19" s="1">
+        <f>IF(ISBLANK(AB19),0, LOOKUP(AB19,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC19/100)</f>
+        <v>0</v>
+      </c>
       <c r="AB19" s="1"/>
       <c r="AC19" s="1"/>
-      <c r="AD19" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="AD19" s="1"/>
       <c r="AE19" s="1" t="s">
         <v>34</v>
       </c>
       <c r="AF19" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG19" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="20" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A20" s="1">
         <v>21300002</v>
       </c>
@@ -6297,14 +6381,14 @@
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1">
-        <f t="shared" ref="D20:D21" si="10">IF(P20&gt;=23,4,IF(AND(P20&gt;=18,P20&lt;23),3,IF(AND(P20&gt;=13,P20&lt;18),2,IF(AND(P20&gt;=8,P20&lt;13),1,0))))</f>
+        <f t="shared" ref="D20:D21" si="12">IF(P20&gt;=23,4,IF(AND(P20&gt;=18,P20&lt;23),3,IF(AND(P20&gt;=13,P20&lt;18),2,IF(AND(P20&gt;=8,P20&lt;13),1,0))))</f>
         <v>1</v>
       </c>
       <c r="E20" s="1">
         <v>3</v>
       </c>
       <c r="F20" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="G20" s="1">
@@ -6335,46 +6419,49 @@
         <v>0</v>
       </c>
       <c r="P20" s="24">
-        <f t="shared" ref="P20:P21" si="11">G20+H20+ SUM(I20:O20)*5+Y20+Z20</f>
+        <f t="shared" ref="P20:P21" si="13">G20+H20+ SUM(I20:O20)*5+Z20+AA20</f>
         <v>9</v>
       </c>
       <c r="Q20" s="1"/>
-      <c r="R20" s="1"/>
-      <c r="S20" s="1" t="s">
+      <c r="R20" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="S20" s="1"/>
+      <c r="T20" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="T20" s="1">
+      <c r="U20" s="1">
         <v>10</v>
       </c>
-      <c r="U20" s="1"/>
       <c r="V20" s="1"/>
       <c r="W20" s="1"/>
       <c r="X20" s="1"/>
-      <c r="Y20" s="1">
-        <v>0</v>
-      </c>
+      <c r="Y20" s="1"/>
       <c r="Z20" s="1">
-        <f>IF(ISBLANK(AA20),0, LOOKUP(AA20,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AB20/100)</f>
+        <v>0</v>
+      </c>
+      <c r="AA20" s="1">
+        <f>IF(ISBLANK(AB20),0, LOOKUP(AB20,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC20/100)</f>
         <v>3</v>
       </c>
-      <c r="AA20" s="1">
+      <c r="AB20" s="1">
         <v>55510010</v>
       </c>
-      <c r="AB20" s="1">
+      <c r="AC20" s="1">
         <v>60</v>
       </c>
-      <c r="AC20" s="1"/>
-      <c r="AD20" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="AD20" s="1"/>
       <c r="AE20" s="1" t="s">
         <v>34</v>
       </c>
       <c r="AF20" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG20" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="21" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A21" s="1">
         <v>21300003</v>
       </c>
@@ -6383,14 +6470,14 @@
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
       <c r="E21" s="1">
         <v>3</v>
       </c>
       <c r="F21" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>150</v>
       </c>
       <c r="G21" s="1">
@@ -6421,42 +6508,45 @@
         <v>0</v>
       </c>
       <c r="P21" s="24">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>16</v>
       </c>
       <c r="Q21" s="1"/>
-      <c r="R21" s="1"/>
-      <c r="S21" s="1" t="s">
+      <c r="R21" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="S21" s="1"/>
+      <c r="T21" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="T21" s="1">
+      <c r="U21" s="1">
         <v>10</v>
       </c>
-      <c r="U21" s="1"/>
       <c r="V21" s="1"/>
       <c r="W21" s="1"/>
       <c r="X21" s="1"/>
-      <c r="Y21" s="1">
-        <v>0</v>
-      </c>
+      <c r="Y21" s="1"/>
       <c r="Z21" s="1">
-        <f>IF(ISBLANK(AA21),0, LOOKUP(AA21,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AB21/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AA21" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="AA21" s="1">
+        <f>IF(ISBLANK(AB21),0, LOOKUP(AB21,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC21/100)</f>
+        <v>0</v>
+      </c>
       <c r="AB21" s="1"/>
       <c r="AC21" s="1"/>
-      <c r="AD21" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="AD21" s="1"/>
       <c r="AE21" s="1" t="s">
         <v>34</v>
       </c>
       <c r="AF21" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG21" s="1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="22" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A22" s="1">
         <v>21300004</v>
       </c>
@@ -6465,14 +6555,14 @@
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1">
-        <f t="shared" ref="D22:D23" si="12">IF(P22&gt;=23,4,IF(AND(P22&gt;=18,P22&lt;23),3,IF(AND(P22&gt;=13,P22&lt;18),2,IF(AND(P22&gt;=8,P22&lt;13),1,0))))</f>
+        <f t="shared" ref="D22:D23" si="14">IF(P22&gt;=23,4,IF(AND(P22&gt;=18,P22&lt;23),3,IF(AND(P22&gt;=13,P22&lt;18),2,IF(AND(P22&gt;=8,P22&lt;13),1,0))))</f>
         <v>2</v>
       </c>
       <c r="E22" s="1">
         <v>3</v>
       </c>
       <c r="F22" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>150</v>
       </c>
       <c r="G22" s="1">
@@ -6503,46 +6593,49 @@
         <v>0</v>
       </c>
       <c r="P22" s="24">
-        <f t="shared" ref="P22:P23" si="13">G22+H22+ SUM(I22:O22)*5+Y22+Z22</f>
+        <f t="shared" ref="P22:P23" si="15">G22+H22+ SUM(I22:O22)*5+Z22+AA22</f>
         <v>17.3</v>
       </c>
       <c r="Q22" s="1"/>
-      <c r="R22" s="1"/>
-      <c r="S22" s="1" t="s">
+      <c r="R22" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="S22" s="1"/>
+      <c r="T22" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="T22" s="1">
+      <c r="U22" s="1">
         <v>10</v>
       </c>
-      <c r="U22" s="1"/>
       <c r="V22" s="1"/>
       <c r="W22" s="1"/>
       <c r="X22" s="1"/>
-      <c r="Y22" s="1">
-        <v>0</v>
-      </c>
+      <c r="Y22" s="1"/>
       <c r="Z22" s="1">
-        <f>IF(ISBLANK(AA22),0, LOOKUP(AA22,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AB22/100)</f>
+        <v>0</v>
+      </c>
+      <c r="AA22" s="1">
+        <f>IF(ISBLANK(AB22),0, LOOKUP(AB22,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC22/100)</f>
         <v>9.3000000000000007</v>
       </c>
-      <c r="AA22" s="1">
+      <c r="AB22" s="1">
         <v>55510012</v>
       </c>
-      <c r="AB22" s="1">
+      <c r="AC22" s="1">
         <v>15</v>
       </c>
-      <c r="AC22" s="1"/>
-      <c r="AD22" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="AD22" s="1"/>
       <c r="AE22" s="1" t="s">
         <v>34</v>
       </c>
       <c r="AF22" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG22" s="1" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="23" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A23" s="1">
         <v>21300005</v>
       </c>
@@ -6551,14 +6644,14 @@
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="E23" s="1">
         <v>3</v>
       </c>
       <c r="F23" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="G23" s="1">
@@ -6589,42 +6682,45 @@
         <v>0</v>
       </c>
       <c r="P23" s="24">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>12</v>
       </c>
       <c r="Q23" s="1"/>
-      <c r="R23" s="1"/>
-      <c r="S23" s="1" t="s">
+      <c r="R23" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="S23" s="1"/>
+      <c r="T23" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="T23" s="1">
+      <c r="U23" s="1">
         <v>10</v>
       </c>
-      <c r="U23" s="1"/>
       <c r="V23" s="1"/>
       <c r="W23" s="1"/>
       <c r="X23" s="1"/>
-      <c r="Y23" s="1">
-        <v>0</v>
-      </c>
+      <c r="Y23" s="1"/>
       <c r="Z23" s="1">
-        <f>IF(ISBLANK(AA23),0, LOOKUP(AA23,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AB23/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AA23" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="AA23" s="1">
+        <f>IF(ISBLANK(AB23),0, LOOKUP(AB23,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC23/100)</f>
+        <v>0</v>
+      </c>
       <c r="AB23" s="1"/>
       <c r="AC23" s="1"/>
-      <c r="AD23" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="AD23" s="1"/>
       <c r="AE23" s="1" t="s">
         <v>34</v>
       </c>
       <c r="AF23" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG23" s="1" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="24" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A24" s="1">
         <v>21300006</v>
       </c>
@@ -6633,14 +6729,14 @@
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1">
-        <f t="shared" ref="D24:D25" si="14">IF(P24&gt;=23,4,IF(AND(P24&gt;=18,P24&lt;23),3,IF(AND(P24&gt;=13,P24&lt;18),2,IF(AND(P24&gt;=8,P24&lt;13),1,0))))</f>
+        <f t="shared" ref="D24:D25" si="16">IF(P24&gt;=23,4,IF(AND(P24&gt;=18,P24&lt;23),3,IF(AND(P24&gt;=13,P24&lt;18),2,IF(AND(P24&gt;=8,P24&lt;13),1,0))))</f>
         <v>3</v>
       </c>
       <c r="E24" s="1">
         <v>3</v>
       </c>
       <c r="F24" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>200</v>
       </c>
       <c r="G24" s="1">
@@ -6671,42 +6767,45 @@
         <v>0</v>
       </c>
       <c r="P24" s="24">
-        <f t="shared" ref="P24:P25" si="15">G24+H24+ SUM(I24:O24)*5+Y24+Z24</f>
+        <f t="shared" ref="P24:P25" si="17">G24+H24+ SUM(I24:O24)*5+Z24+AA24</f>
         <v>20</v>
       </c>
       <c r="Q24" s="1"/>
-      <c r="R24" s="1"/>
-      <c r="S24" s="1" t="s">
+      <c r="R24" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="S24" s="1"/>
+      <c r="T24" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="T24" s="1">
+      <c r="U24" s="1">
         <v>10</v>
       </c>
-      <c r="U24" s="1"/>
       <c r="V24" s="1"/>
       <c r="W24" s="1"/>
       <c r="X24" s="1"/>
-      <c r="Y24" s="1">
-        <v>0</v>
-      </c>
+      <c r="Y24" s="1"/>
       <c r="Z24" s="1">
-        <f>IF(ISBLANK(AA24),0, LOOKUP(AA24,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AB24/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AA24" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="AA24" s="1">
+        <f>IF(ISBLANK(AB24),0, LOOKUP(AB24,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC24/100)</f>
+        <v>0</v>
+      </c>
       <c r="AB24" s="1"/>
       <c r="AC24" s="1"/>
-      <c r="AD24" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="AD24" s="1"/>
       <c r="AE24" s="1" t="s">
         <v>34</v>
       </c>
       <c r="AF24" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG24" s="1" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="25" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A25" s="1">
         <v>21300007</v>
       </c>
@@ -6715,14 +6814,14 @@
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>4</v>
       </c>
       <c r="E25" s="1">
         <v>3</v>
       </c>
       <c r="F25" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>250</v>
       </c>
       <c r="G25" s="1">
@@ -6753,42 +6852,45 @@
         <v>0</v>
       </c>
       <c r="P25" s="24">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>30</v>
       </c>
       <c r="Q25" s="1"/>
-      <c r="R25" s="1"/>
-      <c r="S25" s="1" t="s">
+      <c r="R25" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="S25" s="1"/>
+      <c r="T25" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="T25" s="1">
+      <c r="U25" s="1">
         <v>10</v>
       </c>
-      <c r="U25" s="1"/>
       <c r="V25" s="1"/>
       <c r="W25" s="1"/>
       <c r="X25" s="1"/>
-      <c r="Y25" s="1">
-        <v>0</v>
-      </c>
+      <c r="Y25" s="1"/>
       <c r="Z25" s="1">
-        <f>IF(ISBLANK(AA25),0, LOOKUP(AA25,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AB25/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AA25" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="AA25" s="1">
+        <f>IF(ISBLANK(AB25),0, LOOKUP(AB25,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC25/100)</f>
+        <v>0</v>
+      </c>
       <c r="AB25" s="1"/>
       <c r="AC25" s="1"/>
-      <c r="AD25" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="AD25" s="1"/>
       <c r="AE25" s="1" t="s">
         <v>34</v>
       </c>
       <c r="AF25" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG25" s="1" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="26" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A26" s="1">
         <v>21300008</v>
       </c>
@@ -6797,14 +6899,14 @@
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1">
-        <f t="shared" ref="D26:D27" si="16">IF(P26&gt;=23,4,IF(AND(P26&gt;=18,P26&lt;23),3,IF(AND(P26&gt;=13,P26&lt;18),2,IF(AND(P26&gt;=8,P26&lt;13),1,0))))</f>
+        <f t="shared" ref="D26:D27" si="18">IF(P26&gt;=23,4,IF(AND(P26&gt;=18,P26&lt;23),3,IF(AND(P26&gt;=13,P26&lt;18),2,IF(AND(P26&gt;=8,P26&lt;13),1,0))))</f>
         <v>0</v>
       </c>
       <c r="E26" s="1">
         <v>3</v>
       </c>
       <c r="F26" s="1">
-        <f t="shared" ref="F26:F27" si="17">D26*50+50</f>
+        <f t="shared" ref="F26:F27" si="19">D26*50+50</f>
         <v>50</v>
       </c>
       <c r="G26" s="1">
@@ -6835,42 +6937,45 @@
         <v>0</v>
       </c>
       <c r="P26" s="24">
-        <f t="shared" ref="P26:P27" si="18">G26+H26+ SUM(I26:O26)*5+Y26+Z26</f>
+        <f t="shared" ref="P26:P27" si="20">G26+H26+ SUM(I26:O26)*5+Z26+AA26</f>
         <v>1</v>
       </c>
       <c r="Q26" s="1"/>
-      <c r="R26" s="1"/>
-      <c r="S26" s="1" t="s">
+      <c r="R26" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="S26" s="1"/>
+      <c r="T26" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="T26" s="1">
+      <c r="U26" s="1">
         <v>10</v>
       </c>
-      <c r="U26" s="1"/>
       <c r="V26" s="1"/>
       <c r="W26" s="1"/>
       <c r="X26" s="1"/>
-      <c r="Y26" s="1">
-        <v>0</v>
-      </c>
+      <c r="Y26" s="1"/>
       <c r="Z26" s="1">
-        <f>IF(ISBLANK(AA26),0, LOOKUP(AA26,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AB26/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AA26" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="AA26" s="1">
+        <f>IF(ISBLANK(AB26),0, LOOKUP(AB26,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC26/100)</f>
+        <v>0</v>
+      </c>
       <c r="AB26" s="1"/>
       <c r="AC26" s="1"/>
-      <c r="AD26" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="AD26" s="1"/>
       <c r="AE26" s="1" t="s">
         <v>34</v>
       </c>
       <c r="AF26" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG26" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="27" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A27" s="1">
         <v>21300009</v>
       </c>
@@ -6879,14 +6984,14 @@
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>3</v>
       </c>
       <c r="E27" s="1">
         <v>3</v>
       </c>
       <c r="F27" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>200</v>
       </c>
       <c r="G27" s="1">
@@ -6917,46 +7022,49 @@
         <v>0</v>
       </c>
       <c r="P27" s="24">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>20</v>
       </c>
       <c r="Q27" s="1"/>
-      <c r="R27" s="1"/>
-      <c r="S27" s="1" t="s">
+      <c r="R27" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="S27" s="1"/>
+      <c r="T27" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="T27" s="1">
+      <c r="U27" s="1">
         <v>10</v>
       </c>
-      <c r="U27" s="1"/>
       <c r="V27" s="1"/>
       <c r="W27" s="1"/>
       <c r="X27" s="1"/>
-      <c r="Y27" s="1">
-        <v>0</v>
-      </c>
+      <c r="Y27" s="1"/>
       <c r="Z27" s="1">
-        <f>IF(ISBLANK(AA27),0, LOOKUP(AA27,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AB27/100)</f>
+        <v>0</v>
+      </c>
+      <c r="AA27" s="1">
+        <f>IF(ISBLANK(AB27),0, LOOKUP(AB27,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC27/100)</f>
         <v>35</v>
       </c>
-      <c r="AA27" s="1">
+      <c r="AB27" s="1">
         <v>55100007</v>
       </c>
-      <c r="AB27" s="1">
+      <c r="AC27" s="1">
         <v>100</v>
       </c>
-      <c r="AC27" s="1"/>
-      <c r="AD27" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="AD27" s="1"/>
       <c r="AE27" s="1" t="s">
         <v>34</v>
       </c>
       <c r="AF27" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG27" s="1" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="28" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>21400001</v>
       </c>
@@ -6965,14 +7073,14 @@
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="22">
-        <f t="shared" ref="D28" si="19">IF(P28&gt;=23,4,IF(AND(P28&gt;=18,P28&lt;23),3,IF(AND(P28&gt;=13,P28&lt;18),2,IF(AND(P28&gt;=8,P28&lt;13),1,0))))</f>
+        <f t="shared" ref="D28" si="21">IF(P28&gt;=23,4,IF(AND(P28&gt;=18,P28&lt;23),3,IF(AND(P28&gt;=13,P28&lt;18),2,IF(AND(P28&gt;=8,P28&lt;13),1,0))))</f>
         <v>0</v>
       </c>
       <c r="E28" s="1">
         <v>4</v>
       </c>
       <c r="F28" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>50</v>
       </c>
       <c r="G28" s="7">
@@ -7003,36 +7111,37 @@
         <v>0</v>
       </c>
       <c r="P28" s="24">
-        <f t="shared" ref="P28" si="20">G28+H28+ SUM(I28:O28)*5+Y28+Z28</f>
+        <f t="shared" ref="P28" si="22">G28+H28+ SUM(I28:O28)*5+Z28+AA28</f>
         <v>5</v>
       </c>
       <c r="Q28" s="7"/>
       <c r="R28" s="7"/>
-      <c r="S28" s="12" t="s">
+      <c r="S28" s="7"/>
+      <c r="T28" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="T28">
+      <c r="U28">
         <v>10</v>
       </c>
-      <c r="Y28">
-        <v>0</v>
-      </c>
       <c r="Z28">
-        <f>IF(ISBLANK(AA28),0, LOOKUP(AA28,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AB28/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AC28" s="12"/>
-      <c r="AD28" s="12" t="s">
-        <v>34</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="AA28">
+        <f>IF(ISBLANK(AB28),0, LOOKUP(AB28,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC28/100)</f>
+        <v>0</v>
+      </c>
+      <c r="AD28" s="12"/>
       <c r="AE28" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="AF28" s="2" t="s">
+      <c r="AF28" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG28" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="29" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>21400002</v>
       </c>
@@ -7041,14 +7150,14 @@
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="22">
-        <f t="shared" ref="D29:D30" si="21">IF(P29&gt;=23,4,IF(AND(P29&gt;=18,P29&lt;23),3,IF(AND(P29&gt;=13,P29&lt;18),2,IF(AND(P29&gt;=8,P29&lt;13),1,0))))</f>
+        <f t="shared" ref="D29:D30" si="23">IF(P29&gt;=23,4,IF(AND(P29&gt;=18,P29&lt;23),3,IF(AND(P29&gt;=13,P29&lt;18),2,IF(AND(P29&gt;=8,P29&lt;13),1,0))))</f>
         <v>1</v>
       </c>
       <c r="E29" s="1">
         <v>4</v>
       </c>
       <c r="F29" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="G29" s="7">
@@ -7079,36 +7188,37 @@
         <v>0</v>
       </c>
       <c r="P29" s="24">
-        <f t="shared" ref="P29:P30" si="22">G29+H29+ SUM(I29:O29)*5+Y29+Z29</f>
+        <f t="shared" ref="P29:P30" si="24">G29+H29+ SUM(I29:O29)*5+Z29+AA29</f>
         <v>10</v>
       </c>
       <c r="Q29" s="7"/>
       <c r="R29" s="7"/>
-      <c r="S29" s="12" t="s">
+      <c r="S29" s="7"/>
+      <c r="T29" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="T29">
+      <c r="U29">
         <v>10</v>
       </c>
-      <c r="Y29">
-        <v>0</v>
-      </c>
       <c r="Z29">
-        <f>IF(ISBLANK(AA29),0, LOOKUP(AA29,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AB29/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AC29" s="12"/>
-      <c r="AD29" s="12" t="s">
-        <v>34</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="AA29">
+        <f>IF(ISBLANK(AB29),0, LOOKUP(AB29,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC29/100)</f>
+        <v>0</v>
+      </c>
+      <c r="AD29" s="12"/>
       <c r="AE29" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="AF29" s="2" t="s">
+      <c r="AF29" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG29" s="2" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="30" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A30">
         <v>21400003</v>
       </c>
@@ -7117,14 +7227,14 @@
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="22">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>2</v>
       </c>
       <c r="E30" s="1">
         <v>4</v>
       </c>
       <c r="F30" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>150</v>
       </c>
       <c r="G30" s="7">
@@ -7155,42 +7265,43 @@
         <v>0</v>
       </c>
       <c r="P30" s="24">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>15</v>
       </c>
       <c r="Q30" s="7"/>
       <c r="R30" s="7"/>
-      <c r="S30" s="12" t="s">
+      <c r="S30" s="7"/>
+      <c r="T30" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="T30">
+      <c r="U30">
         <v>10</v>
       </c>
-      <c r="Y30">
-        <v>0</v>
-      </c>
       <c r="Z30">
-        <f>IF(ISBLANK(AA30),0, LOOKUP(AA30,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AB30/100)</f>
+        <v>0</v>
+      </c>
+      <c r="AA30">
+        <f>IF(ISBLANK(AB30),0, LOOKUP(AB30,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC30/100)</f>
         <v>10</v>
       </c>
-      <c r="AA30">
+      <c r="AB30">
         <v>55110005</v>
       </c>
-      <c r="AB30">
+      <c r="AC30">
         <v>50</v>
       </c>
-      <c r="AC30" s="12"/>
-      <c r="AD30" s="12" t="s">
-        <v>34</v>
-      </c>
+      <c r="AD30" s="12"/>
       <c r="AE30" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="AF30" s="2" t="s">
+      <c r="AF30" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG30" s="2" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="31" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A31">
         <v>21400004</v>
       </c>
@@ -7199,14 +7310,14 @@
       </c>
       <c r="C31" s="1"/>
       <c r="D31" s="22">
-        <f t="shared" ref="D31:D32" si="23">IF(P31&gt;=23,4,IF(AND(P31&gt;=18,P31&lt;23),3,IF(AND(P31&gt;=13,P31&lt;18),2,IF(AND(P31&gt;=8,P31&lt;13),1,0))))</f>
+        <f t="shared" ref="D31:D32" si="25">IF(P31&gt;=23,4,IF(AND(P31&gt;=18,P31&lt;23),3,IF(AND(P31&gt;=13,P31&lt;18),2,IF(AND(P31&gt;=8,P31&lt;13),1,0))))</f>
         <v>3</v>
       </c>
       <c r="E31" s="1">
         <v>4</v>
       </c>
       <c r="F31" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>200</v>
       </c>
       <c r="G31" s="7">
@@ -7237,36 +7348,37 @@
         <v>0</v>
       </c>
       <c r="P31" s="24">
-        <f t="shared" ref="P31:P32" si="24">G31+H31+ SUM(I31:O31)*5+Y31+Z31</f>
+        <f t="shared" ref="P31:P32" si="26">G31+H31+ SUM(I31:O31)*5+Z31+AA31</f>
         <v>20</v>
       </c>
       <c r="Q31" s="7"/>
       <c r="R31" s="7"/>
-      <c r="S31" s="12" t="s">
+      <c r="S31" s="7"/>
+      <c r="T31" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="T31">
+      <c r="U31">
         <v>10</v>
       </c>
-      <c r="Y31">
-        <v>0</v>
-      </c>
       <c r="Z31">
-        <f>IF(ISBLANK(AA31),0, LOOKUP(AA31,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AB31/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AC31" s="12"/>
-      <c r="AD31" s="12" t="s">
-        <v>34</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="AA31">
+        <f>IF(ISBLANK(AB31),0, LOOKUP(AB31,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC31/100)</f>
+        <v>0</v>
+      </c>
+      <c r="AD31" s="12"/>
       <c r="AE31" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="AF31" s="2" t="s">
+      <c r="AF31" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG31" s="2" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="32" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A32">
         <v>21400005</v>
       </c>
@@ -7275,14 +7387,14 @@
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="22">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>1</v>
       </c>
       <c r="E32" s="1">
         <v>4</v>
       </c>
       <c r="F32" s="1">
-        <f t="shared" ref="F32:F33" si="25">D32*50+50</f>
+        <f t="shared" ref="F32:F33" si="27">D32*50+50</f>
         <v>100</v>
       </c>
       <c r="G32" s="7">
@@ -7313,36 +7425,37 @@
         <v>0</v>
       </c>
       <c r="P32" s="24">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>8</v>
       </c>
       <c r="Q32" s="7"/>
       <c r="R32" s="7"/>
-      <c r="S32" s="12" t="s">
+      <c r="S32" s="7"/>
+      <c r="T32" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="T32">
+      <c r="U32">
         <v>10</v>
       </c>
-      <c r="Y32">
-        <v>0</v>
-      </c>
       <c r="Z32">
-        <f>IF(ISBLANK(AA32),0, LOOKUP(AA32,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AB32/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AC32" s="12"/>
-      <c r="AD32" s="12" t="s">
-        <v>34</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="AA32">
+        <f>IF(ISBLANK(AB32),0, LOOKUP(AB32,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC32/100)</f>
+        <v>0</v>
+      </c>
+      <c r="AD32" s="12"/>
       <c r="AE32" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="AF32" s="2" t="s">
+      <c r="AF32" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG32" s="2" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="33" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A33">
         <v>21400006</v>
       </c>
@@ -7351,14 +7464,14 @@
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="22">
-        <f t="shared" ref="D33:D34" si="26">IF(P33&gt;=23,4,IF(AND(P33&gt;=18,P33&lt;23),3,IF(AND(P33&gt;=13,P33&lt;18),2,IF(AND(P33&gt;=8,P33&lt;13),1,0))))</f>
+        <f t="shared" ref="D33:D34" si="28">IF(P33&gt;=23,4,IF(AND(P33&gt;=18,P33&lt;23),3,IF(AND(P33&gt;=13,P33&lt;18),2,IF(AND(P33&gt;=8,P33&lt;13),1,0))))</f>
         <v>2</v>
       </c>
       <c r="E33" s="1">
         <v>4</v>
       </c>
       <c r="F33" s="1">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>150</v>
       </c>
       <c r="G33" s="7">
@@ -7389,36 +7502,37 @@
         <v>0</v>
       </c>
       <c r="P33" s="24">
-        <f t="shared" ref="P33:P34" si="27">G33+H33+ SUM(I33:O33)*5+Y33+Z33</f>
+        <f t="shared" ref="P33:P34" si="29">G33+H33+ SUM(I33:O33)*5+Z33+AA33</f>
         <v>14</v>
       </c>
       <c r="Q33" s="7"/>
       <c r="R33" s="7"/>
-      <c r="S33" s="12" t="s">
+      <c r="S33" s="7"/>
+      <c r="T33" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="T33">
+      <c r="U33">
         <v>10</v>
       </c>
-      <c r="Y33">
-        <v>0</v>
-      </c>
       <c r="Z33">
-        <f>IF(ISBLANK(AA33),0, LOOKUP(AA33,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AB33/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AC33" s="12"/>
-      <c r="AD33" s="12" t="s">
-        <v>34</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="AA33">
+        <f>IF(ISBLANK(AB33),0, LOOKUP(AB33,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC33/100)</f>
+        <v>0</v>
+      </c>
+      <c r="AD33" s="12"/>
       <c r="AE33" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="AF33" s="2" t="s">
+      <c r="AF33" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG33" s="2" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="34" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A34">
         <v>21400007</v>
       </c>
@@ -7427,14 +7541,14 @@
       </c>
       <c r="C34" s="1"/>
       <c r="D34" s="22">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>3</v>
       </c>
       <c r="E34" s="1">
         <v>4</v>
       </c>
       <c r="F34" s="1">
-        <f t="shared" ref="F34:F35" si="28">D34*50+50</f>
+        <f t="shared" ref="F34:F35" si="30">D34*50+50</f>
         <v>200</v>
       </c>
       <c r="G34" s="7">
@@ -7465,36 +7579,37 @@
         <v>0</v>
       </c>
       <c r="P34" s="24">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>20</v>
       </c>
       <c r="Q34" s="7"/>
       <c r="R34" s="7"/>
-      <c r="S34" s="12" t="s">
+      <c r="S34" s="7"/>
+      <c r="T34" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="T34">
+      <c r="U34">
         <v>10</v>
       </c>
-      <c r="Y34">
-        <v>0</v>
-      </c>
       <c r="Z34">
-        <f>IF(ISBLANK(AA34),0, LOOKUP(AA34,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AB34/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AC34" s="12"/>
-      <c r="AD34" s="12" t="s">
-        <v>34</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="AA34">
+        <f>IF(ISBLANK(AB34),0, LOOKUP(AB34,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC34/100)</f>
+        <v>0</v>
+      </c>
+      <c r="AD34" s="12"/>
       <c r="AE34" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="AF34" s="2" t="s">
+      <c r="AF34" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG34" s="2" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="35" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A35">
         <v>21400008</v>
       </c>
@@ -7503,14 +7618,14 @@
       </c>
       <c r="C35" s="1"/>
       <c r="D35" s="22">
-        <f t="shared" ref="D35:D36" si="29">IF(P35&gt;=23,4,IF(AND(P35&gt;=18,P35&lt;23),3,IF(AND(P35&gt;=13,P35&lt;18),2,IF(AND(P35&gt;=8,P35&lt;13),1,0))))</f>
+        <f t="shared" ref="D35:D36" si="31">IF(P35&gt;=23,4,IF(AND(P35&gt;=18,P35&lt;23),3,IF(AND(P35&gt;=13,P35&lt;18),2,IF(AND(P35&gt;=8,P35&lt;13),1,0))))</f>
         <v>0</v>
       </c>
       <c r="E35" s="1">
         <v>4</v>
       </c>
       <c r="F35" s="1">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>50</v>
       </c>
       <c r="G35" s="7">
@@ -7541,36 +7656,37 @@
         <v>0</v>
       </c>
       <c r="P35" s="24">
-        <f t="shared" ref="P35:P36" si="30">G35+H35+ SUM(I35:O35)*5+Y35+Z35</f>
+        <f t="shared" ref="P35:P36" si="32">G35+H35+ SUM(I35:O35)*5+Z35+AA35</f>
         <v>0</v>
       </c>
       <c r="Q35" s="7"/>
       <c r="R35" s="7"/>
-      <c r="S35" s="12" t="s">
+      <c r="S35" s="7"/>
+      <c r="T35" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="T35">
+      <c r="U35">
         <v>10</v>
       </c>
-      <c r="Y35">
-        <v>0</v>
-      </c>
       <c r="Z35">
-        <f>IF(ISBLANK(AA35),0, LOOKUP(AA35,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AB35/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AC35" s="12"/>
-      <c r="AD35" s="12" t="s">
-        <v>34</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="AA35">
+        <f>IF(ISBLANK(AB35),0, LOOKUP(AB35,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC35/100)</f>
+        <v>0</v>
+      </c>
+      <c r="AD35" s="12"/>
       <c r="AE35" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="AF35" s="2" t="s">
+      <c r="AF35" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG35" s="2" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="36" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A36">
         <v>21400009</v>
       </c>
@@ -7579,14 +7695,14 @@
       </c>
       <c r="C36" s="1"/>
       <c r="D36" s="22">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>2</v>
       </c>
       <c r="E36" s="1">
         <v>4</v>
       </c>
       <c r="F36" s="1">
-        <f t="shared" ref="F36:F37" si="31">D36*50+50</f>
+        <f t="shared" ref="F36:F37" si="33">D36*50+50</f>
         <v>150</v>
       </c>
       <c r="G36" s="7">
@@ -7617,36 +7733,37 @@
         <v>0</v>
       </c>
       <c r="P36" s="24">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>13</v>
       </c>
       <c r="Q36" s="7"/>
       <c r="R36" s="7"/>
-      <c r="S36" s="12" t="s">
+      <c r="S36" s="7"/>
+      <c r="T36" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="T36">
+      <c r="U36">
         <v>10</v>
       </c>
-      <c r="Y36">
-        <v>0</v>
-      </c>
       <c r="Z36">
-        <f>IF(ISBLANK(AA36),0, LOOKUP(AA36,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AB36/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AC36" s="12"/>
-      <c r="AD36" s="12" t="s">
-        <v>34</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="AA36">
+        <f>IF(ISBLANK(AB36),0, LOOKUP(AB36,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC36/100)</f>
+        <v>0</v>
+      </c>
+      <c r="AD36" s="12"/>
       <c r="AE36" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="AF36" s="2" t="s">
+      <c r="AF36" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG36" s="2" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="37" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A37">
         <v>21400010</v>
       </c>
@@ -7655,14 +7772,14 @@
       </c>
       <c r="C37" s="1"/>
       <c r="D37" s="22">
-        <f t="shared" ref="D37:D38" si="32">IF(P37&gt;=23,4,IF(AND(P37&gt;=18,P37&lt;23),3,IF(AND(P37&gt;=13,P37&lt;18),2,IF(AND(P37&gt;=8,P37&lt;13),1,0))))</f>
+        <f t="shared" ref="D37:D38" si="34">IF(P37&gt;=23,4,IF(AND(P37&gt;=18,P37&lt;23),3,IF(AND(P37&gt;=13,P37&lt;18),2,IF(AND(P37&gt;=8,P37&lt;13),1,0))))</f>
         <v>2</v>
       </c>
       <c r="E37" s="1">
         <v>4</v>
       </c>
       <c r="F37" s="1">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>150</v>
       </c>
       <c r="G37" s="7">
@@ -7693,36 +7810,37 @@
         <v>0</v>
       </c>
       <c r="P37" s="24">
-        <f t="shared" ref="P37:P38" si="33">G37+H37+ SUM(I37:O37)*5+Y37+Z37</f>
+        <f t="shared" ref="P37:P38" si="35">G37+H37+ SUM(I37:O37)*5+Z37+AA37</f>
         <v>15</v>
       </c>
       <c r="Q37" s="7"/>
       <c r="R37" s="7"/>
-      <c r="S37" s="12" t="s">
+      <c r="S37" s="7"/>
+      <c r="T37" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="T37">
+      <c r="U37">
         <v>10</v>
       </c>
-      <c r="Y37">
-        <v>0</v>
-      </c>
       <c r="Z37">
-        <f>IF(ISBLANK(AA37),0, LOOKUP(AA37,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AB37/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AC37" s="12"/>
-      <c r="AD37" s="12" t="s">
-        <v>34</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="AA37">
+        <f>IF(ISBLANK(AB37),0, LOOKUP(AB37,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC37/100)</f>
+        <v>0</v>
+      </c>
+      <c r="AD37" s="12"/>
       <c r="AE37" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="AF37" s="2" t="s">
+      <c r="AF37" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG37" s="2" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="38" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A38">
         <v>21400011</v>
       </c>
@@ -7731,14 +7849,14 @@
       </c>
       <c r="C38" s="1"/>
       <c r="D38" s="22">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v>4</v>
       </c>
       <c r="E38" s="1">
         <v>4</v>
       </c>
       <c r="F38" s="1">
-        <f t="shared" ref="F38" si="34">D38*50+50</f>
+        <f t="shared" ref="F38" si="36">D38*50+50</f>
         <v>250</v>
       </c>
       <c r="G38" s="7">
@@ -7769,36 +7887,37 @@
         <v>0</v>
       </c>
       <c r="P38" s="24">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>30</v>
       </c>
       <c r="Q38" s="7"/>
       <c r="R38" s="7"/>
-      <c r="S38" s="12" t="s">
+      <c r="S38" s="7"/>
+      <c r="T38" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="T38">
+      <c r="U38">
         <v>10</v>
       </c>
-      <c r="Y38">
-        <v>0</v>
-      </c>
       <c r="Z38">
-        <f>IF(ISBLANK(AA38),0, LOOKUP(AA38,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AB38/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AC38" s="12"/>
-      <c r="AD38" s="12" t="s">
-        <v>34</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="AA38">
+        <f>IF(ISBLANK(AB38),0, LOOKUP(AB38,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC38/100)</f>
+        <v>0</v>
+      </c>
+      <c r="AD38" s="12"/>
       <c r="AE38" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="AF38" s="2" t="s">
+      <c r="AF38" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG38" s="2" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="39" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A39">
         <v>21500001</v>
       </c>
@@ -7807,14 +7926,14 @@
       </c>
       <c r="C39" s="1"/>
       <c r="D39" s="22">
-        <f t="shared" ref="D39" si="35">IF(P39&gt;=23,4,IF(AND(P39&gt;=18,P39&lt;23),3,IF(AND(P39&gt;=13,P39&lt;18),2,IF(AND(P39&gt;=8,P39&lt;13),1,0))))</f>
+        <f t="shared" ref="D39" si="37">IF(P39&gt;=23,4,IF(AND(P39&gt;=18,P39&lt;23),3,IF(AND(P39&gt;=13,P39&lt;18),2,IF(AND(P39&gt;=8,P39&lt;13),1,0))))</f>
         <v>1</v>
       </c>
       <c r="E39" s="1">
         <v>5</v>
       </c>
       <c r="F39" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="G39" s="7">
@@ -7845,38 +7964,39 @@
         <v>0</v>
       </c>
       <c r="P39" s="24">
-        <f t="shared" ref="P39" si="36">G39+H39+ SUM(I39:O39)*5+Y39+Z39</f>
+        <f t="shared" ref="P39" si="38">G39+H39+ SUM(I39:O39)*5+Z39+AA39</f>
         <v>10</v>
       </c>
       <c r="Q39" s="7">
         <v>5</v>
       </c>
       <c r="R39" s="7"/>
-      <c r="S39" s="12" t="s">
+      <c r="S39" s="7"/>
+      <c r="T39" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="T39">
+      <c r="U39">
         <v>10</v>
       </c>
-      <c r="Y39">
+      <c r="Z39">
         <v>10</v>
       </c>
-      <c r="Z39">
-        <f>IF(ISBLANK(AA39),0, LOOKUP(AA39,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AB39/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AC39" s="12"/>
-      <c r="AD39" s="12" t="s">
-        <v>34</v>
-      </c>
+      <c r="AA39">
+        <f>IF(ISBLANK(AB39),0, LOOKUP(AB39,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC39/100)</f>
+        <v>0</v>
+      </c>
+      <c r="AD39" s="12"/>
       <c r="AE39" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="AF39" s="2" t="s">
+      <c r="AF39" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG39" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="40" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A40">
         <v>21500002</v>
       </c>
@@ -7885,14 +8005,14 @@
       </c>
       <c r="C40" s="1"/>
       <c r="D40" s="22">
-        <f t="shared" ref="D40:D41" si="37">IF(P40&gt;=23,4,IF(AND(P40&gt;=18,P40&lt;23),3,IF(AND(P40&gt;=13,P40&lt;18),2,IF(AND(P40&gt;=8,P40&lt;13),1,0))))</f>
+        <f t="shared" ref="D40:D41" si="39">IF(P40&gt;=23,4,IF(AND(P40&gt;=18,P40&lt;23),3,IF(AND(P40&gt;=13,P40&lt;18),2,IF(AND(P40&gt;=8,P40&lt;13),1,0))))</f>
         <v>1</v>
       </c>
       <c r="E40" s="1">
         <v>5</v>
       </c>
       <c r="F40" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="G40" s="7">
@@ -7923,36 +8043,37 @@
         <v>0</v>
       </c>
       <c r="P40" s="24">
-        <f t="shared" ref="P40:P41" si="38">G40+H40+ SUM(I40:O40)*5+Y40+Z40</f>
+        <f t="shared" ref="P40:P41" si="40">G40+H40+ SUM(I40:O40)*5+Z40+AA40</f>
         <v>10</v>
       </c>
       <c r="Q40" s="7"/>
       <c r="R40" s="7"/>
-      <c r="S40" s="12" t="s">
+      <c r="S40" s="7"/>
+      <c r="T40" s="12" t="s">
         <v>138</v>
       </c>
-      <c r="T40">
+      <c r="U40">
         <v>10</v>
       </c>
-      <c r="Y40">
+      <c r="Z40">
         <v>5</v>
       </c>
-      <c r="Z40">
-        <f>IF(ISBLANK(AA40),0, LOOKUP(AA40,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AB40/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AC40" s="12"/>
-      <c r="AD40" s="12" t="s">
-        <v>34</v>
-      </c>
+      <c r="AA40">
+        <f>IF(ISBLANK(AB40),0, LOOKUP(AB40,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC40/100)</f>
+        <v>0</v>
+      </c>
+      <c r="AD40" s="12"/>
       <c r="AE40" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="AF40" s="2" t="s">
+      <c r="AF40" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG40" s="2" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="41" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A41">
         <v>21500003</v>
       </c>
@@ -7961,14 +8082,14 @@
       </c>
       <c r="C41" s="1"/>
       <c r="D41" s="22">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>1</v>
       </c>
       <c r="E41" s="1">
         <v>5</v>
       </c>
       <c r="F41" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="G41" s="7">
@@ -7999,38 +8120,39 @@
         <v>0</v>
       </c>
       <c r="P41" s="24">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v>11</v>
       </c>
       <c r="Q41" s="7">
         <v>6</v>
       </c>
       <c r="R41" s="7"/>
-      <c r="S41" s="12" t="s">
+      <c r="S41" s="7"/>
+      <c r="T41" s="12" t="s">
         <v>144</v>
       </c>
-      <c r="T41">
+      <c r="U41">
         <v>10</v>
       </c>
-      <c r="Y41">
+      <c r="Z41">
         <v>6</v>
       </c>
-      <c r="Z41">
-        <f>IF(ISBLANK(AA41),0, LOOKUP(AA41,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AB41/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AC41" s="12"/>
-      <c r="AD41" s="12" t="s">
-        <v>34</v>
-      </c>
+      <c r="AA41">
+        <f>IF(ISBLANK(AB41),0, LOOKUP(AB41,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC41/100)</f>
+        <v>0</v>
+      </c>
+      <c r="AD41" s="12"/>
       <c r="AE41" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="AF41" s="2" t="s">
+      <c r="AF41" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG41" s="2" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="42" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A42">
         <v>21500004</v>
       </c>
@@ -8039,14 +8161,14 @@
       </c>
       <c r="C42" s="1"/>
       <c r="D42" s="22">
-        <f t="shared" ref="D42:D43" si="39">IF(P42&gt;=23,4,IF(AND(P42&gt;=18,P42&lt;23),3,IF(AND(P42&gt;=13,P42&lt;18),2,IF(AND(P42&gt;=8,P42&lt;13),1,0))))</f>
+        <f t="shared" ref="D42:D43" si="41">IF(P42&gt;=23,4,IF(AND(P42&gt;=18,P42&lt;23),3,IF(AND(P42&gt;=13,P42&lt;18),2,IF(AND(P42&gt;=8,P42&lt;13),1,0))))</f>
         <v>1</v>
       </c>
       <c r="E42" s="1">
         <v>5</v>
       </c>
       <c r="F42" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="G42" s="7">
@@ -8077,42 +8199,43 @@
         <v>0</v>
       </c>
       <c r="P42" s="24">
-        <f t="shared" ref="P42:P43" si="40">G42+H42+ SUM(I42:O42)*5+Y42+Z42</f>
+        <f t="shared" ref="P42:P43" si="42">G42+H42+ SUM(I42:O42)*5+Z42+AA42</f>
         <v>8</v>
       </c>
       <c r="Q42" s="7"/>
       <c r="R42" s="7"/>
-      <c r="S42" s="12" t="s">
+      <c r="S42" s="7"/>
+      <c r="T42" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="T42">
+      <c r="U42">
         <v>10</v>
       </c>
-      <c r="Y42">
-        <v>0</v>
-      </c>
       <c r="Z42">
-        <f>IF(ISBLANK(AA42),0, LOOKUP(AA42,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AB42/100)</f>
+        <v>0</v>
+      </c>
+      <c r="AA42">
+        <f>IF(ISBLANK(AB42),0, LOOKUP(AB42,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC42/100)</f>
         <v>4</v>
       </c>
-      <c r="AA42">
+      <c r="AB42">
         <v>55990108</v>
       </c>
-      <c r="AB42">
+      <c r="AC42">
         <v>100</v>
       </c>
-      <c r="AC42" s="12"/>
-      <c r="AD42" s="12" t="s">
-        <v>34</v>
-      </c>
+      <c r="AD42" s="12"/>
       <c r="AE42" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="AF42" s="2" t="s">
+      <c r="AF42" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG42" s="2" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="43" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A43">
         <v>21500005</v>
       </c>
@@ -8121,14 +8244,14 @@
       </c>
       <c r="C43" s="1"/>
       <c r="D43" s="22">
-        <f t="shared" si="39"/>
+        <f t="shared" si="41"/>
         <v>2</v>
       </c>
       <c r="E43" s="1">
         <v>5</v>
       </c>
       <c r="F43" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>150</v>
       </c>
       <c r="G43" s="7">
@@ -8159,36 +8282,37 @@
         <v>1</v>
       </c>
       <c r="P43" s="24">
-        <f t="shared" si="40"/>
+        <f t="shared" si="42"/>
         <v>15</v>
       </c>
       <c r="Q43" s="7"/>
       <c r="R43" s="7"/>
-      <c r="S43" s="12" t="s">
+      <c r="S43" s="7"/>
+      <c r="T43" s="12" t="s">
         <v>148</v>
       </c>
-      <c r="T43">
+      <c r="U43">
         <v>10</v>
       </c>
-      <c r="Y43">
+      <c r="Z43">
         <v>10</v>
       </c>
-      <c r="Z43">
-        <f>IF(ISBLANK(AA43),0, LOOKUP(AA43,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AB43/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AC43" s="12"/>
-      <c r="AD43" s="12" t="s">
-        <v>34</v>
-      </c>
+      <c r="AA43">
+        <f>IF(ISBLANK(AB43),0, LOOKUP(AB43,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC43/100)</f>
+        <v>0</v>
+      </c>
+      <c r="AD43" s="12"/>
       <c r="AE43" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="AF43" s="2" t="s">
+      <c r="AF43" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG43" s="2" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="44" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A44">
         <v>21500006</v>
       </c>
@@ -8197,14 +8321,14 @@
       </c>
       <c r="C44" s="1"/>
       <c r="D44" s="22">
-        <f t="shared" ref="D44:D45" si="41">IF(P44&gt;=23,4,IF(AND(P44&gt;=18,P44&lt;23),3,IF(AND(P44&gt;=13,P44&lt;18),2,IF(AND(P44&gt;=8,P44&lt;13),1,0))))</f>
+        <f t="shared" ref="D44:D45" si="43">IF(P44&gt;=23,4,IF(AND(P44&gt;=18,P44&lt;23),3,IF(AND(P44&gt;=13,P44&lt;18),2,IF(AND(P44&gt;=8,P44&lt;13),1,0))))</f>
         <v>2</v>
       </c>
       <c r="E44" s="1">
         <v>5</v>
       </c>
       <c r="F44" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>150</v>
       </c>
       <c r="G44" s="7">
@@ -8235,42 +8359,43 @@
         <v>0</v>
       </c>
       <c r="P44" s="24">
-        <f t="shared" ref="P44:P45" si="42">G44+H44+ SUM(I44:O44)*5+Y44+Z44</f>
+        <f t="shared" ref="P44:P45" si="44">G44+H44+ SUM(I44:O44)*5+Z44+AA44</f>
         <v>15</v>
       </c>
       <c r="Q44" s="7"/>
       <c r="R44" s="7"/>
-      <c r="S44" s="12" t="s">
+      <c r="S44" s="7"/>
+      <c r="T44" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="T44">
+      <c r="U44">
         <v>10</v>
       </c>
-      <c r="Y44">
-        <v>0</v>
-      </c>
       <c r="Z44">
-        <f>IF(ISBLANK(AA44),0, LOOKUP(AA44,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AB44/100)</f>
+        <v>0</v>
+      </c>
+      <c r="AA44">
+        <f>IF(ISBLANK(AB44),0, LOOKUP(AB44,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC44/100)</f>
         <v>15</v>
       </c>
-      <c r="AA44">
+      <c r="AB44">
         <v>55990109</v>
       </c>
-      <c r="AB44">
+      <c r="AC44">
         <v>100</v>
       </c>
-      <c r="AC44" s="12"/>
-      <c r="AD44" s="12" t="s">
-        <v>34</v>
-      </c>
+      <c r="AD44" s="12"/>
       <c r="AE44" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="AF44" s="2" t="s">
+      <c r="AF44" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG44" s="2" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="45" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A45">
         <v>21500007</v>
       </c>
@@ -8279,14 +8404,14 @@
       </c>
       <c r="C45" s="1"/>
       <c r="D45" s="22">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>1</v>
       </c>
       <c r="E45" s="1">
         <v>5</v>
       </c>
       <c r="F45" s="1">
-        <f t="shared" ref="F45:F46" si="43">D45*50+50</f>
+        <f t="shared" ref="F45:F46" si="45">D45*50+50</f>
         <v>100</v>
       </c>
       <c r="G45" s="7">
@@ -8317,36 +8442,37 @@
         <v>0</v>
       </c>
       <c r="P45" s="24">
-        <f t="shared" si="42"/>
+        <f t="shared" si="44"/>
         <v>8</v>
       </c>
       <c r="Q45" s="7"/>
       <c r="R45" s="7"/>
-      <c r="S45" s="12" t="s">
+      <c r="S45" s="7"/>
+      <c r="T45" s="12" t="s">
         <v>175</v>
       </c>
-      <c r="T45">
+      <c r="U45">
         <v>10</v>
       </c>
-      <c r="Y45">
+      <c r="Z45">
         <v>8</v>
       </c>
-      <c r="Z45">
-        <f>IF(ISBLANK(AA45),0, LOOKUP(AA45,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AB45/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AC45" s="12"/>
-      <c r="AD45" s="12" t="s">
-        <v>34</v>
-      </c>
+      <c r="AA45">
+        <f>IF(ISBLANK(AB45),0, LOOKUP(AB45,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC45/100)</f>
+        <v>0</v>
+      </c>
+      <c r="AD45" s="12"/>
       <c r="AE45" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="AF45" s="2" t="s">
+      <c r="AF45" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG45" s="2" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="46" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A46">
         <v>21500008</v>
       </c>
@@ -8355,14 +8481,14 @@
       </c>
       <c r="C46" s="1"/>
       <c r="D46" s="22">
-        <f t="shared" ref="D46" si="44">IF(P46&gt;=23,4,IF(AND(P46&gt;=18,P46&lt;23),3,IF(AND(P46&gt;=13,P46&lt;18),2,IF(AND(P46&gt;=8,P46&lt;13),1,0))))</f>
+        <f t="shared" ref="D46" si="46">IF(P46&gt;=23,4,IF(AND(P46&gt;=18,P46&lt;23),3,IF(AND(P46&gt;=13,P46&lt;18),2,IF(AND(P46&gt;=8,P46&lt;13),1,0))))</f>
         <v>4</v>
       </c>
       <c r="E46" s="1">
         <v>5</v>
       </c>
       <c r="F46" s="1">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v>250</v>
       </c>
       <c r="G46" s="7">
@@ -8393,57 +8519,58 @@
         <v>0</v>
       </c>
       <c r="P46" s="24">
-        <f t="shared" ref="P46" si="45">G46+H46+ SUM(I46:O46)*5+Y46+Z46</f>
+        <f t="shared" ref="P46" si="47">G46+H46+ SUM(I46:O46)*5+Z46+AA46</f>
         <v>25</v>
       </c>
       <c r="Q46" s="7"/>
       <c r="R46" s="7"/>
-      <c r="S46" s="12" t="s">
+      <c r="S46" s="7"/>
+      <c r="T46" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="T46">
+      <c r="U46">
         <v>10</v>
       </c>
-      <c r="Y46">
-        <v>0</v>
-      </c>
       <c r="Z46">
-        <f>IF(ISBLANK(AA46),0, LOOKUP(AA46,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AB46/100)</f>
+        <v>0</v>
+      </c>
+      <c r="AA46">
+        <f>IF(ISBLANK(AB46),0, LOOKUP(AB46,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC46/100)</f>
         <v>10</v>
       </c>
-      <c r="AA46">
+      <c r="AB46">
         <v>55110003</v>
       </c>
-      <c r="AB46">
+      <c r="AC46">
         <v>40</v>
       </c>
-      <c r="AC46" s="12"/>
-      <c r="AD46" s="12" t="s">
-        <v>34</v>
-      </c>
+      <c r="AD46" s="12"/>
       <c r="AE46" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="AF46" s="2" t="s">
+      <c r="AF46" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG46" s="2" t="s">
         <v>180</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="D4:D46">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThanOrEqual">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
add some new equips. remove some useless module
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Equip.xlsx
+++ b/ConfigData/Xlsx/Equip.xlsx
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="242">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -816,6 +816,148 @@
   </si>
   <si>
     <t>laser</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>zhulou12</t>
+  </si>
+  <si>
+    <t>1;3;6</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>霍格沃兹</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>zhulou13</t>
+  </si>
+  <si>
+    <t>帕特农神庙</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>2;3</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>zhulou14</t>
+  </si>
+  <si>
+    <t>竹楼</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>1;3;7</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>zhulou15</t>
+  </si>
+  <si>
+    <t>圣托里尼</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>1;3;9</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>qizhi5</t>
+  </si>
+  <si>
+    <t>0;0;0</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>联合旗帜</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>提升我方所有单位6%最大生命值</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>qizhi6</t>
+  </si>
+  <si>
+    <t>海盗旗帜</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>提升我方所有单位6%攻击</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>公牛旗帜</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>m.IsRace("Beast")</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>提升我方野兽12%攻击和6%最大生命值</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>qizhi7</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>qizhi8</t>
+  </si>
+  <si>
+    <t>m.IsRace("Machine") || m.IsRace("Element")</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>科学旗帜</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>提升我方机械和元素单位12%攻击和最大生命值</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>qizhi9</t>
+  </si>
+  <si>
+    <t>m.IsRace("Totem") || m.IsRace("Element")</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>提升我方图腾和元素单位10%攻击和最大生命值</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>药水旗帜</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>qizhi10</t>
+  </si>
+  <si>
+    <t>m.Star&gt;5</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>提升我方5星以上单位10%攻击和最大生命值</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>英雄旗帜</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>m.Star&gt;0</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>jianzhu9</t>
+  </si>
+  <si>
+    <t>护盾发生器</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1718,64 +1860,7 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="27">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9148C8"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B0F0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="32">
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
@@ -1877,6 +1962,25 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -2176,6 +2280,82 @@
         <vertical/>
         <horizontal/>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9148C8"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B0F0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9148C8"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B0F0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -4287,52 +4467,52 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:AG46" totalsRowShown="0">
-  <autoFilter ref="A3:AG46"/>
-  <sortState ref="A4:AG28">
-    <sortCondition ref="A3:A28"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:AG57" totalsRowShown="0">
+  <autoFilter ref="A3:AG57"/>
+  <sortState ref="A4:AG38">
+    <sortCondition ref="A3:A38"/>
   </sortState>
   <tableColumns count="33">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="Name"/>
-    <tableColumn id="32" name="Des" dataDxfId="26"/>
-    <tableColumn id="3" name="Quality" dataDxfId="25">
+    <tableColumn id="32" name="Des" dataDxfId="21"/>
+    <tableColumn id="3" name="Quality" dataDxfId="20">
       <calculatedColumnFormula>IF(P4&gt;=23,4,IF(AND(P4&gt;=18,P4&lt;23),3,IF(AND(P4&gt;=13,P4&lt;18),2,IF(AND(P4&gt;=8,P4&lt;13),1,0))))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" name="Position"/>
-    <tableColumn id="19" name="Value" dataDxfId="24">
+    <tableColumn id="19" name="Value" dataDxfId="19">
       <calculatedColumnFormula>D4*50+50</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="11" name="AtkR"/>
     <tableColumn id="8" name="VitR"/>
-    <tableColumn id="6" name="Def" dataDxfId="23"/>
-    <tableColumn id="22" name="Mag" dataDxfId="22"/>
-    <tableColumn id="27" name="Spd" dataDxfId="21"/>
-    <tableColumn id="26" name="Hit" dataDxfId="20"/>
-    <tableColumn id="25" name="Dhit" dataDxfId="19"/>
-    <tableColumn id="24" name="Crt" dataDxfId="18"/>
-    <tableColumn id="23" name="Luk" dataDxfId="17"/>
-    <tableColumn id="28" name="Sum" dataDxfId="16">
+    <tableColumn id="6" name="Def" dataDxfId="18"/>
+    <tableColumn id="22" name="Mag" dataDxfId="17"/>
+    <tableColumn id="27" name="Spd" dataDxfId="16"/>
+    <tableColumn id="26" name="Hit" dataDxfId="15"/>
+    <tableColumn id="25" name="Dhit" dataDxfId="14"/>
+    <tableColumn id="24" name="Crt" dataDxfId="13"/>
+    <tableColumn id="23" name="Luk" dataDxfId="12"/>
+    <tableColumn id="28" name="Sum" dataDxfId="11">
       <calculatedColumnFormula>G4+H4+ SUM(I4:O4)*5+Z4+AA4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="Range" dataDxfId="15"/>
-    <tableColumn id="33" name="Arrow" dataDxfId="0"/>
-    <tableColumn id="4" name="SlotId" dataDxfId="14"/>
-    <tableColumn id="9" name="EnergyRate" dataDxfId="13"/>
+    <tableColumn id="12" name="Range" dataDxfId="10"/>
+    <tableColumn id="33" name="Arrow" dataDxfId="9"/>
+    <tableColumn id="4" name="SlotId" dataDxfId="8"/>
+    <tableColumn id="9" name="EnergyRate" dataDxfId="7"/>
     <tableColumn id="7" name="Durable"/>
     <tableColumn id="20" name="HeroSkillId"/>
-    <tableColumn id="29" name="MonsterAtk" dataDxfId="12"/>
-    <tableColumn id="30" name="MonsterHp" dataDxfId="11"/>
-    <tableColumn id="31" name="PickMethod" dataDxfId="10"/>
+    <tableColumn id="29" name="MonsterAtk" dataDxfId="6"/>
+    <tableColumn id="30" name="MonsterHp" dataDxfId="5"/>
+    <tableColumn id="31" name="PickMethod" dataDxfId="4"/>
     <tableColumn id="21" name="~SkillMark2"/>
-    <tableColumn id="18" name="~SkillMark22" dataDxfId="9">
+    <tableColumn id="18" name="~SkillMark22" dataDxfId="3">
       <calculatedColumnFormula>IF(ISBLANK(AB4),0, LOOKUP(AB4,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC4/100)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="13" name="CommonSkillId"/>
     <tableColumn id="14" name="CommonSkillRate"/>
-    <tableColumn id="15" name="Disable" dataDxfId="8"/>
-    <tableColumn id="17" name="RandomDrop" dataDxfId="7"/>
-    <tableColumn id="16" name="CanMerge" dataDxfId="6"/>
+    <tableColumn id="15" name="Disable" dataDxfId="2"/>
+    <tableColumn id="17" name="RandomDrop" dataDxfId="1"/>
+    <tableColumn id="16" name="CanMerge" dataDxfId="0"/>
     <tableColumn id="10" name="Url"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -4660,10 +4840,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG46"/>
+  <dimension ref="A1:AG57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R15" sqref="R15"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -4675,7 +4855,7 @@
     <col min="7" max="8" width="5.125" customWidth="1"/>
     <col min="9" max="16" width="4.5" customWidth="1"/>
     <col min="17" max="18" width="5.125" customWidth="1"/>
-    <col min="19" max="19" width="16.875" customWidth="1"/>
+    <col min="19" max="19" width="10.875" customWidth="1"/>
     <col min="20" max="20" width="8.625" customWidth="1"/>
     <col min="21" max="21" width="5" customWidth="1"/>
     <col min="22" max="22" width="8.625" customWidth="1"/>
@@ -5039,7 +5219,7 @@
         <v>0</v>
       </c>
       <c r="P4" s="24">
-        <f t="shared" ref="P4:P15" si="1">G4+H4+ SUM(I4:O4)*5+Z4+AA4</f>
+        <f t="shared" ref="P4:P38" si="1">G4+H4+ SUM(I4:O4)*5+Z4+AA4</f>
         <v>-5</v>
       </c>
       <c r="Q4" s="1"/>
@@ -5093,7 +5273,7 @@
         <v>1</v>
       </c>
       <c r="F5" s="1">
-        <f t="shared" ref="F5:F44" si="2">D5*50+50</f>
+        <f t="shared" ref="F5:F54" si="2">D5*50+50</f>
         <v>100</v>
       </c>
       <c r="G5" s="1">
@@ -5124,7 +5304,7 @@
         <v>0</v>
       </c>
       <c r="P5" s="24">
-        <f t="shared" ref="P5:P14" si="3">G5+H5+ SUM(I5:O5)*5+Z5+AA5</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="Q5" s="25"/>
@@ -5209,7 +5389,7 @@
         <v>0</v>
       </c>
       <c r="P6" s="27">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="Q6" s="25"/>
@@ -5294,7 +5474,7 @@
         <v>0</v>
       </c>
       <c r="P7" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="Q7" s="25"/>
@@ -5379,7 +5559,7 @@
         <v>0</v>
       </c>
       <c r="P8" s="27">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="Q8" s="25"/>
@@ -5464,7 +5644,7 @@
         <v>0</v>
       </c>
       <c r="P9" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
       <c r="Q9" s="25"/>
@@ -5549,7 +5729,7 @@
         <v>0</v>
       </c>
       <c r="P10" s="27">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="Q10" s="25"/>
@@ -5603,7 +5783,7 @@
         <v>1</v>
       </c>
       <c r="F11" s="1">
-        <f t="shared" ref="F11:F12" si="4">D11*50+50</f>
+        <f t="shared" ref="F11:F12" si="3">D11*50+50</f>
         <v>250</v>
       </c>
       <c r="G11" s="1">
@@ -5634,7 +5814,7 @@
         <v>0</v>
       </c>
       <c r="P11" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
       <c r="Q11" s="25"/>
@@ -5688,7 +5868,7 @@
         <v>1</v>
       </c>
       <c r="F12" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>200</v>
       </c>
       <c r="G12" s="1">
@@ -5719,7 +5899,7 @@
         <v>0</v>
       </c>
       <c r="P12" s="27">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="Q12" s="25"/>
@@ -5773,7 +5953,7 @@
         <v>1</v>
       </c>
       <c r="F13" s="1">
-        <f t="shared" ref="F13:F14" si="5">D13*50+50</f>
+        <f t="shared" ref="F13:F14" si="4">D13*50+50</f>
         <v>50</v>
       </c>
       <c r="G13" s="1">
@@ -5804,7 +5984,7 @@
         <v>0</v>
       </c>
       <c r="P13" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="Q13" s="25"/>
@@ -5858,7 +6038,7 @@
         <v>1</v>
       </c>
       <c r="F14" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>200</v>
       </c>
       <c r="G14" s="1">
@@ -5889,7 +6069,7 @@
         <v>0</v>
       </c>
       <c r="P14" s="27">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="Q14" s="25"/>
@@ -5929,36 +6109,34 @@
     </row>
     <row r="15" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A15" s="1">
-        <v>21200001</v>
+        <v>21100012</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>129</v>
-      </c>
+        <v>206</v>
+      </c>
+      <c r="C15" s="1"/>
       <c r="D15" s="1">
-        <f t="shared" ref="D15:D19" si="6">IF(P15&gt;=23,4,IF(AND(P15&gt;=18,P15&lt;23),3,IF(AND(P15&gt;=13,P15&lt;18),2,IF(AND(P15&gt;=8,P15&lt;13),1,0))))</f>
+        <f t="shared" ref="D15:D16" si="5">IF(P15&gt;=23,4,IF(AND(P15&gt;=18,P15&lt;23),3,IF(AND(P15&gt;=13,P15&lt;18),2,IF(AND(P15&gt;=8,P15&lt;13),1,0))))</f>
+        <v>3</v>
+      </c>
+      <c r="E15" s="1">
         <v>1</v>
       </c>
-      <c r="E15" s="1">
+      <c r="F15" s="1">
+        <f t="shared" ref="F15:F16" si="6">D15*50+50</f>
+        <v>200</v>
+      </c>
+      <c r="G15" s="1">
+        <v>0</v>
+      </c>
+      <c r="H15" s="1">
         <v>2</v>
       </c>
-      <c r="F15" s="1">
-        <f t="shared" si="2"/>
-        <v>100</v>
-      </c>
-      <c r="G15" s="1">
-        <v>0</v>
-      </c>
-      <c r="H15" s="1">
-        <v>0</v>
-      </c>
       <c r="I15" s="23">
         <v>0</v>
       </c>
       <c r="J15" s="7">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K15" s="7">
         <v>0</v>
@@ -5977,35 +6155,33 @@
       </c>
       <c r="P15" s="24">
         <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="Q15" s="1"/>
-      <c r="R15" s="1"/>
-      <c r="S15" s="1"/>
+        <v>22</v>
+      </c>
+      <c r="Q15" s="25"/>
+      <c r="R15" s="25"/>
+      <c r="S15" s="25" t="s">
+        <v>205</v>
+      </c>
       <c r="T15" s="1" t="s">
-        <v>18</v>
+        <v>101</v>
       </c>
       <c r="U15" s="1">
         <v>10</v>
       </c>
       <c r="V15" s="1"/>
       <c r="W15" s="1"/>
-      <c r="X15" s="1">
-        <v>20</v>
-      </c>
-      <c r="Y15" s="1" t="s">
-        <v>91</v>
-      </c>
+      <c r="X15" s="1"/>
+      <c r="Y15" s="1"/>
       <c r="Z15" s="1">
-        <v>10</v>
-      </c>
-      <c r="AA15" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA15" s="28">
         <f>IF(ISBLANK(AB15),0, LOOKUP(AB15,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC15/100)</f>
         <v>0</v>
       </c>
       <c r="AB15" s="1"/>
       <c r="AC15" s="1"/>
-      <c r="AD15" s="1"/>
+      <c r="AD15" s="26"/>
       <c r="AE15" s="1" t="s">
         <v>34</v>
       </c>
@@ -6013,37 +6189,35 @@
         <v>34</v>
       </c>
       <c r="AG15" s="1" t="s">
-        <v>74</v>
+        <v>204</v>
       </c>
     </row>
     <row r="16" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A16" s="1">
-        <v>21200002</v>
+        <v>21100013</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>128</v>
-      </c>
+        <v>208</v>
+      </c>
+      <c r="C16" s="1"/>
       <c r="D16" s="1">
-        <f t="shared" ref="D16:D17" si="7">IF(P16&gt;=23,4,IF(AND(P16&gt;=18,P16&lt;23),3,IF(AND(P16&gt;=13,P16&lt;18),2,IF(AND(P16&gt;=8,P16&lt;13),1,0))))</f>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="E16" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F16" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>150</v>
       </c>
       <c r="G16" s="1">
         <v>0</v>
       </c>
       <c r="H16" s="1">
-        <v>0</v>
-      </c>
-      <c r="I16" s="23">
+        <v>5</v>
+      </c>
+      <c r="I16" s="29">
         <v>0</v>
       </c>
       <c r="J16" s="7">
@@ -6062,41 +6236,37 @@
         <v>0</v>
       </c>
       <c r="O16" s="7">
-        <v>0</v>
-      </c>
-      <c r="P16" s="24">
-        <f t="shared" ref="P16:P17" si="8">G16+H16+ SUM(I16:O16)*5+Z16+AA16</f>
-        <v>14</v>
-      </c>
-      <c r="Q16" s="1"/>
-      <c r="R16" s="1"/>
-      <c r="S16" s="1"/>
+        <v>4</v>
+      </c>
+      <c r="P16" s="27">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="Q16" s="25"/>
+      <c r="R16" s="25"/>
+      <c r="S16" s="25" t="s">
+        <v>209</v>
+      </c>
       <c r="T16" s="1" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="U16" s="1">
         <v>10</v>
       </c>
       <c r="V16" s="1"/>
-      <c r="W16" s="1">
-        <v>14</v>
-      </c>
-      <c r="X16" s="1">
-        <v>14</v>
-      </c>
-      <c r="Y16" s="1" t="s">
-        <v>114</v>
-      </c>
+      <c r="W16" s="1"/>
+      <c r="X16" s="1"/>
+      <c r="Y16" s="1"/>
       <c r="Z16" s="1">
-        <v>14</v>
-      </c>
-      <c r="AA16" s="1">
+        <v>-10</v>
+      </c>
+      <c r="AA16" s="28">
         <f>IF(ISBLANK(AB16),0, LOOKUP(AB16,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC16/100)</f>
         <v>0</v>
       </c>
       <c r="AB16" s="1"/>
       <c r="AC16" s="1"/>
-      <c r="AD16" s="1"/>
+      <c r="AD16" s="26"/>
       <c r="AE16" s="1" t="s">
         <v>34</v>
       </c>
@@ -6104,35 +6274,33 @@
         <v>34</v>
       </c>
       <c r="AG16" s="1" t="s">
-        <v>113</v>
+        <v>207</v>
       </c>
     </row>
     <row r="17" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A17" s="1">
-        <v>21200003</v>
+        <v>21100014</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>130</v>
-      </c>
+        <v>211</v>
+      </c>
+      <c r="C17" s="1"/>
       <c r="D17" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="D17:D18" si="7">IF(P17&gt;=23,4,IF(AND(P17&gt;=18,P17&lt;23),3,IF(AND(P17&gt;=13,P17&lt;18),2,IF(AND(P17&gt;=8,P17&lt;13),1,0))))</f>
         <v>1</v>
       </c>
       <c r="E17" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F17" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="F17:F18" si="8">D17*50+50</f>
         <v>100</v>
       </c>
       <c r="G17" s="1">
         <v>0</v>
       </c>
       <c r="H17" s="1">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="I17" s="23">
         <v>0</v>
@@ -6147,7 +6315,7 @@
         <v>0</v>
       </c>
       <c r="M17" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N17" s="7">
         <v>0</v>
@@ -6156,12 +6324,14 @@
         <v>0</v>
       </c>
       <c r="P17" s="24">
-        <f t="shared" si="8"/>
-        <v>12.5</v>
-      </c>
-      <c r="Q17" s="1"/>
-      <c r="R17" s="1"/>
-      <c r="S17" s="1"/>
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="Q17" s="25"/>
+      <c r="R17" s="25"/>
+      <c r="S17" s="25" t="s">
+        <v>212</v>
+      </c>
       <c r="T17" s="1" t="s">
         <v>101</v>
       </c>
@@ -6169,23 +6339,19 @@
         <v>10</v>
       </c>
       <c r="V17" s="1"/>
-      <c r="W17" s="1">
-        <v>25</v>
-      </c>
+      <c r="W17" s="1"/>
       <c r="X17" s="1"/>
-      <c r="Y17" s="1" t="s">
-        <v>118</v>
-      </c>
+      <c r="Y17" s="1"/>
       <c r="Z17" s="1">
-        <v>12.5</v>
-      </c>
-      <c r="AA17" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA17" s="28">
         <f>IF(ISBLANK(AB17),0, LOOKUP(AB17,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC17/100)</f>
         <v>0</v>
       </c>
       <c r="AB17" s="1"/>
       <c r="AC17" s="1"/>
-      <c r="AD17" s="1"/>
+      <c r="AD17" s="26"/>
       <c r="AE17" s="1" t="s">
         <v>34</v>
       </c>
@@ -6193,37 +6359,35 @@
         <v>34</v>
       </c>
       <c r="AG17" s="1" t="s">
-        <v>116</v>
+        <v>210</v>
       </c>
     </row>
     <row r="18" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A18" s="1">
-        <v>21200004</v>
+        <v>21100015</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>131</v>
-      </c>
+        <v>214</v>
+      </c>
+      <c r="C18" s="1"/>
       <c r="D18" s="1">
-        <f t="shared" ref="D18" si="9">IF(P18&gt;=23,4,IF(AND(P18&gt;=18,P18&lt;23),3,IF(AND(P18&gt;=13,P18&lt;18),2,IF(AND(P18&gt;=8,P18&lt;13),1,0))))</f>
-        <v>2</v>
+        <f t="shared" si="7"/>
+        <v>1</v>
       </c>
       <c r="E18" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F18" s="1">
-        <f t="shared" si="2"/>
-        <v>150</v>
+        <f t="shared" si="8"/>
+        <v>100</v>
       </c>
       <c r="G18" s="1">
         <v>0</v>
       </c>
       <c r="H18" s="1">
-        <v>0</v>
-      </c>
-      <c r="I18" s="23">
+        <v>11</v>
+      </c>
+      <c r="I18" s="29">
         <v>0</v>
       </c>
       <c r="J18" s="7">
@@ -6244,13 +6408,15 @@
       <c r="O18" s="7">
         <v>0</v>
       </c>
-      <c r="P18" s="24">
-        <f t="shared" ref="P18" si="10">G18+H18+ SUM(I18:O18)*5+Z18+AA18</f>
-        <v>14</v>
-      </c>
-      <c r="Q18" s="1"/>
-      <c r="R18" s="1"/>
-      <c r="S18" s="1"/>
+      <c r="P18" s="27">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="Q18" s="25"/>
+      <c r="R18" s="25"/>
+      <c r="S18" s="25" t="s">
+        <v>215</v>
+      </c>
       <c r="T18" s="1" t="s">
         <v>101</v>
       </c>
@@ -6258,25 +6424,19 @@
         <v>10</v>
       </c>
       <c r="V18" s="1"/>
-      <c r="W18" s="1">
-        <v>14</v>
-      </c>
-      <c r="X18" s="1">
-        <v>14</v>
-      </c>
-      <c r="Y18" s="1" t="s">
-        <v>119</v>
-      </c>
+      <c r="W18" s="1"/>
+      <c r="X18" s="1"/>
+      <c r="Y18" s="1"/>
       <c r="Z18" s="1">
-        <v>14</v>
-      </c>
-      <c r="AA18" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA18" s="28">
         <f>IF(ISBLANK(AB18),0, LOOKUP(AB18,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC18/100)</f>
         <v>0</v>
       </c>
       <c r="AB18" s="1"/>
       <c r="AC18" s="1"/>
-      <c r="AD18" s="1"/>
+      <c r="AD18" s="26"/>
       <c r="AE18" s="1" t="s">
         <v>34</v>
       </c>
@@ -6284,30 +6444,32 @@
         <v>34</v>
       </c>
       <c r="AG18" s="1" t="s">
-        <v>117</v>
+        <v>213</v>
       </c>
     </row>
     <row r="19" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A19" s="1">
-        <v>21300001</v>
+        <v>21200001</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C19" s="1"/>
+        <v>75</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>129</v>
+      </c>
       <c r="D19" s="1">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f t="shared" ref="D19:D29" si="9">IF(P19&gt;=23,4,IF(AND(P19&gt;=18,P19&lt;23),3,IF(AND(P19&gt;=13,P19&lt;18),2,IF(AND(P19&gt;=8,P19&lt;13),1,0))))</f>
+        <v>1</v>
       </c>
       <c r="E19" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F19" s="1">
         <f t="shared" si="2"/>
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="G19" s="1">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H19" s="1">
         <v>0</v>
@@ -6334,13 +6496,11 @@
         <v>0</v>
       </c>
       <c r="P19" s="24">
-        <f t="shared" ref="P19" si="11">G19+H19+ SUM(I19:O19)*5+Z19+AA19</f>
-        <v>5</v>
+        <f t="shared" si="1"/>
+        <v>10</v>
       </c>
       <c r="Q19" s="1"/>
-      <c r="R19" s="1" t="s">
-        <v>197</v>
-      </c>
+      <c r="R19" s="1"/>
       <c r="S19" s="1"/>
       <c r="T19" s="1" t="s">
         <v>18</v>
@@ -6350,10 +6510,14 @@
       </c>
       <c r="V19" s="1"/>
       <c r="W19" s="1"/>
-      <c r="X19" s="1"/>
-      <c r="Y19" s="1"/>
+      <c r="X19" s="1">
+        <v>20</v>
+      </c>
+      <c r="Y19" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="Z19" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AA19" s="1">
         <f>IF(ISBLANK(AB19),0, LOOKUP(AB19,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC19/100)</f>
@@ -6369,30 +6533,32 @@
         <v>34</v>
       </c>
       <c r="AG19" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A20" s="1">
-        <v>21300002</v>
+        <v>21200002</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="C20" s="1"/>
+        <v>120</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>128</v>
+      </c>
       <c r="D20" s="1">
-        <f t="shared" ref="D20:D21" si="12">IF(P20&gt;=23,4,IF(AND(P20&gt;=18,P20&lt;23),3,IF(AND(P20&gt;=13,P20&lt;18),2,IF(AND(P20&gt;=8,P20&lt;13),1,0))))</f>
-        <v>1</v>
+        <f t="shared" ref="D20:D21" si="10">IF(P20&gt;=23,4,IF(AND(P20&gt;=18,P20&lt;23),3,IF(AND(P20&gt;=13,P20&lt;18),2,IF(AND(P20&gt;=8,P20&lt;13),1,0))))</f>
+        <v>2</v>
       </c>
       <c r="E20" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F20" s="1">
         <f t="shared" si="2"/>
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="G20" s="1">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="H20" s="1">
         <v>0</v>
@@ -6419,13 +6585,11 @@
         <v>0</v>
       </c>
       <c r="P20" s="24">
-        <f t="shared" ref="P20:P21" si="13">G20+H20+ SUM(I20:O20)*5+Z20+AA20</f>
-        <v>9</v>
+        <f t="shared" si="1"/>
+        <v>14</v>
       </c>
       <c r="Q20" s="1"/>
-      <c r="R20" s="1" t="s">
-        <v>198</v>
-      </c>
+      <c r="R20" s="1"/>
       <c r="S20" s="1"/>
       <c r="T20" s="1" t="s">
         <v>115</v>
@@ -6434,22 +6598,24 @@
         <v>10</v>
       </c>
       <c r="V20" s="1"/>
-      <c r="W20" s="1"/>
-      <c r="X20" s="1"/>
-      <c r="Y20" s="1"/>
+      <c r="W20" s="1">
+        <v>14</v>
+      </c>
+      <c r="X20" s="1">
+        <v>14</v>
+      </c>
+      <c r="Y20" s="1" t="s">
+        <v>114</v>
+      </c>
       <c r="Z20" s="1">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="AA20" s="1">
         <f>IF(ISBLANK(AB20),0, LOOKUP(AB20,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC20/100)</f>
-        <v>3</v>
-      </c>
-      <c r="AB20" s="1">
-        <v>55510010</v>
-      </c>
-      <c r="AC20" s="1">
-        <v>60</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="AB20" s="1"/>
+      <c r="AC20" s="1"/>
       <c r="AD20" s="1"/>
       <c r="AE20" s="1" t="s">
         <v>34</v>
@@ -6458,30 +6624,32 @@
         <v>34</v>
       </c>
       <c r="AG20" s="1" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
     </row>
     <row r="21" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A21" s="1">
-        <v>21300003</v>
+        <v>21200003</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="C21" s="1"/>
+        <v>121</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>130</v>
+      </c>
       <c r="D21" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="E21" s="1">
         <v>2</v>
-      </c>
-      <c r="E21" s="1">
-        <v>3</v>
       </c>
       <c r="F21" s="1">
         <f t="shared" si="2"/>
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="G21" s="1">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="H21" s="1">
         <v>0</v>
@@ -6502,19 +6670,17 @@
         <v>0</v>
       </c>
       <c r="N21" s="7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O21" s="7">
         <v>0</v>
       </c>
       <c r="P21" s="24">
-        <f t="shared" si="13"/>
-        <v>16</v>
+        <f t="shared" si="1"/>
+        <v>12.5</v>
       </c>
       <c r="Q21" s="1"/>
-      <c r="R21" s="1" t="s">
-        <v>199</v>
-      </c>
+      <c r="R21" s="1"/>
       <c r="S21" s="1"/>
       <c r="T21" s="1" t="s">
         <v>101</v>
@@ -6523,11 +6689,15 @@
         <v>10</v>
       </c>
       <c r="V21" s="1"/>
-      <c r="W21" s="1"/>
+      <c r="W21" s="1">
+        <v>25</v>
+      </c>
       <c r="X21" s="1"/>
-      <c r="Y21" s="1"/>
+      <c r="Y21" s="1" t="s">
+        <v>118</v>
+      </c>
       <c r="Z21" s="1">
-        <v>0</v>
+        <v>12.5</v>
       </c>
       <c r="AA21" s="1">
         <f>IF(ISBLANK(AB21),0, LOOKUP(AB21,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC21/100)</f>
@@ -6543,30 +6713,32 @@
         <v>34</v>
       </c>
       <c r="AG21" s="1" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="22" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A22" s="1">
-        <v>21300004</v>
+        <v>21200004</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="C22" s="1"/>
+        <v>122</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>131</v>
+      </c>
       <c r="D22" s="1">
-        <f t="shared" ref="D22:D23" si="14">IF(P22&gt;=23,4,IF(AND(P22&gt;=18,P22&lt;23),3,IF(AND(P22&gt;=13,P22&lt;18),2,IF(AND(P22&gt;=8,P22&lt;13),1,0))))</f>
+        <f t="shared" ref="D22" si="11">IF(P22&gt;=23,4,IF(AND(P22&gt;=18,P22&lt;23),3,IF(AND(P22&gt;=13,P22&lt;18),2,IF(AND(P22&gt;=8,P22&lt;13),1,0))))</f>
         <v>2</v>
       </c>
       <c r="E22" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F22" s="1">
         <f t="shared" si="2"/>
         <v>150</v>
       </c>
       <c r="G22" s="1">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="H22" s="1">
         <v>0</v>
@@ -6593,13 +6765,11 @@
         <v>0</v>
       </c>
       <c r="P22" s="24">
-        <f t="shared" ref="P22:P23" si="15">G22+H22+ SUM(I22:O22)*5+Z22+AA22</f>
-        <v>17.3</v>
+        <f t="shared" si="1"/>
+        <v>14</v>
       </c>
       <c r="Q22" s="1"/>
-      <c r="R22" s="1" t="s">
-        <v>200</v>
-      </c>
+      <c r="R22" s="1"/>
       <c r="S22" s="1"/>
       <c r="T22" s="1" t="s">
         <v>101</v>
@@ -6608,22 +6778,24 @@
         <v>10</v>
       </c>
       <c r="V22" s="1"/>
-      <c r="W22" s="1"/>
-      <c r="X22" s="1"/>
-      <c r="Y22" s="1"/>
+      <c r="W22" s="1">
+        <v>14</v>
+      </c>
+      <c r="X22" s="1">
+        <v>14</v>
+      </c>
+      <c r="Y22" s="1" t="s">
+        <v>119</v>
+      </c>
       <c r="Z22" s="1">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="AA22" s="1">
         <f>IF(ISBLANK(AB22),0, LOOKUP(AB22,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC22/100)</f>
-        <v>9.3000000000000007</v>
-      </c>
-      <c r="AB22" s="1">
-        <v>55510012</v>
-      </c>
-      <c r="AC22" s="1">
-        <v>15</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="AB22" s="1"/>
+      <c r="AC22" s="1"/>
       <c r="AD22" s="1"/>
       <c r="AE22" s="1" t="s">
         <v>34</v>
@@ -6632,30 +6804,32 @@
         <v>34</v>
       </c>
       <c r="AG22" s="1" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
     </row>
     <row r="23" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A23" s="1">
-        <v>21300005</v>
+        <v>21200005</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="C23" s="1"/>
+        <v>218</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>219</v>
+      </c>
       <c r="D23" s="1">
-        <f t="shared" si="14"/>
-        <v>1</v>
+        <f t="shared" ref="D23:D25" si="12">IF(P23&gt;=23,4,IF(AND(P23&gt;=18,P23&lt;23),3,IF(AND(P23&gt;=13,P23&lt;18),2,IF(AND(P23&gt;=8,P23&lt;13),1,0))))</f>
+        <v>0</v>
       </c>
       <c r="E23" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F23" s="1">
-        <f t="shared" si="2"/>
-        <v>100</v>
+        <f t="shared" ref="F23:F25" si="13">D23*50+50</f>
+        <v>50</v>
       </c>
       <c r="G23" s="1">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="H23" s="1">
         <v>0</v>
@@ -6682,26 +6856,28 @@
         <v>0</v>
       </c>
       <c r="P23" s="24">
-        <f t="shared" si="15"/>
-        <v>12</v>
+        <f t="shared" si="1"/>
+        <v>6</v>
       </c>
       <c r="Q23" s="1"/>
-      <c r="R23" s="1" t="s">
-        <v>199</v>
-      </c>
+      <c r="R23" s="1"/>
       <c r="S23" s="1"/>
       <c r="T23" s="1" t="s">
-        <v>101</v>
+        <v>217</v>
       </c>
       <c r="U23" s="1">
         <v>10</v>
       </c>
       <c r="V23" s="1"/>
       <c r="W23" s="1"/>
-      <c r="X23" s="1"/>
-      <c r="Y23" s="1"/>
+      <c r="X23" s="1">
+        <v>6</v>
+      </c>
+      <c r="Y23" s="26" t="s">
+        <v>239</v>
+      </c>
       <c r="Z23" s="1">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AA23" s="1">
         <f>IF(ISBLANK(AB23),0, LOOKUP(AB23,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC23/100)</f>
@@ -6717,30 +6893,32 @@
         <v>34</v>
       </c>
       <c r="AG23" s="1" t="s">
-        <v>152</v>
+        <v>216</v>
       </c>
     </row>
     <row r="24" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A24" s="1">
-        <v>21300006</v>
+        <v>21200006</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C24" s="1"/>
+        <v>221</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>222</v>
+      </c>
       <c r="D24" s="1">
-        <f t="shared" ref="D24:D25" si="16">IF(P24&gt;=23,4,IF(AND(P24&gt;=18,P24&lt;23),3,IF(AND(P24&gt;=13,P24&lt;18),2,IF(AND(P24&gt;=8,P24&lt;13),1,0))))</f>
-        <v>3</v>
+        <f t="shared" si="12"/>
+        <v>0</v>
       </c>
       <c r="E24" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F24" s="1">
-        <f t="shared" si="2"/>
-        <v>200</v>
+        <f t="shared" si="13"/>
+        <v>50</v>
       </c>
       <c r="G24" s="1">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="H24" s="1">
         <v>0</v>
@@ -6767,13 +6945,11 @@
         <v>0</v>
       </c>
       <c r="P24" s="24">
-        <f t="shared" ref="P24:P25" si="17">G24+H24+ SUM(I24:O24)*5+Z24+AA24</f>
-        <v>20</v>
+        <f t="shared" si="1"/>
+        <v>6</v>
       </c>
       <c r="Q24" s="1"/>
-      <c r="R24" s="1" t="s">
-        <v>200</v>
-      </c>
+      <c r="R24" s="1"/>
       <c r="S24" s="1"/>
       <c r="T24" s="1" t="s">
         <v>101</v>
@@ -6782,11 +6958,15 @@
         <v>10</v>
       </c>
       <c r="V24" s="1"/>
-      <c r="W24" s="1"/>
+      <c r="W24" s="1">
+        <v>6</v>
+      </c>
       <c r="X24" s="1"/>
-      <c r="Y24" s="1"/>
+      <c r="Y24" s="26" t="s">
+        <v>239</v>
+      </c>
       <c r="Z24" s="1">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AA24" s="1">
         <f>IF(ISBLANK(AB24),0, LOOKUP(AB24,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC24/100)</f>
@@ -6802,30 +6982,32 @@
         <v>34</v>
       </c>
       <c r="AG24" s="1" t="s">
-        <v>154</v>
+        <v>220</v>
       </c>
     </row>
     <row r="25" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A25" s="1">
-        <v>21300007</v>
+        <v>21200007</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="C25" s="1"/>
+        <v>223</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>225</v>
+      </c>
       <c r="D25" s="1">
-        <f t="shared" si="16"/>
-        <v>4</v>
+        <f t="shared" si="12"/>
+        <v>1</v>
       </c>
       <c r="E25" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F25" s="1">
-        <f t="shared" si="2"/>
-        <v>250</v>
+        <f t="shared" si="13"/>
+        <v>100</v>
       </c>
       <c r="G25" s="1">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H25" s="1">
         <v>0</v>
@@ -6837,7 +7019,7 @@
         <v>0</v>
       </c>
       <c r="K25" s="7">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="L25" s="7">
         <v>0</v>
@@ -6852,13 +7034,11 @@
         <v>0</v>
       </c>
       <c r="P25" s="24">
-        <f t="shared" si="17"/>
-        <v>30</v>
+        <f t="shared" si="1"/>
+        <v>9</v>
       </c>
       <c r="Q25" s="1"/>
-      <c r="R25" s="1" t="s">
-        <v>203</v>
-      </c>
+      <c r="R25" s="1"/>
       <c r="S25" s="1"/>
       <c r="T25" s="1" t="s">
         <v>101</v>
@@ -6867,11 +7047,17 @@
         <v>10</v>
       </c>
       <c r="V25" s="1"/>
-      <c r="W25" s="1"/>
-      <c r="X25" s="1"/>
-      <c r="Y25" s="1"/>
+      <c r="W25" s="1">
+        <v>12</v>
+      </c>
+      <c r="X25" s="1">
+        <v>6</v>
+      </c>
+      <c r="Y25" s="1" t="s">
+        <v>224</v>
+      </c>
       <c r="Z25" s="1">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AA25" s="1">
         <f>IF(ISBLANK(AB25),0, LOOKUP(AB25,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC25/100)</f>
@@ -6887,30 +7073,32 @@
         <v>34</v>
       </c>
       <c r="AG25" s="1" t="s">
-        <v>156</v>
+        <v>226</v>
       </c>
     </row>
     <row r="26" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A26" s="1">
-        <v>21300008</v>
+        <v>21200008</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="C26" s="1"/>
+        <v>229</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>230</v>
+      </c>
       <c r="D26" s="1">
-        <f t="shared" ref="D26:D27" si="18">IF(P26&gt;=23,4,IF(AND(P26&gt;=18,P26&lt;23),3,IF(AND(P26&gt;=13,P26&lt;18),2,IF(AND(P26&gt;=8,P26&lt;13),1,0))))</f>
-        <v>0</v>
+        <f t="shared" ref="D26:D27" si="14">IF(P26&gt;=23,4,IF(AND(P26&gt;=18,P26&lt;23),3,IF(AND(P26&gt;=13,P26&lt;18),2,IF(AND(P26&gt;=8,P26&lt;13),1,0))))</f>
+        <v>3</v>
       </c>
       <c r="E26" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F26" s="1">
-        <f t="shared" ref="F26:F27" si="19">D26*50+50</f>
-        <v>50</v>
+        <f t="shared" ref="F26:F27" si="15">D26*50+50</f>
+        <v>200</v>
       </c>
       <c r="G26" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H26" s="1">
         <v>0</v>
@@ -6937,13 +7125,11 @@
         <v>0</v>
       </c>
       <c r="P26" s="24">
-        <f t="shared" ref="P26:P27" si="20">G26+H26+ SUM(I26:O26)*5+Z26+AA26</f>
-        <v>1</v>
+        <f t="shared" ref="P26:P27" si="16">G26+H26+ SUM(I26:O26)*5+Z26+AA26</f>
+        <v>18</v>
       </c>
       <c r="Q26" s="1"/>
-      <c r="R26" s="1" t="s">
-        <v>201</v>
-      </c>
+      <c r="R26" s="1"/>
       <c r="S26" s="1"/>
       <c r="T26" s="1" t="s">
         <v>101</v>
@@ -6952,11 +7138,17 @@
         <v>10</v>
       </c>
       <c r="V26" s="1"/>
-      <c r="W26" s="1"/>
-      <c r="X26" s="1"/>
-      <c r="Y26" s="1"/>
+      <c r="W26" s="1">
+        <v>12</v>
+      </c>
+      <c r="X26" s="1">
+        <v>12</v>
+      </c>
+      <c r="Y26" s="1" t="s">
+        <v>228</v>
+      </c>
       <c r="Z26" s="1">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="AA26" s="1">
         <f>IF(ISBLANK(AB26),0, LOOKUP(AB26,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC26/100)</f>
@@ -6972,30 +7164,32 @@
         <v>34</v>
       </c>
       <c r="AG26" s="1" t="s">
-        <v>172</v>
+        <v>227</v>
       </c>
     </row>
     <row r="27" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A27" s="1">
-        <v>21300009</v>
+        <v>21200009</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="C27" s="1"/>
+        <v>234</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>233</v>
+      </c>
       <c r="D27" s="1">
-        <f t="shared" si="18"/>
-        <v>3</v>
+        <f t="shared" si="14"/>
+        <v>2</v>
       </c>
       <c r="E27" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F27" s="1">
-        <f t="shared" si="19"/>
-        <v>200</v>
+        <f t="shared" si="15"/>
+        <v>150</v>
       </c>
       <c r="G27" s="1">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H27" s="1">
         <v>0</v>
@@ -7007,7 +7201,7 @@
         <v>0</v>
       </c>
       <c r="K27" s="7">
-        <v>-4</v>
+        <v>0</v>
       </c>
       <c r="L27" s="7">
         <v>0</v>
@@ -7022,13 +7216,11 @@
         <v>0</v>
       </c>
       <c r="P27" s="24">
-        <f t="shared" si="20"/>
-        <v>20</v>
+        <f t="shared" si="16"/>
+        <v>15</v>
       </c>
       <c r="Q27" s="1"/>
-      <c r="R27" s="1" t="s">
-        <v>202</v>
-      </c>
+      <c r="R27" s="1"/>
       <c r="S27" s="1"/>
       <c r="T27" s="1" t="s">
         <v>101</v>
@@ -7037,22 +7229,24 @@
         <v>10</v>
       </c>
       <c r="V27" s="1"/>
-      <c r="W27" s="1"/>
-      <c r="X27" s="1"/>
-      <c r="Y27" s="1"/>
+      <c r="W27" s="1">
+        <v>10</v>
+      </c>
+      <c r="X27" s="1">
+        <v>10</v>
+      </c>
+      <c r="Y27" s="1" t="s">
+        <v>232</v>
+      </c>
       <c r="Z27" s="1">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AA27" s="1">
         <f>IF(ISBLANK(AB27),0, LOOKUP(AB27,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC27/100)</f>
-        <v>35</v>
-      </c>
-      <c r="AB27" s="1">
-        <v>55100007</v>
-      </c>
-      <c r="AC27" s="1">
-        <v>100</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="AB27" s="1"/>
+      <c r="AC27" s="1"/>
       <c r="AD27" s="1"/>
       <c r="AE27" s="1" t="s">
         <v>34</v>
@@ -7061,577 +7255,641 @@
         <v>34</v>
       </c>
       <c r="AG27" s="1" t="s">
-        <v>178</v>
+        <v>231</v>
       </c>
     </row>
     <row r="28" spans="1:33" x14ac:dyDescent="0.15">
-      <c r="A28">
-        <v>21400001</v>
+      <c r="A28" s="1">
+        <v>21200010</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="C28" s="1"/>
-      <c r="D28" s="22">
-        <f t="shared" ref="D28" si="21">IF(P28&gt;=23,4,IF(AND(P28&gt;=18,P28&lt;23),3,IF(AND(P28&gt;=13,P28&lt;18),2,IF(AND(P28&gt;=8,P28&lt;13),1,0))))</f>
-        <v>0</v>
+        <v>238</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="D28" s="1">
+        <f t="shared" ref="D28" si="17">IF(P28&gt;=23,4,IF(AND(P28&gt;=18,P28&lt;23),3,IF(AND(P28&gt;=13,P28&lt;18),2,IF(AND(P28&gt;=8,P28&lt;13),1,0))))</f>
+        <v>4</v>
       </c>
       <c r="E28" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F28" s="1">
+        <f t="shared" ref="F28" si="18">D28*50+50</f>
+        <v>250</v>
+      </c>
+      <c r="G28" s="1">
+        <v>0</v>
+      </c>
+      <c r="H28" s="1">
+        <v>0</v>
+      </c>
+      <c r="I28" s="23">
+        <v>0</v>
+      </c>
+      <c r="J28" s="7">
+        <v>0</v>
+      </c>
+      <c r="K28" s="7">
+        <v>0</v>
+      </c>
+      <c r="L28" s="7">
+        <v>0</v>
+      </c>
+      <c r="M28" s="7">
+        <v>0</v>
+      </c>
+      <c r="N28" s="7">
+        <v>0</v>
+      </c>
+      <c r="O28" s="7">
+        <v>0</v>
+      </c>
+      <c r="P28" s="24">
+        <f t="shared" ref="P28" si="19">G28+H28+ SUM(I28:O28)*5+Z28+AA28</f>
+        <v>25</v>
+      </c>
+      <c r="Q28" s="1"/>
+      <c r="R28" s="1"/>
+      <c r="S28" s="1"/>
+      <c r="T28" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="U28" s="1">
+        <v>10</v>
+      </c>
+      <c r="V28" s="1"/>
+      <c r="W28" s="1">
+        <v>10</v>
+      </c>
+      <c r="X28" s="1">
+        <v>10</v>
+      </c>
+      <c r="Y28" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="Z28" s="1">
+        <v>25</v>
+      </c>
+      <c r="AA28" s="1">
+        <f>IF(ISBLANK(AB28),0, LOOKUP(AB28,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC28/100)</f>
+        <v>0</v>
+      </c>
+      <c r="AB28" s="1"/>
+      <c r="AC28" s="1"/>
+      <c r="AD28" s="1"/>
+      <c r="AE28" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AF28" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG28" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="29" spans="1:33" x14ac:dyDescent="0.15">
+      <c r="A29" s="1">
+        <v>21300001</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="E29" s="1">
+        <v>3</v>
+      </c>
+      <c r="F29" s="1">
         <f t="shared" si="2"/>
         <v>50</v>
       </c>
-      <c r="G28" s="7">
-        <v>0</v>
-      </c>
-      <c r="H28" s="7">
-        <v>0</v>
-      </c>
-      <c r="I28" s="23">
+      <c r="G29" s="1">
+        <v>5</v>
+      </c>
+      <c r="H29" s="1">
+        <v>0</v>
+      </c>
+      <c r="I29" s="23">
+        <v>0</v>
+      </c>
+      <c r="J29" s="7">
+        <v>0</v>
+      </c>
+      <c r="K29" s="7">
+        <v>0</v>
+      </c>
+      <c r="L29" s="7">
+        <v>0</v>
+      </c>
+      <c r="M29" s="7">
+        <v>0</v>
+      </c>
+      <c r="N29" s="7">
+        <v>0</v>
+      </c>
+      <c r="O29" s="7">
+        <v>0</v>
+      </c>
+      <c r="P29" s="24">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="Q29" s="1"/>
+      <c r="R29" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="S29" s="1"/>
+      <c r="T29" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="U29" s="1">
+        <v>10</v>
+      </c>
+      <c r="V29" s="1"/>
+      <c r="W29" s="1"/>
+      <c r="X29" s="1"/>
+      <c r="Y29" s="1"/>
+      <c r="Z29" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA29" s="1">
+        <f>IF(ISBLANK(AB29),0, LOOKUP(AB29,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC29/100)</f>
+        <v>0</v>
+      </c>
+      <c r="AB29" s="1"/>
+      <c r="AC29" s="1"/>
+      <c r="AD29" s="1"/>
+      <c r="AE29" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AF29" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG29" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="30" spans="1:33" x14ac:dyDescent="0.15">
+      <c r="A30" s="1">
+        <v>21300002</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1">
+        <f t="shared" ref="D30:D31" si="20">IF(P30&gt;=23,4,IF(AND(P30&gt;=18,P30&lt;23),3,IF(AND(P30&gt;=13,P30&lt;18),2,IF(AND(P30&gt;=8,P30&lt;13),1,0))))</f>
         <v>1</v>
       </c>
-      <c r="J28" s="7">
-        <v>0</v>
-      </c>
-      <c r="K28" s="7">
-        <v>0</v>
-      </c>
-      <c r="L28" s="7">
-        <v>0</v>
-      </c>
-      <c r="M28" s="7">
-        <v>0</v>
-      </c>
-      <c r="N28" s="7">
-        <v>0</v>
-      </c>
-      <c r="O28" s="7">
-        <v>0</v>
-      </c>
-      <c r="P28" s="24">
-        <f t="shared" ref="P28" si="22">G28+H28+ SUM(I28:O28)*5+Z28+AA28</f>
-        <v>5</v>
-      </c>
-      <c r="Q28" s="7"/>
-      <c r="R28" s="7"/>
-      <c r="S28" s="7"/>
-      <c r="T28" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="U28">
-        <v>10</v>
-      </c>
-      <c r="Z28">
-        <v>0</v>
-      </c>
-      <c r="AA28">
-        <f>IF(ISBLANK(AB28),0, LOOKUP(AB28,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC28/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AD28" s="12"/>
-      <c r="AE28" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="AF28" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="AG28" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="29" spans="1:33" x14ac:dyDescent="0.15">
-      <c r="A29">
-        <v>21400002</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="C29" s="1"/>
-      <c r="D29" s="22">
-        <f t="shared" ref="D29:D30" si="23">IF(P29&gt;=23,4,IF(AND(P29&gt;=18,P29&lt;23),3,IF(AND(P29&gt;=13,P29&lt;18),2,IF(AND(P29&gt;=8,P29&lt;13),1,0))))</f>
-        <v>1</v>
-      </c>
-      <c r="E29" s="1">
-        <v>4</v>
-      </c>
-      <c r="F29" s="1">
+      <c r="E30" s="1">
+        <v>3</v>
+      </c>
+      <c r="F30" s="1">
         <f t="shared" si="2"/>
         <v>100</v>
       </c>
-      <c r="G29" s="7">
-        <v>0</v>
-      </c>
-      <c r="H29" s="7">
-        <v>0</v>
-      </c>
-      <c r="I29" s="23">
+      <c r="G30" s="1">
+        <v>6</v>
+      </c>
+      <c r="H30" s="1">
+        <v>0</v>
+      </c>
+      <c r="I30" s="23">
+        <v>0</v>
+      </c>
+      <c r="J30" s="7">
+        <v>0</v>
+      </c>
+      <c r="K30" s="7">
+        <v>0</v>
+      </c>
+      <c r="L30" s="7">
+        <v>0</v>
+      </c>
+      <c r="M30" s="7">
+        <v>0</v>
+      </c>
+      <c r="N30" s="7">
+        <v>0</v>
+      </c>
+      <c r="O30" s="7">
+        <v>0</v>
+      </c>
+      <c r="P30" s="24">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="Q30" s="1"/>
+      <c r="R30" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="S30" s="1"/>
+      <c r="T30" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="U30" s="1">
+        <v>10</v>
+      </c>
+      <c r="V30" s="1"/>
+      <c r="W30" s="1"/>
+      <c r="X30" s="1"/>
+      <c r="Y30" s="1"/>
+      <c r="Z30" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA30" s="1">
+        <f>IF(ISBLANK(AB30),0, LOOKUP(AB30,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC30/100)</f>
+        <v>3</v>
+      </c>
+      <c r="AB30" s="1">
+        <v>55510010</v>
+      </c>
+      <c r="AC30" s="1">
+        <v>60</v>
+      </c>
+      <c r="AD30" s="1"/>
+      <c r="AE30" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AF30" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG30" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="31" spans="1:33" x14ac:dyDescent="0.15">
+      <c r="A31" s="1">
+        <v>21300003</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1">
+        <f t="shared" si="20"/>
         <v>2</v>
       </c>
-      <c r="J29" s="7">
-        <v>0</v>
-      </c>
-      <c r="K29" s="7">
-        <v>0</v>
-      </c>
-      <c r="L29" s="7">
-        <v>0</v>
-      </c>
-      <c r="M29" s="7">
-        <v>0</v>
-      </c>
-      <c r="N29" s="7">
-        <v>0</v>
-      </c>
-      <c r="O29" s="7">
-        <v>0</v>
-      </c>
-      <c r="P29" s="24">
-        <f t="shared" ref="P29:P30" si="24">G29+H29+ SUM(I29:O29)*5+Z29+AA29</f>
-        <v>10</v>
-      </c>
-      <c r="Q29" s="7"/>
-      <c r="R29" s="7"/>
-      <c r="S29" s="7"/>
-      <c r="T29" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="U29">
-        <v>10</v>
-      </c>
-      <c r="Z29">
-        <v>0</v>
-      </c>
-      <c r="AA29">
-        <f>IF(ISBLANK(AB29),0, LOOKUP(AB29,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC29/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AD29" s="12"/>
-      <c r="AE29" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="AF29" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="AG29" s="2" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="30" spans="1:33" x14ac:dyDescent="0.15">
-      <c r="A30">
-        <v>21400003</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="C30" s="1"/>
-      <c r="D30" s="22">
-        <f t="shared" si="23"/>
-        <v>2</v>
-      </c>
-      <c r="E30" s="1">
-        <v>4</v>
-      </c>
-      <c r="F30" s="1">
+      <c r="E31" s="1">
+        <v>3</v>
+      </c>
+      <c r="F31" s="1">
         <f t="shared" si="2"/>
         <v>150</v>
       </c>
-      <c r="G30" s="7">
-        <v>0</v>
-      </c>
-      <c r="H30" s="7">
-        <v>0</v>
-      </c>
-      <c r="I30" s="23">
+      <c r="G31" s="1">
+        <v>6</v>
+      </c>
+      <c r="H31" s="1">
+        <v>0</v>
+      </c>
+      <c r="I31" s="23">
+        <v>0</v>
+      </c>
+      <c r="J31" s="7">
+        <v>0</v>
+      </c>
+      <c r="K31" s="7">
+        <v>0</v>
+      </c>
+      <c r="L31" s="7">
+        <v>0</v>
+      </c>
+      <c r="M31" s="7">
+        <v>0</v>
+      </c>
+      <c r="N31" s="7">
+        <v>2</v>
+      </c>
+      <c r="O31" s="7">
+        <v>0</v>
+      </c>
+      <c r="P31" s="24">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="Q31" s="1"/>
+      <c r="R31" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="S31" s="1"/>
+      <c r="T31" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="U31" s="1">
+        <v>10</v>
+      </c>
+      <c r="V31" s="1"/>
+      <c r="W31" s="1"/>
+      <c r="X31" s="1"/>
+      <c r="Y31" s="1"/>
+      <c r="Z31" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA31" s="1">
+        <f>IF(ISBLANK(AB31),0, LOOKUP(AB31,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC31/100)</f>
+        <v>0</v>
+      </c>
+      <c r="AB31" s="1"/>
+      <c r="AC31" s="1"/>
+      <c r="AD31" s="1"/>
+      <c r="AE31" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AF31" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG31" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="32" spans="1:33" x14ac:dyDescent="0.15">
+      <c r="A32" s="1">
+        <v>21300004</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1">
+        <f t="shared" ref="D32:D33" si="21">IF(P32&gt;=23,4,IF(AND(P32&gt;=18,P32&lt;23),3,IF(AND(P32&gt;=13,P32&lt;18),2,IF(AND(P32&gt;=8,P32&lt;13),1,0))))</f>
+        <v>2</v>
+      </c>
+      <c r="E32" s="1">
+        <v>3</v>
+      </c>
+      <c r="F32" s="1">
+        <f t="shared" si="2"/>
+        <v>150</v>
+      </c>
+      <c r="G32" s="1">
+        <v>8</v>
+      </c>
+      <c r="H32" s="1">
+        <v>0</v>
+      </c>
+      <c r="I32" s="23">
+        <v>0</v>
+      </c>
+      <c r="J32" s="7">
+        <v>0</v>
+      </c>
+      <c r="K32" s="7">
+        <v>0</v>
+      </c>
+      <c r="L32" s="7">
+        <v>0</v>
+      </c>
+      <c r="M32" s="7">
+        <v>0</v>
+      </c>
+      <c r="N32" s="7">
+        <v>0</v>
+      </c>
+      <c r="O32" s="7">
+        <v>0</v>
+      </c>
+      <c r="P32" s="24">
+        <f t="shared" si="1"/>
+        <v>17.3</v>
+      </c>
+      <c r="Q32" s="1"/>
+      <c r="R32" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="S32" s="1"/>
+      <c r="T32" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="U32" s="1">
+        <v>10</v>
+      </c>
+      <c r="V32" s="1"/>
+      <c r="W32" s="1"/>
+      <c r="X32" s="1"/>
+      <c r="Y32" s="1"/>
+      <c r="Z32" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA32" s="1">
+        <f>IF(ISBLANK(AB32),0, LOOKUP(AB32,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC32/100)</f>
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="AB32" s="1">
+        <v>55510012</v>
+      </c>
+      <c r="AC32" s="1">
+        <v>15</v>
+      </c>
+      <c r="AD32" s="1"/>
+      <c r="AE32" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AF32" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG32" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="33" spans="1:33" x14ac:dyDescent="0.15">
+      <c r="A33" s="1">
+        <v>21300005</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1">
+        <f t="shared" si="21"/>
         <v>1</v>
       </c>
-      <c r="J30" s="7">
-        <v>0</v>
-      </c>
-      <c r="K30" s="7">
-        <v>0</v>
-      </c>
-      <c r="L30" s="7">
-        <v>0</v>
-      </c>
-      <c r="M30" s="7">
-        <v>0</v>
-      </c>
-      <c r="N30" s="7">
-        <v>0</v>
-      </c>
-      <c r="O30" s="7">
-        <v>0</v>
-      </c>
-      <c r="P30" s="24">
-        <f t="shared" si="24"/>
-        <v>15</v>
-      </c>
-      <c r="Q30" s="7"/>
-      <c r="R30" s="7"/>
-      <c r="S30" s="7"/>
-      <c r="T30" s="12" t="s">
+      <c r="E33" s="1">
+        <v>3</v>
+      </c>
+      <c r="F33" s="1">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="G33" s="1">
+        <v>12</v>
+      </c>
+      <c r="H33" s="1">
+        <v>0</v>
+      </c>
+      <c r="I33" s="23">
+        <v>0</v>
+      </c>
+      <c r="J33" s="7">
+        <v>0</v>
+      </c>
+      <c r="K33" s="7">
+        <v>0</v>
+      </c>
+      <c r="L33" s="7">
+        <v>0</v>
+      </c>
+      <c r="M33" s="7">
+        <v>0</v>
+      </c>
+      <c r="N33" s="7">
+        <v>0</v>
+      </c>
+      <c r="O33" s="7">
+        <v>0</v>
+      </c>
+      <c r="P33" s="24">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="Q33" s="1"/>
+      <c r="R33" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="S33" s="1"/>
+      <c r="T33" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="U30">
+      <c r="U33" s="1">
         <v>10</v>
       </c>
-      <c r="Z30">
-        <v>0</v>
-      </c>
-      <c r="AA30">
-        <f>IF(ISBLANK(AB30),0, LOOKUP(AB30,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC30/100)</f>
-        <v>10</v>
-      </c>
-      <c r="AB30">
-        <v>55110005</v>
-      </c>
-      <c r="AC30">
-        <v>50</v>
-      </c>
-      <c r="AD30" s="12"/>
-      <c r="AE30" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="AF30" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="AG30" s="2" t="s">
-        <v>135</v>
+      <c r="V33" s="1"/>
+      <c r="W33" s="1"/>
+      <c r="X33" s="1"/>
+      <c r="Y33" s="1"/>
+      <c r="Z33" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA33" s="1">
+        <f>IF(ISBLANK(AB33),0, LOOKUP(AB33,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC33/100)</f>
+        <v>0</v>
+      </c>
+      <c r="AB33" s="1"/>
+      <c r="AC33" s="1"/>
+      <c r="AD33" s="1"/>
+      <c r="AE33" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AF33" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG33" s="1" t="s">
+        <v>152</v>
       </c>
     </row>
-    <row r="31" spans="1:33" x14ac:dyDescent="0.15">
-      <c r="A31">
-        <v>21400004</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="C31" s="1"/>
-      <c r="D31" s="22">
-        <f t="shared" ref="D31:D32" si="25">IF(P31&gt;=23,4,IF(AND(P31&gt;=18,P31&lt;23),3,IF(AND(P31&gt;=13,P31&lt;18),2,IF(AND(P31&gt;=8,P31&lt;13),1,0))))</f>
+    <row r="34" spans="1:33" x14ac:dyDescent="0.15">
+      <c r="A34" s="1">
+        <v>21300006</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1">
+        <f t="shared" ref="D34:D35" si="22">IF(P34&gt;=23,4,IF(AND(P34&gt;=18,P34&lt;23),3,IF(AND(P34&gt;=13,P34&lt;18),2,IF(AND(P34&gt;=8,P34&lt;13),1,0))))</f>
         <v>3</v>
       </c>
-      <c r="E31" s="1">
-        <v>4</v>
-      </c>
-      <c r="F31" s="1">
+      <c r="E34" s="1">
+        <v>3</v>
+      </c>
+      <c r="F34" s="1">
         <f t="shared" si="2"/>
         <v>200</v>
       </c>
-      <c r="G31" s="7">
-        <v>0</v>
-      </c>
-      <c r="H31" s="7">
-        <v>0</v>
-      </c>
-      <c r="I31" s="23">
-        <v>4</v>
-      </c>
-      <c r="J31" s="7">
-        <v>0</v>
-      </c>
-      <c r="K31" s="7">
-        <v>0</v>
-      </c>
-      <c r="L31" s="7">
-        <v>0</v>
-      </c>
-      <c r="M31" s="7">
-        <v>0</v>
-      </c>
-      <c r="N31" s="7">
-        <v>0</v>
-      </c>
-      <c r="O31" s="7">
-        <v>0</v>
-      </c>
-      <c r="P31" s="24">
-        <f t="shared" ref="P31:P32" si="26">G31+H31+ SUM(I31:O31)*5+Z31+AA31</f>
+      <c r="G34" s="1">
         <v>20</v>
       </c>
-      <c r="Q31" s="7"/>
-      <c r="R31" s="7"/>
-      <c r="S31" s="7"/>
-      <c r="T31" s="12" t="s">
+      <c r="H34" s="1">
+        <v>0</v>
+      </c>
+      <c r="I34" s="23">
+        <v>0</v>
+      </c>
+      <c r="J34" s="7">
+        <v>0</v>
+      </c>
+      <c r="K34" s="7">
+        <v>0</v>
+      </c>
+      <c r="L34" s="7">
+        <v>0</v>
+      </c>
+      <c r="M34" s="7">
+        <v>0</v>
+      </c>
+      <c r="N34" s="7">
+        <v>0</v>
+      </c>
+      <c r="O34" s="7">
+        <v>0</v>
+      </c>
+      <c r="P34" s="24">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="Q34" s="1"/>
+      <c r="R34" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="S34" s="1"/>
+      <c r="T34" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="U31">
+      <c r="U34" s="1">
         <v>10</v>
       </c>
-      <c r="Z31">
-        <v>0</v>
-      </c>
-      <c r="AA31">
-        <f>IF(ISBLANK(AB31),0, LOOKUP(AB31,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC31/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AD31" s="12"/>
-      <c r="AE31" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="AF31" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="AG31" s="2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="32" spans="1:33" x14ac:dyDescent="0.15">
-      <c r="A32">
-        <v>21400005</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="C32" s="1"/>
-      <c r="D32" s="22">
-        <f t="shared" si="25"/>
-        <v>1</v>
-      </c>
-      <c r="E32" s="1">
-        <v>4</v>
-      </c>
-      <c r="F32" s="1">
-        <f t="shared" ref="F32:F33" si="27">D32*50+50</f>
-        <v>100</v>
-      </c>
-      <c r="G32" s="7">
-        <v>0</v>
-      </c>
-      <c r="H32" s="7">
-        <v>3</v>
-      </c>
-      <c r="I32" s="23">
-        <v>1</v>
-      </c>
-      <c r="J32" s="7">
-        <v>0</v>
-      </c>
-      <c r="K32" s="7">
-        <v>0</v>
-      </c>
-      <c r="L32" s="7">
-        <v>0</v>
-      </c>
-      <c r="M32" s="7">
-        <v>0</v>
-      </c>
-      <c r="N32" s="7">
-        <v>0</v>
-      </c>
-      <c r="O32" s="7">
-        <v>0</v>
-      </c>
-      <c r="P32" s="24">
-        <f t="shared" si="26"/>
-        <v>8</v>
-      </c>
-      <c r="Q32" s="7"/>
-      <c r="R32" s="7"/>
-      <c r="S32" s="7"/>
-      <c r="T32" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="U32">
-        <v>10</v>
-      </c>
-      <c r="Z32">
-        <v>0</v>
-      </c>
-      <c r="AA32">
-        <f>IF(ISBLANK(AB32),0, LOOKUP(AB32,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC32/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AD32" s="12"/>
-      <c r="AE32" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="AF32" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="AG32" s="2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="33" spans="1:33" x14ac:dyDescent="0.15">
-      <c r="A33">
-        <v>21400006</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="C33" s="1"/>
-      <c r="D33" s="22">
-        <f t="shared" ref="D33:D34" si="28">IF(P33&gt;=23,4,IF(AND(P33&gt;=18,P33&lt;23),3,IF(AND(P33&gt;=13,P33&lt;18),2,IF(AND(P33&gt;=8,P33&lt;13),1,0))))</f>
-        <v>2</v>
-      </c>
-      <c r="E33" s="1">
-        <v>4</v>
-      </c>
-      <c r="F33" s="1">
-        <f t="shared" si="27"/>
-        <v>150</v>
-      </c>
-      <c r="G33" s="7">
-        <v>0</v>
-      </c>
-      <c r="H33" s="7">
-        <v>4</v>
-      </c>
-      <c r="I33" s="23">
-        <v>2</v>
-      </c>
-      <c r="J33" s="7">
-        <v>0</v>
-      </c>
-      <c r="K33" s="7">
-        <v>0</v>
-      </c>
-      <c r="L33" s="7">
-        <v>0</v>
-      </c>
-      <c r="M33" s="7">
-        <v>0</v>
-      </c>
-      <c r="N33" s="7">
-        <v>0</v>
-      </c>
-      <c r="O33" s="7">
-        <v>0</v>
-      </c>
-      <c r="P33" s="24">
-        <f t="shared" ref="P33:P34" si="29">G33+H33+ SUM(I33:O33)*5+Z33+AA33</f>
-        <v>14</v>
-      </c>
-      <c r="Q33" s="7"/>
-      <c r="R33" s="7"/>
-      <c r="S33" s="7"/>
-      <c r="T33" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="U33">
-        <v>10</v>
-      </c>
-      <c r="Z33">
-        <v>0</v>
-      </c>
-      <c r="AA33">
-        <f>IF(ISBLANK(AB33),0, LOOKUP(AB33,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC33/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AD33" s="12"/>
-      <c r="AE33" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="AF33" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="AG33" s="2" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="34" spans="1:33" x14ac:dyDescent="0.15">
-      <c r="A34">
-        <v>21400007</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C34" s="1"/>
-      <c r="D34" s="22">
-        <f t="shared" si="28"/>
-        <v>3</v>
-      </c>
-      <c r="E34" s="1">
-        <v>4</v>
-      </c>
-      <c r="F34" s="1">
-        <f t="shared" ref="F34:F35" si="30">D34*50+50</f>
-        <v>200</v>
-      </c>
-      <c r="G34" s="7">
-        <v>0</v>
-      </c>
-      <c r="H34" s="7">
-        <v>0</v>
-      </c>
-      <c r="I34" s="23">
-        <v>0</v>
-      </c>
-      <c r="J34" s="7">
-        <v>0</v>
-      </c>
-      <c r="K34" s="7">
-        <v>0</v>
-      </c>
-      <c r="L34" s="7">
-        <v>0</v>
-      </c>
-      <c r="M34" s="7">
-        <v>4</v>
-      </c>
-      <c r="N34" s="7">
-        <v>0</v>
-      </c>
-      <c r="O34" s="7">
-        <v>0</v>
-      </c>
-      <c r="P34" s="24">
-        <f t="shared" si="29"/>
-        <v>20</v>
-      </c>
-      <c r="Q34" s="7"/>
-      <c r="R34" s="7"/>
-      <c r="S34" s="7"/>
-      <c r="T34" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="U34">
-        <v>10</v>
-      </c>
-      <c r="Z34">
-        <v>0</v>
-      </c>
-      <c r="AA34">
+      <c r="V34" s="1"/>
+      <c r="W34" s="1"/>
+      <c r="X34" s="1"/>
+      <c r="Y34" s="1"/>
+      <c r="Z34" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA34" s="1">
         <f>IF(ISBLANK(AB34),0, LOOKUP(AB34,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC34/100)</f>
         <v>0</v>
       </c>
-      <c r="AD34" s="12"/>
-      <c r="AE34" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="AF34" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="AG34" s="2" t="s">
-        <v>162</v>
+      <c r="AB34" s="1"/>
+      <c r="AC34" s="1"/>
+      <c r="AD34" s="1"/>
+      <c r="AE34" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AF34" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG34" s="1" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="35" spans="1:33" x14ac:dyDescent="0.15">
-      <c r="A35">
-        <v>21400008</v>
+      <c r="A35" s="1">
+        <v>21300007</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="C35" s="1"/>
-      <c r="D35" s="22">
-        <f t="shared" ref="D35:D36" si="31">IF(P35&gt;=23,4,IF(AND(P35&gt;=18,P35&lt;23),3,IF(AND(P35&gt;=13,P35&lt;18),2,IF(AND(P35&gt;=8,P35&lt;13),1,0))))</f>
-        <v>0</v>
+      <c r="D35" s="1">
+        <f t="shared" si="22"/>
+        <v>4</v>
       </c>
       <c r="E35" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F35" s="1">
-        <f t="shared" si="30"/>
-        <v>50</v>
-      </c>
-      <c r="G35" s="7">
-        <v>0</v>
-      </c>
-      <c r="H35" s="7">
+        <f t="shared" si="2"/>
+        <v>250</v>
+      </c>
+      <c r="G35" s="1">
+        <v>5</v>
+      </c>
+      <c r="H35" s="1">
         <v>0</v>
       </c>
       <c r="I35" s="23">
@@ -7641,7 +7899,7 @@
         <v>0</v>
       </c>
       <c r="K35" s="7">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L35" s="7">
         <v>0</v>
@@ -7656,63 +7914,71 @@
         <v>0</v>
       </c>
       <c r="P35" s="24">
-        <f t="shared" ref="P35:P36" si="32">G35+H35+ SUM(I35:O35)*5+Z35+AA35</f>
-        <v>0</v>
-      </c>
-      <c r="Q35" s="7"/>
-      <c r="R35" s="7"/>
-      <c r="S35" s="7"/>
-      <c r="T35" s="12" t="s">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="Q35" s="1"/>
+      <c r="R35" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="S35" s="1"/>
+      <c r="T35" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="U35">
+      <c r="U35" s="1">
         <v>10</v>
       </c>
-      <c r="Z35">
-        <v>0</v>
-      </c>
-      <c r="AA35">
+      <c r="V35" s="1"/>
+      <c r="W35" s="1"/>
+      <c r="X35" s="1"/>
+      <c r="Y35" s="1"/>
+      <c r="Z35" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA35" s="1">
         <f>IF(ISBLANK(AB35),0, LOOKUP(AB35,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC35/100)</f>
         <v>0</v>
       </c>
-      <c r="AD35" s="12"/>
-      <c r="AE35" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="AF35" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="AG35" s="2" t="s">
-        <v>164</v>
+      <c r="AB35" s="1"/>
+      <c r="AC35" s="1"/>
+      <c r="AD35" s="1"/>
+      <c r="AE35" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AF35" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG35" s="1" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="36" spans="1:33" x14ac:dyDescent="0.15">
-      <c r="A36">
-        <v>21400009</v>
+      <c r="A36" s="1">
+        <v>21300008</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="C36" s="1"/>
-      <c r="D36" s="22">
-        <f t="shared" si="31"/>
-        <v>2</v>
+      <c r="D36" s="1">
+        <f t="shared" ref="D36:D37" si="23">IF(P36&gt;=23,4,IF(AND(P36&gt;=18,P36&lt;23),3,IF(AND(P36&gt;=13,P36&lt;18),2,IF(AND(P36&gt;=8,P36&lt;13),1,0))))</f>
+        <v>0</v>
       </c>
       <c r="E36" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F36" s="1">
-        <f t="shared" ref="F36:F37" si="33">D36*50+50</f>
-        <v>150</v>
-      </c>
-      <c r="G36" s="7">
-        <v>0</v>
-      </c>
-      <c r="H36" s="7">
-        <v>3</v>
+        <f t="shared" ref="F36:F37" si="24">D36*50+50</f>
+        <v>50</v>
+      </c>
+      <c r="G36" s="1">
+        <v>1</v>
+      </c>
+      <c r="H36" s="1">
+        <v>0</v>
       </c>
       <c r="I36" s="23">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J36" s="7">
         <v>0</v>
@@ -7733,69 +7999,77 @@
         <v>0</v>
       </c>
       <c r="P36" s="24">
-        <f t="shared" si="32"/>
-        <v>13</v>
-      </c>
-      <c r="Q36" s="7"/>
-      <c r="R36" s="7"/>
-      <c r="S36" s="7"/>
-      <c r="T36" s="12" t="s">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="Q36" s="1"/>
+      <c r="R36" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="S36" s="1"/>
+      <c r="T36" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="U36">
+      <c r="U36" s="1">
         <v>10</v>
       </c>
-      <c r="Z36">
-        <v>0</v>
-      </c>
-      <c r="AA36">
+      <c r="V36" s="1"/>
+      <c r="W36" s="1"/>
+      <c r="X36" s="1"/>
+      <c r="Y36" s="1"/>
+      <c r="Z36" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA36" s="1">
         <f>IF(ISBLANK(AB36),0, LOOKUP(AB36,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC36/100)</f>
         <v>0</v>
       </c>
-      <c r="AD36" s="12"/>
-      <c r="AE36" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="AF36" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="AG36" s="2" t="s">
-        <v>166</v>
+      <c r="AB36" s="1"/>
+      <c r="AC36" s="1"/>
+      <c r="AD36" s="1"/>
+      <c r="AE36" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AF36" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG36" s="1" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="37" spans="1:33" x14ac:dyDescent="0.15">
-      <c r="A37">
-        <v>21400010</v>
+      <c r="A37" s="1">
+        <v>21300009</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="C37" s="1"/>
-      <c r="D37" s="22">
-        <f t="shared" ref="D37:D38" si="34">IF(P37&gt;=23,4,IF(AND(P37&gt;=18,P37&lt;23),3,IF(AND(P37&gt;=13,P37&lt;18),2,IF(AND(P37&gt;=8,P37&lt;13),1,0))))</f>
-        <v>2</v>
+      <c r="D37" s="1">
+        <f t="shared" si="23"/>
+        <v>3</v>
       </c>
       <c r="E37" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F37" s="1">
-        <f t="shared" si="33"/>
-        <v>150</v>
-      </c>
-      <c r="G37" s="7">
-        <v>0</v>
-      </c>
-      <c r="H37" s="7">
+        <f t="shared" si="24"/>
+        <v>200</v>
+      </c>
+      <c r="G37" s="1">
+        <v>5</v>
+      </c>
+      <c r="H37" s="1">
         <v>0</v>
       </c>
       <c r="I37" s="23">
         <v>0</v>
       </c>
       <c r="J37" s="7">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K37" s="7">
-        <v>0</v>
+        <v>-4</v>
       </c>
       <c r="L37" s="7">
         <v>0</v>
@@ -7810,91 +8084,103 @@
         <v>0</v>
       </c>
       <c r="P37" s="24">
-        <f t="shared" ref="P37:P38" si="35">G37+H37+ SUM(I37:O37)*5+Z37+AA37</f>
-        <v>15</v>
-      </c>
-      <c r="Q37" s="7"/>
-      <c r="R37" s="7"/>
-      <c r="S37" s="7"/>
-      <c r="T37" s="12" t="s">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="Q37" s="1"/>
+      <c r="R37" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="S37" s="1"/>
+      <c r="T37" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="U37">
+      <c r="U37" s="1">
         <v>10</v>
       </c>
-      <c r="Z37">
-        <v>0</v>
-      </c>
-      <c r="AA37">
+      <c r="V37" s="1"/>
+      <c r="W37" s="1"/>
+      <c r="X37" s="1"/>
+      <c r="Y37" s="1"/>
+      <c r="Z37" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA37" s="1">
         <f>IF(ISBLANK(AB37),0, LOOKUP(AB37,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC37/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AD37" s="12"/>
-      <c r="AE37" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="AF37" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="AG37" s="2" t="s">
-        <v>168</v>
+        <v>35</v>
+      </c>
+      <c r="AB37" s="1">
+        <v>55100007</v>
+      </c>
+      <c r="AC37" s="1">
+        <v>100</v>
+      </c>
+      <c r="AD37" s="1"/>
+      <c r="AE37" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AF37" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG37" s="1" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="38" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A38">
-        <v>21400011</v>
+        <v>21400001</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>171</v>
+        <v>133</v>
       </c>
       <c r="C38" s="1"/>
       <c r="D38" s="22">
-        <f t="shared" si="34"/>
-        <v>4</v>
+        <f t="shared" ref="D38" si="25">IF(P38&gt;=23,4,IF(AND(P38&gt;=18,P38&lt;23),3,IF(AND(P38&gt;=13,P38&lt;18),2,IF(AND(P38&gt;=8,P38&lt;13),1,0))))</f>
+        <v>0</v>
       </c>
       <c r="E38" s="1">
         <v>4</v>
       </c>
       <c r="F38" s="1">
-        <f t="shared" ref="F38" si="36">D38*50+50</f>
-        <v>250</v>
+        <f t="shared" si="2"/>
+        <v>50</v>
       </c>
       <c r="G38" s="7">
         <v>0</v>
       </c>
       <c r="H38" s="7">
+        <v>0</v>
+      </c>
+      <c r="I38" s="23">
+        <v>1</v>
+      </c>
+      <c r="J38" s="7">
+        <v>0</v>
+      </c>
+      <c r="K38" s="7">
+        <v>0</v>
+      </c>
+      <c r="L38" s="7">
+        <v>0</v>
+      </c>
+      <c r="M38" s="7">
+        <v>0</v>
+      </c>
+      <c r="N38" s="7">
+        <v>0</v>
+      </c>
+      <c r="O38" s="7">
+        <v>0</v>
+      </c>
+      <c r="P38" s="24">
+        <f t="shared" si="1"/>
         <v>5</v>
-      </c>
-      <c r="I38" s="23">
-        <v>3</v>
-      </c>
-      <c r="J38" s="7">
-        <v>0</v>
-      </c>
-      <c r="K38" s="7">
-        <v>0</v>
-      </c>
-      <c r="L38" s="7">
-        <v>0</v>
-      </c>
-      <c r="M38" s="7">
-        <v>2</v>
-      </c>
-      <c r="N38" s="7">
-        <v>0</v>
-      </c>
-      <c r="O38" s="7">
-        <v>0</v>
-      </c>
-      <c r="P38" s="24">
-        <f t="shared" si="35"/>
-        <v>30</v>
       </c>
       <c r="Q38" s="7"/>
       <c r="R38" s="7"/>
       <c r="S38" s="7"/>
       <c r="T38" s="12" t="s">
-        <v>101</v>
+        <v>18</v>
       </c>
       <c r="U38">
         <v>10</v>
@@ -7914,23 +8200,23 @@
         <v>34</v>
       </c>
       <c r="AG38" s="2" t="s">
-        <v>170</v>
+        <v>79</v>
       </c>
     </row>
     <row r="39" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A39">
-        <v>21500001</v>
+        <v>21400002</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>80</v>
+        <v>134</v>
       </c>
       <c r="C39" s="1"/>
       <c r="D39" s="22">
-        <f t="shared" ref="D39" si="37">IF(P39&gt;=23,4,IF(AND(P39&gt;=18,P39&lt;23),3,IF(AND(P39&gt;=13,P39&lt;18),2,IF(AND(P39&gt;=8,P39&lt;13),1,0))))</f>
+        <f t="shared" ref="D39:D40" si="26">IF(P39&gt;=23,4,IF(AND(P39&gt;=18,P39&lt;23),3,IF(AND(P39&gt;=13,P39&lt;18),2,IF(AND(P39&gt;=8,P39&lt;13),1,0))))</f>
         <v>1</v>
       </c>
       <c r="E39" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F39" s="1">
         <f t="shared" si="2"/>
@@ -7943,7 +8229,7 @@
         <v>0</v>
       </c>
       <c r="I39" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J39" s="7">
         <v>0</v>
@@ -7964,22 +8250,20 @@
         <v>0</v>
       </c>
       <c r="P39" s="24">
-        <f t="shared" ref="P39" si="38">G39+H39+ SUM(I39:O39)*5+Z39+AA39</f>
+        <f t="shared" ref="P39:P56" si="27">G39+H39+ SUM(I39:O39)*5+Z39+AA39</f>
         <v>10</v>
       </c>
-      <c r="Q39" s="7">
-        <v>5</v>
-      </c>
+      <c r="Q39" s="7"/>
       <c r="R39" s="7"/>
       <c r="S39" s="7"/>
       <c r="T39" s="12" t="s">
-        <v>78</v>
+        <v>18</v>
       </c>
       <c r="U39">
         <v>10</v>
       </c>
       <c r="Z39">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="AA39">
         <f>IF(ISBLANK(AB39),0, LOOKUP(AB39,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC39/100)</f>
@@ -7993,27 +8277,27 @@
         <v>34</v>
       </c>
       <c r="AG39" s="2" t="s">
-        <v>81</v>
+        <v>132</v>
       </c>
     </row>
     <row r="40" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A40">
-        <v>21500002</v>
+        <v>21400003</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C40" s="1"/>
       <c r="D40" s="22">
-        <f t="shared" ref="D40:D41" si="39">IF(P40&gt;=23,4,IF(AND(P40&gt;=18,P40&lt;23),3,IF(AND(P40&gt;=13,P40&lt;18),2,IF(AND(P40&gt;=8,P40&lt;13),1,0))))</f>
-        <v>1</v>
+        <f t="shared" si="26"/>
+        <v>2</v>
       </c>
       <c r="E40" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F40" s="1">
         <f t="shared" si="2"/>
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="G40" s="7">
         <v>0</v>
@@ -8022,10 +8306,10 @@
         <v>0</v>
       </c>
       <c r="I40" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J40" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K40" s="7">
         <v>0</v>
@@ -8043,24 +8327,30 @@
         <v>0</v>
       </c>
       <c r="P40" s="24">
-        <f t="shared" ref="P40:P41" si="40">G40+H40+ SUM(I40:O40)*5+Z40+AA40</f>
-        <v>10</v>
+        <f t="shared" si="27"/>
+        <v>15</v>
       </c>
       <c r="Q40" s="7"/>
       <c r="R40" s="7"/>
       <c r="S40" s="7"/>
       <c r="T40" s="12" t="s">
-        <v>138</v>
+        <v>101</v>
       </c>
       <c r="U40">
         <v>10</v>
       </c>
       <c r="Z40">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="AA40">
         <f>IF(ISBLANK(AB40),0, LOOKUP(AB40,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC40/100)</f>
-        <v>0</v>
+        <v>10</v>
+      </c>
+      <c r="AB40">
+        <v>55110005</v>
+      </c>
+      <c r="AC40">
+        <v>50</v>
       </c>
       <c r="AD40" s="12"/>
       <c r="AE40" s="12" t="s">
@@ -8070,27 +8360,27 @@
         <v>34</v>
       </c>
       <c r="AG40" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="41" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A41">
-        <v>21500003</v>
+        <v>21400004</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C41" s="1"/>
       <c r="D41" s="22">
-        <f t="shared" si="39"/>
-        <v>1</v>
+        <f t="shared" ref="D41:D42" si="28">IF(P41&gt;=23,4,IF(AND(P41&gt;=18,P41&lt;23),3,IF(AND(P41&gt;=13,P41&lt;18),2,IF(AND(P41&gt;=8,P41&lt;13),1,0))))</f>
+        <v>3</v>
       </c>
       <c r="E41" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F41" s="1">
         <f t="shared" si="2"/>
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="G41" s="7">
         <v>0</v>
@@ -8099,7 +8389,7 @@
         <v>0</v>
       </c>
       <c r="I41" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J41" s="7">
         <v>0</v>
@@ -8108,7 +8398,7 @@
         <v>0</v>
       </c>
       <c r="L41" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M41" s="7">
         <v>0</v>
@@ -8120,22 +8410,20 @@
         <v>0</v>
       </c>
       <c r="P41" s="24">
-        <f t="shared" si="40"/>
-        <v>11</v>
-      </c>
-      <c r="Q41" s="7">
-        <v>6</v>
-      </c>
+        <f t="shared" si="27"/>
+        <v>20</v>
+      </c>
+      <c r="Q41" s="7"/>
       <c r="R41" s="7"/>
       <c r="S41" s="7"/>
       <c r="T41" s="12" t="s">
-        <v>144</v>
+        <v>101</v>
       </c>
       <c r="U41">
         <v>10</v>
       </c>
       <c r="Z41">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="AA41">
         <f>IF(ISBLANK(AB41),0, LOOKUP(AB41,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC41/100)</f>
@@ -8149,36 +8437,36 @@
         <v>34</v>
       </c>
       <c r="AG41" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="42" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A42">
-        <v>21500004</v>
+        <v>21400005</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>146</v>
+        <v>159</v>
       </c>
       <c r="C42" s="1"/>
       <c r="D42" s="22">
-        <f t="shared" ref="D42:D43" si="41">IF(P42&gt;=23,4,IF(AND(P42&gt;=18,P42&lt;23),3,IF(AND(P42&gt;=13,P42&lt;18),2,IF(AND(P42&gt;=8,P42&lt;13),1,0))))</f>
+        <f t="shared" si="28"/>
         <v>1</v>
       </c>
       <c r="E42" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F42" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="F42:F43" si="29">D42*50+50</f>
         <v>100</v>
       </c>
       <c r="G42" s="7">
         <v>0</v>
       </c>
       <c r="H42" s="7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I42" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J42" s="7">
         <v>0</v>
@@ -8199,14 +8487,14 @@
         <v>0</v>
       </c>
       <c r="P42" s="24">
-        <f t="shared" ref="P42:P43" si="42">G42+H42+ SUM(I42:O42)*5+Z42+AA42</f>
+        <f t="shared" si="27"/>
         <v>8</v>
       </c>
       <c r="Q42" s="7"/>
       <c r="R42" s="7"/>
       <c r="S42" s="7"/>
       <c r="T42" s="12" t="s">
-        <v>78</v>
+        <v>101</v>
       </c>
       <c r="U42">
         <v>10</v>
@@ -8216,13 +8504,7 @@
       </c>
       <c r="AA42">
         <f>IF(ISBLANK(AB42),0, LOOKUP(AB42,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC42/100)</f>
-        <v>4</v>
-      </c>
-      <c r="AB42">
-        <v>55990108</v>
-      </c>
-      <c r="AC42">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="AD42" s="12"/>
       <c r="AE42" s="12" t="s">
@@ -8232,36 +8514,36 @@
         <v>34</v>
       </c>
       <c r="AG42" s="2" t="s">
-        <v>145</v>
+        <v>158</v>
       </c>
     </row>
     <row r="43" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A43">
-        <v>21500005</v>
+        <v>21400006</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>149</v>
+        <v>161</v>
       </c>
       <c r="C43" s="1"/>
       <c r="D43" s="22">
-        <f t="shared" si="41"/>
+        <f t="shared" ref="D43:D44" si="30">IF(P43&gt;=23,4,IF(AND(P43&gt;=18,P43&lt;23),3,IF(AND(P43&gt;=13,P43&lt;18),2,IF(AND(P43&gt;=8,P43&lt;13),1,0))))</f>
         <v>2</v>
       </c>
       <c r="E43" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F43" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="29"/>
         <v>150</v>
       </c>
       <c r="G43" s="7">
         <v>0</v>
       </c>
       <c r="H43" s="7">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I43" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J43" s="7">
         <v>0</v>
@@ -8279,23 +8561,23 @@
         <v>0</v>
       </c>
       <c r="O43" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P43" s="24">
-        <f t="shared" si="42"/>
-        <v>15</v>
+        <f t="shared" si="27"/>
+        <v>14</v>
       </c>
       <c r="Q43" s="7"/>
       <c r="R43" s="7"/>
       <c r="S43" s="7"/>
       <c r="T43" s="12" t="s">
-        <v>148</v>
+        <v>101</v>
       </c>
       <c r="U43">
         <v>10</v>
       </c>
       <c r="Z43">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="AA43">
         <f>IF(ISBLANK(AB43),0, LOOKUP(AB43,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC43/100)</f>
@@ -8309,27 +8591,27 @@
         <v>34</v>
       </c>
       <c r="AG43" s="2" t="s">
-        <v>147</v>
+        <v>160</v>
       </c>
     </row>
     <row r="44" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A44">
-        <v>21500006</v>
+        <v>21400007</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>151</v>
+        <v>163</v>
       </c>
       <c r="C44" s="1"/>
       <c r="D44" s="22">
-        <f t="shared" ref="D44:D45" si="43">IF(P44&gt;=23,4,IF(AND(P44&gt;=18,P44&lt;23),3,IF(AND(P44&gt;=13,P44&lt;18),2,IF(AND(P44&gt;=8,P44&lt;13),1,0))))</f>
-        <v>2</v>
+        <f t="shared" si="30"/>
+        <v>3</v>
       </c>
       <c r="E44" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F44" s="1">
-        <f t="shared" si="2"/>
-        <v>150</v>
+        <f t="shared" ref="F44:F45" si="31">D44*50+50</f>
+        <v>200</v>
       </c>
       <c r="G44" s="7">
         <v>0</v>
@@ -8350,7 +8632,7 @@
         <v>0</v>
       </c>
       <c r="M44" s="7">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="N44" s="7">
         <v>0</v>
@@ -8359,14 +8641,14 @@
         <v>0</v>
       </c>
       <c r="P44" s="24">
-        <f t="shared" ref="P44:P45" si="44">G44+H44+ SUM(I44:O44)*5+Z44+AA44</f>
-        <v>15</v>
+        <f t="shared" si="27"/>
+        <v>20</v>
       </c>
       <c r="Q44" s="7"/>
       <c r="R44" s="7"/>
       <c r="S44" s="7"/>
       <c r="T44" s="12" t="s">
-        <v>78</v>
+        <v>101</v>
       </c>
       <c r="U44">
         <v>10</v>
@@ -8376,13 +8658,7 @@
       </c>
       <c r="AA44">
         <f>IF(ISBLANK(AB44),0, LOOKUP(AB44,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC44/100)</f>
-        <v>15</v>
-      </c>
-      <c r="AB44">
-        <v>55990109</v>
-      </c>
-      <c r="AC44">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="AD44" s="12"/>
       <c r="AE44" s="12" t="s">
@@ -8392,27 +8668,27 @@
         <v>34</v>
       </c>
       <c r="AG44" s="2" t="s">
-        <v>150</v>
+        <v>162</v>
       </c>
     </row>
     <row r="45" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A45">
-        <v>21500007</v>
+        <v>21400008</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="C45" s="1"/>
       <c r="D45" s="22">
-        <f t="shared" si="43"/>
-        <v>1</v>
+        <f t="shared" ref="D45:D46" si="32">IF(P45&gt;=23,4,IF(AND(P45&gt;=18,P45&lt;23),3,IF(AND(P45&gt;=13,P45&lt;18),2,IF(AND(P45&gt;=8,P45&lt;13),1,0))))</f>
+        <v>0</v>
       </c>
       <c r="E45" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F45" s="1">
-        <f t="shared" ref="F45:F46" si="45">D45*50+50</f>
-        <v>100</v>
+        <f t="shared" si="31"/>
+        <v>50</v>
       </c>
       <c r="G45" s="7">
         <v>0</v>
@@ -8442,20 +8718,20 @@
         <v>0</v>
       </c>
       <c r="P45" s="24">
-        <f t="shared" si="44"/>
-        <v>8</v>
+        <f t="shared" si="27"/>
+        <v>0</v>
       </c>
       <c r="Q45" s="7"/>
       <c r="R45" s="7"/>
       <c r="S45" s="7"/>
       <c r="T45" s="12" t="s">
-        <v>175</v>
+        <v>101</v>
       </c>
       <c r="U45">
         <v>10</v>
       </c>
       <c r="Z45">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AA45">
         <f>IF(ISBLANK(AB45),0, LOOKUP(AB45,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC45/100)</f>
@@ -8469,36 +8745,36 @@
         <v>34</v>
       </c>
       <c r="AG45" s="2" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
     </row>
     <row r="46" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A46">
-        <v>21500008</v>
+        <v>21400009</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>181</v>
+        <v>167</v>
       </c>
       <c r="C46" s="1"/>
       <c r="D46" s="22">
-        <f t="shared" ref="D46" si="46">IF(P46&gt;=23,4,IF(AND(P46&gt;=18,P46&lt;23),3,IF(AND(P46&gt;=13,P46&lt;18),2,IF(AND(P46&gt;=8,P46&lt;13),1,0))))</f>
+        <f t="shared" si="32"/>
+        <v>2</v>
+      </c>
+      <c r="E46" s="1">
         <v>4</v>
       </c>
-      <c r="E46" s="1">
-        <v>5</v>
-      </c>
       <c r="F46" s="1">
-        <f t="shared" si="45"/>
-        <v>250</v>
+        <f t="shared" ref="F46:F47" si="33">D46*50+50</f>
+        <v>150</v>
       </c>
       <c r="G46" s="7">
         <v>0</v>
       </c>
       <c r="H46" s="7">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I46" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J46" s="7">
         <v>0</v>
@@ -8507,7 +8783,7 @@
         <v>0</v>
       </c>
       <c r="L46" s="7">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M46" s="7">
         <v>0</v>
@@ -8519,14 +8795,14 @@
         <v>0</v>
       </c>
       <c r="P46" s="24">
-        <f t="shared" ref="P46" si="47">G46+H46+ SUM(I46:O46)*5+Z46+AA46</f>
-        <v>25</v>
+        <f t="shared" si="27"/>
+        <v>13</v>
       </c>
       <c r="Q46" s="7"/>
       <c r="R46" s="7"/>
       <c r="S46" s="7"/>
       <c r="T46" s="12" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="U46">
         <v>10</v>
@@ -8536,13 +8812,7 @@
       </c>
       <c r="AA46">
         <f>IF(ISBLANK(AB46),0, LOOKUP(AB46,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC46/100)</f>
-        <v>10</v>
-      </c>
-      <c r="AB46">
-        <v>55110003</v>
-      </c>
-      <c r="AC46">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="AD46" s="12"/>
       <c r="AE46" s="12" t="s">
@@ -8552,25 +8822,912 @@
         <v>34</v>
       </c>
       <c r="AG46" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="47" spans="1:33" x14ac:dyDescent="0.15">
+      <c r="A47">
+        <v>21400010</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C47" s="1"/>
+      <c r="D47" s="22">
+        <f t="shared" ref="D47:D48" si="34">IF(P47&gt;=23,4,IF(AND(P47&gt;=18,P47&lt;23),3,IF(AND(P47&gt;=13,P47&lt;18),2,IF(AND(P47&gt;=8,P47&lt;13),1,0))))</f>
+        <v>2</v>
+      </c>
+      <c r="E47" s="1">
+        <v>4</v>
+      </c>
+      <c r="F47" s="1">
+        <f t="shared" si="33"/>
+        <v>150</v>
+      </c>
+      <c r="G47" s="7">
+        <v>0</v>
+      </c>
+      <c r="H47" s="7">
+        <v>0</v>
+      </c>
+      <c r="I47" s="23">
+        <v>0</v>
+      </c>
+      <c r="J47" s="7">
+        <v>3</v>
+      </c>
+      <c r="K47" s="7">
+        <v>0</v>
+      </c>
+      <c r="L47" s="7">
+        <v>0</v>
+      </c>
+      <c r="M47" s="7">
+        <v>0</v>
+      </c>
+      <c r="N47" s="7">
+        <v>0</v>
+      </c>
+      <c r="O47" s="7">
+        <v>0</v>
+      </c>
+      <c r="P47" s="24">
+        <f t="shared" si="27"/>
+        <v>15</v>
+      </c>
+      <c r="Q47" s="7"/>
+      <c r="R47" s="7"/>
+      <c r="S47" s="7"/>
+      <c r="T47" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="U47">
+        <v>10</v>
+      </c>
+      <c r="Z47">
+        <v>0</v>
+      </c>
+      <c r="AA47">
+        <f>IF(ISBLANK(AB47),0, LOOKUP(AB47,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC47/100)</f>
+        <v>0</v>
+      </c>
+      <c r="AD47" s="12"/>
+      <c r="AE47" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="AF47" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG47" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="48" spans="1:33" x14ac:dyDescent="0.15">
+      <c r="A48">
+        <v>21400011</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C48" s="1"/>
+      <c r="D48" s="22">
+        <f t="shared" si="34"/>
+        <v>4</v>
+      </c>
+      <c r="E48" s="1">
+        <v>4</v>
+      </c>
+      <c r="F48" s="1">
+        <f t="shared" ref="F48" si="35">D48*50+50</f>
+        <v>250</v>
+      </c>
+      <c r="G48" s="7">
+        <v>0</v>
+      </c>
+      <c r="H48" s="7">
+        <v>5</v>
+      </c>
+      <c r="I48" s="23">
+        <v>3</v>
+      </c>
+      <c r="J48" s="7">
+        <v>0</v>
+      </c>
+      <c r="K48" s="7">
+        <v>0</v>
+      </c>
+      <c r="L48" s="7">
+        <v>0</v>
+      </c>
+      <c r="M48" s="7">
+        <v>2</v>
+      </c>
+      <c r="N48" s="7">
+        <v>0</v>
+      </c>
+      <c r="O48" s="7">
+        <v>0</v>
+      </c>
+      <c r="P48" s="24">
+        <f t="shared" si="27"/>
+        <v>30</v>
+      </c>
+      <c r="Q48" s="7"/>
+      <c r="R48" s="7"/>
+      <c r="S48" s="7"/>
+      <c r="T48" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="U48">
+        <v>10</v>
+      </c>
+      <c r="Z48">
+        <v>0</v>
+      </c>
+      <c r="AA48">
+        <f>IF(ISBLANK(AB48),0, LOOKUP(AB48,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC48/100)</f>
+        <v>0</v>
+      </c>
+      <c r="AD48" s="12"/>
+      <c r="AE48" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="AF48" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG48" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="49" spans="1:33" x14ac:dyDescent="0.15">
+      <c r="A49">
+        <v>21500001</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C49" s="1"/>
+      <c r="D49" s="22">
+        <f t="shared" ref="D49" si="36">IF(P49&gt;=23,4,IF(AND(P49&gt;=18,P49&lt;23),3,IF(AND(P49&gt;=13,P49&lt;18),2,IF(AND(P49&gt;=8,P49&lt;13),1,0))))</f>
+        <v>1</v>
+      </c>
+      <c r="E49" s="1">
+        <v>5</v>
+      </c>
+      <c r="F49" s="1">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="G49" s="7">
+        <v>0</v>
+      </c>
+      <c r="H49" s="7">
+        <v>0</v>
+      </c>
+      <c r="I49" s="23">
+        <v>0</v>
+      </c>
+      <c r="J49" s="7">
+        <v>0</v>
+      </c>
+      <c r="K49" s="7">
+        <v>0</v>
+      </c>
+      <c r="L49" s="7">
+        <v>0</v>
+      </c>
+      <c r="M49" s="7">
+        <v>0</v>
+      </c>
+      <c r="N49" s="7">
+        <v>0</v>
+      </c>
+      <c r="O49" s="7">
+        <v>0</v>
+      </c>
+      <c r="P49" s="24">
+        <f t="shared" si="27"/>
+        <v>10</v>
+      </c>
+      <c r="Q49" s="7">
+        <v>5</v>
+      </c>
+      <c r="R49" s="7"/>
+      <c r="S49" s="7"/>
+      <c r="T49" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="U49">
+        <v>10</v>
+      </c>
+      <c r="Z49">
+        <v>10</v>
+      </c>
+      <c r="AA49">
+        <f>IF(ISBLANK(AB49),0, LOOKUP(AB49,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC49/100)</f>
+        <v>0</v>
+      </c>
+      <c r="AD49" s="12"/>
+      <c r="AE49" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="AF49" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG49" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="50" spans="1:33" x14ac:dyDescent="0.15">
+      <c r="A50">
+        <v>21500002</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C50" s="1"/>
+      <c r="D50" s="22">
+        <f t="shared" ref="D50:D51" si="37">IF(P50&gt;=23,4,IF(AND(P50&gt;=18,P50&lt;23),3,IF(AND(P50&gt;=13,P50&lt;18),2,IF(AND(P50&gt;=8,P50&lt;13),1,0))))</f>
+        <v>1</v>
+      </c>
+      <c r="E50" s="1">
+        <v>5</v>
+      </c>
+      <c r="F50" s="1">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="G50" s="7">
+        <v>0</v>
+      </c>
+      <c r="H50" s="7">
+        <v>0</v>
+      </c>
+      <c r="I50" s="23">
+        <v>0</v>
+      </c>
+      <c r="J50" s="7">
+        <v>1</v>
+      </c>
+      <c r="K50" s="7">
+        <v>0</v>
+      </c>
+      <c r="L50" s="7">
+        <v>0</v>
+      </c>
+      <c r="M50" s="7">
+        <v>0</v>
+      </c>
+      <c r="N50" s="7">
+        <v>0</v>
+      </c>
+      <c r="O50" s="7">
+        <v>0</v>
+      </c>
+      <c r="P50" s="24">
+        <f t="shared" si="27"/>
+        <v>10</v>
+      </c>
+      <c r="Q50" s="7"/>
+      <c r="R50" s="7"/>
+      <c r="S50" s="7"/>
+      <c r="T50" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="U50">
+        <v>10</v>
+      </c>
+      <c r="Z50">
+        <v>5</v>
+      </c>
+      <c r="AA50">
+        <f>IF(ISBLANK(AB50),0, LOOKUP(AB50,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC50/100)</f>
+        <v>0</v>
+      </c>
+      <c r="AD50" s="12"/>
+      <c r="AE50" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="AF50" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG50" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="51" spans="1:33" x14ac:dyDescent="0.15">
+      <c r="A51">
+        <v>21500003</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C51" s="1"/>
+      <c r="D51" s="22">
+        <f t="shared" si="37"/>
+        <v>1</v>
+      </c>
+      <c r="E51" s="1">
+        <v>5</v>
+      </c>
+      <c r="F51" s="1">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="G51" s="7">
+        <v>0</v>
+      </c>
+      <c r="H51" s="7">
+        <v>0</v>
+      </c>
+      <c r="I51" s="23">
+        <v>0</v>
+      </c>
+      <c r="J51" s="7">
+        <v>0</v>
+      </c>
+      <c r="K51" s="7">
+        <v>0</v>
+      </c>
+      <c r="L51" s="7">
+        <v>1</v>
+      </c>
+      <c r="M51" s="7">
+        <v>0</v>
+      </c>
+      <c r="N51" s="7">
+        <v>0</v>
+      </c>
+      <c r="O51" s="7">
+        <v>0</v>
+      </c>
+      <c r="P51" s="24">
+        <f t="shared" si="27"/>
+        <v>11</v>
+      </c>
+      <c r="Q51" s="7"/>
+      <c r="R51" s="7"/>
+      <c r="S51" s="7"/>
+      <c r="T51" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="U51">
+        <v>10</v>
+      </c>
+      <c r="Z51">
+        <v>6</v>
+      </c>
+      <c r="AA51">
+        <f>IF(ISBLANK(AB51),0, LOOKUP(AB51,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC51/100)</f>
+        <v>0</v>
+      </c>
+      <c r="AD51" s="12"/>
+      <c r="AE51" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="AF51" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG51" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="52" spans="1:33" x14ac:dyDescent="0.15">
+      <c r="A52">
+        <v>21500004</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C52" s="1"/>
+      <c r="D52" s="22">
+        <f t="shared" ref="D52:D53" si="38">IF(P52&gt;=23,4,IF(AND(P52&gt;=18,P52&lt;23),3,IF(AND(P52&gt;=13,P52&lt;18),2,IF(AND(P52&gt;=8,P52&lt;13),1,0))))</f>
+        <v>1</v>
+      </c>
+      <c r="E52" s="1">
+        <v>5</v>
+      </c>
+      <c r="F52" s="1">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="G52" s="7">
+        <v>0</v>
+      </c>
+      <c r="H52" s="7">
+        <v>4</v>
+      </c>
+      <c r="I52" s="23">
+        <v>0</v>
+      </c>
+      <c r="J52" s="7">
+        <v>0</v>
+      </c>
+      <c r="K52" s="7">
+        <v>0</v>
+      </c>
+      <c r="L52" s="7">
+        <v>0</v>
+      </c>
+      <c r="M52" s="7">
+        <v>0</v>
+      </c>
+      <c r="N52" s="7">
+        <v>0</v>
+      </c>
+      <c r="O52" s="7">
+        <v>0</v>
+      </c>
+      <c r="P52" s="24">
+        <f t="shared" si="27"/>
+        <v>8</v>
+      </c>
+      <c r="Q52" s="7"/>
+      <c r="R52" s="7"/>
+      <c r="S52" s="7"/>
+      <c r="T52" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="U52">
+        <v>10</v>
+      </c>
+      <c r="Z52">
+        <v>0</v>
+      </c>
+      <c r="AA52">
+        <f>IF(ISBLANK(AB52),0, LOOKUP(AB52,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC52/100)</f>
+        <v>4</v>
+      </c>
+      <c r="AB52">
+        <v>55990108</v>
+      </c>
+      <c r="AC52">
+        <v>100</v>
+      </c>
+      <c r="AD52" s="12"/>
+      <c r="AE52" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="AF52" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG52" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="53" spans="1:33" x14ac:dyDescent="0.15">
+      <c r="A53">
+        <v>21500005</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C53" s="1"/>
+      <c r="D53" s="22">
+        <f t="shared" si="38"/>
+        <v>2</v>
+      </c>
+      <c r="E53" s="1">
+        <v>5</v>
+      </c>
+      <c r="F53" s="1">
+        <f t="shared" si="2"/>
+        <v>150</v>
+      </c>
+      <c r="G53" s="7">
+        <v>0</v>
+      </c>
+      <c r="H53" s="7">
+        <v>0</v>
+      </c>
+      <c r="I53" s="23">
+        <v>0</v>
+      </c>
+      <c r="J53" s="7">
+        <v>0</v>
+      </c>
+      <c r="K53" s="7">
+        <v>0</v>
+      </c>
+      <c r="L53" s="7">
+        <v>0</v>
+      </c>
+      <c r="M53" s="7">
+        <v>0</v>
+      </c>
+      <c r="N53" s="7">
+        <v>0</v>
+      </c>
+      <c r="O53" s="7">
+        <v>1</v>
+      </c>
+      <c r="P53" s="24">
+        <f t="shared" si="27"/>
+        <v>15</v>
+      </c>
+      <c r="Q53" s="7"/>
+      <c r="R53" s="7"/>
+      <c r="S53" s="7"/>
+      <c r="T53" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="U53">
+        <v>10</v>
+      </c>
+      <c r="Z53">
+        <v>10</v>
+      </c>
+      <c r="AA53">
+        <f>IF(ISBLANK(AB53),0, LOOKUP(AB53,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC53/100)</f>
+        <v>0</v>
+      </c>
+      <c r="AD53" s="12"/>
+      <c r="AE53" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="AF53" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG53" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="54" spans="1:33" x14ac:dyDescent="0.15">
+      <c r="A54">
+        <v>21500006</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C54" s="1"/>
+      <c r="D54" s="22">
+        <f t="shared" ref="D54:D55" si="39">IF(P54&gt;=23,4,IF(AND(P54&gt;=18,P54&lt;23),3,IF(AND(P54&gt;=13,P54&lt;18),2,IF(AND(P54&gt;=8,P54&lt;13),1,0))))</f>
+        <v>2</v>
+      </c>
+      <c r="E54" s="1">
+        <v>5</v>
+      </c>
+      <c r="F54" s="1">
+        <f t="shared" si="2"/>
+        <v>150</v>
+      </c>
+      <c r="G54" s="7">
+        <v>0</v>
+      </c>
+      <c r="H54" s="7">
+        <v>0</v>
+      </c>
+      <c r="I54" s="23">
+        <v>0</v>
+      </c>
+      <c r="J54" s="7">
+        <v>0</v>
+      </c>
+      <c r="K54" s="7">
+        <v>0</v>
+      </c>
+      <c r="L54" s="7">
+        <v>0</v>
+      </c>
+      <c r="M54" s="7">
+        <v>0</v>
+      </c>
+      <c r="N54" s="7">
+        <v>0</v>
+      </c>
+      <c r="O54" s="7">
+        <v>0</v>
+      </c>
+      <c r="P54" s="24">
+        <f t="shared" si="27"/>
+        <v>15</v>
+      </c>
+      <c r="Q54" s="7"/>
+      <c r="R54" s="7"/>
+      <c r="S54" s="7"/>
+      <c r="T54" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="U54">
+        <v>10</v>
+      </c>
+      <c r="Z54">
+        <v>0</v>
+      </c>
+      <c r="AA54">
+        <f>IF(ISBLANK(AB54),0, LOOKUP(AB54,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC54/100)</f>
+        <v>15</v>
+      </c>
+      <c r="AB54">
+        <v>55990109</v>
+      </c>
+      <c r="AC54">
+        <v>100</v>
+      </c>
+      <c r="AD54" s="12"/>
+      <c r="AE54" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="AF54" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG54" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="55" spans="1:33" x14ac:dyDescent="0.15">
+      <c r="A55">
+        <v>21500007</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C55" s="1"/>
+      <c r="D55" s="22">
+        <f t="shared" si="39"/>
+        <v>1</v>
+      </c>
+      <c r="E55" s="1">
+        <v>5</v>
+      </c>
+      <c r="F55" s="1">
+        <f t="shared" ref="F55:F56" si="40">D55*50+50</f>
+        <v>100</v>
+      </c>
+      <c r="G55" s="7">
+        <v>0</v>
+      </c>
+      <c r="H55" s="7">
+        <v>0</v>
+      </c>
+      <c r="I55" s="23">
+        <v>0</v>
+      </c>
+      <c r="J55" s="7">
+        <v>0</v>
+      </c>
+      <c r="K55" s="7">
+        <v>0</v>
+      </c>
+      <c r="L55" s="7">
+        <v>0</v>
+      </c>
+      <c r="M55" s="7">
+        <v>0</v>
+      </c>
+      <c r="N55" s="7">
+        <v>0</v>
+      </c>
+      <c r="O55" s="7">
+        <v>0</v>
+      </c>
+      <c r="P55" s="24">
+        <f t="shared" si="27"/>
+        <v>8</v>
+      </c>
+      <c r="Q55" s="7"/>
+      <c r="R55" s="7"/>
+      <c r="S55" s="7"/>
+      <c r="T55" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="U55">
+        <v>10</v>
+      </c>
+      <c r="Z55">
+        <v>8</v>
+      </c>
+      <c r="AA55">
+        <f>IF(ISBLANK(AB55),0, LOOKUP(AB55,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC55/100)</f>
+        <v>0</v>
+      </c>
+      <c r="AD55" s="12"/>
+      <c r="AE55" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="AF55" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG55" s="2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="56" spans="1:33" x14ac:dyDescent="0.15">
+      <c r="A56">
+        <v>21500008</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C56" s="1"/>
+      <c r="D56" s="22">
+        <f t="shared" ref="D56:D57" si="41">IF(P56&gt;=23,4,IF(AND(P56&gt;=18,P56&lt;23),3,IF(AND(P56&gt;=13,P56&lt;18),2,IF(AND(P56&gt;=8,P56&lt;13),1,0))))</f>
+        <v>4</v>
+      </c>
+      <c r="E56" s="1">
+        <v>5</v>
+      </c>
+      <c r="F56" s="1">
+        <f t="shared" si="40"/>
+        <v>250</v>
+      </c>
+      <c r="G56" s="7">
+        <v>0</v>
+      </c>
+      <c r="H56" s="7">
+        <v>0</v>
+      </c>
+      <c r="I56" s="23">
+        <v>0</v>
+      </c>
+      <c r="J56" s="7">
+        <v>0</v>
+      </c>
+      <c r="K56" s="7">
+        <v>0</v>
+      </c>
+      <c r="L56" s="7">
+        <v>3</v>
+      </c>
+      <c r="M56" s="7">
+        <v>0</v>
+      </c>
+      <c r="N56" s="7">
+        <v>0</v>
+      </c>
+      <c r="O56" s="7">
+        <v>0</v>
+      </c>
+      <c r="P56" s="24">
+        <f t="shared" si="27"/>
+        <v>25</v>
+      </c>
+      <c r="Q56" s="7"/>
+      <c r="R56" s="7"/>
+      <c r="S56" s="7"/>
+      <c r="T56" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="U56">
+        <v>10</v>
+      </c>
+      <c r="Z56">
+        <v>0</v>
+      </c>
+      <c r="AA56">
+        <f>IF(ISBLANK(AB56),0, LOOKUP(AB56,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC56/100)</f>
+        <v>10</v>
+      </c>
+      <c r="AB56">
+        <v>55110003</v>
+      </c>
+      <c r="AC56">
+        <v>40</v>
+      </c>
+      <c r="AD56" s="12"/>
+      <c r="AE56" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="AF56" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG56" s="2" t="s">
         <v>180</v>
+      </c>
+    </row>
+    <row r="57" spans="1:33" x14ac:dyDescent="0.15">
+      <c r="A57">
+        <v>21500009</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="C57" s="1"/>
+      <c r="D57" s="22">
+        <f t="shared" si="41"/>
+        <v>1</v>
+      </c>
+      <c r="E57" s="1">
+        <v>5</v>
+      </c>
+      <c r="F57" s="1">
+        <f t="shared" ref="F57" si="42">D57*50+50</f>
+        <v>100</v>
+      </c>
+      <c r="G57" s="7">
+        <v>0</v>
+      </c>
+      <c r="H57" s="7">
+        <v>0</v>
+      </c>
+      <c r="I57" s="23">
+        <v>0</v>
+      </c>
+      <c r="J57" s="7">
+        <v>0</v>
+      </c>
+      <c r="K57" s="7">
+        <v>0</v>
+      </c>
+      <c r="L57" s="7">
+        <v>0</v>
+      </c>
+      <c r="M57" s="7">
+        <v>0</v>
+      </c>
+      <c r="N57" s="7">
+        <v>0</v>
+      </c>
+      <c r="O57" s="7">
+        <v>0</v>
+      </c>
+      <c r="P57" s="24">
+        <f t="shared" ref="P57" si="43">G57+H57+ SUM(I57:O57)*5+Z57+AA57</f>
+        <v>10</v>
+      </c>
+      <c r="Q57" s="7"/>
+      <c r="R57" s="7"/>
+      <c r="S57" s="7"/>
+      <c r="T57" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="U57">
+        <v>10</v>
+      </c>
+      <c r="V57">
+        <v>31100001</v>
+      </c>
+      <c r="Z57">
+        <v>10</v>
+      </c>
+      <c r="AA57">
+        <f>IF(ISBLANK(AB57),0, LOOKUP(AB57,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC57/100)</f>
+        <v>0</v>
+      </c>
+      <c r="AD57" s="12"/>
+      <c r="AE57" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="AF57" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG57" s="2" t="s">
+        <v>240</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="D4:D46">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThanOrEqual">
+  <conditionalFormatting sqref="D4:D24 D26 D28:D57">
+    <cfRule type="cellIs" dxfId="31" priority="6" operator="greaterThanOrEqual">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="7" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="8" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="9" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="10" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D25 D27">
+    <cfRule type="cellIs" dxfId="26" priority="1" operator="greaterThanOrEqual">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="25" priority="2" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="3" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="23" priority="4" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="5" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
add some new equips.and fix bug of equip compose showing
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Equip.xlsx
+++ b/ConfigData/Xlsx/Equip.xlsx
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="246">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -958,6 +958,20 @@
   </si>
   <si>
     <t>护盾发生器</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>jianzhu10</t>
+  </si>
+  <si>
+    <t>猎手大厅</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>jianzhu11</t>
+  </si>
+  <si>
+    <t>传送阵</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -4467,8 +4481,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:AG57" totalsRowShown="0">
-  <autoFilter ref="A3:AG57"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:AG59" totalsRowShown="0">
+  <autoFilter ref="A3:AG59"/>
   <sortState ref="A4:AG38">
     <sortCondition ref="A3:A38"/>
   </sortState>
@@ -4840,10 +4854,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG57"/>
+  <dimension ref="A1:AG59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -9631,7 +9645,7 @@
         <v>5</v>
       </c>
       <c r="F57" s="1">
-        <f t="shared" ref="F57" si="42">D57*50+50</f>
+        <f t="shared" ref="F57:F58" si="42">D57*50+50</f>
         <v>100</v>
       </c>
       <c r="G57" s="7">
@@ -9695,9 +9709,169 @@
         <v>240</v>
       </c>
     </row>
+    <row r="58" spans="1:33" x14ac:dyDescent="0.15">
+      <c r="A58">
+        <v>21500010</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="C58" s="1"/>
+      <c r="D58" s="22">
+        <f t="shared" ref="D58:D59" si="44">IF(P58&gt;=23,4,IF(AND(P58&gt;=18,P58&lt;23),3,IF(AND(P58&gt;=13,P58&lt;18),2,IF(AND(P58&gt;=8,P58&lt;13),1,0))))</f>
+        <v>2</v>
+      </c>
+      <c r="E58" s="1">
+        <v>5</v>
+      </c>
+      <c r="F58" s="1">
+        <f t="shared" si="42"/>
+        <v>150</v>
+      </c>
+      <c r="G58" s="7">
+        <v>0</v>
+      </c>
+      <c r="H58" s="7">
+        <v>0</v>
+      </c>
+      <c r="I58" s="23">
+        <v>0</v>
+      </c>
+      <c r="J58" s="7">
+        <v>0</v>
+      </c>
+      <c r="K58" s="7">
+        <v>0</v>
+      </c>
+      <c r="L58" s="7">
+        <v>0</v>
+      </c>
+      <c r="M58" s="7">
+        <v>0</v>
+      </c>
+      <c r="N58" s="7">
+        <v>0</v>
+      </c>
+      <c r="O58" s="7">
+        <v>0</v>
+      </c>
+      <c r="P58" s="24">
+        <f t="shared" ref="P58" si="45">G58+H58+ SUM(I58:O58)*5+Z58+AA58</f>
+        <v>15</v>
+      </c>
+      <c r="Q58" s="7"/>
+      <c r="R58" s="7"/>
+      <c r="S58" s="7"/>
+      <c r="T58" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="U58">
+        <v>10</v>
+      </c>
+      <c r="V58">
+        <v>31100002</v>
+      </c>
+      <c r="Z58">
+        <v>15</v>
+      </c>
+      <c r="AA58">
+        <f>IF(ISBLANK(AB58),0, LOOKUP(AB58,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC58/100)</f>
+        <v>0</v>
+      </c>
+      <c r="AD58" s="12"/>
+      <c r="AE58" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="AF58" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG58" s="2" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="59" spans="1:33" x14ac:dyDescent="0.15">
+      <c r="A59">
+        <v>21500011</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="C59" s="1"/>
+      <c r="D59" s="22">
+        <f t="shared" si="44"/>
+        <v>4</v>
+      </c>
+      <c r="E59" s="1">
+        <v>5</v>
+      </c>
+      <c r="F59" s="1">
+        <f t="shared" ref="F59" si="46">D59*50+50</f>
+        <v>250</v>
+      </c>
+      <c r="G59" s="7">
+        <v>0</v>
+      </c>
+      <c r="H59" s="7">
+        <v>0</v>
+      </c>
+      <c r="I59" s="23">
+        <v>0</v>
+      </c>
+      <c r="J59" s="7">
+        <v>0</v>
+      </c>
+      <c r="K59" s="7">
+        <v>0</v>
+      </c>
+      <c r="L59" s="7">
+        <v>0</v>
+      </c>
+      <c r="M59" s="7">
+        <v>0</v>
+      </c>
+      <c r="N59" s="7">
+        <v>0</v>
+      </c>
+      <c r="O59" s="7">
+        <v>0</v>
+      </c>
+      <c r="P59" s="24">
+        <f t="shared" ref="P59" si="47">G59+H59+ SUM(I59:O59)*5+Z59+AA59</f>
+        <v>25</v>
+      </c>
+      <c r="Q59" s="7"/>
+      <c r="R59" s="7"/>
+      <c r="S59" s="7"/>
+      <c r="T59" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="U59">
+        <v>10</v>
+      </c>
+      <c r="V59">
+        <v>31100003</v>
+      </c>
+      <c r="Z59">
+        <v>25</v>
+      </c>
+      <c r="AA59">
+        <f>IF(ISBLANK(AB59),0, LOOKUP(AB59,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AC59/100)</f>
+        <v>0</v>
+      </c>
+      <c r="AD59" s="12"/>
+      <c r="AE59" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="AF59" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG59" s="2" t="s">
+        <v>244</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="D4:D24 D26 D28:D57">
+  <conditionalFormatting sqref="D4:D24 D26 D28:D59">
     <cfRule type="cellIs" dxfId="31" priority="6" operator="greaterThanOrEqual">
       <formula>5</formula>
     </cfRule>

</xml_diff>

<commit_message>
split the LiveMonster to 2 files. with one do the act with excel script
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Equip.xlsx
+++ b/ConfigData/Xlsx/Equip.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18067"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TOMClassic\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -410,10 +410,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>m.IsRace("Human")</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>描述</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -495,10 +491,6 @@
     <t>qizhi2</t>
   </si>
   <si>
-    <t>m.IsRace("Undead")</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>0;0;0</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -509,14 +501,6 @@
     <t>qizhi4</t>
   </si>
   <si>
-    <t>m.IsRace("Orc")</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>m.IsRace("Spirit")</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>鬼怪旗帜</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -893,10 +877,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>m.IsRace("Beast")</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>提升我方野兽12%攻击和6%最大生命值</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -908,10 +888,6 @@
     <t>qizhi8</t>
   </si>
   <si>
-    <t>m.IsRace("Machine") || m.IsRace("Element")</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>科学旗帜</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -923,10 +899,6 @@
     <t>qizhi9</t>
   </si>
   <si>
-    <t>m.IsRace("Totem") || m.IsRace("Element")</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>提升我方图腾和元素单位10%攻击和最大生命值</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -973,6 +945,27 @@
   <si>
     <t>传送阵</t>
     <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>m.Action.IsRace("Human")</t>
+  </si>
+  <si>
+    <t>m.Action.IsRace("Undead")</t>
+  </si>
+  <si>
+    <t>m.Action.IsRace("Orc")</t>
+  </si>
+  <si>
+    <t>m.Action.IsRace("Spirit")</t>
+  </si>
+  <si>
+    <t>m.Action.IsRace("Beast")</t>
+  </si>
+  <si>
+    <t>m.Action.IsRace("Machine") || m.Action.IsRace("Element")</t>
+  </si>
+  <si>
+    <t>m.Action.IsRace("Totem") || m.Action.IsRace("Element")</t>
   </si>
 </sst>
 </file>
@@ -3685,7 +3678,6 @@
           <cell r="A162">
             <v>55900028</v>
           </cell>
-          <cell r="Y162"/>
         </row>
         <row r="163">
           <cell r="A163">
@@ -4856,8 +4848,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C56" sqref="C56"/>
+    <sheetView tabSelected="1" topLeftCell="I7" workbookViewId="0">
+      <selection activeCell="W16" sqref="W16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -4891,7 +4883,7 @@
         <v>3</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>4</v>
@@ -4936,7 +4928,7 @@
         <v>45</v>
       </c>
       <c r="R1" s="16" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="S1" s="16" t="s">
         <v>69</v>
@@ -4992,7 +4984,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>0</v>
@@ -5037,7 +5029,7 @@
         <v>0</v>
       </c>
       <c r="R2" s="17" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="S2" s="17" t="s">
         <v>70</v>
@@ -5093,7 +5085,7 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
@@ -5138,7 +5130,7 @@
         <v>26</v>
       </c>
       <c r="R3" s="18" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="S3" s="18" t="s">
         <v>71</v>
@@ -5276,7 +5268,7 @@
         <v>21100002</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1">
@@ -5324,7 +5316,7 @@
       <c r="Q5" s="25"/>
       <c r="R5" s="25"/>
       <c r="S5" s="25" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="T5" s="1" t="s">
         <v>18</v>
@@ -5353,7 +5345,7 @@
         <v>34</v>
       </c>
       <c r="AG5" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.15">
@@ -5361,7 +5353,7 @@
         <v>21100003</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1">
@@ -5409,7 +5401,7 @@
       <c r="Q6" s="25"/>
       <c r="R6" s="25"/>
       <c r="S6" s="25" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="T6" s="1" t="s">
         <v>18</v>
@@ -5438,7 +5430,7 @@
         <v>34</v>
       </c>
       <c r="AG6" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.15">
@@ -5446,7 +5438,7 @@
         <v>21100004</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1">
@@ -5494,10 +5486,10 @@
       <c r="Q7" s="25"/>
       <c r="R7" s="25"/>
       <c r="S7" s="25" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="T7" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="U7" s="1">
         <v>10</v>
@@ -5523,7 +5515,7 @@
         <v>34</v>
       </c>
       <c r="AG7" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="8" spans="1:33" x14ac:dyDescent="0.15">
@@ -5531,7 +5523,7 @@
         <v>21100005</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1">
@@ -5579,10 +5571,10 @@
       <c r="Q8" s="25"/>
       <c r="R8" s="25"/>
       <c r="S8" s="25" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="T8" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="U8" s="1">
         <v>10</v>
@@ -5608,7 +5600,7 @@
         <v>34</v>
       </c>
       <c r="AG8" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" spans="1:33" x14ac:dyDescent="0.15">
@@ -5616,7 +5608,7 @@
         <v>21100006</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1">
@@ -5664,10 +5656,10 @@
       <c r="Q9" s="25"/>
       <c r="R9" s="25"/>
       <c r="S9" s="25" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="T9" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="U9" s="1">
         <v>10</v>
@@ -5693,7 +5685,7 @@
         <v>34</v>
       </c>
       <c r="AG9" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.15">
@@ -5701,7 +5693,7 @@
         <v>21100007</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1">
@@ -5749,10 +5741,10 @@
       <c r="Q10" s="25"/>
       <c r="R10" s="25"/>
       <c r="S10" s="25" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="T10" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="U10" s="1">
         <v>10</v>
@@ -5778,7 +5770,7 @@
         <v>34</v>
       </c>
       <c r="AG10" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.15">
@@ -5786,7 +5778,7 @@
         <v>21100008</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1">
@@ -5834,10 +5826,10 @@
       <c r="Q11" s="25"/>
       <c r="R11" s="25"/>
       <c r="S11" s="25" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="T11" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="U11" s="1">
         <v>10</v>
@@ -5863,7 +5855,7 @@
         <v>34</v>
       </c>
       <c r="AG11" s="1" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.15">
@@ -5871,7 +5863,7 @@
         <v>21100009</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1">
@@ -5919,10 +5911,10 @@
       <c r="Q12" s="25"/>
       <c r="R12" s="25"/>
       <c r="S12" s="25" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="T12" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="U12" s="1">
         <v>10</v>
@@ -5948,7 +5940,7 @@
         <v>34</v>
       </c>
       <c r="AG12" s="1" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.15">
@@ -5956,7 +5948,7 @@
         <v>21100010</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1">
@@ -6004,10 +5996,10 @@
       <c r="Q13" s="25"/>
       <c r="R13" s="25"/>
       <c r="S13" s="25" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="T13" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="U13" s="1">
         <v>10</v>
@@ -6033,7 +6025,7 @@
         <v>34</v>
       </c>
       <c r="AG13" s="1" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
     </row>
     <row r="14" spans="1:33" x14ac:dyDescent="0.15">
@@ -6041,7 +6033,7 @@
         <v>21100011</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1">
@@ -6089,10 +6081,10 @@
       <c r="Q14" s="25"/>
       <c r="R14" s="25"/>
       <c r="S14" s="25" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="T14" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="U14" s="1">
         <v>10</v>
@@ -6118,7 +6110,7 @@
         <v>34</v>
       </c>
       <c r="AG14" s="1" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
     </row>
     <row r="15" spans="1:33" x14ac:dyDescent="0.15">
@@ -6126,7 +6118,7 @@
         <v>21100012</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1">
@@ -6174,10 +6166,10 @@
       <c r="Q15" s="25"/>
       <c r="R15" s="25"/>
       <c r="S15" s="25" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="T15" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="U15" s="1">
         <v>10</v>
@@ -6203,7 +6195,7 @@
         <v>34</v>
       </c>
       <c r="AG15" s="1" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
     <row r="16" spans="1:33" x14ac:dyDescent="0.15">
@@ -6211,7 +6203,7 @@
         <v>21100013</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1">
@@ -6259,10 +6251,10 @@
       <c r="Q16" s="25"/>
       <c r="R16" s="25"/>
       <c r="S16" s="25" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="T16" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="U16" s="1">
         <v>10</v>
@@ -6288,7 +6280,7 @@
         <v>34</v>
       </c>
       <c r="AG16" s="1" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
     </row>
     <row r="17" spans="1:33" x14ac:dyDescent="0.15">
@@ -6296,7 +6288,7 @@
         <v>21100014</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1">
@@ -6344,10 +6336,10 @@
       <c r="Q17" s="25"/>
       <c r="R17" s="25"/>
       <c r="S17" s="25" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="T17" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="U17" s="1">
         <v>10</v>
@@ -6373,7 +6365,7 @@
         <v>34</v>
       </c>
       <c r="AG17" s="1" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="18" spans="1:33" x14ac:dyDescent="0.15">
@@ -6381,7 +6373,7 @@
         <v>21100015</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1">
@@ -6429,10 +6421,10 @@
       <c r="Q18" s="25"/>
       <c r="R18" s="25"/>
       <c r="S18" s="25" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="T18" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="U18" s="1">
         <v>10</v>
@@ -6458,7 +6450,7 @@
         <v>34</v>
       </c>
       <c r="AG18" s="1" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="19" spans="1:33" x14ac:dyDescent="0.15">
@@ -6469,7 +6461,7 @@
         <v>75</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D19" s="1">
         <f t="shared" ref="D19:D29" si="9">IF(P19&gt;=23,4,IF(AND(P19&gt;=18,P19&lt;23),3,IF(AND(P19&gt;=13,P19&lt;18),2,IF(AND(P19&gt;=8,P19&lt;13),1,0))))</f>
@@ -6528,7 +6520,7 @@
         <v>20</v>
       </c>
       <c r="Y19" s="1" t="s">
-        <v>91</v>
+        <v>239</v>
       </c>
       <c r="Z19" s="1">
         <v>10</v>
@@ -6555,10 +6547,10 @@
         <v>21200002</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="D20" s="1">
         <f t="shared" ref="D20:D21" si="10">IF(P20&gt;=23,4,IF(AND(P20&gt;=18,P20&lt;23),3,IF(AND(P20&gt;=13,P20&lt;18),2,IF(AND(P20&gt;=8,P20&lt;13),1,0))))</f>
@@ -6606,7 +6598,7 @@
       <c r="R20" s="1"/>
       <c r="S20" s="1"/>
       <c r="T20" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="U20" s="1">
         <v>10</v>
@@ -6619,7 +6611,7 @@
         <v>14</v>
       </c>
       <c r="Y20" s="1" t="s">
-        <v>114</v>
+        <v>240</v>
       </c>
       <c r="Z20" s="1">
         <v>14</v>
@@ -6638,7 +6630,7 @@
         <v>34</v>
       </c>
       <c r="AG20" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="21" spans="1:33" x14ac:dyDescent="0.15">
@@ -6646,10 +6638,10 @@
         <v>21200003</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="D21" s="1">
         <f t="shared" si="10"/>
@@ -6697,7 +6689,7 @@
       <c r="R21" s="1"/>
       <c r="S21" s="1"/>
       <c r="T21" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="U21" s="1">
         <v>10</v>
@@ -6708,7 +6700,7 @@
       </c>
       <c r="X21" s="1"/>
       <c r="Y21" s="1" t="s">
-        <v>118</v>
+        <v>241</v>
       </c>
       <c r="Z21" s="1">
         <v>12.5</v>
@@ -6727,7 +6719,7 @@
         <v>34</v>
       </c>
       <c r="AG21" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="22" spans="1:33" x14ac:dyDescent="0.15">
@@ -6735,10 +6727,10 @@
         <v>21200004</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D22" s="1">
         <f t="shared" ref="D22" si="11">IF(P22&gt;=23,4,IF(AND(P22&gt;=18,P22&lt;23),3,IF(AND(P22&gt;=13,P22&lt;18),2,IF(AND(P22&gt;=8,P22&lt;13),1,0))))</f>
@@ -6786,7 +6778,7 @@
       <c r="R22" s="1"/>
       <c r="S22" s="1"/>
       <c r="T22" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="U22" s="1">
         <v>10</v>
@@ -6799,7 +6791,7 @@
         <v>14</v>
       </c>
       <c r="Y22" s="1" t="s">
-        <v>119</v>
+        <v>242</v>
       </c>
       <c r="Z22" s="1">
         <v>14</v>
@@ -6818,7 +6810,7 @@
         <v>34</v>
       </c>
       <c r="AG22" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="23" spans="1:33" x14ac:dyDescent="0.15">
@@ -6826,10 +6818,10 @@
         <v>21200005</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="D23" s="1">
         <f t="shared" ref="D23:D25" si="12">IF(P23&gt;=23,4,IF(AND(P23&gt;=18,P23&lt;23),3,IF(AND(P23&gt;=13,P23&lt;18),2,IF(AND(P23&gt;=8,P23&lt;13),1,0))))</f>
@@ -6877,7 +6869,7 @@
       <c r="R23" s="1"/>
       <c r="S23" s="1"/>
       <c r="T23" s="1" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="U23" s="1">
         <v>10</v>
@@ -6888,7 +6880,7 @@
         <v>6</v>
       </c>
       <c r="Y23" s="26" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="Z23" s="1">
         <v>6</v>
@@ -6907,7 +6899,7 @@
         <v>34</v>
       </c>
       <c r="AG23" s="1" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="24" spans="1:33" x14ac:dyDescent="0.15">
@@ -6915,10 +6907,10 @@
         <v>21200006</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="D24" s="1">
         <f t="shared" si="12"/>
@@ -6966,7 +6958,7 @@
       <c r="R24" s="1"/>
       <c r="S24" s="1"/>
       <c r="T24" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="U24" s="1">
         <v>10</v>
@@ -6977,7 +6969,7 @@
       </c>
       <c r="X24" s="1"/>
       <c r="Y24" s="26" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="Z24" s="1">
         <v>6</v>
@@ -6996,7 +6988,7 @@
         <v>34</v>
       </c>
       <c r="AG24" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="25" spans="1:33" x14ac:dyDescent="0.15">
@@ -7004,10 +6996,10 @@
         <v>21200007</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="D25" s="1">
         <f t="shared" si="12"/>
@@ -7055,7 +7047,7 @@
       <c r="R25" s="1"/>
       <c r="S25" s="1"/>
       <c r="T25" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="U25" s="1">
         <v>10</v>
@@ -7068,7 +7060,7 @@
         <v>6</v>
       </c>
       <c r="Y25" s="1" t="s">
-        <v>224</v>
+        <v>243</v>
       </c>
       <c r="Z25" s="1">
         <v>9</v>
@@ -7087,7 +7079,7 @@
         <v>34</v>
       </c>
       <c r="AG25" s="1" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
     </row>
     <row r="26" spans="1:33" x14ac:dyDescent="0.15">
@@ -7095,10 +7087,10 @@
         <v>21200008</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="D26" s="1">
         <f t="shared" ref="D26:D27" si="14">IF(P26&gt;=23,4,IF(AND(P26&gt;=18,P26&lt;23),3,IF(AND(P26&gt;=13,P26&lt;18),2,IF(AND(P26&gt;=8,P26&lt;13),1,0))))</f>
@@ -7146,7 +7138,7 @@
       <c r="R26" s="1"/>
       <c r="S26" s="1"/>
       <c r="T26" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="U26" s="1">
         <v>10</v>
@@ -7159,7 +7151,7 @@
         <v>12</v>
       </c>
       <c r="Y26" s="1" t="s">
-        <v>228</v>
+        <v>244</v>
       </c>
       <c r="Z26" s="1">
         <v>18</v>
@@ -7178,7 +7170,7 @@
         <v>34</v>
       </c>
       <c r="AG26" s="1" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
     </row>
     <row r="27" spans="1:33" x14ac:dyDescent="0.15">
@@ -7186,10 +7178,10 @@
         <v>21200009</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="D27" s="1">
         <f t="shared" si="14"/>
@@ -7237,7 +7229,7 @@
       <c r="R27" s="1"/>
       <c r="S27" s="1"/>
       <c r="T27" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="U27" s="1">
         <v>10</v>
@@ -7250,7 +7242,7 @@
         <v>10</v>
       </c>
       <c r="Y27" s="1" t="s">
-        <v>232</v>
+        <v>245</v>
       </c>
       <c r="Z27" s="1">
         <v>15</v>
@@ -7269,7 +7261,7 @@
         <v>34</v>
       </c>
       <c r="AG27" s="1" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
     </row>
     <row r="28" spans="1:33" x14ac:dyDescent="0.15">
@@ -7277,10 +7269,10 @@
         <v>21200010</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="D28" s="1">
         <f t="shared" ref="D28" si="17">IF(P28&gt;=23,4,IF(AND(P28&gt;=18,P28&lt;23),3,IF(AND(P28&gt;=13,P28&lt;18),2,IF(AND(P28&gt;=8,P28&lt;13),1,0))))</f>
@@ -7328,7 +7320,7 @@
       <c r="R28" s="1"/>
       <c r="S28" s="1"/>
       <c r="T28" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="U28" s="1">
         <v>10</v>
@@ -7341,7 +7333,7 @@
         <v>10</v>
       </c>
       <c r="Y28" s="1" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="Z28" s="1">
         <v>25</v>
@@ -7360,7 +7352,7 @@
         <v>34</v>
       </c>
       <c r="AG28" s="1" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
     </row>
     <row r="29" spans="1:33" x14ac:dyDescent="0.15">
@@ -7415,7 +7407,7 @@
       </c>
       <c r="Q29" s="1"/>
       <c r="R29" s="1" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="S29" s="1"/>
       <c r="T29" s="1" t="s">
@@ -7453,7 +7445,7 @@
         <v>21300002</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="1">
@@ -7500,11 +7492,11 @@
       </c>
       <c r="Q30" s="1"/>
       <c r="R30" s="1" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="S30" s="1"/>
       <c r="T30" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="U30" s="1">
         <v>10</v>
@@ -7534,7 +7526,7 @@
         <v>34</v>
       </c>
       <c r="AG30" s="1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="31" spans="1:33" x14ac:dyDescent="0.15">
@@ -7542,7 +7534,7 @@
         <v>21300003</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C31" s="1"/>
       <c r="D31" s="1">
@@ -7589,11 +7581,11 @@
       </c>
       <c r="Q31" s="1"/>
       <c r="R31" s="1" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="S31" s="1"/>
       <c r="T31" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="U31" s="1">
         <v>10</v>
@@ -7619,7 +7611,7 @@
         <v>34</v>
       </c>
       <c r="AG31" s="1" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="32" spans="1:33" x14ac:dyDescent="0.15">
@@ -7627,7 +7619,7 @@
         <v>21300004</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="1">
@@ -7674,11 +7666,11 @@
       </c>
       <c r="Q32" s="1"/>
       <c r="R32" s="1" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="S32" s="1"/>
       <c r="T32" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="U32" s="1">
         <v>10</v>
@@ -7708,7 +7700,7 @@
         <v>34</v>
       </c>
       <c r="AG32" s="1" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="33" spans="1:33" x14ac:dyDescent="0.15">
@@ -7716,7 +7708,7 @@
         <v>21300005</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="1">
@@ -7763,11 +7755,11 @@
       </c>
       <c r="Q33" s="1"/>
       <c r="R33" s="1" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="S33" s="1"/>
       <c r="T33" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="U33" s="1">
         <v>10</v>
@@ -7793,7 +7785,7 @@
         <v>34</v>
       </c>
       <c r="AG33" s="1" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="34" spans="1:33" x14ac:dyDescent="0.15">
@@ -7801,7 +7793,7 @@
         <v>21300006</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C34" s="1"/>
       <c r="D34" s="1">
@@ -7848,11 +7840,11 @@
       </c>
       <c r="Q34" s="1"/>
       <c r="R34" s="1" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="S34" s="1"/>
       <c r="T34" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="U34" s="1">
         <v>10</v>
@@ -7878,7 +7870,7 @@
         <v>34</v>
       </c>
       <c r="AG34" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="35" spans="1:33" x14ac:dyDescent="0.15">
@@ -7886,7 +7878,7 @@
         <v>21300007</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C35" s="1"/>
       <c r="D35" s="1">
@@ -7933,11 +7925,11 @@
       </c>
       <c r="Q35" s="1"/>
       <c r="R35" s="1" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="S35" s="1"/>
       <c r="T35" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="U35" s="1">
         <v>10</v>
@@ -7963,7 +7955,7 @@
         <v>34</v>
       </c>
       <c r="AG35" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="36" spans="1:33" x14ac:dyDescent="0.15">
@@ -7971,7 +7963,7 @@
         <v>21300008</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C36" s="1"/>
       <c r="D36" s="1">
@@ -8018,11 +8010,11 @@
       </c>
       <c r="Q36" s="1"/>
       <c r="R36" s="1" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="S36" s="1"/>
       <c r="T36" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="U36" s="1">
         <v>10</v>
@@ -8048,7 +8040,7 @@
         <v>34</v>
       </c>
       <c r="AG36" s="1" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="37" spans="1:33" x14ac:dyDescent="0.15">
@@ -8056,7 +8048,7 @@
         <v>21300009</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C37" s="1"/>
       <c r="D37" s="1">
@@ -8103,11 +8095,11 @@
       </c>
       <c r="Q37" s="1"/>
       <c r="R37" s="1" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="S37" s="1"/>
       <c r="T37" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="U37" s="1">
         <v>10</v>
@@ -8137,7 +8129,7 @@
         <v>34</v>
       </c>
       <c r="AG37" s="1" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="38" spans="1:33" x14ac:dyDescent="0.15">
@@ -8145,7 +8137,7 @@
         <v>21400001</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C38" s="1"/>
       <c r="D38" s="22">
@@ -8222,7 +8214,7 @@
         <v>21400002</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C39" s="1"/>
       <c r="D39" s="22">
@@ -8291,7 +8283,7 @@
         <v>34</v>
       </c>
       <c r="AG39" s="2" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="40" spans="1:33" x14ac:dyDescent="0.15">
@@ -8299,7 +8291,7 @@
         <v>21400003</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C40" s="1"/>
       <c r="D40" s="22">
@@ -8348,7 +8340,7 @@
       <c r="R40" s="7"/>
       <c r="S40" s="7"/>
       <c r="T40" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="U40">
         <v>10</v>
@@ -8374,7 +8366,7 @@
         <v>34</v>
       </c>
       <c r="AG40" s="2" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="41" spans="1:33" x14ac:dyDescent="0.15">
@@ -8382,7 +8374,7 @@
         <v>21400004</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C41" s="1"/>
       <c r="D41" s="22">
@@ -8431,7 +8423,7 @@
       <c r="R41" s="7"/>
       <c r="S41" s="7"/>
       <c r="T41" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="U41">
         <v>10</v>
@@ -8451,7 +8443,7 @@
         <v>34</v>
       </c>
       <c r="AG41" s="2" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="42" spans="1:33" x14ac:dyDescent="0.15">
@@ -8459,7 +8451,7 @@
         <v>21400005</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C42" s="1"/>
       <c r="D42" s="22">
@@ -8508,7 +8500,7 @@
       <c r="R42" s="7"/>
       <c r="S42" s="7"/>
       <c r="T42" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="U42">
         <v>10</v>
@@ -8528,7 +8520,7 @@
         <v>34</v>
       </c>
       <c r="AG42" s="2" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="43" spans="1:33" x14ac:dyDescent="0.15">
@@ -8536,7 +8528,7 @@
         <v>21400006</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C43" s="1"/>
       <c r="D43" s="22">
@@ -8585,7 +8577,7 @@
       <c r="R43" s="7"/>
       <c r="S43" s="7"/>
       <c r="T43" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="U43">
         <v>10</v>
@@ -8605,7 +8597,7 @@
         <v>34</v>
       </c>
       <c r="AG43" s="2" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="44" spans="1:33" x14ac:dyDescent="0.15">
@@ -8613,7 +8605,7 @@
         <v>21400007</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C44" s="1"/>
       <c r="D44" s="22">
@@ -8662,7 +8654,7 @@
       <c r="R44" s="7"/>
       <c r="S44" s="7"/>
       <c r="T44" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="U44">
         <v>10</v>
@@ -8682,7 +8674,7 @@
         <v>34</v>
       </c>
       <c r="AG44" s="2" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="45" spans="1:33" x14ac:dyDescent="0.15">
@@ -8690,7 +8682,7 @@
         <v>21400008</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C45" s="1"/>
       <c r="D45" s="22">
@@ -8739,7 +8731,7 @@
       <c r="R45" s="7"/>
       <c r="S45" s="7"/>
       <c r="T45" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="U45">
         <v>10</v>
@@ -8759,7 +8751,7 @@
         <v>34</v>
       </c>
       <c r="AG45" s="2" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="46" spans="1:33" x14ac:dyDescent="0.15">
@@ -8767,7 +8759,7 @@
         <v>21400009</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C46" s="1"/>
       <c r="D46" s="22">
@@ -8816,7 +8808,7 @@
       <c r="R46" s="7"/>
       <c r="S46" s="7"/>
       <c r="T46" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="U46">
         <v>10</v>
@@ -8836,7 +8828,7 @@
         <v>34</v>
       </c>
       <c r="AG46" s="2" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="47" spans="1:33" x14ac:dyDescent="0.15">
@@ -8844,7 +8836,7 @@
         <v>21400010</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C47" s="1"/>
       <c r="D47" s="22">
@@ -8893,7 +8885,7 @@
       <c r="R47" s="7"/>
       <c r="S47" s="7"/>
       <c r="T47" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="U47">
         <v>10</v>
@@ -8913,7 +8905,7 @@
         <v>34</v>
       </c>
       <c r="AG47" s="2" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="48" spans="1:33" x14ac:dyDescent="0.15">
@@ -8921,7 +8913,7 @@
         <v>21400011</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C48" s="1"/>
       <c r="D48" s="22">
@@ -8970,7 +8962,7 @@
       <c r="R48" s="7"/>
       <c r="S48" s="7"/>
       <c r="T48" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="U48">
         <v>10</v>
@@ -8990,7 +8982,7 @@
         <v>34</v>
       </c>
       <c r="AG48" s="2" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="49" spans="1:33" x14ac:dyDescent="0.15">
@@ -9077,7 +9069,7 @@
         <v>21500002</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C50" s="1"/>
       <c r="D50" s="22">
@@ -9126,7 +9118,7 @@
       <c r="R50" s="7"/>
       <c r="S50" s="7"/>
       <c r="T50" s="12" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="U50">
         <v>10</v>
@@ -9146,7 +9138,7 @@
         <v>34</v>
       </c>
       <c r="AG50" s="2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="51" spans="1:33" x14ac:dyDescent="0.15">
@@ -9154,7 +9146,7 @@
         <v>21500003</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C51" s="1"/>
       <c r="D51" s="22">
@@ -9203,7 +9195,7 @@
       <c r="R51" s="7"/>
       <c r="S51" s="7"/>
       <c r="T51" s="12" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="U51">
         <v>10</v>
@@ -9223,7 +9215,7 @@
         <v>34</v>
       </c>
       <c r="AG51" s="2" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="52" spans="1:33" x14ac:dyDescent="0.15">
@@ -9231,7 +9223,7 @@
         <v>21500004</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C52" s="1"/>
       <c r="D52" s="22">
@@ -9306,7 +9298,7 @@
         <v>34</v>
       </c>
       <c r="AG52" s="2" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="53" spans="1:33" x14ac:dyDescent="0.15">
@@ -9314,7 +9306,7 @@
         <v>21500005</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C53" s="1"/>
       <c r="D53" s="22">
@@ -9363,7 +9355,7 @@
       <c r="R53" s="7"/>
       <c r="S53" s="7"/>
       <c r="T53" s="12" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="U53">
         <v>10</v>
@@ -9383,7 +9375,7 @@
         <v>34</v>
       </c>
       <c r="AG53" s="2" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="54" spans="1:33" x14ac:dyDescent="0.15">
@@ -9391,7 +9383,7 @@
         <v>21500006</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C54" s="1"/>
       <c r="D54" s="22">
@@ -9466,7 +9458,7 @@
         <v>34</v>
       </c>
       <c r="AG54" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="55" spans="1:33" x14ac:dyDescent="0.15">
@@ -9474,7 +9466,7 @@
         <v>21500007</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="C55" s="1"/>
       <c r="D55" s="22">
@@ -9523,7 +9515,7 @@
       <c r="R55" s="7"/>
       <c r="S55" s="7"/>
       <c r="T55" s="12" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="U55">
         <v>10</v>
@@ -9543,7 +9535,7 @@
         <v>34</v>
       </c>
       <c r="AG55" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="56" spans="1:33" x14ac:dyDescent="0.15">
@@ -9551,7 +9543,7 @@
         <v>21500008</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C56" s="1"/>
       <c r="D56" s="22">
@@ -9600,7 +9592,7 @@
       <c r="R56" s="7"/>
       <c r="S56" s="7"/>
       <c r="T56" s="12" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="U56">
         <v>10</v>
@@ -9626,7 +9618,7 @@
         <v>34</v>
       </c>
       <c r="AG56" s="2" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="57" spans="1:33" x14ac:dyDescent="0.15">
@@ -9634,7 +9626,7 @@
         <v>21500009</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="C57" s="1"/>
       <c r="D57" s="22">
@@ -9683,7 +9675,7 @@
       <c r="R57" s="7"/>
       <c r="S57" s="7"/>
       <c r="T57" s="12" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="U57">
         <v>10</v>
@@ -9706,7 +9698,7 @@
         <v>34</v>
       </c>
       <c r="AG57" s="2" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
     </row>
     <row r="58" spans="1:33" x14ac:dyDescent="0.15">
@@ -9714,7 +9706,7 @@
         <v>21500010</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="C58" s="1"/>
       <c r="D58" s="22">
@@ -9763,7 +9755,7 @@
       <c r="R58" s="7"/>
       <c r="S58" s="7"/>
       <c r="T58" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="U58">
         <v>10</v>
@@ -9786,7 +9778,7 @@
         <v>34</v>
       </c>
       <c r="AG58" s="2" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
     </row>
     <row r="59" spans="1:33" x14ac:dyDescent="0.15">
@@ -9794,7 +9786,7 @@
         <v>21500011</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="C59" s="1"/>
       <c r="D59" s="22">
@@ -9843,7 +9835,7 @@
       <c r="R59" s="7"/>
       <c r="S59" s="7"/>
       <c r="T59" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="U59">
         <v>10</v>
@@ -9866,7 +9858,7 @@
         <v>34</v>
       </c>
       <c r="AG59" s="2" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
set the item compose cost
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Equip.xlsx
+++ b/ConfigData/Xlsx/Equip.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -2015,25 +2015,6 @@
   </cellStyles>
   <dxfs count="40">
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FF00B050"/>
@@ -2621,6 +2602,54 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
         <scheme val="minor"/>
       </font>
       <fill>
@@ -2698,104 +2727,9 @@
         <horizontal/>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
     <mruColors>
       <color rgb="FF9751CB"/>
     </mruColors>
@@ -4568,47 +4502,47 @@
     <tableColumn id="2" name="Name"/>
     <tableColumn id="34" name="Ename" dataDxfId="39"/>
     <tableColumn id="32" name="Des" dataDxfId="38"/>
-    <tableColumn id="3" name="Quality" dataDxfId="36">
+    <tableColumn id="3" name="Quality" dataDxfId="37">
       <calculatedColumnFormula>IF(T4&gt;=23,4,IF(AND(T4&gt;=18,T4&lt;23),3,IF(AND(T4&gt;=13,T4&lt;18),2,IF(AND(T4&gt;=8,T4&lt;13),1,0))))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" name="Position"/>
-    <tableColumn id="19" name="Value" dataDxfId="37">
+    <tableColumn id="19" name="Value" dataDxfId="36">
       <calculatedColumnFormula>E4*50+50</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="35" name="ComposeStone" dataDxfId="35"/>
     <tableColumn id="36" name="ComposeWood" dataDxfId="34"/>
-    <tableColumn id="15" name="ComposeItemId" dataDxfId="0"/>
-    <tableColumn id="11" name="AtkR" dataDxfId="33"/>
-    <tableColumn id="8" name="VitR" dataDxfId="32"/>
-    <tableColumn id="6" name="Def" dataDxfId="31"/>
-    <tableColumn id="22" name="Mag" dataDxfId="30"/>
-    <tableColumn id="27" name="Spd" dataDxfId="29"/>
-    <tableColumn id="26" name="Hit" dataDxfId="28"/>
-    <tableColumn id="25" name="Dhit" dataDxfId="27"/>
-    <tableColumn id="24" name="Crt" dataDxfId="26"/>
-    <tableColumn id="23" name="Luk" dataDxfId="25"/>
-    <tableColumn id="28" name="Sum" dataDxfId="24">
+    <tableColumn id="15" name="ComposeItemId" dataDxfId="33"/>
+    <tableColumn id="11" name="AtkR" dataDxfId="32"/>
+    <tableColumn id="8" name="VitR" dataDxfId="31"/>
+    <tableColumn id="6" name="Def" dataDxfId="30"/>
+    <tableColumn id="22" name="Mag" dataDxfId="29"/>
+    <tableColumn id="27" name="Spd" dataDxfId="28"/>
+    <tableColumn id="26" name="Hit" dataDxfId="27"/>
+    <tableColumn id="25" name="Dhit" dataDxfId="26"/>
+    <tableColumn id="24" name="Crt" dataDxfId="25"/>
+    <tableColumn id="23" name="Luk" dataDxfId="24"/>
+    <tableColumn id="28" name="Sum" dataDxfId="23">
       <calculatedColumnFormula>K4+L4+ SUM(M4:S4)*5+AE4+AF4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="Range" dataDxfId="23"/>
-    <tableColumn id="33" name="Arrow" dataDxfId="22"/>
-    <tableColumn id="4" name="SlotId" dataDxfId="21"/>
-    <tableColumn id="9" name="EnergyRate" dataDxfId="20"/>
-    <tableColumn id="37" name="DungeonAttrs" dataDxfId="19"/>
-    <tableColumn id="7" name="Durable" dataDxfId="18"/>
-    <tableColumn id="20" name="HeroSkillId" dataDxfId="17"/>
-    <tableColumn id="29" name="MonsterAtk" dataDxfId="16"/>
-    <tableColumn id="30" name="MonsterHp" dataDxfId="15"/>
-    <tableColumn id="31" name="PickMethod" dataDxfId="14"/>
-    <tableColumn id="21" name="~SkillMark2" dataDxfId="13"/>
-    <tableColumn id="18" name="~SkillMark22" dataDxfId="12">
+    <tableColumn id="12" name="Range" dataDxfId="22"/>
+    <tableColumn id="33" name="Arrow" dataDxfId="21"/>
+    <tableColumn id="4" name="SlotId" dataDxfId="20"/>
+    <tableColumn id="9" name="EnergyRate" dataDxfId="19"/>
+    <tableColumn id="37" name="DungeonAttrs" dataDxfId="18"/>
+    <tableColumn id="7" name="Durable" dataDxfId="17"/>
+    <tableColumn id="20" name="HeroSkillId" dataDxfId="16"/>
+    <tableColumn id="29" name="MonsterAtk" dataDxfId="15"/>
+    <tableColumn id="30" name="MonsterHp" dataDxfId="14"/>
+    <tableColumn id="31" name="PickMethod" dataDxfId="13"/>
+    <tableColumn id="21" name="~SkillMark2" dataDxfId="12"/>
+    <tableColumn id="18" name="~SkillMark22" dataDxfId="11">
       <calculatedColumnFormula>IF(ISBLANK(AG4),0, LOOKUP(AG4,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AH4/100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="CommonSkillId" dataDxfId="11"/>
-    <tableColumn id="14" name="CommonSkillRate" dataDxfId="10"/>
-    <tableColumn id="17" name="RandomDrop" dataDxfId="9"/>
-    <tableColumn id="16" name="CanMerge" dataDxfId="8"/>
-    <tableColumn id="10" name="Url" dataDxfId="7"/>
+    <tableColumn id="13" name="CommonSkillId" dataDxfId="10"/>
+    <tableColumn id="14" name="CommonSkillRate" dataDxfId="9"/>
+    <tableColumn id="17" name="RandomDrop" dataDxfId="8"/>
+    <tableColumn id="16" name="CanMerge" dataDxfId="7"/>
+    <tableColumn id="10" name="Url" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4622,7 +4556,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="C7EDCC"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -4938,7 +4872,7 @@
   <dimension ref="A1:AK59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -5331,7 +5265,7 @@
       </c>
       <c r="I4" s="18"/>
       <c r="J4" s="18">
-        <v>22100402</v>
+        <v>22100401</v>
       </c>
       <c r="K4" s="18">
         <v>0</v>
@@ -5521,7 +5455,7 @@
         <v>100</v>
       </c>
       <c r="J6" s="18">
-        <v>22100402</v>
+        <v>22100205</v>
       </c>
       <c r="K6" s="18">
         <v>0</v>
@@ -5618,7 +5552,7 @@
         <v>50</v>
       </c>
       <c r="J7" s="18">
-        <v>22100402</v>
+        <v>22100406</v>
       </c>
       <c r="K7" s="18">
         <v>0</v>
@@ -5713,7 +5647,7 @@
         <v>100</v>
       </c>
       <c r="J8" s="18">
-        <v>22100402</v>
+        <v>22100206</v>
       </c>
       <c r="K8" s="18">
         <v>0</v>
@@ -5808,7 +5742,7 @@
         <v>100</v>
       </c>
       <c r="J9" s="18">
-        <v>22100402</v>
+        <v>22100208</v>
       </c>
       <c r="K9" s="18">
         <v>0</v>
@@ -5905,7 +5839,7 @@
         <v>70</v>
       </c>
       <c r="J10" s="18">
-        <v>22100402</v>
+        <v>22100214</v>
       </c>
       <c r="K10" s="18">
         <v>0</v>
@@ -6000,7 +5934,7 @@
         <v>100</v>
       </c>
       <c r="J11" s="18">
-        <v>22100402</v>
+        <v>22100218</v>
       </c>
       <c r="K11" s="18">
         <v>0</v>
@@ -6095,7 +6029,7 @@
         <v>100</v>
       </c>
       <c r="J12" s="18">
-        <v>22100402</v>
+        <v>22100210</v>
       </c>
       <c r="K12" s="18">
         <v>0</v>
@@ -6190,7 +6124,7 @@
         <v>100</v>
       </c>
       <c r="J13" s="18">
-        <v>22100402</v>
+        <v>22100201</v>
       </c>
       <c r="K13" s="18">
         <v>0</v>
@@ -6285,7 +6219,7 @@
         <v>100</v>
       </c>
       <c r="J14" s="18">
-        <v>22100402</v>
+        <v>22100207</v>
       </c>
       <c r="K14" s="18">
         <v>0</v>
@@ -6380,7 +6314,7 @@
         <v>100</v>
       </c>
       <c r="J15" s="18">
-        <v>22100402</v>
+        <v>22100213</v>
       </c>
       <c r="K15" s="18">
         <v>0</v>
@@ -6475,7 +6409,7 @@
         <v>100</v>
       </c>
       <c r="J16" s="18">
-        <v>22100402</v>
+        <v>22100205</v>
       </c>
       <c r="K16" s="18">
         <v>0</v>
@@ -6570,7 +6504,7 @@
       </c>
       <c r="I17" s="18"/>
       <c r="J17" s="18">
-        <v>22100402</v>
+        <v>22100401</v>
       </c>
       <c r="K17" s="18">
         <v>0</v>
@@ -6665,7 +6599,7 @@
         <v>100</v>
       </c>
       <c r="J18" s="18">
-        <v>22100402</v>
+        <v>22100219</v>
       </c>
       <c r="K18" s="18">
         <v>0</v>
@@ -6762,7 +6696,7 @@
       </c>
       <c r="I19" s="18"/>
       <c r="J19" s="18">
-        <v>22100402</v>
+        <v>22100406</v>
       </c>
       <c r="K19" s="18">
         <v>0</v>
@@ -6861,7 +6795,7 @@
       </c>
       <c r="I20" s="18"/>
       <c r="J20" s="18">
-        <v>22100402</v>
+        <v>22100405</v>
       </c>
       <c r="K20" s="18">
         <v>0</v>
@@ -6962,7 +6896,7 @@
       </c>
       <c r="I21" s="18"/>
       <c r="J21" s="18">
-        <v>22100402</v>
+        <v>22100406</v>
       </c>
       <c r="K21" s="18">
         <v>0</v>
@@ -7061,7 +6995,7 @@
       </c>
       <c r="I22" s="18"/>
       <c r="J22" s="18">
-        <v>22100402</v>
+        <v>22100405</v>
       </c>
       <c r="K22" s="18">
         <v>0</v>
@@ -7162,7 +7096,7 @@
       </c>
       <c r="I23" s="18"/>
       <c r="J23" s="18">
-        <v>22100402</v>
+        <v>22100416</v>
       </c>
       <c r="K23" s="18">
         <v>0</v>
@@ -7261,7 +7195,7 @@
       </c>
       <c r="I24" s="18"/>
       <c r="J24" s="18">
-        <v>22100402</v>
+        <v>22100416</v>
       </c>
       <c r="K24" s="18">
         <v>0</v>
@@ -7360,7 +7294,7 @@
       </c>
       <c r="I25" s="18"/>
       <c r="J25" s="18">
-        <v>22100402</v>
+        <v>22100406</v>
       </c>
       <c r="K25" s="18">
         <v>0</v>
@@ -7461,7 +7395,7 @@
       </c>
       <c r="I26" s="18"/>
       <c r="J26" s="18">
-        <v>22100402</v>
+        <v>22100404</v>
       </c>
       <c r="K26" s="18">
         <v>0</v>
@@ -7562,7 +7496,7 @@
       </c>
       <c r="I27" s="18"/>
       <c r="J27" s="18">
-        <v>22100402</v>
+        <v>22100410</v>
       </c>
       <c r="K27" s="18">
         <v>0</v>
@@ -7663,7 +7597,7 @@
       </c>
       <c r="I28" s="18"/>
       <c r="J28" s="18">
-        <v>22100402</v>
+        <v>22100412</v>
       </c>
       <c r="K28" s="18">
         <v>0</v>
@@ -7958,7 +7892,7 @@
         <v>50</v>
       </c>
       <c r="J31" s="18">
-        <v>22100402</v>
+        <v>22100415</v>
       </c>
       <c r="K31" s="18">
         <v>6</v>
@@ -8055,7 +7989,7 @@
         <v>50</v>
       </c>
       <c r="J32" s="18">
-        <v>22100402</v>
+        <v>22100407</v>
       </c>
       <c r="K32" s="18">
         <v>8</v>
@@ -8156,7 +8090,7 @@
         <v>30</v>
       </c>
       <c r="J33" s="18">
-        <v>22100402</v>
+        <v>22100407</v>
       </c>
       <c r="K33" s="18">
         <v>12</v>
@@ -8251,7 +8185,7 @@
       </c>
       <c r="I34" s="18"/>
       <c r="J34" s="18">
-        <v>22100402</v>
+        <v>22100408</v>
       </c>
       <c r="K34" s="18">
         <v>20</v>
@@ -8348,7 +8282,7 @@
         <v>50</v>
       </c>
       <c r="J35" s="18">
-        <v>22100402</v>
+        <v>22100411</v>
       </c>
       <c r="K35" s="18">
         <v>5</v>
@@ -8443,7 +8377,7 @@
       </c>
       <c r="I36" s="18"/>
       <c r="J36" s="18">
-        <v>22100402</v>
+        <v>22100416</v>
       </c>
       <c r="K36" s="18">
         <v>1</v>
@@ -8732,7 +8666,7 @@
         <v>100</v>
       </c>
       <c r="J39" s="18">
-        <v>22100402</v>
+        <v>22100202</v>
       </c>
       <c r="K39" s="18">
         <v>0</v>
@@ -8825,7 +8759,7 @@
       </c>
       <c r="I40" s="18"/>
       <c r="J40" s="18">
-        <v>22100402</v>
+        <v>22100414</v>
       </c>
       <c r="K40" s="18">
         <v>0</v>
@@ -8922,7 +8856,7 @@
         <v>100</v>
       </c>
       <c r="J41" s="18">
-        <v>22100402</v>
+        <v>22100209</v>
       </c>
       <c r="K41" s="18">
         <v>0</v>
@@ -9015,7 +8949,7 @@
         <v>100</v>
       </c>
       <c r="J42" s="18">
-        <v>22100402</v>
+        <v>22100201</v>
       </c>
       <c r="K42" s="18">
         <v>0</v>
@@ -9110,7 +9044,7 @@
         <v>50</v>
       </c>
       <c r="J43" s="18">
-        <v>22100402</v>
+        <v>22100202</v>
       </c>
       <c r="K43" s="18">
         <v>0</v>
@@ -9203,7 +9137,7 @@
         <v>100</v>
       </c>
       <c r="J44" s="18">
-        <v>22100402</v>
+        <v>22100213</v>
       </c>
       <c r="K44" s="18">
         <v>0</v>
@@ -9296,7 +9230,7 @@
       </c>
       <c r="I45" s="18"/>
       <c r="J45" s="18">
-        <v>22100402</v>
+        <v>22100414</v>
       </c>
       <c r="K45" s="18">
         <v>0</v>
@@ -9391,7 +9325,7 @@
         <v>50</v>
       </c>
       <c r="J46" s="18">
-        <v>22100402</v>
+        <v>22100215</v>
       </c>
       <c r="K46" s="18">
         <v>0</v>
@@ -9486,7 +9420,7 @@
         <v>50</v>
       </c>
       <c r="J47" s="18">
-        <v>22100402</v>
+        <v>22100205</v>
       </c>
       <c r="K47" s="18">
         <v>0</v>
@@ -9581,7 +9515,7 @@
         <v>50</v>
       </c>
       <c r="J48" s="18">
-        <v>22100402</v>
+        <v>22100411</v>
       </c>
       <c r="K48" s="18">
         <v>0</v>
@@ -9674,7 +9608,7 @@
         <v>100</v>
       </c>
       <c r="J49" s="18">
-        <v>22100402</v>
+        <v>22100204</v>
       </c>
       <c r="K49" s="18">
         <v>0</v>
@@ -9769,7 +9703,7 @@
         <v>100</v>
       </c>
       <c r="J50" s="18">
-        <v>22100402</v>
+        <v>22100204</v>
       </c>
       <c r="K50" s="18">
         <v>0</v>
@@ -9864,7 +9798,7 @@
         <v>100</v>
       </c>
       <c r="J51" s="18">
-        <v>22100402</v>
+        <v>22100215</v>
       </c>
       <c r="K51" s="18">
         <v>0</v>
@@ -9959,7 +9893,7 @@
         <v>100</v>
       </c>
       <c r="J52" s="18">
-        <v>22100402</v>
+        <v>22100215</v>
       </c>
       <c r="K52" s="18">
         <v>0</v>
@@ -10056,7 +9990,7 @@
         <v>100</v>
       </c>
       <c r="J53" s="18">
-        <v>22100402</v>
+        <v>22100206</v>
       </c>
       <c r="K53" s="18">
         <v>0</v>
@@ -10151,7 +10085,7 @@
         <v>100</v>
       </c>
       <c r="J54" s="18">
-        <v>22100402</v>
+        <v>22100203</v>
       </c>
       <c r="K54" s="18">
         <v>0</v>
@@ -10248,7 +10182,7 @@
         <v>100</v>
       </c>
       <c r="J55" s="18">
-        <v>22100402</v>
+        <v>22100203</v>
       </c>
       <c r="K55" s="18">
         <v>0</v>
@@ -10341,7 +10275,7 @@
         <v>100</v>
       </c>
       <c r="J56" s="18">
-        <v>22100402</v>
+        <v>22100214</v>
       </c>
       <c r="K56" s="18">
         <v>0</v>
@@ -10438,7 +10372,7 @@
         <v>100</v>
       </c>
       <c r="J57" s="18">
-        <v>22100402</v>
+        <v>22100219</v>
       </c>
       <c r="K57" s="18">
         <v>0</v>
@@ -10533,7 +10467,7 @@
         <v>100</v>
       </c>
       <c r="J58" s="18">
-        <v>22100402</v>
+        <v>22100214</v>
       </c>
       <c r="K58" s="18">
         <v>0</v>
@@ -10630,7 +10564,7 @@
         <v>100</v>
       </c>
       <c r="J59" s="18">
-        <v>22100402</v>
+        <v>22100218</v>
       </c>
       <c r="K59" s="18">
         <v>0</v>
@@ -10701,24 +10635,24 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="E4:E59">
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="greaterThanOrEqual">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="8" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="9" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="10" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="11" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:AK59">
-    <cfRule type="containsBlanks" dxfId="1" priority="1">
+    <cfRule type="containsBlanks" dxfId="0" priority="1">
       <formula>LEN(TRIM(H4))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
fix the showing bug on equip form
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Equip.xlsx
+++ b/ConfigData/Xlsx/Equip.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TOMClassic\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -2013,7 +2013,10 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="40">
+  <dxfs count="46">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2066,6 +2069,71 @@
       <fill>
         <patternFill>
           <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF9751CB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2141,9 +2209,6 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -2758,1329 +2823,1814 @@
           <cell r="A1" t="str">
             <v>序列</v>
           </cell>
-          <cell r="Y1" t="str">
-            <v>卡牌表面特效</v>
+          <cell r="AB1" t="str">
+            <v>评分</v>
           </cell>
         </row>
         <row r="2">
           <cell r="A2" t="str">
             <v>int</v>
           </cell>
-          <cell r="Y2" t="str">
-            <v>string</v>
+          <cell r="AB2" t="str">
+            <v>int</v>
           </cell>
         </row>
         <row r="3">
           <cell r="A3" t="str">
             <v>Id</v>
           </cell>
-          <cell r="Y3" t="str">
-            <v>Cover</v>
+          <cell r="AB3" t="str">
+            <v>Mark</v>
           </cell>
         </row>
         <row r="4">
           <cell r="A4">
             <v>55100001</v>
           </cell>
-          <cell r="Y4"/>
+          <cell r="AB4">
+            <v>10</v>
+          </cell>
         </row>
         <row r="5">
           <cell r="A5">
             <v>55100002</v>
           </cell>
-          <cell r="Y5"/>
+          <cell r="AB5">
+            <v>15</v>
+          </cell>
         </row>
         <row r="6">
           <cell r="A6">
             <v>55100003</v>
           </cell>
-          <cell r="Y6"/>
+          <cell r="AB6">
+            <v>15</v>
+          </cell>
         </row>
         <row r="7">
           <cell r="A7">
             <v>55100004</v>
           </cell>
-          <cell r="Y7"/>
+          <cell r="AB7">
+            <v>15</v>
+          </cell>
         </row>
         <row r="8">
           <cell r="A8">
             <v>55100005</v>
           </cell>
-          <cell r="Y8"/>
+          <cell r="AB8">
+            <v>30</v>
+          </cell>
         </row>
         <row r="9">
           <cell r="A9">
             <v>55100006</v>
           </cell>
-          <cell r="Y9"/>
+          <cell r="AB9">
+            <v>45</v>
+          </cell>
         </row>
         <row r="10">
           <cell r="A10">
             <v>55100007</v>
           </cell>
-          <cell r="Y10"/>
+          <cell r="AB10">
+            <v>35</v>
+          </cell>
         </row>
         <row r="11">
           <cell r="A11">
             <v>55100008</v>
           </cell>
-          <cell r="Y11"/>
+          <cell r="AB11">
+            <v>15</v>
+          </cell>
         </row>
         <row r="12">
           <cell r="A12">
-            <v>55100010</v>
-          </cell>
-          <cell r="Y12" t="str">
-            <v>coverstar</v>
+            <v>55100009</v>
+          </cell>
+          <cell r="AB12">
+            <v>15</v>
           </cell>
         </row>
         <row r="13">
           <cell r="A13">
-            <v>55100011</v>
-          </cell>
-          <cell r="Y13"/>
+            <v>55100010</v>
+          </cell>
+          <cell r="AB13">
+            <v>30</v>
+          </cell>
         </row>
         <row r="14">
           <cell r="A14">
-            <v>55100012</v>
-          </cell>
-          <cell r="Y14" t="str">
-            <v>coverstar</v>
+            <v>55100011</v>
+          </cell>
+          <cell r="AB14">
+            <v>6</v>
           </cell>
         </row>
         <row r="15">
           <cell r="A15">
-            <v>55100013</v>
-          </cell>
-          <cell r="Y15"/>
+            <v>55100012</v>
+          </cell>
+          <cell r="AB15">
+            <v>15</v>
+          </cell>
         </row>
         <row r="16">
           <cell r="A16">
-            <v>55100014</v>
-          </cell>
-          <cell r="Y16"/>
+            <v>55100013</v>
+          </cell>
+          <cell r="AB16">
+            <v>10</v>
+          </cell>
         </row>
         <row r="17">
           <cell r="A17">
-            <v>55100015</v>
-          </cell>
-          <cell r="Y17"/>
+            <v>55100014</v>
+          </cell>
+          <cell r="AB17">
+            <v>24</v>
+          </cell>
         </row>
         <row r="18">
           <cell r="A18">
-            <v>55110001</v>
-          </cell>
-          <cell r="Y18"/>
+            <v>55100015</v>
+          </cell>
+          <cell r="AB18">
+            <v>16</v>
+          </cell>
         </row>
         <row r="19">
           <cell r="A19">
-            <v>55110002</v>
-          </cell>
-          <cell r="Y19"/>
+            <v>55100016</v>
+          </cell>
+          <cell r="AB19">
+            <v>0</v>
+          </cell>
         </row>
         <row r="20">
           <cell r="A20">
-            <v>55110003</v>
-          </cell>
-          <cell r="Y20"/>
+            <v>55100017</v>
+          </cell>
+          <cell r="AB20">
+            <v>35</v>
+          </cell>
         </row>
         <row r="21">
           <cell r="A21">
-            <v>55110004</v>
-          </cell>
-          <cell r="Y21"/>
+            <v>55100018</v>
+          </cell>
+          <cell r="AB21">
+            <v>40</v>
+          </cell>
         </row>
         <row r="22">
           <cell r="A22">
-            <v>55110005</v>
-          </cell>
-          <cell r="Y22"/>
+            <v>55100019</v>
+          </cell>
+          <cell r="AB22">
+            <v>10</v>
+          </cell>
         </row>
         <row r="23">
           <cell r="A23">
-            <v>55110006</v>
-          </cell>
-          <cell r="Y23"/>
+            <v>55110001</v>
+          </cell>
+          <cell r="AB23">
+            <v>5</v>
+          </cell>
         </row>
         <row r="24">
           <cell r="A24">
-            <v>55110007</v>
-          </cell>
-          <cell r="Y24"/>
+            <v>55110002</v>
+          </cell>
+          <cell r="AB24">
+            <v>8</v>
+          </cell>
         </row>
         <row r="25">
           <cell r="A25">
-            <v>55110008</v>
-          </cell>
-          <cell r="Y25"/>
+            <v>55110003</v>
+          </cell>
+          <cell r="AB25">
+            <v>25</v>
+          </cell>
         </row>
         <row r="26">
           <cell r="A26">
-            <v>55110009</v>
-          </cell>
-          <cell r="Y26"/>
+            <v>55110004</v>
+          </cell>
+          <cell r="AB26">
+            <v>25</v>
+          </cell>
         </row>
         <row r="27">
           <cell r="A27">
-            <v>55110010</v>
-          </cell>
-          <cell r="Y27"/>
+            <v>55110005</v>
+          </cell>
+          <cell r="AB27">
+            <v>20</v>
+          </cell>
         </row>
         <row r="28">
           <cell r="A28">
-            <v>55110011</v>
-          </cell>
-          <cell r="Y28"/>
+            <v>55110006</v>
+          </cell>
+          <cell r="AB28">
+            <v>15</v>
+          </cell>
         </row>
         <row r="29">
           <cell r="A29">
-            <v>55110012</v>
-          </cell>
-          <cell r="Y29"/>
+            <v>55110007</v>
+          </cell>
+          <cell r="AB29">
+            <v>10</v>
+          </cell>
         </row>
         <row r="30">
           <cell r="A30">
-            <v>55110013</v>
-          </cell>
-          <cell r="Y30"/>
+            <v>55110008</v>
+          </cell>
+          <cell r="AB30">
+            <v>50</v>
+          </cell>
         </row>
         <row r="31">
           <cell r="A31">
-            <v>55110014</v>
-          </cell>
-          <cell r="Y31"/>
+            <v>55110009</v>
+          </cell>
+          <cell r="AB31">
+            <v>12</v>
+          </cell>
         </row>
         <row r="32">
           <cell r="A32">
-            <v>55110015</v>
-          </cell>
-          <cell r="Y32"/>
+            <v>55110010</v>
+          </cell>
+          <cell r="AB32">
+            <v>20</v>
+          </cell>
         </row>
         <row r="33">
           <cell r="A33">
-            <v>55110016</v>
-          </cell>
-          <cell r="Y33"/>
+            <v>55110011</v>
+          </cell>
+          <cell r="AB33">
+            <v>10</v>
+          </cell>
         </row>
         <row r="34">
           <cell r="A34">
-            <v>55110017</v>
-          </cell>
-          <cell r="Y34"/>
+            <v>55110012</v>
+          </cell>
+          <cell r="AB34">
+            <v>30</v>
+          </cell>
         </row>
         <row r="35">
           <cell r="A35">
-            <v>55110018</v>
-          </cell>
-          <cell r="Y35"/>
+            <v>55110013</v>
+          </cell>
+          <cell r="AB35">
+            <v>200</v>
+          </cell>
         </row>
         <row r="36">
           <cell r="A36">
-            <v>55110019</v>
-          </cell>
-          <cell r="Y36"/>
+            <v>55110014</v>
+          </cell>
+          <cell r="AB36">
+            <v>50</v>
+          </cell>
         </row>
         <row r="37">
           <cell r="A37">
-            <v>55110020</v>
-          </cell>
-          <cell r="Y37"/>
+            <v>55110015</v>
+          </cell>
+          <cell r="AB37">
+            <v>20</v>
+          </cell>
         </row>
         <row r="38">
           <cell r="A38">
-            <v>55200001</v>
-          </cell>
-          <cell r="Y38" t="str">
-            <v>coveraoe</v>
+            <v>55110016</v>
+          </cell>
+          <cell r="AB38">
+            <v>15</v>
           </cell>
         </row>
         <row r="39">
           <cell r="A39">
-            <v>55200002</v>
-          </cell>
-          <cell r="Y39"/>
+            <v>55110017</v>
+          </cell>
+          <cell r="AB39">
+            <v>8</v>
+          </cell>
         </row>
         <row r="40">
           <cell r="A40">
-            <v>55200003</v>
-          </cell>
-          <cell r="Y40"/>
+            <v>55110018</v>
+          </cell>
+          <cell r="AB40">
+            <v>20</v>
+          </cell>
         </row>
         <row r="41">
           <cell r="A41">
-            <v>55200004</v>
-          </cell>
-          <cell r="Y41"/>
+            <v>55110019</v>
+          </cell>
+          <cell r="AB41">
+            <v>30</v>
+          </cell>
         </row>
         <row r="42">
           <cell r="A42">
-            <v>55200005</v>
-          </cell>
-          <cell r="Y42"/>
+            <v>55110020</v>
+          </cell>
+          <cell r="AB42">
+            <v>40</v>
+          </cell>
         </row>
         <row r="43">
           <cell r="A43">
-            <v>55200006</v>
-          </cell>
-          <cell r="Y43" t="str">
-            <v>coveraoe</v>
+            <v>55200001</v>
+          </cell>
+          <cell r="AB43">
+            <v>40</v>
           </cell>
         </row>
         <row r="44">
           <cell r="A44">
-            <v>55200007</v>
-          </cell>
-          <cell r="Y44" t="str">
-            <v>coveraoe</v>
+            <v>55200002</v>
+          </cell>
+          <cell r="AB44">
+            <v>28</v>
           </cell>
         </row>
         <row r="45">
           <cell r="A45">
-            <v>55200008</v>
-          </cell>
-          <cell r="Y45" t="str">
-            <v>coveraoe</v>
+            <v>55200003</v>
+          </cell>
+          <cell r="AB45">
+            <v>25</v>
           </cell>
         </row>
         <row r="46">
           <cell r="A46">
-            <v>55200009</v>
-          </cell>
-          <cell r="Y46" t="str">
-            <v>coveraoe</v>
+            <v>55200004</v>
+          </cell>
+          <cell r="AB46">
+            <v>40</v>
           </cell>
         </row>
         <row r="47">
           <cell r="A47">
-            <v>55200010</v>
-          </cell>
-          <cell r="Y47"/>
+            <v>55200005</v>
+          </cell>
+          <cell r="AB47">
+            <v>20</v>
+          </cell>
         </row>
         <row r="48">
           <cell r="A48">
-            <v>55200011</v>
-          </cell>
-          <cell r="Y48"/>
+            <v>55200006</v>
+          </cell>
+          <cell r="AB48">
+            <v>20</v>
+          </cell>
         </row>
         <row r="49">
           <cell r="A49">
-            <v>55200012</v>
-          </cell>
-          <cell r="Y49"/>
+            <v>55200007</v>
+          </cell>
+          <cell r="AB49">
+            <v>20</v>
+          </cell>
         </row>
         <row r="50">
           <cell r="A50">
-            <v>55200013</v>
-          </cell>
-          <cell r="Y50"/>
+            <v>55200008</v>
+          </cell>
+          <cell r="AB50">
+            <v>25</v>
+          </cell>
         </row>
         <row r="51">
           <cell r="A51">
-            <v>55200014</v>
-          </cell>
-          <cell r="Y51"/>
+            <v>55200009</v>
+          </cell>
+          <cell r="AB51">
+            <v>25</v>
+          </cell>
         </row>
         <row r="52">
           <cell r="A52">
-            <v>55200015</v>
-          </cell>
-          <cell r="Y52"/>
+            <v>55200010</v>
+          </cell>
+          <cell r="AB52">
+            <v>25</v>
+          </cell>
         </row>
         <row r="53">
           <cell r="A53">
-            <v>55300001</v>
-          </cell>
-          <cell r="Y53" t="str">
-            <v>coverauro</v>
+            <v>55200011</v>
+          </cell>
+          <cell r="AB53">
+            <v>20</v>
           </cell>
         </row>
         <row r="54">
           <cell r="A54">
-            <v>55300002</v>
-          </cell>
-          <cell r="Y54"/>
+            <v>55200012</v>
+          </cell>
+          <cell r="AB54">
+            <v>30</v>
+          </cell>
         </row>
         <row r="55">
           <cell r="A55">
-            <v>55300003</v>
-          </cell>
-          <cell r="Y55"/>
+            <v>55200013</v>
+          </cell>
+          <cell r="AB55">
+            <v>10</v>
+          </cell>
         </row>
         <row r="56">
           <cell r="A56">
-            <v>55300004</v>
-          </cell>
-          <cell r="Y56"/>
+            <v>55200014</v>
+          </cell>
+          <cell r="AB56">
+            <v>25</v>
+          </cell>
         </row>
         <row r="57">
           <cell r="A57">
-            <v>55300005</v>
-          </cell>
-          <cell r="Y57"/>
+            <v>55200015</v>
+          </cell>
+          <cell r="AB57">
+            <v>20</v>
+          </cell>
         </row>
         <row r="58">
           <cell r="A58">
-            <v>55300006</v>
-          </cell>
-          <cell r="Y58"/>
+            <v>55200016</v>
+          </cell>
+          <cell r="AB58">
+            <v>30</v>
+          </cell>
         </row>
         <row r="59">
           <cell r="A59">
-            <v>55300007</v>
-          </cell>
-          <cell r="Y59"/>
+            <v>55200017</v>
+          </cell>
+          <cell r="AB59">
+            <v>35</v>
+          </cell>
         </row>
         <row r="60">
           <cell r="A60">
-            <v>55300008</v>
-          </cell>
-          <cell r="Y60"/>
+            <v>55200018</v>
+          </cell>
+          <cell r="AB60">
+            <v>50</v>
+          </cell>
         </row>
         <row r="61">
           <cell r="A61">
-            <v>55300009</v>
-          </cell>
-          <cell r="Y61"/>
+            <v>55300001</v>
+          </cell>
+          <cell r="AB61">
+            <v>40</v>
+          </cell>
         </row>
         <row r="62">
           <cell r="A62">
-            <v>55300010</v>
-          </cell>
-          <cell r="Y62"/>
+            <v>55300002</v>
+          </cell>
+          <cell r="AB62">
+            <v>30</v>
+          </cell>
         </row>
         <row r="63">
           <cell r="A63">
-            <v>55300011</v>
-          </cell>
-          <cell r="Y63"/>
+            <v>55300003</v>
+          </cell>
+          <cell r="AB63">
+            <v>30</v>
+          </cell>
         </row>
         <row r="64">
           <cell r="A64">
-            <v>55300012</v>
-          </cell>
-          <cell r="Y64"/>
+            <v>55300004</v>
+          </cell>
+          <cell r="AB64">
+            <v>30</v>
+          </cell>
         </row>
         <row r="65">
           <cell r="A65">
-            <v>55300013</v>
-          </cell>
-          <cell r="Y65"/>
+            <v>55300005</v>
+          </cell>
+          <cell r="AB65">
+            <v>30</v>
+          </cell>
         </row>
         <row r="66">
           <cell r="A66">
-            <v>55310001</v>
-          </cell>
-          <cell r="Y66"/>
+            <v>55300006</v>
+          </cell>
+          <cell r="AB66">
+            <v>25</v>
+          </cell>
         </row>
         <row r="67">
           <cell r="A67">
-            <v>55310002</v>
-          </cell>
-          <cell r="Y67"/>
+            <v>55300007</v>
+          </cell>
+          <cell r="AB67">
+            <v>25</v>
+          </cell>
         </row>
         <row r="68">
           <cell r="A68">
-            <v>55310003</v>
-          </cell>
-          <cell r="Y68"/>
+            <v>55300008</v>
+          </cell>
+          <cell r="AB68">
+            <v>30</v>
+          </cell>
         </row>
         <row r="69">
           <cell r="A69">
-            <v>55400001</v>
-          </cell>
-          <cell r="Y69"/>
+            <v>55300009</v>
+          </cell>
+          <cell r="AB69">
+            <v>30</v>
+          </cell>
         </row>
         <row r="70">
           <cell r="A70">
-            <v>55400002</v>
-          </cell>
-          <cell r="Y70"/>
+            <v>55300010</v>
+          </cell>
+          <cell r="AB70">
+            <v>35</v>
+          </cell>
         </row>
         <row r="71">
           <cell r="A71">
-            <v>55400003</v>
-          </cell>
-          <cell r="Y71"/>
+            <v>55300011</v>
+          </cell>
+          <cell r="AB71">
+            <v>25</v>
+          </cell>
         </row>
         <row r="72">
           <cell r="A72">
-            <v>55400005</v>
-          </cell>
-          <cell r="Y72"/>
+            <v>55300012</v>
+          </cell>
+          <cell r="AB72">
+            <v>5</v>
+          </cell>
         </row>
         <row r="73">
           <cell r="A73">
-            <v>55400006</v>
-          </cell>
-          <cell r="Y73"/>
+            <v>55300013</v>
+          </cell>
+          <cell r="AB73">
+            <v>25</v>
+          </cell>
         </row>
         <row r="74">
           <cell r="A74">
-            <v>55400007</v>
-          </cell>
-          <cell r="Y74"/>
+            <v>55310001</v>
+          </cell>
+          <cell r="AB74">
+            <v>100</v>
+          </cell>
         </row>
         <row r="75">
           <cell r="A75">
-            <v>55410001</v>
-          </cell>
-          <cell r="Y75"/>
+            <v>55310002</v>
+          </cell>
+          <cell r="AB75">
+            <v>15</v>
+          </cell>
         </row>
         <row r="76">
           <cell r="A76">
-            <v>55500001</v>
-          </cell>
-          <cell r="Y76"/>
+            <v>55310003</v>
+          </cell>
+          <cell r="AB76">
+            <v>13</v>
+          </cell>
         </row>
         <row r="77">
           <cell r="A77">
-            <v>55500002</v>
-          </cell>
-          <cell r="Y77"/>
+            <v>55400001</v>
+          </cell>
+          <cell r="AB77">
+            <v>80</v>
+          </cell>
         </row>
         <row r="78">
           <cell r="A78">
-            <v>55500003</v>
-          </cell>
-          <cell r="Y78"/>
+            <v>55400002</v>
+          </cell>
+          <cell r="AB78">
+            <v>80</v>
+          </cell>
         </row>
         <row r="79">
           <cell r="A79">
-            <v>55500004</v>
-          </cell>
-          <cell r="Y79"/>
+            <v>55400003</v>
+          </cell>
+          <cell r="AB79">
+            <v>80</v>
+          </cell>
         </row>
         <row r="80">
           <cell r="A80">
-            <v>55500005</v>
-          </cell>
-          <cell r="Y80"/>
+            <v>55400005</v>
+          </cell>
+          <cell r="AB80">
+            <v>55</v>
+          </cell>
         </row>
         <row r="81">
           <cell r="A81">
-            <v>55500006</v>
-          </cell>
-          <cell r="Y81"/>
+            <v>55400006</v>
+          </cell>
+          <cell r="AB81">
+            <v>30</v>
+          </cell>
         </row>
         <row r="82">
           <cell r="A82">
-            <v>55500007</v>
-          </cell>
-          <cell r="Y82"/>
+            <v>55400007</v>
+          </cell>
+          <cell r="AB82">
+            <v>25</v>
+          </cell>
         </row>
         <row r="83">
           <cell r="A83">
-            <v>55500008</v>
-          </cell>
-          <cell r="Y83"/>
+            <v>55400008</v>
+          </cell>
+          <cell r="AB83">
+            <v>35</v>
+          </cell>
         </row>
         <row r="84">
           <cell r="A84">
-            <v>55500009</v>
-          </cell>
-          <cell r="Y84"/>
+            <v>55410001</v>
+          </cell>
+          <cell r="AB84">
+            <v>50</v>
+          </cell>
         </row>
         <row r="85">
           <cell r="A85">
-            <v>55500010</v>
-          </cell>
-          <cell r="Y85"/>
+            <v>55500001</v>
+          </cell>
+          <cell r="AB85">
+            <v>5</v>
+          </cell>
         </row>
         <row r="86">
           <cell r="A86">
-            <v>55500011</v>
-          </cell>
-          <cell r="Y86"/>
+            <v>55500002</v>
+          </cell>
+          <cell r="AB86">
+            <v>5</v>
+          </cell>
         </row>
         <row r="87">
           <cell r="A87">
-            <v>55500012</v>
-          </cell>
-          <cell r="Y87"/>
+            <v>55500003</v>
+          </cell>
+          <cell r="AB87">
+            <v>5</v>
+          </cell>
         </row>
         <row r="88">
           <cell r="A88">
-            <v>55500013</v>
-          </cell>
-          <cell r="Y88"/>
+            <v>55500004</v>
+          </cell>
+          <cell r="AB88">
+            <v>5</v>
+          </cell>
         </row>
         <row r="89">
           <cell r="A89">
-            <v>55500014</v>
-          </cell>
-          <cell r="Y89"/>
+            <v>55500005</v>
+          </cell>
+          <cell r="AB89">
+            <v>5</v>
+          </cell>
         </row>
         <row r="90">
           <cell r="A90">
-            <v>55500015</v>
-          </cell>
-          <cell r="Y90"/>
+            <v>55500006</v>
+          </cell>
+          <cell r="AB90">
+            <v>5</v>
+          </cell>
         </row>
         <row r="91">
           <cell r="A91">
-            <v>55500016</v>
-          </cell>
-          <cell r="Y91"/>
+            <v>55500007</v>
+          </cell>
+          <cell r="AB91">
+            <v>5</v>
+          </cell>
         </row>
         <row r="92">
           <cell r="A92">
-            <v>55510001</v>
-          </cell>
-          <cell r="Y92"/>
+            <v>55500008</v>
+          </cell>
+          <cell r="AB92">
+            <v>5</v>
+          </cell>
         </row>
         <row r="93">
           <cell r="A93">
-            <v>55510002</v>
-          </cell>
-          <cell r="Y93"/>
+            <v>55500009</v>
+          </cell>
+          <cell r="AB93">
+            <v>5</v>
+          </cell>
         </row>
         <row r="94">
           <cell r="A94">
-            <v>55510003</v>
-          </cell>
-          <cell r="Y94"/>
+            <v>55500010</v>
+          </cell>
+          <cell r="AB94">
+            <v>5</v>
+          </cell>
         </row>
         <row r="95">
           <cell r="A95">
-            <v>55510004</v>
-          </cell>
-          <cell r="Y95"/>
+            <v>55500011</v>
+          </cell>
+          <cell r="AB95">
+            <v>5</v>
+          </cell>
         </row>
         <row r="96">
           <cell r="A96">
-            <v>55510006</v>
-          </cell>
-          <cell r="Y96"/>
+            <v>55500012</v>
+          </cell>
+          <cell r="AB96">
+            <v>5</v>
+          </cell>
         </row>
         <row r="97">
           <cell r="A97">
-            <v>55510007</v>
-          </cell>
-          <cell r="Y97"/>
+            <v>55500013</v>
+          </cell>
+          <cell r="AB97">
+            <v>5</v>
+          </cell>
         </row>
         <row r="98">
           <cell r="A98">
-            <v>55510009</v>
-          </cell>
-          <cell r="Y98"/>
+            <v>55500014</v>
+          </cell>
+          <cell r="AB98">
+            <v>5</v>
+          </cell>
         </row>
         <row r="99">
           <cell r="A99">
-            <v>55510010</v>
-          </cell>
-          <cell r="Y99"/>
+            <v>55500015</v>
+          </cell>
+          <cell r="AB99">
+            <v>5</v>
+          </cell>
         </row>
         <row r="100">
           <cell r="A100">
-            <v>55510011</v>
-          </cell>
-          <cell r="Y100"/>
+            <v>55500016</v>
+          </cell>
+          <cell r="AB100">
+            <v>5</v>
+          </cell>
         </row>
         <row r="101">
           <cell r="A101">
-            <v>55510012</v>
-          </cell>
-          <cell r="Y101"/>
+            <v>55510001</v>
+          </cell>
+          <cell r="AB101">
+            <v>12</v>
+          </cell>
         </row>
         <row r="102">
           <cell r="A102">
-            <v>55510013</v>
-          </cell>
-          <cell r="Y102"/>
+            <v>55510002</v>
+          </cell>
+          <cell r="AB102">
+            <v>15</v>
+          </cell>
         </row>
         <row r="103">
           <cell r="A103">
-            <v>55510014</v>
-          </cell>
-          <cell r="Y103"/>
+            <v>55510003</v>
+          </cell>
+          <cell r="AB103">
+            <v>15</v>
+          </cell>
         </row>
         <row r="104">
           <cell r="A104">
-            <v>55510018</v>
-          </cell>
-          <cell r="Y104"/>
+            <v>55510004</v>
+          </cell>
+          <cell r="AB104">
+            <v>12</v>
+          </cell>
         </row>
         <row r="105">
           <cell r="A105">
-            <v>55510019</v>
-          </cell>
-          <cell r="Y105"/>
+            <v>55510006</v>
+          </cell>
+          <cell r="AB105">
+            <v>25</v>
+          </cell>
         </row>
         <row r="106">
           <cell r="A106">
-            <v>55520001</v>
-          </cell>
-          <cell r="Y106"/>
+            <v>55510007</v>
+          </cell>
+          <cell r="AB106">
+            <v>10</v>
+          </cell>
         </row>
         <row r="107">
           <cell r="A107">
-            <v>55520002</v>
-          </cell>
-          <cell r="Y107"/>
+            <v>55510009</v>
+          </cell>
+          <cell r="AB107">
+            <v>50</v>
+          </cell>
         </row>
         <row r="108">
           <cell r="A108">
-            <v>55520003</v>
-          </cell>
-          <cell r="Y108"/>
+            <v>55510010</v>
+          </cell>
+          <cell r="AB108">
+            <v>10</v>
+          </cell>
         </row>
         <row r="109">
           <cell r="A109">
-            <v>55600001</v>
-          </cell>
-          <cell r="Y109" t="str">
-            <v>coverauro</v>
+            <v>55510011</v>
+          </cell>
+          <cell r="AB109">
+            <v>15</v>
           </cell>
         </row>
         <row r="110">
           <cell r="A110">
-            <v>55600002</v>
-          </cell>
-          <cell r="Y110" t="str">
-            <v>coverauro</v>
+            <v>55510012</v>
+          </cell>
+          <cell r="AB110">
+            <v>62</v>
           </cell>
         </row>
         <row r="111">
           <cell r="A111">
-            <v>55600004</v>
-          </cell>
-          <cell r="Y111" t="str">
-            <v>coverauro</v>
+            <v>55510013</v>
+          </cell>
+          <cell r="AB111">
+            <v>12</v>
           </cell>
         </row>
         <row r="112">
           <cell r="A112">
-            <v>55600005</v>
-          </cell>
-          <cell r="Y112" t="str">
-            <v>coverauro</v>
+            <v>55510014</v>
+          </cell>
+          <cell r="AB112">
+            <v>25</v>
           </cell>
         </row>
         <row r="113">
           <cell r="A113">
-            <v>55600006</v>
-          </cell>
-          <cell r="Y113" t="str">
-            <v>coverauro</v>
+            <v>55510018</v>
+          </cell>
+          <cell r="AB113">
+            <v>37</v>
           </cell>
         </row>
         <row r="114">
           <cell r="A114">
-            <v>55600007</v>
-          </cell>
-          <cell r="Y114" t="str">
-            <v>coverauro</v>
+            <v>55510019</v>
+          </cell>
+          <cell r="AB114">
+            <v>37</v>
           </cell>
         </row>
         <row r="115">
           <cell r="A115">
-            <v>55600008</v>
-          </cell>
-          <cell r="Y115" t="str">
-            <v>coverauro</v>
+            <v>55520001</v>
+          </cell>
+          <cell r="AB115">
+            <v>-25</v>
           </cell>
         </row>
         <row r="116">
           <cell r="A116">
-            <v>55600009</v>
-          </cell>
-          <cell r="Y116" t="str">
-            <v>coverauro</v>
+            <v>55520002</v>
+          </cell>
+          <cell r="AB116">
+            <v>62</v>
           </cell>
         </row>
         <row r="117">
           <cell r="A117">
-            <v>55600010</v>
-          </cell>
-          <cell r="Y117" t="str">
-            <v>coverauro</v>
+            <v>55520003</v>
+          </cell>
+          <cell r="AB117">
+            <v>27</v>
           </cell>
         </row>
         <row r="118">
           <cell r="A118">
-            <v>55600011</v>
-          </cell>
-          <cell r="Y118" t="str">
-            <v>coverauro</v>
+            <v>55600001</v>
+          </cell>
+          <cell r="AB118">
+            <v>8</v>
           </cell>
         </row>
         <row r="119">
           <cell r="A119">
-            <v>55600012</v>
-          </cell>
-          <cell r="Y119" t="str">
-            <v>coverauro</v>
+            <v>55600002</v>
+          </cell>
+          <cell r="AB119">
+            <v>10</v>
           </cell>
         </row>
         <row r="120">
           <cell r="A120">
-            <v>55600013</v>
-          </cell>
-          <cell r="Y120" t="str">
-            <v>coverauro</v>
+            <v>55600004</v>
+          </cell>
+          <cell r="AB120">
+            <v>8</v>
           </cell>
         </row>
         <row r="121">
           <cell r="A121">
-            <v>55600014</v>
-          </cell>
-          <cell r="Y121" t="str">
-            <v>coverauro</v>
+            <v>55600005</v>
+          </cell>
+          <cell r="AB121">
+            <v>15</v>
           </cell>
         </row>
         <row r="122">
           <cell r="A122">
-            <v>55600015</v>
-          </cell>
-          <cell r="Y122" t="str">
-            <v>coverauro</v>
+            <v>55600006</v>
+          </cell>
+          <cell r="AB122">
+            <v>15</v>
           </cell>
         </row>
         <row r="123">
           <cell r="A123">
-            <v>55600016</v>
-          </cell>
-          <cell r="Y123" t="str">
-            <v>coverauro</v>
+            <v>55600007</v>
+          </cell>
+          <cell r="AB123">
+            <v>20</v>
           </cell>
         </row>
         <row r="124">
           <cell r="A124">
-            <v>55610001</v>
-          </cell>
-          <cell r="Y124"/>
+            <v>55600008</v>
+          </cell>
+          <cell r="AB124">
+            <v>30</v>
+          </cell>
         </row>
         <row r="125">
           <cell r="A125">
-            <v>55610002</v>
-          </cell>
-          <cell r="Y125"/>
+            <v>55600009</v>
+          </cell>
+          <cell r="AB125">
+            <v>13</v>
+          </cell>
         </row>
         <row r="126">
           <cell r="A126">
-            <v>55610003</v>
-          </cell>
-          <cell r="Y126"/>
+            <v>55600010</v>
+          </cell>
+          <cell r="AB126">
+            <v>30</v>
+          </cell>
         </row>
         <row r="127">
           <cell r="A127">
-            <v>55610004</v>
-          </cell>
-          <cell r="Y127"/>
+            <v>55600011</v>
+          </cell>
+          <cell r="AB127">
+            <v>20</v>
+          </cell>
         </row>
         <row r="128">
           <cell r="A128">
-            <v>55700001</v>
-          </cell>
-          <cell r="Y128"/>
+            <v>55600012</v>
+          </cell>
+          <cell r="AB128">
+            <v>30</v>
+          </cell>
         </row>
         <row r="129">
           <cell r="A129">
-            <v>55700002</v>
-          </cell>
-          <cell r="Y129"/>
+            <v>55600013</v>
+          </cell>
+          <cell r="AB129">
+            <v>15</v>
+          </cell>
         </row>
         <row r="130">
           <cell r="A130">
-            <v>55700003</v>
-          </cell>
-          <cell r="Y130"/>
+            <v>55600014</v>
+          </cell>
+          <cell r="AB130">
+            <v>30</v>
+          </cell>
         </row>
         <row r="131">
           <cell r="A131">
-            <v>55700004</v>
-          </cell>
-          <cell r="Y131"/>
+            <v>55600015</v>
+          </cell>
+          <cell r="AB131">
+            <v>10</v>
+          </cell>
         </row>
         <row r="132">
           <cell r="A132">
-            <v>55700005</v>
-          </cell>
-          <cell r="Y132"/>
+            <v>55600016</v>
+          </cell>
+          <cell r="AB132">
+            <v>15</v>
+          </cell>
         </row>
         <row r="133">
           <cell r="A133">
-            <v>55700006</v>
-          </cell>
-          <cell r="Y133"/>
+            <v>55600017</v>
+          </cell>
+          <cell r="AB133">
+            <v>20</v>
+          </cell>
         </row>
         <row r="134">
           <cell r="A134">
-            <v>55700007</v>
-          </cell>
-          <cell r="Y134"/>
+            <v>55610001</v>
+          </cell>
+          <cell r="AB134">
+            <v>30</v>
+          </cell>
         </row>
         <row r="135">
           <cell r="A135">
-            <v>55900001</v>
-          </cell>
-          <cell r="Y135" t="str">
-            <v>covertrans</v>
+            <v>55610002</v>
+          </cell>
+          <cell r="AB135">
+            <v>5</v>
           </cell>
         </row>
         <row r="136">
           <cell r="A136">
-            <v>55900002</v>
-          </cell>
-          <cell r="Y136"/>
+            <v>55610003</v>
+          </cell>
+          <cell r="AB136">
+            <v>5</v>
+          </cell>
         </row>
         <row r="137">
           <cell r="A137">
-            <v>55900003</v>
-          </cell>
-          <cell r="Y137"/>
+            <v>55610004</v>
+          </cell>
+          <cell r="AB137">
+            <v>10</v>
+          </cell>
         </row>
         <row r="138">
           <cell r="A138">
-            <v>55900004</v>
-          </cell>
-          <cell r="Y138"/>
+            <v>55700001</v>
+          </cell>
+          <cell r="AB138">
+            <v>20</v>
+          </cell>
         </row>
         <row r="139">
           <cell r="A139">
-            <v>55900005</v>
-          </cell>
-          <cell r="Y139"/>
+            <v>55700002</v>
+          </cell>
+          <cell r="AB139">
+            <v>20</v>
+          </cell>
         </row>
         <row r="140">
           <cell r="A140">
-            <v>55900006</v>
-          </cell>
-          <cell r="Y140"/>
+            <v>55700003</v>
+          </cell>
+          <cell r="AB140">
+            <v>20</v>
+          </cell>
         </row>
         <row r="141">
           <cell r="A141">
-            <v>55900007</v>
-          </cell>
-          <cell r="Y141"/>
+            <v>55700004</v>
+          </cell>
+          <cell r="AB141">
+            <v>20</v>
+          </cell>
         </row>
         <row r="142">
           <cell r="A142">
-            <v>55900008</v>
-          </cell>
-          <cell r="Y142"/>
+            <v>55700005</v>
+          </cell>
+          <cell r="AB142">
+            <v>40</v>
+          </cell>
         </row>
         <row r="143">
           <cell r="A143">
-            <v>55900009</v>
-          </cell>
-          <cell r="Y143"/>
+            <v>55700006</v>
+          </cell>
+          <cell r="AB143">
+            <v>50</v>
+          </cell>
         </row>
         <row r="144">
           <cell r="A144">
-            <v>55900010</v>
-          </cell>
-          <cell r="Y144"/>
+            <v>55700007</v>
+          </cell>
+          <cell r="AB144">
+            <v>35</v>
+          </cell>
         </row>
         <row r="145">
           <cell r="A145">
-            <v>55900011</v>
-          </cell>
-          <cell r="Y145"/>
+            <v>55900001</v>
+          </cell>
+          <cell r="AB145">
+            <v>35</v>
+          </cell>
         </row>
         <row r="146">
           <cell r="A146">
-            <v>55900012</v>
-          </cell>
-          <cell r="Y146"/>
+            <v>55900002</v>
+          </cell>
+          <cell r="AB146">
+            <v>30</v>
+          </cell>
         </row>
         <row r="147">
           <cell r="A147">
-            <v>55900013</v>
-          </cell>
-          <cell r="Y147"/>
+            <v>55900003</v>
+          </cell>
+          <cell r="AB147">
+            <v>80</v>
+          </cell>
         </row>
         <row r="148">
           <cell r="A148">
-            <v>55900014</v>
-          </cell>
-          <cell r="Y148"/>
+            <v>55900004</v>
+          </cell>
+          <cell r="AB148">
+            <v>15</v>
+          </cell>
         </row>
         <row r="149">
           <cell r="A149">
-            <v>55900015</v>
-          </cell>
-          <cell r="Y149"/>
+            <v>55900005</v>
+          </cell>
+          <cell r="AB149">
+            <v>20</v>
+          </cell>
         </row>
         <row r="150">
           <cell r="A150">
-            <v>55900016</v>
-          </cell>
-          <cell r="Y150"/>
+            <v>55900006</v>
+          </cell>
+          <cell r="AB150">
+            <v>35</v>
+          </cell>
         </row>
         <row r="151">
           <cell r="A151">
-            <v>55900017</v>
-          </cell>
-          <cell r="Y151" t="str">
-            <v>covertrans</v>
+            <v>55900007</v>
+          </cell>
+          <cell r="AB151">
+            <v>25</v>
           </cell>
         </row>
         <row r="152">
           <cell r="A152">
-            <v>55900018</v>
-          </cell>
-          <cell r="Y152" t="str">
-            <v>covertrans</v>
+            <v>55900008</v>
+          </cell>
+          <cell r="AB152">
+            <v>40</v>
           </cell>
         </row>
         <row r="153">
           <cell r="A153">
-            <v>55900019</v>
-          </cell>
-          <cell r="Y153" t="str">
-            <v>covertrans</v>
+            <v>55900009</v>
+          </cell>
+          <cell r="AB153">
+            <v>30</v>
           </cell>
         </row>
         <row r="154">
           <cell r="A154">
-            <v>55900020</v>
-          </cell>
-          <cell r="Y154"/>
+            <v>55900010</v>
+          </cell>
+          <cell r="AB154">
+            <v>20</v>
+          </cell>
         </row>
         <row r="155">
           <cell r="A155">
-            <v>55900021</v>
-          </cell>
-          <cell r="Y155"/>
+            <v>55900011</v>
+          </cell>
+          <cell r="AB155">
+            <v>15</v>
+          </cell>
         </row>
         <row r="156">
           <cell r="A156">
-            <v>55900022</v>
-          </cell>
-          <cell r="Y156"/>
+            <v>55900012</v>
+          </cell>
+          <cell r="AB156">
+            <v>25</v>
+          </cell>
         </row>
         <row r="157">
           <cell r="A157">
-            <v>55900023</v>
-          </cell>
-          <cell r="Y157"/>
+            <v>55900013</v>
+          </cell>
+          <cell r="AB157">
+            <v>10</v>
+          </cell>
         </row>
         <row r="158">
           <cell r="A158">
-            <v>55900024</v>
-          </cell>
-          <cell r="Y158"/>
+            <v>55900014</v>
+          </cell>
+          <cell r="AB158">
+            <v>20</v>
+          </cell>
         </row>
         <row r="159">
           <cell r="A159">
-            <v>55900025</v>
-          </cell>
-          <cell r="Y159"/>
+            <v>55900015</v>
+          </cell>
+          <cell r="AB159">
+            <v>30</v>
+          </cell>
         </row>
         <row r="160">
           <cell r="A160">
-            <v>55900026</v>
-          </cell>
-          <cell r="Y160"/>
+            <v>55900016</v>
+          </cell>
+          <cell r="AB160">
+            <v>45</v>
+          </cell>
         </row>
         <row r="161">
           <cell r="A161">
-            <v>55900027</v>
-          </cell>
-          <cell r="Y161"/>
+            <v>55900017</v>
+          </cell>
+          <cell r="AB161">
+            <v>10</v>
+          </cell>
         </row>
         <row r="162">
           <cell r="A162">
-            <v>55900028</v>
-          </cell>
-          <cell r="Y162"/>
+            <v>55900018</v>
+          </cell>
+          <cell r="AB162">
+            <v>30</v>
+          </cell>
         </row>
         <row r="163">
           <cell r="A163">
-            <v>55900029</v>
-          </cell>
-          <cell r="Y163"/>
+            <v>55900019</v>
+          </cell>
+          <cell r="AB163">
+            <v>80</v>
+          </cell>
         </row>
         <row r="164">
           <cell r="A164">
-            <v>55900030</v>
-          </cell>
-          <cell r="Y164"/>
+            <v>55900020</v>
+          </cell>
+          <cell r="AB164">
+            <v>20</v>
+          </cell>
         </row>
         <row r="165">
           <cell r="A165">
-            <v>55900031</v>
-          </cell>
-          <cell r="Y165"/>
+            <v>55900021</v>
+          </cell>
+          <cell r="AB165">
+            <v>10</v>
+          </cell>
         </row>
         <row r="166">
           <cell r="A166">
-            <v>55900032</v>
-          </cell>
-          <cell r="Y166"/>
+            <v>55900022</v>
+          </cell>
+          <cell r="AB166">
+            <v>20</v>
+          </cell>
         </row>
         <row r="167">
           <cell r="A167">
-            <v>55900033</v>
-          </cell>
-          <cell r="Y167"/>
+            <v>55900023</v>
+          </cell>
+          <cell r="AB167">
+            <v>25</v>
+          </cell>
         </row>
         <row r="168">
           <cell r="A168">
-            <v>55900034</v>
-          </cell>
-          <cell r="Y168"/>
+            <v>55900024</v>
+          </cell>
+          <cell r="AB168">
+            <v>10</v>
+          </cell>
         </row>
         <row r="169">
           <cell r="A169">
-            <v>55900035</v>
-          </cell>
-          <cell r="Y169"/>
+            <v>55900025</v>
+          </cell>
+          <cell r="AB169">
+            <v>10</v>
+          </cell>
         </row>
         <row r="170">
           <cell r="A170">
-            <v>55900036</v>
-          </cell>
-          <cell r="Y170"/>
+            <v>55900026</v>
+          </cell>
+          <cell r="AB170">
+            <v>20</v>
+          </cell>
         </row>
         <row r="171">
           <cell r="A171">
-            <v>55900037</v>
-          </cell>
-          <cell r="Y171"/>
+            <v>55900027</v>
+          </cell>
+          <cell r="AB171">
+            <v>35</v>
+          </cell>
         </row>
         <row r="172">
           <cell r="A172">
-            <v>55900038</v>
-          </cell>
-          <cell r="Y172"/>
+            <v>55900028</v>
+          </cell>
         </row>
         <row r="173">
           <cell r="A173">
-            <v>55900039</v>
-          </cell>
-          <cell r="Y173" t="str">
-            <v>coverstar</v>
+            <v>55900029</v>
+          </cell>
+          <cell r="AB173">
+            <v>15</v>
           </cell>
         </row>
         <row r="174">
           <cell r="A174">
-            <v>55900040</v>
-          </cell>
-          <cell r="Y174"/>
+            <v>55900030</v>
+          </cell>
+          <cell r="AB174">
+            <v>15</v>
+          </cell>
         </row>
         <row r="175">
           <cell r="A175">
-            <v>55900041</v>
-          </cell>
-          <cell r="Y175"/>
+            <v>55900031</v>
+          </cell>
+          <cell r="AB175">
+            <v>5</v>
+          </cell>
         </row>
         <row r="176">
           <cell r="A176">
-            <v>55900042</v>
-          </cell>
-          <cell r="Y176"/>
+            <v>55900032</v>
+          </cell>
+          <cell r="AB176">
+            <v>20</v>
+          </cell>
         </row>
         <row r="177">
           <cell r="A177">
-            <v>55900043</v>
-          </cell>
-          <cell r="Y177"/>
+            <v>55900033</v>
+          </cell>
+          <cell r="AB177">
+            <v>20</v>
+          </cell>
         </row>
         <row r="178">
           <cell r="A178">
-            <v>55900044</v>
-          </cell>
-          <cell r="Y178"/>
+            <v>55900034</v>
+          </cell>
+          <cell r="AB178">
+            <v>14</v>
+          </cell>
         </row>
         <row r="179">
           <cell r="A179">
-            <v>55900045</v>
-          </cell>
-          <cell r="Y179"/>
+            <v>55900035</v>
+          </cell>
+          <cell r="AB179">
+            <v>14</v>
+          </cell>
         </row>
         <row r="180">
           <cell r="A180">
-            <v>55900046</v>
-          </cell>
-          <cell r="Y180"/>
+            <v>55900036</v>
+          </cell>
+          <cell r="AB180">
+            <v>50</v>
+          </cell>
         </row>
         <row r="181">
           <cell r="A181">
-            <v>55900047</v>
-          </cell>
-          <cell r="Y181"/>
+            <v>55900037</v>
+          </cell>
+          <cell r="AB181">
+            <v>35</v>
+          </cell>
         </row>
         <row r="182">
           <cell r="A182">
-            <v>55900048</v>
-          </cell>
-          <cell r="Y182"/>
+            <v>55900038</v>
+          </cell>
+          <cell r="AB182">
+            <v>40</v>
+          </cell>
         </row>
         <row r="183">
           <cell r="A183">
-            <v>55900049</v>
-          </cell>
-          <cell r="Y183"/>
+            <v>55900039</v>
+          </cell>
+          <cell r="AB183">
+            <v>40</v>
+          </cell>
         </row>
         <row r="184">
           <cell r="A184">
-            <v>55900050</v>
-          </cell>
-          <cell r="Y184"/>
+            <v>55900040</v>
+          </cell>
+          <cell r="AB184">
+            <v>30</v>
+          </cell>
         </row>
         <row r="185">
           <cell r="A185">
-            <v>55900051</v>
-          </cell>
-          <cell r="Y185"/>
+            <v>55900041</v>
+          </cell>
+          <cell r="AB185">
+            <v>0</v>
+          </cell>
         </row>
         <row r="186">
           <cell r="A186">
-            <v>55900052</v>
-          </cell>
-          <cell r="Y186"/>
+            <v>55900042</v>
+          </cell>
+          <cell r="AB186">
+            <v>25</v>
+          </cell>
         </row>
         <row r="187">
           <cell r="A187">
-            <v>55900053</v>
-          </cell>
-          <cell r="Y187"/>
+            <v>55900043</v>
+          </cell>
+          <cell r="AB187">
+            <v>30</v>
+          </cell>
         </row>
         <row r="188">
           <cell r="A188">
-            <v>55900054</v>
-          </cell>
-          <cell r="Y188"/>
+            <v>55900044</v>
+          </cell>
+          <cell r="AB188">
+            <v>40</v>
+          </cell>
         </row>
         <row r="189">
           <cell r="A189">
-            <v>55900055</v>
-          </cell>
-          <cell r="Y189"/>
+            <v>55900045</v>
+          </cell>
+          <cell r="AB189">
+            <v>25</v>
+          </cell>
         </row>
         <row r="190">
           <cell r="A190">
-            <v>55900056</v>
-          </cell>
-          <cell r="Y190"/>
+            <v>55900046</v>
+          </cell>
+          <cell r="AB190">
+            <v>25</v>
+          </cell>
         </row>
         <row r="191">
           <cell r="A191">
-            <v>55990001</v>
-          </cell>
-          <cell r="Y191"/>
+            <v>55900047</v>
+          </cell>
+          <cell r="AB191">
+            <v>30</v>
+          </cell>
         </row>
         <row r="192">
           <cell r="A192">
-            <v>55990002</v>
-          </cell>
-          <cell r="Y192"/>
+            <v>55900048</v>
+          </cell>
+          <cell r="AB192">
+            <v>60</v>
+          </cell>
         </row>
         <row r="193">
           <cell r="A193">
-            <v>55990003</v>
-          </cell>
-          <cell r="Y193"/>
+            <v>55900049</v>
+          </cell>
+          <cell r="AB193">
+            <v>25</v>
+          </cell>
         </row>
         <row r="194">
           <cell r="A194">
-            <v>55990004</v>
-          </cell>
-          <cell r="Y194"/>
+            <v>55900050</v>
+          </cell>
+          <cell r="AB194">
+            <v>20</v>
+          </cell>
         </row>
         <row r="195">
           <cell r="A195">
-            <v>55990005</v>
-          </cell>
-          <cell r="Y195"/>
+            <v>55900051</v>
+          </cell>
+          <cell r="AB195">
+            <v>25</v>
+          </cell>
         </row>
         <row r="196">
           <cell r="A196">
-            <v>55990006</v>
-          </cell>
-          <cell r="Y196"/>
+            <v>55900052</v>
+          </cell>
+          <cell r="AB196">
+            <v>5</v>
+          </cell>
         </row>
         <row r="197">
           <cell r="A197">
-            <v>55990011</v>
-          </cell>
-          <cell r="Y197"/>
+            <v>55900053</v>
+          </cell>
+          <cell r="AB197">
+            <v>30</v>
+          </cell>
         </row>
         <row r="198">
           <cell r="A198">
-            <v>55990012</v>
-          </cell>
-          <cell r="Y198"/>
+            <v>55900054</v>
+          </cell>
+          <cell r="AB198">
+            <v>15</v>
+          </cell>
         </row>
         <row r="199">
           <cell r="A199">
-            <v>55990013</v>
-          </cell>
-          <cell r="Y199"/>
+            <v>55900055</v>
+          </cell>
+          <cell r="AB199">
+            <v>15</v>
+          </cell>
         </row>
         <row r="200">
           <cell r="A200">
-            <v>55990014</v>
-          </cell>
-          <cell r="Y200"/>
+            <v>55900056</v>
+          </cell>
+          <cell r="AB200">
+            <v>10</v>
+          </cell>
         </row>
         <row r="201">
           <cell r="A201">
-            <v>55990015</v>
-          </cell>
-          <cell r="Y201"/>
+            <v>55900057</v>
+          </cell>
+          <cell r="AB201">
+            <v>40</v>
+          </cell>
         </row>
         <row r="202">
           <cell r="A202">
-            <v>55990016</v>
-          </cell>
-          <cell r="Y202"/>
+            <v>55900058</v>
+          </cell>
+          <cell r="AB202">
+            <v>80</v>
+          </cell>
         </row>
         <row r="203">
           <cell r="A203">
-            <v>55990101</v>
-          </cell>
-          <cell r="Y203"/>
+            <v>55900059</v>
+          </cell>
+          <cell r="AB203">
+            <v>-30</v>
+          </cell>
         </row>
         <row r="204">
           <cell r="A204">
-            <v>55990102</v>
-          </cell>
-          <cell r="Y204"/>
+            <v>55900060</v>
+          </cell>
+          <cell r="AB204">
+            <v>60</v>
+          </cell>
         </row>
         <row r="205">
           <cell r="A205">
-            <v>55990103</v>
-          </cell>
-          <cell r="Y205"/>
+            <v>55900061</v>
+          </cell>
+          <cell r="AB205">
+            <v>20</v>
+          </cell>
         </row>
         <row r="206">
           <cell r="A206">
-            <v>55990104</v>
-          </cell>
-          <cell r="Y206"/>
+            <v>55900062</v>
+          </cell>
+          <cell r="AB206">
+            <v>15</v>
+          </cell>
         </row>
         <row r="207">
           <cell r="A207">
-            <v>55990105</v>
-          </cell>
-          <cell r="Y207"/>
+            <v>55990001</v>
+          </cell>
+          <cell r="AB207">
+            <v>10</v>
+          </cell>
         </row>
         <row r="208">
           <cell r="A208">
-            <v>55990106</v>
-          </cell>
-          <cell r="Y208"/>
+            <v>55990002</v>
+          </cell>
+          <cell r="AB208">
+            <v>10</v>
+          </cell>
         </row>
         <row r="209">
           <cell r="A209">
-            <v>55990107</v>
-          </cell>
-          <cell r="Y209"/>
+            <v>55990003</v>
+          </cell>
+          <cell r="AB209">
+            <v>10</v>
+          </cell>
         </row>
         <row r="210">
           <cell r="A210">
-            <v>55990108</v>
-          </cell>
-          <cell r="Y210"/>
+            <v>55990004</v>
+          </cell>
+          <cell r="AB210">
+            <v>10</v>
+          </cell>
         </row>
         <row r="211">
           <cell r="A211">
+            <v>55990005</v>
+          </cell>
+          <cell r="AB211">
+            <v>10</v>
+          </cell>
+        </row>
+        <row r="212">
+          <cell r="A212">
+            <v>55990006</v>
+          </cell>
+          <cell r="AB212">
+            <v>10</v>
+          </cell>
+        </row>
+        <row r="213">
+          <cell r="A213">
+            <v>55990011</v>
+          </cell>
+          <cell r="AB213">
+            <v>10</v>
+          </cell>
+        </row>
+        <row r="214">
+          <cell r="A214">
+            <v>55990012</v>
+          </cell>
+          <cell r="AB214">
+            <v>10</v>
+          </cell>
+        </row>
+        <row r="215">
+          <cell r="A215">
+            <v>55990013</v>
+          </cell>
+          <cell r="AB215">
+            <v>10</v>
+          </cell>
+        </row>
+        <row r="216">
+          <cell r="A216">
+            <v>55990014</v>
+          </cell>
+          <cell r="AB216">
+            <v>10</v>
+          </cell>
+        </row>
+        <row r="217">
+          <cell r="A217">
+            <v>55990015</v>
+          </cell>
+          <cell r="AB217">
+            <v>10</v>
+          </cell>
+        </row>
+        <row r="218">
+          <cell r="A218">
+            <v>55990016</v>
+          </cell>
+          <cell r="AB218">
+            <v>10</v>
+          </cell>
+        </row>
+        <row r="219">
+          <cell r="A219">
+            <v>55990101</v>
+          </cell>
+          <cell r="AB219">
+            <v>15</v>
+          </cell>
+        </row>
+        <row r="220">
+          <cell r="A220">
+            <v>55990102</v>
+          </cell>
+          <cell r="AB220">
+            <v>25</v>
+          </cell>
+        </row>
+        <row r="221">
+          <cell r="A221">
+            <v>55990103</v>
+          </cell>
+          <cell r="AB221">
+            <v>35</v>
+          </cell>
+        </row>
+        <row r="222">
+          <cell r="A222">
+            <v>55990104</v>
+          </cell>
+          <cell r="AB222">
+            <v>50</v>
+          </cell>
+        </row>
+        <row r="223">
+          <cell r="A223">
+            <v>55990105</v>
+          </cell>
+          <cell r="AB223">
+            <v>150</v>
+          </cell>
+        </row>
+        <row r="224">
+          <cell r="A224">
+            <v>55990106</v>
+          </cell>
+          <cell r="AB224">
+            <v>80</v>
+          </cell>
+        </row>
+        <row r="225">
+          <cell r="A225">
+            <v>55990107</v>
+          </cell>
+          <cell r="AB225">
+            <v>50</v>
+          </cell>
+        </row>
+        <row r="226">
+          <cell r="A226">
+            <v>55990108</v>
+          </cell>
+          <cell r="AB226">
+            <v>4</v>
+          </cell>
+        </row>
+        <row r="227">
+          <cell r="A227">
             <v>55990109</v>
           </cell>
-          <cell r="Y211"/>
+          <cell r="AB227">
+            <v>15</v>
+          </cell>
         </row>
       </sheetData>
       <sheetData sheetId="1"/>
@@ -4500,49 +5050,49 @@
   <tableColumns count="37">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="Name"/>
-    <tableColumn id="34" name="Ename" dataDxfId="39"/>
-    <tableColumn id="32" name="Des" dataDxfId="38"/>
-    <tableColumn id="3" name="Quality" dataDxfId="37">
+    <tableColumn id="34" name="Ename" dataDxfId="45"/>
+    <tableColumn id="32" name="Des" dataDxfId="44"/>
+    <tableColumn id="3" name="Quality" dataDxfId="43">
       <calculatedColumnFormula>IF(T4&gt;=23,4,IF(AND(T4&gt;=18,T4&lt;23),3,IF(AND(T4&gt;=13,T4&lt;18),2,IF(AND(T4&gt;=8,T4&lt;13),1,0))))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" name="Position"/>
-    <tableColumn id="19" name="Value" dataDxfId="36">
+    <tableColumn id="19" name="Value" dataDxfId="42">
       <calculatedColumnFormula>E4*50+50</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="35" name="ComposeStone" dataDxfId="35"/>
-    <tableColumn id="36" name="ComposeWood" dataDxfId="34"/>
-    <tableColumn id="15" name="ComposeItemId" dataDxfId="33"/>
-    <tableColumn id="11" name="AtkR" dataDxfId="32"/>
-    <tableColumn id="8" name="VitR" dataDxfId="31"/>
-    <tableColumn id="6" name="Def" dataDxfId="30"/>
-    <tableColumn id="22" name="Mag" dataDxfId="29"/>
-    <tableColumn id="27" name="Spd" dataDxfId="28"/>
-    <tableColumn id="26" name="Hit" dataDxfId="27"/>
-    <tableColumn id="25" name="Dhit" dataDxfId="26"/>
-    <tableColumn id="24" name="Crt" dataDxfId="25"/>
-    <tableColumn id="23" name="Luk" dataDxfId="24"/>
-    <tableColumn id="28" name="Sum" dataDxfId="23">
+    <tableColumn id="35" name="ComposeStone" dataDxfId="41"/>
+    <tableColumn id="36" name="ComposeWood" dataDxfId="40"/>
+    <tableColumn id="15" name="ComposeItemId" dataDxfId="39"/>
+    <tableColumn id="11" name="AtkR" dataDxfId="38"/>
+    <tableColumn id="8" name="VitR" dataDxfId="37"/>
+    <tableColumn id="6" name="Def" dataDxfId="36"/>
+    <tableColumn id="22" name="Mag" dataDxfId="35"/>
+    <tableColumn id="27" name="Spd" dataDxfId="34"/>
+    <tableColumn id="26" name="Hit" dataDxfId="33"/>
+    <tableColumn id="25" name="Dhit" dataDxfId="32"/>
+    <tableColumn id="24" name="Crt" dataDxfId="31"/>
+    <tableColumn id="23" name="Luk" dataDxfId="30"/>
+    <tableColumn id="28" name="Sum" dataDxfId="29">
       <calculatedColumnFormula>K4+L4+ SUM(M4:S4)*5+AE4+AF4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="Range" dataDxfId="22"/>
-    <tableColumn id="33" name="Arrow" dataDxfId="21"/>
-    <tableColumn id="4" name="SlotId" dataDxfId="20"/>
-    <tableColumn id="9" name="EnergyRate" dataDxfId="19"/>
-    <tableColumn id="37" name="DungeonAttrs" dataDxfId="18"/>
-    <tableColumn id="7" name="Durable" dataDxfId="17"/>
-    <tableColumn id="20" name="HeroSkillId" dataDxfId="16"/>
-    <tableColumn id="29" name="MonsterAtk" dataDxfId="15"/>
-    <tableColumn id="30" name="MonsterHp" dataDxfId="14"/>
-    <tableColumn id="31" name="PickMethod" dataDxfId="13"/>
-    <tableColumn id="21" name="~SkillMark2" dataDxfId="12"/>
-    <tableColumn id="18" name="~SkillMark22" dataDxfId="11">
-      <calculatedColumnFormula>IF(ISBLANK(AG4),0, LOOKUP(AG4,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AH4/100)</calculatedColumnFormula>
+    <tableColumn id="12" name="Range" dataDxfId="28"/>
+    <tableColumn id="33" name="Arrow" dataDxfId="27"/>
+    <tableColumn id="4" name="SlotId" dataDxfId="26"/>
+    <tableColumn id="9" name="EnergyRate" dataDxfId="25"/>
+    <tableColumn id="37" name="DungeonAttrs" dataDxfId="24"/>
+    <tableColumn id="7" name="Durable" dataDxfId="23"/>
+    <tableColumn id="20" name="HeroSkillId" dataDxfId="22"/>
+    <tableColumn id="29" name="MonsterAtk" dataDxfId="21"/>
+    <tableColumn id="30" name="MonsterHp" dataDxfId="20"/>
+    <tableColumn id="31" name="PickMethod" dataDxfId="19"/>
+    <tableColumn id="21" name="~SkillMark2" dataDxfId="18"/>
+    <tableColumn id="18" name="~SkillMark22" dataDxfId="0">
+      <calculatedColumnFormula>IF(ISBLANK(AG4),0, LOOKUP(AG4,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AH4/100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="CommonSkillId" dataDxfId="10"/>
-    <tableColumn id="14" name="CommonSkillRate" dataDxfId="9"/>
-    <tableColumn id="17" name="RandomDrop" dataDxfId="8"/>
-    <tableColumn id="16" name="CanMerge" dataDxfId="7"/>
-    <tableColumn id="10" name="Url" dataDxfId="6"/>
+    <tableColumn id="13" name="CommonSkillId" dataDxfId="17"/>
+    <tableColumn id="14" name="CommonSkillRate" dataDxfId="16"/>
+    <tableColumn id="17" name="RandomDrop" dataDxfId="15"/>
+    <tableColumn id="16" name="CanMerge" dataDxfId="14"/>
+    <tableColumn id="10" name="Url" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4871,8 +5421,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="AF30" sqref="AF30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -5318,7 +5868,7 @@
         <v>-10</v>
       </c>
       <c r="AF4" s="18">
-        <f>IF(ISBLANK(AG4),0, LOOKUP(AG4,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AH4/100)</f>
+        <f>IF(ISBLANK(AG4),0, LOOKUP(AG4,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AH4/100)</f>
         <v>0</v>
       </c>
       <c r="AG4" s="18"/>
@@ -5413,7 +5963,7 @@
         <v>0</v>
       </c>
       <c r="AF5" s="18">
-        <f>IF(ISBLANK(AG5),0, LOOKUP(AG5,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AH5/100)</f>
+        <f>IF(ISBLANK(AG5),0, LOOKUP(AG5,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AH5/100)</f>
         <v>0</v>
       </c>
       <c r="AG5" s="18"/>
@@ -5508,7 +6058,7 @@
         <v>0</v>
       </c>
       <c r="AF6" s="18">
-        <f>IF(ISBLANK(AG6),0, LOOKUP(AG6,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AH6/100)</f>
+        <f>IF(ISBLANK(AG6),0, LOOKUP(AG6,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AH6/100)</f>
         <v>0</v>
       </c>
       <c r="AG6" s="18"/>
@@ -5605,7 +6155,7 @@
         <v>0</v>
       </c>
       <c r="AF7" s="18">
-        <f>IF(ISBLANK(AG7),0, LOOKUP(AG7,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AH7/100)</f>
+        <f>IF(ISBLANK(AG7),0, LOOKUP(AG7,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AH7/100)</f>
         <v>0</v>
       </c>
       <c r="AG7" s="18"/>
@@ -5700,7 +6250,7 @@
         <v>0</v>
       </c>
       <c r="AF8" s="18">
-        <f>IF(ISBLANK(AG8),0, LOOKUP(AG8,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AH8/100)</f>
+        <f>IF(ISBLANK(AG8),0, LOOKUP(AG8,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AH8/100)</f>
         <v>0</v>
       </c>
       <c r="AG8" s="18"/>
@@ -5795,7 +6345,7 @@
         <v>10</v>
       </c>
       <c r="AF9" s="18">
-        <f>IF(ISBLANK(AG9),0, LOOKUP(AG9,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AH9/100)</f>
+        <f>IF(ISBLANK(AG9),0, LOOKUP(AG9,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AH9/100)</f>
         <v>0</v>
       </c>
       <c r="AG9" s="18"/>
@@ -5892,7 +6442,7 @@
         <v>0</v>
       </c>
       <c r="AF10" s="18">
-        <f>IF(ISBLANK(AG10),0, LOOKUP(AG10,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AH10/100)</f>
+        <f>IF(ISBLANK(AG10),0, LOOKUP(AG10,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AH10/100)</f>
         <v>0</v>
       </c>
       <c r="AG10" s="18"/>
@@ -5987,7 +6537,7 @@
         <v>0</v>
       </c>
       <c r="AF11" s="18">
-        <f>IF(ISBLANK(AG11),0, LOOKUP(AG11,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AH11/100)</f>
+        <f>IF(ISBLANK(AG11),0, LOOKUP(AG11,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AH11/100)</f>
         <v>0</v>
       </c>
       <c r="AG11" s="18"/>
@@ -6082,7 +6632,7 @@
         <v>0</v>
       </c>
       <c r="AF12" s="18">
-        <f>IF(ISBLANK(AG12),0, LOOKUP(AG12,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AH12/100)</f>
+        <f>IF(ISBLANK(AG12),0, LOOKUP(AG12,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AH12/100)</f>
         <v>0</v>
       </c>
       <c r="AG12" s="18"/>
@@ -6177,7 +6727,7 @@
         <v>-10</v>
       </c>
       <c r="AF13" s="18">
-        <f>IF(ISBLANK(AG13),0, LOOKUP(AG13,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AH13/100)</f>
+        <f>IF(ISBLANK(AG13),0, LOOKUP(AG13,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AH13/100)</f>
         <v>0</v>
       </c>
       <c r="AG13" s="18"/>
@@ -6272,7 +6822,7 @@
         <v>0</v>
       </c>
       <c r="AF14" s="18">
-        <f>IF(ISBLANK(AG14),0, LOOKUP(AG14,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AH14/100)</f>
+        <f>IF(ISBLANK(AG14),0, LOOKUP(AG14,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AH14/100)</f>
         <v>0</v>
       </c>
       <c r="AG14" s="18"/>
@@ -6367,7 +6917,7 @@
         <v>0</v>
       </c>
       <c r="AF15" s="18">
-        <f>IF(ISBLANK(AG15),0, LOOKUP(AG15,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AH15/100)</f>
+        <f>IF(ISBLANK(AG15),0, LOOKUP(AG15,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AH15/100)</f>
         <v>0</v>
       </c>
       <c r="AG15" s="18"/>
@@ -6462,7 +7012,7 @@
         <v>-10</v>
       </c>
       <c r="AF16" s="18">
-        <f>IF(ISBLANK(AG16),0, LOOKUP(AG16,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AH16/100)</f>
+        <f>IF(ISBLANK(AG16),0, LOOKUP(AG16,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AH16/100)</f>
         <v>0</v>
       </c>
       <c r="AG16" s="18"/>
@@ -6557,7 +7107,7 @@
         <v>0</v>
       </c>
       <c r="AF17" s="18">
-        <f>IF(ISBLANK(AG17),0, LOOKUP(AG17,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AH17/100)</f>
+        <f>IF(ISBLANK(AG17),0, LOOKUP(AG17,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AH17/100)</f>
         <v>0</v>
       </c>
       <c r="AG17" s="18"/>
@@ -6652,7 +7202,7 @@
         <v>0</v>
       </c>
       <c r="AF18" s="18">
-        <f>IF(ISBLANK(AG18),0, LOOKUP(AG18,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AH18/100)</f>
+        <f>IF(ISBLANK(AG18),0, LOOKUP(AG18,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AH18/100)</f>
         <v>0</v>
       </c>
       <c r="AG18" s="18"/>
@@ -6751,7 +7301,7 @@
         <v>10</v>
       </c>
       <c r="AF19" s="18">
-        <f>IF(ISBLANK(AG19),0, LOOKUP(AG19,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AH19/100)</f>
+        <f>IF(ISBLANK(AG19),0, LOOKUP(AG19,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AH19/100)</f>
         <v>0</v>
       </c>
       <c r="AG19" s="18"/>
@@ -6852,7 +7402,7 @@
         <v>14</v>
       </c>
       <c r="AF20" s="18">
-        <f>IF(ISBLANK(AG20),0, LOOKUP(AG20,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AH20/100)</f>
+        <f>IF(ISBLANK(AG20),0, LOOKUP(AG20,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AH20/100)</f>
         <v>0</v>
       </c>
       <c r="AG20" s="18"/>
@@ -6951,7 +7501,7 @@
         <v>12.5</v>
       </c>
       <c r="AF21" s="18">
-        <f>IF(ISBLANK(AG21),0, LOOKUP(AG21,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AH21/100)</f>
+        <f>IF(ISBLANK(AG21),0, LOOKUP(AG21,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AH21/100)</f>
         <v>0</v>
       </c>
       <c r="AG21" s="18"/>
@@ -7052,7 +7602,7 @@
         <v>14</v>
       </c>
       <c r="AF22" s="18">
-        <f>IF(ISBLANK(AG22),0, LOOKUP(AG22,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AH22/100)</f>
+        <f>IF(ISBLANK(AG22),0, LOOKUP(AG22,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AH22/100)</f>
         <v>0</v>
       </c>
       <c r="AG22" s="18"/>
@@ -7151,7 +7701,7 @@
         <v>6</v>
       </c>
       <c r="AF23" s="18">
-        <f>IF(ISBLANK(AG23),0, LOOKUP(AG23,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AH23/100)</f>
+        <f>IF(ISBLANK(AG23),0, LOOKUP(AG23,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AH23/100)</f>
         <v>0</v>
       </c>
       <c r="AG23" s="18"/>
@@ -7250,7 +7800,7 @@
         <v>6</v>
       </c>
       <c r="AF24" s="18">
-        <f>IF(ISBLANK(AG24),0, LOOKUP(AG24,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AH24/100)</f>
+        <f>IF(ISBLANK(AG24),0, LOOKUP(AG24,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AH24/100)</f>
         <v>0</v>
       </c>
       <c r="AG24" s="18"/>
@@ -7351,7 +7901,7 @@
         <v>9</v>
       </c>
       <c r="AF25" s="18">
-        <f>IF(ISBLANK(AG25),0, LOOKUP(AG25,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AH25/100)</f>
+        <f>IF(ISBLANK(AG25),0, LOOKUP(AG25,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AH25/100)</f>
         <v>0</v>
       </c>
       <c r="AG25" s="18"/>
@@ -7452,7 +8002,7 @@
         <v>18</v>
       </c>
       <c r="AF26" s="18">
-        <f>IF(ISBLANK(AG26),0, LOOKUP(AG26,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AH26/100)</f>
+        <f>IF(ISBLANK(AG26),0, LOOKUP(AG26,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AH26/100)</f>
         <v>0</v>
       </c>
       <c r="AG26" s="18"/>
@@ -7553,7 +8103,7 @@
         <v>15</v>
       </c>
       <c r="AF27" s="18">
-        <f>IF(ISBLANK(AG27),0, LOOKUP(AG27,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AH27/100)</f>
+        <f>IF(ISBLANK(AG27),0, LOOKUP(AG27,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AH27/100)</f>
         <v>0</v>
       </c>
       <c r="AG27" s="18"/>
@@ -7654,7 +8204,7 @@
         <v>25</v>
       </c>
       <c r="AF28" s="18">
-        <f>IF(ISBLANK(AG28),0, LOOKUP(AG28,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AH28/100)</f>
+        <f>IF(ISBLANK(AG28),0, LOOKUP(AG28,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AH28/100)</f>
         <v>0</v>
       </c>
       <c r="AG28" s="18"/>
@@ -7749,7 +8299,7 @@
         <v>0</v>
       </c>
       <c r="AF29" s="18">
-        <f>IF(ISBLANK(AG29),0, LOOKUP(AG29,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AH29/100)</f>
+        <f>IF(ISBLANK(AG29),0, LOOKUP(AG29,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AH29/100)</f>
         <v>0</v>
       </c>
       <c r="AG29" s="18"/>
@@ -7777,14 +8327,14 @@
       <c r="D30" s="1"/>
       <c r="E30" s="1">
         <f t="shared" ref="E30:E31" si="20">IF(T30&gt;=23,4,IF(AND(T30&gt;=18,T30&lt;23),3,IF(AND(T30&gt;=13,T30&lt;18),2,IF(AND(T30&gt;=8,T30&lt;13),1,0))))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F30" s="1">
         <v>3</v>
       </c>
       <c r="G30" s="1">
         <f t="shared" si="2"/>
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="H30" s="18">
         <v>100</v>
@@ -7822,7 +8372,7 @@
       </c>
       <c r="T30" s="18">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="U30" s="18"/>
       <c r="V30" s="18" t="s">
@@ -7844,8 +8394,8 @@
         <v>0</v>
       </c>
       <c r="AF30" s="18">
-        <f>IF(ISBLANK(AG30),0, LOOKUP(AG30,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AH30/100)</f>
-        <v>0</v>
+        <f>IF(ISBLANK(AG30),0, LOOKUP(AG30,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AH30/100)</f>
+        <v>6</v>
       </c>
       <c r="AG30" s="18">
         <v>55510010</v>
@@ -7945,7 +8495,7 @@
         <v>0</v>
       </c>
       <c r="AF31" s="18">
-        <f>IF(ISBLANK(AG31),0, LOOKUP(AG31,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AH31/100)</f>
+        <f>IF(ISBLANK(AG31),0, LOOKUP(AG31,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AH31/100)</f>
         <v>0</v>
       </c>
       <c r="AG31" s="18"/>
@@ -7973,14 +8523,14 @@
       <c r="D32" s="1"/>
       <c r="E32" s="1">
         <f t="shared" ref="E32:E33" si="21">IF(T32&gt;=23,4,IF(AND(T32&gt;=18,T32&lt;23),3,IF(AND(T32&gt;=13,T32&lt;18),2,IF(AND(T32&gt;=8,T32&lt;13),1,0))))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F32" s="1">
         <v>3</v>
       </c>
       <c r="G32" s="1">
         <f t="shared" si="2"/>
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="H32" s="18">
         <v>50</v>
@@ -8020,7 +8570,7 @@
       </c>
       <c r="T32" s="18">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>17.3</v>
       </c>
       <c r="U32" s="18"/>
       <c r="V32" s="18" t="s">
@@ -8042,8 +8592,8 @@
         <v>0</v>
       </c>
       <c r="AF32" s="18">
-        <f>IF(ISBLANK(AG32),0, LOOKUP(AG32,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AH32/100)</f>
-        <v>0</v>
+        <f>IF(ISBLANK(AG32),0, LOOKUP(AG32,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AH32/100)</f>
+        <v>9.3000000000000007</v>
       </c>
       <c r="AG32" s="18">
         <v>55510012</v>
@@ -8143,7 +8693,7 @@
         <v>0</v>
       </c>
       <c r="AF33" s="18">
-        <f>IF(ISBLANK(AG33),0, LOOKUP(AG33,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AH33/100)</f>
+        <f>IF(ISBLANK(AG33),0, LOOKUP(AG33,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AH33/100)</f>
         <v>0</v>
       </c>
       <c r="AG33" s="18"/>
@@ -8238,7 +8788,7 @@
         <v>0</v>
       </c>
       <c r="AF34" s="18">
-        <f>IF(ISBLANK(AG34),0, LOOKUP(AG34,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AH34/100)</f>
+        <f>IF(ISBLANK(AG34),0, LOOKUP(AG34,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AH34/100)</f>
         <v>0</v>
       </c>
       <c r="AG34" s="18"/>
@@ -8335,7 +8885,7 @@
         <v>0</v>
       </c>
       <c r="AF35" s="18">
-        <f>IF(ISBLANK(AG35),0, LOOKUP(AG35,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AH35/100)</f>
+        <f>IF(ISBLANK(AG35),0, LOOKUP(AG35,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AH35/100)</f>
         <v>0</v>
       </c>
       <c r="AG35" s="18"/>
@@ -8430,7 +8980,7 @@
         <v>0</v>
       </c>
       <c r="AF36" s="18">
-        <f>IF(ISBLANK(AG36),0, LOOKUP(AG36,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AH36/100)</f>
+        <f>IF(ISBLANK(AG36),0, LOOKUP(AG36,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AH36/100)</f>
         <v>0</v>
       </c>
       <c r="AG36" s="18"/>
@@ -8458,14 +9008,14 @@
       <c r="D37" s="1"/>
       <c r="E37" s="1">
         <f t="shared" si="23"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F37" s="1">
         <v>3</v>
       </c>
       <c r="G37" s="1">
         <f t="shared" si="24"/>
-        <v>50</v>
+        <v>200</v>
       </c>
       <c r="H37" s="18">
         <v>70</v>
@@ -8505,7 +9055,7 @@
       </c>
       <c r="T37" s="18">
         <f t="shared" si="1"/>
-        <v>-15</v>
+        <v>20</v>
       </c>
       <c r="U37" s="18"/>
       <c r="V37" s="18" t="s">
@@ -8527,8 +9077,8 @@
         <v>0</v>
       </c>
       <c r="AF37" s="18">
-        <f>IF(ISBLANK(AG37),0, LOOKUP(AG37,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AH37/100)</f>
-        <v>0</v>
+        <f>IF(ISBLANK(AG37),0, LOOKUP(AG37,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AH37/100)</f>
+        <v>35</v>
       </c>
       <c r="AG37" s="18">
         <v>55100007</v>
@@ -8624,7 +9174,7 @@
         <v>0</v>
       </c>
       <c r="AF38" s="18">
-        <f>IF(ISBLANK(AG38),0, LOOKUP(AG38,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AH38/100)</f>
+        <f>IF(ISBLANK(AG38),0, LOOKUP(AG38,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AH38/100)</f>
         <v>0</v>
       </c>
       <c r="AG38" s="18"/>
@@ -8717,7 +9267,7 @@
         <v>0</v>
       </c>
       <c r="AF39" s="18">
-        <f>IF(ISBLANK(AG39),0, LOOKUP(AG39,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AH39/100)</f>
+        <f>IF(ISBLANK(AG39),0, LOOKUP(AG39,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AH39/100)</f>
         <v>0</v>
       </c>
       <c r="AG39" s="18"/>
@@ -8745,14 +9295,14 @@
       <c r="D40" s="1"/>
       <c r="E40" s="1">
         <f t="shared" si="26"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F40" s="1">
         <v>4</v>
       </c>
       <c r="G40" s="1">
         <f t="shared" si="2"/>
-        <v>50</v>
+        <v>150</v>
       </c>
       <c r="H40" s="18">
         <v>100</v>
@@ -8790,7 +9340,7 @@
       </c>
       <c r="T40" s="18">
         <f t="shared" si="27"/>
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="U40" s="18"/>
       <c r="V40" s="18"/>
@@ -8810,8 +9360,8 @@
         <v>0</v>
       </c>
       <c r="AF40" s="18">
-        <f>IF(ISBLANK(AG40),0, LOOKUP(AG40,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AH40/100)</f>
-        <v>0</v>
+        <f>IF(ISBLANK(AG40),0, LOOKUP(AG40,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AH40/100)</f>
+        <v>10</v>
       </c>
       <c r="AG40" s="18">
         <v>55110005</v>
@@ -8907,7 +9457,7 @@
         <v>0</v>
       </c>
       <c r="AF41" s="18">
-        <f>IF(ISBLANK(AG41),0, LOOKUP(AG41,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AH41/100)</f>
+        <f>IF(ISBLANK(AG41),0, LOOKUP(AG41,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AH41/100)</f>
         <v>0</v>
       </c>
       <c r="AG41" s="18"/>
@@ -9000,7 +9550,7 @@
         <v>0</v>
       </c>
       <c r="AF42" s="18">
-        <f>IF(ISBLANK(AG42),0, LOOKUP(AG42,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AH42/100)</f>
+        <f>IF(ISBLANK(AG42),0, LOOKUP(AG42,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AH42/100)</f>
         <v>0</v>
       </c>
       <c r="AG42" s="18"/>
@@ -9095,7 +9645,7 @@
         <v>0</v>
       </c>
       <c r="AF43" s="18">
-        <f>IF(ISBLANK(AG43),0, LOOKUP(AG43,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AH43/100)</f>
+        <f>IF(ISBLANK(AG43),0, LOOKUP(AG43,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AH43/100)</f>
         <v>0</v>
       </c>
       <c r="AG43" s="18"/>
@@ -9188,7 +9738,7 @@
         <v>0</v>
       </c>
       <c r="AF44" s="18">
-        <f>IF(ISBLANK(AG44),0, LOOKUP(AG44,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AH44/100)</f>
+        <f>IF(ISBLANK(AG44),0, LOOKUP(AG44,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AH44/100)</f>
         <v>0</v>
       </c>
       <c r="AG44" s="18"/>
@@ -9281,7 +9831,7 @@
         <v>0</v>
       </c>
       <c r="AF45" s="18">
-        <f>IF(ISBLANK(AG45),0, LOOKUP(AG45,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AH45/100)</f>
+        <f>IF(ISBLANK(AG45),0, LOOKUP(AG45,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AH45/100)</f>
         <v>0</v>
       </c>
       <c r="AG45" s="18"/>
@@ -9376,7 +9926,7 @@
         <v>0</v>
       </c>
       <c r="AF46" s="18">
-        <f>IF(ISBLANK(AG46),0, LOOKUP(AG46,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AH46/100)</f>
+        <f>IF(ISBLANK(AG46),0, LOOKUP(AG46,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AH46/100)</f>
         <v>0</v>
       </c>
       <c r="AG46" s="18"/>
@@ -9471,7 +10021,7 @@
         <v>0</v>
       </c>
       <c r="AF47" s="18">
-        <f>IF(ISBLANK(AG47),0, LOOKUP(AG47,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AH47/100)</f>
+        <f>IF(ISBLANK(AG47),0, LOOKUP(AG47,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AH47/100)</f>
         <v>0</v>
       </c>
       <c r="AG47" s="18"/>
@@ -9566,7 +10116,7 @@
         <v>0</v>
       </c>
       <c r="AF48" s="18">
-        <f>IF(ISBLANK(AG48),0, LOOKUP(AG48,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AH48/100)</f>
+        <f>IF(ISBLANK(AG48),0, LOOKUP(AG48,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AH48/100)</f>
         <v>0</v>
       </c>
       <c r="AG48" s="18"/>
@@ -9661,7 +10211,7 @@
         <v>10</v>
       </c>
       <c r="AF49" s="18">
-        <f>IF(ISBLANK(AG49),0, LOOKUP(AG49,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AH49/100)</f>
+        <f>IF(ISBLANK(AG49),0, LOOKUP(AG49,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AH49/100)</f>
         <v>0</v>
       </c>
       <c r="AG49" s="18"/>
@@ -9756,7 +10306,7 @@
         <v>5</v>
       </c>
       <c r="AF50" s="18">
-        <f>IF(ISBLANK(AG50),0, LOOKUP(AG50,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AH50/100)</f>
+        <f>IF(ISBLANK(AG50),0, LOOKUP(AG50,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AH50/100)</f>
         <v>0</v>
       </c>
       <c r="AG50" s="18"/>
@@ -9851,7 +10401,7 @@
         <v>6</v>
       </c>
       <c r="AF51" s="18">
-        <f>IF(ISBLANK(AG51),0, LOOKUP(AG51,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AH51/100)</f>
+        <f>IF(ISBLANK(AG51),0, LOOKUP(AG51,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AH51/100)</f>
         <v>0</v>
       </c>
       <c r="AG51" s="18"/>
@@ -9879,14 +10429,14 @@
       <c r="D52" s="1"/>
       <c r="E52" s="1">
         <f t="shared" ref="E52:E53" si="38">IF(T52&gt;=23,4,IF(AND(T52&gt;=18,T52&lt;23),3,IF(AND(T52&gt;=13,T52&lt;18),2,IF(AND(T52&gt;=8,T52&lt;13),1,0))))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F52" s="1">
         <v>5</v>
       </c>
       <c r="G52" s="1">
         <f t="shared" si="2"/>
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="H52" s="18"/>
       <c r="I52" s="18">
@@ -9924,7 +10474,7 @@
       </c>
       <c r="T52" s="18">
         <f t="shared" si="27"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="U52" s="18"/>
       <c r="V52" s="18"/>
@@ -9944,8 +10494,8 @@
         <v>0</v>
       </c>
       <c r="AF52" s="18">
-        <f>IF(ISBLANK(AG52),0, LOOKUP(AG52,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AH52/100)</f>
-        <v>0</v>
+        <f>IF(ISBLANK(AG52),0, LOOKUP(AG52,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AH52/100)</f>
+        <v>4</v>
       </c>
       <c r="AG52" s="18">
         <v>55990108</v>
@@ -10043,7 +10593,7 @@
         <v>10</v>
       </c>
       <c r="AF53" s="18">
-        <f>IF(ISBLANK(AG53),0, LOOKUP(AG53,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AH53/100)</f>
+        <f>IF(ISBLANK(AG53),0, LOOKUP(AG53,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AH53/100)</f>
         <v>0</v>
       </c>
       <c r="AG53" s="18"/>
@@ -10071,14 +10621,14 @@
       <c r="D54" s="1"/>
       <c r="E54" s="1">
         <f t="shared" ref="E54:E55" si="39">IF(T54&gt;=23,4,IF(AND(T54&gt;=18,T54&lt;23),3,IF(AND(T54&gt;=13,T54&lt;18),2,IF(AND(T54&gt;=8,T54&lt;13),1,0))))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F54" s="1">
         <v>5</v>
       </c>
       <c r="G54" s="1">
         <f t="shared" si="2"/>
-        <v>50</v>
+        <v>150</v>
       </c>
       <c r="H54" s="18"/>
       <c r="I54" s="18">
@@ -10116,7 +10666,7 @@
       </c>
       <c r="T54" s="18">
         <f t="shared" si="27"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="U54" s="18"/>
       <c r="V54" s="18"/>
@@ -10136,8 +10686,8 @@
         <v>0</v>
       </c>
       <c r="AF54" s="18">
-        <f>IF(ISBLANK(AG54),0, LOOKUP(AG54,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AH54/100)</f>
-        <v>0</v>
+        <f>IF(ISBLANK(AG54),0, LOOKUP(AG54,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AH54/100)</f>
+        <v>15</v>
       </c>
       <c r="AG54" s="18">
         <v>55990109</v>
@@ -10233,7 +10783,7 @@
         <v>8</v>
       </c>
       <c r="AF55" s="18">
-        <f>IF(ISBLANK(AG55),0, LOOKUP(AG55,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AH55/100)</f>
+        <f>IF(ISBLANK(AG55),0, LOOKUP(AG55,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AH55/100)</f>
         <v>0</v>
       </c>
       <c r="AG55" s="18"/>
@@ -10261,14 +10811,14 @@
       <c r="D56" s="1"/>
       <c r="E56" s="1">
         <f t="shared" ref="E56:E57" si="41">IF(T56&gt;=23,4,IF(AND(T56&gt;=18,T56&lt;23),3,IF(AND(T56&gt;=13,T56&lt;18),2,IF(AND(T56&gt;=8,T56&lt;13),1,0))))</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F56" s="1">
         <v>5</v>
       </c>
       <c r="G56" s="1">
         <f t="shared" si="40"/>
-        <v>150</v>
+        <v>250</v>
       </c>
       <c r="H56" s="18"/>
       <c r="I56" s="18">
@@ -10306,7 +10856,7 @@
       </c>
       <c r="T56" s="18">
         <f t="shared" si="27"/>
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="U56" s="18"/>
       <c r="V56" s="18"/>
@@ -10326,8 +10876,8 @@
         <v>0</v>
       </c>
       <c r="AF56" s="18">
-        <f>IF(ISBLANK(AG56),0, LOOKUP(AG56,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AH56/100)</f>
-        <v>0</v>
+        <f>IF(ISBLANK(AG56),0, LOOKUP(AG56,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AH56/100)</f>
+        <v>10</v>
       </c>
       <c r="AG56" s="18">
         <v>55110003</v>
@@ -10425,7 +10975,7 @@
         <v>10</v>
       </c>
       <c r="AF57" s="18">
-        <f>IF(ISBLANK(AG57),0, LOOKUP(AG57,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AH57/100)</f>
+        <f>IF(ISBLANK(AG57),0, LOOKUP(AG57,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AH57/100)</f>
         <v>0</v>
       </c>
       <c r="AG57" s="18"/>
@@ -10522,7 +11072,7 @@
         <v>15</v>
       </c>
       <c r="AF58" s="18">
-        <f>IF(ISBLANK(AG58),0, LOOKUP(AG58,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AH58/100)</f>
+        <f>IF(ISBLANK(AG58),0, LOOKUP(AG58,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AH58/100)</f>
         <v>0</v>
       </c>
       <c r="AG58" s="18"/>
@@ -10617,7 +11167,7 @@
         <v>25</v>
       </c>
       <c r="AF59" s="18">
-        <f>IF(ISBLANK(AG59),0, LOOKUP(AG59,[1]Skill!$A:$A,[1]Skill!$Y:$Y)*AH59/100)</f>
+        <f>IF(ISBLANK(AG59),0, LOOKUP(AG59,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AH59/100)</f>
         <v>0</v>
       </c>
       <c r="AG59" s="18"/>
@@ -10635,24 +11185,24 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="E4:E59">
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="12" priority="7" operator="greaterThanOrEqual">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="9" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="10" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="11" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:AK59">
-    <cfRule type="containsBlanks" dxfId="0" priority="1">
+    <cfRule type="containsBlanks" dxfId="8" priority="1">
       <formula>LEN(TRIM(H4))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
give equips on initial quests
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Equip.xlsx
+++ b/ConfigData/Xlsx/Equip.xlsx
@@ -956,236 +956,239 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
+    <t>eqxiyongchengbao</t>
+  </si>
+  <si>
+    <t>eqgaibeiyichengbao</t>
+  </si>
+  <si>
+    <t>eqtianshouge</t>
+  </si>
+  <si>
+    <t>eqwaxilijiaotang</t>
+  </si>
+  <si>
+    <t>eqjinzita</t>
+  </si>
+  <si>
+    <t>eqzijincheng</t>
+  </si>
+  <si>
+    <t>eqtianebao</t>
+  </si>
+  <si>
+    <t>eqmayashenmiao</t>
+  </si>
+  <si>
+    <t>eqdishinichengbao</t>
+  </si>
+  <si>
+    <t>eqtielubao</t>
+  </si>
+  <si>
+    <t>eqhuogewozi</t>
+  </si>
+  <si>
+    <t>eqpatenongshenmiao</t>
+  </si>
+  <si>
+    <t>eqzhulou</t>
+  </si>
+  <si>
+    <t>eqshengtuolini</t>
+  </si>
+  <si>
+    <t>eqlanseqizhi</t>
+  </si>
+  <si>
+    <t>eqguiguaiqizhi</t>
+  </si>
+  <si>
+    <t>eqyexingqizhi</t>
+  </si>
+  <si>
+    <t>eqanyeqizhi</t>
+  </si>
+  <si>
+    <t>eqlianheqizhi</t>
+  </si>
+  <si>
+    <t>eqhaidaoqizhi</t>
+  </si>
+  <si>
+    <t>eqgongniuqizhi</t>
+  </si>
+  <si>
+    <t>eqkexueqizhi</t>
+  </si>
+  <si>
+    <t>eqyaoshuiqizhi</t>
+  </si>
+  <si>
+    <t>eqyingxiongqizhi</t>
+  </si>
+  <si>
+    <t>eqgongjian</t>
+  </si>
+  <si>
+    <t>eqhuoyanjian</t>
+  </si>
+  <si>
+    <t>eqhuoqiang</t>
+  </si>
+  <si>
+    <t>eqfeichui</t>
+  </si>
+  <si>
+    <t>eqairenhuopao</t>
+  </si>
+  <si>
+    <t>eqjunu</t>
+  </si>
+  <si>
+    <t>eqjiguang</t>
+  </si>
+  <si>
+    <t>eqbaoliepao</t>
+  </si>
+  <si>
+    <t>eqmuqiang</t>
+  </si>
+  <si>
+    <t>eqshiqiang</t>
+  </si>
+  <si>
+    <t>eqciqiang</t>
+  </si>
+  <si>
+    <t>eqhuangjinqiang</t>
+  </si>
+  <si>
+    <t>eqzhuanqiang</t>
+  </si>
+  <si>
+    <t>eqtiepi</t>
+  </si>
+  <si>
+    <t>eqzhufukuangshi</t>
+  </si>
+  <si>
+    <t>eqtongqiang</t>
+  </si>
+  <si>
+    <t>eqboliqiang</t>
+  </si>
+  <si>
+    <t>eqlonglin</t>
+  </si>
+  <si>
+    <t>eqtushuguan</t>
+  </si>
+  <si>
+    <t>eqxunlianfang</t>
+  </si>
+  <si>
+    <t>eqwenshi</t>
+  </si>
+  <si>
+    <t>eqzhanbuxiaowu</t>
+  </si>
+  <si>
+    <t>eqbingying</t>
+  </si>
+  <si>
+    <t>eqtiejiangpu</t>
+  </si>
+  <si>
+    <t>eqwuduta</t>
+  </si>
+  <si>
+    <t>eqhudunfashengqi</t>
+  </si>
+  <si>
+    <t>eqlieshoudating</t>
+  </si>
+  <si>
+    <t>eqchuansongzhen</t>
+  </si>
+  <si>
+    <t>价值</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>合成消耗木材</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>合成消耗石头</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ComposeStone</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ComposeWood</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>eqliaowangtai</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>副本属性加成</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int[]</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>DungeonAttrs</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>-1;0;2;0;0</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>1;1;-1;0;0</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>0;0;0;2;0</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>0;1;0;0;0</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>合成消耗道具</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ComposeItemId</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
     <t>eqcaowu</t>
-  </si>
-  <si>
-    <t>eqxiyongchengbao</t>
-  </si>
-  <si>
-    <t>eqgaibeiyichengbao</t>
-  </si>
-  <si>
-    <t>eqtianshouge</t>
-  </si>
-  <si>
-    <t>eqwaxilijiaotang</t>
-  </si>
-  <si>
-    <t>eqjinzita</t>
-  </si>
-  <si>
-    <t>eqzijincheng</t>
-  </si>
-  <si>
-    <t>eqtianebao</t>
-  </si>
-  <si>
-    <t>eqmayashenmiao</t>
-  </si>
-  <si>
-    <t>eqdishinichengbao</t>
-  </si>
-  <si>
-    <t>eqtielubao</t>
-  </si>
-  <si>
-    <t>eqhuogewozi</t>
-  </si>
-  <si>
-    <t>eqpatenongshenmiao</t>
-  </si>
-  <si>
-    <t>eqzhulou</t>
-  </si>
-  <si>
-    <t>eqshengtuolini</t>
-  </si>
-  <si>
-    <t>eqlanseqizhi</t>
-  </si>
-  <si>
-    <t>eqguiguaiqizhi</t>
-  </si>
-  <si>
-    <t>eqyexingqizhi</t>
-  </si>
-  <si>
-    <t>eqanyeqizhi</t>
-  </si>
-  <si>
-    <t>eqlianheqizhi</t>
-  </si>
-  <si>
-    <t>eqhaidaoqizhi</t>
-  </si>
-  <si>
-    <t>eqgongniuqizhi</t>
-  </si>
-  <si>
-    <t>eqkexueqizhi</t>
-  </si>
-  <si>
-    <t>eqyaoshuiqizhi</t>
-  </si>
-  <si>
-    <t>eqyingxiongqizhi</t>
-  </si>
-  <si>
-    <t>eqgongjian</t>
-  </si>
-  <si>
-    <t>eqhuoyanjian</t>
-  </si>
-  <si>
-    <t>eqhuoqiang</t>
-  </si>
-  <si>
-    <t>eqfeichui</t>
-  </si>
-  <si>
-    <t>eqairenhuopao</t>
-  </si>
-  <si>
-    <t>eqjunu</t>
-  </si>
-  <si>
-    <t>eqjiguang</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>eqzhibanqiang</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
     <t>eqdangong</t>
-  </si>
-  <si>
-    <t>eqbaoliepao</t>
-  </si>
-  <si>
-    <t>eqmuqiang</t>
-  </si>
-  <si>
-    <t>eqshiqiang</t>
-  </si>
-  <si>
-    <t>eqciqiang</t>
-  </si>
-  <si>
-    <t>eqhuangjinqiang</t>
-  </si>
-  <si>
-    <t>eqzhuanqiang</t>
-  </si>
-  <si>
-    <t>eqtiepi</t>
-  </si>
-  <si>
-    <t>eqzhufukuangshi</t>
-  </si>
-  <si>
-    <t>eqzhibanqiang</t>
-  </si>
-  <si>
-    <t>eqtongqiang</t>
-  </si>
-  <si>
-    <t>eqboliqiang</t>
-  </si>
-  <si>
-    <t>eqlonglin</t>
-  </si>
-  <si>
-    <t>eqtushuguan</t>
-  </si>
-  <si>
-    <t>eqxunlianfang</t>
-  </si>
-  <si>
-    <t>eqwenshi</t>
-  </si>
-  <si>
-    <t>eqzhanbuxiaowu</t>
-  </si>
-  <si>
-    <t>eqbingying</t>
-  </si>
-  <si>
-    <t>eqtiejiangpu</t>
-  </si>
-  <si>
-    <t>eqwuduta</t>
-  </si>
-  <si>
-    <t>eqhudunfashengqi</t>
-  </si>
-  <si>
-    <t>eqlieshoudating</t>
-  </si>
-  <si>
-    <t>eqchuansongzhen</t>
-  </si>
-  <si>
-    <t>价值</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>合成消耗木材</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>合成消耗石头</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>ComposeStone</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>ComposeWood</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>eqliaowangtai</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>副本属性加成</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>int[]</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>DungeonAttrs</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>-1;0;2;0;0</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>1;1;-1;0;0</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>0;0;0;2;0</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>0;1;0;0;0</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>合成消耗道具</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>ComposeItemId</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -2007,71 +2010,6 @@
   </cellStyles>
   <dxfs count="39">
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF9751CB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -2700,6 +2638,71 @@
         <horizontal/>
       </border>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF9751CB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -4959,48 +4962,48 @@
   <tableColumns count="36">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="Name"/>
-    <tableColumn id="34" name="Ename" dataDxfId="38"/>
-    <tableColumn id="32" name="Des" dataDxfId="37"/>
-    <tableColumn id="3" name="Quality" dataDxfId="36">
+    <tableColumn id="34" name="Ename" dataDxfId="32"/>
+    <tableColumn id="32" name="Des" dataDxfId="31"/>
+    <tableColumn id="3" name="Quality" dataDxfId="30">
       <calculatedColumnFormula>IF(T4&gt;=23,4,IF(AND(T4&gt;=18,T4&lt;23),3,IF(AND(T4&gt;=13,T4&lt;18),2,IF(AND(T4&gt;=8,T4&lt;13),1,0))))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" name="Position"/>
-    <tableColumn id="19" name="Value" dataDxfId="35">
+    <tableColumn id="19" name="Value" dataDxfId="29">
       <calculatedColumnFormula>E4*50+50</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="35" name="ComposeStone" dataDxfId="34"/>
-    <tableColumn id="36" name="ComposeWood" dataDxfId="33"/>
-    <tableColumn id="15" name="ComposeItemId" dataDxfId="32"/>
-    <tableColumn id="11" name="AtkR" dataDxfId="31"/>
-    <tableColumn id="8" name="VitR" dataDxfId="30"/>
-    <tableColumn id="6" name="Def" dataDxfId="29"/>
-    <tableColumn id="22" name="Mag" dataDxfId="28"/>
-    <tableColumn id="27" name="Spd" dataDxfId="27"/>
-    <tableColumn id="26" name="Hit" dataDxfId="26"/>
-    <tableColumn id="25" name="Dhit" dataDxfId="25"/>
-    <tableColumn id="24" name="Crt" dataDxfId="24"/>
-    <tableColumn id="23" name="Luk" dataDxfId="23"/>
-    <tableColumn id="28" name="Sum" dataDxfId="22">
+    <tableColumn id="35" name="ComposeStone" dataDxfId="28"/>
+    <tableColumn id="36" name="ComposeWood" dataDxfId="27"/>
+    <tableColumn id="15" name="ComposeItemId" dataDxfId="26"/>
+    <tableColumn id="11" name="AtkR" dataDxfId="25"/>
+    <tableColumn id="8" name="VitR" dataDxfId="24"/>
+    <tableColumn id="6" name="Def" dataDxfId="23"/>
+    <tableColumn id="22" name="Mag" dataDxfId="22"/>
+    <tableColumn id="27" name="Spd" dataDxfId="21"/>
+    <tableColumn id="26" name="Hit" dataDxfId="20"/>
+    <tableColumn id="25" name="Dhit" dataDxfId="19"/>
+    <tableColumn id="24" name="Crt" dataDxfId="18"/>
+    <tableColumn id="23" name="Luk" dataDxfId="17"/>
+    <tableColumn id="28" name="Sum" dataDxfId="16">
       <calculatedColumnFormula>K4+L4+ SUM(M4:S4)*5+AD4+AE4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="Range" dataDxfId="21"/>
-    <tableColumn id="33" name="Arrow" dataDxfId="20"/>
-    <tableColumn id="4" name="SlotId" dataDxfId="19"/>
-    <tableColumn id="9" name="EnergyRate" dataDxfId="18"/>
-    <tableColumn id="37" name="DungeonAttrs" dataDxfId="17"/>
-    <tableColumn id="20" name="HeroSkillId" dataDxfId="16"/>
-    <tableColumn id="29" name="MonsterAtk" dataDxfId="15"/>
-    <tableColumn id="30" name="MonsterHp" dataDxfId="14"/>
-    <tableColumn id="31" name="PickMethod" dataDxfId="13"/>
-    <tableColumn id="21" name="~SkillMark2" dataDxfId="12"/>
-    <tableColumn id="18" name="~SkillMark22" dataDxfId="11">
+    <tableColumn id="12" name="Range" dataDxfId="15"/>
+    <tableColumn id="33" name="Arrow" dataDxfId="14"/>
+    <tableColumn id="4" name="SlotId" dataDxfId="13"/>
+    <tableColumn id="9" name="EnergyRate" dataDxfId="12"/>
+    <tableColumn id="37" name="DungeonAttrs" dataDxfId="11"/>
+    <tableColumn id="20" name="HeroSkillId" dataDxfId="10"/>
+    <tableColumn id="29" name="MonsterAtk" dataDxfId="9"/>
+    <tableColumn id="30" name="MonsterHp" dataDxfId="8"/>
+    <tableColumn id="31" name="PickMethod" dataDxfId="7"/>
+    <tableColumn id="21" name="~SkillMark2" dataDxfId="6"/>
+    <tableColumn id="18" name="~SkillMark22" dataDxfId="5">
       <calculatedColumnFormula>IF(ISBLANK(AF4),0, LOOKUP(AF4,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AG4/100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="CommonSkillId" dataDxfId="10"/>
-    <tableColumn id="14" name="CommonSkillRate" dataDxfId="9"/>
-    <tableColumn id="17" name="RandomDrop" dataDxfId="8"/>
-    <tableColumn id="16" name="CanMerge" dataDxfId="7"/>
-    <tableColumn id="10" name="Url" dataDxfId="6"/>
+    <tableColumn id="13" name="CommonSkillId" dataDxfId="4"/>
+    <tableColumn id="14" name="CommonSkillRate" dataDxfId="3"/>
+    <tableColumn id="17" name="RandomDrop" dataDxfId="2"/>
+    <tableColumn id="16" name="CanMerge" dataDxfId="1"/>
+    <tableColumn id="10" name="Url" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5329,8 +5332,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AA10" sqref="AA10"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -5375,16 +5378,16 @@
         <v>5</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="H1" s="13" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="I1" s="13" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="J1" s="13" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="K1" s="14" t="s">
         <v>13</v>
@@ -5429,7 +5432,7 @@
         <v>41</v>
       </c>
       <c r="Y1" s="17" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="Z1" s="17" t="s">
         <v>42</v>
@@ -5488,13 +5491,13 @@
         <v>0</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="K2" s="3" t="s">
         <v>14</v>
@@ -5539,7 +5542,7 @@
         <v>43</v>
       </c>
       <c r="Y2" s="9" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="Z2" s="9" t="s">
         <v>0</v>
@@ -5598,13 +5601,13 @@
         <v>11</v>
       </c>
       <c r="H3" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="I3" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="J3" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="K3" s="4" t="s">
         <v>21</v>
@@ -5649,7 +5652,7 @@
         <v>28</v>
       </c>
       <c r="Y3" s="10" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="Z3" s="10" t="s">
         <v>25</v>
@@ -5693,7 +5696,7 @@
         <v>66</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>243</v>
+        <v>312</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1">
@@ -5742,7 +5745,7 @@
         <v>0</v>
       </c>
       <c r="T4" s="18">
-        <f>K4+L4+ SUM(M4:S4)*5+AD4+AE4</f>
+        <f t="shared" ref="T4:T35" si="1">K4+L4+ SUM(M4:S4)*5+AD4+AE4</f>
         <v>-5</v>
       </c>
       <c r="U4" s="18"/>
@@ -5785,7 +5788,7 @@
         <v>88</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1">
@@ -5796,7 +5799,7 @@
         <v>1</v>
       </c>
       <c r="G5" s="1">
-        <f t="shared" ref="G5:G54" si="1">E5*50+50</f>
+        <f t="shared" ref="G5:G54" si="2">E5*50+50</f>
         <v>100</v>
       </c>
       <c r="H5" s="18"/>
@@ -5834,7 +5837,7 @@
         <v>0</v>
       </c>
       <c r="T5" s="18">
-        <f>K5+L5+ SUM(M5:S5)*5+AD5+AE5</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="U5" s="18"/>
@@ -5877,7 +5880,7 @@
         <v>91</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1">
@@ -5888,7 +5891,7 @@
         <v>1</v>
       </c>
       <c r="G6" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>150</v>
       </c>
       <c r="H6" s="18"/>
@@ -5926,7 +5929,7 @@
         <v>0</v>
       </c>
       <c r="T6" s="18">
-        <f>K6+L6+ SUM(M6:S6)*5+AD6+AE6</f>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="U6" s="18"/>
@@ -5969,7 +5972,7 @@
         <v>96</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1">
@@ -5980,7 +5983,7 @@
         <v>1</v>
       </c>
       <c r="G7" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="H7" s="18">
@@ -6020,7 +6023,7 @@
         <v>0</v>
       </c>
       <c r="T7" s="18">
-        <f>K7+L7+ SUM(M7:S7)*5+AD7+AE7</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="U7" s="18"/>
@@ -6063,7 +6066,7 @@
         <v>99</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1">
@@ -6074,7 +6077,7 @@
         <v>1</v>
       </c>
       <c r="G8" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>150</v>
       </c>
       <c r="H8" s="18"/>
@@ -6112,7 +6115,7 @@
         <v>0</v>
       </c>
       <c r="T8" s="18">
-        <f>K8+L8+ SUM(M8:S8)*5+AD8+AE8</f>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="U8" s="18"/>
@@ -6155,7 +6158,7 @@
         <v>102</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1">
@@ -6166,7 +6169,7 @@
         <v>1</v>
       </c>
       <c r="G9" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>250</v>
       </c>
       <c r="H9" s="18"/>
@@ -6204,7 +6207,7 @@
         <v>0</v>
       </c>
       <c r="T9" s="18">
-        <f>K9+L9+ SUM(M9:S9)*5+AD9+AE9</f>
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
       <c r="U9" s="18"/>
@@ -6247,7 +6250,7 @@
         <v>105</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1">
@@ -6258,7 +6261,7 @@
         <v>1</v>
       </c>
       <c r="G10" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>150</v>
       </c>
       <c r="H10" s="18">
@@ -6298,7 +6301,7 @@
         <v>0</v>
       </c>
       <c r="T10" s="18">
-        <f>K10+L10+ SUM(M10:S10)*5+AD10+AE10</f>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="U10" s="18"/>
@@ -6341,7 +6344,7 @@
         <v>174</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1">
@@ -6352,7 +6355,7 @@
         <v>1</v>
       </c>
       <c r="G11" s="1">
-        <f t="shared" ref="G11:G12" si="2">E11*50+50</f>
+        <f t="shared" ref="G11:G12" si="3">E11*50+50</f>
         <v>250</v>
       </c>
       <c r="H11" s="18"/>
@@ -6390,7 +6393,7 @@
         <v>0</v>
       </c>
       <c r="T11" s="18">
-        <f>K11+L11+ SUM(M11:S11)*5+AD11+AE11</f>
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
       <c r="U11" s="18"/>
@@ -6433,7 +6436,7 @@
         <v>176</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1">
@@ -6444,7 +6447,7 @@
         <v>1</v>
       </c>
       <c r="G12" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>200</v>
       </c>
       <c r="H12" s="18"/>
@@ -6482,7 +6485,7 @@
         <v>0</v>
       </c>
       <c r="T12" s="18">
-        <f>K12+L12+ SUM(M12:S12)*5+AD12+AE12</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="U12" s="18"/>
@@ -6525,19 +6528,19 @@
         <v>179</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F13" s="1">
         <v>1</v>
       </c>
       <c r="G13" s="1">
-        <f t="shared" ref="G13:G14" si="3">E13*50+50</f>
-        <v>50</v>
+        <f t="shared" ref="G13:G14" si="4">E13*50+50</f>
+        <v>100</v>
       </c>
       <c r="H13" s="18"/>
       <c r="I13" s="18">
@@ -6550,7 +6553,7 @@
         <v>0</v>
       </c>
       <c r="L13" s="18">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="M13" s="18">
         <v>0</v>
@@ -6574,8 +6577,8 @@
         <v>0</v>
       </c>
       <c r="T13" s="18">
-        <f>K13+L13+ SUM(M13:S13)*5+AD13+AE13</f>
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>8</v>
       </c>
       <c r="U13" s="18"/>
       <c r="V13" s="18"/>
@@ -6617,7 +6620,7 @@
         <v>182</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1">
@@ -6628,7 +6631,7 @@
         <v>1</v>
       </c>
       <c r="G14" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>200</v>
       </c>
       <c r="H14" s="18"/>
@@ -6666,7 +6669,7 @@
         <v>0</v>
       </c>
       <c r="T14" s="18">
-        <f>K14+L14+ SUM(M14:S14)*5+AD14+AE14</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="U14" s="18"/>
@@ -6709,18 +6712,18 @@
         <v>196</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1">
-        <f t="shared" ref="E15:E16" si="4">IF(T15&gt;=23,4,IF(AND(T15&gt;=18,T15&lt;23),3,IF(AND(T15&gt;=13,T15&lt;18),2,IF(AND(T15&gt;=8,T15&lt;13),1,0))))</f>
+        <f t="shared" ref="E15:E16" si="5">IF(T15&gt;=23,4,IF(AND(T15&gt;=18,T15&lt;23),3,IF(AND(T15&gt;=13,T15&lt;18),2,IF(AND(T15&gt;=8,T15&lt;13),1,0))))</f>
         <v>3</v>
       </c>
       <c r="F15" s="1">
         <v>1</v>
       </c>
       <c r="G15" s="1">
-        <f t="shared" ref="G15:G16" si="5">E15*50+50</f>
+        <f t="shared" ref="G15:G16" si="6">E15*50+50</f>
         <v>200</v>
       </c>
       <c r="H15" s="18"/>
@@ -6758,7 +6761,7 @@
         <v>0</v>
       </c>
       <c r="T15" s="18">
-        <f>K15+L15+ SUM(M15:S15)*5+AD15+AE15</f>
+        <f t="shared" si="1"/>
         <v>22</v>
       </c>
       <c r="U15" s="18"/>
@@ -6801,18 +6804,18 @@
         <v>198</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="F16" s="1">
         <v>1</v>
       </c>
       <c r="G16" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>150</v>
       </c>
       <c r="H16" s="18"/>
@@ -6850,7 +6853,7 @@
         <v>4</v>
       </c>
       <c r="T16" s="18">
-        <f>K16+L16+ SUM(M16:S16)*5+AD16+AE16</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="U16" s="18"/>
@@ -6893,18 +6896,18 @@
         <v>201</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1">
-        <f t="shared" ref="E17:E18" si="6">IF(T17&gt;=23,4,IF(AND(T17&gt;=18,T17&lt;23),3,IF(AND(T17&gt;=13,T17&lt;18),2,IF(AND(T17&gt;=8,T17&lt;13),1,0))))</f>
+        <f t="shared" ref="E17:E18" si="7">IF(T17&gt;=23,4,IF(AND(T17&gt;=18,T17&lt;23),3,IF(AND(T17&gt;=13,T17&lt;18),2,IF(AND(T17&gt;=8,T17&lt;13),1,0))))</f>
         <v>1</v>
       </c>
       <c r="F17" s="1">
         <v>1</v>
       </c>
       <c r="G17" s="1">
-        <f t="shared" ref="G17:G18" si="7">E17*50+50</f>
+        <f t="shared" ref="G17:G18" si="8">E17*50+50</f>
         <v>100</v>
       </c>
       <c r="H17" s="18">
@@ -6942,7 +6945,7 @@
         <v>0</v>
       </c>
       <c r="T17" s="18">
-        <f>K17+L17+ SUM(M17:S17)*5+AD17+AE17</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="U17" s="18"/>
@@ -6985,18 +6988,18 @@
         <v>204</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="F18" s="1">
         <v>1</v>
       </c>
       <c r="G18" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>100</v>
       </c>
       <c r="H18" s="18"/>
@@ -7034,7 +7037,7 @@
         <v>0</v>
       </c>
       <c r="T18" s="18">
-        <f>K18+L18+ SUM(M18:S18)*5+AD18+AE18</f>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="U18" s="18"/>
@@ -7077,20 +7080,20 @@
         <v>69</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>119</v>
       </c>
       <c r="E19" s="1">
-        <f t="shared" ref="E19:E29" si="8">IF(T19&gt;=23,4,IF(AND(T19&gt;=18,T19&lt;23),3,IF(AND(T19&gt;=13,T19&lt;18),2,IF(AND(T19&gt;=8,T19&lt;13),1,0))))</f>
+        <f t="shared" ref="E19:E29" si="9">IF(T19&gt;=23,4,IF(AND(T19&gt;=18,T19&lt;23),3,IF(AND(T19&gt;=13,T19&lt;18),2,IF(AND(T19&gt;=8,T19&lt;13),1,0))))</f>
         <v>1</v>
       </c>
       <c r="F19" s="1">
         <v>2</v>
       </c>
       <c r="G19" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="H19" s="18">
@@ -7128,7 +7131,7 @@
         <v>0</v>
       </c>
       <c r="T19" s="18">
-        <f>K19+L19+ SUM(M19:S19)*5+AD19+AE19</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="U19" s="18"/>
@@ -7173,20 +7176,20 @@
         <v>110</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>118</v>
       </c>
       <c r="E20" s="1">
-        <f t="shared" ref="E20:E21" si="9">IF(T20&gt;=23,4,IF(AND(T20&gt;=18,T20&lt;23),3,IF(AND(T20&gt;=13,T20&lt;18),2,IF(AND(T20&gt;=8,T20&lt;13),1,0))))</f>
+        <f t="shared" ref="E20:E21" si="10">IF(T20&gt;=23,4,IF(AND(T20&gt;=18,T20&lt;23),3,IF(AND(T20&gt;=13,T20&lt;18),2,IF(AND(T20&gt;=8,T20&lt;13),1,0))))</f>
         <v>2</v>
       </c>
       <c r="F20" s="1">
         <v>2</v>
       </c>
       <c r="G20" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>150</v>
       </c>
       <c r="H20" s="18">
@@ -7224,7 +7227,7 @@
         <v>0</v>
       </c>
       <c r="T20" s="18">
-        <f>K20+L20+ SUM(M20:S20)*5+AD20+AE20</f>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="U20" s="18"/>
@@ -7271,20 +7274,20 @@
         <v>111</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>120</v>
       </c>
       <c r="E21" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="F21" s="1">
         <v>2</v>
       </c>
       <c r="G21" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="H21" s="18">
@@ -7322,7 +7325,7 @@
         <v>0</v>
       </c>
       <c r="T21" s="18">
-        <f>K21+L21+ SUM(M21:S21)*5+AD21+AE21</f>
+        <f t="shared" si="1"/>
         <v>12.5</v>
       </c>
       <c r="U21" s="18"/>
@@ -7367,20 +7370,20 @@
         <v>112</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>121</v>
       </c>
       <c r="E22" s="1">
-        <f t="shared" ref="E22" si="10">IF(T22&gt;=23,4,IF(AND(T22&gt;=18,T22&lt;23),3,IF(AND(T22&gt;=13,T22&lt;18),2,IF(AND(T22&gt;=8,T22&lt;13),1,0))))</f>
+        <f t="shared" ref="E22" si="11">IF(T22&gt;=23,4,IF(AND(T22&gt;=18,T22&lt;23),3,IF(AND(T22&gt;=13,T22&lt;18),2,IF(AND(T22&gt;=8,T22&lt;13),1,0))))</f>
         <v>2</v>
       </c>
       <c r="F22" s="1">
         <v>2</v>
       </c>
       <c r="G22" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>150</v>
       </c>
       <c r="H22" s="18">
@@ -7418,7 +7421,7 @@
         <v>0</v>
       </c>
       <c r="T22" s="18">
-        <f>K22+L22+ SUM(M22:S22)*5+AD22+AE22</f>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="U22" s="18"/>
@@ -7465,20 +7468,20 @@
         <v>208</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>209</v>
       </c>
       <c r="E23" s="1">
-        <f t="shared" ref="E23:E25" si="11">IF(T23&gt;=23,4,IF(AND(T23&gt;=18,T23&lt;23),3,IF(AND(T23&gt;=13,T23&lt;18),2,IF(AND(T23&gt;=8,T23&lt;13),1,0))))</f>
+        <f t="shared" ref="E23:E25" si="12">IF(T23&gt;=23,4,IF(AND(T23&gt;=18,T23&lt;23),3,IF(AND(T23&gt;=13,T23&lt;18),2,IF(AND(T23&gt;=8,T23&lt;13),1,0))))</f>
         <v>0</v>
       </c>
       <c r="F23" s="1">
         <v>2</v>
       </c>
       <c r="G23" s="1">
-        <f t="shared" ref="G23:G25" si="12">E23*50+50</f>
+        <f t="shared" ref="G23:G25" si="13">E23*50+50</f>
         <v>50</v>
       </c>
       <c r="H23" s="18">
@@ -7516,7 +7519,7 @@
         <v>0</v>
       </c>
       <c r="T23" s="18">
-        <f>K23+L23+ SUM(M23:S23)*5+AD23+AE23</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="U23" s="18"/>
@@ -7561,20 +7564,20 @@
         <v>211</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>212</v>
       </c>
       <c r="E24" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="F24" s="1">
         <v>2</v>
       </c>
       <c r="G24" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>50</v>
       </c>
       <c r="H24" s="18">
@@ -7612,7 +7615,7 @@
         <v>0</v>
       </c>
       <c r="T24" s="18">
-        <f>K24+L24+ SUM(M24:S24)*5+AD24+AE24</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="U24" s="18"/>
@@ -7657,20 +7660,20 @@
         <v>213</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>214</v>
       </c>
       <c r="E25" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="F25" s="1">
         <v>2</v>
       </c>
       <c r="G25" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>100</v>
       </c>
       <c r="H25" s="18">
@@ -7708,7 +7711,7 @@
         <v>0</v>
       </c>
       <c r="T25" s="18">
-        <f>K25+L25+ SUM(M25:S25)*5+AD25+AE25</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="U25" s="18"/>
@@ -7755,20 +7758,20 @@
         <v>217</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>218</v>
       </c>
       <c r="E26" s="1">
-        <f t="shared" ref="E26:E27" si="13">IF(T26&gt;=23,4,IF(AND(T26&gt;=18,T26&lt;23),3,IF(AND(T26&gt;=13,T26&lt;18),2,IF(AND(T26&gt;=8,T26&lt;13),1,0))))</f>
+        <f t="shared" ref="E26:E27" si="14">IF(T26&gt;=23,4,IF(AND(T26&gt;=18,T26&lt;23),3,IF(AND(T26&gt;=13,T26&lt;18),2,IF(AND(T26&gt;=8,T26&lt;13),1,0))))</f>
         <v>3</v>
       </c>
       <c r="F26" s="1">
         <v>2</v>
       </c>
       <c r="G26" s="1">
-        <f t="shared" ref="G26:G27" si="14">E26*50+50</f>
+        <f t="shared" ref="G26:G27" si="15">E26*50+50</f>
         <v>200</v>
       </c>
       <c r="H26" s="18">
@@ -7806,7 +7809,7 @@
         <v>0</v>
       </c>
       <c r="T26" s="18">
-        <f>K26+L26+ SUM(M26:S26)*5+AD26+AE26</f>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="U26" s="18"/>
@@ -7853,20 +7856,20 @@
         <v>221</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>220</v>
       </c>
       <c r="E27" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>2</v>
       </c>
       <c r="F27" s="1">
         <v>2</v>
       </c>
       <c r="G27" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>150</v>
       </c>
       <c r="H27" s="18">
@@ -7904,7 +7907,7 @@
         <v>0</v>
       </c>
       <c r="T27" s="18">
-        <f>K27+L27+ SUM(M27:S27)*5+AD27+AE27</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="U27" s="18"/>
@@ -7951,20 +7954,20 @@
         <v>225</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>224</v>
       </c>
       <c r="E28" s="1">
-        <f t="shared" ref="E28" si="15">IF(T28&gt;=23,4,IF(AND(T28&gt;=18,T28&lt;23),3,IF(AND(T28&gt;=13,T28&lt;18),2,IF(AND(T28&gt;=8,T28&lt;13),1,0))))</f>
+        <f t="shared" ref="E28" si="16">IF(T28&gt;=23,4,IF(AND(T28&gt;=18,T28&lt;23),3,IF(AND(T28&gt;=13,T28&lt;18),2,IF(AND(T28&gt;=8,T28&lt;13),1,0))))</f>
         <v>4</v>
       </c>
       <c r="F28" s="1">
         <v>2</v>
       </c>
       <c r="G28" s="1">
-        <f t="shared" ref="G28" si="16">E28*50+50</f>
+        <f t="shared" ref="G28" si="17">E28*50+50</f>
         <v>250</v>
       </c>
       <c r="H28" s="18">
@@ -8002,7 +8005,7 @@
         <v>0</v>
       </c>
       <c r="T28" s="18">
-        <f>K28+L28+ SUM(M28:S28)*5+AD28+AE28</f>
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
       <c r="U28" s="18"/>
@@ -8049,18 +8052,18 @@
         <v>71</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F29" s="1">
         <v>3</v>
       </c>
       <c r="G29" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>50</v>
       </c>
       <c r="H29" s="18">
@@ -8098,7 +8101,7 @@
         <v>0</v>
       </c>
       <c r="T29" s="18">
-        <f>K29+L29+ SUM(M29:S29)*5+AD29+AE29</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="U29" s="18"/>
@@ -8141,18 +8144,18 @@
         <v>167</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="1">
-        <f t="shared" ref="E30:E31" si="17">IF(T30&gt;=23,4,IF(AND(T30&gt;=18,T30&lt;23),3,IF(AND(T30&gt;=13,T30&lt;18),2,IF(AND(T30&gt;=8,T30&lt;13),1,0))))</f>
+        <f t="shared" ref="E30:E31" si="18">IF(T30&gt;=23,4,IF(AND(T30&gt;=18,T30&lt;23),3,IF(AND(T30&gt;=13,T30&lt;18),2,IF(AND(T30&gt;=8,T30&lt;13),1,0))))</f>
         <v>1</v>
       </c>
       <c r="F30" s="1">
         <v>3</v>
       </c>
       <c r="G30" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="H30" s="18">
@@ -8190,7 +8193,7 @@
         <v>0</v>
       </c>
       <c r="T30" s="18">
-        <f>K30+L30+ SUM(M30:S30)*5+AD30+AE30</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="U30" s="18"/>
@@ -8237,18 +8240,18 @@
         <v>115</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>2</v>
       </c>
       <c r="F31" s="1">
         <v>3</v>
       </c>
       <c r="G31" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>150</v>
       </c>
       <c r="H31" s="18">
@@ -8288,7 +8291,7 @@
         <v>0</v>
       </c>
       <c r="T31" s="18">
-        <f>K31+L31+ SUM(M31:S31)*5+AD31+AE31</f>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="U31" s="18"/>
@@ -8331,18 +8334,18 @@
         <v>117</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="1">
-        <f t="shared" ref="E32:E33" si="18">IF(T32&gt;=23,4,IF(AND(T32&gt;=18,T32&lt;23),3,IF(AND(T32&gt;=13,T32&lt;18),2,IF(AND(T32&gt;=8,T32&lt;13),1,0))))</f>
+        <f t="shared" ref="E32:E33" si="19">IF(T32&gt;=23,4,IF(AND(T32&gt;=18,T32&lt;23),3,IF(AND(T32&gt;=13,T32&lt;18),2,IF(AND(T32&gt;=8,T32&lt;13),1,0))))</f>
         <v>2</v>
       </c>
       <c r="F32" s="1">
         <v>3</v>
       </c>
       <c r="G32" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>150</v>
       </c>
       <c r="H32" s="18">
@@ -8382,7 +8385,7 @@
         <v>0</v>
       </c>
       <c r="T32" s="18">
-        <f>K32+L32+ SUM(M32:S32)*5+AD32+AE32</f>
+        <f t="shared" si="1"/>
         <v>17.3</v>
       </c>
       <c r="U32" s="18"/>
@@ -8429,18 +8432,18 @@
         <v>143</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
       <c r="F33" s="1">
         <v>3</v>
       </c>
       <c r="G33" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="H33" s="18">
@@ -8480,7 +8483,7 @@
         <v>0</v>
       </c>
       <c r="T33" s="18">
-        <f>K33+L33+ SUM(M33:S33)*5+AD33+AE33</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="U33" s="18"/>
@@ -8523,18 +8526,18 @@
         <v>145</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="1">
-        <f t="shared" ref="E34:E35" si="19">IF(T34&gt;=23,4,IF(AND(T34&gt;=18,T34&lt;23),3,IF(AND(T34&gt;=13,T34&lt;18),2,IF(AND(T34&gt;=8,T34&lt;13),1,0))))</f>
+        <f t="shared" ref="E34:E35" si="20">IF(T34&gt;=23,4,IF(AND(T34&gt;=18,T34&lt;23),3,IF(AND(T34&gt;=13,T34&lt;18),2,IF(AND(T34&gt;=8,T34&lt;13),1,0))))</f>
         <v>3</v>
       </c>
       <c r="F34" s="1">
         <v>3</v>
       </c>
       <c r="G34" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>200</v>
       </c>
       <c r="H34" s="18">
@@ -8572,7 +8575,7 @@
         <v>0</v>
       </c>
       <c r="T34" s="18">
-        <f>K34+L34+ SUM(M34:S34)*5+AD34+AE34</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="U34" s="18"/>
@@ -8615,18 +8618,18 @@
         <v>147</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D35" s="1"/>
       <c r="E35" s="1">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>4</v>
       </c>
       <c r="F35" s="1">
         <v>3</v>
       </c>
       <c r="G35" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>250</v>
       </c>
       <c r="H35" s="18">
@@ -8666,7 +8669,7 @@
         <v>0</v>
       </c>
       <c r="T35" s="18">
-        <f>K35+L35+ SUM(M35:S35)*5+AD35+AE35</f>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="U35" s="18"/>
@@ -8709,18 +8712,18 @@
         <v>163</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>275</v>
+        <v>314</v>
       </c>
       <c r="D36" s="1"/>
       <c r="E36" s="1">
-        <f t="shared" ref="E36:E37" si="20">IF(T36&gt;=23,4,IF(AND(T36&gt;=18,T36&lt;23),3,IF(AND(T36&gt;=13,T36&lt;18),2,IF(AND(T36&gt;=8,T36&lt;13),1,0))))</f>
+        <f t="shared" ref="E36:E37" si="21">IF(T36&gt;=23,4,IF(AND(T36&gt;=18,T36&lt;23),3,IF(AND(T36&gt;=13,T36&lt;18),2,IF(AND(T36&gt;=8,T36&lt;13),1,0))))</f>
         <v>0</v>
       </c>
       <c r="F36" s="1">
         <v>3</v>
       </c>
       <c r="G36" s="1">
-        <f t="shared" ref="G36:G37" si="21">E36*50+50</f>
+        <f t="shared" ref="G36:G37" si="22">E36*50+50</f>
         <v>50</v>
       </c>
       <c r="H36" s="18">
@@ -8758,7 +8761,7 @@
         <v>0</v>
       </c>
       <c r="T36" s="18">
-        <f>K36+L36+ SUM(M36:S36)*5+AD36+AE36</f>
+        <f t="shared" ref="T36:T67" si="23">K36+L36+ SUM(M36:S36)*5+AD36+AE36</f>
         <v>1</v>
       </c>
       <c r="U36" s="18"/>
@@ -8801,18 +8804,18 @@
         <v>169</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D37" s="1"/>
       <c r="E37" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>3</v>
       </c>
       <c r="F37" s="1">
         <v>3</v>
       </c>
       <c r="G37" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>200</v>
       </c>
       <c r="H37" s="18">
@@ -8852,7 +8855,7 @@
         <v>0</v>
       </c>
       <c r="T37" s="18">
-        <f>K37+L37+ SUM(M37:S37)*5+AD37+AE37</f>
+        <f t="shared" si="23"/>
         <v>20</v>
       </c>
       <c r="U37" s="18"/>
@@ -8899,18 +8902,18 @@
         <v>123</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D38" s="1"/>
       <c r="E38" s="1">
-        <f t="shared" ref="E38" si="22">IF(T38&gt;=23,4,IF(AND(T38&gt;=18,T38&lt;23),3,IF(AND(T38&gt;=13,T38&lt;18),2,IF(AND(T38&gt;=8,T38&lt;13),1,0))))</f>
+        <f t="shared" ref="E38" si="24">IF(T38&gt;=23,4,IF(AND(T38&gt;=18,T38&lt;23),3,IF(AND(T38&gt;=13,T38&lt;18),2,IF(AND(T38&gt;=8,T38&lt;13),1,0))))</f>
         <v>0</v>
       </c>
       <c r="F38" s="1">
         <v>4</v>
       </c>
       <c r="G38" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>50</v>
       </c>
       <c r="H38" s="18">
@@ -8924,7 +8927,7 @@
         <v>0</v>
       </c>
       <c r="L38" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M38" s="18">
         <v>1</v>
@@ -8948,8 +8951,8 @@
         <v>0</v>
       </c>
       <c r="T38" s="18">
-        <f>K38+L38+ SUM(M38:S38)*5+AD38+AE38</f>
-        <v>5</v>
+        <f t="shared" si="23"/>
+        <v>6</v>
       </c>
       <c r="U38" s="18"/>
       <c r="V38" s="18"/>
@@ -8989,18 +8992,18 @@
         <v>124</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D39" s="1"/>
       <c r="E39" s="1">
-        <f t="shared" ref="E39:E40" si="23">IF(T39&gt;=23,4,IF(AND(T39&gt;=18,T39&lt;23),3,IF(AND(T39&gt;=13,T39&lt;18),2,IF(AND(T39&gt;=8,T39&lt;13),1,0))))</f>
+        <f t="shared" ref="E39:E40" si="25">IF(T39&gt;=23,4,IF(AND(T39&gt;=18,T39&lt;23),3,IF(AND(T39&gt;=13,T39&lt;18),2,IF(AND(T39&gt;=8,T39&lt;13),1,0))))</f>
         <v>1</v>
       </c>
       <c r="F39" s="1">
         <v>4</v>
       </c>
       <c r="G39" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="H39" s="18"/>
@@ -9038,7 +9041,7 @@
         <v>0</v>
       </c>
       <c r="T39" s="18">
-        <f>K39+L39+ SUM(M39:S39)*5+AD39+AE39</f>
+        <f t="shared" si="23"/>
         <v>10</v>
       </c>
       <c r="U39" s="18"/>
@@ -9079,18 +9082,18 @@
         <v>126</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D40" s="1"/>
       <c r="E40" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>2</v>
       </c>
       <c r="F40" s="1">
         <v>4</v>
       </c>
       <c r="G40" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>150</v>
       </c>
       <c r="H40" s="18">
@@ -9128,7 +9131,7 @@
         <v>0</v>
       </c>
       <c r="T40" s="18">
-        <f>K40+L40+ SUM(M40:S40)*5+AD40+AE40</f>
+        <f t="shared" si="23"/>
         <v>15</v>
       </c>
       <c r="U40" s="18"/>
@@ -9173,18 +9176,18 @@
         <v>131</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D41" s="1"/>
       <c r="E41" s="1">
-        <f t="shared" ref="E41:E42" si="24">IF(T41&gt;=23,4,IF(AND(T41&gt;=18,T41&lt;23),3,IF(AND(T41&gt;=13,T41&lt;18),2,IF(AND(T41&gt;=8,T41&lt;13),1,0))))</f>
+        <f t="shared" ref="E41:E42" si="26">IF(T41&gt;=23,4,IF(AND(T41&gt;=18,T41&lt;23),3,IF(AND(T41&gt;=13,T41&lt;18),2,IF(AND(T41&gt;=8,T41&lt;13),1,0))))</f>
         <v>3</v>
       </c>
       <c r="F41" s="1">
         <v>4</v>
       </c>
       <c r="G41" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>200</v>
       </c>
       <c r="H41" s="18"/>
@@ -9222,7 +9225,7 @@
         <v>0</v>
       </c>
       <c r="T41" s="18">
-        <f>K41+L41+ SUM(M41:S41)*5+AD41+AE41</f>
+        <f t="shared" si="23"/>
         <v>20</v>
       </c>
       <c r="U41" s="18"/>
@@ -9263,18 +9266,18 @@
         <v>149</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D42" s="1"/>
       <c r="E42" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>1</v>
       </c>
       <c r="F42" s="1">
         <v>4</v>
       </c>
       <c r="G42" s="1">
-        <f t="shared" ref="G42:G43" si="25">E42*50+50</f>
+        <f t="shared" ref="G42:G43" si="27">E42*50+50</f>
         <v>100</v>
       </c>
       <c r="H42" s="18"/>
@@ -9312,7 +9315,7 @@
         <v>0</v>
       </c>
       <c r="T42" s="18">
-        <f>K42+L42+ SUM(M42:S42)*5+AD42+AE42</f>
+        <f t="shared" si="23"/>
         <v>8</v>
       </c>
       <c r="U42" s="18"/>
@@ -9353,18 +9356,18 @@
         <v>151</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D43" s="1"/>
       <c r="E43" s="1">
-        <f t="shared" ref="E43:E44" si="26">IF(T43&gt;=23,4,IF(AND(T43&gt;=18,T43&lt;23),3,IF(AND(T43&gt;=13,T43&lt;18),2,IF(AND(T43&gt;=8,T43&lt;13),1,0))))</f>
+        <f t="shared" ref="E43:E44" si="28">IF(T43&gt;=23,4,IF(AND(T43&gt;=18,T43&lt;23),3,IF(AND(T43&gt;=13,T43&lt;18),2,IF(AND(T43&gt;=8,T43&lt;13),1,0))))</f>
         <v>2</v>
       </c>
       <c r="F43" s="1">
         <v>4</v>
       </c>
       <c r="G43" s="1">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>150</v>
       </c>
       <c r="H43" s="18">
@@ -9404,7 +9407,7 @@
         <v>0</v>
       </c>
       <c r="T43" s="18">
-        <f>K43+L43+ SUM(M43:S43)*5+AD43+AE43</f>
+        <f t="shared" si="23"/>
         <v>14</v>
       </c>
       <c r="U43" s="18"/>
@@ -9445,18 +9448,18 @@
         <v>153</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D44" s="1"/>
       <c r="E44" s="1">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>3</v>
       </c>
       <c r="F44" s="1">
         <v>4</v>
       </c>
       <c r="G44" s="1">
-        <f t="shared" ref="G44:G45" si="27">E44*50+50</f>
+        <f t="shared" ref="G44:G45" si="29">E44*50+50</f>
         <v>200</v>
       </c>
       <c r="H44" s="18"/>
@@ -9494,7 +9497,7 @@
         <v>0</v>
       </c>
       <c r="T44" s="18">
-        <f>K44+L44+ SUM(M44:S44)*5+AD44+AE44</f>
+        <f t="shared" si="23"/>
         <v>20</v>
       </c>
       <c r="U44" s="18"/>
@@ -9535,18 +9538,18 @@
         <v>155</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>284</v>
+        <v>313</v>
       </c>
       <c r="D45" s="1"/>
       <c r="E45" s="1">
-        <f t="shared" ref="E45:E46" si="28">IF(T45&gt;=23,4,IF(AND(T45&gt;=18,T45&lt;23),3,IF(AND(T45&gt;=13,T45&lt;18),2,IF(AND(T45&gt;=8,T45&lt;13),1,0))))</f>
+        <f t="shared" ref="E45:E46" si="30">IF(T45&gt;=23,4,IF(AND(T45&gt;=18,T45&lt;23),3,IF(AND(T45&gt;=13,T45&lt;18),2,IF(AND(T45&gt;=8,T45&lt;13),1,0))))</f>
         <v>0</v>
       </c>
       <c r="F45" s="1">
         <v>4</v>
       </c>
       <c r="G45" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>50</v>
       </c>
       <c r="H45" s="18">
@@ -9581,11 +9584,11 @@
         <v>0</v>
       </c>
       <c r="S45" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T45" s="18">
-        <f>K45+L45+ SUM(M45:S45)*5+AD45+AE45</f>
-        <v>0</v>
+        <f t="shared" si="23"/>
+        <v>5</v>
       </c>
       <c r="U45" s="18"/>
       <c r="V45" s="18"/>
@@ -9625,18 +9628,18 @@
         <v>157</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="D46" s="1"/>
       <c r="E46" s="1">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>2</v>
       </c>
       <c r="F46" s="1">
         <v>4</v>
       </c>
       <c r="G46" s="1">
-        <f t="shared" ref="G46:G47" si="29">E46*50+50</f>
+        <f t="shared" ref="G46:G47" si="31">E46*50+50</f>
         <v>150</v>
       </c>
       <c r="H46" s="18">
@@ -9676,7 +9679,7 @@
         <v>0</v>
       </c>
       <c r="T46" s="18">
-        <f>K46+L46+ SUM(M46:S46)*5+AD46+AE46</f>
+        <f t="shared" si="23"/>
         <v>13</v>
       </c>
       <c r="U46" s="18"/>
@@ -9717,18 +9720,18 @@
         <v>159</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="D47" s="1"/>
       <c r="E47" s="1">
-        <f t="shared" ref="E47:E48" si="30">IF(T47&gt;=23,4,IF(AND(T47&gt;=18,T47&lt;23),3,IF(AND(T47&gt;=13,T47&lt;18),2,IF(AND(T47&gt;=8,T47&lt;13),1,0))))</f>
+        <f t="shared" ref="E47:E48" si="32">IF(T47&gt;=23,4,IF(AND(T47&gt;=18,T47&lt;23),3,IF(AND(T47&gt;=13,T47&lt;18),2,IF(AND(T47&gt;=8,T47&lt;13),1,0))))</f>
         <v>2</v>
       </c>
       <c r="F47" s="1">
         <v>4</v>
       </c>
       <c r="G47" s="1">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>150</v>
       </c>
       <c r="H47" s="18">
@@ -9768,7 +9771,7 @@
         <v>0</v>
       </c>
       <c r="T47" s="18">
-        <f>K47+L47+ SUM(M47:S47)*5+AD47+AE47</f>
+        <f t="shared" si="23"/>
         <v>15</v>
       </c>
       <c r="U47" s="18"/>
@@ -9809,18 +9812,18 @@
         <v>161</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="D48" s="1"/>
       <c r="E48" s="1">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>4</v>
       </c>
       <c r="F48" s="1">
         <v>4</v>
       </c>
       <c r="G48" s="1">
-        <f t="shared" ref="G48" si="31">E48*50+50</f>
+        <f t="shared" ref="G48" si="33">E48*50+50</f>
         <v>250</v>
       </c>
       <c r="H48" s="18">
@@ -9860,7 +9863,7 @@
         <v>0</v>
       </c>
       <c r="T48" s="18">
-        <f>K48+L48+ SUM(M48:S48)*5+AD48+AE48</f>
+        <f t="shared" si="23"/>
         <v>30</v>
       </c>
       <c r="U48" s="18"/>
@@ -9901,18 +9904,18 @@
         <v>74</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="D49" s="1"/>
       <c r="E49" s="1">
-        <f t="shared" ref="E49" si="32">IF(T49&gt;=23,4,IF(AND(T49&gt;=18,T49&lt;23),3,IF(AND(T49&gt;=13,T49&lt;18),2,IF(AND(T49&gt;=8,T49&lt;13),1,0))))</f>
+        <f t="shared" ref="E49" si="34">IF(T49&gt;=23,4,IF(AND(T49&gt;=18,T49&lt;23),3,IF(AND(T49&gt;=13,T49&lt;18),2,IF(AND(T49&gt;=8,T49&lt;13),1,0))))</f>
         <v>1</v>
       </c>
       <c r="F49" s="1">
         <v>5</v>
       </c>
       <c r="G49" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="H49" s="18"/>
@@ -9950,7 +9953,7 @@
         <v>0</v>
       </c>
       <c r="T49" s="18">
-        <f>K49+L49+ SUM(M49:S49)*5+AD49+AE49</f>
+        <f t="shared" si="23"/>
         <v>10</v>
       </c>
       <c r="U49" s="18">
@@ -9993,18 +9996,18 @@
         <v>129</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="D50" s="1"/>
       <c r="E50" s="1">
-        <f t="shared" ref="E50:E51" si="33">IF(T50&gt;=23,4,IF(AND(T50&gt;=18,T50&lt;23),3,IF(AND(T50&gt;=13,T50&lt;18),2,IF(AND(T50&gt;=8,T50&lt;13),1,0))))</f>
+        <f t="shared" ref="E50:E51" si="35">IF(T50&gt;=23,4,IF(AND(T50&gt;=18,T50&lt;23),3,IF(AND(T50&gt;=13,T50&lt;18),2,IF(AND(T50&gt;=8,T50&lt;13),1,0))))</f>
         <v>1</v>
       </c>
       <c r="F50" s="1">
         <v>5</v>
       </c>
       <c r="G50" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="H50" s="18"/>
@@ -10042,7 +10045,7 @@
         <v>0</v>
       </c>
       <c r="T50" s="18">
-        <f>K50+L50+ SUM(M50:S50)*5+AD50+AE50</f>
+        <f t="shared" si="23"/>
         <v>10</v>
       </c>
       <c r="U50" s="18"/>
@@ -10052,7 +10055,7 @@
         <v>128</v>
       </c>
       <c r="Y50" s="18" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="Z50" s="18"/>
       <c r="AA50" s="18"/>
@@ -10085,18 +10088,18 @@
         <v>133</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="D51" s="1"/>
       <c r="E51" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>1</v>
       </c>
       <c r="F51" s="1">
         <v>5</v>
       </c>
       <c r="G51" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="H51" s="18"/>
@@ -10134,7 +10137,7 @@
         <v>0</v>
       </c>
       <c r="T51" s="18">
-        <f>K51+L51+ SUM(M51:S51)*5+AD51+AE51</f>
+        <f t="shared" si="23"/>
         <v>11</v>
       </c>
       <c r="U51" s="18"/>
@@ -10144,7 +10147,7 @@
         <v>134</v>
       </c>
       <c r="Y51" s="18" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="Z51" s="18"/>
       <c r="AA51" s="18"/>
@@ -10177,18 +10180,18 @@
         <v>136</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="D52" s="1"/>
       <c r="E52" s="1">
-        <f t="shared" ref="E52:E53" si="34">IF(T52&gt;=23,4,IF(AND(T52&gt;=18,T52&lt;23),3,IF(AND(T52&gt;=13,T52&lt;18),2,IF(AND(T52&gt;=8,T52&lt;13),1,0))))</f>
+        <f t="shared" ref="E52:E53" si="36">IF(T52&gt;=23,4,IF(AND(T52&gt;=18,T52&lt;23),3,IF(AND(T52&gt;=13,T52&lt;18),2,IF(AND(T52&gt;=8,T52&lt;13),1,0))))</f>
         <v>1</v>
       </c>
       <c r="F52" s="1">
         <v>5</v>
       </c>
       <c r="G52" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="H52" s="18"/>
@@ -10226,7 +10229,7 @@
         <v>0</v>
       </c>
       <c r="T52" s="18">
-        <f>K52+L52+ SUM(M52:S52)*5+AD52+AE52</f>
+        <f t="shared" si="23"/>
         <v>8</v>
       </c>
       <c r="U52" s="18"/>
@@ -10271,18 +10274,18 @@
         <v>139</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="D53" s="1"/>
       <c r="E53" s="1">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>2</v>
       </c>
       <c r="F53" s="1">
         <v>5</v>
       </c>
       <c r="G53" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>150</v>
       </c>
       <c r="H53" s="18"/>
@@ -10320,7 +10323,7 @@
         <v>1</v>
       </c>
       <c r="T53" s="18">
-        <f>K53+L53+ SUM(M53:S53)*5+AD53+AE53</f>
+        <f t="shared" si="23"/>
         <v>15</v>
       </c>
       <c r="U53" s="18"/>
@@ -10330,7 +10333,7 @@
         <v>138</v>
       </c>
       <c r="Y53" s="18" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="Z53" s="18"/>
       <c r="AA53" s="18"/>
@@ -10363,18 +10366,18 @@
         <v>141</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="D54" s="1"/>
       <c r="E54" s="1">
-        <f t="shared" ref="E54:E55" si="35">IF(T54&gt;=23,4,IF(AND(T54&gt;=18,T54&lt;23),3,IF(AND(T54&gt;=13,T54&lt;18),2,IF(AND(T54&gt;=8,T54&lt;13),1,0))))</f>
+        <f t="shared" ref="E54:E55" si="37">IF(T54&gt;=23,4,IF(AND(T54&gt;=18,T54&lt;23),3,IF(AND(T54&gt;=13,T54&lt;18),2,IF(AND(T54&gt;=8,T54&lt;13),1,0))))</f>
         <v>2</v>
       </c>
       <c r="F54" s="1">
         <v>5</v>
       </c>
       <c r="G54" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>150</v>
       </c>
       <c r="H54" s="18"/>
@@ -10412,7 +10415,7 @@
         <v>0</v>
       </c>
       <c r="T54" s="18">
-        <f>K54+L54+ SUM(M54:S54)*5+AD54+AE54</f>
+        <f t="shared" si="23"/>
         <v>15</v>
       </c>
       <c r="U54" s="18"/>
@@ -10457,18 +10460,18 @@
         <v>166</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="D55" s="1"/>
       <c r="E55" s="1">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>1</v>
       </c>
       <c r="F55" s="1">
         <v>5</v>
       </c>
       <c r="G55" s="1">
-        <f t="shared" ref="G55:G56" si="36">E55*50+50</f>
+        <f t="shared" ref="G55:G56" si="38">E55*50+50</f>
         <v>100</v>
       </c>
       <c r="H55" s="18"/>
@@ -10506,7 +10509,7 @@
         <v>0</v>
       </c>
       <c r="T55" s="18">
-        <f>K55+L55+ SUM(M55:S55)*5+AD55+AE55</f>
+        <f t="shared" si="23"/>
         <v>8</v>
       </c>
       <c r="U55" s="18"/>
@@ -10547,18 +10550,18 @@
         <v>171</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="D56" s="1"/>
       <c r="E56" s="1">
-        <f t="shared" ref="E56:E57" si="37">IF(T56&gt;=23,4,IF(AND(T56&gt;=18,T56&lt;23),3,IF(AND(T56&gt;=13,T56&lt;18),2,IF(AND(T56&gt;=8,T56&lt;13),1,0))))</f>
+        <f t="shared" ref="E56:E57" si="39">IF(T56&gt;=23,4,IF(AND(T56&gt;=18,T56&lt;23),3,IF(AND(T56&gt;=13,T56&lt;18),2,IF(AND(T56&gt;=8,T56&lt;13),1,0))))</f>
         <v>4</v>
       </c>
       <c r="F56" s="1">
         <v>5</v>
       </c>
       <c r="G56" s="1">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>250</v>
       </c>
       <c r="H56" s="18"/>
@@ -10596,7 +10599,7 @@
         <v>0</v>
       </c>
       <c r="T56" s="18">
-        <f>K56+L56+ SUM(M56:S56)*5+AD56+AE56</f>
+        <f t="shared" si="23"/>
         <v>25</v>
       </c>
       <c r="U56" s="18"/>
@@ -10641,18 +10644,18 @@
         <v>228</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="D57" s="1"/>
       <c r="E57" s="1">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>1</v>
       </c>
       <c r="F57" s="1">
         <v>5</v>
       </c>
       <c r="G57" s="1">
-        <f t="shared" ref="G57:G58" si="38">E57*50+50</f>
+        <f t="shared" ref="G57:G58" si="40">E57*50+50</f>
         <v>100</v>
       </c>
       <c r="H57" s="18"/>
@@ -10690,7 +10693,7 @@
         <v>0</v>
       </c>
       <c r="T57" s="18">
-        <f>K57+L57+ SUM(M57:S57)*5+AD57+AE57</f>
+        <f t="shared" si="23"/>
         <v>10</v>
       </c>
       <c r="U57" s="18"/>
@@ -10733,18 +10736,18 @@
         <v>230</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="D58" s="1"/>
       <c r="E58" s="1">
-        <f t="shared" ref="E58:E59" si="39">IF(T58&gt;=23,4,IF(AND(T58&gt;=18,T58&lt;23),3,IF(AND(T58&gt;=13,T58&lt;18),2,IF(AND(T58&gt;=8,T58&lt;13),1,0))))</f>
+        <f t="shared" ref="E58:E59" si="41">IF(T58&gt;=23,4,IF(AND(T58&gt;=18,T58&lt;23),3,IF(AND(T58&gt;=13,T58&lt;18),2,IF(AND(T58&gt;=8,T58&lt;13),1,0))))</f>
         <v>2</v>
       </c>
       <c r="F58" s="1">
         <v>5</v>
       </c>
       <c r="G58" s="1">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v>150</v>
       </c>
       <c r="H58" s="18"/>
@@ -10782,7 +10785,7 @@
         <v>0</v>
       </c>
       <c r="T58" s="18">
-        <f>K58+L58+ SUM(M58:S58)*5+AD58+AE58</f>
+        <f t="shared" si="23"/>
         <v>15</v>
       </c>
       <c r="U58" s="18"/>
@@ -10792,7 +10795,7 @@
         <v>94</v>
       </c>
       <c r="Y58" s="18" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="Z58" s="18">
         <v>31100002</v>
@@ -10827,18 +10830,18 @@
         <v>232</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="D59" s="1"/>
       <c r="E59" s="1">
-        <f t="shared" si="39"/>
+        <f t="shared" si="41"/>
         <v>4</v>
       </c>
       <c r="F59" s="1">
         <v>5</v>
       </c>
       <c r="G59" s="1">
-        <f t="shared" ref="G59" si="40">E59*50+50</f>
+        <f t="shared" ref="G59" si="42">E59*50+50</f>
         <v>250</v>
       </c>
       <c r="H59" s="18"/>
@@ -10876,7 +10879,7 @@
         <v>0</v>
       </c>
       <c r="T59" s="18">
-        <f>K59+L59+ SUM(M59:S59)*5+AD59+AE59</f>
+        <f t="shared" si="23"/>
         <v>25</v>
       </c>
       <c r="U59" s="18"/>
@@ -10914,24 +10917,24 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="E4:E59">
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="38" priority="7" operator="greaterThanOrEqual">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="8" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="9" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="10" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="11" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:AJ59">
-    <cfRule type="containsBlanks" dxfId="0" priority="1">
+    <cfRule type="containsBlanks" dxfId="33" priority="1">
       <formula>LEN(TRIM(H4))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
use adder data on equip plus
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Equip.xlsx
+++ b/ConfigData/Xlsx/Equip.xlsx
@@ -124,14 +124,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>AtkR</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>VitR</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>Spd</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -1252,6 +1244,14 @@
   </si>
   <si>
     <t>22100203;22100401</t>
+  </si>
+  <si>
+    <t>AtkP</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>VitP</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1967,7 +1967,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2022,6 +2022,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - 着色 1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2068,6 +2071,34 @@
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="38">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2416,34 +2447,6 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -4594,8 +4597,8 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:AI59" totalsRowShown="0">
   <autoFilter ref="A3:AI59"/>
-  <sortState ref="A4:AI38">
-    <sortCondition ref="A3:A38"/>
+  <sortState ref="A4:AI59">
+    <sortCondition ref="A3:A59"/>
   </sortState>
   <tableColumns count="35">
     <tableColumn id="1" name="Id"/>
@@ -4609,10 +4612,10 @@
     <tableColumn id="19" name="Value" dataDxfId="34">
       <calculatedColumnFormula>E4*50+50</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="ComposeRes" dataDxfId="6"/>
+    <tableColumn id="7" name="ComposeRes" dataDxfId="7"/>
     <tableColumn id="15" name="ComposeItemId" dataDxfId="33"/>
-    <tableColumn id="11" name="AtkR" dataDxfId="32"/>
-    <tableColumn id="8" name="VitR" dataDxfId="31"/>
+    <tableColumn id="11" name="AtkP" dataDxfId="32"/>
+    <tableColumn id="8" name="VitP" dataDxfId="31"/>
     <tableColumn id="6" name="Def" dataDxfId="30"/>
     <tableColumn id="22" name="Mag" dataDxfId="29"/>
     <tableColumn id="27" name="Spd" dataDxfId="28"/>
@@ -4620,27 +4623,27 @@
     <tableColumn id="25" name="Dhit" dataDxfId="26"/>
     <tableColumn id="24" name="Crt" dataDxfId="25"/>
     <tableColumn id="23" name="Luk" dataDxfId="24"/>
-    <tableColumn id="28" name="Sum" dataDxfId="23">
+    <tableColumn id="28" name="Sum" dataDxfId="0">
       <calculatedColumnFormula>J4+K4+ SUM(L4:R4)*5+AC4+AD4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="Range" dataDxfId="22"/>
-    <tableColumn id="33" name="Arrow" dataDxfId="21"/>
-    <tableColumn id="4" name="SlotId" dataDxfId="20"/>
-    <tableColumn id="9" name="EnergyRate" dataDxfId="19"/>
-    <tableColumn id="37" name="DungeonAttrs" dataDxfId="18"/>
-    <tableColumn id="20" name="HeroSkillId" dataDxfId="17"/>
-    <tableColumn id="29" name="MonsterAtk" dataDxfId="16"/>
-    <tableColumn id="30" name="MonsterHp" dataDxfId="15"/>
-    <tableColumn id="31" name="PickMethod" dataDxfId="14"/>
-    <tableColumn id="21" name="~SkillMark2" dataDxfId="13"/>
-    <tableColumn id="18" name="~SkillMark22" dataDxfId="12">
+    <tableColumn id="12" name="Range" dataDxfId="23"/>
+    <tableColumn id="33" name="Arrow" dataDxfId="22"/>
+    <tableColumn id="4" name="SlotId" dataDxfId="21"/>
+    <tableColumn id="9" name="EnergyRate" dataDxfId="20"/>
+    <tableColumn id="37" name="DungeonAttrs" dataDxfId="19"/>
+    <tableColumn id="20" name="HeroSkillId" dataDxfId="18"/>
+    <tableColumn id="29" name="MonsterAtk" dataDxfId="17"/>
+    <tableColumn id="30" name="MonsterHp" dataDxfId="16"/>
+    <tableColumn id="31" name="PickMethod" dataDxfId="15"/>
+    <tableColumn id="21" name="~SkillMark2" dataDxfId="14"/>
+    <tableColumn id="18" name="~SkillMark22" dataDxfId="13">
       <calculatedColumnFormula>IF(ISBLANK(AE4),0, LOOKUP(AE4,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AF4/100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="CommonSkillId" dataDxfId="11"/>
-    <tableColumn id="14" name="CommonSkillRate" dataDxfId="10"/>
-    <tableColumn id="17" name="RandomDrop" dataDxfId="9"/>
-    <tableColumn id="16" name="CanMerge" dataDxfId="8"/>
-    <tableColumn id="10" name="Url" dataDxfId="7"/>
+    <tableColumn id="13" name="CommonSkillId" dataDxfId="12"/>
+    <tableColumn id="14" name="CommonSkillRate" dataDxfId="11"/>
+    <tableColumn id="17" name="RandomDrop" dataDxfId="10"/>
+    <tableColumn id="16" name="CanMerge" dataDxfId="9"/>
+    <tableColumn id="10" name="Url" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4970,7 +4973,7 @@
   <dimension ref="A1:AI59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4:H59"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -5003,10 +5006,10 @@
         <v>3</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E1" s="11" t="s">
         <v>4</v>
@@ -5015,13 +5018,13 @@
         <v>5</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="H1" s="11" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="I1" s="11" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="J1" s="12" t="s">
         <v>13</v>
@@ -5030,73 +5033,73 @@
         <v>15</v>
       </c>
       <c r="L1" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="M1" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="N1" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="M1" s="13" t="s">
+      <c r="O1" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="N1" s="13" t="s">
+      <c r="P1" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="O1" s="13" t="s">
+      <c r="Q1" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="P1" s="13" t="s">
+      <c r="R1" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="Q1" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="R1" s="13" t="s">
-        <v>49</v>
-      </c>
       <c r="S1" s="14" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="T1" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="U1" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="V1" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="W1" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="X1" s="15" t="s">
+        <v>292</v>
+      </c>
+      <c r="Y1" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="U1" s="15" t="s">
-        <v>181</v>
-      </c>
-      <c r="V1" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="W1" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="X1" s="15" t="s">
-        <v>294</v>
-      </c>
-      <c r="Y1" s="15" t="s">
+      <c r="Z1" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA1" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="AB1" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="AC1" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD1" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="AE1" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="Z1" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="AA1" s="15" t="s">
-        <v>77</v>
-      </c>
-      <c r="AB1" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="AC1" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="AD1" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="AE1" s="14" t="s">
-        <v>41</v>
-      </c>
       <c r="AF1" s="14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="AG1" s="11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="AH1" s="11" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="AI1" s="11" t="s">
         <v>6</v>
@@ -5110,10 +5113,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>0</v>
@@ -5125,10 +5128,10 @@
         <v>0</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>14</v>
@@ -5140,7 +5143,7 @@
         <v>0</v>
       </c>
       <c r="M2" s="9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="N2" s="9" t="s">
         <v>0</v>
@@ -5158,52 +5161,52 @@
         <v>0</v>
       </c>
       <c r="S2" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="T2" s="7" t="s">
         <v>0</v>
       </c>
       <c r="U2" s="7" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="V2" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="W2" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="X2" s="7" t="s">
+        <v>293</v>
+      </c>
+      <c r="Y2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z2" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="AA2" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="AB2" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="AC2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="AD2" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AE2" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="X2" s="7" t="s">
-        <v>295</v>
-      </c>
-      <c r="Y2" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="Z2" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="AA2" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="AB2" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="AC2" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="AD2" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="AE2" s="5" t="s">
-        <v>42</v>
-      </c>
       <c r="AF2" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="AG2" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="AH2" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="AI2" s="2" t="s">
         <v>1</v>
@@ -5217,10 +5220,10 @@
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E3" t="s">
         <v>9</v>
@@ -5232,85 +5235,85 @@
         <v>11</v>
       </c>
       <c r="H3" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="I3" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="J3" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="L3" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="M3" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="N3" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="O3" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="P3" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q3" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="R3" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="S3" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="T3" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="L3" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="M3" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="N3" s="10" t="s">
+      <c r="U3" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="V3" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="W3" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="X3" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="Y3" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="O3" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="P3" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q3" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="R3" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="S3" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="T3" s="8" t="s">
+      <c r="Z3" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="AA3" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="AB3" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC3" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="AD3" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE3" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="U3" s="8" t="s">
-        <v>183</v>
-      </c>
-      <c r="V3" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="W3" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="X3" s="8" t="s">
-        <v>296</v>
-      </c>
-      <c r="Y3" s="8" t="s">
+      <c r="AF3" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="Z3" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="AA3" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="AB3" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="AC3" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="AD3" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="AE3" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="AF3" s="6" t="s">
-        <v>24</v>
-      </c>
       <c r="AG3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="AH3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="AI3" t="s">
         <v>12</v>
@@ -5321,14 +5324,14 @@
         <v>21100001</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1">
-        <f t="shared" ref="E4:E14" si="0">IF(S4&gt;=23,4,IF(AND(S4&gt;=18,S4&lt;23),3,IF(AND(S4&gt;=13,S4&lt;18),2,IF(AND(S4&gt;=8,S4&lt;13),1,0))))</f>
+        <f>IF(S4&gt;=23,4,IF(AND(S4&gt;=18,S4&lt;23),3,IF(AND(S4&gt;=13,S4&lt;18),2,IF(AND(S4&gt;=8,S4&lt;13),1,0))))</f>
         <v>0</v>
       </c>
       <c r="F4" s="1">
@@ -5342,13 +5345,13 @@
         <v>1</v>
       </c>
       <c r="I4" s="16" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="J4" s="16">
         <v>0</v>
       </c>
       <c r="K4" s="16">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L4" s="16">
         <v>0</v>
@@ -5372,13 +5375,13 @@
         <v>0</v>
       </c>
       <c r="S4" s="16">
-        <f t="shared" ref="S4:S35" si="1">J4+K4+ SUM(L4:R4)*5+AC4+AD4</f>
-        <v>-5</v>
+        <f>J4+K4+ SUM(L4:R4)*5+AC4+AD4</f>
+        <v>-4</v>
       </c>
       <c r="T4" s="16"/>
       <c r="U4" s="16"/>
       <c r="V4" s="16" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="W4" s="16" t="s">
         <v>17</v>
@@ -5398,13 +5401,13 @@
       <c r="AE4" s="16"/>
       <c r="AF4" s="16"/>
       <c r="AG4" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AH4" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AI4" s="16" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.15">
@@ -5412,28 +5415,28 @@
         <v>21100002</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1">
-        <f t="shared" si="0"/>
+        <f>IF(S5&gt;=23,4,IF(AND(S5&gt;=18,S5&lt;23),3,IF(AND(S5&gt;=13,S5&lt;18),2,IF(AND(S5&gt;=8,S5&lt;13),1,0))))</f>
         <v>1</v>
       </c>
       <c r="F5" s="1">
         <v>1</v>
       </c>
       <c r="G5" s="1">
-        <f t="shared" ref="G5:G54" si="2">E5*50+50</f>
+        <f>E5*50+50</f>
         <v>100</v>
       </c>
       <c r="H5" s="17">
         <v>1</v>
       </c>
       <c r="I5" s="16" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="J5" s="16">
         <v>0</v>
@@ -5463,13 +5466,13 @@
         <v>0</v>
       </c>
       <c r="S5" s="16">
-        <f t="shared" si="1"/>
+        <f>J5+K5+ SUM(L5:R5)*5+AC5+AD5</f>
         <v>10</v>
       </c>
       <c r="T5" s="16"/>
       <c r="U5" s="16"/>
       <c r="V5" s="16" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="W5" s="16" t="s">
         <v>17</v>
@@ -5489,13 +5492,13 @@
       <c r="AE5" s="16"/>
       <c r="AF5" s="16"/>
       <c r="AG5" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AH5" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AI5" s="16" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.15">
@@ -5503,28 +5506,28 @@
         <v>21100003</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1">
-        <f t="shared" si="0"/>
+        <f>IF(S6&gt;=23,4,IF(AND(S6&gt;=18,S6&lt;23),3,IF(AND(S6&gt;=13,S6&lt;18),2,IF(AND(S6&gt;=8,S6&lt;13),1,0))))</f>
         <v>2</v>
       </c>
       <c r="F6" s="1">
         <v>1</v>
       </c>
       <c r="G6" s="1">
-        <f t="shared" si="2"/>
+        <f>E6*50+50</f>
         <v>150</v>
       </c>
       <c r="H6" s="17">
         <v>1</v>
       </c>
       <c r="I6" s="16" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="J6" s="16">
         <v>0</v>
@@ -5554,13 +5557,13 @@
         <v>0</v>
       </c>
       <c r="S6" s="16">
-        <f t="shared" si="1"/>
+        <f>J6+K6+ SUM(L6:R6)*5+AC6+AD6</f>
         <v>14</v>
       </c>
       <c r="T6" s="16"/>
       <c r="U6" s="16"/>
       <c r="V6" s="16" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="W6" s="16" t="s">
         <v>17</v>
@@ -5580,13 +5583,13 @@
       <c r="AE6" s="16"/>
       <c r="AF6" s="16"/>
       <c r="AG6" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AH6" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AI6" s="16" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:35" x14ac:dyDescent="0.15">
@@ -5594,28 +5597,28 @@
         <v>21100004</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1">
-        <f t="shared" si="0"/>
+        <f>IF(S7&gt;=23,4,IF(AND(S7&gt;=18,S7&lt;23),3,IF(AND(S7&gt;=13,S7&lt;18),2,IF(AND(S7&gt;=8,S7&lt;13),1,0))))</f>
         <v>1</v>
       </c>
       <c r="F7" s="1">
         <v>1</v>
       </c>
       <c r="G7" s="1">
-        <f t="shared" si="2"/>
+        <f>E7*50+50</f>
         <v>100</v>
       </c>
       <c r="H7" s="17">
         <v>1</v>
       </c>
       <c r="I7" s="16" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="J7" s="16">
         <v>0</v>
@@ -5645,16 +5648,16 @@
         <v>0</v>
       </c>
       <c r="S7" s="16">
-        <f t="shared" si="1"/>
+        <f>J7+K7+ SUM(L7:R7)*5+AC7+AD7</f>
         <v>9</v>
       </c>
       <c r="T7" s="16"/>
       <c r="U7" s="16"/>
       <c r="V7" s="16" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="W7" s="16" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="X7" s="16"/>
       <c r="Y7" s="16"/>
@@ -5671,13 +5674,13 @@
       <c r="AE7" s="16"/>
       <c r="AF7" s="16"/>
       <c r="AG7" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AH7" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AI7" s="16" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:35" x14ac:dyDescent="0.15">
@@ -5685,28 +5688,28 @@
         <v>21100005</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1">
-        <f t="shared" si="0"/>
+        <f>IF(S8&gt;=23,4,IF(AND(S8&gt;=18,S8&lt;23),3,IF(AND(S8&gt;=13,S8&lt;18),2,IF(AND(S8&gt;=8,S8&lt;13),1,0))))</f>
         <v>2</v>
       </c>
       <c r="F8" s="1">
         <v>1</v>
       </c>
       <c r="G8" s="1">
-        <f t="shared" si="2"/>
+        <f>E8*50+50</f>
         <v>150</v>
       </c>
       <c r="H8" s="17">
         <v>1</v>
       </c>
       <c r="I8" s="16" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="J8" s="16">
         <v>0</v>
@@ -5736,16 +5739,16 @@
         <v>0</v>
       </c>
       <c r="S8" s="16">
-        <f t="shared" si="1"/>
+        <f>J8+K8+ SUM(L8:R8)*5+AC8+AD8</f>
         <v>13</v>
       </c>
       <c r="T8" s="16"/>
       <c r="U8" s="16"/>
       <c r="V8" s="16" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="W8" s="16" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="X8" s="16"/>
       <c r="Y8" s="16"/>
@@ -5762,13 +5765,13 @@
       <c r="AE8" s="16"/>
       <c r="AF8" s="16"/>
       <c r="AG8" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AH8" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AI8" s="16" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:35" x14ac:dyDescent="0.15">
@@ -5776,28 +5779,28 @@
         <v>21100006</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1">
-        <f t="shared" si="0"/>
+        <f>IF(S9&gt;=23,4,IF(AND(S9&gt;=18,S9&lt;23),3,IF(AND(S9&gt;=13,S9&lt;18),2,IF(AND(S9&gt;=8,S9&lt;13),1,0))))</f>
         <v>4</v>
       </c>
       <c r="F9" s="1">
         <v>1</v>
       </c>
       <c r="G9" s="1">
-        <f t="shared" si="2"/>
+        <f>E9*50+50</f>
         <v>250</v>
       </c>
       <c r="H9" s="17">
         <v>1</v>
       </c>
       <c r="I9" s="16" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="J9" s="16">
         <v>0</v>
@@ -5827,16 +5830,16 @@
         <v>0</v>
       </c>
       <c r="S9" s="16">
-        <f t="shared" si="1"/>
+        <f>J9+K9+ SUM(L9:R9)*5+AC9+AD9</f>
         <v>25</v>
       </c>
       <c r="T9" s="16"/>
       <c r="U9" s="16"/>
       <c r="V9" s="16" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="W9" s="16" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="X9" s="16"/>
       <c r="Y9" s="16"/>
@@ -5853,13 +5856,13 @@
       <c r="AE9" s="16"/>
       <c r="AF9" s="16"/>
       <c r="AG9" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AH9" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AI9" s="16" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10" spans="1:35" x14ac:dyDescent="0.15">
@@ -5867,28 +5870,28 @@
         <v>21100007</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1">
-        <f t="shared" si="0"/>
+        <f>IF(S10&gt;=23,4,IF(AND(S10&gt;=18,S10&lt;23),3,IF(AND(S10&gt;=13,S10&lt;18),2,IF(AND(S10&gt;=8,S10&lt;13),1,0))))</f>
         <v>2</v>
       </c>
       <c r="F10" s="1">
         <v>1</v>
       </c>
       <c r="G10" s="1">
-        <f t="shared" si="2"/>
+        <f>E10*50+50</f>
         <v>150</v>
       </c>
       <c r="H10" s="17">
         <v>1</v>
       </c>
       <c r="I10" s="16" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="J10" s="16">
         <v>0</v>
@@ -5918,16 +5921,16 @@
         <v>0</v>
       </c>
       <c r="S10" s="16">
-        <f t="shared" si="1"/>
+        <f>J10+K10+ SUM(L10:R10)*5+AC10+AD10</f>
         <v>14</v>
       </c>
       <c r="T10" s="16"/>
       <c r="U10" s="16"/>
       <c r="V10" s="16" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="W10" s="16" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="X10" s="16"/>
       <c r="Y10" s="16"/>
@@ -5944,13 +5947,13 @@
       <c r="AE10" s="16"/>
       <c r="AF10" s="16"/>
       <c r="AG10" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AH10" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AI10" s="16" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:35" x14ac:dyDescent="0.15">
@@ -5958,28 +5961,28 @@
         <v>21100008</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1">
-        <f t="shared" si="0"/>
+        <f>IF(S11&gt;=23,4,IF(AND(S11&gt;=18,S11&lt;23),3,IF(AND(S11&gt;=13,S11&lt;18),2,IF(AND(S11&gt;=8,S11&lt;13),1,0))))</f>
         <v>4</v>
       </c>
       <c r="F11" s="1">
         <v>1</v>
       </c>
       <c r="G11" s="1">
-        <f t="shared" ref="G11:G12" si="3">E11*50+50</f>
+        <f>E11*50+50</f>
         <v>250</v>
       </c>
       <c r="H11" s="17">
         <v>1</v>
       </c>
       <c r="I11" s="16" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="J11" s="16">
         <v>0</v>
@@ -6009,16 +6012,16 @@
         <v>0</v>
       </c>
       <c r="S11" s="16">
-        <f t="shared" si="1"/>
+        <f>J11+K11+ SUM(L11:R11)*5+AC11+AD11</f>
         <v>25</v>
       </c>
       <c r="T11" s="16"/>
       <c r="U11" s="16"/>
       <c r="V11" s="16" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="W11" s="16" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="X11" s="16"/>
       <c r="Y11" s="16"/>
@@ -6035,13 +6038,13 @@
       <c r="AE11" s="16"/>
       <c r="AF11" s="16"/>
       <c r="AG11" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AH11" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AI11" s="16" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="12" spans="1:35" x14ac:dyDescent="0.15">
@@ -6049,28 +6052,28 @@
         <v>21100009</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1">
-        <f t="shared" si="0"/>
+        <f>IF(S12&gt;=23,4,IF(AND(S12&gt;=18,S12&lt;23),3,IF(AND(S12&gt;=13,S12&lt;18),2,IF(AND(S12&gt;=8,S12&lt;13),1,0))))</f>
         <v>3</v>
       </c>
       <c r="F12" s="1">
         <v>1</v>
       </c>
       <c r="G12" s="1">
-        <f t="shared" si="3"/>
+        <f>E12*50+50</f>
         <v>200</v>
       </c>
       <c r="H12" s="17">
         <v>1</v>
       </c>
       <c r="I12" s="16" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="J12" s="16">
         <v>0</v>
@@ -6100,16 +6103,16 @@
         <v>0</v>
       </c>
       <c r="S12" s="16">
-        <f t="shared" si="1"/>
+        <f>J12+K12+ SUM(L12:R12)*5+AC12+AD12</f>
         <v>20</v>
       </c>
       <c r="T12" s="16"/>
       <c r="U12" s="16"/>
       <c r="V12" s="16" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="W12" s="16" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="X12" s="16"/>
       <c r="Y12" s="16"/>
@@ -6126,13 +6129,13 @@
       <c r="AE12" s="16"/>
       <c r="AF12" s="16"/>
       <c r="AG12" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AH12" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AI12" s="16" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="13" spans="1:35" x14ac:dyDescent="0.15">
@@ -6140,28 +6143,28 @@
         <v>21100010</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1">
-        <f t="shared" si="0"/>
+        <f>IF(S13&gt;=23,4,IF(AND(S13&gt;=18,S13&lt;23),3,IF(AND(S13&gt;=13,S13&lt;18),2,IF(AND(S13&gt;=8,S13&lt;13),1,0))))</f>
         <v>1</v>
       </c>
       <c r="F13" s="1">
         <v>1</v>
       </c>
       <c r="G13" s="1">
-        <f t="shared" ref="G13:G14" si="4">E13*50+50</f>
+        <f>E13*50+50</f>
         <v>100</v>
       </c>
       <c r="H13" s="17">
         <v>1</v>
       </c>
       <c r="I13" s="16" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="J13" s="16">
         <v>0</v>
@@ -6191,16 +6194,16 @@
         <v>0</v>
       </c>
       <c r="S13" s="16">
-        <f t="shared" si="1"/>
+        <f>J13+K13+ SUM(L13:R13)*5+AC13+AD13</f>
         <v>8</v>
       </c>
       <c r="T13" s="16"/>
       <c r="U13" s="16"/>
       <c r="V13" s="16" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="W13" s="16" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="X13" s="16"/>
       <c r="Y13" s="16"/>
@@ -6217,13 +6220,13 @@
       <c r="AE13" s="16"/>
       <c r="AF13" s="16"/>
       <c r="AG13" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AH13" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AI13" s="16" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="14" spans="1:35" x14ac:dyDescent="0.15">
@@ -6231,28 +6234,28 @@
         <v>21100011</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1">
-        <f t="shared" si="0"/>
+        <f>IF(S14&gt;=23,4,IF(AND(S14&gt;=18,S14&lt;23),3,IF(AND(S14&gt;=13,S14&lt;18),2,IF(AND(S14&gt;=8,S14&lt;13),1,0))))</f>
         <v>3</v>
       </c>
       <c r="F14" s="1">
         <v>1</v>
       </c>
       <c r="G14" s="1">
-        <f t="shared" si="4"/>
+        <f>E14*50+50</f>
         <v>200</v>
       </c>
       <c r="H14" s="17">
         <v>1</v>
       </c>
       <c r="I14" s="16" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="J14" s="16">
         <v>0</v>
@@ -6282,16 +6285,16 @@
         <v>0</v>
       </c>
       <c r="S14" s="16">
-        <f t="shared" si="1"/>
+        <f>J14+K14+ SUM(L14:R14)*5+AC14+AD14</f>
         <v>20</v>
       </c>
       <c r="T14" s="16"/>
       <c r="U14" s="16"/>
       <c r="V14" s="16" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="W14" s="16" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="X14" s="16"/>
       <c r="Y14" s="16"/>
@@ -6308,13 +6311,13 @@
       <c r="AE14" s="16"/>
       <c r="AF14" s="16"/>
       <c r="AG14" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AH14" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AI14" s="16" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="15" spans="1:35" x14ac:dyDescent="0.15">
@@ -6322,28 +6325,28 @@
         <v>21100012</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1">
-        <f t="shared" ref="E15:E16" si="5">IF(S15&gt;=23,4,IF(AND(S15&gt;=18,S15&lt;23),3,IF(AND(S15&gt;=13,S15&lt;18),2,IF(AND(S15&gt;=8,S15&lt;13),1,0))))</f>
+        <f>IF(S15&gt;=23,4,IF(AND(S15&gt;=18,S15&lt;23),3,IF(AND(S15&gt;=13,S15&lt;18),2,IF(AND(S15&gt;=8,S15&lt;13),1,0))))</f>
         <v>3</v>
       </c>
       <c r="F15" s="1">
         <v>1</v>
       </c>
       <c r="G15" s="1">
-        <f t="shared" ref="G15:G16" si="6">E15*50+50</f>
+        <f>E15*50+50</f>
         <v>200</v>
       </c>
       <c r="H15" s="17">
         <v>1</v>
       </c>
       <c r="I15" s="16" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="J15" s="16">
         <v>0</v>
@@ -6373,16 +6376,16 @@
         <v>0</v>
       </c>
       <c r="S15" s="16">
-        <f t="shared" si="1"/>
+        <f>J15+K15+ SUM(L15:R15)*5+AC15+AD15</f>
         <v>22</v>
       </c>
       <c r="T15" s="16"/>
       <c r="U15" s="16"/>
       <c r="V15" s="16" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="W15" s="16" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="X15" s="16"/>
       <c r="Y15" s="16"/>
@@ -6399,13 +6402,13 @@
       <c r="AE15" s="16"/>
       <c r="AF15" s="16"/>
       <c r="AG15" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AH15" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AI15" s="16" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="16" spans="1:35" x14ac:dyDescent="0.15">
@@ -6413,28 +6416,28 @@
         <v>21100013</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1">
-        <f t="shared" si="5"/>
+        <f>IF(S16&gt;=23,4,IF(AND(S16&gt;=18,S16&lt;23),3,IF(AND(S16&gt;=13,S16&lt;18),2,IF(AND(S16&gt;=8,S16&lt;13),1,0))))</f>
         <v>2</v>
       </c>
       <c r="F16" s="1">
         <v>1</v>
       </c>
       <c r="G16" s="1">
-        <f t="shared" si="6"/>
+        <f>E16*50+50</f>
         <v>150</v>
       </c>
       <c r="H16" s="17">
         <v>1</v>
       </c>
       <c r="I16" s="16" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="J16" s="16">
         <v>0</v>
@@ -6464,16 +6467,16 @@
         <v>4</v>
       </c>
       <c r="S16" s="16">
-        <f t="shared" si="1"/>
+        <f>J16+K16+ SUM(L16:R16)*5+AC16+AD16</f>
         <v>15</v>
       </c>
       <c r="T16" s="16"/>
       <c r="U16" s="16"/>
       <c r="V16" s="16" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="W16" s="16" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="X16" s="16"/>
       <c r="Y16" s="16"/>
@@ -6490,13 +6493,13 @@
       <c r="AE16" s="16"/>
       <c r="AF16" s="16"/>
       <c r="AG16" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AH16" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AI16" s="16" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="17" spans="1:35" x14ac:dyDescent="0.15">
@@ -6504,28 +6507,28 @@
         <v>21100014</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1">
-        <f t="shared" ref="E17:E18" si="7">IF(S17&gt;=23,4,IF(AND(S17&gt;=18,S17&lt;23),3,IF(AND(S17&gt;=13,S17&lt;18),2,IF(AND(S17&gt;=8,S17&lt;13),1,0))))</f>
+        <f>IF(S17&gt;=23,4,IF(AND(S17&gt;=18,S17&lt;23),3,IF(AND(S17&gt;=13,S17&lt;18),2,IF(AND(S17&gt;=8,S17&lt;13),1,0))))</f>
         <v>1</v>
       </c>
       <c r="F17" s="1">
         <v>1</v>
       </c>
       <c r="G17" s="1">
-        <f t="shared" ref="G17:G18" si="8">E17*50+50</f>
+        <f>E17*50+50</f>
         <v>100</v>
       </c>
       <c r="H17" s="17">
         <v>1</v>
       </c>
       <c r="I17" s="16" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="J17" s="16">
         <v>0</v>
@@ -6555,16 +6558,16 @@
         <v>0</v>
       </c>
       <c r="S17" s="16">
-        <f t="shared" si="1"/>
+        <f>J17+K17+ SUM(L17:R17)*5+AC17+AD17</f>
         <v>12</v>
       </c>
       <c r="T17" s="16"/>
       <c r="U17" s="16"/>
       <c r="V17" s="16" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="W17" s="16" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="X17" s="16"/>
       <c r="Y17" s="16"/>
@@ -6581,13 +6584,13 @@
       <c r="AE17" s="16"/>
       <c r="AF17" s="16"/>
       <c r="AG17" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AH17" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AI17" s="16" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="18" spans="1:35" x14ac:dyDescent="0.15">
@@ -6595,28 +6598,28 @@
         <v>21100015</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1">
-        <f t="shared" si="7"/>
+        <f>IF(S18&gt;=23,4,IF(AND(S18&gt;=18,S18&lt;23),3,IF(AND(S18&gt;=13,S18&lt;18),2,IF(AND(S18&gt;=8,S18&lt;13),1,0))))</f>
         <v>1</v>
       </c>
       <c r="F18" s="1">
         <v>1</v>
       </c>
       <c r="G18" s="1">
-        <f t="shared" si="8"/>
+        <f>E18*50+50</f>
         <v>100</v>
       </c>
       <c r="H18" s="17">
         <v>1</v>
       </c>
       <c r="I18" s="16" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="J18" s="16">
         <v>0</v>
@@ -6646,16 +6649,16 @@
         <v>0</v>
       </c>
       <c r="S18" s="16">
-        <f t="shared" si="1"/>
+        <f>J18+K18+ SUM(L18:R18)*5+AC18+AD18</f>
         <v>11</v>
       </c>
       <c r="T18" s="16"/>
       <c r="U18" s="16"/>
       <c r="V18" s="16" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="W18" s="16" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="X18" s="16"/>
       <c r="Y18" s="16"/>
@@ -6672,13 +6675,13 @@
       <c r="AE18" s="16"/>
       <c r="AF18" s="16"/>
       <c r="AG18" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AH18" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AI18" s="16" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="19" spans="1:35" x14ac:dyDescent="0.15">
@@ -6686,30 +6689,30 @@
         <v>21200001</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E19" s="1">
-        <f t="shared" ref="E19:E29" si="9">IF(S19&gt;=23,4,IF(AND(S19&gt;=18,S19&lt;23),3,IF(AND(S19&gt;=13,S19&lt;18),2,IF(AND(S19&gt;=8,S19&lt;13),1,0))))</f>
+        <f>IF(S19&gt;=23,4,IF(AND(S19&gt;=18,S19&lt;23),3,IF(AND(S19&gt;=13,S19&lt;18),2,IF(AND(S19&gt;=8,S19&lt;13),1,0))))</f>
         <v>1</v>
       </c>
       <c r="F19" s="1">
         <v>2</v>
       </c>
       <c r="G19" s="1">
-        <f t="shared" si="2"/>
+        <f>E19*50+50</f>
         <v>100</v>
       </c>
       <c r="H19" s="17">
         <v>1</v>
       </c>
       <c r="I19" s="16" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="J19" s="16">
         <v>0</v>
@@ -6739,7 +6742,7 @@
         <v>0</v>
       </c>
       <c r="S19" s="16">
-        <f t="shared" si="1"/>
+        <f>J19+K19+ SUM(L19:R19)*5+AC19+AD19</f>
         <v>10</v>
       </c>
       <c r="T19" s="16"/>
@@ -6755,7 +6758,7 @@
         <v>20</v>
       </c>
       <c r="AB19" s="16" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="AC19" s="16">
         <v>10</v>
@@ -6767,13 +6770,13 @@
       <c r="AE19" s="16"/>
       <c r="AF19" s="16"/>
       <c r="AG19" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AH19" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AI19" s="16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:35" x14ac:dyDescent="0.15">
@@ -6781,30 +6784,30 @@
         <v>21200002</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E20" s="1">
-        <f t="shared" ref="E20:E21" si="10">IF(S20&gt;=23,4,IF(AND(S20&gt;=18,S20&lt;23),3,IF(AND(S20&gt;=13,S20&lt;18),2,IF(AND(S20&gt;=8,S20&lt;13),1,0))))</f>
+        <f>IF(S20&gt;=23,4,IF(AND(S20&gt;=18,S20&lt;23),3,IF(AND(S20&gt;=13,S20&lt;18),2,IF(AND(S20&gt;=8,S20&lt;13),1,0))))</f>
         <v>2</v>
       </c>
       <c r="F20" s="1">
         <v>2</v>
       </c>
       <c r="G20" s="1">
-        <f t="shared" si="2"/>
+        <f>E20*50+50</f>
         <v>150</v>
       </c>
       <c r="H20" s="17">
         <v>1</v>
       </c>
       <c r="I20" s="16" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="J20" s="16">
         <v>0</v>
@@ -6834,14 +6837,14 @@
         <v>0</v>
       </c>
       <c r="S20" s="16">
-        <f t="shared" si="1"/>
+        <f>J20+K20+ SUM(L20:R20)*5+AC20+AD20</f>
         <v>14</v>
       </c>
       <c r="T20" s="16"/>
       <c r="U20" s="16"/>
       <c r="V20" s="16"/>
       <c r="W20" s="16" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="X20" s="16"/>
       <c r="Y20" s="16"/>
@@ -6852,7 +6855,7 @@
         <v>14</v>
       </c>
       <c r="AB20" s="16" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="AC20" s="16">
         <v>14</v>
@@ -6864,13 +6867,13 @@
       <c r="AE20" s="16"/>
       <c r="AF20" s="16"/>
       <c r="AG20" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AH20" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AI20" s="16" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="21" spans="1:35" x14ac:dyDescent="0.15">
@@ -6878,30 +6881,30 @@
         <v>21200003</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E21" s="1">
-        <f t="shared" si="10"/>
+        <f>IF(S21&gt;=23,4,IF(AND(S21&gt;=18,S21&lt;23),3,IF(AND(S21&gt;=13,S21&lt;18),2,IF(AND(S21&gt;=8,S21&lt;13),1,0))))</f>
         <v>1</v>
       </c>
       <c r="F21" s="1">
         <v>2</v>
       </c>
       <c r="G21" s="1">
-        <f t="shared" si="2"/>
+        <f>E21*50+50</f>
         <v>100</v>
       </c>
       <c r="H21" s="17">
         <v>1</v>
       </c>
       <c r="I21" s="16" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="J21" s="16">
         <v>0</v>
@@ -6931,14 +6934,14 @@
         <v>0</v>
       </c>
       <c r="S21" s="16">
-        <f t="shared" si="1"/>
+        <f>J21+K21+ SUM(L21:R21)*5+AC21+AD21</f>
         <v>12.5</v>
       </c>
       <c r="T21" s="16"/>
       <c r="U21" s="16"/>
       <c r="V21" s="16"/>
       <c r="W21" s="16" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="X21" s="16"/>
       <c r="Y21" s="16"/>
@@ -6947,7 +6950,7 @@
       </c>
       <c r="AA21" s="16"/>
       <c r="AB21" s="16" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="AC21" s="16">
         <v>12.5</v>
@@ -6959,13 +6962,13 @@
       <c r="AE21" s="16"/>
       <c r="AF21" s="16"/>
       <c r="AG21" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AH21" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AI21" s="16" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="22" spans="1:35" x14ac:dyDescent="0.15">
@@ -6973,30 +6976,30 @@
         <v>21200004</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E22" s="1">
-        <f t="shared" ref="E22" si="11">IF(S22&gt;=23,4,IF(AND(S22&gt;=18,S22&lt;23),3,IF(AND(S22&gt;=13,S22&lt;18),2,IF(AND(S22&gt;=8,S22&lt;13),1,0))))</f>
+        <f>IF(S22&gt;=23,4,IF(AND(S22&gt;=18,S22&lt;23),3,IF(AND(S22&gt;=13,S22&lt;18),2,IF(AND(S22&gt;=8,S22&lt;13),1,0))))</f>
         <v>2</v>
       </c>
       <c r="F22" s="1">
         <v>2</v>
       </c>
       <c r="G22" s="1">
-        <f t="shared" si="2"/>
+        <f>E22*50+50</f>
         <v>150</v>
       </c>
       <c r="H22" s="17">
         <v>1</v>
       </c>
       <c r="I22" s="16" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="J22" s="16">
         <v>0</v>
@@ -7026,14 +7029,14 @@
         <v>0</v>
       </c>
       <c r="S22" s="16">
-        <f t="shared" si="1"/>
+        <f>J22+K22+ SUM(L22:R22)*5+AC22+AD22</f>
         <v>14</v>
       </c>
       <c r="T22" s="16"/>
       <c r="U22" s="16"/>
       <c r="V22" s="16"/>
       <c r="W22" s="16" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="X22" s="16"/>
       <c r="Y22" s="16"/>
@@ -7044,7 +7047,7 @@
         <v>14</v>
       </c>
       <c r="AB22" s="16" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="AC22" s="16">
         <v>14</v>
@@ -7056,13 +7059,13 @@
       <c r="AE22" s="16"/>
       <c r="AF22" s="16"/>
       <c r="AG22" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AH22" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AI22" s="16" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="23" spans="1:35" x14ac:dyDescent="0.15">
@@ -7070,30 +7073,30 @@
         <v>21200005</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E23" s="1">
-        <f t="shared" ref="E23:E25" si="12">IF(S23&gt;=23,4,IF(AND(S23&gt;=18,S23&lt;23),3,IF(AND(S23&gt;=13,S23&lt;18),2,IF(AND(S23&gt;=8,S23&lt;13),1,0))))</f>
+        <f>IF(S23&gt;=23,4,IF(AND(S23&gt;=18,S23&lt;23),3,IF(AND(S23&gt;=13,S23&lt;18),2,IF(AND(S23&gt;=8,S23&lt;13),1,0))))</f>
         <v>0</v>
       </c>
       <c r="F23" s="1">
         <v>2</v>
       </c>
       <c r="G23" s="1">
-        <f t="shared" ref="G23:G25" si="13">E23*50+50</f>
+        <f>E23*50+50</f>
         <v>50</v>
       </c>
       <c r="H23" s="17">
         <v>1</v>
       </c>
       <c r="I23" s="16" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="J23" s="16">
         <v>0</v>
@@ -7123,14 +7126,14 @@
         <v>0</v>
       </c>
       <c r="S23" s="16">
-        <f t="shared" si="1"/>
+        <f>J23+K23+ SUM(L23:R23)*5+AC23+AD23</f>
         <v>6</v>
       </c>
       <c r="T23" s="16"/>
       <c r="U23" s="16"/>
       <c r="V23" s="16"/>
       <c r="W23" s="16" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="X23" s="16"/>
       <c r="Y23" s="16"/>
@@ -7139,7 +7142,7 @@
         <v>6</v>
       </c>
       <c r="AB23" s="16" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="AC23" s="16">
         <v>6</v>
@@ -7151,13 +7154,13 @@
       <c r="AE23" s="16"/>
       <c r="AF23" s="16"/>
       <c r="AG23" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AH23" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AI23" s="16" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="24" spans="1:35" x14ac:dyDescent="0.15">
@@ -7165,30 +7168,30 @@
         <v>21200006</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E24" s="1">
-        <f t="shared" si="12"/>
+        <f>IF(S24&gt;=23,4,IF(AND(S24&gt;=18,S24&lt;23),3,IF(AND(S24&gt;=13,S24&lt;18),2,IF(AND(S24&gt;=8,S24&lt;13),1,0))))</f>
         <v>0</v>
       </c>
       <c r="F24" s="1">
         <v>2</v>
       </c>
       <c r="G24" s="1">
-        <f t="shared" si="13"/>
+        <f>E24*50+50</f>
         <v>50</v>
       </c>
       <c r="H24" s="17">
         <v>1</v>
       </c>
       <c r="I24" s="16" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="J24" s="16">
         <v>0</v>
@@ -7218,14 +7221,14 @@
         <v>0</v>
       </c>
       <c r="S24" s="16">
-        <f t="shared" si="1"/>
+        <f>J24+K24+ SUM(L24:R24)*5+AC24+AD24</f>
         <v>6</v>
       </c>
       <c r="T24" s="16"/>
       <c r="U24" s="16"/>
       <c r="V24" s="16"/>
       <c r="W24" s="16" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="X24" s="16"/>
       <c r="Y24" s="16"/>
@@ -7234,7 +7237,7 @@
       </c>
       <c r="AA24" s="16"/>
       <c r="AB24" s="16" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="AC24" s="16">
         <v>6</v>
@@ -7246,13 +7249,13 @@
       <c r="AE24" s="16"/>
       <c r="AF24" s="16"/>
       <c r="AG24" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AH24" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AI24" s="16" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="25" spans="1:35" x14ac:dyDescent="0.15">
@@ -7260,30 +7263,30 @@
         <v>21200007</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E25" s="1">
-        <f t="shared" si="12"/>
+        <f>IF(S25&gt;=23,4,IF(AND(S25&gt;=18,S25&lt;23),3,IF(AND(S25&gt;=13,S25&lt;18),2,IF(AND(S25&gt;=8,S25&lt;13),1,0))))</f>
         <v>1</v>
       </c>
       <c r="F25" s="1">
         <v>2</v>
       </c>
       <c r="G25" s="1">
-        <f t="shared" si="13"/>
+        <f>E25*50+50</f>
         <v>100</v>
       </c>
       <c r="H25" s="17">
         <v>1</v>
       </c>
       <c r="I25" s="16" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="J25" s="16">
         <v>0</v>
@@ -7313,14 +7316,14 @@
         <v>0</v>
       </c>
       <c r="S25" s="16">
-        <f t="shared" si="1"/>
+        <f>J25+K25+ SUM(L25:R25)*5+AC25+AD25</f>
         <v>9</v>
       </c>
       <c r="T25" s="16"/>
       <c r="U25" s="16"/>
       <c r="V25" s="16"/>
       <c r="W25" s="16" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="X25" s="16"/>
       <c r="Y25" s="16"/>
@@ -7331,7 +7334,7 @@
         <v>6</v>
       </c>
       <c r="AB25" s="16" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="AC25" s="16">
         <v>9</v>
@@ -7343,13 +7346,13 @@
       <c r="AE25" s="16"/>
       <c r="AF25" s="16"/>
       <c r="AG25" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AH25" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AI25" s="16" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="26" spans="1:35" x14ac:dyDescent="0.15">
@@ -7357,30 +7360,30 @@
         <v>21200008</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="E26" s="1">
-        <f t="shared" ref="E26:E27" si="14">IF(S26&gt;=23,4,IF(AND(S26&gt;=18,S26&lt;23),3,IF(AND(S26&gt;=13,S26&lt;18),2,IF(AND(S26&gt;=8,S26&lt;13),1,0))))</f>
+        <f>IF(S26&gt;=23,4,IF(AND(S26&gt;=18,S26&lt;23),3,IF(AND(S26&gt;=13,S26&lt;18),2,IF(AND(S26&gt;=8,S26&lt;13),1,0))))</f>
         <v>3</v>
       </c>
       <c r="F26" s="1">
         <v>2</v>
       </c>
       <c r="G26" s="1">
-        <f t="shared" ref="G26:G27" si="15">E26*50+50</f>
+        <f>E26*50+50</f>
         <v>200</v>
       </c>
       <c r="H26" s="17">
         <v>1</v>
       </c>
       <c r="I26" s="16" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="J26" s="16">
         <v>0</v>
@@ -7410,14 +7413,14 @@
         <v>0</v>
       </c>
       <c r="S26" s="16">
-        <f t="shared" si="1"/>
+        <f>J26+K26+ SUM(L26:R26)*5+AC26+AD26</f>
         <v>18</v>
       </c>
       <c r="T26" s="16"/>
       <c r="U26" s="16"/>
       <c r="V26" s="16"/>
       <c r="W26" s="16" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="X26" s="16"/>
       <c r="Y26" s="16"/>
@@ -7428,7 +7431,7 @@
         <v>12</v>
       </c>
       <c r="AB26" s="16" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="AC26" s="16">
         <v>18</v>
@@ -7440,13 +7443,13 @@
       <c r="AE26" s="16"/>
       <c r="AF26" s="16"/>
       <c r="AG26" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AH26" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AI26" s="16" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="27" spans="1:35" x14ac:dyDescent="0.15">
@@ -7454,30 +7457,30 @@
         <v>21200009</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E27" s="1">
-        <f t="shared" si="14"/>
+        <f>IF(S27&gt;=23,4,IF(AND(S27&gt;=18,S27&lt;23),3,IF(AND(S27&gt;=13,S27&lt;18),2,IF(AND(S27&gt;=8,S27&lt;13),1,0))))</f>
         <v>2</v>
       </c>
       <c r="F27" s="1">
         <v>2</v>
       </c>
       <c r="G27" s="1">
-        <f t="shared" si="15"/>
+        <f>E27*50+50</f>
         <v>150</v>
       </c>
       <c r="H27" s="17">
         <v>1</v>
       </c>
       <c r="I27" s="16" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="J27" s="16">
         <v>0</v>
@@ -7507,14 +7510,14 @@
         <v>0</v>
       </c>
       <c r="S27" s="16">
-        <f t="shared" si="1"/>
+        <f>J27+K27+ SUM(L27:R27)*5+AC27+AD27</f>
         <v>15</v>
       </c>
       <c r="T27" s="16"/>
       <c r="U27" s="16"/>
       <c r="V27" s="16"/>
       <c r="W27" s="16" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="X27" s="16"/>
       <c r="Y27" s="16"/>
@@ -7525,7 +7528,7 @@
         <v>10</v>
       </c>
       <c r="AB27" s="16" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="AC27" s="16">
         <v>15</v>
@@ -7537,13 +7540,13 @@
       <c r="AE27" s="16"/>
       <c r="AF27" s="16"/>
       <c r="AG27" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AH27" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AI27" s="16" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="28" spans="1:35" x14ac:dyDescent="0.15">
@@ -7551,30 +7554,30 @@
         <v>21200010</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E28" s="1">
-        <f t="shared" ref="E28" si="16">IF(S28&gt;=23,4,IF(AND(S28&gt;=18,S28&lt;23),3,IF(AND(S28&gt;=13,S28&lt;18),2,IF(AND(S28&gt;=8,S28&lt;13),1,0))))</f>
+        <f>IF(S28&gt;=23,4,IF(AND(S28&gt;=18,S28&lt;23),3,IF(AND(S28&gt;=13,S28&lt;18),2,IF(AND(S28&gt;=8,S28&lt;13),1,0))))</f>
         <v>4</v>
       </c>
       <c r="F28" s="1">
         <v>2</v>
       </c>
       <c r="G28" s="1">
-        <f t="shared" ref="G28" si="17">E28*50+50</f>
+        <f>E28*50+50</f>
         <v>250</v>
       </c>
       <c r="H28" s="17">
         <v>1</v>
       </c>
       <c r="I28" s="16" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="J28" s="16">
         <v>0</v>
@@ -7604,14 +7607,14 @@
         <v>0</v>
       </c>
       <c r="S28" s="16">
-        <f t="shared" si="1"/>
+        <f>J28+K28+ SUM(L28:R28)*5+AC28+AD28</f>
         <v>25</v>
       </c>
       <c r="T28" s="16"/>
       <c r="U28" s="16"/>
       <c r="V28" s="16"/>
       <c r="W28" s="16" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="X28" s="16"/>
       <c r="Y28" s="16"/>
@@ -7622,7 +7625,7 @@
         <v>10</v>
       </c>
       <c r="AB28" s="16" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="AC28" s="16">
         <v>25</v>
@@ -7634,13 +7637,13 @@
       <c r="AE28" s="16"/>
       <c r="AF28" s="16"/>
       <c r="AG28" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AH28" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AI28" s="16" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="29" spans="1:35" x14ac:dyDescent="0.15">
@@ -7648,28 +7651,28 @@
         <v>21300001</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="1">
-        <f t="shared" si="9"/>
+        <f>IF(S29&gt;=23,4,IF(AND(S29&gt;=18,S29&lt;23),3,IF(AND(S29&gt;=13,S29&lt;18),2,IF(AND(S29&gt;=8,S29&lt;13),1,0))))</f>
         <v>0</v>
       </c>
       <c r="F29" s="1">
         <v>3</v>
       </c>
       <c r="G29" s="1">
-        <f t="shared" si="2"/>
+        <f>E29*50+50</f>
         <v>50</v>
       </c>
       <c r="H29" s="17">
         <v>1</v>
       </c>
       <c r="I29" s="16" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="J29" s="16">
         <v>5</v>
@@ -7699,12 +7702,12 @@
         <v>0</v>
       </c>
       <c r="S29" s="16">
-        <f t="shared" si="1"/>
+        <f>J29+K29+ SUM(L29:R29)*5+AC29+AD29</f>
         <v>5</v>
       </c>
       <c r="T29" s="16"/>
       <c r="U29" s="16" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="V29" s="16"/>
       <c r="W29" s="16" t="s">
@@ -7725,13 +7728,13 @@
       <c r="AE29" s="16"/>
       <c r="AF29" s="16"/>
       <c r="AG29" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AH29" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AI29" s="16" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="30" spans="1:35" x14ac:dyDescent="0.15">
@@ -7739,28 +7742,28 @@
         <v>21300002</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="1">
-        <f t="shared" ref="E30:E31" si="18">IF(S30&gt;=23,4,IF(AND(S30&gt;=18,S30&lt;23),3,IF(AND(S30&gt;=13,S30&lt;18),2,IF(AND(S30&gt;=8,S30&lt;13),1,0))))</f>
+        <f>IF(S30&gt;=23,4,IF(AND(S30&gt;=18,S30&lt;23),3,IF(AND(S30&gt;=13,S30&lt;18),2,IF(AND(S30&gt;=8,S30&lt;13),1,0))))</f>
         <v>1</v>
       </c>
       <c r="F30" s="1">
         <v>3</v>
       </c>
       <c r="G30" s="1">
-        <f t="shared" si="2"/>
+        <f>E30*50+50</f>
         <v>100</v>
       </c>
       <c r="H30" s="17">
         <v>1</v>
       </c>
       <c r="I30" s="16" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="J30" s="16">
         <v>6</v>
@@ -7790,16 +7793,16 @@
         <v>0</v>
       </c>
       <c r="S30" s="16">
-        <f t="shared" si="1"/>
+        <f>J30+K30+ SUM(L30:R30)*5+AC30+AD30</f>
         <v>12</v>
       </c>
       <c r="T30" s="16"/>
       <c r="U30" s="16" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="V30" s="16"/>
       <c r="W30" s="16" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="X30" s="16"/>
       <c r="Y30" s="16"/>
@@ -7820,13 +7823,13 @@
         <v>60</v>
       </c>
       <c r="AG30" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AH30" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AI30" s="16" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="31" spans="1:35" x14ac:dyDescent="0.15">
@@ -7834,28 +7837,28 @@
         <v>21300003</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="1">
-        <f t="shared" si="18"/>
+        <f>IF(S31&gt;=23,4,IF(AND(S31&gt;=18,S31&lt;23),3,IF(AND(S31&gt;=13,S31&lt;18),2,IF(AND(S31&gt;=8,S31&lt;13),1,0))))</f>
         <v>2</v>
       </c>
       <c r="F31" s="1">
         <v>3</v>
       </c>
       <c r="G31" s="1">
-        <f t="shared" si="2"/>
+        <f>E31*50+50</f>
         <v>150</v>
       </c>
       <c r="H31" s="17">
         <v>1</v>
       </c>
       <c r="I31" s="16" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="J31" s="16">
         <v>6</v>
@@ -7885,16 +7888,16 @@
         <v>0</v>
       </c>
       <c r="S31" s="16">
-        <f t="shared" si="1"/>
+        <f>J31+K31+ SUM(L31:R31)*5+AC31+AD31</f>
         <v>16</v>
       </c>
       <c r="T31" s="16"/>
       <c r="U31" s="16" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="V31" s="16"/>
       <c r="W31" s="16" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="X31" s="16"/>
       <c r="Y31" s="16"/>
@@ -7911,13 +7914,13 @@
       <c r="AE31" s="16"/>
       <c r="AF31" s="16"/>
       <c r="AG31" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AH31" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AI31" s="16" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="32" spans="1:35" x14ac:dyDescent="0.15">
@@ -7925,28 +7928,28 @@
         <v>21300004</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="1">
-        <f t="shared" ref="E32:E33" si="19">IF(S32&gt;=23,4,IF(AND(S32&gt;=18,S32&lt;23),3,IF(AND(S32&gt;=13,S32&lt;18),2,IF(AND(S32&gt;=8,S32&lt;13),1,0))))</f>
+        <f>IF(S32&gt;=23,4,IF(AND(S32&gt;=18,S32&lt;23),3,IF(AND(S32&gt;=13,S32&lt;18),2,IF(AND(S32&gt;=8,S32&lt;13),1,0))))</f>
         <v>2</v>
       </c>
       <c r="F32" s="1">
         <v>3</v>
       </c>
       <c r="G32" s="1">
-        <f t="shared" si="2"/>
+        <f>E32*50+50</f>
         <v>150</v>
       </c>
       <c r="H32" s="17">
         <v>1</v>
       </c>
       <c r="I32" s="16" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="J32" s="16">
         <v>8</v>
@@ -7976,16 +7979,16 @@
         <v>0</v>
       </c>
       <c r="S32" s="16">
-        <f t="shared" si="1"/>
+        <f>J32+K32+ SUM(L32:R32)*5+AC32+AD32</f>
         <v>17.3</v>
       </c>
       <c r="T32" s="16"/>
       <c r="U32" s="16" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="V32" s="16"/>
       <c r="W32" s="16" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="X32" s="16"/>
       <c r="Y32" s="16"/>
@@ -8006,13 +8009,13 @@
         <v>15</v>
       </c>
       <c r="AG32" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AH32" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AI32" s="16" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="33" spans="1:35" x14ac:dyDescent="0.15">
@@ -8020,28 +8023,28 @@
         <v>21300005</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="1">
-        <f t="shared" si="19"/>
+        <f>IF(S33&gt;=23,4,IF(AND(S33&gt;=18,S33&lt;23),3,IF(AND(S33&gt;=13,S33&lt;18),2,IF(AND(S33&gt;=8,S33&lt;13),1,0))))</f>
         <v>1</v>
       </c>
       <c r="F33" s="1">
         <v>3</v>
       </c>
       <c r="G33" s="1">
-        <f t="shared" si="2"/>
+        <f>E33*50+50</f>
         <v>100</v>
       </c>
       <c r="H33" s="17">
         <v>1</v>
       </c>
       <c r="I33" s="16" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="J33" s="16">
         <v>12</v>
@@ -8071,16 +8074,16 @@
         <v>0</v>
       </c>
       <c r="S33" s="16">
-        <f t="shared" si="1"/>
+        <f>J33+K33+ SUM(L33:R33)*5+AC33+AD33</f>
         <v>12</v>
       </c>
       <c r="T33" s="16"/>
       <c r="U33" s="16" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="V33" s="16"/>
       <c r="W33" s="16" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="X33" s="16"/>
       <c r="Y33" s="16"/>
@@ -8097,13 +8100,13 @@
       <c r="AE33" s="16"/>
       <c r="AF33" s="16"/>
       <c r="AG33" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AH33" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AI33" s="16" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="34" spans="1:35" x14ac:dyDescent="0.15">
@@ -8111,28 +8114,28 @@
         <v>21300006</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="1">
-        <f t="shared" ref="E34:E35" si="20">IF(S34&gt;=23,4,IF(AND(S34&gt;=18,S34&lt;23),3,IF(AND(S34&gt;=13,S34&lt;18),2,IF(AND(S34&gt;=8,S34&lt;13),1,0))))</f>
+        <f>IF(S34&gt;=23,4,IF(AND(S34&gt;=18,S34&lt;23),3,IF(AND(S34&gt;=13,S34&lt;18),2,IF(AND(S34&gt;=8,S34&lt;13),1,0))))</f>
         <v>3</v>
       </c>
       <c r="F34" s="1">
         <v>3</v>
       </c>
       <c r="G34" s="1">
-        <f t="shared" si="2"/>
+        <f>E34*50+50</f>
         <v>200</v>
       </c>
       <c r="H34" s="17">
         <v>1</v>
       </c>
       <c r="I34" s="16" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="J34" s="16">
         <v>20</v>
@@ -8162,16 +8165,16 @@
         <v>0</v>
       </c>
       <c r="S34" s="16">
-        <f t="shared" si="1"/>
+        <f>J34+K34+ SUM(L34:R34)*5+AC34+AD34</f>
         <v>20</v>
       </c>
       <c r="T34" s="16"/>
       <c r="U34" s="16" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="V34" s="16"/>
       <c r="W34" s="16" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="X34" s="16"/>
       <c r="Y34" s="16"/>
@@ -8188,13 +8191,13 @@
       <c r="AE34" s="16"/>
       <c r="AF34" s="16"/>
       <c r="AG34" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AH34" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AI34" s="16" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="35" spans="1:35" x14ac:dyDescent="0.15">
@@ -8202,28 +8205,28 @@
         <v>21300007</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D35" s="1"/>
       <c r="E35" s="1">
-        <f t="shared" si="20"/>
+        <f>IF(S35&gt;=23,4,IF(AND(S35&gt;=18,S35&lt;23),3,IF(AND(S35&gt;=13,S35&lt;18),2,IF(AND(S35&gt;=8,S35&lt;13),1,0))))</f>
         <v>4</v>
       </c>
       <c r="F35" s="1">
         <v>3</v>
       </c>
       <c r="G35" s="1">
-        <f t="shared" si="2"/>
+        <f>E35*50+50</f>
         <v>250</v>
       </c>
       <c r="H35" s="17">
         <v>1</v>
       </c>
       <c r="I35" s="16" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="J35" s="16">
         <v>5</v>
@@ -8253,16 +8256,16 @@
         <v>0</v>
       </c>
       <c r="S35" s="16">
-        <f t="shared" si="1"/>
+        <f>J35+K35+ SUM(L35:R35)*5+AC35+AD35</f>
         <v>30</v>
       </c>
       <c r="T35" s="16"/>
       <c r="U35" s="16" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="V35" s="16"/>
       <c r="W35" s="16" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="X35" s="16"/>
       <c r="Y35" s="16"/>
@@ -8279,13 +8282,13 @@
       <c r="AE35" s="16"/>
       <c r="AF35" s="16"/>
       <c r="AG35" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AH35" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AI35" s="16" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="36" spans="1:35" x14ac:dyDescent="0.15">
@@ -8293,28 +8296,28 @@
         <v>21300008</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D36" s="1"/>
       <c r="E36" s="1">
-        <f t="shared" ref="E36:E37" si="21">IF(S36&gt;=23,4,IF(AND(S36&gt;=18,S36&lt;23),3,IF(AND(S36&gt;=13,S36&lt;18),2,IF(AND(S36&gt;=8,S36&lt;13),1,0))))</f>
+        <f>IF(S36&gt;=23,4,IF(AND(S36&gt;=18,S36&lt;23),3,IF(AND(S36&gt;=13,S36&lt;18),2,IF(AND(S36&gt;=8,S36&lt;13),1,0))))</f>
         <v>0</v>
       </c>
       <c r="F36" s="1">
         <v>3</v>
       </c>
       <c r="G36" s="1">
-        <f t="shared" ref="G36:G37" si="22">E36*50+50</f>
+        <f>E36*50+50</f>
         <v>50</v>
       </c>
       <c r="H36" s="17">
         <v>1</v>
       </c>
       <c r="I36" s="16" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="J36" s="16">
         <v>1</v>
@@ -8344,16 +8347,16 @@
         <v>0</v>
       </c>
       <c r="S36" s="16">
-        <f t="shared" ref="S36:S59" si="23">J36+K36+ SUM(L36:R36)*5+AC36+AD36</f>
+        <f>J36+K36+ SUM(L36:R36)*5+AC36+AD36</f>
         <v>1</v>
       </c>
       <c r="T36" s="16"/>
       <c r="U36" s="16" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="V36" s="16"/>
       <c r="W36" s="16" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="X36" s="16"/>
       <c r="Y36" s="16"/>
@@ -8370,13 +8373,13 @@
       <c r="AE36" s="16"/>
       <c r="AF36" s="16"/>
       <c r="AG36" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AH36" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AI36" s="16" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="37" spans="1:35" x14ac:dyDescent="0.15">
@@ -8384,28 +8387,28 @@
         <v>21300009</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D37" s="1"/>
       <c r="E37" s="1">
-        <f t="shared" si="21"/>
+        <f>IF(S37&gt;=23,4,IF(AND(S37&gt;=18,S37&lt;23),3,IF(AND(S37&gt;=13,S37&lt;18),2,IF(AND(S37&gt;=8,S37&lt;13),1,0))))</f>
         <v>3</v>
       </c>
       <c r="F37" s="1">
         <v>3</v>
       </c>
       <c r="G37" s="1">
-        <f t="shared" si="22"/>
+        <f>E37*50+50</f>
         <v>200</v>
       </c>
       <c r="H37" s="17">
         <v>1</v>
       </c>
       <c r="I37" s="16" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="J37" s="16">
         <v>5</v>
@@ -8435,16 +8438,16 @@
         <v>0</v>
       </c>
       <c r="S37" s="16">
-        <f t="shared" si="23"/>
+        <f>J37+K37+ SUM(L37:R37)*5+AC37+AD37</f>
         <v>20</v>
       </c>
       <c r="T37" s="16"/>
       <c r="U37" s="16" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="V37" s="16"/>
       <c r="W37" s="16" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="X37" s="16"/>
       <c r="Y37" s="16"/>
@@ -8465,42 +8468,42 @@
         <v>100</v>
       </c>
       <c r="AG37" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AH37" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AI37" s="16" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="38" spans="1:35" x14ac:dyDescent="0.15">
-      <c r="A38">
+      <c r="A38" s="18">
         <v>21400001</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D38" s="1"/>
       <c r="E38" s="1">
-        <f t="shared" ref="E38" si="24">IF(S38&gt;=23,4,IF(AND(S38&gt;=18,S38&lt;23),3,IF(AND(S38&gt;=13,S38&lt;18),2,IF(AND(S38&gt;=8,S38&lt;13),1,0))))</f>
+        <f>IF(S38&gt;=23,4,IF(AND(S38&gt;=18,S38&lt;23),3,IF(AND(S38&gt;=13,S38&lt;18),2,IF(AND(S38&gt;=8,S38&lt;13),1,0))))</f>
         <v>0</v>
       </c>
       <c r="F38" s="1">
         <v>4</v>
       </c>
       <c r="G38" s="1">
-        <f t="shared" si="2"/>
+        <f>E38*50+50</f>
         <v>50</v>
       </c>
       <c r="H38" s="17">
         <v>1</v>
       </c>
       <c r="I38" s="16" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="J38" s="16">
         <v>0</v>
@@ -8530,7 +8533,7 @@
         <v>0</v>
       </c>
       <c r="S38" s="16">
-        <f t="shared" si="23"/>
+        <f>J38+K38+ SUM(L38:R38)*5+AC38+AD38</f>
         <v>6</v>
       </c>
       <c r="T38" s="16"/>
@@ -8554,42 +8557,42 @@
       <c r="AE38" s="16"/>
       <c r="AF38" s="16"/>
       <c r="AG38" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AH38" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AI38" s="16" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="39" spans="1:35" x14ac:dyDescent="0.15">
-      <c r="A39">
+      <c r="A39" s="18">
         <v>21400002</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D39" s="1"/>
       <c r="E39" s="1">
-        <f t="shared" ref="E39:E40" si="25">IF(S39&gt;=23,4,IF(AND(S39&gt;=18,S39&lt;23),3,IF(AND(S39&gt;=13,S39&lt;18),2,IF(AND(S39&gt;=8,S39&lt;13),1,0))))</f>
+        <f>IF(S39&gt;=23,4,IF(AND(S39&gt;=18,S39&lt;23),3,IF(AND(S39&gt;=13,S39&lt;18),2,IF(AND(S39&gt;=8,S39&lt;13),1,0))))</f>
         <v>1</v>
       </c>
       <c r="F39" s="1">
         <v>4</v>
       </c>
       <c r="G39" s="1">
-        <f t="shared" si="2"/>
+        <f>E39*50+50</f>
         <v>100</v>
       </c>
       <c r="H39" s="17">
         <v>1</v>
       </c>
       <c r="I39" s="16" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="J39" s="16">
         <v>0</v>
@@ -8619,7 +8622,7 @@
         <v>0</v>
       </c>
       <c r="S39" s="16">
-        <f t="shared" si="23"/>
+        <f>J39+K39+ SUM(L39:R39)*5+AC39+AD39</f>
         <v>10</v>
       </c>
       <c r="T39" s="16"/>
@@ -8643,42 +8646,42 @@
       <c r="AE39" s="16"/>
       <c r="AF39" s="16"/>
       <c r="AG39" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AH39" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AI39" s="16" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="40" spans="1:35" x14ac:dyDescent="0.15">
-      <c r="A40">
+      <c r="A40" s="18">
         <v>21400003</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D40" s="1"/>
       <c r="E40" s="1">
-        <f t="shared" si="25"/>
+        <f>IF(S40&gt;=23,4,IF(AND(S40&gt;=18,S40&lt;23),3,IF(AND(S40&gt;=13,S40&lt;18),2,IF(AND(S40&gt;=8,S40&lt;13),1,0))))</f>
         <v>2</v>
       </c>
       <c r="F40" s="1">
         <v>4</v>
       </c>
       <c r="G40" s="1">
-        <f t="shared" si="2"/>
+        <f>E40*50+50</f>
         <v>150</v>
       </c>
       <c r="H40" s="17">
         <v>1</v>
       </c>
       <c r="I40" s="16" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="J40" s="16">
         <v>0</v>
@@ -8708,14 +8711,14 @@
         <v>0</v>
       </c>
       <c r="S40" s="16">
-        <f t="shared" si="23"/>
+        <f>J40+K40+ SUM(L40:R40)*5+AC40+AD40</f>
         <v>15</v>
       </c>
       <c r="T40" s="16"/>
       <c r="U40" s="16"/>
       <c r="V40" s="16"/>
       <c r="W40" s="16" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="X40" s="16"/>
       <c r="Y40" s="16"/>
@@ -8736,13 +8739,13 @@
         <v>50</v>
       </c>
       <c r="AG40" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AH40" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AI40" s="16" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="41" spans="1:35" x14ac:dyDescent="0.15">
@@ -8750,28 +8753,28 @@
         <v>21400004</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D41" s="1"/>
       <c r="E41" s="1">
-        <f t="shared" ref="E41:E42" si="26">IF(S41&gt;=23,4,IF(AND(S41&gt;=18,S41&lt;23),3,IF(AND(S41&gt;=13,S41&lt;18),2,IF(AND(S41&gt;=8,S41&lt;13),1,0))))</f>
+        <f>IF(S41&gt;=23,4,IF(AND(S41&gt;=18,S41&lt;23),3,IF(AND(S41&gt;=13,S41&lt;18),2,IF(AND(S41&gt;=8,S41&lt;13),1,0))))</f>
         <v>3</v>
       </c>
       <c r="F41" s="1">
         <v>4</v>
       </c>
       <c r="G41" s="1">
-        <f t="shared" si="2"/>
+        <f>E41*50+50</f>
         <v>200</v>
       </c>
       <c r="H41" s="17">
         <v>1</v>
       </c>
       <c r="I41" s="16" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="J41" s="16">
         <v>0</v>
@@ -8801,14 +8804,14 @@
         <v>0</v>
       </c>
       <c r="S41" s="16">
-        <f t="shared" si="23"/>
+        <f>J41+K41+ SUM(L41:R41)*5+AC41+AD41</f>
         <v>20</v>
       </c>
       <c r="T41" s="16"/>
       <c r="U41" s="16"/>
       <c r="V41" s="16"/>
       <c r="W41" s="16" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="X41" s="16"/>
       <c r="Y41" s="16"/>
@@ -8825,42 +8828,42 @@
       <c r="AE41" s="16"/>
       <c r="AF41" s="16"/>
       <c r="AG41" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AH41" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AI41" s="16" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="42" spans="1:35" x14ac:dyDescent="0.15">
-      <c r="A42">
+      <c r="A42" s="18">
         <v>21400005</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D42" s="1"/>
       <c r="E42" s="1">
-        <f t="shared" si="26"/>
+        <f>IF(S42&gt;=23,4,IF(AND(S42&gt;=18,S42&lt;23),3,IF(AND(S42&gt;=13,S42&lt;18),2,IF(AND(S42&gt;=8,S42&lt;13),1,0))))</f>
         <v>1</v>
       </c>
       <c r="F42" s="1">
         <v>4</v>
       </c>
       <c r="G42" s="1">
-        <f t="shared" ref="G42:G43" si="27">E42*50+50</f>
+        <f>E42*50+50</f>
         <v>100</v>
       </c>
       <c r="H42" s="17">
         <v>1</v>
       </c>
       <c r="I42" s="16" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="J42" s="16">
         <v>0</v>
@@ -8890,14 +8893,14 @@
         <v>0</v>
       </c>
       <c r="S42" s="16">
-        <f t="shared" si="23"/>
+        <f>J42+K42+ SUM(L42:R42)*5+AC42+AD42</f>
         <v>8</v>
       </c>
       <c r="T42" s="16"/>
       <c r="U42" s="16"/>
       <c r="V42" s="16"/>
       <c r="W42" s="16" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="X42" s="16"/>
       <c r="Y42" s="16"/>
@@ -8914,13 +8917,13 @@
       <c r="AE42" s="16"/>
       <c r="AF42" s="16"/>
       <c r="AG42" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AH42" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AI42" s="16" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="43" spans="1:35" x14ac:dyDescent="0.15">
@@ -8928,28 +8931,28 @@
         <v>21400006</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D43" s="1"/>
       <c r="E43" s="1">
-        <f t="shared" ref="E43:E44" si="28">IF(S43&gt;=23,4,IF(AND(S43&gt;=18,S43&lt;23),3,IF(AND(S43&gt;=13,S43&lt;18),2,IF(AND(S43&gt;=8,S43&lt;13),1,0))))</f>
+        <f>IF(S43&gt;=23,4,IF(AND(S43&gt;=18,S43&lt;23),3,IF(AND(S43&gt;=13,S43&lt;18),2,IF(AND(S43&gt;=8,S43&lt;13),1,0))))</f>
         <v>2</v>
       </c>
       <c r="F43" s="1">
         <v>4</v>
       </c>
       <c r="G43" s="1">
-        <f t="shared" si="27"/>
+        <f>E43*50+50</f>
         <v>150</v>
       </c>
       <c r="H43" s="17">
         <v>1</v>
       </c>
       <c r="I43" s="16" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="J43" s="16">
         <v>0</v>
@@ -8979,14 +8982,14 @@
         <v>0</v>
       </c>
       <c r="S43" s="16">
-        <f t="shared" si="23"/>
+        <f>J43+K43+ SUM(L43:R43)*5+AC43+AD43</f>
         <v>14</v>
       </c>
       <c r="T43" s="16"/>
       <c r="U43" s="16"/>
       <c r="V43" s="16"/>
       <c r="W43" s="16" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="X43" s="16"/>
       <c r="Y43" s="16"/>
@@ -9003,13 +9006,13 @@
       <c r="AE43" s="16"/>
       <c r="AF43" s="16"/>
       <c r="AG43" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AH43" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AI43" s="16" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="44" spans="1:35" x14ac:dyDescent="0.15">
@@ -9017,28 +9020,28 @@
         <v>21400007</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D44" s="1"/>
       <c r="E44" s="1">
-        <f t="shared" si="28"/>
+        <f>IF(S44&gt;=23,4,IF(AND(S44&gt;=18,S44&lt;23),3,IF(AND(S44&gt;=13,S44&lt;18),2,IF(AND(S44&gt;=8,S44&lt;13),1,0))))</f>
         <v>3</v>
       </c>
       <c r="F44" s="1">
         <v>4</v>
       </c>
       <c r="G44" s="1">
-        <f t="shared" ref="G44:G45" si="29">E44*50+50</f>
+        <f>E44*50+50</f>
         <v>200</v>
       </c>
       <c r="H44" s="17">
         <v>1</v>
       </c>
       <c r="I44" s="16" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="J44" s="16">
         <v>0</v>
@@ -9068,14 +9071,14 @@
         <v>0</v>
       </c>
       <c r="S44" s="16">
-        <f t="shared" si="23"/>
+        <f>J44+K44+ SUM(L44:R44)*5+AC44+AD44</f>
         <v>20</v>
       </c>
       <c r="T44" s="16"/>
       <c r="U44" s="16"/>
       <c r="V44" s="16"/>
       <c r="W44" s="16" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="X44" s="16"/>
       <c r="Y44" s="16"/>
@@ -9092,42 +9095,42 @@
       <c r="AE44" s="16"/>
       <c r="AF44" s="16"/>
       <c r="AG44" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AH44" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AI44" s="16" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="45" spans="1:35" x14ac:dyDescent="0.15">
-      <c r="A45">
+      <c r="A45" s="18">
         <v>21400008</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D45" s="1"/>
       <c r="E45" s="1">
-        <f t="shared" ref="E45:E46" si="30">IF(S45&gt;=23,4,IF(AND(S45&gt;=18,S45&lt;23),3,IF(AND(S45&gt;=13,S45&lt;18),2,IF(AND(S45&gt;=8,S45&lt;13),1,0))))</f>
+        <f>IF(S45&gt;=23,4,IF(AND(S45&gt;=18,S45&lt;23),3,IF(AND(S45&gt;=13,S45&lt;18),2,IF(AND(S45&gt;=8,S45&lt;13),1,0))))</f>
         <v>0</v>
       </c>
       <c r="F45" s="1">
         <v>4</v>
       </c>
       <c r="G45" s="1">
-        <f t="shared" si="29"/>
+        <f>E45*50+50</f>
         <v>50</v>
       </c>
       <c r="H45" s="17">
         <v>1</v>
       </c>
       <c r="I45" s="16" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="J45" s="16">
         <v>0</v>
@@ -9157,14 +9160,14 @@
         <v>1</v>
       </c>
       <c r="S45" s="16">
-        <f t="shared" si="23"/>
+        <f>J45+K45+ SUM(L45:R45)*5+AC45+AD45</f>
         <v>5</v>
       </c>
       <c r="T45" s="16"/>
       <c r="U45" s="16"/>
       <c r="V45" s="16"/>
       <c r="W45" s="16" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="X45" s="16"/>
       <c r="Y45" s="16"/>
@@ -9181,13 +9184,13 @@
       <c r="AE45" s="16"/>
       <c r="AF45" s="16"/>
       <c r="AG45" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AH45" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AI45" s="16" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="46" spans="1:35" x14ac:dyDescent="0.15">
@@ -9195,28 +9198,28 @@
         <v>21400009</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D46" s="1"/>
       <c r="E46" s="1">
-        <f t="shared" si="30"/>
+        <f>IF(S46&gt;=23,4,IF(AND(S46&gt;=18,S46&lt;23),3,IF(AND(S46&gt;=13,S46&lt;18),2,IF(AND(S46&gt;=8,S46&lt;13),1,0))))</f>
         <v>2</v>
       </c>
       <c r="F46" s="1">
         <v>4</v>
       </c>
       <c r="G46" s="1">
-        <f t="shared" ref="G46:G47" si="31">E46*50+50</f>
+        <f>E46*50+50</f>
         <v>150</v>
       </c>
       <c r="H46" s="17">
         <v>1</v>
       </c>
       <c r="I46" s="16" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="J46" s="16">
         <v>0</v>
@@ -9246,14 +9249,14 @@
         <v>0</v>
       </c>
       <c r="S46" s="16">
-        <f t="shared" si="23"/>
+        <f>J46+K46+ SUM(L46:R46)*5+AC46+AD46</f>
         <v>13</v>
       </c>
       <c r="T46" s="16"/>
       <c r="U46" s="16"/>
       <c r="V46" s="16"/>
       <c r="W46" s="16" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="X46" s="16"/>
       <c r="Y46" s="16"/>
@@ -9270,13 +9273,13 @@
       <c r="AE46" s="16"/>
       <c r="AF46" s="16"/>
       <c r="AG46" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AH46" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AI46" s="16" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="47" spans="1:35" x14ac:dyDescent="0.15">
@@ -9284,28 +9287,28 @@
         <v>21400010</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D47" s="1"/>
       <c r="E47" s="1">
-        <f t="shared" ref="E47:E48" si="32">IF(S47&gt;=23,4,IF(AND(S47&gt;=18,S47&lt;23),3,IF(AND(S47&gt;=13,S47&lt;18),2,IF(AND(S47&gt;=8,S47&lt;13),1,0))))</f>
+        <f>IF(S47&gt;=23,4,IF(AND(S47&gt;=18,S47&lt;23),3,IF(AND(S47&gt;=13,S47&lt;18),2,IF(AND(S47&gt;=8,S47&lt;13),1,0))))</f>
         <v>2</v>
       </c>
       <c r="F47" s="1">
         <v>4</v>
       </c>
       <c r="G47" s="1">
-        <f t="shared" si="31"/>
+        <f>E47*50+50</f>
         <v>150</v>
       </c>
       <c r="H47" s="17">
         <v>1</v>
       </c>
       <c r="I47" s="16" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="J47" s="16">
         <v>0</v>
@@ -9335,14 +9338,14 @@
         <v>0</v>
       </c>
       <c r="S47" s="16">
-        <f t="shared" si="23"/>
+        <f>J47+K47+ SUM(L47:R47)*5+AC47+AD47</f>
         <v>15</v>
       </c>
       <c r="T47" s="16"/>
       <c r="U47" s="16"/>
       <c r="V47" s="16"/>
       <c r="W47" s="16" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="X47" s="16"/>
       <c r="Y47" s="16"/>
@@ -9359,13 +9362,13 @@
       <c r="AE47" s="16"/>
       <c r="AF47" s="16"/>
       <c r="AG47" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AH47" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AI47" s="16" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="48" spans="1:35" x14ac:dyDescent="0.15">
@@ -9373,28 +9376,28 @@
         <v>21400011</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D48" s="1"/>
       <c r="E48" s="1">
-        <f t="shared" si="32"/>
+        <f>IF(S48&gt;=23,4,IF(AND(S48&gt;=18,S48&lt;23),3,IF(AND(S48&gt;=13,S48&lt;18),2,IF(AND(S48&gt;=8,S48&lt;13),1,0))))</f>
         <v>4</v>
       </c>
       <c r="F48" s="1">
         <v>4</v>
       </c>
       <c r="G48" s="1">
-        <f t="shared" ref="G48" si="33">E48*50+50</f>
+        <f>E48*50+50</f>
         <v>250</v>
       </c>
       <c r="H48" s="17">
         <v>1</v>
       </c>
       <c r="I48" s="16" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="J48" s="16">
         <v>0</v>
@@ -9424,14 +9427,14 @@
         <v>0</v>
       </c>
       <c r="S48" s="16">
-        <f t="shared" si="23"/>
+        <f>J48+K48+ SUM(L48:R48)*5+AC48+AD48</f>
         <v>30</v>
       </c>
       <c r="T48" s="16"/>
       <c r="U48" s="16"/>
       <c r="V48" s="16"/>
       <c r="W48" s="16" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="X48" s="16"/>
       <c r="Y48" s="16"/>
@@ -9448,42 +9451,42 @@
       <c r="AE48" s="16"/>
       <c r="AF48" s="16"/>
       <c r="AG48" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AH48" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AI48" s="16" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="49" spans="1:35" x14ac:dyDescent="0.15">
-      <c r="A49">
+      <c r="A49" s="18">
         <v>21500001</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D49" s="1"/>
       <c r="E49" s="1">
-        <f t="shared" ref="E49" si="34">IF(S49&gt;=23,4,IF(AND(S49&gt;=18,S49&lt;23),3,IF(AND(S49&gt;=13,S49&lt;18),2,IF(AND(S49&gt;=8,S49&lt;13),1,0))))</f>
+        <f>IF(S49&gt;=23,4,IF(AND(S49&gt;=18,S49&lt;23),3,IF(AND(S49&gt;=13,S49&lt;18),2,IF(AND(S49&gt;=8,S49&lt;13),1,0))))</f>
         <v>1</v>
       </c>
       <c r="F49" s="1">
         <v>5</v>
       </c>
       <c r="G49" s="1">
-        <f t="shared" si="2"/>
+        <f>E49*50+50</f>
         <v>100</v>
       </c>
       <c r="H49" s="17">
         <v>1</v>
       </c>
       <c r="I49" s="16" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="J49" s="16">
         <v>0</v>
@@ -9513,7 +9516,7 @@
         <v>0</v>
       </c>
       <c r="S49" s="16">
-        <f t="shared" si="23"/>
+        <f>J49+K49+ SUM(L49:R49)*5+AC49+AD49</f>
         <v>10</v>
       </c>
       <c r="T49" s="16">
@@ -9522,7 +9525,7 @@
       <c r="U49" s="16"/>
       <c r="V49" s="16"/>
       <c r="W49" s="16" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="X49" s="16"/>
       <c r="Y49" s="16"/>
@@ -9539,42 +9542,42 @@
       <c r="AE49" s="16"/>
       <c r="AF49" s="16"/>
       <c r="AG49" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AH49" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AI49" s="16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="50" spans="1:35" x14ac:dyDescent="0.15">
-      <c r="A50">
+      <c r="A50" s="18">
         <v>21500002</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D50" s="1"/>
       <c r="E50" s="1">
-        <f t="shared" ref="E50:E51" si="35">IF(S50&gt;=23,4,IF(AND(S50&gt;=18,S50&lt;23),3,IF(AND(S50&gt;=13,S50&lt;18),2,IF(AND(S50&gt;=8,S50&lt;13),1,0))))</f>
+        <f>IF(S50&gt;=23,4,IF(AND(S50&gt;=18,S50&lt;23),3,IF(AND(S50&gt;=13,S50&lt;18),2,IF(AND(S50&gt;=8,S50&lt;13),1,0))))</f>
         <v>1</v>
       </c>
       <c r="F50" s="1">
         <v>5</v>
       </c>
       <c r="G50" s="1">
-        <f t="shared" si="2"/>
+        <f>E50*50+50</f>
         <v>100</v>
       </c>
       <c r="H50" s="17">
         <v>1</v>
       </c>
       <c r="I50" s="16" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="J50" s="16">
         <v>0</v>
@@ -9604,17 +9607,17 @@
         <v>0</v>
       </c>
       <c r="S50" s="16">
-        <f t="shared" si="23"/>
+        <f>J50+K50+ SUM(L50:R50)*5+AC50+AD50</f>
         <v>10</v>
       </c>
       <c r="T50" s="16"/>
       <c r="U50" s="16"/>
       <c r="V50" s="16"/>
       <c r="W50" s="16" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="X50" s="16" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="Y50" s="16"/>
       <c r="Z50" s="16"/>
@@ -9630,42 +9633,42 @@
       <c r="AE50" s="16"/>
       <c r="AF50" s="16"/>
       <c r="AG50" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AH50" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AI50" s="16" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="51" spans="1:35" x14ac:dyDescent="0.15">
-      <c r="A51">
+      <c r="A51" s="18">
         <v>21500003</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D51" s="1"/>
       <c r="E51" s="1">
-        <f t="shared" si="35"/>
+        <f>IF(S51&gt;=23,4,IF(AND(S51&gt;=18,S51&lt;23),3,IF(AND(S51&gt;=13,S51&lt;18),2,IF(AND(S51&gt;=8,S51&lt;13),1,0))))</f>
         <v>1</v>
       </c>
       <c r="F51" s="1">
         <v>5</v>
       </c>
       <c r="G51" s="1">
-        <f t="shared" si="2"/>
+        <f>E51*50+50</f>
         <v>100</v>
       </c>
       <c r="H51" s="17">
         <v>1</v>
       </c>
       <c r="I51" s="16" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="J51" s="16">
         <v>0</v>
@@ -9695,17 +9698,17 @@
         <v>0</v>
       </c>
       <c r="S51" s="16">
-        <f t="shared" si="23"/>
+        <f>J51+K51+ SUM(L51:R51)*5+AC51+AD51</f>
         <v>11</v>
       </c>
       <c r="T51" s="16"/>
       <c r="U51" s="16"/>
       <c r="V51" s="16"/>
       <c r="W51" s="16" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="X51" s="16" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="Y51" s="16"/>
       <c r="Z51" s="16"/>
@@ -9721,42 +9724,42 @@
       <c r="AE51" s="16"/>
       <c r="AF51" s="16"/>
       <c r="AG51" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AH51" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AI51" s="16" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="52" spans="1:35" x14ac:dyDescent="0.15">
-      <c r="A52">
+      <c r="A52" s="18">
         <v>21500004</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D52" s="1"/>
       <c r="E52" s="1">
-        <f t="shared" ref="E52:E53" si="36">IF(S52&gt;=23,4,IF(AND(S52&gt;=18,S52&lt;23),3,IF(AND(S52&gt;=13,S52&lt;18),2,IF(AND(S52&gt;=8,S52&lt;13),1,0))))</f>
+        <f>IF(S52&gt;=23,4,IF(AND(S52&gt;=18,S52&lt;23),3,IF(AND(S52&gt;=13,S52&lt;18),2,IF(AND(S52&gt;=8,S52&lt;13),1,0))))</f>
         <v>1</v>
       </c>
       <c r="F52" s="1">
         <v>5</v>
       </c>
       <c r="G52" s="1">
-        <f t="shared" si="2"/>
+        <f>E52*50+50</f>
         <v>100</v>
       </c>
       <c r="H52" s="17">
         <v>1</v>
       </c>
       <c r="I52" s="16" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="J52" s="16">
         <v>0</v>
@@ -9786,14 +9789,14 @@
         <v>0</v>
       </c>
       <c r="S52" s="16">
-        <f t="shared" si="23"/>
+        <f>J52+K52+ SUM(L52:R52)*5+AC52+AD52</f>
         <v>8</v>
       </c>
       <c r="T52" s="16"/>
       <c r="U52" s="16"/>
       <c r="V52" s="16"/>
       <c r="W52" s="16" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="X52" s="16"/>
       <c r="Y52" s="16"/>
@@ -9814,13 +9817,13 @@
         <v>100</v>
       </c>
       <c r="AG52" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AH52" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AI52" s="16" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="53" spans="1:35" x14ac:dyDescent="0.15">
@@ -9828,28 +9831,28 @@
         <v>21500005</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D53" s="1"/>
       <c r="E53" s="1">
-        <f t="shared" si="36"/>
+        <f>IF(S53&gt;=23,4,IF(AND(S53&gt;=18,S53&lt;23),3,IF(AND(S53&gt;=13,S53&lt;18),2,IF(AND(S53&gt;=8,S53&lt;13),1,0))))</f>
         <v>2</v>
       </c>
       <c r="F53" s="1">
         <v>5</v>
       </c>
       <c r="G53" s="1">
-        <f t="shared" si="2"/>
+        <f>E53*50+50</f>
         <v>150</v>
       </c>
       <c r="H53" s="17">
         <v>1</v>
       </c>
       <c r="I53" s="16" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="J53" s="16">
         <v>0</v>
@@ -9879,17 +9882,17 @@
         <v>1</v>
       </c>
       <c r="S53" s="16">
-        <f t="shared" si="23"/>
+        <f>J53+K53+ SUM(L53:R53)*5+AC53+AD53</f>
         <v>15</v>
       </c>
       <c r="T53" s="16"/>
       <c r="U53" s="16"/>
       <c r="V53" s="16"/>
       <c r="W53" s="16" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="X53" s="16" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="Y53" s="16"/>
       <c r="Z53" s="16"/>
@@ -9905,13 +9908,13 @@
       <c r="AE53" s="16"/>
       <c r="AF53" s="16"/>
       <c r="AG53" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AH53" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AI53" s="16" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="54" spans="1:35" x14ac:dyDescent="0.15">
@@ -9919,28 +9922,28 @@
         <v>21500006</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D54" s="1"/>
       <c r="E54" s="1">
-        <f t="shared" ref="E54:E55" si="37">IF(S54&gt;=23,4,IF(AND(S54&gt;=18,S54&lt;23),3,IF(AND(S54&gt;=13,S54&lt;18),2,IF(AND(S54&gt;=8,S54&lt;13),1,0))))</f>
+        <f>IF(S54&gt;=23,4,IF(AND(S54&gt;=18,S54&lt;23),3,IF(AND(S54&gt;=13,S54&lt;18),2,IF(AND(S54&gt;=8,S54&lt;13),1,0))))</f>
         <v>2</v>
       </c>
       <c r="F54" s="1">
         <v>5</v>
       </c>
       <c r="G54" s="1">
-        <f t="shared" si="2"/>
+        <f>E54*50+50</f>
         <v>150</v>
       </c>
       <c r="H54" s="17">
         <v>1</v>
       </c>
       <c r="I54" s="16" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="J54" s="16">
         <v>0</v>
@@ -9970,14 +9973,14 @@
         <v>0</v>
       </c>
       <c r="S54" s="16">
-        <f t="shared" si="23"/>
+        <f>J54+K54+ SUM(L54:R54)*5+AC54+AD54</f>
         <v>15</v>
       </c>
       <c r="T54" s="16"/>
       <c r="U54" s="16"/>
       <c r="V54" s="16"/>
       <c r="W54" s="16" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="X54" s="16"/>
       <c r="Y54" s="16"/>
@@ -9998,42 +10001,42 @@
         <v>100</v>
       </c>
       <c r="AG54" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AH54" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AI54" s="16" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="55" spans="1:35" x14ac:dyDescent="0.15">
-      <c r="A55">
+      <c r="A55" s="18">
         <v>21500007</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D55" s="1"/>
       <c r="E55" s="1">
-        <f t="shared" si="37"/>
+        <f>IF(S55&gt;=23,4,IF(AND(S55&gt;=18,S55&lt;23),3,IF(AND(S55&gt;=13,S55&lt;18),2,IF(AND(S55&gt;=8,S55&lt;13),1,0))))</f>
         <v>1</v>
       </c>
       <c r="F55" s="1">
         <v>5</v>
       </c>
       <c r="G55" s="1">
-        <f t="shared" ref="G55:G56" si="38">E55*50+50</f>
+        <f>E55*50+50</f>
         <v>100</v>
       </c>
       <c r="H55" s="17">
         <v>1</v>
       </c>
       <c r="I55" s="16" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="J55" s="16">
         <v>0</v>
@@ -10063,14 +10066,14 @@
         <v>0</v>
       </c>
       <c r="S55" s="16">
-        <f t="shared" si="23"/>
+        <f>J55+K55+ SUM(L55:R55)*5+AC55+AD55</f>
         <v>8</v>
       </c>
       <c r="T55" s="16"/>
       <c r="U55" s="16"/>
       <c r="V55" s="16"/>
       <c r="W55" s="16" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="X55" s="16"/>
       <c r="Y55" s="16"/>
@@ -10087,13 +10090,13 @@
       <c r="AE55" s="16"/>
       <c r="AF55" s="16"/>
       <c r="AG55" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AH55" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AI55" s="16" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="56" spans="1:35" x14ac:dyDescent="0.15">
@@ -10101,28 +10104,28 @@
         <v>21500008</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D56" s="1"/>
       <c r="E56" s="1">
-        <f t="shared" ref="E56:E57" si="39">IF(S56&gt;=23,4,IF(AND(S56&gt;=18,S56&lt;23),3,IF(AND(S56&gt;=13,S56&lt;18),2,IF(AND(S56&gt;=8,S56&lt;13),1,0))))</f>
+        <f>IF(S56&gt;=23,4,IF(AND(S56&gt;=18,S56&lt;23),3,IF(AND(S56&gt;=13,S56&lt;18),2,IF(AND(S56&gt;=8,S56&lt;13),1,0))))</f>
         <v>4</v>
       </c>
       <c r="F56" s="1">
         <v>5</v>
       </c>
       <c r="G56" s="1">
-        <f t="shared" si="38"/>
+        <f>E56*50+50</f>
         <v>250</v>
       </c>
       <c r="H56" s="17">
         <v>1</v>
       </c>
       <c r="I56" s="16" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="J56" s="16">
         <v>0</v>
@@ -10152,14 +10155,14 @@
         <v>0</v>
       </c>
       <c r="S56" s="16">
-        <f t="shared" si="23"/>
+        <f>J56+K56+ SUM(L56:R56)*5+AC56+AD56</f>
         <v>25</v>
       </c>
       <c r="T56" s="16"/>
       <c r="U56" s="16"/>
       <c r="V56" s="16"/>
       <c r="W56" s="16" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="X56" s="16"/>
       <c r="Y56" s="16"/>
@@ -10180,42 +10183,42 @@
         <v>40</v>
       </c>
       <c r="AG56" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AH56" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AI56" s="16" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="57" spans="1:35" x14ac:dyDescent="0.15">
-      <c r="A57">
+      <c r="A57" s="18">
         <v>21500009</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D57" s="1"/>
       <c r="E57" s="1">
-        <f t="shared" si="39"/>
+        <f>IF(S57&gt;=23,4,IF(AND(S57&gt;=18,S57&lt;23),3,IF(AND(S57&gt;=13,S57&lt;18),2,IF(AND(S57&gt;=8,S57&lt;13),1,0))))</f>
         <v>1</v>
       </c>
       <c r="F57" s="1">
         <v>5</v>
       </c>
       <c r="G57" s="1">
-        <f t="shared" ref="G57:G58" si="40">E57*50+50</f>
+        <f>E57*50+50</f>
         <v>100</v>
       </c>
       <c r="H57" s="17">
         <v>1</v>
       </c>
       <c r="I57" s="16" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="J57" s="16">
         <v>0</v>
@@ -10245,14 +10248,14 @@
         <v>0</v>
       </c>
       <c r="S57" s="16">
-        <f t="shared" si="23"/>
+        <f>J57+K57+ SUM(L57:R57)*5+AC57+AD57</f>
         <v>10</v>
       </c>
       <c r="T57" s="16"/>
       <c r="U57" s="16"/>
       <c r="V57" s="16"/>
       <c r="W57" s="16" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="X57" s="16"/>
       <c r="Y57" s="16">
@@ -10271,13 +10274,13 @@
       <c r="AE57" s="16"/>
       <c r="AF57" s="16"/>
       <c r="AG57" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AH57" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AI57" s="16" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="58" spans="1:35" x14ac:dyDescent="0.15">
@@ -10285,28 +10288,28 @@
         <v>21500010</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="D58" s="1"/>
       <c r="E58" s="1">
-        <f t="shared" ref="E58:E59" si="41">IF(S58&gt;=23,4,IF(AND(S58&gt;=18,S58&lt;23),3,IF(AND(S58&gt;=13,S58&lt;18),2,IF(AND(S58&gt;=8,S58&lt;13),1,0))))</f>
+        <f>IF(S58&gt;=23,4,IF(AND(S58&gt;=18,S58&lt;23),3,IF(AND(S58&gt;=13,S58&lt;18),2,IF(AND(S58&gt;=8,S58&lt;13),1,0))))</f>
         <v>2</v>
       </c>
       <c r="F58" s="1">
         <v>5</v>
       </c>
       <c r="G58" s="1">
-        <f t="shared" si="40"/>
+        <f>E58*50+50</f>
         <v>150</v>
       </c>
       <c r="H58" s="17">
         <v>1</v>
       </c>
       <c r="I58" s="16" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="J58" s="16">
         <v>0</v>
@@ -10336,17 +10339,17 @@
         <v>0</v>
       </c>
       <c r="S58" s="16">
-        <f t="shared" si="23"/>
+        <f>J58+K58+ SUM(L58:R58)*5+AC58+AD58</f>
         <v>15</v>
       </c>
       <c r="T58" s="16"/>
       <c r="U58" s="16"/>
       <c r="V58" s="16"/>
       <c r="W58" s="16" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="X58" s="16" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="Y58" s="16">
         <v>31100002</v>
@@ -10364,13 +10367,13 @@
       <c r="AE58" s="16"/>
       <c r="AF58" s="16"/>
       <c r="AG58" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AH58" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AI58" s="16" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="59" spans="1:35" x14ac:dyDescent="0.15">
@@ -10378,28 +10381,28 @@
         <v>21500011</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D59" s="1"/>
       <c r="E59" s="1">
-        <f t="shared" si="41"/>
+        <f>IF(S59&gt;=23,4,IF(AND(S59&gt;=18,S59&lt;23),3,IF(AND(S59&gt;=13,S59&lt;18),2,IF(AND(S59&gt;=8,S59&lt;13),1,0))))</f>
         <v>4</v>
       </c>
       <c r="F59" s="1">
         <v>5</v>
       </c>
       <c r="G59" s="1">
-        <f t="shared" ref="G59" si="42">E59*50+50</f>
+        <f>E59*50+50</f>
         <v>250</v>
       </c>
       <c r="H59" s="17">
         <v>1</v>
       </c>
       <c r="I59" s="16" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="J59" s="16">
         <v>0</v>
@@ -10429,14 +10432,14 @@
         <v>0</v>
       </c>
       <c r="S59" s="16">
-        <f t="shared" si="23"/>
+        <f>J59+K59+ SUM(L59:R59)*5+AC59+AD59</f>
         <v>25</v>
       </c>
       <c r="T59" s="16"/>
       <c r="U59" s="16"/>
       <c r="V59" s="16"/>
       <c r="W59" s="16" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="X59" s="16"/>
       <c r="Y59" s="16">
@@ -10455,36 +10458,36 @@
       <c r="AE59" s="16"/>
       <c r="AF59" s="16"/>
       <c r="AG59" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AH59" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AI59" s="16" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="E4:E59">
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="greaterThanOrEqual">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="8" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="9" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="10" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="11" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4:AI59">
-    <cfRule type="containsBlanks" dxfId="0" priority="1">
+    <cfRule type="containsBlanks" dxfId="1" priority="1">
       <formula>LEN(TRIM(I4))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
fix the equip add monster attr func
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Equip.xlsx
+++ b/ConfigData/Xlsx/Equip.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TOMClassic\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
     <author>Administrator</author>
   </authors>
   <commentList>
-    <comment ref="V1" authorId="0" shapeId="0">
+    <comment ref="W1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="314">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -1150,6 +1150,18 @@
   </si>
   <si>
     <t>AttrId</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>辅助</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Attr</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1969,7 +1981,54 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="35">
+  <dxfs count="36">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2226,34 +2285,6 @@
         <name val="宋体"/>
         <scheme val="minor"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -2565,72 +2596,6 @@
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
     <mruColors>
       <color rgb="FF9751CB"/>
     </mruColors>
@@ -4477,52 +4442,53 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:AF59" totalsRowShown="0">
-  <autoFilter ref="A3:AF59"/>
-  <sortState ref="A4:AF59">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:AG59" totalsRowShown="0">
+  <autoFilter ref="A3:AG59"/>
+  <sortState ref="A4:AG59">
     <sortCondition ref="A3:A59"/>
   </sortState>
-  <tableColumns count="32">
+  <tableColumns count="33">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="Name"/>
-    <tableColumn id="34" name="Ename" dataDxfId="34"/>
-    <tableColumn id="3" name="Quality" dataDxfId="33">
-      <calculatedColumnFormula>IF(R4&gt;=23,4,IF(AND(R4&gt;=18,R4&lt;23),3,IF(AND(R4&gt;=13,R4&lt;18),2,IF(AND(R4&gt;=8,R4&lt;13),1,0))))</calculatedColumnFormula>
+    <tableColumn id="34" name="Ename" dataDxfId="35"/>
+    <tableColumn id="3" name="Quality" dataDxfId="34">
+      <calculatedColumnFormula>IF(S4&gt;=23,4,IF(AND(S4&gt;=18,S4&lt;23),3,IF(AND(S4&gt;=13,S4&lt;18),2,IF(AND(S4&gt;=8,S4&lt;13),1,0))))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" name="Position"/>
-    <tableColumn id="19" name="Value" dataDxfId="32">
+    <tableColumn id="19" name="Value" dataDxfId="33">
       <calculatedColumnFormula>D4*50+50</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="ComposeRes" dataDxfId="31"/>
-    <tableColumn id="15" name="ComposeItemId" dataDxfId="30"/>
-    <tableColumn id="11" name="AtkP" dataDxfId="29"/>
-    <tableColumn id="8" name="VitP" dataDxfId="28"/>
-    <tableColumn id="6" name="Def" dataDxfId="27"/>
-    <tableColumn id="22" name="Mag" dataDxfId="26"/>
-    <tableColumn id="27" name="Spd" dataDxfId="25"/>
-    <tableColumn id="26" name="Hit" dataDxfId="24"/>
-    <tableColumn id="25" name="Dhit" dataDxfId="23"/>
-    <tableColumn id="24" name="Crt" dataDxfId="22"/>
-    <tableColumn id="23" name="Luk" dataDxfId="21"/>
-    <tableColumn id="28" name="Sum" dataDxfId="20">
-      <calculatedColumnFormula>I4+J4+ SUM(K4:Q4)*5+Z4+AA4</calculatedColumnFormula>
+    <tableColumn id="7" name="ComposeRes" dataDxfId="32"/>
+    <tableColumn id="15" name="ComposeItemId" dataDxfId="31"/>
+    <tableColumn id="11" name="AtkP" dataDxfId="30"/>
+    <tableColumn id="8" name="VitP" dataDxfId="29"/>
+    <tableColumn id="30" name="Attr" dataDxfId="1"/>
+    <tableColumn id="6" name="Def" dataDxfId="28"/>
+    <tableColumn id="22" name="Mag" dataDxfId="27"/>
+    <tableColumn id="27" name="Spd" dataDxfId="26"/>
+    <tableColumn id="26" name="Hit" dataDxfId="25"/>
+    <tableColumn id="25" name="Dhit" dataDxfId="24"/>
+    <tableColumn id="24" name="Crt" dataDxfId="23"/>
+    <tableColumn id="23" name="Luk" dataDxfId="22"/>
+    <tableColumn id="28" name="Sum" dataDxfId="0">
+      <calculatedColumnFormula>I4+J4+K4+ SUM(L4:R4)*5+AA4+AB4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="Range" dataDxfId="19"/>
-    <tableColumn id="33" name="Arrow" dataDxfId="18"/>
-    <tableColumn id="4" name="SlotId" dataDxfId="17"/>
-    <tableColumn id="9" name="EnergyRate" dataDxfId="16"/>
-    <tableColumn id="37" name="DungeonAttrs" dataDxfId="15"/>
-    <tableColumn id="20" name="HeroSkillId" dataDxfId="14"/>
-    <tableColumn id="29" name="AttrId" dataDxfId="13"/>
-    <tableColumn id="21" name="~SkillMark2" dataDxfId="12"/>
-    <tableColumn id="18" name="~SkillMark22" dataDxfId="11">
-      <calculatedColumnFormula>IF(ISBLANK(AB4),0, LOOKUP(AB4,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AC4/100)</calculatedColumnFormula>
+    <tableColumn id="12" name="Range" dataDxfId="21"/>
+    <tableColumn id="33" name="Arrow" dataDxfId="20"/>
+    <tableColumn id="4" name="SlotId" dataDxfId="19"/>
+    <tableColumn id="9" name="EnergyRate" dataDxfId="18"/>
+    <tableColumn id="37" name="DungeonAttrs" dataDxfId="17"/>
+    <tableColumn id="20" name="HeroSkillId" dataDxfId="16"/>
+    <tableColumn id="29" name="AttrId" dataDxfId="15"/>
+    <tableColumn id="21" name="~SkillMark2" dataDxfId="14"/>
+    <tableColumn id="18" name="~SkillMark22" dataDxfId="13">
+      <calculatedColumnFormula>IF(ISBLANK(AC4),0, LOOKUP(AC4,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AD4/100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="CommonSkillId" dataDxfId="10"/>
-    <tableColumn id="14" name="CommonSkillRate" dataDxfId="9"/>
-    <tableColumn id="17" name="RandomDrop" dataDxfId="8"/>
-    <tableColumn id="16" name="CanMerge" dataDxfId="7"/>
-    <tableColumn id="10" name="Url" dataDxfId="6"/>
+    <tableColumn id="13" name="CommonSkillId" dataDxfId="12"/>
+    <tableColumn id="14" name="CommonSkillRate" dataDxfId="11"/>
+    <tableColumn id="17" name="RandomDrop" dataDxfId="10"/>
+    <tableColumn id="16" name="CanMerge" dataDxfId="9"/>
+    <tableColumn id="10" name="Url" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4536,7 +4502,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="C7EDCC"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -4849,10 +4815,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF59"/>
+  <dimension ref="A1:AG59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="W3" sqref="W3"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -4861,21 +4827,21 @@
     <col min="4" max="5" width="5.5" customWidth="1"/>
     <col min="6" max="7" width="6.5" customWidth="1"/>
     <col min="8" max="8" width="19" customWidth="1"/>
-    <col min="9" max="10" width="5.125" customWidth="1"/>
-    <col min="11" max="18" width="4.5" customWidth="1"/>
-    <col min="19" max="20" width="5.125" customWidth="1"/>
-    <col min="21" max="21" width="10.875" customWidth="1"/>
-    <col min="22" max="24" width="8.625" customWidth="1"/>
-    <col min="25" max="25" width="4.875" customWidth="1"/>
-    <col min="26" max="26" width="8.625" customWidth="1"/>
-    <col min="27" max="27" width="5.875" customWidth="1"/>
-    <col min="28" max="28" width="8.625" customWidth="1"/>
-    <col min="29" max="29" width="5.25" customWidth="1"/>
-    <col min="30" max="31" width="6" customWidth="1"/>
-    <col min="34" max="34" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="5.125" customWidth="1"/>
+    <col min="12" max="19" width="4.5" customWidth="1"/>
+    <col min="20" max="21" width="5.125" customWidth="1"/>
+    <col min="22" max="22" width="10.875" customWidth="1"/>
+    <col min="23" max="25" width="8.625" customWidth="1"/>
+    <col min="26" max="26" width="4.875" customWidth="1"/>
+    <col min="27" max="27" width="8.625" customWidth="1"/>
+    <col min="28" max="28" width="5.875" customWidth="1"/>
+    <col min="29" max="29" width="8.625" customWidth="1"/>
+    <col min="30" max="30" width="5.25" customWidth="1"/>
+    <col min="31" max="32" width="6" customWidth="1"/>
+    <col min="35" max="35" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" ht="60.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:33" ht="60.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
         <v>2</v>
       </c>
@@ -4906,74 +4872,77 @@
       <c r="J1" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="K1" s="12" t="s">
+        <v>311</v>
+      </c>
+      <c r="L1" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="L1" s="13" t="s">
+      <c r="M1" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="M1" s="13" t="s">
+      <c r="N1" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="N1" s="13" t="s">
+      <c r="O1" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="O1" s="13" t="s">
+      <c r="P1" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="P1" s="13" t="s">
+      <c r="Q1" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="Q1" s="13" t="s">
+      <c r="R1" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="R1" s="14" t="s">
+      <c r="S1" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="S1" s="15" t="s">
+      <c r="T1" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="T1" s="15" t="s">
+      <c r="U1" s="15" t="s">
         <v>165</v>
       </c>
-      <c r="U1" s="15" t="s">
+      <c r="V1" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="V1" s="15" t="s">
+      <c r="W1" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="W1" s="15" t="s">
+      <c r="X1" s="15" t="s">
         <v>263</v>
       </c>
-      <c r="X1" s="15" t="s">
+      <c r="Y1" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="Y1" s="15" t="s">
+      <c r="Z1" s="15" t="s">
         <v>309</v>
       </c>
-      <c r="Z1" s="15" t="s">
+      <c r="AA1" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="AA1" s="14" t="s">
+      <c r="AB1" s="14" t="s">
         <v>30</v>
-      </c>
-      <c r="AB1" s="14" t="s">
-        <v>39</v>
       </c>
       <c r="AC1" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="AD1" s="11" t="s">
+      <c r="AD1" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="AE1" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="AE1" s="11" t="s">
+      <c r="AF1" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="AF1" s="11" t="s">
+      <c r="AG1" s="11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -5004,15 +4973,15 @@
       <c r="J2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="K2" s="9" t="s">
-        <v>0</v>
+      <c r="K2" s="3" t="s">
+        <v>312</v>
       </c>
       <c r="L2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="M2" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="M2" s="9" t="s">
-        <v>0</v>
-      </c>
       <c r="N2" s="9" t="s">
         <v>0</v>
       </c>
@@ -5025,53 +4994,56 @@
       <c r="Q2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="R2" s="5" t="s">
+      <c r="R2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="S2" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="S2" s="7" t="s">
-        <v>0</v>
-      </c>
       <c r="T2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="U2" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="U2" s="7" t="s">
+      <c r="V2" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="V2" s="7" t="s">
+      <c r="W2" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="W2" s="7" t="s">
+      <c r="X2" s="7" t="s">
         <v>264</v>
       </c>
-      <c r="X2" s="7" t="s">
-        <v>0</v>
-      </c>
       <c r="Y2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z2" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="Z2" s="7" t="s">
+      <c r="AA2" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="AA2" s="5" t="s">
+      <c r="AB2" s="5" t="s">
         <v>31</v>
-      </c>
-      <c r="AB2" s="5" t="s">
-        <v>40</v>
       </c>
       <c r="AC2" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="AD2" s="2" t="s">
-        <v>26</v>
+      <c r="AD2" s="5" t="s">
+        <v>40</v>
       </c>
       <c r="AE2" s="2" t="s">
         <v>26</v>
       </c>
       <c r="AF2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AG2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -5102,74 +5074,77 @@
       <c r="J3" s="4" t="s">
         <v>308</v>
       </c>
-      <c r="K3" s="10" t="s">
+      <c r="K3" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="L3" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="L3" s="10" t="s">
+      <c r="M3" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="M3" s="10" t="s">
+      <c r="N3" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="N3" s="10" t="s">
+      <c r="O3" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="O3" s="10" t="s">
+      <c r="P3" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="P3" s="10" t="s">
+      <c r="Q3" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="Q3" s="10" t="s">
+      <c r="R3" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="R3" s="6" t="s">
+      <c r="S3" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="S3" s="8" t="s">
+      <c r="T3" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="T3" s="8" t="s">
+      <c r="U3" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="U3" s="8" t="s">
+      <c r="V3" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="V3" s="8" t="s">
+      <c r="W3" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="W3" s="8" t="s">
+      <c r="X3" s="8" t="s">
         <v>265</v>
       </c>
-      <c r="X3" s="8" t="s">
+      <c r="Y3" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="Y3" s="8" t="s">
+      <c r="Z3" s="8" t="s">
         <v>310</v>
       </c>
-      <c r="Z3" s="8" t="s">
+      <c r="AA3" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="AA3" s="6" t="s">
+      <c r="AB3" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="AB3" s="6" t="s">
+      <c r="AC3" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="AC3" s="6" t="s">
+      <c r="AD3" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="AD3" t="s">
+      <c r="AE3" t="s">
         <v>29</v>
       </c>
-      <c r="AE3" t="s">
+      <c r="AF3" t="s">
         <v>27</v>
       </c>
-      <c r="AF3" t="s">
+      <c r="AG3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A4" s="1">
         <v>21100001</v>
       </c>
@@ -5180,7 +5155,7 @@
         <v>272</v>
       </c>
       <c r="D4" s="1">
-        <f t="shared" ref="D4:D35" si="0">IF(R4&gt;=23,4,IF(AND(R4&gt;=18,R4&lt;23),3,IF(AND(R4&gt;=13,R4&lt;18),2,IF(AND(R4&gt;=8,R4&lt;13),1,0))))</f>
+        <f t="shared" ref="D4:D35" si="0">IF(S4&gt;=23,4,IF(AND(S4&gt;=18,S4&lt;23),3,IF(AND(S4&gt;=13,S4&lt;18),2,IF(AND(S4&gt;=8,S4&lt;13),1,0))))</f>
         <v>0</v>
       </c>
       <c r="E4" s="1">
@@ -5224,40 +5199,43 @@
         <v>0</v>
       </c>
       <c r="R4" s="16">
-        <f>I4+J4+ SUM(K4:Q4)*5+Z4+AA4</f>
+        <v>0</v>
+      </c>
+      <c r="S4" s="16">
+        <f t="shared" ref="S4:S59" si="2">I4+J4+K4+ SUM(L4:R4)*5+AA4+AB4</f>
         <v>-4</v>
       </c>
-      <c r="S4" s="16"/>
       <c r="T4" s="16"/>
-      <c r="U4" s="16" t="s">
+      <c r="U4" s="16"/>
+      <c r="V4" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="V4" s="16" t="s">
+      <c r="W4" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="W4" s="16"/>
       <c r="X4" s="16"/>
       <c r="Y4" s="16"/>
-      <c r="Z4" s="16">
+      <c r="Z4" s="16"/>
+      <c r="AA4" s="16">
         <v>-10</v>
       </c>
-      <c r="AA4" s="16">
-        <f>IF(ISBLANK(AB4),0, LOOKUP(AB4,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AC4/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AB4" s="16"/>
+      <c r="AB4" s="16">
+        <f>IF(ISBLANK(AC4),0, LOOKUP(AC4,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AD4/100)</f>
+        <v>0</v>
+      </c>
       <c r="AC4" s="16"/>
-      <c r="AD4" s="16" t="s">
-        <v>24</v>
-      </c>
+      <c r="AD4" s="16"/>
       <c r="AE4" s="16" t="s">
         <v>24</v>
       </c>
       <c r="AF4" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG4" s="16" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A5" s="1">
         <v>21100002</v>
       </c>
@@ -5312,40 +5290,43 @@
         <v>0</v>
       </c>
       <c r="R5" s="16">
-        <f>I5+J5+ SUM(K5:Q5)*5+Z5+AA5</f>
+        <v>0</v>
+      </c>
+      <c r="S5" s="16">
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="S5" s="16"/>
       <c r="T5" s="16"/>
-      <c r="U5" s="16" t="s">
+      <c r="U5" s="16"/>
+      <c r="V5" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="V5" s="16" t="s">
+      <c r="W5" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="W5" s="16"/>
       <c r="X5" s="16"/>
       <c r="Y5" s="16"/>
-      <c r="Z5" s="16">
-        <v>0</v>
-      </c>
+      <c r="Z5" s="16"/>
       <c r="AA5" s="16">
-        <f>IF(ISBLANK(AB5),0, LOOKUP(AB5,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AC5/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AB5" s="16"/>
+        <v>0</v>
+      </c>
+      <c r="AB5" s="16">
+        <f>IF(ISBLANK(AC5),0, LOOKUP(AC5,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AD5/100)</f>
+        <v>0</v>
+      </c>
       <c r="AC5" s="16"/>
-      <c r="AD5" s="16" t="s">
-        <v>24</v>
-      </c>
+      <c r="AD5" s="16"/>
       <c r="AE5" s="16" t="s">
         <v>24</v>
       </c>
       <c r="AF5" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG5" s="16" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A6" s="1">
         <v>21100003</v>
       </c>
@@ -5400,40 +5381,43 @@
         <v>0</v>
       </c>
       <c r="R6" s="16">
-        <f>I6+J6+ SUM(K6:Q6)*5+Z6+AA6</f>
+        <v>0</v>
+      </c>
+      <c r="S6" s="16">
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
-      <c r="S6" s="16"/>
       <c r="T6" s="16"/>
-      <c r="U6" s="16" t="s">
+      <c r="U6" s="16"/>
+      <c r="V6" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="V6" s="16" t="s">
+      <c r="W6" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="W6" s="16"/>
       <c r="X6" s="16"/>
       <c r="Y6" s="16"/>
-      <c r="Z6" s="16">
-        <v>0</v>
-      </c>
+      <c r="Z6" s="16"/>
       <c r="AA6" s="16">
-        <f>IF(ISBLANK(AB6),0, LOOKUP(AB6,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AC6/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AB6" s="16"/>
+        <v>0</v>
+      </c>
+      <c r="AB6" s="16">
+        <f>IF(ISBLANK(AC6),0, LOOKUP(AC6,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AD6/100)</f>
+        <v>0</v>
+      </c>
       <c r="AC6" s="16"/>
-      <c r="AD6" s="16" t="s">
-        <v>24</v>
-      </c>
+      <c r="AD6" s="16"/>
       <c r="AE6" s="16" t="s">
         <v>24</v>
       </c>
       <c r="AF6" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG6" s="16" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A7" s="1">
         <v>21100004</v>
       </c>
@@ -5488,40 +5472,43 @@
         <v>0</v>
       </c>
       <c r="R7" s="16">
-        <f>I7+J7+ SUM(K7:Q7)*5+Z7+AA7</f>
+        <v>0</v>
+      </c>
+      <c r="S7" s="16">
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="S7" s="16"/>
       <c r="T7" s="16"/>
-      <c r="U7" s="16" t="s">
+      <c r="U7" s="16"/>
+      <c r="V7" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="V7" s="16" t="s">
+      <c r="W7" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="W7" s="16"/>
       <c r="X7" s="16"/>
       <c r="Y7" s="16"/>
-      <c r="Z7" s="16">
-        <v>0</v>
-      </c>
+      <c r="Z7" s="16"/>
       <c r="AA7" s="16">
-        <f>IF(ISBLANK(AB7),0, LOOKUP(AB7,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AC7/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AB7" s="16"/>
+        <v>0</v>
+      </c>
+      <c r="AB7" s="16">
+        <f>IF(ISBLANK(AC7),0, LOOKUP(AC7,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AD7/100)</f>
+        <v>0</v>
+      </c>
       <c r="AC7" s="16"/>
-      <c r="AD7" s="16" t="s">
-        <v>24</v>
-      </c>
+      <c r="AD7" s="16"/>
       <c r="AE7" s="16" t="s">
         <v>24</v>
       </c>
       <c r="AF7" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG7" s="16" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A8" s="1">
         <v>21100005</v>
       </c>
@@ -5567,49 +5554,52 @@
         <v>0</v>
       </c>
       <c r="O8" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P8" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q8" s="16">
         <v>0</v>
       </c>
       <c r="R8" s="16">
-        <f>I8+J8+ SUM(K8:Q8)*5+Z8+AA8</f>
+        <v>0</v>
+      </c>
+      <c r="S8" s="16">
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
-      <c r="S8" s="16"/>
       <c r="T8" s="16"/>
-      <c r="U8" s="16" t="s">
+      <c r="U8" s="16"/>
+      <c r="V8" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="V8" s="16" t="s">
+      <c r="W8" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="W8" s="16"/>
       <c r="X8" s="16"/>
       <c r="Y8" s="16"/>
-      <c r="Z8" s="16">
-        <v>0</v>
-      </c>
+      <c r="Z8" s="16"/>
       <c r="AA8" s="16">
-        <f>IF(ISBLANK(AB8),0, LOOKUP(AB8,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AC8/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AB8" s="16"/>
+        <v>0</v>
+      </c>
+      <c r="AB8" s="16">
+        <f>IF(ISBLANK(AC8),0, LOOKUP(AC8,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AD8/100)</f>
+        <v>0</v>
+      </c>
       <c r="AC8" s="16"/>
-      <c r="AD8" s="16" t="s">
-        <v>24</v>
-      </c>
+      <c r="AD8" s="16"/>
       <c r="AE8" s="16" t="s">
         <v>24</v>
       </c>
       <c r="AF8" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG8" s="16" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A9" s="1">
         <v>21100006</v>
       </c>
@@ -5643,10 +5633,10 @@
         <v>10</v>
       </c>
       <c r="K9" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L9" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M9" s="16">
         <v>0</v>
@@ -5664,40 +5654,43 @@
         <v>0</v>
       </c>
       <c r="R9" s="16">
-        <f>I9+J9+ SUM(K9:Q9)*5+Z9+AA9</f>
+        <v>0</v>
+      </c>
+      <c r="S9" s="16">
+        <f t="shared" si="2"/>
         <v>25</v>
       </c>
-      <c r="S9" s="16"/>
       <c r="T9" s="16"/>
-      <c r="U9" s="16" t="s">
+      <c r="U9" s="16"/>
+      <c r="V9" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="V9" s="16" t="s">
+      <c r="W9" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="W9" s="16"/>
       <c r="X9" s="16"/>
       <c r="Y9" s="16"/>
-      <c r="Z9" s="16">
+      <c r="Z9" s="16"/>
+      <c r="AA9" s="16">
         <v>10</v>
       </c>
-      <c r="AA9" s="16">
-        <f>IF(ISBLANK(AB9),0, LOOKUP(AB9,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AC9/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AB9" s="16"/>
+      <c r="AB9" s="16">
+        <f>IF(ISBLANK(AC9),0, LOOKUP(AC9,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AD9/100)</f>
+        <v>0</v>
+      </c>
       <c r="AC9" s="16"/>
-      <c r="AD9" s="16" t="s">
-        <v>24</v>
-      </c>
+      <c r="AD9" s="16"/>
       <c r="AE9" s="16" t="s">
         <v>24</v>
       </c>
       <c r="AF9" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG9" s="16" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A10" s="1">
         <v>21100007</v>
       </c>
@@ -5734,10 +5727,10 @@
         <v>0</v>
       </c>
       <c r="L10" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M10" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N10" s="16">
         <v>0</v>
@@ -5752,40 +5745,43 @@
         <v>0</v>
       </c>
       <c r="R10" s="16">
-        <f>I10+J10+ SUM(K10:Q10)*5+Z10+AA10</f>
+        <v>0</v>
+      </c>
+      <c r="S10" s="16">
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
-      <c r="S10" s="16"/>
       <c r="T10" s="16"/>
-      <c r="U10" s="16" t="s">
+      <c r="U10" s="16"/>
+      <c r="V10" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="V10" s="16" t="s">
+      <c r="W10" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="W10" s="16"/>
       <c r="X10" s="16"/>
       <c r="Y10" s="16"/>
-      <c r="Z10" s="16">
-        <v>0</v>
-      </c>
+      <c r="Z10" s="16"/>
       <c r="AA10" s="16">
-        <f>IF(ISBLANK(AB10),0, LOOKUP(AB10,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AC10/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AB10" s="16"/>
+        <v>0</v>
+      </c>
+      <c r="AB10" s="16">
+        <f>IF(ISBLANK(AC10),0, LOOKUP(AC10,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AD10/100)</f>
+        <v>0</v>
+      </c>
       <c r="AC10" s="16"/>
-      <c r="AD10" s="16" t="s">
-        <v>24</v>
-      </c>
+      <c r="AD10" s="16"/>
       <c r="AE10" s="16" t="s">
         <v>24</v>
       </c>
       <c r="AF10" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG10" s="16" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A11" s="1">
         <v>21100008</v>
       </c>
@@ -5819,11 +5815,11 @@
         <v>15</v>
       </c>
       <c r="K11" s="16">
+        <v>0</v>
+      </c>
+      <c r="L11" s="16">
         <v>2</v>
       </c>
-      <c r="L11" s="16">
-        <v>0</v>
-      </c>
       <c r="M11" s="16">
         <v>0</v>
       </c>
@@ -5840,40 +5836,43 @@
         <v>0</v>
       </c>
       <c r="R11" s="16">
-        <f>I11+J11+ SUM(K11:Q11)*5+Z11+AA11</f>
+        <v>0</v>
+      </c>
+      <c r="S11" s="16">
+        <f t="shared" si="2"/>
         <v>25</v>
       </c>
-      <c r="S11" s="16"/>
       <c r="T11" s="16"/>
-      <c r="U11" s="16" t="s">
+      <c r="U11" s="16"/>
+      <c r="V11" s="16" t="s">
         <v>154</v>
       </c>
-      <c r="V11" s="16" t="s">
+      <c r="W11" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="W11" s="16"/>
       <c r="X11" s="16"/>
       <c r="Y11" s="16"/>
-      <c r="Z11" s="16">
-        <v>0</v>
-      </c>
+      <c r="Z11" s="16"/>
       <c r="AA11" s="16">
-        <f>IF(ISBLANK(AB11),0, LOOKUP(AB11,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AC11/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AB11" s="16"/>
+        <v>0</v>
+      </c>
+      <c r="AB11" s="16">
+        <f>IF(ISBLANK(AC11),0, LOOKUP(AC11,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AD11/100)</f>
+        <v>0</v>
+      </c>
       <c r="AC11" s="16"/>
-      <c r="AD11" s="16" t="s">
-        <v>24</v>
-      </c>
+      <c r="AD11" s="16"/>
       <c r="AE11" s="16" t="s">
         <v>24</v>
       </c>
       <c r="AF11" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG11" s="16" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A12" s="1">
         <v>21100009</v>
       </c>
@@ -5907,10 +5906,10 @@
         <v>15</v>
       </c>
       <c r="K12" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L12" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M12" s="16">
         <v>0</v>
@@ -5928,40 +5927,43 @@
         <v>0</v>
       </c>
       <c r="R12" s="16">
-        <f>I12+J12+ SUM(K12:Q12)*5+Z12+AA12</f>
+        <v>0</v>
+      </c>
+      <c r="S12" s="16">
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
-      <c r="S12" s="16"/>
       <c r="T12" s="16"/>
-      <c r="U12" s="16" t="s">
+      <c r="U12" s="16"/>
+      <c r="V12" s="16" t="s">
         <v>158</v>
       </c>
-      <c r="V12" s="16" t="s">
+      <c r="W12" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="W12" s="16"/>
       <c r="X12" s="16"/>
       <c r="Y12" s="16"/>
-      <c r="Z12" s="16">
-        <v>0</v>
-      </c>
+      <c r="Z12" s="16"/>
       <c r="AA12" s="16">
-        <f>IF(ISBLANK(AB12),0, LOOKUP(AB12,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AC12/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AB12" s="16"/>
+        <v>0</v>
+      </c>
+      <c r="AB12" s="16">
+        <f>IF(ISBLANK(AC12),0, LOOKUP(AC12,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AD12/100)</f>
+        <v>0</v>
+      </c>
       <c r="AC12" s="16"/>
-      <c r="AD12" s="16" t="s">
-        <v>24</v>
-      </c>
+      <c r="AD12" s="16"/>
       <c r="AE12" s="16" t="s">
         <v>24</v>
       </c>
       <c r="AF12" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG12" s="16" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A13" s="1">
         <v>21100010</v>
       </c>
@@ -6010,46 +6012,49 @@
         <v>0</v>
       </c>
       <c r="P13" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q13" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R13" s="16">
-        <f>I13+J13+ SUM(K13:Q13)*5+Z13+AA13</f>
+        <v>0</v>
+      </c>
+      <c r="S13" s="16">
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="S13" s="16"/>
       <c r="T13" s="16"/>
-      <c r="U13" s="16" t="s">
+      <c r="U13" s="16"/>
+      <c r="V13" s="16" t="s">
         <v>161</v>
       </c>
-      <c r="V13" s="16" t="s">
+      <c r="W13" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="W13" s="16"/>
       <c r="X13" s="16"/>
       <c r="Y13" s="16"/>
-      <c r="Z13" s="16">
+      <c r="Z13" s="16"/>
+      <c r="AA13" s="16">
         <v>-10</v>
       </c>
-      <c r="AA13" s="16">
-        <f>IF(ISBLANK(AB13),0, LOOKUP(AB13,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AC13/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AB13" s="16"/>
+      <c r="AB13" s="16">
+        <f>IF(ISBLANK(AC13),0, LOOKUP(AC13,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AD13/100)</f>
+        <v>0</v>
+      </c>
       <c r="AC13" s="16"/>
-      <c r="AD13" s="16" t="s">
-        <v>24</v>
-      </c>
+      <c r="AD13" s="16"/>
       <c r="AE13" s="16" t="s">
         <v>24</v>
       </c>
       <c r="AF13" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG13" s="16" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A14" s="1">
         <v>21100011</v>
       </c>
@@ -6083,11 +6088,11 @@
         <v>5</v>
       </c>
       <c r="K14" s="16">
+        <v>0</v>
+      </c>
+      <c r="L14" s="16">
         <v>3</v>
       </c>
-      <c r="L14" s="16">
-        <v>0</v>
-      </c>
       <c r="M14" s="16">
         <v>0</v>
       </c>
@@ -6104,40 +6109,43 @@
         <v>0</v>
       </c>
       <c r="R14" s="16">
-        <f>I14+J14+ SUM(K14:Q14)*5+Z14+AA14</f>
+        <v>0</v>
+      </c>
+      <c r="S14" s="16">
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
-      <c r="S14" s="16"/>
       <c r="T14" s="16"/>
-      <c r="U14" s="16" t="s">
+      <c r="U14" s="16"/>
+      <c r="V14" s="16" t="s">
         <v>164</v>
       </c>
-      <c r="V14" s="16" t="s">
+      <c r="W14" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="W14" s="16"/>
       <c r="X14" s="16"/>
       <c r="Y14" s="16"/>
-      <c r="Z14" s="16">
-        <v>0</v>
-      </c>
+      <c r="Z14" s="16"/>
       <c r="AA14" s="16">
-        <f>IF(ISBLANK(AB14),0, LOOKUP(AB14,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AC14/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AB14" s="16"/>
+        <v>0</v>
+      </c>
+      <c r="AB14" s="16">
+        <f>IF(ISBLANK(AC14),0, LOOKUP(AC14,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AD14/100)</f>
+        <v>0</v>
+      </c>
       <c r="AC14" s="16"/>
-      <c r="AD14" s="16" t="s">
-        <v>24</v>
-      </c>
+      <c r="AD14" s="16"/>
       <c r="AE14" s="16" t="s">
         <v>24</v>
       </c>
       <c r="AF14" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG14" s="16" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A15" s="1">
         <v>21100012</v>
       </c>
@@ -6174,11 +6182,11 @@
         <v>0</v>
       </c>
       <c r="L15" s="16">
+        <v>0</v>
+      </c>
+      <c r="M15" s="16">
         <v>4</v>
       </c>
-      <c r="M15" s="16">
-        <v>0</v>
-      </c>
       <c r="N15" s="16">
         <v>0</v>
       </c>
@@ -6192,40 +6200,43 @@
         <v>0</v>
       </c>
       <c r="R15" s="16">
-        <f>I15+J15+ SUM(K15:Q15)*5+Z15+AA15</f>
+        <v>0</v>
+      </c>
+      <c r="S15" s="16">
+        <f t="shared" si="2"/>
         <v>22</v>
       </c>
-      <c r="S15" s="16"/>
       <c r="T15" s="16"/>
-      <c r="U15" s="16" t="s">
+      <c r="U15" s="16"/>
+      <c r="V15" s="16" t="s">
         <v>176</v>
       </c>
-      <c r="V15" s="16" t="s">
+      <c r="W15" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="W15" s="16"/>
       <c r="X15" s="16"/>
       <c r="Y15" s="16"/>
-      <c r="Z15" s="16">
-        <v>0</v>
-      </c>
+      <c r="Z15" s="16"/>
       <c r="AA15" s="16">
-        <f>IF(ISBLANK(AB15),0, LOOKUP(AB15,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AC15/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AB15" s="16"/>
+        <v>0</v>
+      </c>
+      <c r="AB15" s="16">
+        <f>IF(ISBLANK(AC15),0, LOOKUP(AC15,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AD15/100)</f>
+        <v>0</v>
+      </c>
       <c r="AC15" s="16"/>
-      <c r="AD15" s="16" t="s">
-        <v>24</v>
-      </c>
+      <c r="AD15" s="16"/>
       <c r="AE15" s="16" t="s">
         <v>24</v>
       </c>
       <c r="AF15" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG15" s="16" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A16" s="1">
         <v>21100013</v>
       </c>
@@ -6277,43 +6288,46 @@
         <v>0</v>
       </c>
       <c r="Q16" s="16">
+        <v>0</v>
+      </c>
+      <c r="R16" s="16">
         <v>4</v>
       </c>
-      <c r="R16" s="16">
-        <f>I16+J16+ SUM(K16:Q16)*5+Z16+AA16</f>
+      <c r="S16" s="16">
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
-      <c r="S16" s="16"/>
       <c r="T16" s="16"/>
-      <c r="U16" s="16" t="s">
+      <c r="U16" s="16"/>
+      <c r="V16" s="16" t="s">
         <v>180</v>
       </c>
-      <c r="V16" s="16" t="s">
+      <c r="W16" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="W16" s="16"/>
       <c r="X16" s="16"/>
       <c r="Y16" s="16"/>
-      <c r="Z16" s="16">
+      <c r="Z16" s="16"/>
+      <c r="AA16" s="16">
         <v>-10</v>
       </c>
-      <c r="AA16" s="16">
-        <f>IF(ISBLANK(AB16),0, LOOKUP(AB16,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AC16/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AB16" s="16"/>
+      <c r="AB16" s="16">
+        <f>IF(ISBLANK(AC16),0, LOOKUP(AC16,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AD16/100)</f>
+        <v>0</v>
+      </c>
       <c r="AC16" s="16"/>
-      <c r="AD16" s="16" t="s">
-        <v>24</v>
-      </c>
+      <c r="AD16" s="16"/>
       <c r="AE16" s="16" t="s">
         <v>24</v>
       </c>
       <c r="AF16" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG16" s="16" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="17" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A17" s="1">
         <v>21100014</v>
       </c>
@@ -6359,49 +6373,52 @@
         <v>0</v>
       </c>
       <c r="O17" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P17" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q17" s="16">
         <v>0</v>
       </c>
       <c r="R17" s="16">
-        <f>I17+J17+ SUM(K17:Q17)*5+Z17+AA17</f>
+        <v>0</v>
+      </c>
+      <c r="S17" s="16">
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="S17" s="16"/>
       <c r="T17" s="16"/>
-      <c r="U17" s="16" t="s">
+      <c r="U17" s="16"/>
+      <c r="V17" s="16" t="s">
         <v>183</v>
       </c>
-      <c r="V17" s="16" t="s">
+      <c r="W17" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="W17" s="16"/>
       <c r="X17" s="16"/>
       <c r="Y17" s="16"/>
-      <c r="Z17" s="16">
-        <v>0</v>
-      </c>
+      <c r="Z17" s="16"/>
       <c r="AA17" s="16">
-        <f>IF(ISBLANK(AB17),0, LOOKUP(AB17,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AC17/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AB17" s="16"/>
+        <v>0</v>
+      </c>
+      <c r="AB17" s="16">
+        <f>IF(ISBLANK(AC17),0, LOOKUP(AC17,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AD17/100)</f>
+        <v>0</v>
+      </c>
       <c r="AC17" s="16"/>
-      <c r="AD17" s="16" t="s">
-        <v>24</v>
-      </c>
+      <c r="AD17" s="16"/>
       <c r="AE17" s="16" t="s">
         <v>24</v>
       </c>
       <c r="AF17" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG17" s="16" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A18" s="1">
         <v>21100015</v>
       </c>
@@ -6456,40 +6473,43 @@
         <v>0</v>
       </c>
       <c r="R18" s="16">
-        <f>I18+J18+ SUM(K18:Q18)*5+Z18+AA18</f>
+        <v>0</v>
+      </c>
+      <c r="S18" s="16">
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
-      <c r="S18" s="16"/>
       <c r="T18" s="16"/>
-      <c r="U18" s="16" t="s">
+      <c r="U18" s="16"/>
+      <c r="V18" s="16" t="s">
         <v>186</v>
       </c>
-      <c r="V18" s="16" t="s">
+      <c r="W18" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="W18" s="16"/>
       <c r="X18" s="16"/>
       <c r="Y18" s="16"/>
-      <c r="Z18" s="16">
-        <v>0</v>
-      </c>
+      <c r="Z18" s="16"/>
       <c r="AA18" s="16">
-        <f>IF(ISBLANK(AB18),0, LOOKUP(AB18,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AC18/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AB18" s="16"/>
+        <v>0</v>
+      </c>
+      <c r="AB18" s="16">
+        <f>IF(ISBLANK(AC18),0, LOOKUP(AC18,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AD18/100)</f>
+        <v>0</v>
+      </c>
       <c r="AC18" s="16"/>
-      <c r="AD18" s="16" t="s">
-        <v>24</v>
-      </c>
+      <c r="AD18" s="16"/>
       <c r="AE18" s="16" t="s">
         <v>24</v>
       </c>
       <c r="AF18" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG18" s="16" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="19" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A19" s="1">
         <v>21200001</v>
       </c>
@@ -6523,7 +6543,7 @@
         <v>0</v>
       </c>
       <c r="K19" s="16">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L19" s="16">
         <v>0</v>
@@ -6544,40 +6564,43 @@
         <v>0</v>
       </c>
       <c r="R19" s="16">
-        <f>I19+J19+ SUM(K19:Q19)*5+Z19+AA19</f>
+        <v>0</v>
+      </c>
+      <c r="S19" s="16">
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="S19" s="16"/>
       <c r="T19" s="16"/>
       <c r="U19" s="16"/>
-      <c r="V19" s="16" t="s">
+      <c r="V19" s="16"/>
+      <c r="W19" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="W19" s="16"/>
       <c r="X19" s="16"/>
-      <c r="Y19">
+      <c r="Y19" s="16"/>
+      <c r="Z19">
         <v>100</v>
       </c>
-      <c r="Z19" s="16">
-        <v>10</v>
-      </c>
       <c r="AA19" s="16">
-        <f>IF(ISBLANK(AB19),0, LOOKUP(AB19,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AC19/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AB19" s="16"/>
+        <v>0</v>
+      </c>
+      <c r="AB19" s="16">
+        <f>IF(ISBLANK(AC19),0, LOOKUP(AC19,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AD19/100)</f>
+        <v>0</v>
+      </c>
       <c r="AC19" s="16"/>
-      <c r="AD19" s="16" t="s">
-        <v>24</v>
-      </c>
+      <c r="AD19" s="16"/>
       <c r="AE19" s="16" t="s">
         <v>24</v>
       </c>
       <c r="AF19" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG19" s="16" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="20" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A20" s="1">
         <v>21200002</v>
       </c>
@@ -6611,7 +6634,7 @@
         <v>0</v>
       </c>
       <c r="K20" s="16">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="L20" s="16">
         <v>0</v>
@@ -6632,40 +6655,43 @@
         <v>0</v>
       </c>
       <c r="R20" s="16">
-        <f>I20+J20+ SUM(K20:Q20)*5+Z20+AA20</f>
+        <v>0</v>
+      </c>
+      <c r="S20" s="16">
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
-      <c r="S20" s="16"/>
       <c r="T20" s="16"/>
       <c r="U20" s="16"/>
-      <c r="V20" s="16" t="s">
+      <c r="V20" s="16"/>
+      <c r="W20" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="W20" s="16"/>
       <c r="X20" s="16"/>
-      <c r="Y20">
+      <c r="Y20" s="16"/>
+      <c r="Z20">
         <v>101</v>
       </c>
-      <c r="Z20" s="16">
-        <v>14</v>
-      </c>
       <c r="AA20" s="16">
-        <f>IF(ISBLANK(AB20),0, LOOKUP(AB20,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AC20/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AB20" s="16"/>
+        <v>0</v>
+      </c>
+      <c r="AB20" s="16">
+        <f>IF(ISBLANK(AC20),0, LOOKUP(AC20,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AD20/100)</f>
+        <v>0</v>
+      </c>
       <c r="AC20" s="16"/>
-      <c r="AD20" s="16" t="s">
-        <v>24</v>
-      </c>
+      <c r="AD20" s="16"/>
       <c r="AE20" s="16" t="s">
         <v>24</v>
       </c>
       <c r="AF20" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG20" s="16" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="21" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A21" s="1">
         <v>21200003</v>
       </c>
@@ -6677,14 +6703,14 @@
       </c>
       <c r="D21" s="1">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E21" s="1">
         <v>2</v>
       </c>
       <c r="F21" s="1">
         <f t="shared" si="1"/>
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="G21" s="17">
         <v>1</v>
@@ -6699,7 +6725,7 @@
         <v>0</v>
       </c>
       <c r="K21" s="16">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="L21" s="16">
         <v>0</v>
@@ -6720,40 +6746,43 @@
         <v>0</v>
       </c>
       <c r="R21" s="16">
-        <f>I21+J21+ SUM(K21:Q21)*5+Z21+AA21</f>
-        <v>12.5</v>
-      </c>
-      <c r="S21" s="16"/>
+        <v>0</v>
+      </c>
+      <c r="S21" s="16">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
       <c r="T21" s="16"/>
       <c r="U21" s="16"/>
-      <c r="V21" s="16" t="s">
+      <c r="V21" s="16"/>
+      <c r="W21" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="W21" s="16"/>
       <c r="X21" s="16"/>
-      <c r="Y21">
+      <c r="Y21" s="16"/>
+      <c r="Z21">
         <v>102</v>
       </c>
-      <c r="Z21" s="16">
-        <v>12.5</v>
-      </c>
       <c r="AA21" s="16">
-        <f>IF(ISBLANK(AB21),0, LOOKUP(AB21,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AC21/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AB21" s="16"/>
+        <v>0</v>
+      </c>
+      <c r="AB21" s="16">
+        <f>IF(ISBLANK(AC21),0, LOOKUP(AC21,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AD21/100)</f>
+        <v>0</v>
+      </c>
       <c r="AC21" s="16"/>
-      <c r="AD21" s="16" t="s">
-        <v>24</v>
-      </c>
+      <c r="AD21" s="16"/>
       <c r="AE21" s="16" t="s">
         <v>24</v>
       </c>
       <c r="AF21" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG21" s="16" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="22" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A22" s="1">
         <v>21200004</v>
       </c>
@@ -6787,7 +6816,7 @@
         <v>0</v>
       </c>
       <c r="K22" s="16">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="L22" s="16">
         <v>0</v>
@@ -6808,40 +6837,43 @@
         <v>0</v>
       </c>
       <c r="R22" s="16">
-        <f>I22+J22+ SUM(K22:Q22)*5+Z22+AA22</f>
+        <v>0</v>
+      </c>
+      <c r="S22" s="16">
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
-      <c r="S22" s="16"/>
       <c r="T22" s="16"/>
       <c r="U22" s="16"/>
-      <c r="V22" s="16" t="s">
+      <c r="V22" s="16"/>
+      <c r="W22" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="W22" s="16"/>
       <c r="X22" s="16"/>
-      <c r="Y22">
+      <c r="Y22" s="16"/>
+      <c r="Z22">
         <v>103</v>
       </c>
-      <c r="Z22" s="16">
-        <v>14</v>
-      </c>
       <c r="AA22" s="16">
-        <f>IF(ISBLANK(AB22),0, LOOKUP(AB22,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AC22/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AB22" s="16"/>
+        <v>0</v>
+      </c>
+      <c r="AB22" s="16">
+        <f>IF(ISBLANK(AC22),0, LOOKUP(AC22,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AD22/100)</f>
+        <v>0</v>
+      </c>
       <c r="AC22" s="16"/>
-      <c r="AD22" s="16" t="s">
-        <v>24</v>
-      </c>
+      <c r="AD22" s="16"/>
       <c r="AE22" s="16" t="s">
         <v>24</v>
       </c>
       <c r="AF22" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG22" s="16" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="23" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A23" s="1">
         <v>21200005</v>
       </c>
@@ -6875,7 +6907,7 @@
         <v>0</v>
       </c>
       <c r="K23" s="16">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="L23" s="16">
         <v>0</v>
@@ -6896,40 +6928,43 @@
         <v>0</v>
       </c>
       <c r="R23" s="16">
-        <f>I23+J23+ SUM(K23:Q23)*5+Z23+AA23</f>
+        <v>0</v>
+      </c>
+      <c r="S23" s="16">
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="S23" s="16"/>
       <c r="T23" s="16"/>
       <c r="U23" s="16"/>
-      <c r="V23" s="16" t="s">
+      <c r="V23" s="16"/>
+      <c r="W23" s="16" t="s">
         <v>188</v>
       </c>
-      <c r="W23" s="16"/>
       <c r="X23" s="16"/>
-      <c r="Y23">
+      <c r="Y23" s="16"/>
+      <c r="Z23">
         <v>104</v>
       </c>
-      <c r="Z23" s="16">
-        <v>6</v>
-      </c>
       <c r="AA23" s="16">
-        <f>IF(ISBLANK(AB23),0, LOOKUP(AB23,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AC23/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AB23" s="16"/>
+        <v>0</v>
+      </c>
+      <c r="AB23" s="16">
+        <f>IF(ISBLANK(AC23),0, LOOKUP(AC23,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AD23/100)</f>
+        <v>0</v>
+      </c>
       <c r="AC23" s="16"/>
-      <c r="AD23" s="16" t="s">
-        <v>24</v>
-      </c>
+      <c r="AD23" s="16"/>
       <c r="AE23" s="16" t="s">
         <v>24</v>
       </c>
       <c r="AF23" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG23" s="16" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="24" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A24" s="1">
         <v>21200006</v>
       </c>
@@ -6963,7 +6998,7 @@
         <v>0</v>
       </c>
       <c r="K24" s="16">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="L24" s="16">
         <v>0</v>
@@ -6984,40 +7019,43 @@
         <v>0</v>
       </c>
       <c r="R24" s="16">
-        <f>I24+J24+ SUM(K24:Q24)*5+Z24+AA24</f>
+        <v>0</v>
+      </c>
+      <c r="S24" s="16">
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="S24" s="16"/>
       <c r="T24" s="16"/>
       <c r="U24" s="16"/>
-      <c r="V24" s="16" t="s">
+      <c r="V24" s="16"/>
+      <c r="W24" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="W24" s="16"/>
       <c r="X24" s="16"/>
-      <c r="Y24">
+      <c r="Y24" s="16"/>
+      <c r="Z24">
         <v>105</v>
       </c>
-      <c r="Z24" s="16">
-        <v>6</v>
-      </c>
       <c r="AA24" s="16">
-        <f>IF(ISBLANK(AB24),0, LOOKUP(AB24,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AC24/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AB24" s="16"/>
+        <v>0</v>
+      </c>
+      <c r="AB24" s="16">
+        <f>IF(ISBLANK(AC24),0, LOOKUP(AC24,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AD24/100)</f>
+        <v>0</v>
+      </c>
       <c r="AC24" s="16"/>
-      <c r="AD24" s="16" t="s">
-        <v>24</v>
-      </c>
+      <c r="AD24" s="16"/>
       <c r="AE24" s="16" t="s">
         <v>24</v>
       </c>
       <c r="AF24" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG24" s="16" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="25" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A25" s="1">
         <v>21200007</v>
       </c>
@@ -7051,7 +7089,7 @@
         <v>0</v>
       </c>
       <c r="K25" s="16">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="L25" s="16">
         <v>0</v>
@@ -7072,40 +7110,43 @@
         <v>0</v>
       </c>
       <c r="R25" s="16">
-        <f>I25+J25+ SUM(K25:Q25)*5+Z25+AA25</f>
+        <v>0</v>
+      </c>
+      <c r="S25" s="16">
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="S25" s="16"/>
       <c r="T25" s="16"/>
       <c r="U25" s="16"/>
-      <c r="V25" s="16" t="s">
+      <c r="V25" s="16"/>
+      <c r="W25" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="W25" s="16"/>
       <c r="X25" s="16"/>
-      <c r="Y25">
+      <c r="Y25" s="16"/>
+      <c r="Z25">
         <v>106</v>
       </c>
-      <c r="Z25" s="16">
-        <v>9</v>
-      </c>
       <c r="AA25" s="16">
-        <f>IF(ISBLANK(AB25),0, LOOKUP(AB25,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AC25/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AB25" s="16"/>
+        <v>0</v>
+      </c>
+      <c r="AB25" s="16">
+        <f>IF(ISBLANK(AC25),0, LOOKUP(AC25,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AD25/100)</f>
+        <v>0</v>
+      </c>
       <c r="AC25" s="16"/>
-      <c r="AD25" s="16" t="s">
-        <v>24</v>
-      </c>
+      <c r="AD25" s="16"/>
       <c r="AE25" s="16" t="s">
         <v>24</v>
       </c>
       <c r="AF25" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG25" s="16" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="26" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A26" s="1">
         <v>21200008</v>
       </c>
@@ -7139,7 +7180,7 @@
         <v>0</v>
       </c>
       <c r="K26" s="16">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="L26" s="16">
         <v>0</v>
@@ -7160,40 +7201,43 @@
         <v>0</v>
       </c>
       <c r="R26" s="16">
-        <f>I26+J26+ SUM(K26:Q26)*5+Z26+AA26</f>
+        <v>0</v>
+      </c>
+      <c r="S26" s="16">
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
-      <c r="S26" s="16"/>
       <c r="T26" s="16"/>
       <c r="U26" s="16"/>
-      <c r="V26" s="16" t="s">
+      <c r="V26" s="16"/>
+      <c r="W26" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="W26" s="16"/>
       <c r="X26" s="16"/>
-      <c r="Y26">
+      <c r="Y26" s="16"/>
+      <c r="Z26">
         <v>107</v>
       </c>
-      <c r="Z26" s="16">
-        <v>18</v>
-      </c>
       <c r="AA26" s="16">
-        <f>IF(ISBLANK(AB26),0, LOOKUP(AB26,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AC26/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AB26" s="16"/>
+        <v>0</v>
+      </c>
+      <c r="AB26" s="16">
+        <f>IF(ISBLANK(AC26),0, LOOKUP(AC26,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AD26/100)</f>
+        <v>0</v>
+      </c>
       <c r="AC26" s="16"/>
-      <c r="AD26" s="16" t="s">
-        <v>24</v>
-      </c>
+      <c r="AD26" s="16"/>
       <c r="AE26" s="16" t="s">
         <v>24</v>
       </c>
       <c r="AF26" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG26" s="16" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="27" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A27" s="1">
         <v>21200009</v>
       </c>
@@ -7227,7 +7271,7 @@
         <v>0</v>
       </c>
       <c r="K27" s="16">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="L27" s="16">
         <v>0</v>
@@ -7248,40 +7292,43 @@
         <v>0</v>
       </c>
       <c r="R27" s="16">
-        <f>I27+J27+ SUM(K27:Q27)*5+Z27+AA27</f>
+        <v>0</v>
+      </c>
+      <c r="S27" s="16">
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
-      <c r="S27" s="16"/>
       <c r="T27" s="16"/>
       <c r="U27" s="16"/>
-      <c r="V27" s="16" t="s">
+      <c r="V27" s="16"/>
+      <c r="W27" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="W27" s="16"/>
       <c r="X27" s="16"/>
-      <c r="Y27">
+      <c r="Y27" s="16"/>
+      <c r="Z27">
         <v>108</v>
       </c>
-      <c r="Z27" s="16">
-        <v>15</v>
-      </c>
       <c r="AA27" s="16">
-        <f>IF(ISBLANK(AB27),0, LOOKUP(AB27,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AC27/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AB27" s="16"/>
+        <v>0</v>
+      </c>
+      <c r="AB27" s="16">
+        <f>IF(ISBLANK(AC27),0, LOOKUP(AC27,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AD27/100)</f>
+        <v>0</v>
+      </c>
       <c r="AC27" s="16"/>
-      <c r="AD27" s="16" t="s">
-        <v>24</v>
-      </c>
+      <c r="AD27" s="16"/>
       <c r="AE27" s="16" t="s">
         <v>24</v>
       </c>
       <c r="AF27" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG27" s="16" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="28" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A28" s="1">
         <v>21200010</v>
       </c>
@@ -7315,7 +7362,7 @@
         <v>0</v>
       </c>
       <c r="K28" s="16">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="L28" s="16">
         <v>0</v>
@@ -7336,40 +7383,43 @@
         <v>0</v>
       </c>
       <c r="R28" s="16">
-        <f>I28+J28+ SUM(K28:Q28)*5+Z28+AA28</f>
+        <v>0</v>
+      </c>
+      <c r="S28" s="16">
+        <f t="shared" si="2"/>
         <v>25</v>
       </c>
-      <c r="S28" s="16"/>
       <c r="T28" s="16"/>
       <c r="U28" s="16"/>
-      <c r="V28" s="16" t="s">
+      <c r="V28" s="16"/>
+      <c r="W28" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="W28" s="16"/>
       <c r="X28" s="16"/>
-      <c r="Y28">
+      <c r="Y28" s="16"/>
+      <c r="Z28">
         <v>109</v>
       </c>
-      <c r="Z28" s="16">
-        <v>25</v>
-      </c>
       <c r="AA28" s="16">
-        <f>IF(ISBLANK(AB28),0, LOOKUP(AB28,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AC28/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AB28" s="16"/>
+        <v>0</v>
+      </c>
+      <c r="AB28" s="16">
+        <f>IF(ISBLANK(AC28),0, LOOKUP(AC28,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AD28/100)</f>
+        <v>0</v>
+      </c>
       <c r="AC28" s="16"/>
-      <c r="AD28" s="16" t="s">
-        <v>24</v>
-      </c>
+      <c r="AD28" s="16"/>
       <c r="AE28" s="16" t="s">
         <v>24</v>
       </c>
       <c r="AF28" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG28" s="16" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="29" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A29" s="1">
         <v>21300001</v>
       </c>
@@ -7424,40 +7474,43 @@
         <v>0</v>
       </c>
       <c r="R29" s="16">
-        <f>I29+J29+ SUM(K29:Q29)*5+Z29+AA29</f>
+        <v>0</v>
+      </c>
+      <c r="S29" s="16">
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="S29" s="16"/>
-      <c r="T29" s="16" t="s">
+      <c r="T29" s="16"/>
+      <c r="U29" s="16" t="s">
         <v>168</v>
       </c>
-      <c r="U29" s="16"/>
-      <c r="V29" s="16" t="s">
+      <c r="V29" s="16"/>
+      <c r="W29" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="W29" s="16"/>
       <c r="X29" s="16"/>
       <c r="Y29" s="16"/>
-      <c r="Z29" s="16">
-        <v>0</v>
-      </c>
+      <c r="Z29" s="16"/>
       <c r="AA29" s="16">
-        <f>IF(ISBLANK(AB29),0, LOOKUP(AB29,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AC29/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AB29" s="16"/>
+        <v>0</v>
+      </c>
+      <c r="AB29" s="16">
+        <f>IF(ISBLANK(AC29),0, LOOKUP(AC29,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AD29/100)</f>
+        <v>0</v>
+      </c>
       <c r="AC29" s="16"/>
-      <c r="AD29" s="16" t="s">
-        <v>24</v>
-      </c>
+      <c r="AD29" s="16"/>
       <c r="AE29" s="16" t="s">
         <v>24</v>
       </c>
       <c r="AF29" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG29" s="16" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="30" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A30" s="1">
         <v>21300002</v>
       </c>
@@ -7512,44 +7565,47 @@
         <v>0</v>
       </c>
       <c r="R30" s="16">
-        <f>I30+J30+ SUM(K30:Q30)*5+Z30+AA30</f>
+        <v>0</v>
+      </c>
+      <c r="S30" s="16">
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="S30" s="16"/>
-      <c r="T30" s="16" t="s">
+      <c r="T30" s="16"/>
+      <c r="U30" s="16" t="s">
         <v>169</v>
       </c>
-      <c r="U30" s="16"/>
-      <c r="V30" s="16" t="s">
+      <c r="V30" s="16"/>
+      <c r="W30" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="W30" s="16"/>
       <c r="X30" s="16"/>
       <c r="Y30" s="16"/>
-      <c r="Z30" s="16">
-        <v>0</v>
-      </c>
+      <c r="Z30" s="16"/>
       <c r="AA30" s="16">
-        <f>IF(ISBLANK(AB30),0, LOOKUP(AB30,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AC30/100)</f>
+        <v>0</v>
+      </c>
+      <c r="AB30" s="16">
+        <f>IF(ISBLANK(AC30),0, LOOKUP(AC30,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AD30/100)</f>
         <v>6</v>
       </c>
-      <c r="AB30" s="16">
+      <c r="AC30" s="16">
         <v>55510010</v>
       </c>
-      <c r="AC30" s="16">
+      <c r="AD30" s="16">
         <v>60</v>
       </c>
-      <c r="AD30" s="16" t="s">
-        <v>24</v>
-      </c>
       <c r="AE30" s="16" t="s">
         <v>24</v>
       </c>
       <c r="AF30" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG30" s="16" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="31" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A31" s="1">
         <v>21300003</v>
       </c>
@@ -7598,46 +7654,49 @@
         <v>0</v>
       </c>
       <c r="P31" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q31" s="16">
         <v>2</v>
       </c>
-      <c r="Q31" s="16">
-        <v>0</v>
-      </c>
       <c r="R31" s="16">
-        <f>I31+J31+ SUM(K31:Q31)*5+Z31+AA31</f>
+        <v>0</v>
+      </c>
+      <c r="S31" s="16">
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
-      <c r="S31" s="16"/>
-      <c r="T31" s="16" t="s">
+      <c r="T31" s="16"/>
+      <c r="U31" s="16" t="s">
         <v>170</v>
       </c>
-      <c r="U31" s="16"/>
-      <c r="V31" s="16" t="s">
+      <c r="V31" s="16"/>
+      <c r="W31" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="W31" s="16"/>
       <c r="X31" s="16"/>
       <c r="Y31" s="16"/>
-      <c r="Z31" s="16">
-        <v>0</v>
-      </c>
+      <c r="Z31" s="16"/>
       <c r="AA31" s="16">
-        <f>IF(ISBLANK(AB31),0, LOOKUP(AB31,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AC31/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AB31" s="16"/>
+        <v>0</v>
+      </c>
+      <c r="AB31" s="16">
+        <f>IF(ISBLANK(AC31),0, LOOKUP(AC31,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AD31/100)</f>
+        <v>0</v>
+      </c>
       <c r="AC31" s="16"/>
-      <c r="AD31" s="16" t="s">
-        <v>24</v>
-      </c>
+      <c r="AD31" s="16"/>
       <c r="AE31" s="16" t="s">
         <v>24</v>
       </c>
       <c r="AF31" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG31" s="16" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="32" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A32" s="1">
         <v>21300004</v>
       </c>
@@ -7692,44 +7751,47 @@
         <v>0</v>
       </c>
       <c r="R32" s="16">
-        <f>I32+J32+ SUM(K32:Q32)*5+Z32+AA32</f>
+        <v>0</v>
+      </c>
+      <c r="S32" s="16">
+        <f t="shared" si="2"/>
         <v>17.3</v>
       </c>
-      <c r="S32" s="16"/>
-      <c r="T32" s="16" t="s">
+      <c r="T32" s="16"/>
+      <c r="U32" s="16" t="s">
         <v>171</v>
       </c>
-      <c r="U32" s="16"/>
-      <c r="V32" s="16" t="s">
+      <c r="V32" s="16"/>
+      <c r="W32" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="W32" s="16"/>
       <c r="X32" s="16"/>
       <c r="Y32" s="16"/>
-      <c r="Z32" s="16">
-        <v>0</v>
-      </c>
+      <c r="Z32" s="16"/>
       <c r="AA32" s="16">
-        <f>IF(ISBLANK(AB32),0, LOOKUP(AB32,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AC32/100)</f>
+        <v>0</v>
+      </c>
+      <c r="AB32" s="16">
+        <f>IF(ISBLANK(AC32),0, LOOKUP(AC32,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AD32/100)</f>
         <v>9.3000000000000007</v>
       </c>
-      <c r="AB32" s="16">
+      <c r="AC32" s="16">
         <v>55510012</v>
       </c>
-      <c r="AC32" s="16">
+      <c r="AD32" s="16">
         <v>15</v>
       </c>
-      <c r="AD32" s="16" t="s">
-        <v>24</v>
-      </c>
       <c r="AE32" s="16" t="s">
         <v>24</v>
       </c>
       <c r="AF32" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG32" s="16" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="33" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A33" s="1">
         <v>21300005</v>
       </c>
@@ -7784,40 +7846,43 @@
         <v>0</v>
       </c>
       <c r="R33" s="16">
-        <f>I33+J33+ SUM(K33:Q33)*5+Z33+AA33</f>
+        <v>0</v>
+      </c>
+      <c r="S33" s="16">
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="S33" s="16"/>
-      <c r="T33" s="16" t="s">
+      <c r="T33" s="16"/>
+      <c r="U33" s="16" t="s">
         <v>170</v>
       </c>
-      <c r="U33" s="16"/>
-      <c r="V33" s="16" t="s">
+      <c r="V33" s="16"/>
+      <c r="W33" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="W33" s="16"/>
       <c r="X33" s="16"/>
       <c r="Y33" s="16"/>
-      <c r="Z33" s="16">
-        <v>0</v>
-      </c>
+      <c r="Z33" s="16"/>
       <c r="AA33" s="16">
-        <f>IF(ISBLANK(AB33),0, LOOKUP(AB33,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AC33/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AB33" s="16"/>
+        <v>0</v>
+      </c>
+      <c r="AB33" s="16">
+        <f>IF(ISBLANK(AC33),0, LOOKUP(AC33,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AD33/100)</f>
+        <v>0</v>
+      </c>
       <c r="AC33" s="16"/>
-      <c r="AD33" s="16" t="s">
-        <v>24</v>
-      </c>
+      <c r="AD33" s="16"/>
       <c r="AE33" s="16" t="s">
         <v>24</v>
       </c>
       <c r="AF33" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG33" s="16" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="34" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A34" s="1">
         <v>21300006</v>
       </c>
@@ -7872,40 +7937,43 @@
         <v>0</v>
       </c>
       <c r="R34" s="16">
-        <f>I34+J34+ SUM(K34:Q34)*5+Z34+AA34</f>
+        <v>0</v>
+      </c>
+      <c r="S34" s="16">
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
-      <c r="S34" s="16"/>
-      <c r="T34" s="16" t="s">
+      <c r="T34" s="16"/>
+      <c r="U34" s="16" t="s">
         <v>171</v>
       </c>
-      <c r="U34" s="16"/>
-      <c r="V34" s="16" t="s">
+      <c r="V34" s="16"/>
+      <c r="W34" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="W34" s="16"/>
       <c r="X34" s="16"/>
       <c r="Y34" s="16"/>
-      <c r="Z34" s="16">
-        <v>0</v>
-      </c>
+      <c r="Z34" s="16"/>
       <c r="AA34" s="16">
-        <f>IF(ISBLANK(AB34),0, LOOKUP(AB34,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AC34/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AB34" s="16"/>
+        <v>0</v>
+      </c>
+      <c r="AB34" s="16">
+        <f>IF(ISBLANK(AC34),0, LOOKUP(AC34,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AD34/100)</f>
+        <v>0</v>
+      </c>
       <c r="AC34" s="16"/>
-      <c r="AD34" s="16" t="s">
-        <v>24</v>
-      </c>
+      <c r="AD34" s="16"/>
       <c r="AE34" s="16" t="s">
         <v>24</v>
       </c>
       <c r="AF34" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG34" s="16" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="35" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A35" s="1">
         <v>21300007</v>
       </c>
@@ -7945,11 +8013,11 @@
         <v>0</v>
       </c>
       <c r="M35" s="16">
+        <v>0</v>
+      </c>
+      <c r="N35" s="16">
         <v>5</v>
       </c>
-      <c r="N35" s="16">
-        <v>0</v>
-      </c>
       <c r="O35" s="16">
         <v>0</v>
       </c>
@@ -7960,40 +8028,43 @@
         <v>0</v>
       </c>
       <c r="R35" s="16">
-        <f>I35+J35+ SUM(K35:Q35)*5+Z35+AA35</f>
+        <v>0</v>
+      </c>
+      <c r="S35" s="16">
+        <f t="shared" si="2"/>
         <v>30</v>
       </c>
-      <c r="S35" s="16"/>
-      <c r="T35" s="16" t="s">
+      <c r="T35" s="16"/>
+      <c r="U35" s="16" t="s">
         <v>174</v>
       </c>
-      <c r="U35" s="16"/>
-      <c r="V35" s="16" t="s">
+      <c r="V35" s="16"/>
+      <c r="W35" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="W35" s="16"/>
       <c r="X35" s="16"/>
       <c r="Y35" s="16"/>
-      <c r="Z35" s="16">
-        <v>0</v>
-      </c>
+      <c r="Z35" s="16"/>
       <c r="AA35" s="16">
-        <f>IF(ISBLANK(AB35),0, LOOKUP(AB35,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AC35/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AB35" s="16"/>
+        <v>0</v>
+      </c>
+      <c r="AB35" s="16">
+        <f>IF(ISBLANK(AC35),0, LOOKUP(AC35,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AD35/100)</f>
+        <v>0</v>
+      </c>
       <c r="AC35" s="16"/>
-      <c r="AD35" s="16" t="s">
-        <v>24</v>
-      </c>
+      <c r="AD35" s="16"/>
       <c r="AE35" s="16" t="s">
         <v>24</v>
       </c>
       <c r="AF35" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG35" s="16" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="36" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A36" s="1">
         <v>21300008</v>
       </c>
@@ -8004,14 +8075,14 @@
         <v>274</v>
       </c>
       <c r="D36" s="1">
-        <f t="shared" ref="D36:D59" si="2">IF(R36&gt;=23,4,IF(AND(R36&gt;=18,R36&lt;23),3,IF(AND(R36&gt;=13,R36&lt;18),2,IF(AND(R36&gt;=8,R36&lt;13),1,0))))</f>
+        <f t="shared" ref="D36:D59" si="3">IF(S36&gt;=23,4,IF(AND(S36&gt;=18,S36&lt;23),3,IF(AND(S36&gt;=13,S36&lt;18),2,IF(AND(S36&gt;=8,S36&lt;13),1,0))))</f>
         <v>0</v>
       </c>
       <c r="E36" s="1">
         <v>3</v>
       </c>
       <c r="F36" s="1">
-        <f t="shared" ref="F36:F59" si="3">D36*50+50</f>
+        <f t="shared" ref="F36:F59" si="4">D36*50+50</f>
         <v>50</v>
       </c>
       <c r="G36" s="17">
@@ -8048,40 +8119,43 @@
         <v>0</v>
       </c>
       <c r="R36" s="16">
-        <f>I36+J36+ SUM(K36:Q36)*5+Z36+AA36</f>
-        <v>1</v>
-      </c>
-      <c r="S36" s="16"/>
-      <c r="T36" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="S36" s="16">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="T36" s="16"/>
+      <c r="U36" s="16" t="s">
         <v>172</v>
       </c>
-      <c r="U36" s="16"/>
-      <c r="V36" s="16" t="s">
+      <c r="V36" s="16"/>
+      <c r="W36" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="W36" s="16"/>
       <c r="X36" s="16"/>
       <c r="Y36" s="16"/>
-      <c r="Z36" s="16">
-        <v>0</v>
-      </c>
+      <c r="Z36" s="16"/>
       <c r="AA36" s="16">
-        <f>IF(ISBLANK(AB36),0, LOOKUP(AB36,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AC36/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AB36" s="16"/>
+        <v>0</v>
+      </c>
+      <c r="AB36" s="16">
+        <f>IF(ISBLANK(AC36),0, LOOKUP(AC36,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AD36/100)</f>
+        <v>0</v>
+      </c>
       <c r="AC36" s="16"/>
-      <c r="AD36" s="16" t="s">
-        <v>24</v>
-      </c>
+      <c r="AD36" s="16"/>
       <c r="AE36" s="16" t="s">
         <v>24</v>
       </c>
       <c r="AF36" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG36" s="16" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="37" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A37" s="1">
         <v>21300009</v>
       </c>
@@ -8092,14 +8166,14 @@
         <v>240</v>
       </c>
       <c r="D37" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="E37" s="1">
         <v>3</v>
       </c>
       <c r="F37" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>200</v>
       </c>
       <c r="G37" s="17">
@@ -8121,11 +8195,11 @@
         <v>0</v>
       </c>
       <c r="M37" s="16">
+        <v>0</v>
+      </c>
+      <c r="N37" s="16">
         <v>-4</v>
       </c>
-      <c r="N37" s="16">
-        <v>0</v>
-      </c>
       <c r="O37" s="16">
         <v>0</v>
       </c>
@@ -8136,44 +8210,47 @@
         <v>0</v>
       </c>
       <c r="R37" s="16">
-        <f>I37+J37+ SUM(K37:Q37)*5+Z37+AA37</f>
+        <v>0</v>
+      </c>
+      <c r="S37" s="16">
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
-      <c r="S37" s="16"/>
-      <c r="T37" s="16" t="s">
+      <c r="T37" s="16"/>
+      <c r="U37" s="16" t="s">
         <v>173</v>
       </c>
-      <c r="U37" s="16"/>
-      <c r="V37" s="16" t="s">
+      <c r="V37" s="16"/>
+      <c r="W37" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="W37" s="16"/>
       <c r="X37" s="16"/>
       <c r="Y37" s="16"/>
-      <c r="Z37" s="16">
-        <v>0</v>
-      </c>
+      <c r="Z37" s="16"/>
       <c r="AA37" s="16">
-        <f>IF(ISBLANK(AB37),0, LOOKUP(AB37,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AC37/100)</f>
+        <v>0</v>
+      </c>
+      <c r="AB37" s="16">
+        <f>IF(ISBLANK(AC37),0, LOOKUP(AC37,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AD37/100)</f>
         <v>35</v>
       </c>
-      <c r="AB37" s="16">
+      <c r="AC37" s="16">
         <v>55100007</v>
       </c>
-      <c r="AC37" s="16">
+      <c r="AD37" s="16">
         <v>100</v>
       </c>
-      <c r="AD37" s="16" t="s">
-        <v>24</v>
-      </c>
       <c r="AE37" s="16" t="s">
         <v>24</v>
       </c>
       <c r="AF37" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG37" s="16" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="38" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A38" s="18">
         <v>21400001</v>
       </c>
@@ -8184,14 +8261,14 @@
         <v>241</v>
       </c>
       <c r="D38" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="E38" s="1">
         <v>4</v>
       </c>
       <c r="F38" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>50</v>
       </c>
       <c r="G38" s="17">
@@ -8207,10 +8284,10 @@
         <v>1</v>
       </c>
       <c r="K38" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L38" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M38" s="16">
         <v>0</v>
@@ -8228,38 +8305,41 @@
         <v>0</v>
       </c>
       <c r="R38" s="16">
-        <f>I38+J38+ SUM(K38:Q38)*5+Z38+AA38</f>
+        <v>0</v>
+      </c>
+      <c r="S38" s="16">
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="S38" s="16"/>
       <c r="T38" s="16"/>
       <c r="U38" s="16"/>
-      <c r="V38" s="16" t="s">
+      <c r="V38" s="16"/>
+      <c r="W38" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="W38" s="16"/>
       <c r="X38" s="16"/>
       <c r="Y38" s="16"/>
-      <c r="Z38" s="16">
-        <v>0</v>
-      </c>
+      <c r="Z38" s="16"/>
       <c r="AA38" s="16">
-        <f>IF(ISBLANK(AB38),0, LOOKUP(AB38,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AC38/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AB38" s="16"/>
+        <v>0</v>
+      </c>
+      <c r="AB38" s="16">
+        <f>IF(ISBLANK(AC38),0, LOOKUP(AC38,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AD38/100)</f>
+        <v>0</v>
+      </c>
       <c r="AC38" s="16"/>
-      <c r="AD38" s="16" t="s">
-        <v>24</v>
-      </c>
+      <c r="AD38" s="16"/>
       <c r="AE38" s="16" t="s">
         <v>24</v>
       </c>
       <c r="AF38" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG38" s="16" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="39" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A39" s="18">
         <v>21400002</v>
       </c>
@@ -8270,14 +8350,14 @@
         <v>242</v>
       </c>
       <c r="D39" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="E39" s="1">
         <v>4</v>
       </c>
       <c r="F39" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="G39" s="17">
@@ -8293,11 +8373,11 @@
         <v>0</v>
       </c>
       <c r="K39" s="16">
+        <v>0</v>
+      </c>
+      <c r="L39" s="16">
         <v>2</v>
       </c>
-      <c r="L39" s="16">
-        <v>0</v>
-      </c>
       <c r="M39" s="16">
         <v>0</v>
       </c>
@@ -8314,38 +8394,41 @@
         <v>0</v>
       </c>
       <c r="R39" s="16">
-        <f>I39+J39+ SUM(K39:Q39)*5+Z39+AA39</f>
+        <v>0</v>
+      </c>
+      <c r="S39" s="16">
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="S39" s="16"/>
       <c r="T39" s="16"/>
       <c r="U39" s="16"/>
-      <c r="V39" s="16" t="s">
+      <c r="V39" s="16"/>
+      <c r="W39" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="W39" s="16"/>
       <c r="X39" s="16"/>
       <c r="Y39" s="16"/>
-      <c r="Z39" s="16">
-        <v>0</v>
-      </c>
+      <c r="Z39" s="16"/>
       <c r="AA39" s="16">
-        <f>IF(ISBLANK(AB39),0, LOOKUP(AB39,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AC39/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AB39" s="16"/>
+        <v>0</v>
+      </c>
+      <c r="AB39" s="16">
+        <f>IF(ISBLANK(AC39),0, LOOKUP(AC39,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AD39/100)</f>
+        <v>0</v>
+      </c>
       <c r="AC39" s="16"/>
-      <c r="AD39" s="16" t="s">
-        <v>24</v>
-      </c>
+      <c r="AD39" s="16"/>
       <c r="AE39" s="16" t="s">
         <v>24</v>
       </c>
       <c r="AF39" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG39" s="16" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="40" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A40" s="18">
         <v>21400003</v>
       </c>
@@ -8356,14 +8439,14 @@
         <v>243</v>
       </c>
       <c r="D40" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="E40" s="1">
         <v>4</v>
       </c>
       <c r="F40" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>150</v>
       </c>
       <c r="G40" s="17">
@@ -8379,10 +8462,10 @@
         <v>0</v>
       </c>
       <c r="K40" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L40" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M40" s="16">
         <v>0</v>
@@ -8400,42 +8483,45 @@
         <v>0</v>
       </c>
       <c r="R40" s="16">
-        <f>I40+J40+ SUM(K40:Q40)*5+Z40+AA40</f>
+        <v>0</v>
+      </c>
+      <c r="S40" s="16">
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
-      <c r="S40" s="16"/>
       <c r="T40" s="16"/>
       <c r="U40" s="16"/>
-      <c r="V40" s="16" t="s">
+      <c r="V40" s="16"/>
+      <c r="W40" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="W40" s="16"/>
       <c r="X40" s="16"/>
       <c r="Y40" s="16"/>
-      <c r="Z40" s="16">
-        <v>0</v>
-      </c>
+      <c r="Z40" s="16"/>
       <c r="AA40" s="16">
-        <f>IF(ISBLANK(AB40),0, LOOKUP(AB40,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AC40/100)</f>
+        <v>0</v>
+      </c>
+      <c r="AB40" s="16">
+        <f>IF(ISBLANK(AC40),0, LOOKUP(AC40,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AD40/100)</f>
         <v>10</v>
       </c>
-      <c r="AB40" s="16">
+      <c r="AC40" s="16">
         <v>55110005</v>
       </c>
-      <c r="AC40" s="16">
+      <c r="AD40" s="16">
         <v>50</v>
       </c>
-      <c r="AD40" s="16" t="s">
-        <v>24</v>
-      </c>
       <c r="AE40" s="16" t="s">
         <v>24</v>
       </c>
       <c r="AF40" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG40" s="16" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="41" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A41">
         <v>21400004</v>
       </c>
@@ -8446,14 +8532,14 @@
         <v>244</v>
       </c>
       <c r="D41" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="E41" s="1">
         <v>4</v>
       </c>
       <c r="F41" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>200</v>
       </c>
       <c r="G41" s="17">
@@ -8469,11 +8555,11 @@
         <v>0</v>
       </c>
       <c r="K41" s="16">
+        <v>0</v>
+      </c>
+      <c r="L41" s="16">
         <v>4</v>
       </c>
-      <c r="L41" s="16">
-        <v>0</v>
-      </c>
       <c r="M41" s="16">
         <v>0</v>
       </c>
@@ -8490,38 +8576,41 @@
         <v>0</v>
       </c>
       <c r="R41" s="16">
-        <f>I41+J41+ SUM(K41:Q41)*5+Z41+AA41</f>
+        <v>0</v>
+      </c>
+      <c r="S41" s="16">
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
-      <c r="S41" s="16"/>
       <c r="T41" s="16"/>
       <c r="U41" s="16"/>
-      <c r="V41" s="16" t="s">
+      <c r="V41" s="16"/>
+      <c r="W41" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="W41" s="16"/>
       <c r="X41" s="16"/>
       <c r="Y41" s="16"/>
-      <c r="Z41" s="16">
-        <v>0</v>
-      </c>
+      <c r="Z41" s="16"/>
       <c r="AA41" s="16">
-        <f>IF(ISBLANK(AB41),0, LOOKUP(AB41,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AC41/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AB41" s="16"/>
+        <v>0</v>
+      </c>
+      <c r="AB41" s="16">
+        <f>IF(ISBLANK(AC41),0, LOOKUP(AC41,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AD41/100)</f>
+        <v>0</v>
+      </c>
       <c r="AC41" s="16"/>
-      <c r="AD41" s="16" t="s">
-        <v>24</v>
-      </c>
+      <c r="AD41" s="16"/>
       <c r="AE41" s="16" t="s">
         <v>24</v>
       </c>
       <c r="AF41" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG41" s="16" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="42" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A42" s="18">
         <v>21400005</v>
       </c>
@@ -8532,14 +8621,14 @@
         <v>245</v>
       </c>
       <c r="D42" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="E42" s="1">
         <v>4</v>
       </c>
       <c r="F42" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="G42" s="17">
@@ -8555,10 +8644,10 @@
         <v>3</v>
       </c>
       <c r="K42" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L42" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M42" s="16">
         <v>0</v>
@@ -8576,38 +8665,41 @@
         <v>0</v>
       </c>
       <c r="R42" s="16">
-        <f>I42+J42+ SUM(K42:Q42)*5+Z42+AA42</f>
+        <v>0</v>
+      </c>
+      <c r="S42" s="16">
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="S42" s="16"/>
       <c r="T42" s="16"/>
       <c r="U42" s="16"/>
-      <c r="V42" s="16" t="s">
+      <c r="V42" s="16"/>
+      <c r="W42" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="W42" s="16"/>
       <c r="X42" s="16"/>
       <c r="Y42" s="16"/>
-      <c r="Z42" s="16">
-        <v>0</v>
-      </c>
+      <c r="Z42" s="16"/>
       <c r="AA42" s="16">
-        <f>IF(ISBLANK(AB42),0, LOOKUP(AB42,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AC42/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AB42" s="16"/>
+        <v>0</v>
+      </c>
+      <c r="AB42" s="16">
+        <f>IF(ISBLANK(AC42),0, LOOKUP(AC42,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AD42/100)</f>
+        <v>0</v>
+      </c>
       <c r="AC42" s="16"/>
-      <c r="AD42" s="16" t="s">
-        <v>24</v>
-      </c>
+      <c r="AD42" s="16"/>
       <c r="AE42" s="16" t="s">
         <v>24</v>
       </c>
       <c r="AF42" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG42" s="16" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="43" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A43">
         <v>21400006</v>
       </c>
@@ -8618,14 +8710,14 @@
         <v>246</v>
       </c>
       <c r="D43" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="E43" s="1">
         <v>4</v>
       </c>
       <c r="F43" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>150</v>
       </c>
       <c r="G43" s="17">
@@ -8641,11 +8733,11 @@
         <v>4</v>
       </c>
       <c r="K43" s="16">
+        <v>0</v>
+      </c>
+      <c r="L43" s="16">
         <v>2</v>
       </c>
-      <c r="L43" s="16">
-        <v>0</v>
-      </c>
       <c r="M43" s="16">
         <v>0</v>
       </c>
@@ -8662,38 +8754,41 @@
         <v>0</v>
       </c>
       <c r="R43" s="16">
-        <f>I43+J43+ SUM(K43:Q43)*5+Z43+AA43</f>
+        <v>0</v>
+      </c>
+      <c r="S43" s="16">
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
-      <c r="S43" s="16"/>
       <c r="T43" s="16"/>
       <c r="U43" s="16"/>
-      <c r="V43" s="16" t="s">
+      <c r="V43" s="16"/>
+      <c r="W43" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="W43" s="16"/>
       <c r="X43" s="16"/>
       <c r="Y43" s="16"/>
-      <c r="Z43" s="16">
-        <v>0</v>
-      </c>
+      <c r="Z43" s="16"/>
       <c r="AA43" s="16">
-        <f>IF(ISBLANK(AB43),0, LOOKUP(AB43,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AC43/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AB43" s="16"/>
+        <v>0</v>
+      </c>
+      <c r="AB43" s="16">
+        <f>IF(ISBLANK(AC43),0, LOOKUP(AC43,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AD43/100)</f>
+        <v>0</v>
+      </c>
       <c r="AC43" s="16"/>
-      <c r="AD43" s="16" t="s">
-        <v>24</v>
-      </c>
+      <c r="AD43" s="16"/>
       <c r="AE43" s="16" t="s">
         <v>24</v>
       </c>
       <c r="AF43" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG43" s="16" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="44" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A44">
         <v>21400007</v>
       </c>
@@ -8704,14 +8799,14 @@
         <v>247</v>
       </c>
       <c r="D44" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="E44" s="1">
         <v>4</v>
       </c>
       <c r="F44" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>200</v>
       </c>
       <c r="G44" s="17">
@@ -8739,47 +8834,50 @@
         <v>0</v>
       </c>
       <c r="O44" s="16">
+        <v>0</v>
+      </c>
+      <c r="P44" s="16">
         <v>4</v>
       </c>
-      <c r="P44" s="16">
-        <v>0</v>
-      </c>
       <c r="Q44" s="16">
         <v>0</v>
       </c>
       <c r="R44" s="16">
-        <f>I44+J44+ SUM(K44:Q44)*5+Z44+AA44</f>
+        <v>0</v>
+      </c>
+      <c r="S44" s="16">
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
-      <c r="S44" s="16"/>
       <c r="T44" s="16"/>
       <c r="U44" s="16"/>
-      <c r="V44" s="16" t="s">
+      <c r="V44" s="16"/>
+      <c r="W44" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="W44" s="16"/>
       <c r="X44" s="16"/>
       <c r="Y44" s="16"/>
-      <c r="Z44" s="16">
-        <v>0</v>
-      </c>
+      <c r="Z44" s="16"/>
       <c r="AA44" s="16">
-        <f>IF(ISBLANK(AB44),0, LOOKUP(AB44,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AC44/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AB44" s="16"/>
+        <v>0</v>
+      </c>
+      <c r="AB44" s="16">
+        <f>IF(ISBLANK(AC44),0, LOOKUP(AC44,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AD44/100)</f>
+        <v>0</v>
+      </c>
       <c r="AC44" s="16"/>
-      <c r="AD44" s="16" t="s">
-        <v>24</v>
-      </c>
+      <c r="AD44" s="16"/>
       <c r="AE44" s="16" t="s">
         <v>24</v>
       </c>
       <c r="AF44" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG44" s="16" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="45" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A45" s="18">
         <v>21400008</v>
       </c>
@@ -8790,14 +8888,14 @@
         <v>273</v>
       </c>
       <c r="D45" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="E45" s="1">
         <v>4</v>
       </c>
       <c r="F45" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>50</v>
       </c>
       <c r="G45" s="17">
@@ -8831,41 +8929,44 @@
         <v>0</v>
       </c>
       <c r="Q45" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R45" s="16">
-        <f>I45+J45+ SUM(K45:Q45)*5+Z45+AA45</f>
+        <v>1</v>
+      </c>
+      <c r="S45" s="16">
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="S45" s="16"/>
       <c r="T45" s="16"/>
       <c r="U45" s="16"/>
-      <c r="V45" s="16" t="s">
+      <c r="V45" s="16"/>
+      <c r="W45" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="W45" s="16"/>
       <c r="X45" s="16"/>
       <c r="Y45" s="16"/>
-      <c r="Z45" s="16">
-        <v>0</v>
-      </c>
+      <c r="Z45" s="16"/>
       <c r="AA45" s="16">
-        <f>IF(ISBLANK(AB45),0, LOOKUP(AB45,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AC45/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AB45" s="16"/>
+        <v>0</v>
+      </c>
+      <c r="AB45" s="16">
+        <f>IF(ISBLANK(AC45),0, LOOKUP(AC45,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AD45/100)</f>
+        <v>0</v>
+      </c>
       <c r="AC45" s="16"/>
-      <c r="AD45" s="16" t="s">
-        <v>24</v>
-      </c>
+      <c r="AD45" s="16"/>
       <c r="AE45" s="16" t="s">
         <v>24</v>
       </c>
       <c r="AF45" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG45" s="16" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="46" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A46">
         <v>21400009</v>
       </c>
@@ -8876,14 +8977,14 @@
         <v>248</v>
       </c>
       <c r="D46" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="E46" s="1">
         <v>4</v>
       </c>
       <c r="F46" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>150</v>
       </c>
       <c r="G46" s="17">
@@ -8899,11 +9000,11 @@
         <v>3</v>
       </c>
       <c r="K46" s="16">
+        <v>0</v>
+      </c>
+      <c r="L46" s="16">
         <v>2</v>
       </c>
-      <c r="L46" s="16">
-        <v>0</v>
-      </c>
       <c r="M46" s="16">
         <v>0</v>
       </c>
@@ -8920,38 +9021,41 @@
         <v>0</v>
       </c>
       <c r="R46" s="16">
-        <f>I46+J46+ SUM(K46:Q46)*5+Z46+AA46</f>
+        <v>0</v>
+      </c>
+      <c r="S46" s="16">
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
-      <c r="S46" s="16"/>
       <c r="T46" s="16"/>
       <c r="U46" s="16"/>
-      <c r="V46" s="16" t="s">
+      <c r="V46" s="16"/>
+      <c r="W46" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="W46" s="16"/>
       <c r="X46" s="16"/>
       <c r="Y46" s="16"/>
-      <c r="Z46" s="16">
-        <v>0</v>
-      </c>
+      <c r="Z46" s="16"/>
       <c r="AA46" s="16">
-        <f>IF(ISBLANK(AB46),0, LOOKUP(AB46,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AC46/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AB46" s="16"/>
+        <v>0</v>
+      </c>
+      <c r="AB46" s="16">
+        <f>IF(ISBLANK(AC46),0, LOOKUP(AC46,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AD46/100)</f>
+        <v>0</v>
+      </c>
       <c r="AC46" s="16"/>
-      <c r="AD46" s="16" t="s">
-        <v>24</v>
-      </c>
+      <c r="AD46" s="16"/>
       <c r="AE46" s="16" t="s">
         <v>24</v>
       </c>
       <c r="AF46" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG46" s="16" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="47" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A47">
         <v>21400010</v>
       </c>
@@ -8962,14 +9066,14 @@
         <v>249</v>
       </c>
       <c r="D47" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="E47" s="1">
         <v>4</v>
       </c>
       <c r="F47" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>150</v>
       </c>
       <c r="G47" s="17">
@@ -8988,11 +9092,11 @@
         <v>0</v>
       </c>
       <c r="L47" s="16">
+        <v>0</v>
+      </c>
+      <c r="M47" s="16">
         <v>3</v>
       </c>
-      <c r="M47" s="16">
-        <v>0</v>
-      </c>
       <c r="N47" s="16">
         <v>0</v>
       </c>
@@ -9006,38 +9110,41 @@
         <v>0</v>
       </c>
       <c r="R47" s="16">
-        <f>I47+J47+ SUM(K47:Q47)*5+Z47+AA47</f>
+        <v>0</v>
+      </c>
+      <c r="S47" s="16">
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
-      <c r="S47" s="16"/>
       <c r="T47" s="16"/>
       <c r="U47" s="16"/>
-      <c r="V47" s="16" t="s">
+      <c r="V47" s="16"/>
+      <c r="W47" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="W47" s="16"/>
       <c r="X47" s="16"/>
       <c r="Y47" s="16"/>
-      <c r="Z47" s="16">
-        <v>0</v>
-      </c>
+      <c r="Z47" s="16"/>
       <c r="AA47" s="16">
-        <f>IF(ISBLANK(AB47),0, LOOKUP(AB47,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AC47/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AB47" s="16"/>
+        <v>0</v>
+      </c>
+      <c r="AB47" s="16">
+        <f>IF(ISBLANK(AC47),0, LOOKUP(AC47,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AD47/100)</f>
+        <v>0</v>
+      </c>
       <c r="AC47" s="16"/>
-      <c r="AD47" s="16" t="s">
-        <v>24</v>
-      </c>
+      <c r="AD47" s="16"/>
       <c r="AE47" s="16" t="s">
         <v>24</v>
       </c>
       <c r="AF47" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG47" s="16" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="48" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A48">
         <v>21400011</v>
       </c>
@@ -9048,14 +9155,14 @@
         <v>250</v>
       </c>
       <c r="D48" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="E48" s="1">
         <v>4</v>
       </c>
       <c r="F48" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>250</v>
       </c>
       <c r="G48" s="17">
@@ -9071,11 +9178,11 @@
         <v>5</v>
       </c>
       <c r="K48" s="16">
+        <v>0</v>
+      </c>
+      <c r="L48" s="16">
         <v>3</v>
       </c>
-      <c r="L48" s="16">
-        <v>0</v>
-      </c>
       <c r="M48" s="16">
         <v>0</v>
       </c>
@@ -9083,47 +9190,50 @@
         <v>0</v>
       </c>
       <c r="O48" s="16">
+        <v>0</v>
+      </c>
+      <c r="P48" s="16">
         <v>2</v>
       </c>
-      <c r="P48" s="16">
-        <v>0</v>
-      </c>
       <c r="Q48" s="16">
         <v>0</v>
       </c>
       <c r="R48" s="16">
-        <f>I48+J48+ SUM(K48:Q48)*5+Z48+AA48</f>
+        <v>0</v>
+      </c>
+      <c r="S48" s="16">
+        <f t="shared" si="2"/>
         <v>30</v>
       </c>
-      <c r="S48" s="16"/>
       <c r="T48" s="16"/>
       <c r="U48" s="16"/>
-      <c r="V48" s="16" t="s">
+      <c r="V48" s="16"/>
+      <c r="W48" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="W48" s="16"/>
       <c r="X48" s="16"/>
       <c r="Y48" s="16"/>
-      <c r="Z48" s="16">
-        <v>0</v>
-      </c>
+      <c r="Z48" s="16"/>
       <c r="AA48" s="16">
-        <f>IF(ISBLANK(AB48),0, LOOKUP(AB48,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AC48/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AB48" s="16"/>
+        <v>0</v>
+      </c>
+      <c r="AB48" s="16">
+        <f>IF(ISBLANK(AC48),0, LOOKUP(AC48,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AD48/100)</f>
+        <v>0</v>
+      </c>
       <c r="AC48" s="16"/>
-      <c r="AD48" s="16" t="s">
-        <v>24</v>
-      </c>
+      <c r="AD48" s="16"/>
       <c r="AE48" s="16" t="s">
         <v>24</v>
       </c>
       <c r="AF48" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG48" s="16" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="49" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A49" s="18">
         <v>21500001</v>
       </c>
@@ -9134,14 +9244,14 @@
         <v>262</v>
       </c>
       <c r="D49" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="E49" s="1">
         <v>5</v>
       </c>
       <c r="F49" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="G49" s="17">
@@ -9178,40 +9288,43 @@
         <v>0</v>
       </c>
       <c r="R49" s="16">
-        <f>I49+J49+ SUM(K49:Q49)*5+Z49+AA49</f>
+        <v>0</v>
+      </c>
+      <c r="S49" s="16">
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="S49" s="16">
+      <c r="T49" s="16">
         <v>5</v>
       </c>
-      <c r="T49" s="16"/>
       <c r="U49" s="16"/>
-      <c r="V49" s="16" t="s">
+      <c r="V49" s="16"/>
+      <c r="W49" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="W49" s="16"/>
       <c r="X49" s="16"/>
       <c r="Y49" s="16"/>
-      <c r="Z49" s="16">
+      <c r="Z49" s="16"/>
+      <c r="AA49" s="16">
         <v>10</v>
       </c>
-      <c r="AA49" s="16">
-        <f>IF(ISBLANK(AB49),0, LOOKUP(AB49,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AC49/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AB49" s="16"/>
+      <c r="AB49" s="16">
+        <f>IF(ISBLANK(AC49),0, LOOKUP(AC49,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AD49/100)</f>
+        <v>0</v>
+      </c>
       <c r="AC49" s="16"/>
-      <c r="AD49" s="16" t="s">
-        <v>24</v>
-      </c>
+      <c r="AD49" s="16"/>
       <c r="AE49" s="16" t="s">
         <v>24</v>
       </c>
       <c r="AF49" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG49" s="16" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="50" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A50" s="18">
         <v>21500002</v>
       </c>
@@ -9222,14 +9335,14 @@
         <v>251</v>
       </c>
       <c r="D50" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="E50" s="1">
         <v>5</v>
       </c>
       <c r="F50" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="G50" s="17">
@@ -9248,10 +9361,10 @@
         <v>0</v>
       </c>
       <c r="L50" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M50" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N50" s="16">
         <v>0</v>
@@ -9266,40 +9379,43 @@
         <v>0</v>
       </c>
       <c r="R50" s="16">
-        <f>I50+J50+ SUM(K50:Q50)*5+Z50+AA50</f>
+        <v>0</v>
+      </c>
+      <c r="S50" s="16">
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="S50" s="16"/>
       <c r="T50" s="16"/>
       <c r="U50" s="16"/>
-      <c r="V50" s="16" t="s">
+      <c r="V50" s="16"/>
+      <c r="W50" s="16" t="s">
         <v>109</v>
       </c>
-      <c r="W50" s="16" t="s">
+      <c r="X50" s="16" t="s">
         <v>266</v>
       </c>
-      <c r="X50" s="16"/>
       <c r="Y50" s="16"/>
-      <c r="Z50" s="16">
+      <c r="Z50" s="16"/>
+      <c r="AA50" s="16">
         <v>5</v>
       </c>
-      <c r="AA50" s="16">
-        <f>IF(ISBLANK(AB50),0, LOOKUP(AB50,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AC50/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AB50" s="16"/>
+      <c r="AB50" s="16">
+        <f>IF(ISBLANK(AC50),0, LOOKUP(AC50,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AD50/100)</f>
+        <v>0</v>
+      </c>
       <c r="AC50" s="16"/>
-      <c r="AD50" s="16" t="s">
-        <v>24</v>
-      </c>
+      <c r="AD50" s="16"/>
       <c r="AE50" s="16" t="s">
         <v>24</v>
       </c>
       <c r="AF50" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG50" s="16" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="51" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A51" s="18">
         <v>21500003</v>
       </c>
@@ -9310,14 +9426,14 @@
         <v>252</v>
       </c>
       <c r="D51" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="E51" s="1">
         <v>5</v>
       </c>
       <c r="F51" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="G51" s="17">
@@ -9342,10 +9458,10 @@
         <v>0</v>
       </c>
       <c r="N51" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O51" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P51" s="16">
         <v>0</v>
@@ -9354,40 +9470,43 @@
         <v>0</v>
       </c>
       <c r="R51" s="16">
-        <f>I51+J51+ SUM(K51:Q51)*5+Z51+AA51</f>
+        <v>0</v>
+      </c>
+      <c r="S51" s="16">
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
-      <c r="S51" s="16"/>
       <c r="T51" s="16"/>
       <c r="U51" s="16"/>
-      <c r="V51" s="16" t="s">
+      <c r="V51" s="16"/>
+      <c r="W51" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="W51" s="16" t="s">
+      <c r="X51" s="16" t="s">
         <v>267</v>
       </c>
-      <c r="X51" s="16"/>
       <c r="Y51" s="16"/>
-      <c r="Z51" s="16">
+      <c r="Z51" s="16"/>
+      <c r="AA51" s="16">
         <v>6</v>
       </c>
-      <c r="AA51" s="16">
-        <f>IF(ISBLANK(AB51),0, LOOKUP(AB51,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AC51/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AB51" s="16"/>
+      <c r="AB51" s="16">
+        <f>IF(ISBLANK(AC51),0, LOOKUP(AC51,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AD51/100)</f>
+        <v>0</v>
+      </c>
       <c r="AC51" s="16"/>
-      <c r="AD51" s="16" t="s">
-        <v>24</v>
-      </c>
+      <c r="AD51" s="16"/>
       <c r="AE51" s="16" t="s">
         <v>24</v>
       </c>
       <c r="AF51" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG51" s="16" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="52" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A52" s="18">
         <v>21500004</v>
       </c>
@@ -9398,14 +9517,14 @@
         <v>253</v>
       </c>
       <c r="D52" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="E52" s="1">
         <v>5</v>
       </c>
       <c r="F52" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="G52" s="17">
@@ -9442,42 +9561,45 @@
         <v>0</v>
       </c>
       <c r="R52" s="16">
-        <f>I52+J52+ SUM(K52:Q52)*5+Z52+AA52</f>
+        <v>0</v>
+      </c>
+      <c r="S52" s="16">
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="S52" s="16"/>
       <c r="T52" s="16"/>
       <c r="U52" s="16"/>
-      <c r="V52" s="16" t="s">
+      <c r="V52" s="16"/>
+      <c r="W52" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="W52" s="16"/>
       <c r="X52" s="16"/>
       <c r="Y52" s="16"/>
-      <c r="Z52" s="16">
-        <v>0</v>
-      </c>
+      <c r="Z52" s="16"/>
       <c r="AA52" s="16">
-        <f>IF(ISBLANK(AB52),0, LOOKUP(AB52,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AC52/100)</f>
+        <v>0</v>
+      </c>
+      <c r="AB52" s="16">
+        <f>IF(ISBLANK(AC52),0, LOOKUP(AC52,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AD52/100)</f>
         <v>4</v>
       </c>
-      <c r="AB52" s="16">
+      <c r="AC52" s="16">
         <v>55990108</v>
       </c>
-      <c r="AC52" s="16">
+      <c r="AD52" s="16">
         <v>100</v>
       </c>
-      <c r="AD52" s="16" t="s">
-        <v>24</v>
-      </c>
       <c r="AE52" s="16" t="s">
         <v>24</v>
       </c>
       <c r="AF52" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG52" s="16" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="53" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A53">
         <v>21500005</v>
       </c>
@@ -9488,14 +9610,14 @@
         <v>254</v>
       </c>
       <c r="D53" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="E53" s="1">
         <v>5</v>
       </c>
       <c r="F53" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>150</v>
       </c>
       <c r="G53" s="17">
@@ -9529,43 +9651,46 @@
         <v>0</v>
       </c>
       <c r="Q53" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R53" s="16">
-        <f>I53+J53+ SUM(K53:Q53)*5+Z53+AA53</f>
+        <v>1</v>
+      </c>
+      <c r="S53" s="16">
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
-      <c r="S53" s="16"/>
       <c r="T53" s="16"/>
       <c r="U53" s="16"/>
-      <c r="V53" s="16" t="s">
+      <c r="V53" s="16"/>
+      <c r="W53" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="W53" s="16" t="s">
+      <c r="X53" s="16" t="s">
         <v>268</v>
       </c>
-      <c r="X53" s="16"/>
       <c r="Y53" s="16"/>
-      <c r="Z53" s="16">
+      <c r="Z53" s="16"/>
+      <c r="AA53" s="16">
         <v>10</v>
       </c>
-      <c r="AA53" s="16">
-        <f>IF(ISBLANK(AB53),0, LOOKUP(AB53,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AC53/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AB53" s="16"/>
+      <c r="AB53" s="16">
+        <f>IF(ISBLANK(AC53),0, LOOKUP(AC53,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AD53/100)</f>
+        <v>0</v>
+      </c>
       <c r="AC53" s="16"/>
-      <c r="AD53" s="16" t="s">
-        <v>24</v>
-      </c>
+      <c r="AD53" s="16"/>
       <c r="AE53" s="16" t="s">
         <v>24</v>
       </c>
       <c r="AF53" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG53" s="16" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="54" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A54">
         <v>21500006</v>
       </c>
@@ -9576,14 +9701,14 @@
         <v>255</v>
       </c>
       <c r="D54" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="E54" s="1">
         <v>5</v>
       </c>
       <c r="F54" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>150</v>
       </c>
       <c r="G54" s="17">
@@ -9620,42 +9745,45 @@
         <v>0</v>
       </c>
       <c r="R54" s="16">
-        <f>I54+J54+ SUM(K54:Q54)*5+Z54+AA54</f>
+        <v>0</v>
+      </c>
+      <c r="S54" s="16">
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
-      <c r="S54" s="16"/>
       <c r="T54" s="16"/>
       <c r="U54" s="16"/>
-      <c r="V54" s="16" t="s">
+      <c r="V54" s="16"/>
+      <c r="W54" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="W54" s="16"/>
       <c r="X54" s="16"/>
       <c r="Y54" s="16"/>
-      <c r="Z54" s="16">
-        <v>0</v>
-      </c>
+      <c r="Z54" s="16"/>
       <c r="AA54" s="16">
-        <f>IF(ISBLANK(AB54),0, LOOKUP(AB54,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AC54/100)</f>
+        <v>0</v>
+      </c>
+      <c r="AB54" s="16">
+        <f>IF(ISBLANK(AC54),0, LOOKUP(AC54,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AD54/100)</f>
         <v>15</v>
       </c>
-      <c r="AB54" s="16">
+      <c r="AC54" s="16">
         <v>55990109</v>
       </c>
-      <c r="AC54" s="16">
+      <c r="AD54" s="16">
         <v>100</v>
       </c>
-      <c r="AD54" s="16" t="s">
-        <v>24</v>
-      </c>
       <c r="AE54" s="16" t="s">
         <v>24</v>
       </c>
       <c r="AF54" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG54" s="16" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="55" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A55" s="18">
         <v>21500007</v>
       </c>
@@ -9666,14 +9794,14 @@
         <v>256</v>
       </c>
       <c r="D55" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="E55" s="1">
         <v>5</v>
       </c>
       <c r="F55" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="G55" s="17">
@@ -9710,38 +9838,41 @@
         <v>0</v>
       </c>
       <c r="R55" s="16">
-        <f>I55+J55+ SUM(K55:Q55)*5+Z55+AA55</f>
+        <v>0</v>
+      </c>
+      <c r="S55" s="16">
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="S55" s="16"/>
       <c r="T55" s="16"/>
       <c r="U55" s="16"/>
-      <c r="V55" s="16" t="s">
+      <c r="V55" s="16"/>
+      <c r="W55" s="16" t="s">
         <v>146</v>
       </c>
-      <c r="W55" s="16"/>
       <c r="X55" s="16"/>
       <c r="Y55" s="16"/>
-      <c r="Z55" s="16">
+      <c r="Z55" s="16"/>
+      <c r="AA55" s="16">
         <v>8</v>
       </c>
-      <c r="AA55" s="16">
-        <f>IF(ISBLANK(AB55),0, LOOKUP(AB55,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AC55/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AB55" s="16"/>
+      <c r="AB55" s="16">
+        <f>IF(ISBLANK(AC55),0, LOOKUP(AC55,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AD55/100)</f>
+        <v>0</v>
+      </c>
       <c r="AC55" s="16"/>
-      <c r="AD55" s="16" t="s">
-        <v>24</v>
-      </c>
+      <c r="AD55" s="16"/>
       <c r="AE55" s="16" t="s">
         <v>24</v>
       </c>
       <c r="AF55" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG55" s="16" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="56" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A56">
         <v>21500008</v>
       </c>
@@ -9752,14 +9883,14 @@
         <v>257</v>
       </c>
       <c r="D56" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="E56" s="1">
         <v>5</v>
       </c>
       <c r="F56" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>250</v>
       </c>
       <c r="G56" s="17">
@@ -9784,11 +9915,11 @@
         <v>0</v>
       </c>
       <c r="N56" s="16">
+        <v>0</v>
+      </c>
+      <c r="O56" s="16">
         <v>3</v>
       </c>
-      <c r="O56" s="16">
-        <v>0</v>
-      </c>
       <c r="P56" s="16">
         <v>0</v>
       </c>
@@ -9796,42 +9927,45 @@
         <v>0</v>
       </c>
       <c r="R56" s="16">
-        <f>I56+J56+ SUM(K56:Q56)*5+Z56+AA56</f>
+        <v>0</v>
+      </c>
+      <c r="S56" s="16">
+        <f t="shared" si="2"/>
         <v>25</v>
       </c>
-      <c r="S56" s="16"/>
       <c r="T56" s="16"/>
       <c r="U56" s="16"/>
-      <c r="V56" s="16" t="s">
+      <c r="V56" s="16"/>
+      <c r="W56" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="W56" s="16"/>
       <c r="X56" s="16"/>
       <c r="Y56" s="16"/>
-      <c r="Z56" s="16">
-        <v>0</v>
-      </c>
+      <c r="Z56" s="16"/>
       <c r="AA56" s="16">
-        <f>IF(ISBLANK(AB56),0, LOOKUP(AB56,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AC56/100)</f>
+        <v>0</v>
+      </c>
+      <c r="AB56" s="16">
+        <f>IF(ISBLANK(AC56),0, LOOKUP(AC56,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AD56/100)</f>
         <v>10</v>
       </c>
-      <c r="AB56" s="16">
+      <c r="AC56" s="16">
         <v>55110003</v>
       </c>
-      <c r="AC56" s="16">
+      <c r="AD56" s="16">
         <v>40</v>
       </c>
-      <c r="AD56" s="16" t="s">
-        <v>24</v>
-      </c>
       <c r="AE56" s="16" t="s">
         <v>24</v>
       </c>
       <c r="AF56" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG56" s="16" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="57" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A57" s="18">
         <v>21500009</v>
       </c>
@@ -9842,14 +9976,14 @@
         <v>258</v>
       </c>
       <c r="D57" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="E57" s="1">
         <v>5</v>
       </c>
       <c r="F57" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="G57" s="17">
@@ -9886,40 +10020,43 @@
         <v>0</v>
       </c>
       <c r="R57" s="16">
-        <f>I57+J57+ SUM(K57:Q57)*5+Z57+AA57</f>
+        <v>0</v>
+      </c>
+      <c r="S57" s="16">
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="S57" s="16"/>
       <c r="T57" s="16"/>
       <c r="U57" s="16"/>
-      <c r="V57" s="16" t="s">
+      <c r="V57" s="16"/>
+      <c r="W57" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="W57" s="16"/>
-      <c r="X57" s="16">
+      <c r="X57" s="16"/>
+      <c r="Y57" s="16">
         <v>31100001</v>
       </c>
-      <c r="Y57" s="16"/>
-      <c r="Z57" s="16">
+      <c r="Z57" s="16"/>
+      <c r="AA57" s="16">
         <v>10</v>
       </c>
-      <c r="AA57" s="16">
-        <f>IF(ISBLANK(AB57),0, LOOKUP(AB57,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AC57/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AB57" s="16"/>
+      <c r="AB57" s="16">
+        <f>IF(ISBLANK(AC57),0, LOOKUP(AC57,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AD57/100)</f>
+        <v>0</v>
+      </c>
       <c r="AC57" s="16"/>
-      <c r="AD57" s="16" t="s">
-        <v>24</v>
-      </c>
+      <c r="AD57" s="16"/>
       <c r="AE57" s="16" t="s">
         <v>24</v>
       </c>
       <c r="AF57" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG57" s="16" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="58" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A58">
         <v>21500010</v>
       </c>
@@ -9930,14 +10067,14 @@
         <v>259</v>
       </c>
       <c r="D58" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="E58" s="1">
         <v>5</v>
       </c>
       <c r="F58" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>150</v>
       </c>
       <c r="G58" s="17">
@@ -9974,42 +10111,45 @@
         <v>0</v>
       </c>
       <c r="R58" s="16">
-        <f>I58+J58+ SUM(K58:Q58)*5+Z58+AA58</f>
+        <v>0</v>
+      </c>
+      <c r="S58" s="16">
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
-      <c r="S58" s="16"/>
       <c r="T58" s="16"/>
       <c r="U58" s="16"/>
-      <c r="V58" s="16" t="s">
+      <c r="V58" s="16"/>
+      <c r="W58" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="W58" s="16" t="s">
+      <c r="X58" s="16" t="s">
         <v>269</v>
       </c>
-      <c r="X58" s="16">
+      <c r="Y58" s="16">
         <v>31100002</v>
       </c>
-      <c r="Y58" s="16"/>
-      <c r="Z58" s="16">
+      <c r="Z58" s="16"/>
+      <c r="AA58" s="16">
         <v>15</v>
       </c>
-      <c r="AA58" s="16">
-        <f>IF(ISBLANK(AB58),0, LOOKUP(AB58,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AC58/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AB58" s="16"/>
+      <c r="AB58" s="16">
+        <f>IF(ISBLANK(AC58),0, LOOKUP(AC58,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AD58/100)</f>
+        <v>0</v>
+      </c>
       <c r="AC58" s="16"/>
-      <c r="AD58" s="16" t="s">
-        <v>24</v>
-      </c>
+      <c r="AD58" s="16"/>
       <c r="AE58" s="16" t="s">
         <v>24</v>
       </c>
       <c r="AF58" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG58" s="16" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="59" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A59">
         <v>21500011</v>
       </c>
@@ -10020,14 +10160,14 @@
         <v>260</v>
       </c>
       <c r="D59" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="E59" s="1">
         <v>5</v>
       </c>
       <c r="F59" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>250</v>
       </c>
       <c r="G59" s="17">
@@ -10064,60 +10204,63 @@
         <v>0</v>
       </c>
       <c r="R59" s="16">
-        <f>I59+J59+ SUM(K59:Q59)*5+Z59+AA59</f>
+        <v>0</v>
+      </c>
+      <c r="S59" s="16">
+        <f t="shared" si="2"/>
         <v>25</v>
       </c>
-      <c r="S59" s="16"/>
       <c r="T59" s="16"/>
       <c r="U59" s="16"/>
-      <c r="V59" s="16" t="s">
+      <c r="V59" s="16"/>
+      <c r="W59" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="W59" s="16"/>
-      <c r="X59" s="16">
+      <c r="X59" s="16"/>
+      <c r="Y59" s="16">
         <v>31100003</v>
       </c>
-      <c r="Y59" s="16"/>
-      <c r="Z59" s="16">
+      <c r="Z59" s="16"/>
+      <c r="AA59" s="16">
         <v>25</v>
       </c>
-      <c r="AA59" s="16">
-        <f>IF(ISBLANK(AB59),0, LOOKUP(AB59,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AC59/100)</f>
-        <v>0</v>
-      </c>
-      <c r="AB59" s="16"/>
+      <c r="AB59" s="16">
+        <f>IF(ISBLANK(AC59),0, LOOKUP(AC59,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AD59/100)</f>
+        <v>0</v>
+      </c>
       <c r="AC59" s="16"/>
-      <c r="AD59" s="16" t="s">
-        <v>24</v>
-      </c>
+      <c r="AD59" s="16"/>
       <c r="AE59" s="16" t="s">
         <v>24</v>
       </c>
       <c r="AF59" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG59" s="16" t="s">
         <v>204</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="D4:D59">
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="greaterThanOrEqual">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="9" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="10" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="11" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H4:AF18 H29:AF59 H19:X28 Z19:AF28">
-    <cfRule type="containsBlanks" dxfId="0" priority="1">
+  <conditionalFormatting sqref="H4:AG4 AA19:AG28 T5:AG18 T29:AG59 T19:Y28 H5:S59">
+    <cfRule type="containsBlanks" dxfId="2" priority="1">
       <formula>LEN(TRIM(H4))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
new merge form mechanical
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Equip.xlsx
+++ b/ConfigData/Xlsx/Equip.xlsx
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="283">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -1011,14 +1011,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>合成消耗道具</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>ComposeItemId</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>eqcaowu</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -1035,95 +1027,10 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>int[]</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>合成材料</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>22100401;22100401</t>
-  </si>
-  <si>
-    <t>22100403;22100401</t>
-  </si>
-  <si>
-    <t>22100205;22100401</t>
-  </si>
-  <si>
-    <t>22100406;22100401</t>
-  </si>
-  <si>
-    <t>22100206;22100401</t>
-  </si>
-  <si>
-    <t>22100208;22100401</t>
-  </si>
-  <si>
-    <t>22100214;22100401</t>
-  </si>
-  <si>
-    <t>22100218;22100401</t>
-  </si>
-  <si>
-    <t>22100210;22100401</t>
-  </si>
-  <si>
-    <t>22100201;22100401</t>
-  </si>
-  <si>
-    <t>22100207;22100401</t>
-  </si>
-  <si>
-    <t>22100213;22100401</t>
-  </si>
-  <si>
-    <t>22100219;22100401</t>
-  </si>
-  <si>
-    <t>22100405;22100401</t>
-  </si>
-  <si>
-    <t>22100416;22100401</t>
-  </si>
-  <si>
-    <t>22100404;22100401</t>
-  </si>
-  <si>
-    <t>22100410;22100401</t>
-  </si>
-  <si>
-    <t>22100412;22100401</t>
-  </si>
-  <si>
-    <t>22100402;22100401</t>
-  </si>
-  <si>
-    <t>22100415;22100401</t>
-  </si>
-  <si>
-    <t>22100407;22100401</t>
-  </si>
-  <si>
-    <t>22100408;22100401</t>
-  </si>
-  <si>
-    <t>22100411;22100401</t>
-  </si>
-  <si>
-    <t>22100202;22100401</t>
-  </si>
-  <si>
-    <t>22100414;22100401</t>
-  </si>
-  <si>
-    <t>22100209;22100401</t>
-  </si>
-  <si>
-    <t>22100215;22100401</t>
-  </si>
-  <si>
     <t>AtkP</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -1149,6 +1056,18 @@
   </si>
   <si>
     <t>Attr</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>最大等级</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>MaxLevel</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1970,6 +1889,25 @@
   </cellStyles>
   <dxfs count="35">
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FF00B050"/>
@@ -2484,25 +2422,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
         <scheme val="minor"/>
       </font>
       <fill>
@@ -4413,37 +4332,37 @@
       <calculatedColumnFormula>IF(R4&gt;=23,4,IF(AND(R4&gt;=18,R4&lt;23),3,IF(AND(R4&gt;=13,R4&lt;18),2,IF(AND(R4&gt;=8,R4&lt;13),1,0))))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" name="Position"/>
+    <tableColumn id="15" name="MaxLevel" dataDxfId="0"/>
     <tableColumn id="7" name="ComposeRes" dataDxfId="32"/>
-    <tableColumn id="15" name="ComposeItemId" dataDxfId="31"/>
-    <tableColumn id="11" name="AtkP" dataDxfId="30"/>
-    <tableColumn id="8" name="VitP" dataDxfId="29"/>
-    <tableColumn id="30" name="Attr" dataDxfId="28"/>
-    <tableColumn id="6" name="Def" dataDxfId="27"/>
-    <tableColumn id="22" name="Mag" dataDxfId="26"/>
-    <tableColumn id="27" name="Spd" dataDxfId="25"/>
-    <tableColumn id="26" name="Hit" dataDxfId="24"/>
-    <tableColumn id="25" name="Dhit" dataDxfId="23"/>
-    <tableColumn id="24" name="Crt" dataDxfId="22"/>
-    <tableColumn id="23" name="Luk" dataDxfId="21"/>
-    <tableColumn id="28" name="Sum" dataDxfId="20">
+    <tableColumn id="11" name="AtkP" dataDxfId="31"/>
+    <tableColumn id="8" name="VitP" dataDxfId="30"/>
+    <tableColumn id="30" name="Attr" dataDxfId="29"/>
+    <tableColumn id="6" name="Def" dataDxfId="28"/>
+    <tableColumn id="22" name="Mag" dataDxfId="27"/>
+    <tableColumn id="27" name="Spd" dataDxfId="26"/>
+    <tableColumn id="26" name="Hit" dataDxfId="25"/>
+    <tableColumn id="25" name="Dhit" dataDxfId="24"/>
+    <tableColumn id="24" name="Crt" dataDxfId="23"/>
+    <tableColumn id="23" name="Luk" dataDxfId="22"/>
+    <tableColumn id="28" name="Sum" dataDxfId="21">
       <calculatedColumnFormula>H4+I4+J4+ SUM(K4:Q4)*5+Z4+AA4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="Range" dataDxfId="19"/>
-    <tableColumn id="33" name="Arrow" dataDxfId="18"/>
-    <tableColumn id="4" name="SlotId" dataDxfId="17"/>
-    <tableColumn id="9" name="EnergyRate" dataDxfId="16"/>
-    <tableColumn id="37" name="DungeonAttrs" dataDxfId="15"/>
-    <tableColumn id="20" name="HeroSkillId" dataDxfId="14"/>
-    <tableColumn id="29" name="AttrId" dataDxfId="13"/>
-    <tableColumn id="21" name="~SkillMark2" dataDxfId="12"/>
-    <tableColumn id="18" name="~SkillMark22" dataDxfId="11">
+    <tableColumn id="12" name="Range" dataDxfId="20"/>
+    <tableColumn id="33" name="Arrow" dataDxfId="19"/>
+    <tableColumn id="4" name="SlotId" dataDxfId="18"/>
+    <tableColumn id="9" name="EnergyRate" dataDxfId="17"/>
+    <tableColumn id="37" name="DungeonAttrs" dataDxfId="16"/>
+    <tableColumn id="20" name="HeroSkillId" dataDxfId="15"/>
+    <tableColumn id="29" name="AttrId" dataDxfId="14"/>
+    <tableColumn id="21" name="~SkillMark2" dataDxfId="13"/>
+    <tableColumn id="18" name="~SkillMark22" dataDxfId="12">
       <calculatedColumnFormula>IF(ISBLANK(AB4),0, LOOKUP(AB4,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AC4/100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="CommonSkillId" dataDxfId="10"/>
-    <tableColumn id="14" name="CommonSkillRate" dataDxfId="9"/>
-    <tableColumn id="17" name="RandomDrop" dataDxfId="8"/>
-    <tableColumn id="16" name="CanMerge" dataDxfId="7"/>
-    <tableColumn id="10" name="Url" dataDxfId="6"/>
+    <tableColumn id="13" name="CommonSkillId" dataDxfId="11"/>
+    <tableColumn id="14" name="CommonSkillRate" dataDxfId="10"/>
+    <tableColumn id="17" name="RandomDrop" dataDxfId="9"/>
+    <tableColumn id="16" name="CanMerge" dataDxfId="8"/>
+    <tableColumn id="10" name="Url" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4772,16 +4691,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="F52" sqref="F52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="5.5" customWidth="1"/>
-    <col min="6" max="6" width="6" customWidth="1"/>
-    <col min="7" max="7" width="19" customWidth="1"/>
+    <col min="4" max="6" width="5.5" customWidth="1"/>
+    <col min="7" max="7" width="6" customWidth="1"/>
     <col min="8" max="10" width="5.125" customWidth="1"/>
     <col min="11" max="18" width="4.5" customWidth="1"/>
     <col min="19" max="20" width="5.125" customWidth="1"/>
@@ -4813,10 +4731,10 @@
         <v>5</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>275</v>
+        <v>280</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="H1" s="12" t="s">
         <v>12</v>
@@ -4825,7 +4743,7 @@
         <v>14</v>
       </c>
       <c r="J1" s="12" t="s">
-        <v>307</v>
+        <v>277</v>
       </c>
       <c r="K1" s="13" t="s">
         <v>40</v>
@@ -4870,7 +4788,7 @@
         <v>36</v>
       </c>
       <c r="Y1" s="15" t="s">
-        <v>305</v>
+        <v>275</v>
       </c>
       <c r="Z1" s="15" t="s">
         <v>32</v>
@@ -4911,10 +4829,10 @@
         <v>0</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>274</v>
+        <v>281</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>13</v>
@@ -4923,7 +4841,7 @@
         <v>15</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>308</v>
+        <v>278</v>
       </c>
       <c r="K2" s="9" t="s">
         <v>0</v>
@@ -5009,19 +4927,19 @@
         <v>10</v>
       </c>
       <c r="F3" t="s">
+        <v>282</v>
+      </c>
+      <c r="G3" t="s">
+        <v>271</v>
+      </c>
+      <c r="H3" s="4" t="s">
         <v>273</v>
       </c>
-      <c r="G3" t="s">
-        <v>269</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>303</v>
-      </c>
       <c r="I3" s="4" t="s">
-        <v>304</v>
+        <v>274</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>309</v>
+        <v>279</v>
       </c>
       <c r="K3" s="10" t="s">
         <v>48</v>
@@ -5066,7 +4984,7 @@
         <v>19</v>
       </c>
       <c r="Y3" s="8" t="s">
-        <v>306</v>
+        <v>276</v>
       </c>
       <c r="Z3" s="8" t="s">
         <v>31</v>
@@ -5098,7 +5016,7 @@
         <v>60</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D4" s="1">
         <f t="shared" ref="D4:D35" si="0">IF(R4&gt;=23,4,IF(AND(R4&gt;=18,R4&lt;23),3,IF(AND(R4&gt;=13,R4&lt;18),2,IF(AND(R4&gt;=8,R4&lt;13),1,0))))</f>
@@ -5108,10 +5026,10 @@
         <v>1</v>
       </c>
       <c r="F4" s="17">
+        <v>10</v>
+      </c>
+      <c r="G4" s="17">
         <v>1</v>
-      </c>
-      <c r="G4" s="16" t="s">
-        <v>276</v>
       </c>
       <c r="H4" s="16"/>
       <c r="I4" s="16">
@@ -5177,10 +5095,10 @@
         <v>1</v>
       </c>
       <c r="F5" s="17">
+        <v>10</v>
+      </c>
+      <c r="G5" s="17">
         <v>2</v>
-      </c>
-      <c r="G5" s="16" t="s">
-        <v>277</v>
       </c>
       <c r="H5" s="16"/>
       <c r="I5" s="16">
@@ -5246,10 +5164,10 @@
         <v>1</v>
       </c>
       <c r="F6" s="17">
+        <v>10</v>
+      </c>
+      <c r="G6" s="17">
         <v>2</v>
-      </c>
-      <c r="G6" s="16" t="s">
-        <v>278</v>
       </c>
       <c r="H6" s="16"/>
       <c r="I6" s="16">
@@ -5315,10 +5233,10 @@
         <v>1</v>
       </c>
       <c r="F7" s="17">
+        <v>10</v>
+      </c>
+      <c r="G7" s="17">
         <v>2</v>
-      </c>
-      <c r="G7" s="16" t="s">
-        <v>279</v>
       </c>
       <c r="H7" s="16"/>
       <c r="I7" s="16">
@@ -5384,10 +5302,10 @@
         <v>1</v>
       </c>
       <c r="F8" s="17">
+        <v>10</v>
+      </c>
+      <c r="G8" s="17">
         <v>2</v>
-      </c>
-      <c r="G8" s="16" t="s">
-        <v>280</v>
       </c>
       <c r="H8" s="16"/>
       <c r="I8" s="16">
@@ -5455,10 +5373,10 @@
         <v>1</v>
       </c>
       <c r="F9" s="17">
+        <v>10</v>
+      </c>
+      <c r="G9" s="17">
         <v>2</v>
-      </c>
-      <c r="G9" s="16" t="s">
-        <v>281</v>
       </c>
       <c r="H9" s="16"/>
       <c r="I9" s="16">
@@ -5526,10 +5444,10 @@
         <v>1</v>
       </c>
       <c r="F10" s="17">
+        <v>10</v>
+      </c>
+      <c r="G10" s="17">
         <v>1</v>
-      </c>
-      <c r="G10" s="16" t="s">
-        <v>282</v>
       </c>
       <c r="H10" s="16"/>
       <c r="I10" s="16">
@@ -5597,10 +5515,10 @@
         <v>1</v>
       </c>
       <c r="F11" s="17">
+        <v>10</v>
+      </c>
+      <c r="G11" s="17">
         <v>2</v>
-      </c>
-      <c r="G11" s="16" t="s">
-        <v>283</v>
       </c>
       <c r="H11" s="16"/>
       <c r="I11" s="16">
@@ -5668,10 +5586,10 @@
         <v>1</v>
       </c>
       <c r="F12" s="17">
+        <v>10</v>
+      </c>
+      <c r="G12" s="17">
         <v>1</v>
-      </c>
-      <c r="G12" s="16" t="s">
-        <v>284</v>
       </c>
       <c r="H12" s="16"/>
       <c r="I12" s="16">
@@ -5739,10 +5657,10 @@
         <v>1</v>
       </c>
       <c r="F13" s="17">
+        <v>10</v>
+      </c>
+      <c r="G13" s="17">
         <v>2</v>
-      </c>
-      <c r="G13" s="16" t="s">
-        <v>285</v>
       </c>
       <c r="H13" s="16"/>
       <c r="I13" s="16">
@@ -5810,10 +5728,10 @@
         <v>1</v>
       </c>
       <c r="F14" s="17">
+        <v>10</v>
+      </c>
+      <c r="G14" s="17">
         <v>2</v>
-      </c>
-      <c r="G14" s="16" t="s">
-        <v>286</v>
       </c>
       <c r="H14" s="16"/>
       <c r="I14" s="16">
@@ -5881,10 +5799,10 @@
         <v>1</v>
       </c>
       <c r="F15" s="17">
+        <v>10</v>
+      </c>
+      <c r="G15" s="17">
         <v>1</v>
-      </c>
-      <c r="G15" s="16" t="s">
-        <v>287</v>
       </c>
       <c r="H15" s="16"/>
       <c r="I15" s="16">
@@ -5952,10 +5870,10 @@
         <v>1</v>
       </c>
       <c r="F16" s="17">
+        <v>10</v>
+      </c>
+      <c r="G16" s="17">
         <v>2</v>
-      </c>
-      <c r="G16" s="16" t="s">
-        <v>278</v>
       </c>
       <c r="H16" s="16"/>
       <c r="I16" s="16">
@@ -6023,10 +5941,10 @@
         <v>1</v>
       </c>
       <c r="F17" s="17">
+        <v>10</v>
+      </c>
+      <c r="G17" s="17">
         <v>1</v>
-      </c>
-      <c r="G17" s="16" t="s">
-        <v>276</v>
       </c>
       <c r="H17" s="16"/>
       <c r="I17" s="16">
@@ -6094,10 +6012,10 @@
         <v>1</v>
       </c>
       <c r="F18" s="17">
+        <v>10</v>
+      </c>
+      <c r="G18" s="17">
         <v>2</v>
-      </c>
-      <c r="G18" s="16" t="s">
-        <v>288</v>
       </c>
       <c r="H18" s="16"/>
       <c r="I18" s="16">
@@ -6163,10 +6081,10 @@
         <v>2</v>
       </c>
       <c r="F19" s="17">
+        <v>10</v>
+      </c>
+      <c r="G19" s="17">
         <v>1</v>
-      </c>
-      <c r="G19" s="16" t="s">
-        <v>279</v>
       </c>
       <c r="H19" s="16"/>
       <c r="I19" s="16"/>
@@ -6232,10 +6150,10 @@
         <v>2</v>
       </c>
       <c r="F20" s="17">
+        <v>10</v>
+      </c>
+      <c r="G20" s="17">
         <v>1</v>
-      </c>
-      <c r="G20" s="16" t="s">
-        <v>289</v>
       </c>
       <c r="H20" s="16"/>
       <c r="I20" s="16"/>
@@ -6301,10 +6219,10 @@
         <v>2</v>
       </c>
       <c r="F21" s="17">
+        <v>10</v>
+      </c>
+      <c r="G21" s="17">
         <v>1</v>
-      </c>
-      <c r="G21" s="16" t="s">
-        <v>279</v>
       </c>
       <c r="H21" s="16"/>
       <c r="I21" s="16"/>
@@ -6370,10 +6288,10 @@
         <v>2</v>
       </c>
       <c r="F22" s="17">
+        <v>10</v>
+      </c>
+      <c r="G22" s="17">
         <v>1</v>
-      </c>
-      <c r="G22" s="16" t="s">
-        <v>289</v>
       </c>
       <c r="H22" s="16"/>
       <c r="I22" s="16"/>
@@ -6439,10 +6357,10 @@
         <v>2</v>
       </c>
       <c r="F23" s="17">
+        <v>10</v>
+      </c>
+      <c r="G23" s="17">
         <v>1</v>
-      </c>
-      <c r="G23" s="16" t="s">
-        <v>290</v>
       </c>
       <c r="H23" s="16"/>
       <c r="I23" s="16"/>
@@ -6508,10 +6426,10 @@
         <v>2</v>
       </c>
       <c r="F24" s="17">
+        <v>10</v>
+      </c>
+      <c r="G24" s="17">
         <v>1</v>
-      </c>
-      <c r="G24" s="16" t="s">
-        <v>290</v>
       </c>
       <c r="H24" s="16"/>
       <c r="I24" s="16"/>
@@ -6577,10 +6495,10 @@
         <v>2</v>
       </c>
       <c r="F25" s="17">
+        <v>10</v>
+      </c>
+      <c r="G25" s="17">
         <v>1</v>
-      </c>
-      <c r="G25" s="16" t="s">
-        <v>279</v>
       </c>
       <c r="H25" s="16"/>
       <c r="I25" s="16"/>
@@ -6646,10 +6564,10 @@
         <v>2</v>
       </c>
       <c r="F26" s="17">
+        <v>10</v>
+      </c>
+      <c r="G26" s="17">
         <v>1</v>
-      </c>
-      <c r="G26" s="16" t="s">
-        <v>291</v>
       </c>
       <c r="H26" s="16"/>
       <c r="I26" s="16"/>
@@ -6715,10 +6633,10 @@
         <v>2</v>
       </c>
       <c r="F27" s="17">
+        <v>10</v>
+      </c>
+      <c r="G27" s="17">
         <v>1</v>
-      </c>
-      <c r="G27" s="16" t="s">
-        <v>292</v>
       </c>
       <c r="H27" s="16"/>
       <c r="I27" s="16"/>
@@ -6784,10 +6702,10 @@
         <v>2</v>
       </c>
       <c r="F28" s="17">
+        <v>10</v>
+      </c>
+      <c r="G28" s="17">
         <v>1</v>
-      </c>
-      <c r="G28" s="16" t="s">
-        <v>293</v>
       </c>
       <c r="H28" s="16"/>
       <c r="I28" s="16"/>
@@ -6853,10 +6771,10 @@
         <v>3</v>
       </c>
       <c r="F29" s="17">
+        <v>10</v>
+      </c>
+      <c r="G29" s="17">
         <v>1</v>
-      </c>
-      <c r="G29" s="16" t="s">
-        <v>294</v>
       </c>
       <c r="H29" s="16">
         <v>4</v>
@@ -6924,10 +6842,10 @@
         <v>3</v>
       </c>
       <c r="F30" s="17">
+        <v>10</v>
+      </c>
+      <c r="G30" s="17">
         <v>1</v>
-      </c>
-      <c r="G30" s="16" t="s">
-        <v>294</v>
       </c>
       <c r="H30" s="16">
         <v>7</v>
@@ -6997,10 +6915,10 @@
         <v>3</v>
       </c>
       <c r="F31" s="17">
+        <v>10</v>
+      </c>
+      <c r="G31" s="17">
         <v>2</v>
-      </c>
-      <c r="G31" s="16" t="s">
-        <v>295</v>
       </c>
       <c r="H31" s="16">
         <v>6</v>
@@ -7068,10 +6986,10 @@
         <v>3</v>
       </c>
       <c r="F32" s="17">
+        <v>10</v>
+      </c>
+      <c r="G32" s="17">
         <v>2</v>
-      </c>
-      <c r="G32" s="16" t="s">
-        <v>296</v>
       </c>
       <c r="H32" s="16">
         <v>8</v>
@@ -7141,10 +7059,10 @@
         <v>3</v>
       </c>
       <c r="F33" s="17">
+        <v>10</v>
+      </c>
+      <c r="G33" s="17">
         <v>2</v>
-      </c>
-      <c r="G33" s="16" t="s">
-        <v>296</v>
       </c>
       <c r="H33" s="16">
         <v>11</v>
@@ -7210,10 +7128,10 @@
         <v>3</v>
       </c>
       <c r="F34" s="17">
+        <v>10</v>
+      </c>
+      <c r="G34" s="17">
         <v>1</v>
-      </c>
-      <c r="G34" s="16" t="s">
-        <v>297</v>
       </c>
       <c r="H34" s="16">
         <v>18</v>
@@ -7279,10 +7197,10 @@
         <v>3</v>
       </c>
       <c r="F35" s="17">
+        <v>10</v>
+      </c>
+      <c r="G35" s="17">
         <v>1</v>
-      </c>
-      <c r="G35" s="16" t="s">
-        <v>298</v>
       </c>
       <c r="H35" s="16">
         <v>8</v>
@@ -7340,7 +7258,7 @@
         <v>143</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D36" s="1">
         <f t="shared" ref="D36:D59" si="2">IF(R36&gt;=23,4,IF(AND(R36&gt;=18,R36&lt;23),3,IF(AND(R36&gt;=13,R36&lt;18),2,IF(AND(R36&gt;=8,R36&lt;13),1,0))))</f>
@@ -7350,10 +7268,10 @@
         <v>3</v>
       </c>
       <c r="F36" s="17">
+        <v>10</v>
+      </c>
+      <c r="G36" s="17">
         <v>1</v>
-      </c>
-      <c r="G36" s="16" t="s">
-        <v>290</v>
       </c>
       <c r="H36" s="16">
         <v>3</v>
@@ -7419,10 +7337,10 @@
         <v>3</v>
       </c>
       <c r="F37" s="17">
+        <v>10</v>
+      </c>
+      <c r="G37" s="17">
         <v>2</v>
-      </c>
-      <c r="G37" s="16" t="s">
-        <v>294</v>
       </c>
       <c r="H37" s="16">
         <v>5</v>
@@ -7494,10 +7412,10 @@
         <v>4</v>
       </c>
       <c r="F38" s="17">
+        <v>10</v>
+      </c>
+      <c r="G38" s="17">
         <v>1</v>
-      </c>
-      <c r="G38" s="16" t="s">
-        <v>294</v>
       </c>
       <c r="H38" s="16"/>
       <c r="I38" s="16">
@@ -7561,10 +7479,10 @@
         <v>4</v>
       </c>
       <c r="F39" s="17">
+        <v>10</v>
+      </c>
+      <c r="G39" s="17">
         <v>2</v>
-      </c>
-      <c r="G39" s="16" t="s">
-        <v>299</v>
       </c>
       <c r="H39" s="16"/>
       <c r="I39" s="16">
@@ -7630,10 +7548,10 @@
         <v>4</v>
       </c>
       <c r="F40" s="17">
+        <v>10</v>
+      </c>
+      <c r="G40" s="17">
         <v>1</v>
-      </c>
-      <c r="G40" s="16" t="s">
-        <v>300</v>
       </c>
       <c r="H40" s="16"/>
       <c r="I40" s="16">
@@ -7701,10 +7619,10 @@
         <v>4</v>
       </c>
       <c r="F41" s="17">
+        <v>10</v>
+      </c>
+      <c r="G41" s="17">
         <v>2</v>
-      </c>
-      <c r="G41" s="16" t="s">
-        <v>301</v>
       </c>
       <c r="H41" s="16"/>
       <c r="I41" s="16">
@@ -7770,10 +7688,10 @@
         <v>4</v>
       </c>
       <c r="F42" s="17">
+        <v>10</v>
+      </c>
+      <c r="G42" s="17">
         <v>2</v>
-      </c>
-      <c r="G42" s="16" t="s">
-        <v>285</v>
       </c>
       <c r="H42" s="16"/>
       <c r="I42" s="16">
@@ -7839,10 +7757,10 @@
         <v>4</v>
       </c>
       <c r="F43" s="17">
+        <v>10</v>
+      </c>
+      <c r="G43" s="17">
         <v>2</v>
-      </c>
-      <c r="G43" s="16" t="s">
-        <v>299</v>
       </c>
       <c r="H43" s="16"/>
       <c r="I43" s="16">
@@ -7908,10 +7826,10 @@
         <v>4</v>
       </c>
       <c r="F44" s="17">
+        <v>10</v>
+      </c>
+      <c r="G44" s="17">
         <v>2</v>
-      </c>
-      <c r="G44" s="16" t="s">
-        <v>287</v>
       </c>
       <c r="H44" s="16"/>
       <c r="I44" s="16">
@@ -7967,7 +7885,7 @@
         <v>135</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D45" s="1">
         <f t="shared" si="2"/>
@@ -7977,10 +7895,10 @@
         <v>4</v>
       </c>
       <c r="F45" s="17">
+        <v>10</v>
+      </c>
+      <c r="G45" s="17">
         <v>1</v>
-      </c>
-      <c r="G45" s="16" t="s">
-        <v>300</v>
       </c>
       <c r="H45" s="16"/>
       <c r="I45" s="16">
@@ -8046,10 +7964,10 @@
         <v>4</v>
       </c>
       <c r="F46" s="17">
+        <v>10</v>
+      </c>
+      <c r="G46" s="17">
         <v>2</v>
-      </c>
-      <c r="G46" s="16" t="s">
-        <v>302</v>
       </c>
       <c r="H46" s="16"/>
       <c r="I46" s="16">
@@ -8115,10 +8033,10 @@
         <v>4</v>
       </c>
       <c r="F47" s="17">
+        <v>10</v>
+      </c>
+      <c r="G47" s="17">
         <v>1</v>
-      </c>
-      <c r="G47" s="16" t="s">
-        <v>278</v>
       </c>
       <c r="H47" s="16"/>
       <c r="I47" s="16">
@@ -8184,10 +8102,10 @@
         <v>4</v>
       </c>
       <c r="F48" s="17">
+        <v>10</v>
+      </c>
+      <c r="G48" s="17">
         <v>1</v>
-      </c>
-      <c r="G48" s="16" t="s">
-        <v>298</v>
       </c>
       <c r="H48" s="16"/>
       <c r="I48" s="16">
@@ -8255,9 +8173,11 @@
         <v>5</v>
       </c>
       <c r="F49" s="17">
+        <v>1</v>
+      </c>
+      <c r="G49" s="17">
         <v>2</v>
       </c>
-      <c r="G49" s="16"/>
       <c r="H49" s="16"/>
       <c r="I49" s="16"/>
       <c r="J49" s="16"/>
@@ -8322,7 +8242,9 @@
       <c r="F50" s="17">
         <v>1</v>
       </c>
-      <c r="G50" s="16"/>
+      <c r="G50" s="17">
+        <v>1</v>
+      </c>
       <c r="H50" s="16"/>
       <c r="I50" s="16"/>
       <c r="J50" s="16"/>
@@ -8389,7 +8311,9 @@
       <c r="F51" s="17">
         <v>1</v>
       </c>
-      <c r="G51" s="16"/>
+      <c r="G51" s="17">
+        <v>1</v>
+      </c>
       <c r="H51" s="16"/>
       <c r="I51" s="16"/>
       <c r="J51" s="16"/>
@@ -8456,7 +8380,9 @@
       <c r="F52" s="17">
         <v>1</v>
       </c>
-      <c r="G52" s="16"/>
+      <c r="G52" s="17">
+        <v>1</v>
+      </c>
       <c r="H52" s="16"/>
       <c r="I52" s="16">
         <v>4</v>
@@ -8525,7 +8451,9 @@
       <c r="F53" s="17">
         <v>1</v>
       </c>
-      <c r="G53" s="16"/>
+      <c r="G53" s="17">
+        <v>1</v>
+      </c>
       <c r="H53" s="16"/>
       <c r="I53" s="16"/>
       <c r="J53" s="16"/>
@@ -8590,9 +8518,11 @@
         <v>5</v>
       </c>
       <c r="F54" s="17">
+        <v>1</v>
+      </c>
+      <c r="G54" s="17">
         <v>2</v>
       </c>
-      <c r="G54" s="16"/>
       <c r="H54" s="16"/>
       <c r="I54" s="16"/>
       <c r="J54" s="16"/>
@@ -8657,9 +8587,11 @@
         <v>5</v>
       </c>
       <c r="F55" s="17">
+        <v>1</v>
+      </c>
+      <c r="G55" s="17">
         <v>2</v>
       </c>
-      <c r="G55" s="16"/>
       <c r="H55" s="16"/>
       <c r="I55" s="16"/>
       <c r="J55" s="16"/>
@@ -8720,9 +8652,11 @@
         <v>5</v>
       </c>
       <c r="F56" s="17">
+        <v>1</v>
+      </c>
+      <c r="G56" s="17">
         <v>2</v>
       </c>
-      <c r="G56" s="16"/>
       <c r="H56" s="16"/>
       <c r="I56" s="16"/>
       <c r="J56" s="16"/>
@@ -8791,7 +8725,9 @@
       <c r="F57" s="17">
         <v>1</v>
       </c>
-      <c r="G57" s="16"/>
+      <c r="G57" s="17">
+        <v>1</v>
+      </c>
       <c r="H57" s="16"/>
       <c r="I57" s="16"/>
       <c r="J57" s="16"/>
@@ -8856,7 +8792,9 @@
       <c r="F58" s="17">
         <v>1</v>
       </c>
-      <c r="G58" s="16"/>
+      <c r="G58" s="17">
+        <v>1</v>
+      </c>
       <c r="H58" s="16"/>
       <c r="I58" s="16"/>
       <c r="J58" s="16"/>
@@ -8921,9 +8859,11 @@
         <v>5</v>
       </c>
       <c r="F59" s="17">
+        <v>1</v>
+      </c>
+      <c r="G59" s="17">
         <v>2</v>
       </c>
-      <c r="G59" s="16"/>
       <c r="H59" s="16"/>
       <c r="I59" s="16"/>
       <c r="J59" s="16"/>
@@ -8971,25 +8911,25 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="D4:D59">
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="greaterThanOrEqual">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="8" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="9" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="10" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="11" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G4:AF4 Z19:AF28 S5:AF18 S29:AF59 S19:X28 G5:R59">
-    <cfRule type="containsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(G4))=0</formula>
+  <conditionalFormatting sqref="Z19:AF28 S5:AF18 S29:AF59 S19:X28 H4:AF4 H5:R59">
+    <cfRule type="containsBlanks" dxfId="1" priority="1">
+      <formula>LEN(TRIM(H4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
merge the info equip and castle
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Equip.xlsx
+++ b/ConfigData/Xlsx/Equip.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TOMClassic\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{A488726A-80DD-4E41-BEC0-E0056DED2355}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{31FDC0B8-1341-4D59-8811-61188C467A5E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="5895" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="321">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -1200,6 +1200,21 @@
   </si>
   <si>
     <t>城堡开启农场功能</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>jianzhu13</t>
+  </si>
+  <si>
+    <t>矿山</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>eqkuang</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>城堡开启矿山功能</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -2109,172 +2124,6 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF9751CB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF9751CB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </font>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -2803,6 +2652,172 @@
         <horizontal/>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF9751CB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF9751CB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -4652,52 +4667,52 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表1" displayName="表1" ref="A3:AH63" totalsRowShown="0">
-  <autoFilter ref="A3:AH63" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表1" displayName="表1" ref="A3:AH64" totalsRowShown="0">
+  <autoFilter ref="A3:AH64" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState ref="A4:AH62">
     <sortCondition ref="A3:A62"/>
   </sortState>
   <tableColumns count="34">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name"/>
-    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0000-000022000000}" name="Ename" dataDxfId="43"/>
-    <tableColumn id="31" xr3:uid="{C9E6F01C-30E7-4BB6-9D72-93C8EA7E4905}" name="Des" dataDxfId="0"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="~Comment" dataDxfId="42"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Quality" dataDxfId="41">
+    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0000-000022000000}" name="Ename" dataDxfId="30"/>
+    <tableColumn id="31" xr3:uid="{C9E6F01C-30E7-4BB6-9D72-93C8EA7E4905}" name="Des" dataDxfId="29"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="~Comment" dataDxfId="28"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Quality" dataDxfId="27">
       <calculatedColumnFormula>IF(T4&gt;=23,4,IF(AND(T4&gt;=18,T4&lt;23),3,IF(AND(T4&gt;=13,T4&lt;18),2,IF(AND(T4&gt;=8,T4&lt;13),1,0))))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Position"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="MaxLevel" dataDxfId="40"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="ComposeRes" dataDxfId="39"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="AtkP" dataDxfId="38"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="VitP" dataDxfId="37"/>
-    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="Attr" dataDxfId="36"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Def" dataDxfId="35"/>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="Mag" dataDxfId="34"/>
-    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="Spd" dataDxfId="33"/>
-    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="Hit" dataDxfId="32"/>
-    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="Dhit" dataDxfId="31"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="Crt" dataDxfId="30"/>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="Luk" dataDxfId="29"/>
-    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="Sum" dataDxfId="28">
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="MaxLevel" dataDxfId="26"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="ComposeRes" dataDxfId="25"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="AtkP" dataDxfId="24"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="VitP" dataDxfId="23"/>
+    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="Attr" dataDxfId="22"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Def" dataDxfId="21"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="Mag" dataDxfId="20"/>
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="Spd" dataDxfId="19"/>
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="Hit" dataDxfId="18"/>
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="Dhit" dataDxfId="17"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="Crt" dataDxfId="16"/>
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="Luk" dataDxfId="15"/>
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="Sum" dataDxfId="14">
       <calculatedColumnFormula>J4+K4+L4+ SUM(M4:S4)*5+AB4+AC4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Range" dataDxfId="27"/>
-    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0000-000021000000}" name="Arrow" dataDxfId="26"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="SlotId" dataDxfId="25"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="EnergyRate" dataDxfId="24"/>
-    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0000-000025000000}" name="DungeonAttrs" dataDxfId="23"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="HeroSkillId" dataDxfId="22"/>
-    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="AttrId" dataDxfId="21"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="~SkillMark2" dataDxfId="20"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="~SkillMark22" dataDxfId="19">
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Range" dataDxfId="13"/>
+    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0000-000021000000}" name="Arrow" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="SlotId" dataDxfId="11"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="EnergyRate" dataDxfId="10"/>
+    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0000-000025000000}" name="DungeonAttrs" dataDxfId="9"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="HeroSkillId" dataDxfId="8"/>
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="AttrId" dataDxfId="7"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="~SkillMark2" dataDxfId="6"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="~SkillMark22" dataDxfId="5">
       <calculatedColumnFormula>IF(ISBLANK(AD4),0, LOOKUP(AD4,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AE4/100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="CommonSkillId" dataDxfId="18"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="CommonSkillRate" dataDxfId="17"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="RandomDrop" dataDxfId="16"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="CanMerge" dataDxfId="15"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Url" dataDxfId="14"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="CommonSkillId" dataDxfId="4"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="CommonSkillRate" dataDxfId="3"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="RandomDrop" dataDxfId="2"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="CanMerge" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Url" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5024,10 +5039,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AH63"/>
+  <dimension ref="A1:AH64"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="F62" sqref="F62"/>
+      <selection activeCell="X64" sqref="X64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -9614,54 +9629,123 @@
         <v>308</v>
       </c>
     </row>
+    <row r="64" spans="1:34" x14ac:dyDescent="0.15">
+      <c r="A64">
+        <v>21500013</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="E64" s="19" t="s">
+        <v>310</v>
+      </c>
+      <c r="F64" s="1">
+        <f t="shared" ref="F64" si="9">IF(T64&gt;=23,4,IF(AND(T64&gt;=18,T64&lt;23),3,IF(AND(T64&gt;=13,T64&lt;18),2,IF(AND(T64&gt;=8,T64&lt;13),1,0))))</f>
+        <v>1</v>
+      </c>
+      <c r="G64" s="1">
+        <v>5</v>
+      </c>
+      <c r="H64" s="17">
+        <v>1</v>
+      </c>
+      <c r="I64" s="17">
+        <v>2</v>
+      </c>
+      <c r="J64" s="16"/>
+      <c r="K64" s="16"/>
+      <c r="L64" s="16"/>
+      <c r="M64" s="16"/>
+      <c r="N64" s="16"/>
+      <c r="O64" s="16"/>
+      <c r="P64" s="16"/>
+      <c r="Q64" s="16"/>
+      <c r="R64" s="16"/>
+      <c r="S64" s="16"/>
+      <c r="T64" s="16">
+        <f t="shared" ref="T64" si="10">J64+K64+L64+ SUM(M64:S64)*5+AB64+AC64</f>
+        <v>11</v>
+      </c>
+      <c r="U64" s="16"/>
+      <c r="V64" s="16"/>
+      <c r="W64" s="16"/>
+      <c r="X64" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y64" s="16"/>
+      <c r="Z64" s="16"/>
+      <c r="AA64" s="16"/>
+      <c r="AB64" s="16">
+        <v>11</v>
+      </c>
+      <c r="AC64" s="16">
+        <f>IF(ISBLANK(AD64),0, LOOKUP(AD64,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AE64/100)</f>
+        <v>0</v>
+      </c>
+      <c r="AD64" s="16"/>
+      <c r="AE64" s="16"/>
+      <c r="AF64" s="16"/>
+      <c r="AG64" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="AH64" s="16" t="s">
+        <v>317</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="F4:F38 F41:F63">
-    <cfRule type="cellIs" dxfId="13" priority="14" operator="greaterThanOrEqual">
+  <conditionalFormatting sqref="F4:F38 F41:F64">
+    <cfRule type="cellIs" dxfId="43" priority="14" operator="greaterThanOrEqual">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="15" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="16" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="17" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="18" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L36:M40 J4:AH20 J21:AE22 AG21:AH22 J23:AH38 J41:AH63">
-    <cfRule type="containsBlanks" dxfId="8" priority="8">
+  <conditionalFormatting sqref="L36:M40 J4:AH20 J21:AE22 AG21:AH22 J23:AH38 J41:AH64">
+    <cfRule type="containsBlanks" dxfId="38" priority="8">
       <formula>LEN(TRIM(J4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F39:F40">
-    <cfRule type="cellIs" dxfId="7" priority="3" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="37" priority="3" operator="greaterThanOrEqual">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="4" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="5" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="6" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="7" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J39:AH39 J40:U40 W40:AH40">
-    <cfRule type="containsBlanks" dxfId="2" priority="2">
+    <cfRule type="containsBlanks" dxfId="32" priority="2">
       <formula>LEN(TRIM(J39))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V40">
-    <cfRule type="containsBlanks" dxfId="1" priority="1">
+    <cfRule type="containsBlanks" dxfId="31" priority="1">
       <formula>LEN(TRIM(V40))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
finish the equip ore
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Equip.xlsx
+++ b/ConfigData/Xlsx/Equip.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{31FDC0B8-1341-4D59-8811-61188C467A5E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{FA9FD607-56A9-44A6-8E44-7628A5D1BB55}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="5895" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5041,8 +5041,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AH64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="X64" sqref="X64"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="X43" sqref="X43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
add a new hunt equip
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Equip.xlsx
+++ b/ConfigData/Xlsx/Equip.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{FA9FD607-56A9-44A6-8E44-7628A5D1BB55}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="5895" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="5895"/>
   </bookViews>
   <sheets>
     <sheet name="装备" sheetId="5" r:id="rId1"/>
@@ -23,12 +22,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Administrator</author>
   </authors>
   <commentList>
-    <comment ref="X1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="X1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -59,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="325">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -1215,13 +1214,28 @@
   </si>
   <si>
     <t>城堡开启矿山功能</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>jianzhu14</t>
+  </si>
+  <si>
+    <t>猎场</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>eqliechang</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>城堡开启猎场功能</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2821,6 +2835,72 @@
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
     <mruColors>
       <color rgb="FF9751CB"/>
     </mruColors>
@@ -4667,52 +4747,52 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表1" displayName="表1" ref="A3:AH64" totalsRowShown="0">
-  <autoFilter ref="A3:AH64" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:AH65" totalsRowShown="0">
+  <autoFilter ref="A3:AH65"/>
   <sortState ref="A4:AH62">
     <sortCondition ref="A3:A62"/>
   </sortState>
   <tableColumns count="34">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name"/>
-    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0000-000022000000}" name="Ename" dataDxfId="30"/>
-    <tableColumn id="31" xr3:uid="{C9E6F01C-30E7-4BB6-9D72-93C8EA7E4905}" name="Des" dataDxfId="29"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="~Comment" dataDxfId="28"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Quality" dataDxfId="27">
+    <tableColumn id="1" name="Id"/>
+    <tableColumn id="2" name="Name"/>
+    <tableColumn id="34" name="Ename" dataDxfId="30"/>
+    <tableColumn id="31" name="Des" dataDxfId="29"/>
+    <tableColumn id="19" name="~Comment" dataDxfId="28"/>
+    <tableColumn id="3" name="Quality" dataDxfId="27">
       <calculatedColumnFormula>IF(T4&gt;=23,4,IF(AND(T4&gt;=18,T4&lt;23),3,IF(AND(T4&gt;=13,T4&lt;18),2,IF(AND(T4&gt;=8,T4&lt;13),1,0))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Position"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="MaxLevel" dataDxfId="26"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="ComposeRes" dataDxfId="25"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="AtkP" dataDxfId="24"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="VitP" dataDxfId="23"/>
-    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="Attr" dataDxfId="22"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Def" dataDxfId="21"/>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="Mag" dataDxfId="20"/>
-    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="Spd" dataDxfId="19"/>
-    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="Hit" dataDxfId="18"/>
-    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="Dhit" dataDxfId="17"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="Crt" dataDxfId="16"/>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="Luk" dataDxfId="15"/>
-    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="Sum" dataDxfId="14">
+    <tableColumn id="5" name="Position"/>
+    <tableColumn id="15" name="MaxLevel" dataDxfId="26"/>
+    <tableColumn id="7" name="ComposeRes" dataDxfId="25"/>
+    <tableColumn id="11" name="AtkP" dataDxfId="24"/>
+    <tableColumn id="8" name="VitP" dataDxfId="23"/>
+    <tableColumn id="30" name="Attr" dataDxfId="22"/>
+    <tableColumn id="6" name="Def" dataDxfId="21"/>
+    <tableColumn id="22" name="Mag" dataDxfId="20"/>
+    <tableColumn id="27" name="Spd" dataDxfId="19"/>
+    <tableColumn id="26" name="Hit" dataDxfId="18"/>
+    <tableColumn id="25" name="Dhit" dataDxfId="17"/>
+    <tableColumn id="24" name="Crt" dataDxfId="16"/>
+    <tableColumn id="23" name="Luk" dataDxfId="15"/>
+    <tableColumn id="28" name="Sum" dataDxfId="14">
       <calculatedColumnFormula>J4+K4+L4+ SUM(M4:S4)*5+AB4+AC4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Range" dataDxfId="13"/>
-    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0000-000021000000}" name="Arrow" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="SlotId" dataDxfId="11"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="EnergyRate" dataDxfId="10"/>
-    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0000-000025000000}" name="DungeonAttrs" dataDxfId="9"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="HeroSkillId" dataDxfId="8"/>
-    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="AttrId" dataDxfId="7"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="~SkillMark2" dataDxfId="6"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="~SkillMark22" dataDxfId="5">
+    <tableColumn id="12" name="Range" dataDxfId="13"/>
+    <tableColumn id="33" name="Arrow" dataDxfId="12"/>
+    <tableColumn id="4" name="SlotId" dataDxfId="11"/>
+    <tableColumn id="9" name="EnergyRate" dataDxfId="10"/>
+    <tableColumn id="37" name="DungeonAttrs" dataDxfId="9"/>
+    <tableColumn id="20" name="HeroSkillId" dataDxfId="8"/>
+    <tableColumn id="29" name="AttrId" dataDxfId="7"/>
+    <tableColumn id="21" name="~SkillMark2" dataDxfId="6"/>
+    <tableColumn id="18" name="~SkillMark22" dataDxfId="5">
       <calculatedColumnFormula>IF(ISBLANK(AD4),0, LOOKUP(AD4,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AE4/100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="CommonSkillId" dataDxfId="4"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="CommonSkillRate" dataDxfId="3"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="RandomDrop" dataDxfId="2"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="CanMerge" dataDxfId="1"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Url" dataDxfId="0"/>
+    <tableColumn id="13" name="CommonSkillId" dataDxfId="4"/>
+    <tableColumn id="14" name="CommonSkillRate" dataDxfId="3"/>
+    <tableColumn id="17" name="RandomDrop" dataDxfId="2"/>
+    <tableColumn id="16" name="CanMerge" dataDxfId="1"/>
+    <tableColumn id="10" name="Url" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4726,7 +4806,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="C7EDCC"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -5038,11 +5118,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AH64"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AH65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="X43" sqref="X43"/>
+      <selection activeCell="X65" sqref="X65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -9698,9 +9778,78 @@
         <v>317</v>
       </c>
     </row>
+    <row r="65" spans="1:34" x14ac:dyDescent="0.15">
+      <c r="A65">
+        <v>21500014</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="E65" s="19" t="s">
+        <v>310</v>
+      </c>
+      <c r="F65" s="1">
+        <f t="shared" ref="F65" si="11">IF(T65&gt;=23,4,IF(AND(T65&gt;=18,T65&lt;23),3,IF(AND(T65&gt;=13,T65&lt;18),2,IF(AND(T65&gt;=8,T65&lt;13),1,0))))</f>
+        <v>2</v>
+      </c>
+      <c r="G65" s="1">
+        <v>5</v>
+      </c>
+      <c r="H65" s="17">
+        <v>1</v>
+      </c>
+      <c r="I65" s="17">
+        <v>2</v>
+      </c>
+      <c r="J65" s="16"/>
+      <c r="K65" s="16"/>
+      <c r="L65" s="16"/>
+      <c r="M65" s="16"/>
+      <c r="N65" s="16"/>
+      <c r="O65" s="16"/>
+      <c r="P65" s="16"/>
+      <c r="Q65" s="16"/>
+      <c r="R65" s="16"/>
+      <c r="S65" s="16"/>
+      <c r="T65" s="16">
+        <f t="shared" ref="T65" si="12">J65+K65+L65+ SUM(M65:S65)*5+AB65+AC65</f>
+        <v>16</v>
+      </c>
+      <c r="U65" s="16"/>
+      <c r="V65" s="16"/>
+      <c r="W65" s="16"/>
+      <c r="X65" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y65" s="16"/>
+      <c r="Z65" s="16"/>
+      <c r="AA65" s="16"/>
+      <c r="AB65" s="16">
+        <v>16</v>
+      </c>
+      <c r="AC65" s="16">
+        <f>IF(ISBLANK(AD65),0, LOOKUP(AD65,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AE65/100)</f>
+        <v>0</v>
+      </c>
+      <c r="AD65" s="16"/>
+      <c r="AE65" s="16"/>
+      <c r="AF65" s="16"/>
+      <c r="AG65" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="AH65" s="16" t="s">
+        <v>321</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="F4:F38 F41:F64">
+  <conditionalFormatting sqref="F4:F38 F41:F65">
     <cfRule type="cellIs" dxfId="43" priority="14" operator="greaterThanOrEqual">
       <formula>5</formula>
     </cfRule>
@@ -9717,7 +9866,7 @@
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L36:M40 J4:AH20 J21:AE22 AG21:AH22 J23:AH38 J41:AH64">
+  <conditionalFormatting sqref="L36:M40 J4:AH20 J21:AE22 AG21:AH22 J23:AH38 J41:AH65">
     <cfRule type="containsBlanks" dxfId="38" priority="8">
       <formula>LEN(TRIM(J4))=0</formula>
     </cfRule>

</xml_diff>

<commit_message>
more build support for main
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Equip.xlsx
+++ b/ConfigData/Xlsx/Equip.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="600" yWindow="30" windowWidth="18135" windowHeight="5895"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="5895"/>
   </bookViews>
   <sheets>
     <sheet name="装备" sheetId="5" r:id="rId1"/>
@@ -341,10 +341,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>1;7;9</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>盖贝依城堡</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -353,10 +349,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>1;6;9</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>0;0;0</t>
   </si>
   <si>
@@ -367,10 +359,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>1;2;9</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>zhulou5</t>
   </si>
   <si>
@@ -378,10 +366,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>1;3;9</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>zhulou6</t>
   </si>
   <si>
@@ -389,10 +373,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>1;2;8;9</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>zhulou7</t>
   </si>
   <si>
@@ -618,10 +598,6 @@
     <t>zhulou8</t>
   </si>
   <si>
-    <t>2;6;9</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>天鹅堡</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -633,10 +609,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>4;7;9</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>zhulou10</t>
   </si>
   <si>
@@ -644,10 +616,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>2;7</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>zhulou11</t>
   </si>
   <si>
@@ -655,10 +623,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>3;6;9</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>箭矢</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -698,10 +662,6 @@
     <t>zhulou12</t>
   </si>
   <si>
-    <t>1;3;6</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>霍格沃兹</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -713,10 +673,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>2;3</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>zhulou14</t>
   </si>
   <si>
@@ -724,10 +680,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>1;3;7</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>zhulou15</t>
   </si>
   <si>
@@ -735,10 +687,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>1;3;9</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>qizhi5</t>
   </si>
   <si>
@@ -1244,6 +1192,58 @@
   </si>
   <si>
     <t>城堡开启海盗湾功能</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>2;7;9</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>2;3;9</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>1;3;7;9</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>1;3;6;9</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>1;2;3;9</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>1;3;8;9</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>2;3;6;9</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>3;4;7;9</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>1;3;6;8</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>1;3;7;8</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>1;2;3;8</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>1;2;3;6;9</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>1;4;7;9</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -3278,47 +3278,47 @@
         </row>
         <row r="43">
           <cell r="A43">
-            <v>55200001</v>
+            <v>55110021</v>
           </cell>
           <cell r="AB43">
-            <v>40</v>
+            <v>65</v>
           </cell>
         </row>
         <row r="44">
           <cell r="A44">
-            <v>55200002</v>
+            <v>55200001</v>
           </cell>
           <cell r="AB44">
-            <v>28</v>
+            <v>40</v>
           </cell>
         </row>
         <row r="45">
           <cell r="A45">
-            <v>55200003</v>
+            <v>55200002</v>
           </cell>
           <cell r="AB45">
-            <v>25</v>
+            <v>28</v>
           </cell>
         </row>
         <row r="46">
           <cell r="A46">
-            <v>55200004</v>
+            <v>55200003</v>
           </cell>
           <cell r="AB46">
-            <v>40</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="47">
           <cell r="A47">
-            <v>55200005</v>
+            <v>55200004</v>
           </cell>
           <cell r="AB47">
-            <v>20</v>
+            <v>40</v>
           </cell>
         </row>
         <row r="48">
           <cell r="A48">
-            <v>55200006</v>
+            <v>55200005</v>
           </cell>
           <cell r="AB48">
             <v>20</v>
@@ -3326,7 +3326,7 @@
         </row>
         <row r="49">
           <cell r="A49">
-            <v>55200007</v>
+            <v>55200006</v>
           </cell>
           <cell r="AB49">
             <v>20</v>
@@ -3334,15 +3334,15 @@
         </row>
         <row r="50">
           <cell r="A50">
-            <v>55200008</v>
+            <v>55200007</v>
           </cell>
           <cell r="AB50">
-            <v>25</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="51">
           <cell r="A51">
-            <v>55200009</v>
+            <v>55200008</v>
           </cell>
           <cell r="AB51">
             <v>25</v>
@@ -3350,7 +3350,7 @@
         </row>
         <row r="52">
           <cell r="A52">
-            <v>55200010</v>
+            <v>55200009</v>
           </cell>
           <cell r="AB52">
             <v>25</v>
@@ -3358,87 +3358,87 @@
         </row>
         <row r="53">
           <cell r="A53">
-            <v>55200011</v>
+            <v>55200010</v>
           </cell>
           <cell r="AB53">
-            <v>20</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="54">
           <cell r="A54">
-            <v>55200012</v>
+            <v>55200011</v>
           </cell>
           <cell r="AB54">
-            <v>30</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="55">
           <cell r="A55">
-            <v>55200013</v>
+            <v>55200012</v>
           </cell>
           <cell r="AB55">
-            <v>10</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="56">
           <cell r="A56">
-            <v>55200014</v>
+            <v>55200013</v>
           </cell>
           <cell r="AB56">
-            <v>25</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="57">
           <cell r="A57">
-            <v>55200015</v>
+            <v>55200014</v>
           </cell>
           <cell r="AB57">
-            <v>20</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="58">
           <cell r="A58">
-            <v>55200016</v>
+            <v>55200015</v>
           </cell>
           <cell r="AB58">
-            <v>30</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="59">
           <cell r="A59">
-            <v>55200017</v>
+            <v>55200016</v>
           </cell>
           <cell r="AB59">
-            <v>35</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="60">
           <cell r="A60">
-            <v>55200018</v>
+            <v>55200017</v>
           </cell>
           <cell r="AB60">
-            <v>50</v>
+            <v>35</v>
           </cell>
         </row>
         <row r="61">
           <cell r="A61">
-            <v>55300001</v>
+            <v>55200018</v>
           </cell>
           <cell r="AB61">
-            <v>40</v>
+            <v>50</v>
           </cell>
         </row>
         <row r="62">
           <cell r="A62">
-            <v>55300002</v>
+            <v>55300001</v>
           </cell>
           <cell r="AB62">
-            <v>30</v>
+            <v>40</v>
           </cell>
         </row>
         <row r="63">
           <cell r="A63">
-            <v>55300003</v>
+            <v>55300002</v>
           </cell>
           <cell r="AB63">
             <v>30</v>
@@ -3446,7 +3446,7 @@
         </row>
         <row r="64">
           <cell r="A64">
-            <v>55300004</v>
+            <v>55300003</v>
           </cell>
           <cell r="AB64">
             <v>30</v>
@@ -3454,7 +3454,7 @@
         </row>
         <row r="65">
           <cell r="A65">
-            <v>55300005</v>
+            <v>55300004</v>
           </cell>
           <cell r="AB65">
             <v>30</v>
@@ -3462,15 +3462,15 @@
         </row>
         <row r="66">
           <cell r="A66">
-            <v>55300006</v>
+            <v>55300005</v>
           </cell>
           <cell r="AB66">
-            <v>25</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="67">
           <cell r="A67">
-            <v>55300007</v>
+            <v>55300006</v>
           </cell>
           <cell r="AB67">
             <v>25</v>
@@ -3478,15 +3478,15 @@
         </row>
         <row r="68">
           <cell r="A68">
-            <v>55300008</v>
+            <v>55300007</v>
           </cell>
           <cell r="AB68">
-            <v>30</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="69">
           <cell r="A69">
-            <v>55300009</v>
+            <v>55300008</v>
           </cell>
           <cell r="AB69">
             <v>30</v>
@@ -3494,71 +3494,71 @@
         </row>
         <row r="70">
           <cell r="A70">
-            <v>55300010</v>
+            <v>55300009</v>
           </cell>
           <cell r="AB70">
-            <v>35</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="71">
           <cell r="A71">
-            <v>55300011</v>
+            <v>55300010</v>
           </cell>
           <cell r="AB71">
-            <v>25</v>
+            <v>35</v>
           </cell>
         </row>
         <row r="72">
           <cell r="A72">
-            <v>55300012</v>
+            <v>55300011</v>
           </cell>
           <cell r="AB72">
-            <v>5</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="73">
           <cell r="A73">
-            <v>55300013</v>
+            <v>55300012</v>
           </cell>
           <cell r="AB73">
-            <v>25</v>
+            <v>5</v>
           </cell>
         </row>
         <row r="74">
           <cell r="A74">
-            <v>55310001</v>
+            <v>55300013</v>
           </cell>
           <cell r="AB74">
-            <v>100</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="75">
           <cell r="A75">
-            <v>55310002</v>
+            <v>55310001</v>
           </cell>
           <cell r="AB75">
-            <v>15</v>
+            <v>100</v>
           </cell>
         </row>
         <row r="76">
           <cell r="A76">
-            <v>55310003</v>
+            <v>55310002</v>
           </cell>
           <cell r="AB76">
-            <v>13</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="77">
           <cell r="A77">
-            <v>55400001</v>
+            <v>55310003</v>
           </cell>
           <cell r="AB77">
-            <v>80</v>
+            <v>13</v>
           </cell>
         </row>
         <row r="78">
           <cell r="A78">
-            <v>55400002</v>
+            <v>55400001</v>
           </cell>
           <cell r="AB78">
             <v>80</v>
@@ -3566,7 +3566,7 @@
         </row>
         <row r="79">
           <cell r="A79">
-            <v>55400003</v>
+            <v>55400002</v>
           </cell>
           <cell r="AB79">
             <v>80</v>
@@ -3574,55 +3574,55 @@
         </row>
         <row r="80">
           <cell r="A80">
-            <v>55400005</v>
+            <v>55400003</v>
           </cell>
           <cell r="AB80">
-            <v>55</v>
+            <v>80</v>
           </cell>
         </row>
         <row r="81">
           <cell r="A81">
-            <v>55400006</v>
+            <v>55400005</v>
           </cell>
           <cell r="AB81">
-            <v>30</v>
+            <v>55</v>
           </cell>
         </row>
         <row r="82">
           <cell r="A82">
-            <v>55400007</v>
+            <v>55400006</v>
           </cell>
           <cell r="AB82">
-            <v>25</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="83">
           <cell r="A83">
-            <v>55400008</v>
+            <v>55400007</v>
           </cell>
           <cell r="AB83">
-            <v>35</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="84">
           <cell r="A84">
-            <v>55410001</v>
+            <v>55400008</v>
           </cell>
           <cell r="AB84">
-            <v>50</v>
+            <v>35</v>
           </cell>
         </row>
         <row r="85">
           <cell r="A85">
-            <v>55500001</v>
+            <v>55410001</v>
           </cell>
           <cell r="AB85">
-            <v>5</v>
+            <v>50</v>
           </cell>
         </row>
         <row r="86">
           <cell r="A86">
-            <v>55500002</v>
+            <v>55500001</v>
           </cell>
           <cell r="AB86">
             <v>5</v>
@@ -3630,7 +3630,7 @@
         </row>
         <row r="87">
           <cell r="A87">
-            <v>55500003</v>
+            <v>55500002</v>
           </cell>
           <cell r="AB87">
             <v>5</v>
@@ -3638,7 +3638,7 @@
         </row>
         <row r="88">
           <cell r="A88">
-            <v>55500004</v>
+            <v>55500003</v>
           </cell>
           <cell r="AB88">
             <v>5</v>
@@ -3646,7 +3646,7 @@
         </row>
         <row r="89">
           <cell r="A89">
-            <v>55500005</v>
+            <v>55500004</v>
           </cell>
           <cell r="AB89">
             <v>5</v>
@@ -3654,7 +3654,7 @@
         </row>
         <row r="90">
           <cell r="A90">
-            <v>55500006</v>
+            <v>55500005</v>
           </cell>
           <cell r="AB90">
             <v>5</v>
@@ -3662,7 +3662,7 @@
         </row>
         <row r="91">
           <cell r="A91">
-            <v>55500007</v>
+            <v>55500006</v>
           </cell>
           <cell r="AB91">
             <v>5</v>
@@ -3670,7 +3670,7 @@
         </row>
         <row r="92">
           <cell r="A92">
-            <v>55500008</v>
+            <v>55500007</v>
           </cell>
           <cell r="AB92">
             <v>5</v>
@@ -3678,7 +3678,7 @@
         </row>
         <row r="93">
           <cell r="A93">
-            <v>55500009</v>
+            <v>55500008</v>
           </cell>
           <cell r="AB93">
             <v>5</v>
@@ -3686,7 +3686,7 @@
         </row>
         <row r="94">
           <cell r="A94">
-            <v>55500010</v>
+            <v>55500009</v>
           </cell>
           <cell r="AB94">
             <v>5</v>
@@ -3694,7 +3694,7 @@
         </row>
         <row r="95">
           <cell r="A95">
-            <v>55500011</v>
+            <v>55500010</v>
           </cell>
           <cell r="AB95">
             <v>5</v>
@@ -3702,7 +3702,7 @@
         </row>
         <row r="96">
           <cell r="A96">
-            <v>55500012</v>
+            <v>55500011</v>
           </cell>
           <cell r="AB96">
             <v>5</v>
@@ -3710,7 +3710,7 @@
         </row>
         <row r="97">
           <cell r="A97">
-            <v>55500013</v>
+            <v>55500012</v>
           </cell>
           <cell r="AB97">
             <v>5</v>
@@ -3718,7 +3718,7 @@
         </row>
         <row r="98">
           <cell r="A98">
-            <v>55500014</v>
+            <v>55500013</v>
           </cell>
           <cell r="AB98">
             <v>5</v>
@@ -3726,7 +3726,7 @@
         </row>
         <row r="99">
           <cell r="A99">
-            <v>55500015</v>
+            <v>55500014</v>
           </cell>
           <cell r="AB99">
             <v>5</v>
@@ -3734,7 +3734,7 @@
         </row>
         <row r="100">
           <cell r="A100">
-            <v>55500016</v>
+            <v>55500015</v>
           </cell>
           <cell r="AB100">
             <v>5</v>
@@ -3742,23 +3742,23 @@
         </row>
         <row r="101">
           <cell r="A101">
-            <v>55510001</v>
+            <v>55500016</v>
           </cell>
           <cell r="AB101">
-            <v>12</v>
+            <v>5</v>
           </cell>
         </row>
         <row r="102">
           <cell r="A102">
-            <v>55510002</v>
+            <v>55510001</v>
           </cell>
           <cell r="AB102">
-            <v>15</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="103">
           <cell r="A103">
-            <v>55510003</v>
+            <v>55510002</v>
           </cell>
           <cell r="AB103">
             <v>15</v>
@@ -3766,87 +3766,87 @@
         </row>
         <row r="104">
           <cell r="A104">
-            <v>55510004</v>
+            <v>55510003</v>
           </cell>
           <cell r="AB104">
-            <v>12</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="105">
           <cell r="A105">
-            <v>55510006</v>
+            <v>55510004</v>
           </cell>
           <cell r="AB105">
-            <v>25</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="106">
           <cell r="A106">
-            <v>55510007</v>
+            <v>55510006</v>
           </cell>
           <cell r="AB106">
-            <v>10</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="107">
           <cell r="A107">
-            <v>55510009</v>
+            <v>55510007</v>
           </cell>
           <cell r="AB107">
-            <v>50</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="108">
           <cell r="A108">
-            <v>55510010</v>
+            <v>55510009</v>
           </cell>
           <cell r="AB108">
-            <v>10</v>
+            <v>50</v>
           </cell>
         </row>
         <row r="109">
           <cell r="A109">
-            <v>55510011</v>
+            <v>55510010</v>
           </cell>
           <cell r="AB109">
-            <v>15</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="110">
           <cell r="A110">
-            <v>55510012</v>
+            <v>55510011</v>
           </cell>
           <cell r="AB110">
-            <v>62</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="111">
           <cell r="A111">
-            <v>55510013</v>
+            <v>55510012</v>
           </cell>
           <cell r="AB111">
-            <v>12</v>
+            <v>62</v>
           </cell>
         </row>
         <row r="112">
           <cell r="A112">
-            <v>55510014</v>
+            <v>55510013</v>
           </cell>
           <cell r="AB112">
-            <v>25</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="113">
           <cell r="A113">
-            <v>55510018</v>
+            <v>55510014</v>
           </cell>
           <cell r="AB113">
-            <v>37</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="114">
           <cell r="A114">
-            <v>55510019</v>
+            <v>55510018</v>
           </cell>
           <cell r="AB114">
             <v>37</v>
@@ -3854,63 +3854,63 @@
         </row>
         <row r="115">
           <cell r="A115">
-            <v>55520001</v>
+            <v>55510019</v>
           </cell>
           <cell r="AB115">
-            <v>-25</v>
+            <v>37</v>
           </cell>
         </row>
         <row r="116">
           <cell r="A116">
-            <v>55520002</v>
+            <v>55520001</v>
           </cell>
           <cell r="AB116">
-            <v>62</v>
+            <v>-25</v>
           </cell>
         </row>
         <row r="117">
           <cell r="A117">
-            <v>55520003</v>
+            <v>55520002</v>
           </cell>
           <cell r="AB117">
-            <v>27</v>
+            <v>62</v>
           </cell>
         </row>
         <row r="118">
           <cell r="A118">
-            <v>55600001</v>
+            <v>55520003</v>
           </cell>
           <cell r="AB118">
-            <v>8</v>
+            <v>27</v>
           </cell>
         </row>
         <row r="119">
           <cell r="A119">
-            <v>55600002</v>
+            <v>55600001</v>
           </cell>
           <cell r="AB119">
-            <v>10</v>
+            <v>8</v>
           </cell>
         </row>
         <row r="120">
           <cell r="A120">
-            <v>55600004</v>
+            <v>55600002</v>
           </cell>
           <cell r="AB120">
-            <v>8</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="121">
           <cell r="A121">
-            <v>55600005</v>
+            <v>55600004</v>
           </cell>
           <cell r="AB121">
-            <v>15</v>
+            <v>8</v>
           </cell>
         </row>
         <row r="122">
           <cell r="A122">
-            <v>55600006</v>
+            <v>55600005</v>
           </cell>
           <cell r="AB122">
             <v>15</v>
@@ -3918,111 +3918,111 @@
         </row>
         <row r="123">
           <cell r="A123">
-            <v>55600007</v>
+            <v>55600006</v>
           </cell>
           <cell r="AB123">
-            <v>20</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="124">
           <cell r="A124">
-            <v>55600008</v>
+            <v>55600007</v>
           </cell>
           <cell r="AB124">
-            <v>30</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="125">
           <cell r="A125">
-            <v>55600009</v>
+            <v>55600008</v>
           </cell>
           <cell r="AB125">
-            <v>13</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="126">
           <cell r="A126">
-            <v>55600010</v>
+            <v>55600009</v>
           </cell>
           <cell r="AB126">
-            <v>30</v>
+            <v>13</v>
           </cell>
         </row>
         <row r="127">
           <cell r="A127">
-            <v>55600011</v>
+            <v>55600010</v>
           </cell>
           <cell r="AB127">
-            <v>20</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="128">
           <cell r="A128">
-            <v>55600012</v>
+            <v>55600011</v>
           </cell>
           <cell r="AB128">
-            <v>30</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="129">
           <cell r="A129">
-            <v>55600013</v>
+            <v>55600012</v>
           </cell>
           <cell r="AB129">
-            <v>15</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="130">
           <cell r="A130">
-            <v>55600014</v>
+            <v>55600013</v>
           </cell>
           <cell r="AB130">
-            <v>30</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="131">
           <cell r="A131">
-            <v>55600015</v>
+            <v>55600014</v>
           </cell>
           <cell r="AB131">
-            <v>10</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="132">
           <cell r="A132">
-            <v>55600016</v>
+            <v>55600015</v>
           </cell>
           <cell r="AB132">
-            <v>15</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="133">
           <cell r="A133">
-            <v>55600017</v>
+            <v>55600016</v>
           </cell>
           <cell r="AB133">
-            <v>20</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="134">
           <cell r="A134">
-            <v>55610001</v>
+            <v>55600017</v>
           </cell>
           <cell r="AB134">
-            <v>30</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="135">
           <cell r="A135">
-            <v>55610002</v>
+            <v>55610001</v>
           </cell>
           <cell r="AB135">
-            <v>5</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="136">
           <cell r="A136">
-            <v>55610003</v>
+            <v>55610002</v>
           </cell>
           <cell r="AB136">
             <v>5</v>
@@ -4030,23 +4030,23 @@
         </row>
         <row r="137">
           <cell r="A137">
-            <v>55610004</v>
+            <v>55610003</v>
           </cell>
           <cell r="AB137">
-            <v>10</v>
+            <v>5</v>
           </cell>
         </row>
         <row r="138">
           <cell r="A138">
-            <v>55700001</v>
+            <v>55610004</v>
           </cell>
           <cell r="AB138">
-            <v>20</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="139">
           <cell r="A139">
-            <v>55700002</v>
+            <v>55700001</v>
           </cell>
           <cell r="AB139">
             <v>20</v>
@@ -4054,7 +4054,7 @@
         </row>
         <row r="140">
           <cell r="A140">
-            <v>55700003</v>
+            <v>55700002</v>
           </cell>
           <cell r="AB140">
             <v>20</v>
@@ -4062,7 +4062,7 @@
         </row>
         <row r="141">
           <cell r="A141">
-            <v>55700004</v>
+            <v>55700003</v>
           </cell>
           <cell r="AB141">
             <v>20</v>
@@ -4070,31 +4070,31 @@
         </row>
         <row r="142">
           <cell r="A142">
-            <v>55700005</v>
+            <v>55700004</v>
           </cell>
           <cell r="AB142">
-            <v>40</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="143">
           <cell r="A143">
-            <v>55700006</v>
+            <v>55700005</v>
           </cell>
           <cell r="AB143">
-            <v>50</v>
+            <v>40</v>
           </cell>
         </row>
         <row r="144">
           <cell r="A144">
-            <v>55700007</v>
+            <v>55700006</v>
           </cell>
           <cell r="AB144">
-            <v>35</v>
+            <v>50</v>
           </cell>
         </row>
         <row r="145">
           <cell r="A145">
-            <v>55900001</v>
+            <v>55700007</v>
           </cell>
           <cell r="AB145">
             <v>35</v>
@@ -4102,191 +4102,191 @@
         </row>
         <row r="146">
           <cell r="A146">
-            <v>55900002</v>
+            <v>55900001</v>
           </cell>
           <cell r="AB146">
-            <v>30</v>
+            <v>35</v>
           </cell>
         </row>
         <row r="147">
           <cell r="A147">
-            <v>55900003</v>
+            <v>55900002</v>
           </cell>
           <cell r="AB147">
-            <v>80</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="148">
           <cell r="A148">
-            <v>55900004</v>
+            <v>55900003</v>
           </cell>
           <cell r="AB148">
-            <v>15</v>
+            <v>80</v>
           </cell>
         </row>
         <row r="149">
           <cell r="A149">
-            <v>55900005</v>
+            <v>55900004</v>
           </cell>
           <cell r="AB149">
-            <v>20</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="150">
           <cell r="A150">
-            <v>55900006</v>
+            <v>55900005</v>
           </cell>
           <cell r="AB150">
-            <v>35</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="151">
           <cell r="A151">
-            <v>55900007</v>
+            <v>55900006</v>
           </cell>
           <cell r="AB151">
-            <v>25</v>
+            <v>35</v>
           </cell>
         </row>
         <row r="152">
           <cell r="A152">
-            <v>55900008</v>
+            <v>55900007</v>
           </cell>
           <cell r="AB152">
-            <v>40</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="153">
           <cell r="A153">
-            <v>55900009</v>
+            <v>55900008</v>
           </cell>
           <cell r="AB153">
-            <v>30</v>
+            <v>40</v>
           </cell>
         </row>
         <row r="154">
           <cell r="A154">
-            <v>55900010</v>
+            <v>55900009</v>
           </cell>
           <cell r="AB154">
-            <v>20</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="155">
           <cell r="A155">
-            <v>55900011</v>
+            <v>55900010</v>
           </cell>
           <cell r="AB155">
-            <v>15</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="156">
           <cell r="A156">
-            <v>55900012</v>
+            <v>55900011</v>
           </cell>
           <cell r="AB156">
-            <v>25</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="157">
           <cell r="A157">
-            <v>55900013</v>
+            <v>55900012</v>
           </cell>
           <cell r="AB157">
-            <v>10</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="158">
           <cell r="A158">
-            <v>55900014</v>
+            <v>55900013</v>
           </cell>
           <cell r="AB158">
-            <v>20</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="159">
           <cell r="A159">
-            <v>55900015</v>
+            <v>55900014</v>
           </cell>
           <cell r="AB159">
-            <v>30</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="160">
           <cell r="A160">
-            <v>55900016</v>
+            <v>55900015</v>
           </cell>
           <cell r="AB160">
-            <v>45</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="161">
           <cell r="A161">
-            <v>55900017</v>
+            <v>55900016</v>
           </cell>
           <cell r="AB161">
-            <v>10</v>
+            <v>45</v>
           </cell>
         </row>
         <row r="162">
           <cell r="A162">
-            <v>55900018</v>
+            <v>55900017</v>
           </cell>
           <cell r="AB162">
-            <v>30</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="163">
           <cell r="A163">
-            <v>55900019</v>
+            <v>55900018</v>
           </cell>
           <cell r="AB163">
-            <v>80</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="164">
           <cell r="A164">
-            <v>55900020</v>
+            <v>55900019</v>
           </cell>
           <cell r="AB164">
-            <v>20</v>
+            <v>80</v>
           </cell>
         </row>
         <row r="165">
           <cell r="A165">
-            <v>55900021</v>
+            <v>55900020</v>
           </cell>
           <cell r="AB165">
-            <v>10</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="166">
           <cell r="A166">
-            <v>55900022</v>
+            <v>55900021</v>
           </cell>
           <cell r="AB166">
-            <v>20</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="167">
           <cell r="A167">
-            <v>55900023</v>
+            <v>55900022</v>
           </cell>
           <cell r="AB167">
-            <v>25</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="168">
           <cell r="A168">
-            <v>55900024</v>
+            <v>55900023</v>
           </cell>
           <cell r="AB168">
-            <v>10</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="169">
           <cell r="A169">
-            <v>55900025</v>
+            <v>55900024</v>
           </cell>
           <cell r="AB169">
             <v>10</v>
@@ -4294,37 +4294,37 @@
         </row>
         <row r="170">
           <cell r="A170">
-            <v>55900026</v>
+            <v>55900025</v>
           </cell>
           <cell r="AB170">
-            <v>20</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="171">
           <cell r="A171">
-            <v>55900027</v>
+            <v>55900026</v>
           </cell>
           <cell r="AB171">
-            <v>35</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="172">
           <cell r="A172">
-            <v>55900028</v>
-          </cell>
-          <cell r="AB172"/>
+            <v>55900027</v>
+          </cell>
+          <cell r="AB172">
+            <v>35</v>
+          </cell>
         </row>
         <row r="173">
           <cell r="A173">
-            <v>55900029</v>
-          </cell>
-          <cell r="AB173">
-            <v>15</v>
-          </cell>
+            <v>55900028</v>
+          </cell>
+          <cell r="AB173"/>
         </row>
         <row r="174">
           <cell r="A174">
-            <v>55900030</v>
+            <v>55900029</v>
           </cell>
           <cell r="AB174">
             <v>15</v>
@@ -4332,23 +4332,23 @@
         </row>
         <row r="175">
           <cell r="A175">
-            <v>55900031</v>
+            <v>55900030</v>
           </cell>
           <cell r="AB175">
-            <v>5</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="176">
           <cell r="A176">
-            <v>55900032</v>
+            <v>55900031</v>
           </cell>
           <cell r="AB176">
-            <v>20</v>
+            <v>5</v>
           </cell>
         </row>
         <row r="177">
           <cell r="A177">
-            <v>55900033</v>
+            <v>55900032</v>
           </cell>
           <cell r="AB177">
             <v>20</v>
@@ -4356,15 +4356,15 @@
         </row>
         <row r="178">
           <cell r="A178">
-            <v>55900034</v>
+            <v>55900033</v>
           </cell>
           <cell r="AB178">
-            <v>14</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="179">
           <cell r="A179">
-            <v>55900035</v>
+            <v>55900034</v>
           </cell>
           <cell r="AB179">
             <v>14</v>
@@ -4372,31 +4372,31 @@
         </row>
         <row r="180">
           <cell r="A180">
-            <v>55900036</v>
+            <v>55900035</v>
           </cell>
           <cell r="AB180">
-            <v>50</v>
+            <v>14</v>
           </cell>
         </row>
         <row r="181">
           <cell r="A181">
-            <v>55900037</v>
+            <v>55900036</v>
           </cell>
           <cell r="AB181">
-            <v>35</v>
+            <v>50</v>
           </cell>
         </row>
         <row r="182">
           <cell r="A182">
-            <v>55900038</v>
+            <v>55900037</v>
           </cell>
           <cell r="AB182">
-            <v>40</v>
+            <v>35</v>
           </cell>
         </row>
         <row r="183">
           <cell r="A183">
-            <v>55900039</v>
+            <v>55900038</v>
           </cell>
           <cell r="AB183">
             <v>40</v>
@@ -4404,55 +4404,55 @@
         </row>
         <row r="184">
           <cell r="A184">
-            <v>55900040</v>
+            <v>55900039</v>
           </cell>
           <cell r="AB184">
-            <v>30</v>
+            <v>40</v>
           </cell>
         </row>
         <row r="185">
           <cell r="A185">
-            <v>55900041</v>
+            <v>55900040</v>
           </cell>
           <cell r="AB185">
-            <v>0</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="186">
           <cell r="A186">
-            <v>55900042</v>
+            <v>55900041</v>
           </cell>
           <cell r="AB186">
-            <v>25</v>
+            <v>0</v>
           </cell>
         </row>
         <row r="187">
           <cell r="A187">
-            <v>55900043</v>
+            <v>55900042</v>
           </cell>
           <cell r="AB187">
-            <v>30</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="188">
           <cell r="A188">
-            <v>55900044</v>
+            <v>55900043</v>
           </cell>
           <cell r="AB188">
-            <v>40</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="189">
           <cell r="A189">
-            <v>55900045</v>
+            <v>55900044</v>
           </cell>
           <cell r="AB189">
-            <v>25</v>
+            <v>40</v>
           </cell>
         </row>
         <row r="190">
           <cell r="A190">
-            <v>55900046</v>
+            <v>55900045</v>
           </cell>
           <cell r="AB190">
             <v>25</v>
@@ -4460,71 +4460,71 @@
         </row>
         <row r="191">
           <cell r="A191">
-            <v>55900047</v>
+            <v>55900046</v>
           </cell>
           <cell r="AB191">
-            <v>30</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="192">
           <cell r="A192">
-            <v>55900048</v>
+            <v>55900047</v>
           </cell>
           <cell r="AB192">
-            <v>60</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="193">
           <cell r="A193">
-            <v>55900049</v>
+            <v>55900048</v>
           </cell>
           <cell r="AB193">
-            <v>25</v>
+            <v>60</v>
           </cell>
         </row>
         <row r="194">
           <cell r="A194">
-            <v>55900050</v>
+            <v>55900049</v>
           </cell>
           <cell r="AB194">
-            <v>20</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="195">
           <cell r="A195">
-            <v>55900051</v>
+            <v>55900050</v>
           </cell>
           <cell r="AB195">
-            <v>25</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="196">
           <cell r="A196">
-            <v>55900052</v>
+            <v>55900051</v>
           </cell>
           <cell r="AB196">
-            <v>5</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="197">
           <cell r="A197">
-            <v>55900053</v>
+            <v>55900052</v>
           </cell>
           <cell r="AB197">
-            <v>30</v>
+            <v>5</v>
           </cell>
         </row>
         <row r="198">
           <cell r="A198">
-            <v>55900054</v>
+            <v>55900053</v>
           </cell>
           <cell r="AB198">
-            <v>15</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="199">
           <cell r="A199">
-            <v>55900055</v>
+            <v>55900054</v>
           </cell>
           <cell r="AB199">
             <v>15</v>
@@ -4532,71 +4532,71 @@
         </row>
         <row r="200">
           <cell r="A200">
-            <v>55900056</v>
+            <v>55900055</v>
           </cell>
           <cell r="AB200">
-            <v>10</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="201">
           <cell r="A201">
-            <v>55900057</v>
+            <v>55900056</v>
           </cell>
           <cell r="AB201">
-            <v>40</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="202">
           <cell r="A202">
-            <v>55900058</v>
+            <v>55900057</v>
           </cell>
           <cell r="AB202">
-            <v>80</v>
+            <v>40</v>
           </cell>
         </row>
         <row r="203">
           <cell r="A203">
-            <v>55900059</v>
+            <v>55900058</v>
           </cell>
           <cell r="AB203">
-            <v>-30</v>
+            <v>80</v>
           </cell>
         </row>
         <row r="204">
           <cell r="A204">
-            <v>55900060</v>
+            <v>55900059</v>
           </cell>
           <cell r="AB204">
-            <v>60</v>
+            <v>-30</v>
           </cell>
         </row>
         <row r="205">
           <cell r="A205">
-            <v>55900061</v>
+            <v>55900060</v>
           </cell>
           <cell r="AB205">
-            <v>20</v>
+            <v>60</v>
           </cell>
         </row>
         <row r="206">
           <cell r="A206">
-            <v>55900062</v>
+            <v>55900061</v>
           </cell>
           <cell r="AB206">
-            <v>15</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="207">
           <cell r="A207">
-            <v>55990001</v>
+            <v>55900062</v>
           </cell>
           <cell r="AB207">
-            <v>10</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="208">
           <cell r="A208">
-            <v>55990002</v>
+            <v>55990001</v>
           </cell>
           <cell r="AB208">
             <v>10</v>
@@ -4604,7 +4604,7 @@
         </row>
         <row r="209">
           <cell r="A209">
-            <v>55990003</v>
+            <v>55990002</v>
           </cell>
           <cell r="AB209">
             <v>10</v>
@@ -4612,7 +4612,7 @@
         </row>
         <row r="210">
           <cell r="A210">
-            <v>55990004</v>
+            <v>55990003</v>
           </cell>
           <cell r="AB210">
             <v>10</v>
@@ -4620,7 +4620,7 @@
         </row>
         <row r="211">
           <cell r="A211">
-            <v>55990005</v>
+            <v>55990004</v>
           </cell>
           <cell r="AB211">
             <v>10</v>
@@ -4628,7 +4628,7 @@
         </row>
         <row r="212">
           <cell r="A212">
-            <v>55990006</v>
+            <v>55990005</v>
           </cell>
           <cell r="AB212">
             <v>10</v>
@@ -4636,7 +4636,7 @@
         </row>
         <row r="213">
           <cell r="A213">
-            <v>55990011</v>
+            <v>55990006</v>
           </cell>
           <cell r="AB213">
             <v>10</v>
@@ -4644,7 +4644,7 @@
         </row>
         <row r="214">
           <cell r="A214">
-            <v>55990012</v>
+            <v>55990011</v>
           </cell>
           <cell r="AB214">
             <v>10</v>
@@ -4652,7 +4652,7 @@
         </row>
         <row r="215">
           <cell r="A215">
-            <v>55990013</v>
+            <v>55990012</v>
           </cell>
           <cell r="AB215">
             <v>10</v>
@@ -4660,7 +4660,7 @@
         </row>
         <row r="216">
           <cell r="A216">
-            <v>55990014</v>
+            <v>55990013</v>
           </cell>
           <cell r="AB216">
             <v>10</v>
@@ -4668,7 +4668,7 @@
         </row>
         <row r="217">
           <cell r="A217">
-            <v>55990015</v>
+            <v>55990014</v>
           </cell>
           <cell r="AB217">
             <v>10</v>
@@ -4676,7 +4676,7 @@
         </row>
         <row r="218">
           <cell r="A218">
-            <v>55990016</v>
+            <v>55990015</v>
           </cell>
           <cell r="AB218">
             <v>10</v>
@@ -4684,74 +4684,98 @@
         </row>
         <row r="219">
           <cell r="A219">
-            <v>55990101</v>
+            <v>55990016</v>
           </cell>
           <cell r="AB219">
-            <v>15</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="220">
           <cell r="A220">
-            <v>55990102</v>
+            <v>55990101</v>
           </cell>
           <cell r="AB220">
-            <v>25</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="221">
           <cell r="A221">
-            <v>55990103</v>
+            <v>55990102</v>
           </cell>
           <cell r="AB221">
-            <v>35</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="222">
           <cell r="A222">
-            <v>55990104</v>
+            <v>55990103</v>
           </cell>
           <cell r="AB222">
-            <v>50</v>
+            <v>35</v>
           </cell>
         </row>
         <row r="223">
           <cell r="A223">
-            <v>55990105</v>
+            <v>55990104</v>
           </cell>
           <cell r="AB223">
-            <v>150</v>
+            <v>50</v>
           </cell>
         </row>
         <row r="224">
           <cell r="A224">
-            <v>55990106</v>
+            <v>55990105</v>
           </cell>
           <cell r="AB224">
-            <v>80</v>
+            <v>150</v>
           </cell>
         </row>
         <row r="225">
           <cell r="A225">
-            <v>55990107</v>
+            <v>55990106</v>
           </cell>
           <cell r="AB225">
-            <v>50</v>
+            <v>80</v>
           </cell>
         </row>
         <row r="226">
           <cell r="A226">
-            <v>55990108</v>
+            <v>55990107</v>
           </cell>
           <cell r="AB226">
-            <v>4</v>
+            <v>50</v>
           </cell>
         </row>
         <row r="227">
           <cell r="A227">
+            <v>55990108</v>
+          </cell>
+          <cell r="AB227">
+            <v>4</v>
+          </cell>
+        </row>
+        <row r="228">
+          <cell r="A228">
             <v>55990109</v>
           </cell>
-          <cell r="AB227">
+          <cell r="AB228">
             <v>15</v>
+          </cell>
+        </row>
+        <row r="229">
+          <cell r="A229">
+            <v>55990110</v>
+          </cell>
+          <cell r="AB229">
+            <v>25</v>
+          </cell>
+        </row>
+        <row r="230">
+          <cell r="A230">
+            <v>55990111</v>
+          </cell>
+          <cell r="AB230">
+            <v>50</v>
           </cell>
         </row>
       </sheetData>
@@ -5136,8 +5160,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="H61" sqref="H61"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="W9" sqref="W9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -5168,13 +5192,13 @@
         <v>3</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>204</v>
+        <v>191</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>313</v>
+        <v>300</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>281</v>
+        <v>268</v>
       </c>
       <c r="F1" s="11" t="s">
         <v>4</v>
@@ -5183,10 +5207,10 @@
         <v>5</v>
       </c>
       <c r="H1" s="11" t="s">
-        <v>278</v>
+        <v>265</v>
       </c>
       <c r="I1" s="11" t="s">
-        <v>270</v>
+        <v>257</v>
       </c>
       <c r="J1" s="12" t="s">
         <v>12</v>
@@ -5195,7 +5219,7 @@
         <v>14</v>
       </c>
       <c r="L1" s="12" t="s">
-        <v>275</v>
+        <v>262</v>
       </c>
       <c r="M1" s="13" t="s">
         <v>40</v>
@@ -5225,7 +5249,7 @@
         <v>34</v>
       </c>
       <c r="V1" s="15" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="W1" s="15" t="s">
         <v>57</v>
@@ -5234,13 +5258,13 @@
         <v>35</v>
       </c>
       <c r="Y1" s="15" t="s">
-        <v>259</v>
+        <v>246</v>
       </c>
       <c r="Z1" s="15" t="s">
         <v>36</v>
       </c>
       <c r="AA1" s="15" t="s">
-        <v>273</v>
+        <v>260</v>
       </c>
       <c r="AB1" s="15" t="s">
         <v>32</v>
@@ -5272,13 +5296,13 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>314</v>
+        <v>301</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>282</v>
+        <v>269</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>0</v>
@@ -5287,7 +5311,7 @@
         <v>0</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>279</v>
+        <v>266</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>0</v>
@@ -5299,7 +5323,7 @@
         <v>15</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>276</v>
+        <v>263</v>
       </c>
       <c r="M2" s="9" t="s">
         <v>0</v>
@@ -5329,7 +5353,7 @@
         <v>0</v>
       </c>
       <c r="V2" s="7" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="W2" s="7" t="s">
         <v>58</v>
@@ -5338,7 +5362,7 @@
         <v>37</v>
       </c>
       <c r="Y2" s="7" t="s">
-        <v>260</v>
+        <v>247</v>
       </c>
       <c r="Z2" s="7" t="s">
         <v>0</v>
@@ -5376,13 +5400,13 @@
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>206</v>
+        <v>193</v>
       </c>
       <c r="D3" t="s">
-        <v>315</v>
+        <v>302</v>
       </c>
       <c r="E3" t="s">
-        <v>283</v>
+        <v>270</v>
       </c>
       <c r="F3" t="s">
         <v>9</v>
@@ -5391,19 +5415,19 @@
         <v>10</v>
       </c>
       <c r="H3" t="s">
-        <v>280</v>
+        <v>267</v>
       </c>
       <c r="I3" t="s">
-        <v>269</v>
+        <v>256</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>271</v>
+        <v>258</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>272</v>
+        <v>259</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>277</v>
+        <v>264</v>
       </c>
       <c r="M3" s="10" t="s">
         <v>48</v>
@@ -5433,7 +5457,7 @@
         <v>18</v>
       </c>
       <c r="V3" s="8" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="W3" s="8" t="s">
         <v>59</v>
@@ -5442,13 +5466,13 @@
         <v>22</v>
       </c>
       <c r="Y3" s="8" t="s">
-        <v>261</v>
+        <v>248</v>
       </c>
       <c r="Z3" s="8" t="s">
         <v>19</v>
       </c>
       <c r="AA3" s="8" t="s">
-        <v>274</v>
+        <v>261</v>
       </c>
       <c r="AB3" s="8" t="s">
         <v>31</v>
@@ -5480,7 +5504,7 @@
         <v>60</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>266</v>
+        <v>253</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -5511,11 +5535,11 @@
       <c r="S4" s="16"/>
       <c r="T4" s="16">
         <f t="shared" ref="T4:T62" si="1">J4+K4+L4+ SUM(M4:S4)*5+AB4+AC4</f>
-        <v>-5</v>
+        <v>-15</v>
       </c>
       <c r="U4" s="16"/>
       <c r="V4" s="16"/>
-      <c r="W4" s="16" t="s">
+      <c r="W4" s="25" t="s">
         <v>70</v>
       </c>
       <c r="X4" s="16" t="s">
@@ -5525,7 +5549,7 @@
       <c r="Z4" s="16"/>
       <c r="AA4" s="16"/>
       <c r="AB4" s="16">
-        <v>-10</v>
+        <v>-20</v>
       </c>
       <c r="AC4" s="16">
         <f>IF(ISBLANK(AD4),0, LOOKUP(AD4,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AE4/100)</f>
@@ -5551,7 +5575,7 @@
         <v>72</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -5586,8 +5610,8 @@
       </c>
       <c r="U5" s="16"/>
       <c r="V5" s="16"/>
-      <c r="W5" s="16" t="s">
-        <v>74</v>
+      <c r="W5" s="25" t="s">
+        <v>328</v>
       </c>
       <c r="X5" s="16" t="s">
         <v>16</v>
@@ -5619,10 +5643,10 @@
         <v>21100003</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>208</v>
+        <v>195</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -5657,8 +5681,8 @@
       </c>
       <c r="U6" s="16"/>
       <c r="V6" s="16"/>
-      <c r="W6" s="16" t="s">
-        <v>77</v>
+      <c r="W6" s="25" t="s">
+        <v>319</v>
       </c>
       <c r="X6" s="16" t="s">
         <v>16</v>
@@ -5680,7 +5704,7 @@
         <v>23</v>
       </c>
       <c r="AH6" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.15">
@@ -5688,10 +5712,10 @@
         <v>21100004</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -5728,11 +5752,11 @@
       </c>
       <c r="U7" s="16"/>
       <c r="V7" s="16"/>
-      <c r="W7" s="16" t="s">
-        <v>81</v>
+      <c r="W7" s="25" t="s">
+        <v>320</v>
       </c>
       <c r="X7" s="16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="Y7" s="16"/>
       <c r="Z7" s="16"/>
@@ -5753,7 +5777,7 @@
         <v>23</v>
       </c>
       <c r="AH7" s="16" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.15">
@@ -5761,10 +5785,10 @@
         <v>21100005</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>210</v>
+        <v>197</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -5801,11 +5825,11 @@
       </c>
       <c r="U8" s="16"/>
       <c r="V8" s="16"/>
-      <c r="W8" s="16" t="s">
-        <v>84</v>
+      <c r="W8" s="25" t="s">
+        <v>326</v>
       </c>
       <c r="X8" s="16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="Y8" s="16"/>
       <c r="Z8" s="16"/>
@@ -5824,7 +5848,7 @@
         <v>23</v>
       </c>
       <c r="AH8" s="16" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.15">
@@ -5832,10 +5856,10 @@
         <v>21100006</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>211</v>
+        <v>198</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -5872,11 +5896,11 @@
       </c>
       <c r="U9" s="16"/>
       <c r="V9" s="16"/>
-      <c r="W9" s="16" t="s">
-        <v>87</v>
+      <c r="W9" s="25" t="s">
+        <v>327</v>
       </c>
       <c r="X9" s="16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="Y9" s="16"/>
       <c r="Z9" s="16"/>
@@ -5895,7 +5919,7 @@
         <v>23</v>
       </c>
       <c r="AH9" s="16" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:34" x14ac:dyDescent="0.15">
@@ -5903,10 +5927,10 @@
         <v>21100007</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>212</v>
+        <v>199</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -5943,11 +5967,11 @@
       </c>
       <c r="U10" s="16"/>
       <c r="V10" s="16"/>
-      <c r="W10" s="16" t="s">
-        <v>74</v>
+      <c r="W10" s="25" t="s">
+        <v>318</v>
       </c>
       <c r="X10" s="16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="Y10" s="16"/>
       <c r="Z10" s="16"/>
@@ -5966,7 +5990,7 @@
         <v>23</v>
       </c>
       <c r="AH10" s="16" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:34" x14ac:dyDescent="0.15">
@@ -5974,10 +5998,10 @@
         <v>21100008</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>213</v>
+        <v>200</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -6014,11 +6038,11 @@
       </c>
       <c r="U11" s="16"/>
       <c r="V11" s="16"/>
-      <c r="W11" s="16" t="s">
-        <v>152</v>
+      <c r="W11" s="25" t="s">
+        <v>322</v>
       </c>
       <c r="X11" s="16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="Y11" s="16"/>
       <c r="Z11" s="16"/>
@@ -6037,7 +6061,7 @@
         <v>23</v>
       </c>
       <c r="AH11" s="16" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
     </row>
     <row r="12" spans="1:34" x14ac:dyDescent="0.15">
@@ -6045,10 +6069,10 @@
         <v>21100009</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>214</v>
+        <v>201</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -6085,11 +6109,11 @@
       </c>
       <c r="U12" s="16"/>
       <c r="V12" s="16"/>
-      <c r="W12" s="16" t="s">
-        <v>156</v>
+      <c r="W12" s="25" t="s">
+        <v>323</v>
       </c>
       <c r="X12" s="16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="Y12" s="16"/>
       <c r="Z12" s="16"/>
@@ -6108,7 +6132,7 @@
         <v>23</v>
       </c>
       <c r="AH12" s="16" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
     </row>
     <row r="13" spans="1:34" x14ac:dyDescent="0.15">
@@ -6116,10 +6140,10 @@
         <v>21100010</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>215</v>
+        <v>202</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -6156,11 +6180,11 @@
       </c>
       <c r="U13" s="16"/>
       <c r="V13" s="16"/>
-      <c r="W13" s="16" t="s">
-        <v>159</v>
+      <c r="W13" s="25" t="s">
+        <v>316</v>
       </c>
       <c r="X13" s="16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="Y13" s="16"/>
       <c r="Z13" s="16"/>
@@ -6179,7 +6203,7 @@
         <v>23</v>
       </c>
       <c r="AH13" s="16" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
     </row>
     <row r="14" spans="1:34" x14ac:dyDescent="0.15">
@@ -6187,10 +6211,10 @@
         <v>21100011</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>216</v>
+        <v>203</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -6227,11 +6251,11 @@
       </c>
       <c r="U14" s="16"/>
       <c r="V14" s="16"/>
-      <c r="W14" s="16" t="s">
-        <v>162</v>
+      <c r="W14" s="25" t="s">
+        <v>319</v>
       </c>
       <c r="X14" s="16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="Y14" s="16"/>
       <c r="Z14" s="16"/>
@@ -6250,7 +6274,7 @@
         <v>23</v>
       </c>
       <c r="AH14" s="16" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
     </row>
     <row r="15" spans="1:34" x14ac:dyDescent="0.15">
@@ -6258,10 +6282,10 @@
         <v>21100012</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>217</v>
+        <v>204</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -6298,11 +6322,11 @@
       </c>
       <c r="U15" s="16"/>
       <c r="V15" s="16"/>
-      <c r="W15" s="16" t="s">
-        <v>174</v>
+      <c r="W15" s="25" t="s">
+        <v>324</v>
       </c>
       <c r="X15" s="16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="Y15" s="16"/>
       <c r="Z15" s="16"/>
@@ -6321,7 +6345,7 @@
         <v>23</v>
       </c>
       <c r="AH15" s="16" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
     </row>
     <row r="16" spans="1:34" x14ac:dyDescent="0.15">
@@ -6329,10 +6353,10 @@
         <v>21100013</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>218</v>
+        <v>205</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -6369,11 +6393,11 @@
       </c>
       <c r="U16" s="16"/>
       <c r="V16" s="16"/>
-      <c r="W16" s="16" t="s">
-        <v>178</v>
+      <c r="W16" s="25" t="s">
+        <v>317</v>
       </c>
       <c r="X16" s="16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="Y16" s="16"/>
       <c r="Z16" s="16"/>
@@ -6392,7 +6416,7 @@
         <v>23</v>
       </c>
       <c r="AH16" s="16" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
     </row>
     <row r="17" spans="1:34" x14ac:dyDescent="0.15">
@@ -6400,10 +6424,10 @@
         <v>21100014</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>219</v>
+        <v>206</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -6440,11 +6464,11 @@
       </c>
       <c r="U17" s="16"/>
       <c r="V17" s="16"/>
-      <c r="W17" s="16" t="s">
-        <v>181</v>
+      <c r="W17" s="25" t="s">
+        <v>325</v>
       </c>
       <c r="X17" s="16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="Y17" s="16"/>
       <c r="Z17" s="16"/>
@@ -6465,7 +6489,7 @@
         <v>23</v>
       </c>
       <c r="AH17" s="16" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
     </row>
     <row r="18" spans="1:34" x14ac:dyDescent="0.15">
@@ -6473,10 +6497,10 @@
         <v>21100015</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>220</v>
+        <v>207</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -6511,11 +6535,11 @@
       </c>
       <c r="U18" s="16"/>
       <c r="V18" s="16"/>
-      <c r="W18" s="16" t="s">
-        <v>184</v>
+      <c r="W18" s="25" t="s">
+        <v>321</v>
       </c>
       <c r="X18" s="16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="Y18" s="16"/>
       <c r="Z18" s="16"/>
@@ -6536,7 +6560,7 @@
         <v>23</v>
       </c>
       <c r="AH18" s="16" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="19" spans="1:34" x14ac:dyDescent="0.15">
@@ -6547,7 +6571,7 @@
         <v>63</v>
       </c>
       <c r="C19" s="21" t="s">
-        <v>221</v>
+        <v>208</v>
       </c>
       <c r="D19" s="21"/>
       <c r="E19" s="1"/>
@@ -6615,10 +6639,10 @@
         <v>21200002</v>
       </c>
       <c r="B20" s="21" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C20" s="21" t="s">
-        <v>222</v>
+        <v>209</v>
       </c>
       <c r="D20" s="21"/>
       <c r="E20" s="1"/>
@@ -6655,7 +6679,7 @@
       <c r="V20" s="16"/>
       <c r="W20" s="16"/>
       <c r="X20" s="16" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="Y20" s="16"/>
       <c r="Z20" s="16"/>
@@ -6676,7 +6700,7 @@
         <v>23</v>
       </c>
       <c r="AH20" s="16" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="21" spans="1:34" x14ac:dyDescent="0.15">
@@ -6684,10 +6708,10 @@
         <v>21200003</v>
       </c>
       <c r="B21" s="21" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C21" s="21" t="s">
-        <v>223</v>
+        <v>210</v>
       </c>
       <c r="D21" s="21"/>
       <c r="E21" s="1"/>
@@ -6724,7 +6748,7 @@
       <c r="V21" s="16"/>
       <c r="W21" s="16"/>
       <c r="X21" s="16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="Y21" s="16"/>
       <c r="Z21" s="16"/>
@@ -6745,7 +6769,7 @@
         <v>23</v>
       </c>
       <c r="AH21" s="16" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="22" spans="1:34" x14ac:dyDescent="0.15">
@@ -6753,10 +6777,10 @@
         <v>21200004</v>
       </c>
       <c r="B22" s="21" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C22" s="21" t="s">
-        <v>224</v>
+        <v>211</v>
       </c>
       <c r="D22" s="21"/>
       <c r="E22" s="1"/>
@@ -6793,7 +6817,7 @@
       <c r="V22" s="16"/>
       <c r="W22" s="16"/>
       <c r="X22" s="16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="Y22" s="16"/>
       <c r="Z22" s="16"/>
@@ -6814,7 +6838,7 @@
         <v>23</v>
       </c>
       <c r="AH22" s="16" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="23" spans="1:34" x14ac:dyDescent="0.15">
@@ -6822,10 +6846,10 @@
         <v>21200005</v>
       </c>
       <c r="B23" s="21" t="s">
-        <v>187</v>
+        <v>174</v>
       </c>
       <c r="C23" s="21" t="s">
-        <v>225</v>
+        <v>212</v>
       </c>
       <c r="D23" s="21"/>
       <c r="E23" s="1"/>
@@ -6862,7 +6886,7 @@
       <c r="V23" s="16"/>
       <c r="W23" s="16"/>
       <c r="X23" s="16" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
       <c r="Y23" s="16"/>
       <c r="Z23" s="16"/>
@@ -6883,7 +6907,7 @@
         <v>23</v>
       </c>
       <c r="AH23" s="16" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
     </row>
     <row r="24" spans="1:34" x14ac:dyDescent="0.15">
@@ -6891,10 +6915,10 @@
         <v>21200006</v>
       </c>
       <c r="B24" s="21" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
       <c r="C24" s="21" t="s">
-        <v>226</v>
+        <v>213</v>
       </c>
       <c r="D24" s="21"/>
       <c r="E24" s="1"/>
@@ -6931,7 +6955,7 @@
       <c r="V24" s="16"/>
       <c r="W24" s="16"/>
       <c r="X24" s="16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="Y24" s="16"/>
       <c r="Z24" s="16"/>
@@ -6952,7 +6976,7 @@
         <v>23</v>
       </c>
       <c r="AH24" s="16" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
     </row>
     <row r="25" spans="1:34" x14ac:dyDescent="0.15">
@@ -6960,10 +6984,10 @@
         <v>21200007</v>
       </c>
       <c r="B25" s="21" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
       <c r="C25" s="21" t="s">
-        <v>227</v>
+        <v>214</v>
       </c>
       <c r="D25" s="21"/>
       <c r="E25" s="1"/>
@@ -7000,7 +7024,7 @@
       <c r="V25" s="16"/>
       <c r="W25" s="16"/>
       <c r="X25" s="16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="Y25" s="16"/>
       <c r="Z25" s="16"/>
@@ -7023,7 +7047,7 @@
         <v>23</v>
       </c>
       <c r="AH25" s="16" t="s">
-        <v>191</v>
+        <v>178</v>
       </c>
     </row>
     <row r="26" spans="1:34" x14ac:dyDescent="0.15">
@@ -7031,10 +7055,10 @@
         <v>21200008</v>
       </c>
       <c r="B26" s="21" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
       <c r="C26" s="21" t="s">
-        <v>228</v>
+        <v>215</v>
       </c>
       <c r="D26" s="21"/>
       <c r="E26" s="1"/>
@@ -7071,7 +7095,7 @@
       <c r="V26" s="16"/>
       <c r="W26" s="16"/>
       <c r="X26" s="16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="Y26" s="16"/>
       <c r="Z26" s="16"/>
@@ -7092,7 +7116,7 @@
         <v>23</v>
       </c>
       <c r="AH26" s="16" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
     </row>
     <row r="27" spans="1:34" x14ac:dyDescent="0.15">
@@ -7100,10 +7124,10 @@
         <v>21200009</v>
       </c>
       <c r="B27" s="21" t="s">
-        <v>195</v>
+        <v>182</v>
       </c>
       <c r="C27" s="21" t="s">
-        <v>229</v>
+        <v>216</v>
       </c>
       <c r="D27" s="21"/>
       <c r="E27" s="1"/>
@@ -7140,7 +7164,7 @@
       <c r="V27" s="16"/>
       <c r="W27" s="16"/>
       <c r="X27" s="16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="Y27" s="16"/>
       <c r="Z27" s="16"/>
@@ -7161,7 +7185,7 @@
         <v>23</v>
       </c>
       <c r="AH27" s="16" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
     </row>
     <row r="28" spans="1:34" x14ac:dyDescent="0.15">
@@ -7169,10 +7193,10 @@
         <v>21200010</v>
       </c>
       <c r="B28" s="21" t="s">
-        <v>197</v>
+        <v>184</v>
       </c>
       <c r="C28" s="21" t="s">
-        <v>230</v>
+        <v>217</v>
       </c>
       <c r="D28" s="21"/>
       <c r="E28" s="1"/>
@@ -7209,7 +7233,7 @@
       <c r="V28" s="16"/>
       <c r="W28" s="16"/>
       <c r="X28" s="16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="Y28" s="16"/>
       <c r="Z28" s="16"/>
@@ -7230,7 +7254,7 @@
         <v>23</v>
       </c>
       <c r="AH28" s="16" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
     </row>
     <row r="29" spans="1:34" x14ac:dyDescent="0.15">
@@ -7241,7 +7265,7 @@
         <v>65</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>231</v>
+        <v>218</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
@@ -7278,7 +7302,7 @@
       </c>
       <c r="U29" s="16"/>
       <c r="V29" s="16" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="W29" s="16"/>
       <c r="X29" s="16" t="s">
@@ -7311,14 +7335,14 @@
         <v>21300002</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>232</v>
+        <v>219</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="19" t="s">
-        <v>290</v>
+        <v>277</v>
       </c>
       <c r="F30" s="1">
         <f t="shared" si="0"/>
@@ -7353,11 +7377,11 @@
       </c>
       <c r="U30" s="16"/>
       <c r="V30" s="16" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="W30" s="16"/>
       <c r="X30" s="16" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="Y30" s="16"/>
       <c r="Z30" s="16"/>
@@ -7380,7 +7404,7 @@
         <v>23</v>
       </c>
       <c r="AH30" s="16" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="31" spans="1:34" x14ac:dyDescent="0.15">
@@ -7388,10 +7412,10 @@
         <v>21300003</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>233</v>
+        <v>220</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
@@ -7428,11 +7452,11 @@
       </c>
       <c r="U31" s="16"/>
       <c r="V31" s="16" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="W31" s="16"/>
       <c r="X31" s="16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="Y31" s="16"/>
       <c r="Z31" s="16"/>
@@ -7451,7 +7475,7 @@
         <v>23</v>
       </c>
       <c r="AH31" s="16" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="32" spans="1:34" x14ac:dyDescent="0.15">
@@ -7459,14 +7483,14 @@
         <v>21300004</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="19" t="s">
-        <v>291</v>
+        <v>278</v>
       </c>
       <c r="F32" s="1">
         <f t="shared" si="0"/>
@@ -7499,11 +7523,11 @@
       </c>
       <c r="U32" s="16"/>
       <c r="V32" s="16" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="W32" s="16"/>
       <c r="X32" s="16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="Y32" s="16"/>
       <c r="Z32" s="16"/>
@@ -7526,7 +7550,7 @@
         <v>23</v>
       </c>
       <c r="AH32" s="16" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="33" spans="1:34" x14ac:dyDescent="0.15">
@@ -7534,10 +7558,10 @@
         <v>21300005</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>299</v>
+        <v>286</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>300</v>
+        <v>287</v>
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
@@ -7572,11 +7596,11 @@
       </c>
       <c r="U33" s="16"/>
       <c r="V33" s="16" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="W33" s="16"/>
       <c r="X33" s="16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="Y33" s="16"/>
       <c r="Z33" s="16"/>
@@ -7597,7 +7621,7 @@
         <v>23</v>
       </c>
       <c r="AH33" s="16" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
     <row r="34" spans="1:34" x14ac:dyDescent="0.15">
@@ -7605,10 +7629,10 @@
         <v>21300006</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>235</v>
+        <v>222</v>
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
@@ -7645,11 +7669,11 @@
       </c>
       <c r="U34" s="16"/>
       <c r="V34" s="16" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="W34" s="16"/>
       <c r="X34" s="16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="Y34" s="16"/>
       <c r="Z34" s="16"/>
@@ -7668,7 +7692,7 @@
         <v>23</v>
       </c>
       <c r="AH34" s="16" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
     </row>
     <row r="35" spans="1:34" x14ac:dyDescent="0.15">
@@ -7676,10 +7700,10 @@
         <v>21300007</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>236</v>
+        <v>223</v>
       </c>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
@@ -7716,11 +7740,11 @@
       </c>
       <c r="U35" s="16"/>
       <c r="V35" s="16" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="W35" s="16"/>
       <c r="X35" s="16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="Y35" s="16"/>
       <c r="Z35" s="16"/>
@@ -7739,7 +7763,7 @@
         <v>23</v>
       </c>
       <c r="AH35" s="16" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="36" spans="1:34" x14ac:dyDescent="0.15">
@@ -7747,10 +7771,10 @@
         <v>21300008</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>268</v>
+        <v>255</v>
       </c>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
@@ -7785,11 +7809,11 @@
       </c>
       <c r="U36" s="16"/>
       <c r="V36" s="16" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="W36" s="16"/>
       <c r="X36" s="16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="Y36" s="16"/>
       <c r="Z36" s="16"/>
@@ -7810,7 +7834,7 @@
         <v>23</v>
       </c>
       <c r="AH36" s="16" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
     </row>
     <row r="37" spans="1:34" x14ac:dyDescent="0.15">
@@ -7818,14 +7842,14 @@
         <v>21300009</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>237</v>
+        <v>224</v>
       </c>
       <c r="D37" s="1"/>
       <c r="E37" s="19" t="s">
-        <v>292</v>
+        <v>279</v>
       </c>
       <c r="F37" s="1">
         <f t="shared" si="2"/>
@@ -7860,11 +7884,11 @@
       </c>
       <c r="U37" s="16"/>
       <c r="V37" s="16" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="W37" s="16"/>
       <c r="X37" s="16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="Y37" s="16"/>
       <c r="Z37" s="16"/>
@@ -7887,7 +7911,7 @@
         <v>23</v>
       </c>
       <c r="AH37" s="16" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
     </row>
     <row r="38" spans="1:34" x14ac:dyDescent="0.15">
@@ -7895,14 +7919,14 @@
         <v>21300010</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>294</v>
+        <v>281</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>295</v>
+        <v>282</v>
       </c>
       <c r="D38" s="1"/>
       <c r="E38" s="19" t="s">
-        <v>298</v>
+        <v>285</v>
       </c>
       <c r="F38" s="24">
         <f>IF(T38&gt;=23,4,IF(AND(T38&gt;=18,T38&lt;23),3,IF(AND(T38&gt;=13,T38&lt;18),2,IF(AND(T38&gt;=8,T38&lt;13),1,0))))</f>
@@ -7937,11 +7961,11 @@
       </c>
       <c r="U38" s="26"/>
       <c r="V38" s="26" t="s">
-        <v>296</v>
+        <v>283</v>
       </c>
       <c r="W38" s="26"/>
       <c r="X38" s="16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="Y38" s="28"/>
       <c r="Z38" s="25"/>
@@ -7964,7 +7988,7 @@
         <v>23</v>
       </c>
       <c r="AH38" s="25" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
     </row>
     <row r="39" spans="1:34" x14ac:dyDescent="0.15">
@@ -7972,10 +7996,10 @@
         <v>21300011</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>302</v>
+        <v>289</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>303</v>
+        <v>290</v>
       </c>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
@@ -8012,11 +8036,11 @@
       </c>
       <c r="U39" s="16"/>
       <c r="V39" s="16" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="W39" s="16"/>
       <c r="X39" s="16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="Y39" s="16"/>
       <c r="Z39" s="16"/>
@@ -8035,7 +8059,7 @@
         <v>23</v>
       </c>
       <c r="AH39" s="25" t="s">
-        <v>301</v>
+        <v>288</v>
       </c>
     </row>
     <row r="40" spans="1:34" x14ac:dyDescent="0.15">
@@ -8043,10 +8067,10 @@
         <v>21300012</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>306</v>
+        <v>293</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>307</v>
+        <v>294</v>
       </c>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
@@ -8081,11 +8105,11 @@
       </c>
       <c r="U40" s="16"/>
       <c r="V40" s="16" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="W40" s="16"/>
       <c r="X40" s="25" t="s">
-        <v>305</v>
+        <v>292</v>
       </c>
       <c r="Y40" s="16"/>
       <c r="Z40" s="16"/>
@@ -8104,7 +8128,7 @@
         <v>23</v>
       </c>
       <c r="AH40" s="25" t="s">
-        <v>304</v>
+        <v>291</v>
       </c>
     </row>
     <row r="41" spans="1:34" x14ac:dyDescent="0.15">
@@ -8112,10 +8136,10 @@
         <v>21400001</v>
       </c>
       <c r="B41" s="20" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="C41" s="20" t="s">
-        <v>238</v>
+        <v>225</v>
       </c>
       <c r="D41" s="20"/>
       <c r="E41" s="1"/>
@@ -8181,10 +8205,10 @@
         <v>21400002</v>
       </c>
       <c r="B42" s="20" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C42" s="20" t="s">
-        <v>239</v>
+        <v>226</v>
       </c>
       <c r="D42" s="20"/>
       <c r="E42" s="1"/>
@@ -8244,7 +8268,7 @@
         <v>23</v>
       </c>
       <c r="AH42" s="16" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="43" spans="1:34" x14ac:dyDescent="0.15">
@@ -8252,14 +8276,14 @@
         <v>21400003</v>
       </c>
       <c r="B43" s="20" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C43" s="20" t="s">
-        <v>240</v>
+        <v>227</v>
       </c>
       <c r="D43" s="20"/>
       <c r="E43" s="19" t="s">
-        <v>293</v>
+        <v>280</v>
       </c>
       <c r="F43" s="1">
         <f t="shared" si="2"/>
@@ -8294,7 +8318,7 @@
       <c r="V43" s="16"/>
       <c r="W43" s="16"/>
       <c r="X43" s="16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="Y43" s="16"/>
       <c r="Z43" s="16"/>
@@ -8317,7 +8341,7 @@
         <v>23</v>
       </c>
       <c r="AH43" s="16" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="44" spans="1:34" x14ac:dyDescent="0.15">
@@ -8325,10 +8349,10 @@
         <v>21400004</v>
       </c>
       <c r="B44" s="20" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C44" s="20" t="s">
-        <v>241</v>
+        <v>228</v>
       </c>
       <c r="D44" s="20"/>
       <c r="E44" s="1"/>
@@ -8367,7 +8391,7 @@
       <c r="V44" s="16"/>
       <c r="W44" s="16"/>
       <c r="X44" s="16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="Y44" s="16"/>
       <c r="Z44" s="16"/>
@@ -8386,7 +8410,7 @@
         <v>23</v>
       </c>
       <c r="AH44" s="16" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
     </row>
     <row r="45" spans="1:34" x14ac:dyDescent="0.15">
@@ -8394,10 +8418,10 @@
         <v>21400005</v>
       </c>
       <c r="B45" s="20" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="C45" s="20" t="s">
-        <v>242</v>
+        <v>229</v>
       </c>
       <c r="D45" s="20"/>
       <c r="E45" s="1"/>
@@ -8434,7 +8458,7 @@
       <c r="V45" s="16"/>
       <c r="W45" s="16"/>
       <c r="X45" s="16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="Y45" s="16"/>
       <c r="Z45" s="16"/>
@@ -8455,7 +8479,7 @@
         <v>23</v>
       </c>
       <c r="AH45" s="16" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="46" spans="1:34" x14ac:dyDescent="0.15">
@@ -8463,10 +8487,10 @@
         <v>21400006</v>
       </c>
       <c r="B46" s="20" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C46" s="20" t="s">
-        <v>243</v>
+        <v>230</v>
       </c>
       <c r="D46" s="20"/>
       <c r="E46" s="1"/>
@@ -8505,7 +8529,7 @@
       <c r="V46" s="16"/>
       <c r="W46" s="16"/>
       <c r="X46" s="16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="Y46" s="16"/>
       <c r="Z46" s="16"/>
@@ -8524,7 +8548,7 @@
         <v>23</v>
       </c>
       <c r="AH46" s="16" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
     <row r="47" spans="1:34" x14ac:dyDescent="0.15">
@@ -8532,10 +8556,10 @@
         <v>21400007</v>
       </c>
       <c r="B47" s="20" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="C47" s="20" t="s">
-        <v>244</v>
+        <v>231</v>
       </c>
       <c r="D47" s="20"/>
       <c r="E47" s="1"/>
@@ -8574,7 +8598,7 @@
       <c r="V47" s="16"/>
       <c r="W47" s="16"/>
       <c r="X47" s="16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="Y47" s="16"/>
       <c r="Z47" s="16"/>
@@ -8593,7 +8617,7 @@
         <v>23</v>
       </c>
       <c r="AH47" s="16" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="48" spans="1:34" x14ac:dyDescent="0.15">
@@ -8601,10 +8625,10 @@
         <v>21400008</v>
       </c>
       <c r="B48" s="20" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="C48" s="20" t="s">
-        <v>267</v>
+        <v>254</v>
       </c>
       <c r="D48" s="20"/>
       <c r="E48" s="1"/>
@@ -8643,7 +8667,7 @@
       <c r="V48" s="16"/>
       <c r="W48" s="16"/>
       <c r="X48" s="16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="Y48" s="16"/>
       <c r="Z48" s="16"/>
@@ -8662,7 +8686,7 @@
         <v>23</v>
       </c>
       <c r="AH48" s="16" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="49" spans="1:34" x14ac:dyDescent="0.15">
@@ -8670,10 +8694,10 @@
         <v>21400009</v>
       </c>
       <c r="B49" s="20" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="C49" s="20" t="s">
-        <v>245</v>
+        <v>232</v>
       </c>
       <c r="D49" s="20"/>
       <c r="E49" s="1"/>
@@ -8712,7 +8736,7 @@
       <c r="V49" s="16"/>
       <c r="W49" s="16"/>
       <c r="X49" s="16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="Y49" s="16"/>
       <c r="Z49" s="16"/>
@@ -8731,7 +8755,7 @@
         <v>23</v>
       </c>
       <c r="AH49" s="16" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
     </row>
     <row r="50" spans="1:34" x14ac:dyDescent="0.15">
@@ -8739,10 +8763,10 @@
         <v>21400010</v>
       </c>
       <c r="B50" s="20" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="C50" s="20" t="s">
-        <v>246</v>
+        <v>233</v>
       </c>
       <c r="D50" s="20"/>
       <c r="E50" s="1"/>
@@ -8781,7 +8805,7 @@
       <c r="V50" s="16"/>
       <c r="W50" s="16"/>
       <c r="X50" s="16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="Y50" s="16"/>
       <c r="Z50" s="16"/>
@@ -8800,7 +8824,7 @@
         <v>23</v>
       </c>
       <c r="AH50" s="16" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
     </row>
     <row r="51" spans="1:34" x14ac:dyDescent="0.15">
@@ -8808,10 +8832,10 @@
         <v>21400011</v>
       </c>
       <c r="B51" s="20" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C51" s="20" t="s">
-        <v>247</v>
+        <v>234</v>
       </c>
       <c r="D51" s="20"/>
       <c r="E51" s="1"/>
@@ -8858,7 +8882,7 @@
       <c r="V51" s="16"/>
       <c r="W51" s="16"/>
       <c r="X51" s="16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="Y51" s="16"/>
       <c r="Z51" s="16"/>
@@ -8877,7 +8901,7 @@
         <v>23</v>
       </c>
       <c r="AH51" s="16" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
     </row>
     <row r="52" spans="1:34" x14ac:dyDescent="0.15">
@@ -8888,11 +8912,11 @@
         <v>68</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>258</v>
+        <v>245</v>
       </c>
       <c r="D52" s="1"/>
       <c r="E52" s="19" t="s">
-        <v>284</v>
+        <v>271</v>
       </c>
       <c r="F52" s="1">
         <f t="shared" si="2"/>
@@ -8954,14 +8978,14 @@
         <v>21500002</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>248</v>
+        <v>235</v>
       </c>
       <c r="D53" s="1"/>
       <c r="E53" s="19" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
       <c r="F53" s="1">
         <f t="shared" si="2"/>
@@ -8996,10 +9020,10 @@
       <c r="V53" s="16"/>
       <c r="W53" s="16"/>
       <c r="X53" s="16" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="Y53" s="16" t="s">
-        <v>262</v>
+        <v>249</v>
       </c>
       <c r="Z53" s="16"/>
       <c r="AA53" s="16"/>
@@ -9017,7 +9041,7 @@
         <v>23</v>
       </c>
       <c r="AH53" s="16" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="54" spans="1:34" x14ac:dyDescent="0.15">
@@ -9025,14 +9049,14 @@
         <v>21500003</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>249</v>
+        <v>236</v>
       </c>
       <c r="D54" s="1"/>
       <c r="E54" s="19" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
       <c r="F54" s="1">
         <f t="shared" si="2"/>
@@ -9067,10 +9091,10 @@
       <c r="V54" s="16"/>
       <c r="W54" s="16"/>
       <c r="X54" s="16" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="Y54" s="16" t="s">
-        <v>263</v>
+        <v>250</v>
       </c>
       <c r="Z54" s="16"/>
       <c r="AA54" s="16"/>
@@ -9088,7 +9112,7 @@
         <v>23</v>
       </c>
       <c r="AH54" s="16" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="55" spans="1:34" x14ac:dyDescent="0.15">
@@ -9096,14 +9120,14 @@
         <v>21500004</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>250</v>
+        <v>237</v>
       </c>
       <c r="D55" s="1"/>
       <c r="E55" s="19" t="s">
-        <v>286</v>
+        <v>273</v>
       </c>
       <c r="F55" s="1">
         <f t="shared" si="2"/>
@@ -9161,7 +9185,7 @@
         <v>23</v>
       </c>
       <c r="AH55" s="16" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="56" spans="1:34" x14ac:dyDescent="0.15">
@@ -9169,14 +9193,14 @@
         <v>21500005</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>251</v>
+        <v>238</v>
       </c>
       <c r="D56" s="1"/>
       <c r="E56" s="19" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
       <c r="F56" s="1">
         <f t="shared" si="2"/>
@@ -9211,10 +9235,10 @@
       <c r="V56" s="16"/>
       <c r="W56" s="16"/>
       <c r="X56" s="16" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="Y56" s="16" t="s">
-        <v>264</v>
+        <v>251</v>
       </c>
       <c r="Z56" s="16"/>
       <c r="AA56" s="16"/>
@@ -9232,7 +9256,7 @@
         <v>23</v>
       </c>
       <c r="AH56" s="16" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="57" spans="1:34" x14ac:dyDescent="0.15">
@@ -9240,14 +9264,14 @@
         <v>21500006</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>252</v>
+        <v>239</v>
       </c>
       <c r="D57" s="1"/>
       <c r="E57" s="19" t="s">
-        <v>287</v>
+        <v>274</v>
       </c>
       <c r="F57" s="1">
         <f t="shared" si="2"/>
@@ -9303,7 +9327,7 @@
         <v>23</v>
       </c>
       <c r="AH57" s="16" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="58" spans="1:34" x14ac:dyDescent="0.15">
@@ -9311,14 +9335,14 @@
         <v>21500007</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>253</v>
+        <v>240</v>
       </c>
       <c r="D58" s="1"/>
       <c r="E58" s="19" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
       <c r="F58" s="1">
         <f t="shared" si="2"/>
@@ -9351,7 +9375,7 @@
       <c r="V58" s="16"/>
       <c r="W58" s="16"/>
       <c r="X58" s="16" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="Y58" s="16"/>
       <c r="Z58" s="16"/>
@@ -9370,7 +9394,7 @@
         <v>23</v>
       </c>
       <c r="AH58" s="16" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
     </row>
     <row r="59" spans="1:34" x14ac:dyDescent="0.15">
@@ -9378,14 +9402,14 @@
         <v>21500008</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="D59" s="1"/>
       <c r="E59" s="19" t="s">
-        <v>288</v>
+        <v>275</v>
       </c>
       <c r="F59" s="1">
         <f t="shared" si="2"/>
@@ -9420,7 +9444,7 @@
       <c r="V59" s="16"/>
       <c r="W59" s="16"/>
       <c r="X59" s="16" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="Y59" s="16"/>
       <c r="Z59" s="16"/>
@@ -9443,7 +9467,7 @@
         <v>23</v>
       </c>
       <c r="AH59" s="16" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
     </row>
     <row r="60" spans="1:34" x14ac:dyDescent="0.15">
@@ -9451,14 +9475,14 @@
         <v>21500009</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>199</v>
+        <v>186</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>255</v>
+        <v>242</v>
       </c>
       <c r="D60" s="1"/>
       <c r="E60" s="19" t="s">
-        <v>289</v>
+        <v>276</v>
       </c>
       <c r="F60" s="1">
         <f t="shared" si="2"/>
@@ -9491,7 +9515,7 @@
       <c r="V60" s="16"/>
       <c r="W60" s="16"/>
       <c r="X60" s="16" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="Y60" s="16"/>
       <c r="Z60" s="16">
@@ -9512,7 +9536,7 @@
         <v>23</v>
       </c>
       <c r="AH60" s="16" t="s">
-        <v>198</v>
+        <v>185</v>
       </c>
     </row>
     <row r="61" spans="1:34" x14ac:dyDescent="0.15">
@@ -9520,14 +9544,14 @@
         <v>21500010</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>201</v>
+        <v>188</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>256</v>
+        <v>243</v>
       </c>
       <c r="D61" s="1"/>
       <c r="E61" s="19" t="s">
-        <v>289</v>
+        <v>276</v>
       </c>
       <c r="F61" s="1">
         <f t="shared" si="2"/>
@@ -9560,10 +9584,10 @@
       <c r="V61" s="16"/>
       <c r="W61" s="16"/>
       <c r="X61" s="16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="Y61" s="16" t="s">
-        <v>265</v>
+        <v>252</v>
       </c>
       <c r="Z61" s="16">
         <v>31100002</v>
@@ -9583,7 +9607,7 @@
         <v>23</v>
       </c>
       <c r="AH61" s="16" t="s">
-        <v>200</v>
+        <v>187</v>
       </c>
     </row>
     <row r="62" spans="1:34" x14ac:dyDescent="0.15">
@@ -9591,14 +9615,14 @@
         <v>21500011</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>203</v>
+        <v>190</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>257</v>
+        <v>244</v>
       </c>
       <c r="D62" s="1"/>
       <c r="E62" s="19" t="s">
-        <v>289</v>
+        <v>276</v>
       </c>
       <c r="F62" s="1">
         <f t="shared" si="2"/>
@@ -9631,7 +9655,7 @@
       <c r="V62" s="16"/>
       <c r="W62" s="16"/>
       <c r="X62" s="16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="Y62" s="16"/>
       <c r="Z62" s="16">
@@ -9652,7 +9676,7 @@
         <v>23</v>
       </c>
       <c r="AH62" s="16" t="s">
-        <v>202</v>
+        <v>189</v>
       </c>
     </row>
     <row r="63" spans="1:34" x14ac:dyDescent="0.15">
@@ -9660,16 +9684,16 @@
         <v>21500012</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>312</v>
+        <v>299</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>311</v>
+        <v>298</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>316</v>
+        <v>303</v>
       </c>
       <c r="E63" s="19" t="s">
-        <v>310</v>
+        <v>297</v>
       </c>
       <c r="F63" s="1">
         <f t="shared" ref="F63" si="7">IF(T63&gt;=23,4,IF(AND(T63&gt;=18,T63&lt;23),3,IF(AND(T63&gt;=13,T63&lt;18),2,IF(AND(T63&gt;=8,T63&lt;13),1,0))))</f>
@@ -9702,7 +9726,7 @@
       <c r="V63" s="16"/>
       <c r="W63" s="16"/>
       <c r="X63" s="25" t="s">
-        <v>309</v>
+        <v>296</v>
       </c>
       <c r="Y63" s="16"/>
       <c r="Z63" s="16"/>
@@ -9721,7 +9745,7 @@
         <v>23</v>
       </c>
       <c r="AH63" s="16" t="s">
-        <v>308</v>
+        <v>295</v>
       </c>
     </row>
     <row r="64" spans="1:34" x14ac:dyDescent="0.15">
@@ -9729,16 +9753,16 @@
         <v>21500013</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>318</v>
+        <v>305</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>319</v>
+        <v>306</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>320</v>
+        <v>307</v>
       </c>
       <c r="E64" s="19" t="s">
-        <v>310</v>
+        <v>297</v>
       </c>
       <c r="F64" s="1">
         <f t="shared" ref="F64" si="9">IF(T64&gt;=23,4,IF(AND(T64&gt;=18,T64&lt;23),3,IF(AND(T64&gt;=13,T64&lt;18),2,IF(AND(T64&gt;=8,T64&lt;13),1,0))))</f>
@@ -9790,7 +9814,7 @@
         <v>23</v>
       </c>
       <c r="AH64" s="16" t="s">
-        <v>317</v>
+        <v>304</v>
       </c>
     </row>
     <row r="65" spans="1:34" x14ac:dyDescent="0.15">
@@ -9798,16 +9822,16 @@
         <v>21500014</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>322</v>
+        <v>309</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>323</v>
+        <v>310</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>324</v>
+        <v>311</v>
       </c>
       <c r="E65" s="19" t="s">
-        <v>310</v>
+        <v>297</v>
       </c>
       <c r="F65" s="1">
         <f t="shared" ref="F65" si="11">IF(T65&gt;=23,4,IF(AND(T65&gt;=18,T65&lt;23),3,IF(AND(T65&gt;=13,T65&lt;18),2,IF(AND(T65&gt;=8,T65&lt;13),1,0))))</f>
@@ -9859,7 +9883,7 @@
         <v>23</v>
       </c>
       <c r="AH65" s="16" t="s">
-        <v>321</v>
+        <v>308</v>
       </c>
     </row>
     <row r="66" spans="1:34" x14ac:dyDescent="0.15">
@@ -9867,16 +9891,16 @@
         <v>21500015</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>326</v>
+        <v>313</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>327</v>
+        <v>314</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>328</v>
+        <v>315</v>
       </c>
       <c r="E66" s="19" t="s">
-        <v>310</v>
+        <v>297</v>
       </c>
       <c r="F66" s="1">
         <f t="shared" ref="F66" si="13">IF(T66&gt;=23,4,IF(AND(T66&gt;=18,T66&lt;23),3,IF(AND(T66&gt;=13,T66&lt;18),2,IF(AND(T66&gt;=8,T66&lt;13),1,0))))</f>
@@ -9928,7 +9952,7 @@
         <v>23</v>
       </c>
       <c r="AH66" s="16" t="s">
-        <v>325</v>
+        <v>312</v>
       </c>
     </row>
   </sheetData>

</xml_diff>